<commit_message>
Fixed error with escape not showing
</commit_message>
<xml_diff>
--- a/Documentation/Events.xlsx
+++ b/Documentation/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\happysulla\BarbarianPrince\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{54EED2A3-008E-4038-A2C4-B2BF17802EEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{ADAEDEAE-A89A-46BB-8962-A201B7B4237D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -16201,54 +16201,6 @@
   </si>
   <si>
     <r>
-      <t>&lt;Bold&gt;e218 Escape&lt;/Bold&gt; &lt;InlineUIContainer&gt;&lt;Button Content='r218a' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt; Manage to find an escape path. Move along. Click image to continue.
-&lt;LineBreak/&gt; &lt;LineBreak/&gt; 
-                        &lt;InlineUIContainer&gt;&lt;Image Name='</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>EncounterEnd</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>' Source='../../Images/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Escape</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.gif' Height='400' Width='400'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>&lt;Bold&gt;e005c Fight Amazon&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;Roll for results:
  &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/dieRoll.gif' Name='DieRoll' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
@@ -34632,7 +34584,27 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>' FontFamily='Courier New'  FontSize='12'&gt; &lt;/Button&gt;&lt;/InlineUIContainer&gt; or &lt;InlineUIContainer&gt;&lt;Button Content='</t>
+      <t>' FontFamily='Courier New'  FontSize='12'&gt; &lt;/Button&gt;&lt;/InlineUIContainer&gt; or &lt;InlineUIContainer&gt;&lt;Button Name='</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Begin</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>' Content='</t>
     </r>
     <r>
       <rPr>
@@ -34653,6 +34625,54 @@
         <scheme val="minor"/>
       </rPr>
       <t>' FontFamily='Courier New'  FontSize='12'&gt; &lt;/Button&gt;&lt;/InlineUIContainer&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;Bold&gt;e218 Escape&lt;/Bold&gt; &lt;InlineUIContainer&gt;&lt;Button Content='r218a' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt; Managed to find an escape path. Click image to continue.
+&lt;LineBreak/&gt; &lt;LineBreak/&gt; 
+                        &lt;InlineUIContainer&gt;&lt;Image Name='</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>EncounterEnd</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>' Source='../../Images/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Escape</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.gif' Height='400' Width='400'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
     </r>
   </si>
 </sst>
@@ -35119,8 +35139,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B564"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A489" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B491" sqref="B491"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -35134,7 +35154,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -35142,7 +35162,7 @@
         <v>254</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -35150,7 +35170,7 @@
         <v>255</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -35158,15 +35178,15 @@
         <v>256</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="390" x14ac:dyDescent="0.25">
@@ -35182,7 +35202,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -35190,7 +35210,7 @@
         <v>22</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35222,7 +35242,7 @@
         <v>3</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -35230,7 +35250,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35254,7 +35274,7 @@
         <v>7</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -35262,7 +35282,7 @@
         <v>8</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35270,7 +35290,7 @@
         <v>10</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35278,7 +35298,7 @@
         <v>9</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -35294,7 +35314,7 @@
         <v>12</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35302,7 +35322,7 @@
         <v>13</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35310,7 +35330,7 @@
         <v>14</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -35318,7 +35338,7 @@
         <v>15</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -35326,7 +35346,7 @@
         <v>16</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -35334,7 +35354,7 @@
         <v>17</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -35342,7 +35362,7 @@
         <v>18</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -35350,31 +35370,31 @@
         <v>261</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -35382,7 +35402,7 @@
         <v>19</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -35390,7 +35410,7 @@
         <v>20</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -35398,23 +35418,23 @@
         <v>21</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -35422,23 +35442,23 @@
         <v>25</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -35446,7 +35466,7 @@
         <v>26</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -35470,7 +35490,7 @@
         <v>27</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -35486,7 +35506,7 @@
         <v>29</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -35510,7 +35530,7 @@
         <v>729</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -35518,7 +35538,7 @@
         <v>31</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -35526,7 +35546,7 @@
         <v>32</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -35534,7 +35554,7 @@
         <v>33</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -35590,7 +35610,7 @@
         <v>264</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35598,7 +35618,7 @@
         <v>265</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -35622,7 +35642,7 @@
         <v>35</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -35654,7 +35674,7 @@
         <v>37</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="285" x14ac:dyDescent="0.25">
@@ -35662,7 +35682,7 @@
         <v>38</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -35678,7 +35698,7 @@
         <v>44</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -35686,7 +35706,7 @@
         <v>733</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -35734,7 +35754,7 @@
         <v>42</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35742,7 +35762,7 @@
         <v>46</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -35766,7 +35786,7 @@
         <v>49</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35806,7 +35826,7 @@
         <v>54</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -35814,7 +35834,7 @@
         <v>55</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35822,7 +35842,7 @@
         <v>56</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35830,7 +35850,7 @@
         <v>57</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -35838,31 +35858,31 @@
         <v>58</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
+        <v>817</v>
+      </c>
+      <c r="B92" s="3" t="s">
         <v>818</v>
-      </c>
-      <c r="B92" s="3" t="s">
-        <v>819</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -35870,15 +35890,15 @@
         <v>59</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
+        <v>934</v>
+      </c>
+      <c r="B94" s="3" t="s">
         <v>935</v>
-      </c>
-      <c r="B94" s="3" t="s">
-        <v>936</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -35886,15 +35906,15 @@
         <v>60</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
+        <v>806</v>
+      </c>
+      <c r="B96" s="3" t="s">
         <v>807</v>
-      </c>
-      <c r="B96" s="3" t="s">
-        <v>808</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -35902,7 +35922,7 @@
         <v>61</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -35910,7 +35930,7 @@
         <v>62</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35942,7 +35962,7 @@
         <v>65</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -35950,7 +35970,7 @@
         <v>66</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -36030,7 +36050,7 @@
         <v>70</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -36118,7 +36138,7 @@
         <v>77</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
     </row>
     <row r="125" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -36131,10 +36151,10 @@
     </row>
     <row r="126" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
+        <v>987</v>
+      </c>
+      <c r="B126" s="3" t="s">
         <v>988</v>
-      </c>
-      <c r="B126" s="3" t="s">
-        <v>989</v>
       </c>
     </row>
     <row r="127" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -36142,7 +36162,7 @@
         <v>78</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
     </row>
     <row r="128" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -36150,7 +36170,7 @@
         <v>381</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
     </row>
     <row r="129" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -36190,7 +36210,7 @@
         <v>80</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="134" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -36198,87 +36218,87 @@
         <v>81</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
     </row>
     <row r="135" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="136" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="137" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="138" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="139" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="B139" s="3" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="140" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="141" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="142" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="143" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
+        <v>1003</v>
+      </c>
+      <c r="B143" s="3" t="s">
         <v>1004</v>
-      </c>
-      <c r="B143" s="3" t="s">
-        <v>1005</v>
       </c>
     </row>
     <row r="144" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="145" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -36286,7 +36306,7 @@
         <v>82</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="146" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -36294,7 +36314,7 @@
         <v>83</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
     </row>
     <row r="147" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -36334,7 +36354,7 @@
         <v>570</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="152" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -36342,7 +36362,7 @@
         <v>86</v>
       </c>
       <c r="B152" s="3" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
     </row>
     <row r="153" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -36454,7 +36474,7 @@
         <v>449</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
     </row>
     <row r="167" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -36478,23 +36498,23 @@
         <v>90</v>
       </c>
       <c r="B169" s="3" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
     </row>
     <row r="170" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="B170" s="3" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
     </row>
     <row r="171" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="B171" s="3" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
     </row>
     <row r="172" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -36526,7 +36546,7 @@
         <v>93</v>
       </c>
       <c r="B175" s="3" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
     </row>
     <row r="176" spans="1:2" ht="270" x14ac:dyDescent="0.25">
@@ -36534,7 +36554,7 @@
         <v>94</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="177" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -36542,7 +36562,7 @@
         <v>95</v>
       </c>
       <c r="B177" s="3" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
     </row>
     <row r="178" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -36550,55 +36570,55 @@
         <v>96</v>
       </c>
       <c r="B178" s="3" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
     </row>
     <row r="179" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A179" s="2" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="B179" s="3" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
     </row>
     <row r="180" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A180" s="2" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="B180" s="3" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
     </row>
     <row r="181" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
     </row>
     <row r="182" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="B182" s="3" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
     </row>
     <row r="183" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="B183" s="3" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
     </row>
     <row r="184" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A184" s="2" t="s">
+        <v>905</v>
+      </c>
+      <c r="B184" s="3" t="s">
         <v>906</v>
-      </c>
-      <c r="B184" s="3" t="s">
-        <v>907</v>
       </c>
     </row>
     <row r="185" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -36606,7 +36626,7 @@
         <v>97</v>
       </c>
       <c r="B185" s="3" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="186" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -36638,7 +36658,7 @@
         <v>100</v>
       </c>
       <c r="B189" s="3" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
     </row>
     <row r="190" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -36654,7 +36674,7 @@
         <v>103</v>
       </c>
       <c r="B191" s="3" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="192" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -36662,7 +36682,7 @@
         <v>104</v>
       </c>
       <c r="B192" s="3" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
     </row>
     <row r="193" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -36694,7 +36714,7 @@
         <v>106</v>
       </c>
       <c r="B196" s="3" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="197" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -36702,7 +36722,7 @@
         <v>107</v>
       </c>
       <c r="B197" s="3" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
     </row>
     <row r="198" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -36710,15 +36730,15 @@
         <v>165</v>
       </c>
       <c r="B198" s="3" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
     </row>
     <row r="199" spans="1:2" ht="225" x14ac:dyDescent="0.25">
       <c r="A199" s="2" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="B199" s="3" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
     </row>
     <row r="200" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -36726,7 +36746,7 @@
         <v>108</v>
       </c>
       <c r="B200" s="3" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="201" spans="1:2" ht="285" x14ac:dyDescent="0.25">
@@ -36734,7 +36754,7 @@
         <v>109</v>
       </c>
       <c r="B201" s="3" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
     </row>
     <row r="202" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -36742,7 +36762,7 @@
         <v>110</v>
       </c>
       <c r="B202" s="3" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
     <row r="203" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -36750,7 +36770,7 @@
         <v>166</v>
       </c>
       <c r="B203" s="3" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="204" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -36758,7 +36778,7 @@
         <v>167</v>
       </c>
       <c r="B204" s="3" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="205" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -36766,23 +36786,23 @@
         <v>168</v>
       </c>
       <c r="B205" s="3" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
     </row>
     <row r="206" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A206" s="2" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="B206" s="3" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
     </row>
     <row r="207" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A207" s="2" t="s">
+        <v>920</v>
+      </c>
+      <c r="B207" s="3" t="s">
         <v>921</v>
-      </c>
-      <c r="B207" s="3" t="s">
-        <v>922</v>
       </c>
     </row>
     <row r="208" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -36830,7 +36850,7 @@
         <v>112</v>
       </c>
       <c r="B213" s="3" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
     </row>
     <row r="214" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -36838,7 +36858,7 @@
         <v>169</v>
       </c>
       <c r="B214" s="3" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
     </row>
     <row r="215" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -36846,7 +36866,7 @@
         <v>170</v>
       </c>
       <c r="B215" s="3" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
     </row>
     <row r="216" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -36854,7 +36874,7 @@
         <v>171</v>
       </c>
       <c r="B216" s="3" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
     </row>
     <row r="217" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -36862,7 +36882,7 @@
         <v>113</v>
       </c>
       <c r="B217" s="3" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="218" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -36870,7 +36890,7 @@
         <v>114</v>
       </c>
       <c r="B218" s="3" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
     </row>
     <row r="219" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -36878,15 +36898,15 @@
         <v>266</v>
       </c>
       <c r="B219" s="3" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
     </row>
     <row r="220" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A220" s="2" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="B220" s="3" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
     </row>
     <row r="221" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -36894,15 +36914,15 @@
         <v>115</v>
       </c>
       <c r="B221" s="3" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
     </row>
     <row r="222" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A222" s="2" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="B222" s="3" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
     </row>
     <row r="223" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -36910,15 +36930,15 @@
         <v>116</v>
       </c>
       <c r="B223" s="3" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="224" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A224" s="2" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="B224" s="3" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
     </row>
     <row r="225" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -36926,31 +36946,31 @@
         <v>117</v>
       </c>
       <c r="B225" s="4" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="226" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A226" s="2" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="B226" s="4" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
     </row>
     <row r="227" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A227" s="2" t="s">
+        <v>775</v>
+      </c>
+      <c r="B227" s="4" t="s">
         <v>776</v>
-      </c>
-      <c r="B227" s="4" t="s">
-        <v>777</v>
       </c>
     </row>
     <row r="228" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A228" s="2" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="B228" s="4" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
     </row>
     <row r="229" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -36958,23 +36978,23 @@
         <v>118</v>
       </c>
       <c r="B229" s="3" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
     </row>
     <row r="230" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A230" s="2" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="B230" s="3" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
     </row>
     <row r="231" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A231" s="2" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="B231" s="3" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="232" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -36982,23 +37002,23 @@
         <v>119</v>
       </c>
       <c r="B232" s="3" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
     </row>
     <row r="233" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A233" s="2" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="B233" s="3" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
     </row>
     <row r="234" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A234" s="2" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="B234" s="3" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
     </row>
     <row r="235" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -37006,7 +37026,7 @@
         <v>120</v>
       </c>
       <c r="B235" s="3" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
     </row>
     <row r="236" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -37014,7 +37034,7 @@
         <v>172</v>
       </c>
       <c r="B236" s="3" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
     </row>
     <row r="237" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37022,7 +37042,7 @@
         <v>173</v>
       </c>
       <c r="B237" s="3" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
     </row>
     <row r="238" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37030,7 +37050,7 @@
         <v>174</v>
       </c>
       <c r="B238" s="3" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
     </row>
     <row r="239" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37046,15 +37066,15 @@
         <v>122</v>
       </c>
       <c r="B240" s="3" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
     </row>
     <row r="241" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A241" s="2" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="B241" s="3" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
     </row>
     <row r="242" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -37062,23 +37082,23 @@
         <v>123</v>
       </c>
       <c r="B242" s="3" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
     </row>
     <row r="243" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A243" s="2" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="B243" s="3" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
     </row>
     <row r="244" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A244" s="2" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="B244" s="3" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
     </row>
     <row r="245" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37086,7 +37106,7 @@
         <v>124</v>
       </c>
       <c r="B245" s="3" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="246" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37094,15 +37114,15 @@
         <v>125</v>
       </c>
       <c r="B246" s="3" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="247" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A247" s="2" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="B247" s="3" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="248" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37110,7 +37130,7 @@
         <v>126</v>
       </c>
       <c r="B248" s="3" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="249" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37118,7 +37138,7 @@
         <v>127</v>
       </c>
       <c r="B249" s="3" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
     </row>
     <row r="250" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37126,7 +37146,7 @@
         <v>128</v>
       </c>
       <c r="B250" s="3" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="251" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -37134,7 +37154,7 @@
         <v>129</v>
       </c>
       <c r="B251" s="3" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="252" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37142,7 +37162,7 @@
         <v>130</v>
       </c>
       <c r="B252" s="3" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
     </row>
     <row r="253" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -37150,23 +37170,23 @@
         <v>131</v>
       </c>
       <c r="B253" s="3" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
     </row>
     <row r="254" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A254" s="2" t="s">
+        <v>977</v>
+      </c>
+      <c r="B254" s="3" t="s">
         <v>978</v>
-      </c>
-      <c r="B254" s="3" t="s">
-        <v>979</v>
       </c>
     </row>
     <row r="255" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A255" s="2" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="B255" s="3" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
     </row>
     <row r="256" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -37174,7 +37194,7 @@
         <v>132</v>
       </c>
       <c r="B256" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="257" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -37182,15 +37202,15 @@
         <v>133</v>
       </c>
       <c r="B257" s="3" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="258" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A258" s="2" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="B258" s="3" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="259" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37198,23 +37218,23 @@
         <v>134</v>
       </c>
       <c r="B259" s="3" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="260" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A260" s="2" t="s">
+        <v>1033</v>
+      </c>
+      <c r="B260" s="3" t="s">
         <v>1034</v>
-      </c>
-      <c r="B260" s="3" t="s">
-        <v>1035</v>
       </c>
     </row>
     <row r="261" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A261" s="2" t="s">
+        <v>1035</v>
+      </c>
+      <c r="B261" s="3" t="s">
         <v>1036</v>
-      </c>
-      <c r="B261" s="3" t="s">
-        <v>1037</v>
       </c>
     </row>
     <row r="262" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -37222,15 +37242,15 @@
         <v>135</v>
       </c>
       <c r="B262" s="3" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="263" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A263" s="2" t="s">
+        <v>1038</v>
+      </c>
+      <c r="B263" s="3" t="s">
         <v>1039</v>
-      </c>
-      <c r="B263" s="3" t="s">
-        <v>1040</v>
       </c>
     </row>
     <row r="264" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -37238,7 +37258,7 @@
         <v>136</v>
       </c>
       <c r="B264" s="3" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="265" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -37262,7 +37282,7 @@
         <v>233</v>
       </c>
       <c r="B267" s="3" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
     </row>
     <row r="268" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -37294,7 +37314,7 @@
         <v>139</v>
       </c>
       <c r="B271" s="3" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
     </row>
     <row r="272" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -37302,7 +37322,7 @@
         <v>239</v>
       </c>
       <c r="B272" s="3" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
     </row>
     <row r="273" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37310,7 +37330,7 @@
         <v>240</v>
       </c>
       <c r="B273" s="3" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
     </row>
     <row r="274" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37318,7 +37338,7 @@
         <v>241</v>
       </c>
       <c r="B274" s="3" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
     </row>
     <row r="275" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37326,7 +37346,7 @@
         <v>140</v>
       </c>
       <c r="B275" s="3" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="276" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -37334,7 +37354,7 @@
         <v>236</v>
       </c>
       <c r="B276" s="3" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="277" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37342,7 +37362,7 @@
         <v>237</v>
       </c>
       <c r="B277" s="3" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="278" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37350,7 +37370,7 @@
         <v>238</v>
       </c>
       <c r="B278" s="3" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="279" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -37358,7 +37378,7 @@
         <v>141</v>
       </c>
       <c r="B279" s="3" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="280" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -37366,7 +37386,7 @@
         <v>142</v>
       </c>
       <c r="B280" s="3" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="281" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -37374,7 +37394,7 @@
         <v>143</v>
       </c>
       <c r="B281" s="3" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="282" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -37382,7 +37402,7 @@
         <v>144</v>
       </c>
       <c r="B282" s="3" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="283" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -37390,7 +37410,7 @@
         <v>242</v>
       </c>
       <c r="B283" s="3" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="284" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37398,7 +37418,7 @@
         <v>145</v>
       </c>
       <c r="B284" s="3" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="285" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -37406,7 +37426,7 @@
         <v>146</v>
       </c>
       <c r="B285" s="3" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="286" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37414,7 +37434,7 @@
         <v>147</v>
       </c>
       <c r="B286" s="3" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="287" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -37422,7 +37442,7 @@
         <v>148</v>
       </c>
       <c r="B287" s="3" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="288" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -37430,31 +37450,31 @@
         <v>149</v>
       </c>
       <c r="B288" s="3" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="289" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A289" s="2" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
       <c r="B289" s="3" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="290" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A290" s="2" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="B290" s="3" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="291" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A291" s="2" t="s">
+        <v>1111</v>
+      </c>
+      <c r="B291" s="3" t="s">
         <v>1112</v>
-      </c>
-      <c r="B291" s="3" t="s">
-        <v>1113</v>
       </c>
     </row>
     <row r="292" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37462,15 +37482,15 @@
         <v>150</v>
       </c>
       <c r="B292" s="3" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="293" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A293" s="2" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="B293" s="3" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="294" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -37478,7 +37498,7 @@
         <v>151</v>
       </c>
       <c r="B294" s="3" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
     </row>
     <row r="295" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37486,7 +37506,7 @@
         <v>243</v>
       </c>
       <c r="B295" s="3" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
     </row>
     <row r="296" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37494,7 +37514,7 @@
         <v>244</v>
       </c>
       <c r="B296" s="3" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
     </row>
     <row r="297" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37502,7 +37522,7 @@
         <v>245</v>
       </c>
       <c r="B297" s="3" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="298" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37510,7 +37530,7 @@
         <v>152</v>
       </c>
       <c r="B298" s="3" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
     </row>
     <row r="299" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -37518,7 +37538,7 @@
         <v>153</v>
       </c>
       <c r="B299" s="3" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="300" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37526,7 +37546,7 @@
         <v>154</v>
       </c>
       <c r="B300" s="3" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
     </row>
     <row r="301" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -37534,7 +37554,7 @@
         <v>155</v>
       </c>
       <c r="B301" s="3" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
     </row>
     <row r="302" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37542,7 +37562,7 @@
         <v>156</v>
       </c>
       <c r="B302" s="3" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
     </row>
     <row r="303" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -37550,7 +37570,7 @@
         <v>157</v>
       </c>
       <c r="B303" s="3" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="304" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -37558,7 +37578,7 @@
         <v>246</v>
       </c>
       <c r="B304" s="3" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
     </row>
     <row r="305" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37566,7 +37586,7 @@
         <v>247</v>
       </c>
       <c r="B305" s="3" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="306" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37574,7 +37594,7 @@
         <v>248</v>
       </c>
       <c r="B306" s="3" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
     </row>
     <row r="307" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37582,7 +37602,7 @@
         <v>158</v>
       </c>
       <c r="B307" s="3" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
     </row>
     <row r="308" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -37590,7 +37610,7 @@
         <v>159</v>
       </c>
       <c r="B308" s="3" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
     </row>
     <row r="309" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37598,7 +37618,7 @@
         <v>160</v>
       </c>
       <c r="B309" s="3" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="310" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -37606,7 +37626,7 @@
         <v>161</v>
       </c>
       <c r="B310" s="3" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="311" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37614,31 +37634,31 @@
         <v>162</v>
       </c>
       <c r="B311" s="3" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="312" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A312" s="2" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="B312" s="3" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="313" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A313" s="2" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="B313" s="3" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="314" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A314" s="2" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="B314" s="3" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="315" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37646,7 +37666,7 @@
         <v>163</v>
       </c>
       <c r="B315" s="3" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="316" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -37654,7 +37674,7 @@
         <v>164</v>
       </c>
       <c r="B316" s="3" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="317" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37662,7 +37682,7 @@
         <v>175</v>
       </c>
       <c r="B317" s="3" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="318" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -37670,7 +37690,7 @@
         <v>176</v>
       </c>
       <c r="B318" s="3" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="319" spans="1:2" ht="390" x14ac:dyDescent="0.25">
@@ -37678,7 +37698,7 @@
         <v>177</v>
       </c>
       <c r="B319" s="3" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="320" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -37686,7 +37706,7 @@
         <v>531</v>
       </c>
       <c r="B320" s="3" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="321" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37694,7 +37714,7 @@
         <v>532</v>
       </c>
       <c r="B321" s="3" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="322" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37702,7 +37722,7 @@
         <v>533</v>
       </c>
       <c r="B322" s="3" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="323" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -37718,7 +37738,7 @@
         <v>536</v>
       </c>
       <c r="B324" s="3" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="325" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37726,7 +37746,7 @@
         <v>537</v>
       </c>
       <c r="B325" s="3" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="326" spans="1:2" ht="390" x14ac:dyDescent="0.25">
@@ -37734,7 +37754,7 @@
         <v>178</v>
       </c>
       <c r="B326" s="3" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="327" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -37742,7 +37762,7 @@
         <v>504</v>
       </c>
       <c r="B327" s="3" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="328" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37750,7 +37770,7 @@
         <v>566</v>
       </c>
       <c r="B328" s="3" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="329" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37758,7 +37778,7 @@
         <v>567</v>
       </c>
       <c r="B329" s="3" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="330" spans="1:2" ht="315" x14ac:dyDescent="0.25">
@@ -37766,7 +37786,7 @@
         <v>179</v>
       </c>
       <c r="B330" s="3" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
     </row>
     <row r="331" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -37774,7 +37794,7 @@
         <v>249</v>
       </c>
       <c r="B331" s="3" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
     </row>
     <row r="332" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -37782,7 +37802,7 @@
         <v>250</v>
       </c>
       <c r="B332" s="3" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
     </row>
     <row r="333" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -37790,7 +37810,7 @@
         <v>251</v>
       </c>
       <c r="B333" s="3" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
     </row>
     <row r="334" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -37798,7 +37818,7 @@
         <v>252</v>
       </c>
       <c r="B334" s="3" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
     </row>
     <row r="335" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -37806,23 +37826,23 @@
         <v>253</v>
       </c>
       <c r="B335" s="3" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
     </row>
     <row r="336" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A336" s="2" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="B336" s="3" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
     </row>
     <row r="337" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A337" s="2" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="B337" s="3" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="338" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -37830,7 +37850,7 @@
         <v>180</v>
       </c>
       <c r="B338" s="3" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="339" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -37934,7 +37954,7 @@
         <v>465</v>
       </c>
       <c r="B351" s="3" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
     </row>
     <row r="352" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37998,7 +38018,7 @@
         <v>344</v>
       </c>
       <c r="B359" s="3" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
     </row>
     <row r="360" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -38022,7 +38042,7 @@
         <v>196</v>
       </c>
       <c r="B362" s="3" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
     </row>
     <row r="363" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -38030,7 +38050,7 @@
         <v>333</v>
       </c>
       <c r="B363" s="3" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
     </row>
     <row r="364" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -38086,7 +38106,7 @@
         <v>202</v>
       </c>
       <c r="B370" s="3" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="371" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -38206,7 +38226,7 @@
         <v>608</v>
       </c>
       <c r="B385" s="3" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
     </row>
     <row r="386" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -38214,7 +38234,7 @@
         <v>609</v>
       </c>
       <c r="B386" s="3" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="387" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -38222,7 +38242,7 @@
         <v>610</v>
       </c>
       <c r="B387" s="3" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
     </row>
     <row r="388" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -38230,7 +38250,7 @@
         <v>611</v>
       </c>
       <c r="B388" s="3" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
     </row>
     <row r="389" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38246,7 +38266,7 @@
         <v>613</v>
       </c>
       <c r="B390" s="3" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
     </row>
     <row r="391" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38262,7 +38282,7 @@
         <v>207</v>
       </c>
       <c r="B392" s="3" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="393" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -38286,7 +38306,7 @@
         <v>663</v>
       </c>
       <c r="B395" s="3" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
     </row>
     <row r="396" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -38446,7 +38466,7 @@
         <v>213</v>
       </c>
       <c r="B415" s="3" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
     </row>
     <row r="416" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -38462,7 +38482,7 @@
         <v>215</v>
       </c>
       <c r="B417" s="3" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="418" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38502,7 +38522,7 @@
         <v>220</v>
       </c>
       <c r="B422" s="3" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
     </row>
     <row r="423" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -38534,7 +38554,7 @@
         <v>224</v>
       </c>
       <c r="B426" s="3" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
     </row>
     <row r="427" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -38558,7 +38578,7 @@
         <v>225</v>
       </c>
       <c r="B429" s="3" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
     </row>
     <row r="430" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -38622,7 +38642,7 @@
         <v>453</v>
       </c>
       <c r="B437" s="3" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
     </row>
     <row r="438" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -38646,15 +38666,15 @@
         <v>602</v>
       </c>
       <c r="B440" s="3" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
     </row>
     <row r="441" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A441" s="2" t="s">
+        <v>813</v>
+      </c>
+      <c r="B441" s="3" t="s">
         <v>814</v>
-      </c>
-      <c r="B441" s="3" t="s">
-        <v>815</v>
       </c>
     </row>
     <row r="442" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -38678,7 +38698,7 @@
         <v>321</v>
       </c>
       <c r="B444" s="3" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="445" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -38686,15 +38706,15 @@
         <v>318</v>
       </c>
       <c r="B445" s="3" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="446" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A446" s="2" t="s">
+        <v>1086</v>
+      </c>
+      <c r="B446" s="3" t="s">
         <v>1087</v>
-      </c>
-      <c r="B446" s="3" t="s">
-        <v>1088</v>
       </c>
     </row>
     <row r="447" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -38766,7 +38786,7 @@
         <v>576</v>
       </c>
       <c r="B455" s="3" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="456" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -38790,7 +38810,7 @@
         <v>585</v>
       </c>
       <c r="B458" s="3" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="459" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38814,7 +38834,7 @@
         <v>588</v>
       </c>
       <c r="B461" s="3" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="462" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -38838,7 +38858,7 @@
         <v>591</v>
       </c>
       <c r="B464" s="3" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="465" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -38862,7 +38882,7 @@
         <v>600</v>
       </c>
       <c r="B467" s="3" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
     </row>
     <row r="468" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -38870,7 +38890,7 @@
         <v>622</v>
       </c>
       <c r="B468" s="3" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
     </row>
     <row r="469" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -38878,7 +38898,7 @@
         <v>640</v>
       </c>
       <c r="B469" s="3" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
     </row>
     <row r="470" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -38886,7 +38906,7 @@
         <v>641</v>
       </c>
       <c r="B470" s="3" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
     <row r="471" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -38894,15 +38914,15 @@
         <v>642</v>
       </c>
       <c r="B471" s="3" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
     </row>
     <row r="472" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A472" s="2" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="B472" s="3" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
     </row>
     <row r="473" spans="1:2" ht="255" x14ac:dyDescent="0.25">
@@ -38910,7 +38930,7 @@
         <v>683</v>
       </c>
       <c r="B473" s="1" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="474" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -38958,7 +38978,7 @@
         <v>689</v>
       </c>
       <c r="B479" s="1" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
     </row>
     <row r="480" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -38998,7 +39018,7 @@
         <v>694</v>
       </c>
       <c r="B484" s="1" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
     </row>
     <row r="485" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -39027,18 +39047,18 @@
     </row>
     <row r="488" spans="1:2" ht="255" x14ac:dyDescent="0.25">
       <c r="A488" s="2" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="B488" s="1" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="489" spans="1:2" ht="92.25" x14ac:dyDescent="0.25">
       <c r="A489" s="2" t="s">
+        <v>1064</v>
+      </c>
+      <c r="B489" s="1" t="s">
         <v>1065</v>
-      </c>
-      <c r="B489" s="1" t="s">
-        <v>1066</v>
       </c>
     </row>
     <row r="490" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -39046,7 +39066,7 @@
         <v>713</v>
       </c>
       <c r="B490" s="1" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
     </row>
     <row r="491" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -39054,7 +39074,7 @@
         <v>749</v>
       </c>
       <c r="B491" s="3" t="s">
-        <v>765</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="492" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -39070,7 +39090,7 @@
         <v>562</v>
       </c>
       <c r="B493" s="3" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
     <row r="494" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -39078,7 +39098,7 @@
         <v>563</v>
       </c>
       <c r="B494" s="3" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
     </row>
     <row r="495" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39150,7 +39170,7 @@
         <v>275</v>
       </c>
       <c r="B503" s="1" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="504" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39158,7 +39178,7 @@
         <v>276</v>
       </c>
       <c r="B504" s="1" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="505" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39166,7 +39186,7 @@
         <v>277</v>
       </c>
       <c r="B505" s="1" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="506" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -39214,7 +39234,7 @@
         <v>260</v>
       </c>
       <c r="B511" s="3" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="512" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39222,7 +39242,7 @@
         <v>484</v>
       </c>
       <c r="B512" s="3" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
     </row>
     <row r="513" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -39230,15 +39250,15 @@
         <v>485</v>
       </c>
       <c r="B513" s="1" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
     </row>
     <row r="514" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A514" s="2" t="s">
+        <v>821</v>
+      </c>
+      <c r="B514" s="3" t="s">
         <v>822</v>
-      </c>
-      <c r="B514" s="3" t="s">
-        <v>823</v>
       </c>
     </row>
     <row r="515" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39286,7 +39306,7 @@
         <v>285</v>
       </c>
       <c r="B520" s="1" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
     </row>
     <row r="521" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -39294,7 +39314,7 @@
         <v>286</v>
       </c>
       <c r="B521" s="1" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
     </row>
     <row r="522" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -39374,7 +39394,7 @@
         <v>296</v>
       </c>
       <c r="B531" s="1" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
     </row>
     <row r="532" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -39414,7 +39434,7 @@
         <v>298</v>
       </c>
       <c r="B536" s="1" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="537" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -39454,7 +39474,7 @@
         <v>300</v>
       </c>
       <c r="B541" s="1" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
     </row>
     <row r="542" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -39462,7 +39482,7 @@
         <v>301</v>
       </c>
       <c r="B542" s="1" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
     </row>
     <row r="543" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -39590,7 +39610,7 @@
         <v>307</v>
       </c>
       <c r="B558" s="1" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="559" spans="1:2" ht="375" x14ac:dyDescent="0.25">
@@ -39622,7 +39642,7 @@
         <v>380</v>
       </c>
       <c r="B562" s="3" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="563" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -39638,7 +39658,7 @@
         <v>331</v>
       </c>
       <c r="B564" s="3" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implement startup fixes with mercenary
</commit_message>
<xml_diff>
--- a/Documentation/Events.xlsx
+++ b/Documentation/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\happysulla\BarbarianPrince\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{ADAEDEAE-A89A-46BB-8962-A201B7B4237D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{39B11948-9E01-4F26-BAEB-2491E5169A61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -34408,65 +34408,6 @@
   </si>
   <si>
     <r>
-      <t>&lt;Bold&gt;e002a Encounter Mercenary Royal Guardsmen&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Mercenary thugs, dressed by the usurpers as their royal guardsmen, are riding toward you! Roll one die for the number of men:
- &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>dieRoll</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">.gif' </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Name='DieRoll'</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Height='21'  Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;Each has a combat skill 5, endurance 4, wealth 4. Your options are:
-&lt;LineBreak/&gt;
- &lt;InlineUIContainer&gt;&lt;Button FontFamily='Courier New'  FontSize='12'  Content='Talk ' Name='e002b'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   -&gt;  
- &lt;InlineUIContainer&gt;&lt;Button FontFamily='Courier New'  FontSize='12' Content='e002b'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;&lt;LineBreak/&gt;
- &lt;InlineUIContainer&gt;&lt;Button FontFamily='Courier New'  FontSize='12' Content='Evade' Name='e002c'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   -&gt;  
- &lt;InlineUIContainer&gt;&lt;Button FontFamily='Courier New'  FontSize='12' Content='e002c'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;*&lt;LineBreak/&gt;
- &lt;InlineUIContainer&gt;&lt;Button FontFamily='Courier New'  FontSize='12' Content='Fight' Name='e002d'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   -&gt;  
- &lt;InlineUIContainer&gt;&lt;Button FontFamily='Courier New'  FontSize='12' Content='e002d'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-*If your entire party has some kind of mount, you can attempt the evade option and add one to the die roll. Additionally, if you want to evade using the plus 1 modifier, you must adbandon unmounted members of the party
- &lt;InlineUIContainer&gt;&lt;Button Content='Abandon' Visibility='Hidden' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>&lt;Bold&gt;e000a Cal Arath - Barbarian Prince&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;Each character in the game has a endurance value, combat value, wounds, and starvation days. If endurance reaches zero, the character is dead. If the endurance reaches one, the character is unconscious. Wounds decrease endurance, and starvation days decrease the ability to carry loads. 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;You are Cal Arath, rightful heir to the throne of the Northlands Kingdom. 
@@ -34673,6 +34614,62 @@
         <scheme val="minor"/>
       </rPr>
       <t>.gif' Height='400' Width='400'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;Bold&gt;e002a Encounter Mercenary Royal Guardsmen&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Mercenary thugs, dressed by the usurpers as their royal guardsmen, are riding toward you! Roll one die for the number of men:
+ &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dieRoll</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">.gif' </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Name='DieRoll'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Height='21'  Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;Each has a combat skill 5, endurance 4, wealth 4. Your options are:
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+ &lt;InlineUIContainer&gt;&lt;Button FontFamily='Courier New'  FontSize='12'  Content='Talk ' Name='e002b'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   -&gt;  
+ &lt;InlineUIContainer&gt;&lt;Button FontFamily='Courier New'  FontSize='12' Content='e002b'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;&lt;LineBreak/&gt;
+ &lt;InlineUIContainer&gt;&lt;Button FontFamily='Courier New'  FontSize='12' Content='Evade' Name='e002c'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   -&gt;  
+ &lt;InlineUIContainer&gt;&lt;Button FontFamily='Courier New'  FontSize='12' Content='e002c'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;*&lt;LineBreak/&gt;
+ &lt;InlineUIContainer&gt;&lt;Button FontFamily='Courier New'  FontSize='12' Content='Fight' Name='e002d'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   -&gt;  
+ &lt;InlineUIContainer&gt;&lt;Button FontFamily='Courier New'  FontSize='12' Content='e002d'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;</t>
     </r>
   </si>
 </sst>
@@ -35139,8 +35136,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B564"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A489" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B491" sqref="B491"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -35154,7 +35151,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -35162,7 +35159,7 @@
         <v>254</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -35205,12 +35202,12 @@
         <v>839</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="225" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>1124</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -39074,7 +39071,7 @@
         <v>749</v>
       </c>
       <c r="B491" s="3" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="492" spans="1:2" ht="180" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fix issue with e110a in SS. Add IsDuplicateMount(). Report error if there is duplciate.
</commit_message>
<xml_diff>
--- a/Documentation/Events.xlsx
+++ b/Documentation/Events.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\happysulla\BarbarianPrince\bin\Config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\happysulla\BarbarianPrince\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47E2CD5E-709F-4A11-8D1B-4230E94179E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{37DA222E-B23B-43D7-A099-5ABA6067CB78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -33600,98 +33600,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t>&lt;Bold&gt;e110a Air Spirit Recognized&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;Since you have a magician, wizard, witch, or monk in your party, you recognize it. You can attempt to if you wish.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;To talk to the air spirit, roll one die: &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>dieRoll</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.gif' Name='</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>DieRoll</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>' Height='21'  Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;Roll &gt;= wit and wiles, communication fails. See &lt;InlineUIContainer&gt;&lt;Button Content='e110b' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
-&lt;LineBreak/&gt;Roll &lt; wit and wiles, communication succeeds. See &lt;InlineUIContainer&gt;&lt;Button Content='e110c' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;To continue without communicating with air sprint, click image.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                              &lt;InlineUIContainer&gt;&lt;Image Name='</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>EncounterEnd</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>' Source='../../Images/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>AirSpirit</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.gif' Height='300' Width='300'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-    </r>
-  </si>
-  <si>
     <t>e111a</t>
   </si>
   <si>
@@ -34759,6 +34667,98 @@
         <scheme val="minor"/>
       </rPr>
       <t>.gif' Height='300' Width='240'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;Bold&gt;e110a Air Spirit Recognized&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;Since you have a magician, wizard, witch, or monk in your party, you recognize it. You can attempt to if you wish.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;To talk to the air spirit, roll one die: &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dieRoll</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.gif' Name='</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DieRoll</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>' Height='21'  Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;Roll is greater or equal to your wit and wiles, communication fails. See &lt;InlineUIContainer&gt;&lt;Button Content='e110b' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
+&lt;LineBreak/&gt;Roll is less than wit and wiles, communication succeeds. See &lt;InlineUIContainer&gt;&lt;Button Content='e110c' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;To continue without communicating with air sprint, click image.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                              &lt;InlineUIContainer&gt;&lt;Image Name='</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>EncounterEnd</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>' Source='../../Images/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>AirSpirit</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.gif' Height='300' Width='300'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
     </r>
   </si>
 </sst>
@@ -35225,8 +35225,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B565"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A212" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B216" sqref="B216"/>
+    <sheetView tabSelected="1" topLeftCell="A286" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B289" sqref="B289"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -35240,7 +35240,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -35248,7 +35248,7 @@
         <v>254</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -35256,7 +35256,7 @@
         <v>255</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -35264,15 +35264,15 @@
         <v>256</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="390" x14ac:dyDescent="0.25">
@@ -35296,7 +35296,7 @@
         <v>22</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -36864,7 +36864,7 @@
         <v>167</v>
       </c>
       <c r="B204" s="3" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="205" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -36960,7 +36960,7 @@
         <v>171</v>
       </c>
       <c r="B216" s="3" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="217" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37544,7 +37544,7 @@
         <v>1100</v>
       </c>
       <c r="B289" s="3" t="s">
-        <v>1105</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="290" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37568,15 +37568,15 @@
         <v>150</v>
       </c>
       <c r="B292" s="3" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="293" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A293" s="2" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="B293" s="3" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="294" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -37816,7 +37816,7 @@
         <v>530</v>
       </c>
       <c r="B323" s="3" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="324" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37837,10 +37837,10 @@
     </row>
     <row r="326" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A326" s="2" t="s">
+        <v>1123</v>
+      </c>
+      <c r="B326" s="3" t="s">
         <v>1124</v>
-      </c>
-      <c r="B326" s="3" t="s">
-        <v>1125</v>
       </c>
     </row>
     <row r="327" spans="1:2" ht="390" x14ac:dyDescent="0.25">
@@ -37976,7 +37976,7 @@
         <v>183</v>
       </c>
       <c r="B343" s="3" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="344" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -38576,7 +38576,7 @@
         <v>215</v>
       </c>
       <c r="B418" s="3" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="419" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38736,7 +38736,7 @@
         <v>449</v>
       </c>
       <c r="B438" s="3" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="439" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -38776,7 +38776,7 @@
         <v>319</v>
       </c>
       <c r="B443" s="3" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="444" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -38784,7 +38784,7 @@
         <v>320</v>
       </c>
       <c r="B444" s="3" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="445" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -38792,7 +38792,7 @@
         <v>321</v>
       </c>
       <c r="B445" s="3" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="446" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -38800,7 +38800,7 @@
         <v>318</v>
       </c>
       <c r="B446" s="3" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="447" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -38816,7 +38816,7 @@
         <v>322</v>
       </c>
       <c r="B448" s="3" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="449" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39168,7 +39168,7 @@
         <v>744</v>
       </c>
       <c r="B492" s="3" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="493" spans="1:2" ht="180" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fix errror with Options Selection. Fix issue with Combat... ResetGrid() failed when have poison
</commit_message>
<xml_diff>
--- a/Documentation/Events.xlsx
+++ b/Documentation/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\happysulla\BarbarianPrince\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{37DA222E-B23B-43D7-A099-5ABA6067CB78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9D3BC1FB-D863-48F9-809C-2A87CA8EB0A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -8601,129 +8601,6 @@
   </si>
   <si>
     <r>
-      <t>&lt;Bold&gt;e185 Poison Drug&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;This drug can be applied to the weapons of any one character in your party. Its use means that whenever that character strikes in combat
- &lt;InlineUIContainer&gt;&lt;Button Content='r220' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
- and inflicts wounds, one extra poisoned wound is inflicted in addition to normal wounds.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;After a combat where the poisoned weapon is used, roll one die. A result of 6 means the poison has worn off and the weapon returns to normal.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;Since a character often has multiple weapons, he has the option of using his poisoned weapon or a normal weapon as desired. Click image when ready to continue.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                   &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B0F0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>PoisonDrug</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.gif' Name='EncounterEnd' Height='300' Width='300'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>&lt;Bold&gt;e186 Magic Sword&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;A character can carry this special sword amoung his weapons. The magic sword adds one to the combat skill of the character with it.
-In addition, the blade's magic means that every wound it inflicts counts as a poisoned wound. Click image when ready to continue.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                   &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Sword</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.gif' Name='EncounterEnd' Height='200' Width='600'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>&lt;Bold&gt;e187 Anti-poison Amulet&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;This protects against all poisoned wounds. Any poison wound inflicted is ignored if the target has the amulet. Normal wounds still take effect. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;Each time a poison wound is prevented, roll two die. If the result is 12, the amulet has reached its limit. It cannot absorb more poison and must be discarded. Click image when ready to continue.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                        &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>AmuletAntiPoison</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.gif' Name='EncounterEnd' Height='350' Width='350'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>&lt;Bold&gt;e188a Pegasus Talisman&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-You have acquired a Pegaus Talisman
- &lt;InlineUIContainer&gt;&lt;Button Content='r188a' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Whenever you have any magician, wizard, witch, priest, or monk in your party; they can help you use the talisman to call upon an actual Pegasus winged mount. It will immediately appear and serve as your mount
- &lt;InlineUIContainer&gt;&lt;Button Content='r188'  FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                   &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>TalismanPegasus</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.gif' Name='EncounterEnd' Height='400' Width='400'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>&lt;Bold&gt;e190 Nerve Gas Bomb&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;This sealed jar is filled with a deadly and quick-acting gas created by a master alchemist. If you surprise an enemy in combat
  &lt;InlineUIContainer&gt;&lt;Button Content='r220' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;,
@@ -18493,56 +18370,6 @@
   </si>
   <si>
     <r>
-      <t>&lt;Bold&gt;e026 Search for Treasure One More Time&lt;/Bold&gt;
-Clues suggest the treasure is in adjacent hext. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;Roll one die (1-N, 2-NE, 3-SE- 4-S, 5-SW, 6-NW):
- &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>dieRoll</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.gif' Name='</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>DieRoll</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>' Height='21' Width='21'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-See &lt;InlineUIContainer&gt;&lt;Button Content='e026' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; when you arrive.</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>&lt;Bold&gt;e027 Ancient Treasure&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;You find an ancient treasure that was long lost. It has wealth code 110. See
  &lt;InlineUIContainer&gt;&lt;Button Content='r225' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.  Click image to continue.
@@ -24834,44 +24661,6 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">.gif' Height='300'  Width='300'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt; </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>&lt;Bold&gt;e188 Pegasus Mount&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-You have acquired a Pegaus - a winged horse that allows you to travel airborne. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-The Pegasus is like a normal mount in all other respects including the same transport ability
- &lt;InlineUIContainer&gt;&lt;Button Content='r206' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
-, food requirements
- &lt;InlineUIContainer&gt;&lt;Button Content='r215' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;, 
- and lodging when in towns/castles/temples
- &lt;InlineUIContainer&gt;&lt;Button Content='r217' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-You can use the Pegasus as a normal mount on the ground if desired. Click image when ready to continue.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                 &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Pegasus</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.gif' Name='EncounterEnd' Height='300' Width='300'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
     </r>
   </si>
   <si>
@@ -34759,6 +34548,318 @@
         <scheme val="minor"/>
       </rPr>
       <t>.gif' Height='300' Width='300'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;Bold&gt;e188 Pegasus Mount&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+You have acquired a Pegaus - a winged horse that allows you to travel airborne. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The Pegasus is like a normal mount in all other respects including the same transport ability
+ &lt;InlineUIContainer&gt;&lt;Button Content='r206' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+, food requirements
+ &lt;InlineUIContainer&gt;&lt;Button Content='r215' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;, 
+ and lodging when in towns/castles/temples
+ &lt;InlineUIContainer&gt;&lt;Button Content='r217' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+You can use the Pegasus as a normal mount on the ground if desired. Click image when ready to continue.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                 &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Pegasus</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.gif' Name='</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>EncounterEnd</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>' Height='300' Width='300'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;Bold&gt;e187 Anti-poison Amulet&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;This protects against all poisoned wounds. Any poison wound inflicted is ignored if the target has the amulet. Normal wounds still take effect. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;Each time a poison wound is prevented, roll two die. If the result is 12, the amulet has reached its limit. It cannot absorb more poison and must be discarded. Click image when ready to continue.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                        &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>AmuletAntiPoison</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.gif' Name='</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>EncounterEnd</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>' Height='350' Width='350'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;Bold&gt;e186 Magic Sword&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;A character can carry this special sword amoung his weapons. The magic sword adds one to the combat skill of the character with it.
+In addition, the blade's magic means that every wound it inflicts counts as a poisoned wound. Click image when ready to continue.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                   &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Sword</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.gif' Name='</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>EncounterEnd</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>' Height='200' Width='600'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;Bold&gt;e185 Poison Drug&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;This drug can be applied to the weapons of any one character in your party. Its use means that whenever that character strikes in combat
+ &lt;InlineUIContainer&gt;&lt;Button Content='r220' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+ and inflicts wounds, one extra poisoned wound is inflicted in addition to normal wounds.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;After a combat where the poisoned weapon is used, roll one die. A result of 6 means the poison has worn off and the weapon returns to normal.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;Since a character often has multiple weapons, he has the option of using his poisoned weapon or a normal weapon as desired. Click image when ready to continue.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                   &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>PoisonDrug</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.gif' Name='</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>EncounterEnd</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>' Height='300' Width='300'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;Bold&gt;e188a Pegasus Talisman&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+You have acquired a Pegaus Talisman
+ &lt;InlineUIContainer&gt;&lt;Button Content='r188a' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Whenever you have any magician, wizard, witch, priest, or monk in your party; they can help you use the talisman to call upon an actual Pegasus winged mount. It will immediately appear and serve as your mount
+ &lt;InlineUIContainer&gt;&lt;Button Content='r188'  FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                   &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TalismanPegasus</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.gif' Name='</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>EncounterEnd</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>' Height='400' Width='400'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;Bold&gt;e026 Search for Treasure One More Time&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Clues suggest the treasure is in adjacent hext. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;Roll one die (1-N, 2-NE, 3-SE- 4-S, 5-SW, 6-NW):
+ &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dieRoll</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.gif' Name='</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DieRoll</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>' Height='21' Width='21'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+See &lt;InlineUIContainer&gt;&lt;Button Content='e026' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; when you arrive.</t>
     </r>
   </si>
 </sst>
@@ -35225,8 +35326,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B565"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A286" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B289" sqref="B289"/>
+    <sheetView tabSelected="1" topLeftCell="A94" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B96" sqref="B96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -35240,7 +35341,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1114</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -35248,7 +35349,7 @@
         <v>254</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1113</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -35256,7 +35357,7 @@
         <v>255</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>1112</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -35264,15 +35365,15 @@
         <v>256</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>1110</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>1109</v>
+        <v>1103</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>1111</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="390" x14ac:dyDescent="0.25">
@@ -35288,7 +35389,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>832</v>
+        <v>827</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35296,7 +35397,7 @@
         <v>22</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>1116</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35328,7 +35429,7 @@
         <v>3</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>1037</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -35336,7 +35437,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>855</v>
+        <v>850</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35344,7 +35445,7 @@
         <v>5</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>722</v>
+        <v>718</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35352,7 +35453,7 @@
         <v>6</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>723</v>
+        <v>719</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -35360,7 +35461,7 @@
         <v>7</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>856</v>
+        <v>851</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -35368,7 +35469,7 @@
         <v>8</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>857</v>
+        <v>852</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35376,7 +35477,7 @@
         <v>10</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>858</v>
+        <v>853</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35384,7 +35485,7 @@
         <v>9</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>859</v>
+        <v>854</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -35392,7 +35493,7 @@
         <v>11</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>752</v>
+        <v>748</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -35400,7 +35501,7 @@
         <v>12</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>762</v>
+        <v>758</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35408,7 +35509,7 @@
         <v>13</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>761</v>
+        <v>757</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35416,7 +35517,7 @@
         <v>14</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -35424,7 +35525,7 @@
         <v>15</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>901</v>
+        <v>896</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -35432,7 +35533,7 @@
         <v>16</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>900</v>
+        <v>895</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -35440,7 +35541,7 @@
         <v>17</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>896</v>
+        <v>891</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -35448,7 +35549,7 @@
         <v>18</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>895</v>
+        <v>890</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -35456,31 +35557,31 @@
         <v>261</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>892</v>
+        <v>887</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
+        <v>883</v>
+      </c>
+      <c r="B29" s="3" t="s">
         <v>888</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>893</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>890</v>
+        <v>885</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>903</v>
+        <v>898</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>894</v>
+        <v>889</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>904</v>
+        <v>899</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -35488,7 +35589,7 @@
         <v>19</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>918</v>
+        <v>913</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -35496,7 +35597,7 @@
         <v>20</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>919</v>
+        <v>914</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -35504,23 +35605,23 @@
         <v>21</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>921</v>
+        <v>916</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>910</v>
+        <v>905</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>916</v>
+        <v>911</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>911</v>
+        <v>906</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>917</v>
+        <v>912</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -35528,23 +35629,23 @@
         <v>25</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>1063</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>933</v>
+        <v>927</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>937</v>
+        <v>931</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>934</v>
+        <v>928</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>936</v>
+        <v>930</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -35552,7 +35653,7 @@
         <v>26</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>1053</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -35576,7 +35677,7 @@
         <v>27</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>957</v>
+        <v>951</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -35592,7 +35693,7 @@
         <v>29</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>1055</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -35600,7 +35701,7 @@
         <v>30</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>725</v>
+        <v>721</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -35613,10 +35714,10 @@
     </row>
     <row r="48" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>724</v>
+        <v>720</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>1033</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -35624,7 +35725,7 @@
         <v>31</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>1064</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -35632,7 +35733,7 @@
         <v>32</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>833</v>
+        <v>828</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -35640,7 +35741,7 @@
         <v>33</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>834</v>
+        <v>829</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -35696,7 +35797,7 @@
         <v>264</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>1066</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35704,7 +35805,7 @@
         <v>265</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>1065</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -35717,10 +35818,10 @@
     </row>
     <row r="61" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -35728,7 +35829,7 @@
         <v>35</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>852</v>
+        <v>847</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -35760,7 +35861,7 @@
         <v>37</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>775</v>
+        <v>771</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="285" x14ac:dyDescent="0.25">
@@ -35768,7 +35869,7 @@
         <v>38</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>835</v>
+        <v>830</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -35776,7 +35877,7 @@
         <v>43</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>727</v>
+        <v>723</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35784,23 +35885,23 @@
         <v>44</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>776</v>
+        <v>772</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>728</v>
+        <v>724</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>836</v>
+        <v>831</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>729</v>
+        <v>725</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>730</v>
+        <v>726</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35808,7 +35909,7 @@
         <v>39</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>726</v>
+        <v>722</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -35840,7 +35941,7 @@
         <v>42</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>1035</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35848,7 +35949,7 @@
         <v>46</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>1096</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -35872,7 +35973,7 @@
         <v>49</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>837</v>
+        <v>832</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35912,7 +36013,7 @@
         <v>54</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>843</v>
+        <v>838</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -35920,7 +36021,7 @@
         <v>55</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>799</v>
+        <v>795</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35928,7 +36029,7 @@
         <v>56</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>798</v>
+        <v>794</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35936,7 +36037,7 @@
         <v>57</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>818</v>
+        <v>813</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -35944,31 +36045,31 @@
         <v>58</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>819</v>
+        <v>814</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
-        <v>804</v>
+        <v>799</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>806</v>
+        <v>801</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
+        <v>800</v>
+      </c>
+      <c r="B91" s="3" t="s">
         <v>805</v>
-      </c>
-      <c r="B91" s="3" t="s">
-        <v>810</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
-        <v>811</v>
+        <v>806</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>812</v>
+        <v>807</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -35976,15 +36077,15 @@
         <v>59</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>889</v>
+        <v>884</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
-        <v>927</v>
+        <v>922</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>928</v>
+        <v>923</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -35992,15 +36093,15 @@
         <v>60</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>803</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+        <v>798</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
-        <v>800</v>
+        <v>796</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>801</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -36008,7 +36109,7 @@
         <v>61</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>802</v>
+        <v>797</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -36016,7 +36117,7 @@
         <v>62</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>820</v>
+        <v>815</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -36048,7 +36149,7 @@
         <v>65</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>838</v>
+        <v>833</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -36056,7 +36157,7 @@
         <v>66</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>1006</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -36136,7 +36237,7 @@
         <v>70</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>1042</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -36168,7 +36269,7 @@
         <v>72</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>716</v>
+        <v>712</v>
       </c>
     </row>
     <row r="118" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -36176,7 +36277,7 @@
         <v>73</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>717</v>
+        <v>713</v>
       </c>
     </row>
     <row r="119" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -36224,7 +36325,7 @@
         <v>77</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>982</v>
+        <v>976</v>
       </c>
     </row>
     <row r="125" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -36237,10 +36338,10 @@
     </row>
     <row r="126" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
-        <v>980</v>
+        <v>974</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>981</v>
+        <v>975</v>
       </c>
     </row>
     <row r="127" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -36248,7 +36349,7 @@
         <v>78</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>930</v>
+        <v>924</v>
       </c>
     </row>
     <row r="128" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -36256,7 +36357,7 @@
         <v>377</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>931</v>
+        <v>925</v>
       </c>
     </row>
     <row r="129" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -36296,7 +36397,7 @@
         <v>80</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>839</v>
+        <v>834</v>
       </c>
     </row>
     <row r="134" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -36304,87 +36405,87 @@
         <v>81</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>985</v>
+        <v>979</v>
       </c>
     </row>
     <row r="135" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
-        <v>983</v>
+        <v>977</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>995</v>
+        <v>989</v>
       </c>
     </row>
     <row r="136" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
-        <v>984</v>
+        <v>978</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>994</v>
+        <v>988</v>
       </c>
     </row>
     <row r="137" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
-        <v>986</v>
+        <v>980</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>1001</v>
+        <v>995</v>
       </c>
     </row>
     <row r="138" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
-        <v>987</v>
+        <v>981</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>1002</v>
+        <v>996</v>
       </c>
     </row>
     <row r="139" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
-        <v>988</v>
+        <v>982</v>
       </c>
       <c r="B139" s="3" t="s">
-        <v>1003</v>
+        <v>997</v>
       </c>
     </row>
     <row r="140" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
-        <v>989</v>
+        <v>983</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>993</v>
+        <v>987</v>
       </c>
     </row>
     <row r="141" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
-        <v>991</v>
+        <v>985</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>1005</v>
+        <v>999</v>
       </c>
     </row>
     <row r="142" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
-        <v>992</v>
+        <v>986</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>1004</v>
+        <v>998</v>
       </c>
     </row>
     <row r="143" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
-        <v>996</v>
+        <v>990</v>
       </c>
       <c r="B143" s="3" t="s">
-        <v>997</v>
+        <v>991</v>
       </c>
     </row>
     <row r="144" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
-        <v>998</v>
+        <v>992</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>1000</v>
+        <v>994</v>
       </c>
     </row>
     <row r="145" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -36392,7 +36493,7 @@
         <v>82</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>999</v>
+        <v>993</v>
       </c>
     </row>
     <row r="146" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -36400,15 +36501,15 @@
         <v>83</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>840</v>
+        <v>835</v>
       </c>
     </row>
     <row r="147" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
     </row>
     <row r="148" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -36416,7 +36517,7 @@
         <v>84</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
     </row>
     <row r="149" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -36424,23 +36525,23 @@
         <v>85</v>
       </c>
       <c r="B149" s="3" t="s">
-        <v>569</v>
+        <v>565</v>
       </c>
     </row>
     <row r="150" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
       <c r="B150" s="3" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
     </row>
     <row r="151" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>841</v>
+        <v>836</v>
       </c>
     </row>
     <row r="152" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -36448,7 +36549,7 @@
         <v>86</v>
       </c>
       <c r="B152" s="3" t="s">
-        <v>854</v>
+        <v>849</v>
       </c>
     </row>
     <row r="153" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -36504,7 +36605,7 @@
         <v>346</v>
       </c>
       <c r="B159" s="3" t="s">
-        <v>745</v>
+        <v>741</v>
       </c>
     </row>
     <row r="160" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -36512,7 +36613,7 @@
         <v>348</v>
       </c>
       <c r="B160" s="3" t="s">
-        <v>748</v>
+        <v>744</v>
       </c>
     </row>
     <row r="161" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -36541,10 +36642,10 @@
     </row>
     <row r="164" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
-        <v>738</v>
+        <v>734</v>
       </c>
       <c r="B164" s="3" t="s">
-        <v>739</v>
+        <v>735</v>
       </c>
     </row>
     <row r="165" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -36560,7 +36661,7 @@
         <v>445</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>940</v>
+        <v>934</v>
       </c>
     </row>
     <row r="167" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -36584,23 +36685,23 @@
         <v>90</v>
       </c>
       <c r="B169" s="3" t="s">
-        <v>846</v>
+        <v>841</v>
       </c>
     </row>
     <row r="170" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
-        <v>844</v>
+        <v>839</v>
       </c>
       <c r="B170" s="3" t="s">
-        <v>847</v>
+        <v>842</v>
       </c>
     </row>
     <row r="171" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
-        <v>845</v>
+        <v>840</v>
       </c>
       <c r="B171" s="3" t="s">
-        <v>848</v>
+        <v>843</v>
       </c>
     </row>
     <row r="172" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -36632,7 +36733,7 @@
         <v>93</v>
       </c>
       <c r="B175" s="3" t="s">
-        <v>878</v>
+        <v>873</v>
       </c>
     </row>
     <row r="176" spans="1:2" ht="270" x14ac:dyDescent="0.25">
@@ -36640,7 +36741,7 @@
         <v>94</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>879</v>
+        <v>874</v>
       </c>
     </row>
     <row r="177" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -36648,7 +36749,7 @@
         <v>95</v>
       </c>
       <c r="B177" s="3" t="s">
-        <v>886</v>
+        <v>881</v>
       </c>
     </row>
     <row r="178" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -36656,55 +36757,55 @@
         <v>96</v>
       </c>
       <c r="B178" s="3" t="s">
-        <v>874</v>
+        <v>869</v>
       </c>
     </row>
     <row r="179" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A179" s="2" t="s">
-        <v>871</v>
+        <v>866</v>
       </c>
       <c r="B179" s="3" t="s">
-        <v>875</v>
+        <v>870</v>
       </c>
     </row>
     <row r="180" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A180" s="2" t="s">
+        <v>867</v>
+      </c>
+      <c r="B180" s="3" t="s">
         <v>872</v>
-      </c>
-      <c r="B180" s="3" t="s">
-        <v>877</v>
       </c>
     </row>
     <row r="181" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
-        <v>873</v>
+        <v>868</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>881</v>
+        <v>876</v>
       </c>
     </row>
     <row r="182" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
-        <v>876</v>
+        <v>871</v>
       </c>
       <c r="B182" s="3" t="s">
-        <v>883</v>
+        <v>878</v>
       </c>
     </row>
     <row r="183" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
-        <v>891</v>
+        <v>886</v>
       </c>
       <c r="B183" s="3" t="s">
-        <v>897</v>
+        <v>892</v>
       </c>
     </row>
     <row r="184" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A184" s="2" t="s">
-        <v>898</v>
+        <v>893</v>
       </c>
       <c r="B184" s="3" t="s">
-        <v>899</v>
+        <v>894</v>
       </c>
     </row>
     <row r="185" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -36712,7 +36813,7 @@
         <v>97</v>
       </c>
       <c r="B185" s="3" t="s">
-        <v>882</v>
+        <v>877</v>
       </c>
     </row>
     <row r="186" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -36720,7 +36821,7 @@
         <v>98</v>
       </c>
       <c r="B186" s="3" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
     </row>
     <row r="187" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -36728,7 +36829,7 @@
         <v>99</v>
       </c>
       <c r="B187" s="3" t="s">
-        <v>602</v>
+        <v>598</v>
       </c>
     </row>
     <row r="188" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -36744,7 +36845,7 @@
         <v>100</v>
       </c>
       <c r="B189" s="3" t="s">
-        <v>823</v>
+        <v>818</v>
       </c>
     </row>
     <row r="190" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -36752,7 +36853,7 @@
         <v>102</v>
       </c>
       <c r="B190" s="3" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
     </row>
     <row r="191" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -36760,7 +36861,7 @@
         <v>103</v>
       </c>
       <c r="B191" s="3" t="s">
-        <v>1019</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="192" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -36768,7 +36869,7 @@
         <v>104</v>
       </c>
       <c r="B192" s="3" t="s">
-        <v>979</v>
+        <v>973</v>
       </c>
     </row>
     <row r="193" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -36776,23 +36877,23 @@
         <v>105</v>
       </c>
       <c r="B193" s="3" t="s">
-        <v>749</v>
+        <v>745</v>
       </c>
     </row>
     <row r="194" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A194" s="2" t="s">
-        <v>710</v>
+        <v>706</v>
       </c>
       <c r="B194" s="3" t="s">
-        <v>713</v>
+        <v>709</v>
       </c>
     </row>
     <row r="195" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A195" s="2" t="s">
-        <v>711</v>
+        <v>707</v>
       </c>
       <c r="B195" s="3" t="s">
-        <v>712</v>
+        <v>708</v>
       </c>
     </row>
     <row r="196" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -36800,7 +36901,7 @@
         <v>106</v>
       </c>
       <c r="B196" s="3" t="s">
-        <v>1007</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="197" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -36808,7 +36909,7 @@
         <v>107</v>
       </c>
       <c r="B197" s="3" t="s">
-        <v>850</v>
+        <v>845</v>
       </c>
     </row>
     <row r="198" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -36816,15 +36917,15 @@
         <v>165</v>
       </c>
       <c r="B198" s="3" t="s">
-        <v>851</v>
+        <v>846</v>
       </c>
     </row>
     <row r="199" spans="1:2" ht="225" x14ac:dyDescent="0.25">
       <c r="A199" s="2" t="s">
-        <v>849</v>
+        <v>844</v>
       </c>
       <c r="B199" s="3" t="s">
-        <v>853</v>
+        <v>848</v>
       </c>
     </row>
     <row r="200" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -36832,7 +36933,7 @@
         <v>108</v>
       </c>
       <c r="B200" s="3" t="s">
-        <v>1023</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="201" spans="1:2" ht="285" x14ac:dyDescent="0.25">
@@ -36840,7 +36941,7 @@
         <v>109</v>
       </c>
       <c r="B201" s="3" t="s">
-        <v>951</v>
+        <v>945</v>
       </c>
     </row>
     <row r="202" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -36848,7 +36949,7 @@
         <v>110</v>
       </c>
       <c r="B202" s="3" t="s">
-        <v>821</v>
+        <v>816</v>
       </c>
     </row>
     <row r="203" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -36856,7 +36957,7 @@
         <v>166</v>
       </c>
       <c r="B203" s="3" t="s">
-        <v>1097</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="204" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -36864,7 +36965,7 @@
         <v>167</v>
       </c>
       <c r="B204" s="3" t="s">
-        <v>1108</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="205" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -36872,23 +36973,23 @@
         <v>168</v>
       </c>
       <c r="B205" s="3" t="s">
-        <v>922</v>
+        <v>917</v>
       </c>
     </row>
     <row r="206" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A206" s="2" t="s">
-        <v>912</v>
+        <v>907</v>
       </c>
       <c r="B206" s="3" t="s">
-        <v>915</v>
+        <v>910</v>
       </c>
     </row>
     <row r="207" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A207" s="2" t="s">
-        <v>913</v>
+        <v>908</v>
       </c>
       <c r="B207" s="3" t="s">
-        <v>914</v>
+        <v>909</v>
       </c>
     </row>
     <row r="208" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -36896,39 +36997,39 @@
         <v>111</v>
       </c>
       <c r="B208" s="3" t="s">
-        <v>741</v>
+        <v>737</v>
       </c>
     </row>
     <row r="209" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A209" s="2" t="s">
-        <v>734</v>
+        <v>730</v>
       </c>
       <c r="B209" s="3" t="s">
-        <v>742</v>
+        <v>738</v>
       </c>
     </row>
     <row r="210" spans="1:2" ht="225" x14ac:dyDescent="0.25">
       <c r="A210" s="2" t="s">
-        <v>735</v>
+        <v>731</v>
       </c>
       <c r="B210" s="3" t="s">
-        <v>740</v>
+        <v>736</v>
       </c>
     </row>
     <row r="211" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A211" s="2" t="s">
-        <v>736</v>
+        <v>732</v>
       </c>
       <c r="B211" s="3" t="s">
-        <v>743</v>
+        <v>739</v>
       </c>
     </row>
     <row r="212" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A212" s="2" t="s">
-        <v>746</v>
+        <v>742</v>
       </c>
       <c r="B212" s="3" t="s">
-        <v>747</v>
+        <v>743</v>
       </c>
     </row>
     <row r="213" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -36936,7 +37037,7 @@
         <v>112</v>
       </c>
       <c r="B213" s="3" t="s">
-        <v>795</v>
+        <v>791</v>
       </c>
     </row>
     <row r="214" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -36944,7 +37045,7 @@
         <v>169</v>
       </c>
       <c r="B214" s="3" t="s">
-        <v>797</v>
+        <v>793</v>
       </c>
     </row>
     <row r="215" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -36952,7 +37053,7 @@
         <v>170</v>
       </c>
       <c r="B215" s="3" t="s">
-        <v>796</v>
+        <v>792</v>
       </c>
     </row>
     <row r="216" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -36960,7 +37061,7 @@
         <v>171</v>
       </c>
       <c r="B216" s="3" t="s">
-        <v>1128</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="217" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -36968,7 +37069,7 @@
         <v>113</v>
       </c>
       <c r="B217" s="3" t="s">
-        <v>1054</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="218" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -36976,7 +37077,7 @@
         <v>114</v>
       </c>
       <c r="B218" s="3" t="s">
-        <v>943</v>
+        <v>937</v>
       </c>
     </row>
     <row r="219" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -36984,15 +37085,15 @@
         <v>266</v>
       </c>
       <c r="B219" s="3" t="s">
-        <v>944</v>
+        <v>938</v>
       </c>
     </row>
     <row r="220" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A220" s="2" t="s">
-        <v>942</v>
+        <v>936</v>
       </c>
       <c r="B220" s="3" t="s">
-        <v>945</v>
+        <v>939</v>
       </c>
     </row>
     <row r="221" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37000,15 +37101,15 @@
         <v>115</v>
       </c>
       <c r="B221" s="3" t="s">
-        <v>968</v>
+        <v>962</v>
       </c>
     </row>
     <row r="222" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A222" s="2" t="s">
-        <v>767</v>
+        <v>763</v>
       </c>
       <c r="B222" s="3" t="s">
-        <v>774</v>
+        <v>770</v>
       </c>
     </row>
     <row r="223" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37016,15 +37117,15 @@
         <v>116</v>
       </c>
       <c r="B223" s="3" t="s">
-        <v>1089</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="224" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A224" s="2" t="s">
-        <v>763</v>
+        <v>759</v>
       </c>
       <c r="B224" s="3" t="s">
-        <v>768</v>
+        <v>764</v>
       </c>
     </row>
     <row r="225" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -37032,31 +37133,31 @@
         <v>117</v>
       </c>
       <c r="B225" s="4" t="s">
-        <v>842</v>
+        <v>837</v>
       </c>
     </row>
     <row r="226" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A226" s="2" t="s">
-        <v>769</v>
+        <v>765</v>
       </c>
       <c r="B226" s="4" t="s">
-        <v>772</v>
+        <v>768</v>
       </c>
     </row>
     <row r="227" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A227" s="2" t="s">
-        <v>770</v>
+        <v>766</v>
       </c>
       <c r="B227" s="4" t="s">
-        <v>771</v>
+        <v>767</v>
       </c>
     </row>
     <row r="228" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A228" s="2" t="s">
-        <v>773</v>
+        <v>769</v>
       </c>
       <c r="B228" s="4" t="s">
-        <v>955</v>
+        <v>949</v>
       </c>
     </row>
     <row r="229" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -37064,23 +37165,23 @@
         <v>118</v>
       </c>
       <c r="B229" s="3" t="s">
-        <v>956</v>
+        <v>950</v>
       </c>
     </row>
     <row r="230" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A230" s="2" t="s">
-        <v>952</v>
+        <v>946</v>
       </c>
       <c r="B230" s="3" t="s">
-        <v>954</v>
+        <v>948</v>
       </c>
     </row>
     <row r="231" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A231" s="2" t="s">
-        <v>953</v>
+        <v>947</v>
       </c>
       <c r="B231" s="3" t="s">
-        <v>1085</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="232" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -37088,23 +37189,23 @@
         <v>119</v>
       </c>
       <c r="B232" s="3" t="s">
-        <v>926</v>
+        <v>921</v>
       </c>
     </row>
     <row r="233" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A233" s="2" t="s">
-        <v>924</v>
+        <v>919</v>
       </c>
       <c r="B233" s="3" t="s">
-        <v>935</v>
+        <v>929</v>
       </c>
     </row>
     <row r="234" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A234" s="2" t="s">
-        <v>923</v>
+        <v>918</v>
       </c>
       <c r="B234" s="3" t="s">
-        <v>925</v>
+        <v>920</v>
       </c>
     </row>
     <row r="235" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -37112,7 +37213,7 @@
         <v>120</v>
       </c>
       <c r="B235" s="3" t="s">
-        <v>978</v>
+        <v>972</v>
       </c>
     </row>
     <row r="236" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -37120,7 +37221,7 @@
         <v>172</v>
       </c>
       <c r="B236" s="3" t="s">
-        <v>976</v>
+        <v>970</v>
       </c>
     </row>
     <row r="237" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37128,7 +37229,7 @@
         <v>173</v>
       </c>
       <c r="B237" s="3" t="s">
-        <v>975</v>
+        <v>969</v>
       </c>
     </row>
     <row r="238" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37136,7 +37237,7 @@
         <v>174</v>
       </c>
       <c r="B238" s="3" t="s">
-        <v>977</v>
+        <v>971</v>
       </c>
     </row>
     <row r="239" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37152,15 +37253,15 @@
         <v>122</v>
       </c>
       <c r="B240" s="3" t="s">
-        <v>765</v>
+        <v>761</v>
       </c>
     </row>
     <row r="241" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A241" s="2" t="s">
-        <v>764</v>
+        <v>760</v>
       </c>
       <c r="B241" s="3" t="s">
-        <v>766</v>
+        <v>762</v>
       </c>
     </row>
     <row r="242" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -37168,23 +37269,23 @@
         <v>123</v>
       </c>
       <c r="B242" s="3" t="s">
-        <v>949</v>
+        <v>943</v>
       </c>
     </row>
     <row r="243" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A243" s="2" t="s">
-        <v>946</v>
+        <v>940</v>
       </c>
       <c r="B243" s="3" t="s">
-        <v>948</v>
+        <v>942</v>
       </c>
     </row>
     <row r="244" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A244" s="2" t="s">
-        <v>947</v>
+        <v>941</v>
       </c>
       <c r="B244" s="3" t="s">
-        <v>950</v>
+        <v>944</v>
       </c>
     </row>
     <row r="245" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37192,7 +37293,7 @@
         <v>124</v>
       </c>
       <c r="B245" s="3" t="s">
-        <v>782</v>
+        <v>778</v>
       </c>
     </row>
     <row r="246" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37200,15 +37301,15 @@
         <v>125</v>
       </c>
       <c r="B246" s="3" t="s">
-        <v>1015</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="247" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A247" s="2" t="s">
-        <v>1014</v>
+        <v>1008</v>
       </c>
       <c r="B247" s="3" t="s">
-        <v>1016</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="248" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37216,7 +37317,7 @@
         <v>126</v>
       </c>
       <c r="B248" s="3" t="s">
-        <v>1022</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="249" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37224,7 +37325,7 @@
         <v>127</v>
       </c>
       <c r="B249" s="3" t="s">
-        <v>969</v>
+        <v>963</v>
       </c>
     </row>
     <row r="250" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37232,7 +37333,7 @@
         <v>128</v>
       </c>
       <c r="B250" s="3" t="s">
-        <v>781</v>
+        <v>777</v>
       </c>
     </row>
     <row r="251" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -37240,7 +37341,7 @@
         <v>129</v>
       </c>
       <c r="B251" s="3" t="s">
-        <v>1021</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="252" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37248,7 +37349,7 @@
         <v>130</v>
       </c>
       <c r="B252" s="3" t="s">
-        <v>967</v>
+        <v>961</v>
       </c>
     </row>
     <row r="253" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -37256,23 +37357,23 @@
         <v>131</v>
       </c>
       <c r="B253" s="3" t="s">
-        <v>973</v>
+        <v>967</v>
       </c>
     </row>
     <row r="254" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A254" s="2" t="s">
-        <v>970</v>
+        <v>964</v>
       </c>
       <c r="B254" s="3" t="s">
-        <v>971</v>
+        <v>965</v>
       </c>
     </row>
     <row r="255" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A255" s="2" t="s">
-        <v>972</v>
+        <v>966</v>
       </c>
       <c r="B255" s="3" t="s">
-        <v>974</v>
+        <v>968</v>
       </c>
     </row>
     <row r="256" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -37280,7 +37381,7 @@
         <v>132</v>
       </c>
       <c r="B256" s="3" t="s">
-        <v>1029</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="257" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -37288,15 +37389,15 @@
         <v>133</v>
       </c>
       <c r="B257" s="3" t="s">
-        <v>1058</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="258" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A258" s="2" t="s">
-        <v>966</v>
+        <v>960</v>
       </c>
       <c r="B258" s="3" t="s">
-        <v>1075</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="259" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37304,23 +37405,23 @@
         <v>134</v>
       </c>
       <c r="B259" s="3" t="s">
-        <v>1024</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="260" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A260" s="2" t="s">
-        <v>1025</v>
+        <v>1019</v>
       </c>
       <c r="B260" s="3" t="s">
-        <v>1026</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="261" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A261" s="2" t="s">
-        <v>1027</v>
+        <v>1021</v>
       </c>
       <c r="B261" s="3" t="s">
-        <v>1028</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="262" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -37328,15 +37429,15 @@
         <v>135</v>
       </c>
       <c r="B262" s="3" t="s">
-        <v>1032</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="263" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A263" s="2" t="s">
-        <v>1030</v>
+        <v>1024</v>
       </c>
       <c r="B263" s="3" t="s">
-        <v>1031</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="264" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -37344,7 +37445,7 @@
         <v>136</v>
       </c>
       <c r="B264" s="3" t="s">
-        <v>1034</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="265" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -37368,7 +37469,7 @@
         <v>233</v>
       </c>
       <c r="B267" s="3" t="s">
-        <v>941</v>
+        <v>935</v>
       </c>
     </row>
     <row r="268" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -37376,7 +37477,7 @@
         <v>138</v>
       </c>
       <c r="B268" s="3" t="s">
-        <v>731</v>
+        <v>727</v>
       </c>
     </row>
     <row r="269" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37384,7 +37485,7 @@
         <v>234</v>
       </c>
       <c r="B269" s="3" t="s">
-        <v>732</v>
+        <v>728</v>
       </c>
     </row>
     <row r="270" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37392,7 +37493,7 @@
         <v>235</v>
       </c>
       <c r="B270" s="3" t="s">
-        <v>733</v>
+        <v>729</v>
       </c>
     </row>
     <row r="271" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -37400,7 +37501,7 @@
         <v>139</v>
       </c>
       <c r="B271" s="3" t="s">
-        <v>791</v>
+        <v>787</v>
       </c>
     </row>
     <row r="272" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -37408,7 +37509,7 @@
         <v>239</v>
       </c>
       <c r="B272" s="3" t="s">
-        <v>794</v>
+        <v>790</v>
       </c>
     </row>
     <row r="273" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37416,7 +37517,7 @@
         <v>240</v>
       </c>
       <c r="B273" s="3" t="s">
-        <v>792</v>
+        <v>788</v>
       </c>
     </row>
     <row r="274" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37424,7 +37525,7 @@
         <v>241</v>
       </c>
       <c r="B274" s="3" t="s">
-        <v>793</v>
+        <v>789</v>
       </c>
     </row>
     <row r="275" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37432,7 +37533,7 @@
         <v>140</v>
       </c>
       <c r="B275" s="3" t="s">
-        <v>1092</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="276" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -37440,7 +37541,7 @@
         <v>236</v>
       </c>
       <c r="B276" s="3" t="s">
-        <v>1098</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="277" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37448,7 +37549,7 @@
         <v>237</v>
       </c>
       <c r="B277" s="3" t="s">
-        <v>1090</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="278" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37456,7 +37557,7 @@
         <v>238</v>
       </c>
       <c r="B278" s="3" t="s">
-        <v>1091</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="279" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -37464,7 +37565,7 @@
         <v>141</v>
       </c>
       <c r="B279" s="3" t="s">
-        <v>1078</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="280" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -37472,7 +37573,7 @@
         <v>142</v>
       </c>
       <c r="B280" s="3" t="s">
-        <v>1079</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="281" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -37480,7 +37581,7 @@
         <v>143</v>
       </c>
       <c r="B281" s="3" t="s">
-        <v>1080</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="282" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -37488,7 +37589,7 @@
         <v>144</v>
       </c>
       <c r="B282" s="3" t="s">
-        <v>1084</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="283" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -37496,7 +37597,7 @@
         <v>242</v>
       </c>
       <c r="B283" s="3" t="s">
-        <v>1086</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="284" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37504,7 +37605,7 @@
         <v>145</v>
       </c>
       <c r="B284" s="3" t="s">
-        <v>1083</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="285" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -37512,7 +37613,7 @@
         <v>146</v>
       </c>
       <c r="B285" s="3" t="s">
-        <v>1087</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="286" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37520,7 +37621,7 @@
         <v>147</v>
       </c>
       <c r="B286" s="3" t="s">
-        <v>1082</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="287" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -37528,7 +37629,7 @@
         <v>148</v>
       </c>
       <c r="B287" s="3" t="s">
-        <v>1088</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="288" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -37536,31 +37637,31 @@
         <v>149</v>
       </c>
       <c r="B288" s="3" t="s">
-        <v>1103</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="289" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A289" s="2" t="s">
-        <v>1100</v>
+        <v>1094</v>
       </c>
       <c r="B289" s="3" t="s">
-        <v>1129</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="290" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A290" s="2" t="s">
-        <v>1099</v>
+        <v>1093</v>
       </c>
       <c r="B290" s="3" t="s">
-        <v>1104</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="291" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A291" s="2" t="s">
-        <v>1101</v>
+        <v>1095</v>
       </c>
       <c r="B291" s="3" t="s">
-        <v>1102</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="292" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37568,15 +37669,15 @@
         <v>150</v>
       </c>
       <c r="B292" s="3" t="s">
-        <v>1106</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="293" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A293" s="2" t="s">
-        <v>1105</v>
+        <v>1099</v>
       </c>
       <c r="B293" s="3" t="s">
-        <v>1107</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="294" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -37584,7 +37685,7 @@
         <v>151</v>
       </c>
       <c r="B294" s="3" t="s">
-        <v>783</v>
+        <v>779</v>
       </c>
     </row>
     <row r="295" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37592,7 +37693,7 @@
         <v>243</v>
       </c>
       <c r="B295" s="3" t="s">
-        <v>786</v>
+        <v>782</v>
       </c>
     </row>
     <row r="296" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37600,7 +37701,7 @@
         <v>244</v>
       </c>
       <c r="B296" s="3" t="s">
-        <v>784</v>
+        <v>780</v>
       </c>
     </row>
     <row r="297" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37608,7 +37709,7 @@
         <v>245</v>
       </c>
       <c r="B297" s="3" t="s">
-        <v>785</v>
+        <v>781</v>
       </c>
     </row>
     <row r="298" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37616,7 +37717,7 @@
         <v>152</v>
       </c>
       <c r="B298" s="3" t="s">
-        <v>787</v>
+        <v>783</v>
       </c>
     </row>
     <row r="299" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -37624,7 +37725,7 @@
         <v>153</v>
       </c>
       <c r="B299" s="3" t="s">
-        <v>1081</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="300" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37632,7 +37733,7 @@
         <v>154</v>
       </c>
       <c r="B300" s="3" t="s">
-        <v>788</v>
+        <v>784</v>
       </c>
     </row>
     <row r="301" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -37640,7 +37741,7 @@
         <v>155</v>
       </c>
       <c r="B301" s="3" t="s">
-        <v>789</v>
+        <v>785</v>
       </c>
     </row>
     <row r="302" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37648,7 +37749,7 @@
         <v>156</v>
       </c>
       <c r="B302" s="3" t="s">
-        <v>790</v>
+        <v>786</v>
       </c>
     </row>
     <row r="303" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -37656,7 +37757,7 @@
         <v>157</v>
       </c>
       <c r="B303" s="3" t="s">
-        <v>780</v>
+        <v>776</v>
       </c>
     </row>
     <row r="304" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -37664,7 +37765,7 @@
         <v>246</v>
       </c>
       <c r="B304" s="3" t="s">
-        <v>777</v>
+        <v>773</v>
       </c>
     </row>
     <row r="305" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37672,7 +37773,7 @@
         <v>247</v>
       </c>
       <c r="B305" s="3" t="s">
-        <v>778</v>
+        <v>774</v>
       </c>
     </row>
     <row r="306" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37680,7 +37781,7 @@
         <v>248</v>
       </c>
       <c r="B306" s="3" t="s">
-        <v>779</v>
+        <v>775</v>
       </c>
     </row>
     <row r="307" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37688,7 +37789,7 @@
         <v>158</v>
       </c>
       <c r="B307" s="3" t="s">
-        <v>824</v>
+        <v>819</v>
       </c>
     </row>
     <row r="308" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -37696,7 +37797,7 @@
         <v>159</v>
       </c>
       <c r="B308" s="3" t="s">
-        <v>870</v>
+        <v>865</v>
       </c>
     </row>
     <row r="309" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37704,7 +37805,7 @@
         <v>160</v>
       </c>
       <c r="B309" s="3" t="s">
-        <v>1018</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="310" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -37712,7 +37813,7 @@
         <v>161</v>
       </c>
       <c r="B310" s="3" t="s">
-        <v>1051</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="311" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37720,31 +37821,31 @@
         <v>162</v>
       </c>
       <c r="B311" s="3" t="s">
-        <v>1069</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="312" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A312" s="2" t="s">
-        <v>1067</v>
+        <v>1061</v>
       </c>
       <c r="B312" s="3" t="s">
-        <v>1070</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="313" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A313" s="2" t="s">
-        <v>1068</v>
+        <v>1062</v>
       </c>
       <c r="B313" s="3" t="s">
-        <v>1072</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="314" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A314" s="2" t="s">
-        <v>1071</v>
+        <v>1065</v>
       </c>
       <c r="B314" s="3" t="s">
-        <v>1073</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="315" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37752,7 +37853,7 @@
         <v>163</v>
       </c>
       <c r="B315" s="3" t="s">
-        <v>1074</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="316" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -37760,7 +37861,7 @@
         <v>164</v>
       </c>
       <c r="B316" s="3" t="s">
-        <v>1061</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="317" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37768,7 +37869,7 @@
         <v>175</v>
       </c>
       <c r="B317" s="3" t="s">
-        <v>1060</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="318" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -37776,7 +37877,7 @@
         <v>176</v>
       </c>
       <c r="B318" s="3" t="s">
-        <v>1059</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="319" spans="1:2" ht="390" x14ac:dyDescent="0.25">
@@ -37784,7 +37885,7 @@
         <v>177</v>
       </c>
       <c r="B319" s="3" t="s">
-        <v>1039</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="320" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -37792,7 +37893,7 @@
         <v>527</v>
       </c>
       <c r="B320" s="3" t="s">
-        <v>1049</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="321" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37800,7 +37901,7 @@
         <v>528</v>
       </c>
       <c r="B321" s="3" t="s">
-        <v>1041</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="322" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37808,7 +37909,7 @@
         <v>529</v>
       </c>
       <c r="B322" s="3" t="s">
-        <v>1048</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="323" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -37816,7 +37917,7 @@
         <v>530</v>
       </c>
       <c r="B323" s="3" t="s">
-        <v>1125</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="324" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37824,7 +37925,7 @@
         <v>531</v>
       </c>
       <c r="B324" s="3" t="s">
-        <v>1047</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="325" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37832,15 +37933,15 @@
         <v>532</v>
       </c>
       <c r="B325" s="3" t="s">
-        <v>1040</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="326" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A326" s="2" t="s">
-        <v>1123</v>
+        <v>1117</v>
       </c>
       <c r="B326" s="3" t="s">
-        <v>1124</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="327" spans="1:2" ht="390" x14ac:dyDescent="0.25">
@@ -37848,7 +37949,7 @@
         <v>178</v>
       </c>
       <c r="B327" s="3" t="s">
-        <v>1044</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="328" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -37856,23 +37957,23 @@
         <v>500</v>
       </c>
       <c r="B328" s="3" t="s">
-        <v>1050</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="329" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A329" s="2" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
       <c r="B329" s="3" t="s">
-        <v>1045</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="330" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A330" s="2" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
       <c r="B330" s="3" t="s">
-        <v>1046</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="331" spans="1:2" ht="315" x14ac:dyDescent="0.25">
@@ -37880,7 +37981,7 @@
         <v>179</v>
       </c>
       <c r="B331" s="3" t="s">
-        <v>860</v>
+        <v>855</v>
       </c>
     </row>
     <row r="332" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -37888,7 +37989,7 @@
         <v>249</v>
       </c>
       <c r="B332" s="3" t="s">
-        <v>863</v>
+        <v>858</v>
       </c>
     </row>
     <row r="333" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -37896,7 +37997,7 @@
         <v>250</v>
       </c>
       <c r="B333" s="3" t="s">
-        <v>868</v>
+        <v>863</v>
       </c>
     </row>
     <row r="334" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -37904,7 +38005,7 @@
         <v>251</v>
       </c>
       <c r="B334" s="3" t="s">
-        <v>869</v>
+        <v>864</v>
       </c>
     </row>
     <row r="335" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -37912,7 +38013,7 @@
         <v>252</v>
       </c>
       <c r="B335" s="3" t="s">
-        <v>864</v>
+        <v>859</v>
       </c>
     </row>
     <row r="336" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -37920,23 +38021,23 @@
         <v>253</v>
       </c>
       <c r="B336" s="3" t="s">
-        <v>865</v>
+        <v>860</v>
       </c>
     </row>
     <row r="337" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A337" s="2" t="s">
+        <v>856</v>
+      </c>
+      <c r="B337" s="3" t="s">
         <v>861</v>
-      </c>
-      <c r="B337" s="3" t="s">
-        <v>866</v>
       </c>
     </row>
     <row r="338" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A338" s="2" t="s">
-        <v>862</v>
+        <v>857</v>
       </c>
       <c r="B338" s="3" t="s">
-        <v>1008</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="339" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -37944,7 +38045,7 @@
         <v>180</v>
       </c>
       <c r="B339" s="3" t="s">
-        <v>1020</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="340" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -37976,7 +38077,7 @@
         <v>183</v>
       </c>
       <c r="B343" s="3" t="s">
-        <v>1126</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="344" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -38048,7 +38149,7 @@
         <v>461</v>
       </c>
       <c r="B352" s="3" t="s">
-        <v>822</v>
+        <v>817</v>
       </c>
     </row>
     <row r="353" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -38080,15 +38181,15 @@
         <v>192</v>
       </c>
       <c r="B356" s="3" t="s">
-        <v>618</v>
+        <v>614</v>
       </c>
     </row>
     <row r="357" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A357" s="2" t="s">
-        <v>632</v>
+        <v>628</v>
       </c>
       <c r="B357" s="3" t="s">
-        <v>633</v>
+        <v>629</v>
       </c>
     </row>
     <row r="358" spans="1:2" ht="270" x14ac:dyDescent="0.25">
@@ -38096,7 +38197,7 @@
         <v>193</v>
       </c>
       <c r="B358" s="3" t="s">
-        <v>703</v>
+        <v>699</v>
       </c>
     </row>
     <row r="359" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -38112,7 +38213,7 @@
         <v>341</v>
       </c>
       <c r="B360" s="3" t="s">
-        <v>825</v>
+        <v>820</v>
       </c>
     </row>
     <row r="361" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -38120,7 +38221,7 @@
         <v>194</v>
       </c>
       <c r="B361" s="3" t="s">
-        <v>702</v>
+        <v>698</v>
       </c>
     </row>
     <row r="362" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -38128,7 +38229,7 @@
         <v>195</v>
       </c>
       <c r="B362" s="3" t="s">
-        <v>704</v>
+        <v>700</v>
       </c>
     </row>
     <row r="363" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -38136,7 +38237,7 @@
         <v>196</v>
       </c>
       <c r="B363" s="3" t="s">
-        <v>938</v>
+        <v>932</v>
       </c>
     </row>
     <row r="364" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -38144,7 +38245,7 @@
         <v>331</v>
       </c>
       <c r="B364" s="3" t="s">
-        <v>939</v>
+        <v>933</v>
       </c>
     </row>
     <row r="365" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -38152,15 +38253,15 @@
         <v>197</v>
       </c>
       <c r="B365" s="3" t="s">
-        <v>675</v>
+        <v>671</v>
       </c>
     </row>
     <row r="366" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A366" s="2" t="s">
-        <v>676</v>
+        <v>672</v>
       </c>
       <c r="B366" s="3" t="s">
-        <v>677</v>
+        <v>673</v>
       </c>
     </row>
     <row r="367" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38168,7 +38269,7 @@
         <v>198</v>
       </c>
       <c r="B367" s="3" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
     </row>
     <row r="368" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38176,7 +38277,7 @@
         <v>199</v>
       </c>
       <c r="B368" s="3" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
     </row>
     <row r="369" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -38184,7 +38285,7 @@
         <v>200</v>
       </c>
       <c r="B369" s="3" t="s">
-        <v>640</v>
+        <v>636</v>
       </c>
     </row>
     <row r="370" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -38192,7 +38293,7 @@
         <v>201</v>
       </c>
       <c r="B370" s="3" t="s">
-        <v>641</v>
+        <v>637</v>
       </c>
     </row>
     <row r="371" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38200,7 +38301,7 @@
         <v>202</v>
       </c>
       <c r="B371" s="3" t="s">
-        <v>1009</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="372" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -38208,47 +38309,47 @@
         <v>203</v>
       </c>
       <c r="B372" s="3" t="s">
-        <v>642</v>
+        <v>638</v>
       </c>
     </row>
     <row r="373" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A373" s="2" t="s">
-        <v>612</v>
+        <v>608</v>
       </c>
       <c r="B373" s="3" t="s">
-        <v>673</v>
+        <v>669</v>
       </c>
     </row>
     <row r="374" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A374" s="2" t="s">
-        <v>613</v>
+        <v>609</v>
       </c>
       <c r="B374" s="3" t="s">
-        <v>672</v>
+        <v>668</v>
       </c>
     </row>
     <row r="375" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A375" s="2" t="s">
-        <v>614</v>
+        <v>610</v>
       </c>
       <c r="B375" s="3" t="s">
-        <v>671</v>
+        <v>667</v>
       </c>
     </row>
     <row r="376" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A376" s="2" t="s">
-        <v>615</v>
+        <v>611</v>
       </c>
       <c r="B376" s="3" t="s">
-        <v>670</v>
+        <v>666</v>
       </c>
     </row>
     <row r="377" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A377" s="2" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
       <c r="B377" s="3" t="s">
-        <v>674</v>
+        <v>670</v>
       </c>
     </row>
     <row r="378" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -38256,55 +38357,55 @@
         <v>204</v>
       </c>
       <c r="B378" s="3" t="s">
-        <v>631</v>
+        <v>627</v>
       </c>
     </row>
     <row r="379" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A379" s="2" t="s">
-        <v>620</v>
+        <v>616</v>
       </c>
       <c r="B379" s="3" t="s">
-        <v>623</v>
+        <v>619</v>
       </c>
     </row>
     <row r="380" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A380" s="2" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
       <c r="B380" s="3" t="s">
-        <v>628</v>
+        <v>624</v>
       </c>
     </row>
     <row r="381" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A381" s="2" t="s">
-        <v>622</v>
+        <v>618</v>
       </c>
       <c r="B381" s="3" t="s">
-        <v>627</v>
+        <v>623</v>
       </c>
     </row>
     <row r="382" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A382" s="2" t="s">
-        <v>624</v>
+        <v>620</v>
       </c>
       <c r="B382" s="3" t="s">
-        <v>630</v>
+        <v>626</v>
       </c>
     </row>
     <row r="383" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A383" s="2" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
       <c r="B383" s="3" t="s">
-        <v>634</v>
+        <v>630</v>
       </c>
     </row>
     <row r="384" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A384" s="2" t="s">
-        <v>626</v>
+        <v>622</v>
       </c>
       <c r="B384" s="3" t="s">
-        <v>629</v>
+        <v>625</v>
       </c>
     </row>
     <row r="385" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -38312,55 +38413,55 @@
         <v>205</v>
       </c>
       <c r="B385" s="3" t="s">
-        <v>609</v>
+        <v>605</v>
       </c>
     </row>
     <row r="386" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A386" s="2" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="B386" s="3" t="s">
-        <v>907</v>
+        <v>902</v>
       </c>
     </row>
     <row r="387" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A387" s="2" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="B387" s="3" t="s">
-        <v>908</v>
+        <v>903</v>
       </c>
     </row>
     <row r="388" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A388" s="2" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="B388" s="3" t="s">
-        <v>905</v>
+        <v>900</v>
       </c>
     </row>
     <row r="389" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A389" s="2" t="s">
-        <v>606</v>
+        <v>602</v>
       </c>
       <c r="B389" s="3" t="s">
-        <v>906</v>
+        <v>901</v>
       </c>
     </row>
     <row r="390" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A390" s="2" t="s">
+        <v>603</v>
+      </c>
+      <c r="B390" s="3" t="s">
         <v>607</v>
-      </c>
-      <c r="B390" s="3" t="s">
-        <v>611</v>
       </c>
     </row>
     <row r="391" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A391" s="2" t="s">
-        <v>608</v>
+        <v>604</v>
       </c>
       <c r="B391" s="3" t="s">
-        <v>909</v>
+        <v>904</v>
       </c>
     </row>
     <row r="392" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38368,7 +38469,7 @@
         <v>206</v>
       </c>
       <c r="B392" s="3" t="s">
-        <v>610</v>
+        <v>606</v>
       </c>
     </row>
     <row r="393" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -38376,7 +38477,7 @@
         <v>207</v>
       </c>
       <c r="B393" s="3" t="s">
-        <v>1010</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="394" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -38384,7 +38485,7 @@
         <v>208</v>
       </c>
       <c r="B394" s="3" t="s">
-        <v>619</v>
+        <v>615</v>
       </c>
     </row>
     <row r="395" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -38392,55 +38493,55 @@
         <v>209</v>
       </c>
       <c r="B395" s="3" t="s">
-        <v>664</v>
+        <v>660</v>
       </c>
     </row>
     <row r="396" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A396" s="2" t="s">
-        <v>658</v>
+        <v>654</v>
       </c>
       <c r="B396" s="3" t="s">
-        <v>867</v>
+        <v>862</v>
       </c>
     </row>
     <row r="397" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A397" s="2" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="B397" s="3" t="s">
-        <v>666</v>
+        <v>662</v>
       </c>
     </row>
     <row r="398" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A398" s="2" t="s">
-        <v>660</v>
+        <v>656</v>
       </c>
       <c r="B398" s="3" t="s">
-        <v>665</v>
+        <v>661</v>
       </c>
     </row>
     <row r="399" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A399" s="2" t="s">
-        <v>661</v>
+        <v>657</v>
       </c>
       <c r="B399" s="3" t="s">
-        <v>667</v>
+        <v>663</v>
       </c>
     </row>
     <row r="400" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A400" s="2" t="s">
-        <v>662</v>
+        <v>658</v>
       </c>
       <c r="B400" s="4" t="s">
-        <v>668</v>
+        <v>664</v>
       </c>
     </row>
     <row r="401" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A401" s="2" t="s">
-        <v>663</v>
+        <v>659</v>
       </c>
       <c r="B401" s="3" t="s">
-        <v>669</v>
+        <v>665</v>
       </c>
     </row>
     <row r="402" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -38448,63 +38549,63 @@
         <v>210</v>
       </c>
       <c r="B402" s="3" t="s">
-        <v>649</v>
+        <v>645</v>
       </c>
     </row>
     <row r="403" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A403" s="2" t="s">
-        <v>643</v>
+        <v>639</v>
       </c>
       <c r="B403" s="3" t="s">
-        <v>650</v>
+        <v>646</v>
       </c>
     </row>
     <row r="404" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A404" s="2" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
       <c r="B404" s="3" t="s">
-        <v>651</v>
+        <v>647</v>
       </c>
     </row>
     <row r="405" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A405" s="2" t="s">
-        <v>645</v>
+        <v>641</v>
       </c>
       <c r="B405" s="3" t="s">
-        <v>652</v>
+        <v>648</v>
       </c>
     </row>
     <row r="406" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A406" s="2" t="s">
-        <v>646</v>
+        <v>642</v>
       </c>
       <c r="B406" s="3" t="s">
-        <v>653</v>
+        <v>649</v>
       </c>
     </row>
     <row r="407" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A407" s="2" t="s">
-        <v>647</v>
+        <v>643</v>
       </c>
       <c r="B407" s="3" t="s">
-        <v>656</v>
+        <v>652</v>
       </c>
     </row>
     <row r="408" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A408" s="2" t="s">
-        <v>648</v>
+        <v>644</v>
       </c>
       <c r="B408" s="3" t="s">
-        <v>657</v>
+        <v>653</v>
       </c>
     </row>
     <row r="409" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A409" s="2" t="s">
-        <v>654</v>
+        <v>650</v>
       </c>
       <c r="B409" s="3" t="s">
-        <v>655</v>
+        <v>651</v>
       </c>
     </row>
     <row r="410" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -38512,7 +38613,7 @@
         <v>211</v>
       </c>
       <c r="B410" s="3" t="s">
-        <v>714</v>
+        <v>710</v>
       </c>
     </row>
     <row r="411" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -38520,39 +38621,39 @@
         <v>212</v>
       </c>
       <c r="B411" s="3" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
     </row>
     <row r="412" spans="1:2" ht="300" x14ac:dyDescent="0.25">
       <c r="A412" s="2" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
       <c r="B412" s="3" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
     </row>
     <row r="413" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A413" s="2" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="B413" s="3" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
     </row>
     <row r="414" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A414" s="2" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B414" s="3" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
     </row>
     <row r="415" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A415" s="2" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
       <c r="B415" s="3" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
     </row>
     <row r="416" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -38560,7 +38661,7 @@
         <v>213</v>
       </c>
       <c r="B416" s="3" t="s">
-        <v>887</v>
+        <v>882</v>
       </c>
     </row>
     <row r="417" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -38568,7 +38669,7 @@
         <v>214</v>
       </c>
       <c r="B417" s="3" t="s">
-        <v>750</v>
+        <v>746</v>
       </c>
     </row>
     <row r="418" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -38576,7 +38677,7 @@
         <v>215</v>
       </c>
       <c r="B418" s="3" t="s">
-        <v>1121</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="419" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38608,7 +38709,7 @@
         <v>219</v>
       </c>
       <c r="B422" s="3" t="s">
-        <v>715</v>
+        <v>711</v>
       </c>
     </row>
     <row r="423" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38616,7 +38717,7 @@
         <v>220</v>
       </c>
       <c r="B423" s="3" t="s">
-        <v>813</v>
+        <v>808</v>
       </c>
     </row>
     <row r="424" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -38624,7 +38725,7 @@
         <v>221</v>
       </c>
       <c r="B424" s="3" t="s">
-        <v>540</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="425" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -38632,7 +38733,7 @@
         <v>222</v>
       </c>
       <c r="B425" s="3" t="s">
-        <v>541</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="426" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -38640,7 +38741,7 @@
         <v>223</v>
       </c>
       <c r="B426" s="3" t="s">
-        <v>542</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="427" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -38648,7 +38749,7 @@
         <v>224</v>
       </c>
       <c r="B427" s="3" t="s">
-        <v>929</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="428" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -38656,7 +38757,7 @@
         <v>332</v>
       </c>
       <c r="B428" s="3" t="s">
-        <v>543</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="429" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -38672,7 +38773,7 @@
         <v>225</v>
       </c>
       <c r="B430" s="3" t="s">
-        <v>932</v>
+        <v>926</v>
       </c>
     </row>
     <row r="431" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -38680,7 +38781,7 @@
         <v>226</v>
       </c>
       <c r="B431" s="3" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
     </row>
     <row r="432" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -38688,7 +38789,7 @@
         <v>227</v>
       </c>
       <c r="B432" s="3" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
     </row>
     <row r="433" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -38696,7 +38797,7 @@
         <v>228</v>
       </c>
       <c r="B433" s="3" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
     </row>
     <row r="434" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -38704,7 +38805,7 @@
         <v>229</v>
       </c>
       <c r="B434" s="3" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
     </row>
     <row r="435" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -38712,7 +38813,7 @@
         <v>230</v>
       </c>
       <c r="B435" s="3" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
     </row>
     <row r="436" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -38736,7 +38837,7 @@
         <v>449</v>
       </c>
       <c r="B438" s="3" t="s">
-        <v>1122</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="439" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -38744,31 +38845,31 @@
         <v>451</v>
       </c>
       <c r="B439" s="3" t="s">
-        <v>600</v>
+        <v>596</v>
       </c>
     </row>
     <row r="440" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A440" s="2" t="s">
-        <v>596</v>
+        <v>592</v>
       </c>
       <c r="B440" s="3" t="s">
-        <v>598</v>
+        <v>594</v>
       </c>
     </row>
     <row r="441" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A441" s="2" t="s">
-        <v>597</v>
+        <v>593</v>
       </c>
       <c r="B441" s="3" t="s">
-        <v>809</v>
+        <v>804</v>
       </c>
     </row>
     <row r="442" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A442" s="2" t="s">
-        <v>807</v>
+        <v>802</v>
       </c>
       <c r="B442" s="3" t="s">
-        <v>808</v>
+        <v>803</v>
       </c>
     </row>
     <row r="443" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -38776,7 +38877,7 @@
         <v>319</v>
       </c>
       <c r="B443" s="3" t="s">
-        <v>1117</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="444" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -38784,7 +38885,7 @@
         <v>320</v>
       </c>
       <c r="B444" s="3" t="s">
-        <v>1120</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="445" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -38792,7 +38893,7 @@
         <v>321</v>
       </c>
       <c r="B445" s="3" t="s">
-        <v>1118</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="446" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -38800,15 +38901,15 @@
         <v>318</v>
       </c>
       <c r="B446" s="3" t="s">
-        <v>1119</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="447" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A447" s="2" t="s">
-        <v>1076</v>
+        <v>1070</v>
       </c>
       <c r="B447" s="3" t="s">
-        <v>1077</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="448" spans="1:2" ht="255" x14ac:dyDescent="0.25">
@@ -38816,7 +38917,7 @@
         <v>322</v>
       </c>
       <c r="B448" s="3" t="s">
-        <v>1127</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="449" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38832,7 +38933,7 @@
         <v>491</v>
       </c>
       <c r="B450" s="3" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
     </row>
     <row r="451" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -38864,7 +38965,7 @@
         <v>497</v>
       </c>
       <c r="B454" s="3" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
     </row>
     <row r="455" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -38872,327 +38973,327 @@
         <v>498</v>
       </c>
       <c r="B455" s="3" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
     </row>
     <row r="456" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A456" s="2" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
       <c r="B456" s="3" t="s">
-        <v>1011</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="457" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A457" s="2" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
       <c r="B457" s="3" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
     </row>
     <row r="458" spans="1:2" ht="225" x14ac:dyDescent="0.25">
       <c r="A458" s="2" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="B458" s="3" t="s">
-        <v>751</v>
+        <v>747</v>
       </c>
     </row>
     <row r="459" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A459" s="2" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
       <c r="B459" s="3" t="s">
-        <v>1017</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="460" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A460" s="2" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
       <c r="B460" s="3" t="s">
-        <v>589</v>
+        <v>585</v>
       </c>
     </row>
     <row r="461" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A461" s="2" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
       <c r="B461" s="3" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
     </row>
     <row r="462" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A462" s="2" t="s">
-        <v>583</v>
+        <v>579</v>
       </c>
       <c r="B462" s="3" t="s">
-        <v>1012</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="463" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A463" s="2" t="s">
-        <v>584</v>
+        <v>580</v>
       </c>
       <c r="B463" s="3" t="s">
-        <v>590</v>
+        <v>586</v>
       </c>
     </row>
     <row r="464" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A464" s="2" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="B464" s="3" t="s">
-        <v>593</v>
+        <v>589</v>
       </c>
     </row>
     <row r="465" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A465" s="2" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
       <c r="B465" s="3" t="s">
-        <v>1013</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="466" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A466" s="2" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
       <c r="B466" s="3" t="s">
-        <v>592</v>
+        <v>588</v>
       </c>
     </row>
     <row r="467" spans="1:2" ht="225" x14ac:dyDescent="0.25">
       <c r="A467" s="2" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
       <c r="B467" s="3" t="s">
-        <v>594</v>
+        <v>590</v>
       </c>
     </row>
     <row r="468" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A468" s="2" t="s">
-        <v>595</v>
+        <v>591</v>
       </c>
       <c r="B468" s="3" t="s">
-        <v>826</v>
+        <v>821</v>
       </c>
     </row>
     <row r="469" spans="1:2" ht="225" x14ac:dyDescent="0.25">
       <c r="A469" s="2" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="B469" s="3" t="s">
-        <v>958</v>
+        <v>952</v>
       </c>
     </row>
     <row r="470" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A470" s="2" t="s">
-        <v>635</v>
+        <v>631</v>
       </c>
       <c r="B470" s="3" t="s">
-        <v>959</v>
+        <v>953</v>
       </c>
     </row>
     <row r="471" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A471" s="2" t="s">
-        <v>636</v>
+        <v>632</v>
       </c>
       <c r="B471" s="3" t="s">
-        <v>827</v>
+        <v>822</v>
       </c>
     </row>
     <row r="472" spans="1:2" ht="225" x14ac:dyDescent="0.25">
       <c r="A472" s="2" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="B472" s="3" t="s">
-        <v>960</v>
+        <v>954</v>
       </c>
     </row>
     <row r="473" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A473" s="2" t="s">
-        <v>880</v>
+        <v>875</v>
       </c>
       <c r="B473" s="3" t="s">
-        <v>961</v>
+        <v>955</v>
       </c>
     </row>
     <row r="474" spans="1:2" ht="255" x14ac:dyDescent="0.25">
       <c r="A474" s="2" t="s">
-        <v>678</v>
+        <v>674</v>
       </c>
       <c r="B474" s="1" t="s">
-        <v>828</v>
+        <v>823</v>
       </c>
     </row>
     <row r="475" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A475" s="2" t="s">
-        <v>679</v>
+        <v>675</v>
       </c>
       <c r="B475" s="1" t="s">
-        <v>696</v>
+        <v>692</v>
       </c>
     </row>
     <row r="476" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A476" s="2" t="s">
-        <v>680</v>
+        <v>676</v>
       </c>
       <c r="B476" s="1" t="s">
-        <v>695</v>
+        <v>691</v>
       </c>
     </row>
     <row r="477" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A477" s="2" t="s">
-        <v>681</v>
+        <v>677</v>
       </c>
       <c r="B477" s="1" t="s">
-        <v>694</v>
+        <v>690</v>
       </c>
     </row>
     <row r="478" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A478" s="2" t="s">
-        <v>682</v>
+        <v>678</v>
       </c>
       <c r="B478" s="1" t="s">
-        <v>693</v>
+        <v>689</v>
       </c>
     </row>
     <row r="479" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A479" s="2" t="s">
-        <v>683</v>
+        <v>679</v>
       </c>
       <c r="B479" s="1" t="s">
-        <v>692</v>
+        <v>688</v>
       </c>
     </row>
     <row r="480" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A480" s="2" t="s">
-        <v>684</v>
+        <v>680</v>
       </c>
       <c r="B480" s="1" t="s">
-        <v>962</v>
+        <v>956</v>
       </c>
     </row>
     <row r="481" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A481" s="2" t="s">
-        <v>685</v>
+        <v>681</v>
       </c>
       <c r="B481" s="1" t="s">
-        <v>691</v>
+        <v>687</v>
       </c>
     </row>
     <row r="482" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A482" s="2" t="s">
-        <v>686</v>
+        <v>682</v>
       </c>
       <c r="B482" s="1" t="s">
-        <v>697</v>
+        <v>693</v>
       </c>
     </row>
     <row r="483" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A483" s="2" t="s">
-        <v>687</v>
+        <v>683</v>
       </c>
       <c r="B483" s="1" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
     </row>
     <row r="484" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A484" s="2" t="s">
-        <v>688</v>
+        <v>684</v>
       </c>
       <c r="B484" s="1" t="s">
-        <v>698</v>
+        <v>694</v>
       </c>
     </row>
     <row r="485" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A485" s="2" t="s">
-        <v>689</v>
+        <v>685</v>
       </c>
       <c r="B485" s="1" t="s">
-        <v>963</v>
+        <v>957</v>
       </c>
     </row>
     <row r="486" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A486" s="2" t="s">
-        <v>690</v>
+        <v>686</v>
       </c>
       <c r="B486" s="1" t="s">
-        <v>701</v>
+        <v>697</v>
       </c>
     </row>
     <row r="487" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A487" s="2" t="s">
-        <v>700</v>
+        <v>696</v>
       </c>
       <c r="B487" s="1" t="s">
-        <v>707</v>
+        <v>703</v>
       </c>
     </row>
     <row r="488" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A488" s="2" t="s">
-        <v>705</v>
+        <v>701</v>
       </c>
       <c r="B488" s="1" t="s">
-        <v>706</v>
+        <v>702</v>
       </c>
     </row>
     <row r="489" spans="1:2" ht="255" x14ac:dyDescent="0.25">
       <c r="A489" s="2" t="s">
-        <v>1052</v>
+        <v>1046</v>
       </c>
       <c r="B489" s="1" t="s">
-        <v>1062</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="490" spans="1:2" ht="92.25" x14ac:dyDescent="0.25">
       <c r="A490" s="2" t="s">
-        <v>1056</v>
+        <v>1050</v>
       </c>
       <c r="B490" s="1" t="s">
-        <v>1057</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="491" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A491" s="2" t="s">
-        <v>708</v>
+        <v>704</v>
       </c>
       <c r="B491" s="1" t="s">
-        <v>964</v>
+        <v>958</v>
       </c>
     </row>
     <row r="492" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A492" s="2" t="s">
-        <v>744</v>
+        <v>740</v>
       </c>
       <c r="B492" s="3" t="s">
-        <v>1115</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="493" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A493" s="2" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="B493" s="3" t="s">
-        <v>709</v>
+        <v>705</v>
       </c>
     </row>
     <row r="494" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A494" s="2" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
       <c r="B494" s="3" t="s">
-        <v>829</v>
+        <v>824</v>
       </c>
     </row>
     <row r="495" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A495" s="2" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
       <c r="B495" s="3" t="s">
-        <v>830</v>
+        <v>825</v>
       </c>
     </row>
     <row r="496" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39264,7 +39365,7 @@
         <v>275</v>
       </c>
       <c r="B504" s="1" t="s">
-        <v>1093</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="505" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39272,7 +39373,7 @@
         <v>276</v>
       </c>
       <c r="B505" s="1" t="s">
-        <v>1094</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="506" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39280,7 +39381,7 @@
         <v>277</v>
       </c>
       <c r="B506" s="1" t="s">
-        <v>1095</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="507" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -39328,7 +39429,7 @@
         <v>260</v>
       </c>
       <c r="B512" s="3" t="s">
-        <v>1038</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="513" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39336,7 +39437,7 @@
         <v>480</v>
       </c>
       <c r="B513" s="3" t="s">
-        <v>814</v>
+        <v>809</v>
       </c>
     </row>
     <row r="514" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -39344,15 +39445,15 @@
         <v>481</v>
       </c>
       <c r="B514" s="1" t="s">
-        <v>817</v>
+        <v>812</v>
       </c>
     </row>
     <row r="515" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A515" s="2" t="s">
-        <v>815</v>
+        <v>810</v>
       </c>
       <c r="B515" s="3" t="s">
-        <v>816</v>
+        <v>811</v>
       </c>
     </row>
     <row r="516" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39400,7 +39501,7 @@
         <v>285</v>
       </c>
       <c r="B521" s="1" t="s">
-        <v>884</v>
+        <v>879</v>
       </c>
     </row>
     <row r="522" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -39408,7 +39509,7 @@
         <v>286</v>
       </c>
       <c r="B522" s="1" t="s">
-        <v>885</v>
+        <v>880</v>
       </c>
     </row>
     <row r="523" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -39488,7 +39589,7 @@
         <v>296</v>
       </c>
       <c r="B532" s="1" t="s">
-        <v>831</v>
+        <v>826</v>
       </c>
     </row>
     <row r="533" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -39496,7 +39597,7 @@
         <v>297</v>
       </c>
       <c r="B533" s="1" t="s">
-        <v>718</v>
+        <v>714</v>
       </c>
     </row>
     <row r="534" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -39520,7 +39621,7 @@
         <v>406</v>
       </c>
       <c r="B536" s="1" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
     </row>
     <row r="537" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -39528,7 +39629,7 @@
         <v>298</v>
       </c>
       <c r="B537" s="1" t="s">
-        <v>965</v>
+        <v>959</v>
       </c>
     </row>
     <row r="538" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -39544,7 +39645,7 @@
         <v>299</v>
       </c>
       <c r="B539" s="1" t="s">
-        <v>720</v>
+        <v>716</v>
       </c>
     </row>
     <row r="540" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -39568,7 +39669,7 @@
         <v>300</v>
       </c>
       <c r="B542" s="1" t="s">
-        <v>902</v>
+        <v>897</v>
       </c>
     </row>
     <row r="543" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -39576,7 +39677,7 @@
         <v>301</v>
       </c>
       <c r="B543" s="1" t="s">
-        <v>920</v>
+        <v>915</v>
       </c>
     </row>
     <row r="544" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -39616,7 +39717,7 @@
         <v>396</v>
       </c>
       <c r="B548" s="1" t="s">
-        <v>756</v>
+        <v>752</v>
       </c>
     </row>
     <row r="549" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -39629,10 +39730,10 @@
     </row>
     <row r="550" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A550" s="2" t="s">
+        <v>749</v>
+      </c>
+      <c r="B550" s="1" t="s">
         <v>753</v>
-      </c>
-      <c r="B550" s="1" t="s">
-        <v>757</v>
       </c>
     </row>
     <row r="551" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -39640,7 +39741,7 @@
         <v>305</v>
       </c>
       <c r="B551" s="1" t="s">
-        <v>719</v>
+        <v>715</v>
       </c>
     </row>
     <row r="552" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -39669,10 +39770,10 @@
     </row>
     <row r="555" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A555" s="2" t="s">
-        <v>754</v>
+        <v>750</v>
       </c>
       <c r="B555" s="1" t="s">
-        <v>755</v>
+        <v>751</v>
       </c>
     </row>
     <row r="556" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -39680,7 +39781,7 @@
         <v>306</v>
       </c>
       <c r="B556" s="1" t="s">
-        <v>721</v>
+        <v>717</v>
       </c>
     </row>
     <row r="557" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -39704,7 +39805,7 @@
         <v>307</v>
       </c>
       <c r="B559" s="1" t="s">
-        <v>1043</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="560" spans="1:2" ht="375" x14ac:dyDescent="0.25">
@@ -39712,7 +39813,7 @@
         <v>311</v>
       </c>
       <c r="B560" s="1" t="s">
-        <v>737</v>
+        <v>733</v>
       </c>
     </row>
     <row r="561" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39736,15 +39837,15 @@
         <v>376</v>
       </c>
       <c r="B563" s="3" t="s">
-        <v>1036</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="564" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A564" s="2" t="s">
-        <v>758</v>
+        <v>754</v>
       </c>
       <c r="B564" s="3" t="s">
-        <v>759</v>
+        <v>755</v>
       </c>
     </row>
     <row r="565" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -39752,7 +39853,7 @@
         <v>329</v>
       </c>
       <c r="B565" s="3" t="s">
-        <v>990</v>
+        <v>984</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added TreasureRoomDoor gif. Fix issue with Cavalry. Updated About Dialog. Fix issue with e050a in Events.xlsx file.
</commit_message>
<xml_diff>
--- a/Documentation/Events.xlsx
+++ b/Documentation/Events.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\happysulla\BarbarianPrince\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9D3BC1FB-D863-48F9-809C-2A87CA8EB0A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A1C9DFEB-C5AC-42B2-BA6C-68972E7831A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -9370,9 +9371,6 @@
   </si>
   <si>
     <t>e050d</t>
-  </si>
-  <si>
-    <t>050a</t>
   </si>
   <si>
     <t>e050f</t>
@@ -34861,6 +34859,9 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 See &lt;InlineUIContainer&gt;&lt;Button Content='e026' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; when you arrive.</t>
     </r>
+  </si>
+  <si>
+    <t>e050a</t>
   </si>
 </sst>
 </file>
@@ -35326,8 +35327,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B565"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B96" sqref="B96"/>
+    <sheetView tabSelected="1" topLeftCell="A146" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A147" sqref="A147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -35341,7 +35342,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -35349,7 +35350,7 @@
         <v>254</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -35357,7 +35358,7 @@
         <v>255</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -35365,15 +35366,15 @@
         <v>256</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="390" x14ac:dyDescent="0.25">
@@ -35389,7 +35390,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35397,7 +35398,7 @@
         <v>22</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35429,7 +35430,7 @@
         <v>3</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -35437,7 +35438,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35445,7 +35446,7 @@
         <v>5</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35453,7 +35454,7 @@
         <v>6</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -35461,7 +35462,7 @@
         <v>7</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -35469,7 +35470,7 @@
         <v>8</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35477,7 +35478,7 @@
         <v>10</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35485,7 +35486,7 @@
         <v>9</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -35493,7 +35494,7 @@
         <v>11</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -35501,7 +35502,7 @@
         <v>12</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35509,7 +35510,7 @@
         <v>13</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35517,7 +35518,7 @@
         <v>14</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -35525,7 +35526,7 @@
         <v>15</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -35533,7 +35534,7 @@
         <v>16</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -35541,7 +35542,7 @@
         <v>17</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -35549,7 +35550,7 @@
         <v>18</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -35557,31 +35558,31 @@
         <v>261</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -35589,7 +35590,7 @@
         <v>19</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -35597,7 +35598,7 @@
         <v>20</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -35605,23 +35606,23 @@
         <v>21</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -35629,23 +35630,23 @@
         <v>25</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -35653,7 +35654,7 @@
         <v>26</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -35677,7 +35678,7 @@
         <v>27</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -35693,7 +35694,7 @@
         <v>29</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -35701,7 +35702,7 @@
         <v>30</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -35714,10 +35715,10 @@
     </row>
     <row r="48" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -35725,7 +35726,7 @@
         <v>31</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -35733,7 +35734,7 @@
         <v>32</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -35741,7 +35742,7 @@
         <v>33</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -35797,7 +35798,7 @@
         <v>264</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35805,7 +35806,7 @@
         <v>265</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -35818,10 +35819,10 @@
     </row>
     <row r="61" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -35829,7 +35830,7 @@
         <v>35</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -35861,7 +35862,7 @@
         <v>37</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="285" x14ac:dyDescent="0.25">
@@ -35869,7 +35870,7 @@
         <v>38</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -35877,7 +35878,7 @@
         <v>43</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35885,23 +35886,23 @@
         <v>44</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
+        <v>724</v>
+      </c>
+      <c r="B71" s="3" t="s">
         <v>725</v>
-      </c>
-      <c r="B71" s="3" t="s">
-        <v>726</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35909,7 +35910,7 @@
         <v>39</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -35941,7 +35942,7 @@
         <v>42</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35949,7 +35950,7 @@
         <v>46</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -35973,7 +35974,7 @@
         <v>49</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -36013,7 +36014,7 @@
         <v>54</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -36021,7 +36022,7 @@
         <v>55</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -36029,7 +36030,7 @@
         <v>56</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -36037,7 +36038,7 @@
         <v>57</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -36045,31 +36046,31 @@
         <v>58</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
+        <v>805</v>
+      </c>
+      <c r="B92" s="3" t="s">
         <v>806</v>
-      </c>
-      <c r="B92" s="3" t="s">
-        <v>807</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -36077,15 +36078,15 @@
         <v>59</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
+        <v>921</v>
+      </c>
+      <c r="B94" s="3" t="s">
         <v>922</v>
-      </c>
-      <c r="B94" s="3" t="s">
-        <v>923</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -36093,15 +36094,15 @@
         <v>60</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -36109,7 +36110,7 @@
         <v>61</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -36117,7 +36118,7 @@
         <v>62</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -36149,7 +36150,7 @@
         <v>65</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -36157,7 +36158,7 @@
         <v>66</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -36237,7 +36238,7 @@
         <v>70</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -36269,7 +36270,7 @@
         <v>72</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
     </row>
     <row r="118" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -36277,7 +36278,7 @@
         <v>73</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
     </row>
     <row r="119" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -36325,7 +36326,7 @@
         <v>77</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
     </row>
     <row r="125" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -36338,10 +36339,10 @@
     </row>
     <row r="126" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
+        <v>973</v>
+      </c>
+      <c r="B126" s="3" t="s">
         <v>974</v>
-      </c>
-      <c r="B126" s="3" t="s">
-        <v>975</v>
       </c>
     </row>
     <row r="127" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -36349,7 +36350,7 @@
         <v>78</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
     </row>
     <row r="128" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -36357,7 +36358,7 @@
         <v>377</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
     </row>
     <row r="129" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -36397,7 +36398,7 @@
         <v>80</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
     </row>
     <row r="134" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -36405,87 +36406,87 @@
         <v>81</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
     </row>
     <row r="135" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
     </row>
     <row r="136" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
     </row>
     <row r="137" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
     </row>
     <row r="138" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
     </row>
     <row r="139" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="B139" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="140" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
     </row>
     <row r="141" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
     </row>
     <row r="142" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
     </row>
     <row r="143" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
+        <v>989</v>
+      </c>
+      <c r="B143" s="3" t="s">
         <v>990</v>
-      </c>
-      <c r="B143" s="3" t="s">
-        <v>991</v>
       </c>
     </row>
     <row r="144" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
     </row>
     <row r="145" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -36493,7 +36494,7 @@
         <v>82</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
     </row>
     <row r="146" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -36501,15 +36502,15 @@
         <v>83</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
     <row r="147" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
-        <v>560</v>
+        <v>1129</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="148" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -36517,7 +36518,7 @@
         <v>84</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="149" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -36525,7 +36526,7 @@
         <v>85</v>
       </c>
       <c r="B149" s="3" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="150" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -36533,15 +36534,15 @@
         <v>559</v>
       </c>
       <c r="B150" s="3" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="151" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="152" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -36549,7 +36550,7 @@
         <v>86</v>
       </c>
       <c r="B152" s="3" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="153" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -36605,7 +36606,7 @@
         <v>346</v>
       </c>
       <c r="B159" s="3" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="160" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -36613,7 +36614,7 @@
         <v>348</v>
       </c>
       <c r="B160" s="3" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
     </row>
     <row r="161" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -36642,10 +36643,10 @@
     </row>
     <row r="164" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
+        <v>733</v>
+      </c>
+      <c r="B164" s="3" t="s">
         <v>734</v>
-      </c>
-      <c r="B164" s="3" t="s">
-        <v>735</v>
       </c>
     </row>
     <row r="165" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -36661,7 +36662,7 @@
         <v>445</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
     </row>
     <row r="167" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -36685,23 +36686,23 @@
         <v>90</v>
       </c>
       <c r="B169" s="3" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
     </row>
     <row r="170" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="B170" s="3" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
     </row>
     <row r="171" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="B171" s="3" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
     </row>
     <row r="172" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -36733,7 +36734,7 @@
         <v>93</v>
       </c>
       <c r="B175" s="3" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
     </row>
     <row r="176" spans="1:2" ht="270" x14ac:dyDescent="0.25">
@@ -36741,7 +36742,7 @@
         <v>94</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
     </row>
     <row r="177" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -36749,7 +36750,7 @@
         <v>95</v>
       </c>
       <c r="B177" s="3" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
     </row>
     <row r="178" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -36757,55 +36758,55 @@
         <v>96</v>
       </c>
       <c r="B178" s="3" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
     </row>
     <row r="179" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A179" s="2" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="B179" s="3" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
     </row>
     <row r="180" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A180" s="2" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="B180" s="3" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
     </row>
     <row r="181" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
     </row>
     <row r="182" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="B182" s="3" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
     </row>
     <row r="183" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="B183" s="3" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
     </row>
     <row r="184" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A184" s="2" t="s">
+        <v>892</v>
+      </c>
+      <c r="B184" s="3" t="s">
         <v>893</v>
-      </c>
-      <c r="B184" s="3" t="s">
-        <v>894</v>
       </c>
     </row>
     <row r="185" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -36813,7 +36814,7 @@
         <v>97</v>
       </c>
       <c r="B185" s="3" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
     </row>
     <row r="186" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -36821,7 +36822,7 @@
         <v>98</v>
       </c>
       <c r="B186" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="187" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -36829,7 +36830,7 @@
         <v>99</v>
       </c>
       <c r="B187" s="3" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="188" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -36845,7 +36846,7 @@
         <v>100</v>
       </c>
       <c r="B189" s="3" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
     </row>
     <row r="190" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -36853,7 +36854,7 @@
         <v>102</v>
       </c>
       <c r="B190" s="3" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="191" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -36861,7 +36862,7 @@
         <v>103</v>
       </c>
       <c r="B191" s="3" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="192" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -36869,7 +36870,7 @@
         <v>104</v>
       </c>
       <c r="B192" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="193" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -36877,23 +36878,23 @@
         <v>105</v>
       </c>
       <c r="B193" s="3" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
     </row>
     <row r="194" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A194" s="2" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="B194" s="3" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="195" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A195" s="2" t="s">
+        <v>706</v>
+      </c>
+      <c r="B195" s="3" t="s">
         <v>707</v>
-      </c>
-      <c r="B195" s="3" t="s">
-        <v>708</v>
       </c>
     </row>
     <row r="196" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -36901,7 +36902,7 @@
         <v>106</v>
       </c>
       <c r="B196" s="3" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="197" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -36909,7 +36910,7 @@
         <v>107</v>
       </c>
       <c r="B197" s="3" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="198" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -36917,15 +36918,15 @@
         <v>165</v>
       </c>
       <c r="B198" s="3" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
     </row>
     <row r="199" spans="1:2" ht="225" x14ac:dyDescent="0.25">
       <c r="A199" s="2" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="B199" s="3" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
     </row>
     <row r="200" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -36933,7 +36934,7 @@
         <v>108</v>
       </c>
       <c r="B200" s="3" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="201" spans="1:2" ht="285" x14ac:dyDescent="0.25">
@@ -36941,7 +36942,7 @@
         <v>109</v>
       </c>
       <c r="B201" s="3" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
     </row>
     <row r="202" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -36949,7 +36950,7 @@
         <v>110</v>
       </c>
       <c r="B202" s="3" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
     </row>
     <row r="203" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -36957,7 +36958,7 @@
         <v>166</v>
       </c>
       <c r="B203" s="3" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="204" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -36965,7 +36966,7 @@
         <v>167</v>
       </c>
       <c r="B204" s="3" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="205" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -36973,23 +36974,23 @@
         <v>168</v>
       </c>
       <c r="B205" s="3" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
     </row>
     <row r="206" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A206" s="2" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="B206" s="3" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
     </row>
     <row r="207" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A207" s="2" t="s">
+        <v>907</v>
+      </c>
+      <c r="B207" s="3" t="s">
         <v>908</v>
-      </c>
-      <c r="B207" s="3" t="s">
-        <v>909</v>
       </c>
     </row>
     <row r="208" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -36997,39 +36998,39 @@
         <v>111</v>
       </c>
       <c r="B208" s="3" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="209" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A209" s="2" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="B209" s="3" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="210" spans="1:2" ht="225" x14ac:dyDescent="0.25">
       <c r="A210" s="2" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="B210" s="3" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="211" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A211" s="2" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B211" s="3" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="212" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A212" s="2" t="s">
+        <v>741</v>
+      </c>
+      <c r="B212" s="3" t="s">
         <v>742</v>
-      </c>
-      <c r="B212" s="3" t="s">
-        <v>743</v>
       </c>
     </row>
     <row r="213" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37037,7 +37038,7 @@
         <v>112</v>
       </c>
       <c r="B213" s="3" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="214" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37045,7 +37046,7 @@
         <v>169</v>
       </c>
       <c r="B214" s="3" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
     </row>
     <row r="215" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -37053,7 +37054,7 @@
         <v>170</v>
       </c>
       <c r="B215" s="3" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
     </row>
     <row r="216" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -37061,7 +37062,7 @@
         <v>171</v>
       </c>
       <c r="B216" s="3" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="217" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37069,7 +37070,7 @@
         <v>113</v>
       </c>
       <c r="B217" s="3" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="218" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -37077,7 +37078,7 @@
         <v>114</v>
       </c>
       <c r="B218" s="3" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
     </row>
     <row r="219" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -37085,15 +37086,15 @@
         <v>266</v>
       </c>
       <c r="B219" s="3" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
     </row>
     <row r="220" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A220" s="2" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="B220" s="3" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
     </row>
     <row r="221" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37101,15 +37102,15 @@
         <v>115</v>
       </c>
       <c r="B221" s="3" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
     </row>
     <row r="222" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A222" s="2" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="B222" s="3" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
     </row>
     <row r="223" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37117,15 +37118,15 @@
         <v>116</v>
       </c>
       <c r="B223" s="3" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="224" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A224" s="2" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="B224" s="3" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
     </row>
     <row r="225" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -37133,31 +37134,31 @@
         <v>117</v>
       </c>
       <c r="B225" s="4" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
     <row r="226" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A226" s="2" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="B226" s="4" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
     </row>
     <row r="227" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A227" s="2" t="s">
+        <v>765</v>
+      </c>
+      <c r="B227" s="4" t="s">
         <v>766</v>
-      </c>
-      <c r="B227" s="4" t="s">
-        <v>767</v>
       </c>
     </row>
     <row r="228" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A228" s="2" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="B228" s="4" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
     </row>
     <row r="229" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -37165,23 +37166,23 @@
         <v>118</v>
       </c>
       <c r="B229" s="3" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
     </row>
     <row r="230" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A230" s="2" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="B230" s="3" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
     </row>
     <row r="231" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A231" s="2" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="B231" s="3" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="232" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -37189,23 +37190,23 @@
         <v>119</v>
       </c>
       <c r="B232" s="3" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
     </row>
     <row r="233" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A233" s="2" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="B233" s="3" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
     </row>
     <row r="234" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A234" s="2" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="B234" s="3" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
     </row>
     <row r="235" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -37213,7 +37214,7 @@
         <v>120</v>
       </c>
       <c r="B235" s="3" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
     </row>
     <row r="236" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -37221,7 +37222,7 @@
         <v>172</v>
       </c>
       <c r="B236" s="3" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
     </row>
     <row r="237" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37229,7 +37230,7 @@
         <v>173</v>
       </c>
       <c r="B237" s="3" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
     </row>
     <row r="238" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37237,7 +37238,7 @@
         <v>174</v>
       </c>
       <c r="B238" s="3" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
     </row>
     <row r="239" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37253,15 +37254,15 @@
         <v>122</v>
       </c>
       <c r="B240" s="3" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
     </row>
     <row r="241" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A241" s="2" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="B241" s="3" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
     </row>
     <row r="242" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -37269,23 +37270,23 @@
         <v>123</v>
       </c>
       <c r="B242" s="3" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
     </row>
     <row r="243" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A243" s="2" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="B243" s="3" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
     </row>
     <row r="244" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A244" s="2" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="B244" s="3" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
     </row>
     <row r="245" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37293,7 +37294,7 @@
         <v>124</v>
       </c>
       <c r="B245" s="3" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
     </row>
     <row r="246" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37301,15 +37302,15 @@
         <v>125</v>
       </c>
       <c r="B246" s="3" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="247" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A247" s="2" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="B247" s="3" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="248" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37317,7 +37318,7 @@
         <v>126</v>
       </c>
       <c r="B248" s="3" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="249" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37325,7 +37326,7 @@
         <v>127</v>
       </c>
       <c r="B249" s="3" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
     </row>
     <row r="250" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37333,7 +37334,7 @@
         <v>128</v>
       </c>
       <c r="B250" s="3" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
     </row>
     <row r="251" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -37341,7 +37342,7 @@
         <v>129</v>
       </c>
       <c r="B251" s="3" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="252" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37349,7 +37350,7 @@
         <v>130</v>
       </c>
       <c r="B252" s="3" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
     </row>
     <row r="253" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -37357,23 +37358,23 @@
         <v>131</v>
       </c>
       <c r="B253" s="3" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
     </row>
     <row r="254" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A254" s="2" t="s">
+        <v>963</v>
+      </c>
+      <c r="B254" s="3" t="s">
         <v>964</v>
-      </c>
-      <c r="B254" s="3" t="s">
-        <v>965</v>
       </c>
     </row>
     <row r="255" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A255" s="2" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="B255" s="3" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
     </row>
     <row r="256" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -37381,7 +37382,7 @@
         <v>132</v>
       </c>
       <c r="B256" s="3" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="257" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -37389,15 +37390,15 @@
         <v>133</v>
       </c>
       <c r="B257" s="3" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="258" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A258" s="2" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="B258" s="3" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="259" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37405,23 +37406,23 @@
         <v>134</v>
       </c>
       <c r="B259" s="3" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="260" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A260" s="2" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B260" s="3" t="s">
         <v>1019</v>
-      </c>
-      <c r="B260" s="3" t="s">
-        <v>1020</v>
       </c>
     </row>
     <row r="261" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A261" s="2" t="s">
+        <v>1020</v>
+      </c>
+      <c r="B261" s="3" t="s">
         <v>1021</v>
-      </c>
-      <c r="B261" s="3" t="s">
-        <v>1022</v>
       </c>
     </row>
     <row r="262" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -37429,15 +37430,15 @@
         <v>135</v>
       </c>
       <c r="B262" s="3" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="263" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A263" s="2" t="s">
+        <v>1023</v>
+      </c>
+      <c r="B263" s="3" t="s">
         <v>1024</v>
-      </c>
-      <c r="B263" s="3" t="s">
-        <v>1025</v>
       </c>
     </row>
     <row r="264" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -37445,7 +37446,7 @@
         <v>136</v>
       </c>
       <c r="B264" s="3" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="265" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -37469,7 +37470,7 @@
         <v>233</v>
       </c>
       <c r="B267" s="3" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
     </row>
     <row r="268" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -37477,7 +37478,7 @@
         <v>138</v>
       </c>
       <c r="B268" s="3" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
     </row>
     <row r="269" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37485,7 +37486,7 @@
         <v>234</v>
       </c>
       <c r="B269" s="3" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="270" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37493,7 +37494,7 @@
         <v>235</v>
       </c>
       <c r="B270" s="3" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="271" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -37501,7 +37502,7 @@
         <v>139</v>
       </c>
       <c r="B271" s="3" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="272" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -37509,7 +37510,7 @@
         <v>239</v>
       </c>
       <c r="B272" s="3" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
     </row>
     <row r="273" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37517,7 +37518,7 @@
         <v>240</v>
       </c>
       <c r="B273" s="3" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="274" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37525,7 +37526,7 @@
         <v>241</v>
       </c>
       <c r="B274" s="3" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
     </row>
     <row r="275" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37533,7 +37534,7 @@
         <v>140</v>
       </c>
       <c r="B275" s="3" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="276" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -37541,7 +37542,7 @@
         <v>236</v>
       </c>
       <c r="B276" s="3" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="277" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37549,7 +37550,7 @@
         <v>237</v>
       </c>
       <c r="B277" s="3" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="278" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37557,7 +37558,7 @@
         <v>238</v>
       </c>
       <c r="B278" s="3" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="279" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -37565,7 +37566,7 @@
         <v>141</v>
       </c>
       <c r="B279" s="3" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="280" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -37573,7 +37574,7 @@
         <v>142</v>
       </c>
       <c r="B280" s="3" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="281" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -37581,7 +37582,7 @@
         <v>143</v>
       </c>
       <c r="B281" s="3" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="282" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -37589,7 +37590,7 @@
         <v>144</v>
       </c>
       <c r="B282" s="3" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="283" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -37597,7 +37598,7 @@
         <v>242</v>
       </c>
       <c r="B283" s="3" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="284" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37605,7 +37606,7 @@
         <v>145</v>
       </c>
       <c r="B284" s="3" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="285" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -37613,7 +37614,7 @@
         <v>146</v>
       </c>
       <c r="B285" s="3" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="286" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37621,7 +37622,7 @@
         <v>147</v>
       </c>
       <c r="B286" s="3" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="287" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -37629,7 +37630,7 @@
         <v>148</v>
       </c>
       <c r="B287" s="3" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="288" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -37637,31 +37638,31 @@
         <v>149</v>
       </c>
       <c r="B288" s="3" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="289" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A289" s="2" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="B289" s="3" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="290" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A290" s="2" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="B290" s="3" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="291" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A291" s="2" t="s">
+        <v>1094</v>
+      </c>
+      <c r="B291" s="3" t="s">
         <v>1095</v>
-      </c>
-      <c r="B291" s="3" t="s">
-        <v>1096</v>
       </c>
     </row>
     <row r="292" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37669,15 +37670,15 @@
         <v>150</v>
       </c>
       <c r="B292" s="3" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="293" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A293" s="2" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="B293" s="3" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="294" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -37685,7 +37686,7 @@
         <v>151</v>
       </c>
       <c r="B294" s="3" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
     </row>
     <row r="295" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37693,7 +37694,7 @@
         <v>243</v>
       </c>
       <c r="B295" s="3" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
     </row>
     <row r="296" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37701,7 +37702,7 @@
         <v>244</v>
       </c>
       <c r="B296" s="3" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
     </row>
     <row r="297" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37709,7 +37710,7 @@
         <v>245</v>
       </c>
       <c r="B297" s="3" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="298" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37717,7 +37718,7 @@
         <v>152</v>
       </c>
       <c r="B298" s="3" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
     </row>
     <row r="299" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -37725,7 +37726,7 @@
         <v>153</v>
       </c>
       <c r="B299" s="3" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="300" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37733,7 +37734,7 @@
         <v>154</v>
       </c>
       <c r="B300" s="3" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="301" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -37741,7 +37742,7 @@
         <v>155</v>
       </c>
       <c r="B301" s="3" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
     </row>
     <row r="302" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37749,7 +37750,7 @@
         <v>156</v>
       </c>
       <c r="B302" s="3" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="303" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -37757,7 +37758,7 @@
         <v>157</v>
       </c>
       <c r="B303" s="3" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="304" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -37765,7 +37766,7 @@
         <v>246</v>
       </c>
       <c r="B304" s="3" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
     </row>
     <row r="305" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37773,7 +37774,7 @@
         <v>247</v>
       </c>
       <c r="B305" s="3" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
     </row>
     <row r="306" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37781,7 +37782,7 @@
         <v>248</v>
       </c>
       <c r="B306" s="3" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="307" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37789,7 +37790,7 @@
         <v>158</v>
       </c>
       <c r="B307" s="3" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="308" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -37797,7 +37798,7 @@
         <v>159</v>
       </c>
       <c r="B308" s="3" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="309" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37805,7 +37806,7 @@
         <v>160</v>
       </c>
       <c r="B309" s="3" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="310" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -37813,7 +37814,7 @@
         <v>161</v>
       </c>
       <c r="B310" s="3" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="311" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37821,31 +37822,31 @@
         <v>162</v>
       </c>
       <c r="B311" s="3" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="312" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A312" s="2" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="B312" s="3" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="313" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A313" s="2" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="B313" s="3" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="314" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A314" s="2" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="B314" s="3" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="315" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37853,7 +37854,7 @@
         <v>163</v>
       </c>
       <c r="B315" s="3" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="316" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -37861,7 +37862,7 @@
         <v>164</v>
       </c>
       <c r="B316" s="3" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="317" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37869,7 +37870,7 @@
         <v>175</v>
       </c>
       <c r="B317" s="3" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="318" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -37877,7 +37878,7 @@
         <v>176</v>
       </c>
       <c r="B318" s="3" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="319" spans="1:2" ht="390" x14ac:dyDescent="0.25">
@@ -37885,7 +37886,7 @@
         <v>177</v>
       </c>
       <c r="B319" s="3" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="320" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -37893,7 +37894,7 @@
         <v>527</v>
       </c>
       <c r="B320" s="3" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="321" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37901,7 +37902,7 @@
         <v>528</v>
       </c>
       <c r="B321" s="3" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="322" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37909,7 +37910,7 @@
         <v>529</v>
       </c>
       <c r="B322" s="3" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="323" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -37917,7 +37918,7 @@
         <v>530</v>
       </c>
       <c r="B323" s="3" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="324" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37925,7 +37926,7 @@
         <v>531</v>
       </c>
       <c r="B324" s="3" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="325" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37933,15 +37934,15 @@
         <v>532</v>
       </c>
       <c r="B325" s="3" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="326" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A326" s="2" t="s">
+        <v>1116</v>
+      </c>
+      <c r="B326" s="3" t="s">
         <v>1117</v>
-      </c>
-      <c r="B326" s="3" t="s">
-        <v>1118</v>
       </c>
     </row>
     <row r="327" spans="1:2" ht="390" x14ac:dyDescent="0.25">
@@ -37949,7 +37950,7 @@
         <v>178</v>
       </c>
       <c r="B327" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="328" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -37957,7 +37958,7 @@
         <v>500</v>
       </c>
       <c r="B328" s="3" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="329" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37965,7 +37966,7 @@
         <v>557</v>
       </c>
       <c r="B329" s="3" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="330" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37973,7 +37974,7 @@
         <v>558</v>
       </c>
       <c r="B330" s="3" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="331" spans="1:2" ht="315" x14ac:dyDescent="0.25">
@@ -37981,7 +37982,7 @@
         <v>179</v>
       </c>
       <c r="B331" s="3" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
     </row>
     <row r="332" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -37989,7 +37990,7 @@
         <v>249</v>
       </c>
       <c r="B332" s="3" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
     </row>
     <row r="333" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -37997,7 +37998,7 @@
         <v>250</v>
       </c>
       <c r="B333" s="3" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
     </row>
     <row r="334" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -38005,7 +38006,7 @@
         <v>251</v>
       </c>
       <c r="B334" s="3" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
     </row>
     <row r="335" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38013,7 +38014,7 @@
         <v>252</v>
       </c>
       <c r="B335" s="3" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
     </row>
     <row r="336" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -38021,23 +38022,23 @@
         <v>253</v>
       </c>
       <c r="B336" s="3" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
     </row>
     <row r="337" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A337" s="2" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="B337" s="3" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
     </row>
     <row r="338" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A338" s="2" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="B338" s="3" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="339" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -38045,7 +38046,7 @@
         <v>180</v>
       </c>
       <c r="B339" s="3" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="340" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38077,7 +38078,7 @@
         <v>183</v>
       </c>
       <c r="B343" s="3" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="344" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -38149,7 +38150,7 @@
         <v>461</v>
       </c>
       <c r="B352" s="3" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
     </row>
     <row r="353" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -38181,15 +38182,15 @@
         <v>192</v>
       </c>
       <c r="B356" s="3" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="357" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A357" s="2" t="s">
+        <v>627</v>
+      </c>
+      <c r="B357" s="3" t="s">
         <v>628</v>
-      </c>
-      <c r="B357" s="3" t="s">
-        <v>629</v>
       </c>
     </row>
     <row r="358" spans="1:2" ht="270" x14ac:dyDescent="0.25">
@@ -38197,7 +38198,7 @@
         <v>193</v>
       </c>
       <c r="B358" s="3" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
     </row>
     <row r="359" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -38213,7 +38214,7 @@
         <v>341</v>
       </c>
       <c r="B360" s="3" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
     </row>
     <row r="361" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -38221,7 +38222,7 @@
         <v>194</v>
       </c>
       <c r="B361" s="3" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="362" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -38229,7 +38230,7 @@
         <v>195</v>
       </c>
       <c r="B362" s="3" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
     </row>
     <row r="363" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -38237,7 +38238,7 @@
         <v>196</v>
       </c>
       <c r="B363" s="3" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
     </row>
     <row r="364" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -38245,7 +38246,7 @@
         <v>331</v>
       </c>
       <c r="B364" s="3" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
     </row>
     <row r="365" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -38253,15 +38254,15 @@
         <v>197</v>
       </c>
       <c r="B365" s="3" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="366" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A366" s="2" t="s">
+        <v>671</v>
+      </c>
+      <c r="B366" s="3" t="s">
         <v>672</v>
-      </c>
-      <c r="B366" s="3" t="s">
-        <v>673</v>
       </c>
     </row>
     <row r="367" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38269,7 +38270,7 @@
         <v>198</v>
       </c>
       <c r="B367" s="3" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
     </row>
     <row r="368" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38277,7 +38278,7 @@
         <v>199</v>
       </c>
       <c r="B368" s="3" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
     </row>
     <row r="369" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -38285,7 +38286,7 @@
         <v>200</v>
       </c>
       <c r="B369" s="3" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="370" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -38293,7 +38294,7 @@
         <v>201</v>
       </c>
       <c r="B370" s="3" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
     </row>
     <row r="371" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38301,7 +38302,7 @@
         <v>202</v>
       </c>
       <c r="B371" s="3" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="372" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -38309,47 +38310,47 @@
         <v>203</v>
       </c>
       <c r="B372" s="3" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="373" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A373" s="2" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B373" s="3" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="374" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A374" s="2" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="B374" s="3" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="375" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A375" s="2" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="B375" s="3" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
     </row>
     <row r="376" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A376" s="2" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="B376" s="3" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="377" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A377" s="2" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="B377" s="3" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="378" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -38357,55 +38358,55 @@
         <v>204</v>
       </c>
       <c r="B378" s="3" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="379" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A379" s="2" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="B379" s="3" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="380" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A380" s="2" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="B380" s="3" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="381" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A381" s="2" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="B381" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="382" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A382" s="2" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="B382" s="3" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="383" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A383" s="2" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B383" s="3" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="384" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A384" s="2" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="B384" s="3" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
     </row>
     <row r="385" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -38413,55 +38414,55 @@
         <v>205</v>
       </c>
       <c r="B385" s="3" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="386" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A386" s="2" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="B386" s="3" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
     </row>
     <row r="387" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A387" s="2" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="B387" s="3" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
     </row>
     <row r="388" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A388" s="2" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="B388" s="3" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="389" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A389" s="2" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="B389" s="3" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
     </row>
     <row r="390" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A390" s="2" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="B390" s="3" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="391" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A391" s="2" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="B391" s="3" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
     </row>
     <row r="392" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38469,7 +38470,7 @@
         <v>206</v>
       </c>
       <c r="B392" s="3" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="393" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -38477,7 +38478,7 @@
         <v>207</v>
       </c>
       <c r="B393" s="3" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="394" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -38485,7 +38486,7 @@
         <v>208</v>
       </c>
       <c r="B394" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="395" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -38493,55 +38494,55 @@
         <v>209</v>
       </c>
       <c r="B395" s="3" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
     </row>
     <row r="396" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A396" s="2" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="B396" s="3" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
     </row>
     <row r="397" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A397" s="2" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="B397" s="3" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="398" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A398" s="2" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="B398" s="3" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="399" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A399" s="2" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="B399" s="3" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
     </row>
     <row r="400" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A400" s="2" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="B400" s="4" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
     </row>
     <row r="401" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A401" s="2" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="B401" s="3" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
     </row>
     <row r="402" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -38549,63 +38550,63 @@
         <v>210</v>
       </c>
       <c r="B402" s="3" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="403" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A403" s="2" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="B403" s="3" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
     </row>
     <row r="404" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A404" s="2" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="B404" s="3" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="405" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A405" s="2" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="B405" s="3" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="406" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A406" s="2" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="B406" s="3" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="407" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A407" s="2" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="B407" s="3" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
     <row r="408" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A408" s="2" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="B408" s="3" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="409" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A409" s="2" t="s">
+        <v>649</v>
+      </c>
+      <c r="B409" s="3" t="s">
         <v>650</v>
-      </c>
-      <c r="B409" s="3" t="s">
-        <v>651</v>
       </c>
     </row>
     <row r="410" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -38613,7 +38614,7 @@
         <v>211</v>
       </c>
       <c r="B410" s="3" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
     </row>
     <row r="411" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -38661,7 +38662,7 @@
         <v>213</v>
       </c>
       <c r="B416" s="3" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
     </row>
     <row r="417" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -38669,7 +38670,7 @@
         <v>214</v>
       </c>
       <c r="B417" s="3" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
     </row>
     <row r="418" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -38677,7 +38678,7 @@
         <v>215</v>
       </c>
       <c r="B418" s="3" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="419" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38709,7 +38710,7 @@
         <v>219</v>
       </c>
       <c r="B422" s="3" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
     </row>
     <row r="423" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38717,7 +38718,7 @@
         <v>220</v>
       </c>
       <c r="B423" s="3" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
     </row>
     <row r="424" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -38725,7 +38726,7 @@
         <v>221</v>
       </c>
       <c r="B424" s="3" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="425" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -38733,7 +38734,7 @@
         <v>222</v>
       </c>
       <c r="B425" s="3" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="426" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -38741,7 +38742,7 @@
         <v>223</v>
       </c>
       <c r="B426" s="3" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="427" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -38749,7 +38750,7 @@
         <v>224</v>
       </c>
       <c r="B427" s="3" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="428" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -38757,7 +38758,7 @@
         <v>332</v>
       </c>
       <c r="B428" s="3" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="429" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -38773,7 +38774,7 @@
         <v>225</v>
       </c>
       <c r="B430" s="3" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
     </row>
     <row r="431" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -38837,7 +38838,7 @@
         <v>449</v>
       </c>
       <c r="B438" s="3" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="439" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -38845,31 +38846,31 @@
         <v>451</v>
       </c>
       <c r="B439" s="3" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="440" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A440" s="2" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="B440" s="3" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="441" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A441" s="2" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="B441" s="3" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
     </row>
     <row r="442" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A442" s="2" t="s">
+        <v>801</v>
+      </c>
+      <c r="B442" s="3" t="s">
         <v>802</v>
-      </c>
-      <c r="B442" s="3" t="s">
-        <v>803</v>
       </c>
     </row>
     <row r="443" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -38877,7 +38878,7 @@
         <v>319</v>
       </c>
       <c r="B443" s="3" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="444" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -38885,7 +38886,7 @@
         <v>320</v>
       </c>
       <c r="B444" s="3" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="445" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -38893,7 +38894,7 @@
         <v>321</v>
       </c>
       <c r="B445" s="3" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="446" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -38901,15 +38902,15 @@
         <v>318</v>
       </c>
       <c r="B446" s="3" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="447" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A447" s="2" t="s">
+        <v>1069</v>
+      </c>
+      <c r="B447" s="3" t="s">
         <v>1070</v>
-      </c>
-      <c r="B447" s="3" t="s">
-        <v>1071</v>
       </c>
     </row>
     <row r="448" spans="1:2" ht="255" x14ac:dyDescent="0.25">
@@ -38917,7 +38918,7 @@
         <v>322</v>
       </c>
       <c r="B448" s="3" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="449" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38933,7 +38934,7 @@
         <v>491</v>
       </c>
       <c r="B450" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="451" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -38965,7 +38966,7 @@
         <v>497</v>
       </c>
       <c r="B454" s="3" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="455" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -38973,303 +38974,303 @@
         <v>498</v>
       </c>
       <c r="B455" s="3" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="456" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A456" s="2" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B456" s="3" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="457" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A457" s="2" t="s">
+        <v>570</v>
+      </c>
+      <c r="B457" s="3" t="s">
         <v>571</v>
-      </c>
-      <c r="B457" s="3" t="s">
-        <v>572</v>
       </c>
     </row>
     <row r="458" spans="1:2" ht="225" x14ac:dyDescent="0.25">
       <c r="A458" s="2" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="B458" s="3" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
     </row>
     <row r="459" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A459" s="2" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="B459" s="3" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="460" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A460" s="2" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B460" s="3" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="461" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A461" s="2" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="B461" s="3" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="462" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A462" s="2" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="B462" s="3" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="463" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A463" s="2" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="B463" s="3" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="464" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A464" s="2" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="B464" s="3" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="465" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A465" s="2" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="B465" s="3" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="466" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A466" s="2" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="B466" s="3" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="467" spans="1:2" ht="225" x14ac:dyDescent="0.25">
       <c r="A467" s="2" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="B467" s="3" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="468" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A468" s="2" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="B468" s="3" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
     </row>
     <row r="469" spans="1:2" ht="225" x14ac:dyDescent="0.25">
       <c r="A469" s="2" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="B469" s="3" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
     </row>
     <row r="470" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A470" s="2" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="B470" s="3" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
     </row>
     <row r="471" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A471" s="2" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="B471" s="3" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
     </row>
     <row r="472" spans="1:2" ht="225" x14ac:dyDescent="0.25">
       <c r="A472" s="2" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="B472" s="3" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
     </row>
     <row r="473" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A473" s="2" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="B473" s="3" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
     </row>
     <row r="474" spans="1:2" ht="255" x14ac:dyDescent="0.25">
       <c r="A474" s="2" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="B474" s="1" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
     </row>
     <row r="475" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A475" s="2" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="B475" s="1" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="476" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A476" s="2" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="B476" s="1" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
     </row>
     <row r="477" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A477" s="2" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="B477" s="1" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="478" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A478" s="2" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="B478" s="1" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="479" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A479" s="2" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="B479" s="1" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="480" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A480" s="2" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="B480" s="1" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
     </row>
     <row r="481" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A481" s="2" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="B481" s="1" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
     </row>
     <row r="482" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A482" s="2" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="B482" s="1" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
     </row>
     <row r="483" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A483" s="2" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="B483" s="1" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
     </row>
     <row r="484" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A484" s="2" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="B484" s="1" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
     </row>
     <row r="485" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A485" s="2" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="B485" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
     </row>
     <row r="486" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A486" s="2" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="B486" s="1" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
     </row>
     <row r="487" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A487" s="2" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="B487" s="1" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="488" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A488" s="2" t="s">
+        <v>700</v>
+      </c>
+      <c r="B488" s="1" t="s">
         <v>701</v>
-      </c>
-      <c r="B488" s="1" t="s">
-        <v>702</v>
       </c>
     </row>
     <row r="489" spans="1:2" ht="255" x14ac:dyDescent="0.25">
       <c r="A489" s="2" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="B489" s="1" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="490" spans="1:2" ht="92.25" x14ac:dyDescent="0.25">
       <c r="A490" s="2" t="s">
+        <v>1049</v>
+      </c>
+      <c r="B490" s="1" t="s">
         <v>1050</v>
-      </c>
-      <c r="B490" s="1" t="s">
-        <v>1051</v>
       </c>
     </row>
     <row r="491" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A491" s="2" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="B491" s="1" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
     </row>
     <row r="492" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A492" s="2" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="B492" s="3" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="493" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -39277,7 +39278,7 @@
         <v>552</v>
       </c>
       <c r="B493" s="3" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="494" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -39285,7 +39286,7 @@
         <v>553</v>
       </c>
       <c r="B494" s="3" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
     </row>
     <row r="495" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -39293,7 +39294,7 @@
         <v>554</v>
       </c>
       <c r="B495" s="3" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
     </row>
     <row r="496" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39365,7 +39366,7 @@
         <v>275</v>
       </c>
       <c r="B504" s="1" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="505" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39373,7 +39374,7 @@
         <v>276</v>
       </c>
       <c r="B505" s="1" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="506" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39381,7 +39382,7 @@
         <v>277</v>
       </c>
       <c r="B506" s="1" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="507" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -39429,7 +39430,7 @@
         <v>260</v>
       </c>
       <c r="B512" s="3" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="513" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39437,7 +39438,7 @@
         <v>480</v>
       </c>
       <c r="B513" s="3" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
     </row>
     <row r="514" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -39445,15 +39446,15 @@
         <v>481</v>
       </c>
       <c r="B514" s="1" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
     </row>
     <row r="515" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A515" s="2" t="s">
+        <v>809</v>
+      </c>
+      <c r="B515" s="3" t="s">
         <v>810</v>
-      </c>
-      <c r="B515" s="3" t="s">
-        <v>811</v>
       </c>
     </row>
     <row r="516" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39501,7 +39502,7 @@
         <v>285</v>
       </c>
       <c r="B521" s="1" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
     </row>
     <row r="522" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -39509,7 +39510,7 @@
         <v>286</v>
       </c>
       <c r="B522" s="1" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
     </row>
     <row r="523" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -39589,7 +39590,7 @@
         <v>296</v>
       </c>
       <c r="B532" s="1" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
     </row>
     <row r="533" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -39597,7 +39598,7 @@
         <v>297</v>
       </c>
       <c r="B533" s="1" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="534" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -39621,7 +39622,7 @@
         <v>406</v>
       </c>
       <c r="B536" s="1" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="537" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -39629,7 +39630,7 @@
         <v>298</v>
       </c>
       <c r="B537" s="1" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
     </row>
     <row r="538" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -39645,7 +39646,7 @@
         <v>299</v>
       </c>
       <c r="B539" s="1" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
     </row>
     <row r="540" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -39669,7 +39670,7 @@
         <v>300</v>
       </c>
       <c r="B542" s="1" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
     </row>
     <row r="543" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -39677,7 +39678,7 @@
         <v>301</v>
       </c>
       <c r="B543" s="1" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
     </row>
     <row r="544" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -39717,7 +39718,7 @@
         <v>396</v>
       </c>
       <c r="B548" s="1" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
     </row>
     <row r="549" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -39730,10 +39731,10 @@
     </row>
     <row r="550" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A550" s="2" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="B550" s="1" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
     </row>
     <row r="551" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -39741,7 +39742,7 @@
         <v>305</v>
       </c>
       <c r="B551" s="1" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
     </row>
     <row r="552" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -39770,10 +39771,10 @@
     </row>
     <row r="555" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A555" s="2" t="s">
+        <v>749</v>
+      </c>
+      <c r="B555" s="1" t="s">
         <v>750</v>
-      </c>
-      <c r="B555" s="1" t="s">
-        <v>751</v>
       </c>
     </row>
     <row r="556" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -39781,7 +39782,7 @@
         <v>306</v>
       </c>
       <c r="B556" s="1" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
     </row>
     <row r="557" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -39805,7 +39806,7 @@
         <v>307</v>
       </c>
       <c r="B559" s="1" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="560" spans="1:2" ht="375" x14ac:dyDescent="0.25">
@@ -39813,7 +39814,7 @@
         <v>311</v>
       </c>
       <c r="B560" s="1" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
     </row>
     <row r="561" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39837,15 +39838,15 @@
         <v>376</v>
       </c>
       <c r="B563" s="3" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="564" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A564" s="2" t="s">
+        <v>753</v>
+      </c>
+      <c r="B564" s="3" t="s">
         <v>754</v>
-      </c>
-      <c r="B564" s="3" t="s">
-        <v>755</v>
       </c>
     </row>
     <row r="565" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -39853,7 +39854,7 @@
         <v>329</v>
       </c>
       <c r="B565" s="3" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix issue with prince not assigned to stack on startup.
</commit_message>
<xml_diff>
--- a/Documentation/Events.xlsx
+++ b/Documentation/Events.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\happysulla\BarbarianPrince\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A1C9DFEB-C5AC-42B2-BA6C-68972E7831A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EEB1568B-564D-4985-88BA-BDCADA757DF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21545,55 +21544,6 @@
   </si>
   <si>
     <r>
-      <t>&lt;Bold&gt;e130d High Lord on Travels Arrest You&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-You are arrested. You are jailed at the Lord's residence which is either the appropriate castle, nearest temple, or nearest town. Advance time by one day to represent the time spent reaching the jail. It may be by a magical means to travel in one day. Click image to continue.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                  &lt;InlineUIContainer&gt;&lt;Image Name='</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>JailTravels</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>' Source='../../Images/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>JailOvernight</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.gif' Height='200' Width='200'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>&lt;Bold&gt;e130e Audience With High Lord on Travels&lt;/Bold&gt;
 &lt;LineBreak/&gt;
 &lt;LineBreak/&gt;If you gain an audence with Baron Huldra, see &lt;InlineUIContainer&gt;&lt;Button Content='e130f' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
@@ -34862,6 +34812,55 @@
   </si>
   <si>
     <t>e050a</t>
+  </si>
+  <si>
+    <r>
+      <t>&lt;Bold&gt;e130d High Lord on Travels Arrest You&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+You are arrested. You are jailed at the Lord's residence which is either the appropriate castle, nearest temple, or nearest town. Advance time by one day to represent the time spent reaching the jail. It may be by a magical means to travel in one day. Click image to continue.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                         &lt;InlineUIContainer&gt;&lt;Image Name='</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>JailTravels</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>' Source='../../Images/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>JailOvernight</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.gif' Height='200' Width='200'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -35327,8 +35326,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B565"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A146" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A147" sqref="A147"/>
+    <sheetView tabSelected="1" topLeftCell="A332" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B335" sqref="B335"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -35342,7 +35341,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -35350,7 +35349,7 @@
         <v>254</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -35358,7 +35357,7 @@
         <v>255</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -35366,15 +35365,15 @@
         <v>256</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="390" x14ac:dyDescent="0.25">
@@ -35398,7 +35397,7 @@
         <v>22</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35430,7 +35429,7 @@
         <v>3</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -35526,7 +35525,7 @@
         <v>15</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -35534,7 +35533,7 @@
         <v>16</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -35542,7 +35541,7 @@
         <v>17</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -35550,7 +35549,7 @@
         <v>18</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -35558,31 +35557,31 @@
         <v>261</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -35590,7 +35589,7 @@
         <v>19</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -35598,7 +35597,7 @@
         <v>20</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -35606,23 +35605,23 @@
         <v>21</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -35630,23 +35629,23 @@
         <v>25</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -35654,7 +35653,7 @@
         <v>26</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -35678,7 +35677,7 @@
         <v>27</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -35694,7 +35693,7 @@
         <v>29</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -35718,7 +35717,7 @@
         <v>719</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -35726,7 +35725,7 @@
         <v>31</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -35798,7 +35797,7 @@
         <v>264</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35806,7 +35805,7 @@
         <v>265</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -35942,7 +35941,7 @@
         <v>42</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35950,7 +35949,7 @@
         <v>46</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -36078,15 +36077,15 @@
         <v>59</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
+        <v>920</v>
+      </c>
+      <c r="B94" s="3" t="s">
         <v>921</v>
-      </c>
-      <c r="B94" s="3" t="s">
-        <v>922</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -36102,7 +36101,7 @@
         <v>795</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -36158,7 +36157,7 @@
         <v>66</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -36238,7 +36237,7 @@
         <v>70</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -36326,7 +36325,7 @@
         <v>77</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
     </row>
     <row r="125" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -36339,10 +36338,10 @@
     </row>
     <row r="126" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
+        <v>972</v>
+      </c>
+      <c r="B126" s="3" t="s">
         <v>973</v>
-      </c>
-      <c r="B126" s="3" t="s">
-        <v>974</v>
       </c>
     </row>
     <row r="127" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -36350,7 +36349,7 @@
         <v>78</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
     </row>
     <row r="128" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -36358,7 +36357,7 @@
         <v>377</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
     </row>
     <row r="129" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -36406,87 +36405,87 @@
         <v>81</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="135" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
     </row>
     <row r="136" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
     </row>
     <row r="137" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
     </row>
     <row r="138" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
     </row>
     <row r="139" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="B139" s="3" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
     </row>
     <row r="140" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
     </row>
     <row r="141" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
     </row>
     <row r="142" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="143" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
+        <v>988</v>
+      </c>
+      <c r="B143" s="3" t="s">
         <v>989</v>
-      </c>
-      <c r="B143" s="3" t="s">
-        <v>990</v>
       </c>
     </row>
     <row r="144" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
     </row>
     <row r="145" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -36494,7 +36493,7 @@
         <v>82</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
     </row>
     <row r="146" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -36507,7 +36506,7 @@
     </row>
     <row r="147" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="B147" s="3" t="s">
         <v>561</v>
@@ -36662,7 +36661,7 @@
         <v>445</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
     </row>
     <row r="167" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -36734,7 +36733,7 @@
         <v>93</v>
       </c>
       <c r="B175" s="3" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
     </row>
     <row r="176" spans="1:2" ht="270" x14ac:dyDescent="0.25">
@@ -36742,7 +36741,7 @@
         <v>94</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
     </row>
     <row r="177" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -36750,7 +36749,7 @@
         <v>95</v>
       </c>
       <c r="B177" s="3" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
     </row>
     <row r="178" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -36758,55 +36757,55 @@
         <v>96</v>
       </c>
       <c r="B178" s="3" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
     </row>
     <row r="179" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A179" s="2" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="B179" s="3" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
     </row>
     <row r="180" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A180" s="2" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="B180" s="3" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
     </row>
     <row r="181" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
     </row>
     <row r="182" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="B182" s="3" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
     </row>
     <row r="183" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="B183" s="3" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
     </row>
     <row r="184" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A184" s="2" t="s">
+        <v>891</v>
+      </c>
+      <c r="B184" s="3" t="s">
         <v>892</v>
-      </c>
-      <c r="B184" s="3" t="s">
-        <v>893</v>
       </c>
     </row>
     <row r="185" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -36814,7 +36813,7 @@
         <v>97</v>
       </c>
       <c r="B185" s="3" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
     </row>
     <row r="186" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -36862,7 +36861,7 @@
         <v>103</v>
       </c>
       <c r="B191" s="3" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="192" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -36870,7 +36869,7 @@
         <v>104</v>
       </c>
       <c r="B192" s="3" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
     </row>
     <row r="193" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -36902,7 +36901,7 @@
         <v>106</v>
       </c>
       <c r="B196" s="3" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
     </row>
     <row r="197" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -36934,7 +36933,7 @@
         <v>108</v>
       </c>
       <c r="B200" s="3" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="201" spans="1:2" ht="285" x14ac:dyDescent="0.25">
@@ -36942,7 +36941,7 @@
         <v>109</v>
       </c>
       <c r="B201" s="3" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
     </row>
     <row r="202" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -36958,7 +36957,7 @@
         <v>166</v>
       </c>
       <c r="B203" s="3" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="204" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -36966,7 +36965,7 @@
         <v>167</v>
       </c>
       <c r="B204" s="3" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="205" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -36974,23 +36973,23 @@
         <v>168</v>
       </c>
       <c r="B205" s="3" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="206" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A206" s="2" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="B206" s="3" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
     </row>
     <row r="207" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A207" s="2" t="s">
+        <v>906</v>
+      </c>
+      <c r="B207" s="3" t="s">
         <v>907</v>
-      </c>
-      <c r="B207" s="3" t="s">
-        <v>908</v>
       </c>
     </row>
     <row r="208" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37062,7 +37061,7 @@
         <v>171</v>
       </c>
       <c r="B216" s="3" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="217" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37070,7 +37069,7 @@
         <v>113</v>
       </c>
       <c r="B217" s="3" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="218" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -37078,7 +37077,7 @@
         <v>114</v>
       </c>
       <c r="B218" s="3" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
     </row>
     <row r="219" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -37086,15 +37085,15 @@
         <v>266</v>
       </c>
       <c r="B219" s="3" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
     </row>
     <row r="220" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A220" s="2" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="B220" s="3" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
     </row>
     <row r="221" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37102,7 +37101,7 @@
         <v>115</v>
       </c>
       <c r="B221" s="3" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
     </row>
     <row r="222" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -37118,7 +37117,7 @@
         <v>116</v>
       </c>
       <c r="B223" s="3" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="224" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -37158,7 +37157,7 @@
         <v>768</v>
       </c>
       <c r="B228" s="4" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
     </row>
     <row r="229" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -37166,23 +37165,23 @@
         <v>118</v>
       </c>
       <c r="B229" s="3" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
     </row>
     <row r="230" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A230" s="2" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="B230" s="3" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
     </row>
     <row r="231" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A231" s="2" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="B231" s="3" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="232" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -37190,23 +37189,23 @@
         <v>119</v>
       </c>
       <c r="B232" s="3" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
     </row>
     <row r="233" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A233" s="2" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="B233" s="3" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
     </row>
     <row r="234" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A234" s="2" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="B234" s="3" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
     </row>
     <row r="235" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -37214,7 +37213,7 @@
         <v>120</v>
       </c>
       <c r="B235" s="3" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
     </row>
     <row r="236" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -37222,7 +37221,7 @@
         <v>172</v>
       </c>
       <c r="B236" s="3" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
     </row>
     <row r="237" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37230,7 +37229,7 @@
         <v>173</v>
       </c>
       <c r="B237" s="3" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
     </row>
     <row r="238" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37238,7 +37237,7 @@
         <v>174</v>
       </c>
       <c r="B238" s="3" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
     </row>
     <row r="239" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37270,23 +37269,23 @@
         <v>123</v>
       </c>
       <c r="B242" s="3" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
     </row>
     <row r="243" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A243" s="2" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="B243" s="3" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
     </row>
     <row r="244" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A244" s="2" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="B244" s="3" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
     </row>
     <row r="245" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37302,15 +37301,15 @@
         <v>125</v>
       </c>
       <c r="B246" s="3" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="247" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A247" s="2" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="B247" s="3" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="248" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37318,7 +37317,7 @@
         <v>126</v>
       </c>
       <c r="B248" s="3" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="249" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37326,7 +37325,7 @@
         <v>127</v>
       </c>
       <c r="B249" s="3" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
     </row>
     <row r="250" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37342,7 +37341,7 @@
         <v>129</v>
       </c>
       <c r="B251" s="3" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="252" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37350,7 +37349,7 @@
         <v>130</v>
       </c>
       <c r="B252" s="3" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="253" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -37358,23 +37357,23 @@
         <v>131</v>
       </c>
       <c r="B253" s="3" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
     </row>
     <row r="254" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A254" s="2" t="s">
+        <v>962</v>
+      </c>
+      <c r="B254" s="3" t="s">
         <v>963</v>
-      </c>
-      <c r="B254" s="3" t="s">
-        <v>964</v>
       </c>
     </row>
     <row r="255" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A255" s="2" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="B255" s="3" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
     </row>
     <row r="256" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -37382,7 +37381,7 @@
         <v>132</v>
       </c>
       <c r="B256" s="3" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="257" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -37390,15 +37389,15 @@
         <v>133</v>
       </c>
       <c r="B257" s="3" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="258" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A258" s="2" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="B258" s="3" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="259" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37406,23 +37405,23 @@
         <v>134</v>
       </c>
       <c r="B259" s="3" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="260" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A260" s="2" t="s">
+        <v>1017</v>
+      </c>
+      <c r="B260" s="3" t="s">
         <v>1018</v>
-      </c>
-      <c r="B260" s="3" t="s">
-        <v>1019</v>
       </c>
     </row>
     <row r="261" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A261" s="2" t="s">
+        <v>1019</v>
+      </c>
+      <c r="B261" s="3" t="s">
         <v>1020</v>
-      </c>
-      <c r="B261" s="3" t="s">
-        <v>1021</v>
       </c>
     </row>
     <row r="262" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -37430,15 +37429,15 @@
         <v>135</v>
       </c>
       <c r="B262" s="3" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="263" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A263" s="2" t="s">
+        <v>1022</v>
+      </c>
+      <c r="B263" s="3" t="s">
         <v>1023</v>
-      </c>
-      <c r="B263" s="3" t="s">
-        <v>1024</v>
       </c>
     </row>
     <row r="264" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -37446,7 +37445,7 @@
         <v>136</v>
       </c>
       <c r="B264" s="3" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="265" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -37470,7 +37469,7 @@
         <v>233</v>
       </c>
       <c r="B267" s="3" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
     </row>
     <row r="268" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -37534,7 +37533,7 @@
         <v>140</v>
       </c>
       <c r="B275" s="3" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="276" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -37542,7 +37541,7 @@
         <v>236</v>
       </c>
       <c r="B276" s="3" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="277" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37550,7 +37549,7 @@
         <v>237</v>
       </c>
       <c r="B277" s="3" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="278" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37558,7 +37557,7 @@
         <v>238</v>
       </c>
       <c r="B278" s="3" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="279" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -37566,7 +37565,7 @@
         <v>141</v>
       </c>
       <c r="B279" s="3" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="280" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -37574,7 +37573,7 @@
         <v>142</v>
       </c>
       <c r="B280" s="3" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="281" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -37582,7 +37581,7 @@
         <v>143</v>
       </c>
       <c r="B281" s="3" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="282" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -37590,7 +37589,7 @@
         <v>144</v>
       </c>
       <c r="B282" s="3" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="283" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -37598,7 +37597,7 @@
         <v>242</v>
       </c>
       <c r="B283" s="3" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="284" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37606,7 +37605,7 @@
         <v>145</v>
       </c>
       <c r="B284" s="3" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="285" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -37614,7 +37613,7 @@
         <v>146</v>
       </c>
       <c r="B285" s="3" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="286" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37622,7 +37621,7 @@
         <v>147</v>
       </c>
       <c r="B286" s="3" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="287" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -37630,7 +37629,7 @@
         <v>148</v>
       </c>
       <c r="B287" s="3" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="288" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -37638,31 +37637,31 @@
         <v>149</v>
       </c>
       <c r="B288" s="3" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="289" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A289" s="2" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="B289" s="3" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="290" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A290" s="2" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="B290" s="3" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="291" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A291" s="2" t="s">
+        <v>1093</v>
+      </c>
+      <c r="B291" s="3" t="s">
         <v>1094</v>
-      </c>
-      <c r="B291" s="3" t="s">
-        <v>1095</v>
       </c>
     </row>
     <row r="292" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37670,15 +37669,15 @@
         <v>150</v>
       </c>
       <c r="B292" s="3" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="293" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A293" s="2" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="B293" s="3" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="294" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -37726,7 +37725,7 @@
         <v>153</v>
       </c>
       <c r="B299" s="3" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="300" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37798,7 +37797,7 @@
         <v>159</v>
       </c>
       <c r="B308" s="3" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
     </row>
     <row r="309" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37806,7 +37805,7 @@
         <v>160</v>
       </c>
       <c r="B309" s="3" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="310" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -37814,7 +37813,7 @@
         <v>161</v>
       </c>
       <c r="B310" s="3" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="311" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37822,31 +37821,31 @@
         <v>162</v>
       </c>
       <c r="B311" s="3" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="312" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A312" s="2" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="B312" s="3" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="313" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A313" s="2" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="B313" s="3" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="314" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A314" s="2" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="B314" s="3" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="315" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37854,7 +37853,7 @@
         <v>163</v>
       </c>
       <c r="B315" s="3" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="316" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -37862,7 +37861,7 @@
         <v>164</v>
       </c>
       <c r="B316" s="3" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="317" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37870,7 +37869,7 @@
         <v>175</v>
       </c>
       <c r="B317" s="3" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="318" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -37878,7 +37877,7 @@
         <v>176</v>
       </c>
       <c r="B318" s="3" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="319" spans="1:2" ht="390" x14ac:dyDescent="0.25">
@@ -37886,7 +37885,7 @@
         <v>177</v>
       </c>
       <c r="B319" s="3" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="320" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -37894,7 +37893,7 @@
         <v>527</v>
       </c>
       <c r="B320" s="3" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="321" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37902,7 +37901,7 @@
         <v>528</v>
       </c>
       <c r="B321" s="3" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="322" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37910,7 +37909,7 @@
         <v>529</v>
       </c>
       <c r="B322" s="3" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="323" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -37918,7 +37917,7 @@
         <v>530</v>
       </c>
       <c r="B323" s="3" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="324" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37926,7 +37925,7 @@
         <v>531</v>
       </c>
       <c r="B324" s="3" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="325" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37934,15 +37933,15 @@
         <v>532</v>
       </c>
       <c r="B325" s="3" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="326" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A326" s="2" t="s">
+        <v>1115</v>
+      </c>
+      <c r="B326" s="3" t="s">
         <v>1116</v>
-      </c>
-      <c r="B326" s="3" t="s">
-        <v>1117</v>
       </c>
     </row>
     <row r="327" spans="1:2" ht="390" x14ac:dyDescent="0.25">
@@ -37950,7 +37949,7 @@
         <v>178</v>
       </c>
       <c r="B327" s="3" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="328" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -37958,7 +37957,7 @@
         <v>500</v>
       </c>
       <c r="B328" s="3" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="329" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37966,7 +37965,7 @@
         <v>557</v>
       </c>
       <c r="B329" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="330" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37974,7 +37973,7 @@
         <v>558</v>
       </c>
       <c r="B330" s="3" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="331" spans="1:2" ht="315" x14ac:dyDescent="0.25">
@@ -37998,7 +37997,7 @@
         <v>250</v>
       </c>
       <c r="B333" s="3" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
     </row>
     <row r="334" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -38006,7 +38005,7 @@
         <v>251</v>
       </c>
       <c r="B334" s="3" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
     </row>
     <row r="335" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38014,7 +38013,7 @@
         <v>252</v>
       </c>
       <c r="B335" s="3" t="s">
-        <v>858</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="336" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -38022,7 +38021,7 @@
         <v>253</v>
       </c>
       <c r="B336" s="3" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
     </row>
     <row r="337" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -38030,7 +38029,7 @@
         <v>855</v>
       </c>
       <c r="B337" s="3" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
     </row>
     <row r="338" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38038,7 +38037,7 @@
         <v>856</v>
       </c>
       <c r="B338" s="3" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="339" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -38046,7 +38045,7 @@
         <v>180</v>
       </c>
       <c r="B339" s="3" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="340" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38078,7 +38077,7 @@
         <v>183</v>
       </c>
       <c r="B343" s="3" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="344" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -38238,7 +38237,7 @@
         <v>196</v>
       </c>
       <c r="B363" s="3" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
     </row>
     <row r="364" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -38246,7 +38245,7 @@
         <v>331</v>
       </c>
       <c r="B364" s="3" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
     </row>
     <row r="365" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -38302,7 +38301,7 @@
         <v>202</v>
       </c>
       <c r="B371" s="3" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="372" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -38422,7 +38421,7 @@
         <v>598</v>
       </c>
       <c r="B386" s="3" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
     </row>
     <row r="387" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -38430,7 +38429,7 @@
         <v>599</v>
       </c>
       <c r="B387" s="3" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
     </row>
     <row r="388" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -38438,7 +38437,7 @@
         <v>600</v>
       </c>
       <c r="B388" s="3" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
     </row>
     <row r="389" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -38446,7 +38445,7 @@
         <v>601</v>
       </c>
       <c r="B389" s="3" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="390" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38462,7 +38461,7 @@
         <v>603</v>
       </c>
       <c r="B391" s="3" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
     </row>
     <row r="392" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38478,7 +38477,7 @@
         <v>207</v>
       </c>
       <c r="B393" s="3" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="394" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -38502,7 +38501,7 @@
         <v>653</v>
       </c>
       <c r="B396" s="3" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
     </row>
     <row r="397" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -38662,7 +38661,7 @@
         <v>213</v>
       </c>
       <c r="B416" s="3" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
     </row>
     <row r="417" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -38678,7 +38677,7 @@
         <v>215</v>
       </c>
       <c r="B418" s="3" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="419" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38726,7 +38725,7 @@
         <v>221</v>
       </c>
       <c r="B424" s="3" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="425" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -38734,7 +38733,7 @@
         <v>222</v>
       </c>
       <c r="B425" s="3" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="426" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -38742,7 +38741,7 @@
         <v>223</v>
       </c>
       <c r="B426" s="3" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="427" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -38750,7 +38749,7 @@
         <v>224</v>
       </c>
       <c r="B427" s="3" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="428" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -38758,7 +38757,7 @@
         <v>332</v>
       </c>
       <c r="B428" s="3" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="429" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -38774,7 +38773,7 @@
         <v>225</v>
       </c>
       <c r="B430" s="3" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
     </row>
     <row r="431" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -38838,7 +38837,7 @@
         <v>449</v>
       </c>
       <c r="B438" s="3" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="439" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -38878,7 +38877,7 @@
         <v>319</v>
       </c>
       <c r="B443" s="3" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="444" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -38886,7 +38885,7 @@
         <v>320</v>
       </c>
       <c r="B444" s="3" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="445" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -38894,7 +38893,7 @@
         <v>321</v>
       </c>
       <c r="B445" s="3" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="446" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -38902,15 +38901,15 @@
         <v>318</v>
       </c>
       <c r="B446" s="3" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="447" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A447" s="2" t="s">
+        <v>1068</v>
+      </c>
+      <c r="B447" s="3" t="s">
         <v>1069</v>
-      </c>
-      <c r="B447" s="3" t="s">
-        <v>1070</v>
       </c>
     </row>
     <row r="448" spans="1:2" ht="255" x14ac:dyDescent="0.25">
@@ -38918,7 +38917,7 @@
         <v>322</v>
       </c>
       <c r="B448" s="3" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="449" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38982,7 +38981,7 @@
         <v>566</v>
       </c>
       <c r="B456" s="3" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="457" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -39006,7 +39005,7 @@
         <v>575</v>
       </c>
       <c r="B459" s="3" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="460" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39030,7 +39029,7 @@
         <v>578</v>
       </c>
       <c r="B462" s="3" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="463" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -39054,7 +39053,7 @@
         <v>581</v>
       </c>
       <c r="B465" s="3" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="466" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -39086,7 +39085,7 @@
         <v>612</v>
       </c>
       <c r="B469" s="3" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
     </row>
     <row r="470" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -39094,7 +39093,7 @@
         <v>630</v>
       </c>
       <c r="B470" s="3" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
     </row>
     <row r="471" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -39110,15 +39109,15 @@
         <v>632</v>
       </c>
       <c r="B472" s="3" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
     </row>
     <row r="473" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A473" s="2" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="B473" s="3" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
     </row>
     <row r="474" spans="1:2" ht="255" x14ac:dyDescent="0.25">
@@ -39174,7 +39173,7 @@
         <v>679</v>
       </c>
       <c r="B480" s="1" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
     </row>
     <row r="481" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -39214,7 +39213,7 @@
         <v>684</v>
       </c>
       <c r="B485" s="1" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
     </row>
     <row r="486" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -39243,18 +39242,18 @@
     </row>
     <row r="489" spans="1:2" ht="255" x14ac:dyDescent="0.25">
       <c r="A489" s="2" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="B489" s="1" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="490" spans="1:2" ht="92.25" x14ac:dyDescent="0.25">
       <c r="A490" s="2" t="s">
+        <v>1048</v>
+      </c>
+      <c r="B490" s="1" t="s">
         <v>1049</v>
-      </c>
-      <c r="B490" s="1" t="s">
-        <v>1050</v>
       </c>
     </row>
     <row r="491" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -39262,7 +39261,7 @@
         <v>703</v>
       </c>
       <c r="B491" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
     </row>
     <row r="492" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -39270,7 +39269,7 @@
         <v>739</v>
       </c>
       <c r="B492" s="3" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="493" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -39366,7 +39365,7 @@
         <v>275</v>
       </c>
       <c r="B504" s="1" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="505" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39374,7 +39373,7 @@
         <v>276</v>
       </c>
       <c r="B505" s="1" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="506" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39382,7 +39381,7 @@
         <v>277</v>
       </c>
       <c r="B506" s="1" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="507" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -39430,7 +39429,7 @@
         <v>260</v>
       </c>
       <c r="B512" s="3" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="513" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39502,7 +39501,7 @@
         <v>285</v>
       </c>
       <c r="B521" s="1" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
     </row>
     <row r="522" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -39510,7 +39509,7 @@
         <v>286</v>
       </c>
       <c r="B522" s="1" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
     </row>
     <row r="523" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -39630,7 +39629,7 @@
         <v>298</v>
       </c>
       <c r="B537" s="1" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
     </row>
     <row r="538" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -39670,7 +39669,7 @@
         <v>300</v>
       </c>
       <c r="B542" s="1" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
     </row>
     <row r="543" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -39678,7 +39677,7 @@
         <v>301</v>
       </c>
       <c r="B543" s="1" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
     </row>
     <row r="544" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -39806,7 +39805,7 @@
         <v>307</v>
       </c>
       <c r="B559" s="1" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="560" spans="1:2" ht="375" x14ac:dyDescent="0.25">
@@ -39838,7 +39837,7 @@
         <v>376</v>
       </c>
       <c r="B563" s="3" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="564" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -39854,7 +39853,7 @@
         <v>329</v>
       </c>
       <c r="B565" s="3" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working issues with Wizard's Gift. Failure after sunstroke and redistribute.
</commit_message>
<xml_diff>
--- a/Documentation/Events.xlsx
+++ b/Documentation/Events.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\happysulla\BarbarianPrince\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstewa01\Documents\Visual Studio 2022\Projects\BarbarianPrince2\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EEB1568B-564D-4985-88BA-BDCADA757DF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A6BEE11F-6870-4D6E-B047-8AB729932A61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="-25320" yWindow="15" windowWidth="25440" windowHeight="15390" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" r:id="rId1"/>
@@ -10249,97 +10249,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t>&lt;Bold&gt;e210e Local Guide Available&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;Local guide available
- &lt;InlineUIContainer&gt;&lt;Button Content='r205' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
-. Hires fro 2 gold per day. He has a combat skill of 2 and endurnace 3.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;&lt;InlineUIContainer&gt;&lt;Image Name='</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>EncounterEnd</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>' Source='../../Images/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>CoinsStackedDeny</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.gif' Height='100'  Width='100'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;Click to allow him to join:
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;&lt;InlineUIContainer&gt;&lt;Image Name='</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>HireLocalGuide</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>' Source='../../Images/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>CoinsStacked</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">.gif' Height='100'  Width='100'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt; </t>
-    </r>
-  </si>
-  <si>
     <t>e210i</t>
   </si>
   <si>
@@ -34860,6 +34769,97 @@
         <scheme val="minor"/>
       </rPr>
       <t>.gif' Height='200' Width='200'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;Bold&gt;e210e Local Guide Available&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;Local guide available
+ &lt;InlineUIContainer&gt;&lt;Button Content='r205' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+. Hires for 2 gold per day. He has a combat skill of 2 and endurnace 3.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;&lt;InlineUIContainer&gt;&lt;Image Name='</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>EncounterEnd</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>' Source='../../Images/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CoinsStackedDeny</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.gif' Height='100'  Width='100'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;Click to allow him to join:
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;&lt;InlineUIContainer&gt;&lt;Image Name='</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>HireLocalGuide</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>' Source='../../Images/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CoinsStacked</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">.gif' Height='100'  Width='100'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt; </t>
     </r>
   </si>
 </sst>
@@ -35326,8 +35326,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B565"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A332" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B335" sqref="B335"/>
+    <sheetView tabSelected="1" topLeftCell="B459" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B463" sqref="B463"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -35341,7 +35341,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -35349,7 +35349,7 @@
         <v>254</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -35357,7 +35357,7 @@
         <v>255</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -35365,15 +35365,15 @@
         <v>256</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="390" x14ac:dyDescent="0.25">
@@ -35389,7 +35389,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35397,7 +35397,7 @@
         <v>22</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35429,7 +35429,7 @@
         <v>3</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -35437,7 +35437,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35445,7 +35445,7 @@
         <v>5</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35453,7 +35453,7 @@
         <v>6</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -35461,7 +35461,7 @@
         <v>7</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -35469,7 +35469,7 @@
         <v>8</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35477,7 +35477,7 @@
         <v>10</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35485,7 +35485,7 @@
         <v>9</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -35493,7 +35493,7 @@
         <v>11</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -35501,7 +35501,7 @@
         <v>12</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35509,7 +35509,7 @@
         <v>13</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35517,7 +35517,7 @@
         <v>14</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -35525,7 +35525,7 @@
         <v>15</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -35533,7 +35533,7 @@
         <v>16</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -35541,7 +35541,7 @@
         <v>17</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -35549,7 +35549,7 @@
         <v>18</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -35557,31 +35557,31 @@
         <v>261</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -35589,7 +35589,7 @@
         <v>19</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -35597,7 +35597,7 @@
         <v>20</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -35605,23 +35605,23 @@
         <v>21</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -35629,23 +35629,23 @@
         <v>25</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -35653,7 +35653,7 @@
         <v>26</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -35677,7 +35677,7 @@
         <v>27</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -35693,7 +35693,7 @@
         <v>29</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -35701,7 +35701,7 @@
         <v>30</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -35714,10 +35714,10 @@
     </row>
     <row r="48" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -35725,7 +35725,7 @@
         <v>31</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -35733,7 +35733,7 @@
         <v>32</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -35741,7 +35741,7 @@
         <v>33</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -35797,7 +35797,7 @@
         <v>264</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35805,7 +35805,7 @@
         <v>265</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -35829,7 +35829,7 @@
         <v>35</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -35861,7 +35861,7 @@
         <v>37</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="285" x14ac:dyDescent="0.25">
@@ -35869,7 +35869,7 @@
         <v>38</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -35877,7 +35877,7 @@
         <v>43</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35885,23 +35885,23 @@
         <v>44</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
+        <v>723</v>
+      </c>
+      <c r="B71" s="3" t="s">
         <v>724</v>
-      </c>
-      <c r="B71" s="3" t="s">
-        <v>725</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35909,7 +35909,7 @@
         <v>39</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -35941,7 +35941,7 @@
         <v>42</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35949,7 +35949,7 @@
         <v>46</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -35973,7 +35973,7 @@
         <v>49</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -36013,7 +36013,7 @@
         <v>54</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -36021,7 +36021,7 @@
         <v>55</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -36029,7 +36029,7 @@
         <v>56</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -36037,7 +36037,7 @@
         <v>57</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -36045,31 +36045,31 @@
         <v>58</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
+        <v>804</v>
+      </c>
+      <c r="B92" s="3" t="s">
         <v>805</v>
-      </c>
-      <c r="B92" s="3" t="s">
-        <v>806</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -36077,15 +36077,15 @@
         <v>59</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
+        <v>919</v>
+      </c>
+      <c r="B94" s="3" t="s">
         <v>920</v>
-      </c>
-      <c r="B94" s="3" t="s">
-        <v>921</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -36093,15 +36093,15 @@
         <v>60</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -36109,7 +36109,7 @@
         <v>61</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -36117,7 +36117,7 @@
         <v>62</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -36149,7 +36149,7 @@
         <v>65</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -36157,7 +36157,7 @@
         <v>66</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -36237,7 +36237,7 @@
         <v>70</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -36269,7 +36269,7 @@
         <v>72</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
     </row>
     <row r="118" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -36277,7 +36277,7 @@
         <v>73</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
     </row>
     <row r="119" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -36325,7 +36325,7 @@
         <v>77</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
     </row>
     <row r="125" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -36338,10 +36338,10 @@
     </row>
     <row r="126" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
+        <v>971</v>
+      </c>
+      <c r="B126" s="3" t="s">
         <v>972</v>
-      </c>
-      <c r="B126" s="3" t="s">
-        <v>973</v>
       </c>
     </row>
     <row r="127" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -36349,7 +36349,7 @@
         <v>78</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
     </row>
     <row r="128" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -36357,7 +36357,7 @@
         <v>377</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
     </row>
     <row r="129" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -36397,7 +36397,7 @@
         <v>80</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
     </row>
     <row r="134" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -36405,87 +36405,87 @@
         <v>81</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
     </row>
     <row r="135" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
     </row>
     <row r="136" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
     </row>
     <row r="137" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
     </row>
     <row r="138" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
     </row>
     <row r="139" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="B139" s="3" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
     </row>
     <row r="140" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
     </row>
     <row r="141" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="142" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
     </row>
     <row r="143" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
+        <v>987</v>
+      </c>
+      <c r="B143" s="3" t="s">
         <v>988</v>
-      </c>
-      <c r="B143" s="3" t="s">
-        <v>989</v>
       </c>
     </row>
     <row r="144" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
     </row>
     <row r="145" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -36493,7 +36493,7 @@
         <v>82</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="146" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -36501,12 +36501,12 @@
         <v>83</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
     </row>
     <row r="147" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="B147" s="3" t="s">
         <v>561</v>
@@ -36541,7 +36541,7 @@
         <v>560</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
     <row r="152" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -36549,7 +36549,7 @@
         <v>86</v>
       </c>
       <c r="B152" s="3" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
     </row>
     <row r="153" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -36605,7 +36605,7 @@
         <v>346</v>
       </c>
       <c r="B159" s="3" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="160" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -36613,7 +36613,7 @@
         <v>348</v>
       </c>
       <c r="B160" s="3" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
     <row r="161" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -36642,10 +36642,10 @@
     </row>
     <row r="164" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
+        <v>732</v>
+      </c>
+      <c r="B164" s="3" t="s">
         <v>733</v>
-      </c>
-      <c r="B164" s="3" t="s">
-        <v>734</v>
       </c>
     </row>
     <row r="165" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -36661,7 +36661,7 @@
         <v>445</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
     </row>
     <row r="167" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -36685,23 +36685,23 @@
         <v>90</v>
       </c>
       <c r="B169" s="3" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
     </row>
     <row r="170" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="B170" s="3" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
     </row>
     <row r="171" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="B171" s="3" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
     </row>
     <row r="172" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -36733,7 +36733,7 @@
         <v>93</v>
       </c>
       <c r="B175" s="3" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
     </row>
     <row r="176" spans="1:2" ht="270" x14ac:dyDescent="0.25">
@@ -36741,7 +36741,7 @@
         <v>94</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
     </row>
     <row r="177" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -36749,7 +36749,7 @@
         <v>95</v>
       </c>
       <c r="B177" s="3" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
     </row>
     <row r="178" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -36757,55 +36757,55 @@
         <v>96</v>
       </c>
       <c r="B178" s="3" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
     </row>
     <row r="179" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A179" s="2" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="B179" s="3" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
     </row>
     <row r="180" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A180" s="2" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="B180" s="3" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
     </row>
     <row r="181" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
     </row>
     <row r="182" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="B182" s="3" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
     </row>
     <row r="183" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="B183" s="3" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="184" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A184" s="2" t="s">
+        <v>890</v>
+      </c>
+      <c r="B184" s="3" t="s">
         <v>891</v>
-      </c>
-      <c r="B184" s="3" t="s">
-        <v>892</v>
       </c>
     </row>
     <row r="185" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -36813,7 +36813,7 @@
         <v>97</v>
       </c>
       <c r="B185" s="3" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
     </row>
     <row r="186" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -36821,7 +36821,7 @@
         <v>98</v>
       </c>
       <c r="B186" s="3" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="187" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -36829,7 +36829,7 @@
         <v>99</v>
       </c>
       <c r="B187" s="3" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="188" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -36845,7 +36845,7 @@
         <v>100</v>
       </c>
       <c r="B189" s="3" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
     </row>
     <row r="190" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -36853,7 +36853,7 @@
         <v>102</v>
       </c>
       <c r="B190" s="3" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="191" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -36861,7 +36861,7 @@
         <v>103</v>
       </c>
       <c r="B191" s="3" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="192" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -36869,7 +36869,7 @@
         <v>104</v>
       </c>
       <c r="B192" s="3" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
     </row>
     <row r="193" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -36877,23 +36877,23 @@
         <v>105</v>
       </c>
       <c r="B193" s="3" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
     </row>
     <row r="194" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A194" s="2" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="B194" s="3" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
     </row>
     <row r="195" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A195" s="2" t="s">
+        <v>705</v>
+      </c>
+      <c r="B195" s="3" t="s">
         <v>706</v>
-      </c>
-      <c r="B195" s="3" t="s">
-        <v>707</v>
       </c>
     </row>
     <row r="196" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -36901,7 +36901,7 @@
         <v>106</v>
       </c>
       <c r="B196" s="3" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
     </row>
     <row r="197" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -36909,7 +36909,7 @@
         <v>107</v>
       </c>
       <c r="B197" s="3" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
     </row>
     <row r="198" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -36917,15 +36917,15 @@
         <v>165</v>
       </c>
       <c r="B198" s="3" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="199" spans="1:2" ht="225" x14ac:dyDescent="0.25">
       <c r="A199" s="2" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="B199" s="3" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="200" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -36933,7 +36933,7 @@
         <v>108</v>
       </c>
       <c r="B200" s="3" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="201" spans="1:2" ht="285" x14ac:dyDescent="0.25">
@@ -36941,7 +36941,7 @@
         <v>109</v>
       </c>
       <c r="B201" s="3" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
     </row>
     <row r="202" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -36949,7 +36949,7 @@
         <v>110</v>
       </c>
       <c r="B202" s="3" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
     </row>
     <row r="203" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -36957,7 +36957,7 @@
         <v>166</v>
       </c>
       <c r="B203" s="3" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="204" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -36965,7 +36965,7 @@
         <v>167</v>
       </c>
       <c r="B204" s="3" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="205" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -36973,23 +36973,23 @@
         <v>168</v>
       </c>
       <c r="B205" s="3" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
     </row>
     <row r="206" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A206" s="2" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="B206" s="3" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
     </row>
     <row r="207" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A207" s="2" t="s">
+        <v>905</v>
+      </c>
+      <c r="B207" s="3" t="s">
         <v>906</v>
-      </c>
-      <c r="B207" s="3" t="s">
-        <v>907</v>
       </c>
     </row>
     <row r="208" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -36997,39 +36997,39 @@
         <v>111</v>
       </c>
       <c r="B208" s="3" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="209" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A209" s="2" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="B209" s="3" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="210" spans="1:2" ht="225" x14ac:dyDescent="0.25">
       <c r="A210" s="2" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="B210" s="3" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
     </row>
     <row r="211" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A211" s="2" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="B211" s="3" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="212" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A212" s="2" t="s">
+        <v>740</v>
+      </c>
+      <c r="B212" s="3" t="s">
         <v>741</v>
-      </c>
-      <c r="B212" s="3" t="s">
-        <v>742</v>
       </c>
     </row>
     <row r="213" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37037,7 +37037,7 @@
         <v>112</v>
       </c>
       <c r="B213" s="3" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
     </row>
     <row r="214" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37045,7 +37045,7 @@
         <v>169</v>
       </c>
       <c r="B214" s="3" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
     </row>
     <row r="215" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -37053,7 +37053,7 @@
         <v>170</v>
       </c>
       <c r="B215" s="3" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="216" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -37061,7 +37061,7 @@
         <v>171</v>
       </c>
       <c r="B216" s="3" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="217" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37069,7 +37069,7 @@
         <v>113</v>
       </c>
       <c r="B217" s="3" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="218" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -37077,7 +37077,7 @@
         <v>114</v>
       </c>
       <c r="B218" s="3" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
     </row>
     <row r="219" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -37085,15 +37085,15 @@
         <v>266</v>
       </c>
       <c r="B219" s="3" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
     </row>
     <row r="220" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A220" s="2" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="B220" s="3" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
     </row>
     <row r="221" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37101,15 +37101,15 @@
         <v>115</v>
       </c>
       <c r="B221" s="3" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="222" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A222" s="2" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="B222" s="3" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
     </row>
     <row r="223" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37117,15 +37117,15 @@
         <v>116</v>
       </c>
       <c r="B223" s="3" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="224" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A224" s="2" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="B224" s="3" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
     </row>
     <row r="225" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -37133,31 +37133,31 @@
         <v>117</v>
       </c>
       <c r="B225" s="4" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="226" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A226" s="2" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="B226" s="4" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
     </row>
     <row r="227" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A227" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="B227" s="4" t="s">
         <v>765</v>
-      </c>
-      <c r="B227" s="4" t="s">
-        <v>766</v>
       </c>
     </row>
     <row r="228" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A228" s="2" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="B228" s="4" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
     </row>
     <row r="229" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -37165,23 +37165,23 @@
         <v>118</v>
       </c>
       <c r="B229" s="3" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
     </row>
     <row r="230" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A230" s="2" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="B230" s="3" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
     </row>
     <row r="231" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A231" s="2" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="B231" s="3" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="232" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -37189,23 +37189,23 @@
         <v>119</v>
       </c>
       <c r="B232" s="3" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
     </row>
     <row r="233" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A233" s="2" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="B233" s="3" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
     </row>
     <row r="234" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A234" s="2" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="B234" s="3" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
     </row>
     <row r="235" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -37213,7 +37213,7 @@
         <v>120</v>
       </c>
       <c r="B235" s="3" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
     </row>
     <row r="236" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -37221,7 +37221,7 @@
         <v>172</v>
       </c>
       <c r="B236" s="3" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
     </row>
     <row r="237" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37229,7 +37229,7 @@
         <v>173</v>
       </c>
       <c r="B237" s="3" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
     </row>
     <row r="238" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37237,7 +37237,7 @@
         <v>174</v>
       </c>
       <c r="B238" s="3" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
     </row>
     <row r="239" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37253,15 +37253,15 @@
         <v>122</v>
       </c>
       <c r="B240" s="3" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
     </row>
     <row r="241" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A241" s="2" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="B241" s="3" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
     </row>
     <row r="242" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -37269,23 +37269,23 @@
         <v>123</v>
       </c>
       <c r="B242" s="3" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
     </row>
     <row r="243" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A243" s="2" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="B243" s="3" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
     </row>
     <row r="244" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A244" s="2" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="B244" s="3" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
     </row>
     <row r="245" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37293,7 +37293,7 @@
         <v>124</v>
       </c>
       <c r="B245" s="3" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
     </row>
     <row r="246" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37301,15 +37301,15 @@
         <v>125</v>
       </c>
       <c r="B246" s="3" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="247" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A247" s="2" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="B247" s="3" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="248" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37317,7 +37317,7 @@
         <v>126</v>
       </c>
       <c r="B248" s="3" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="249" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37325,7 +37325,7 @@
         <v>127</v>
       </c>
       <c r="B249" s="3" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
     </row>
     <row r="250" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37333,7 +37333,7 @@
         <v>128</v>
       </c>
       <c r="B250" s="3" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="251" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -37341,7 +37341,7 @@
         <v>129</v>
       </c>
       <c r="B251" s="3" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="252" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37349,7 +37349,7 @@
         <v>130</v>
       </c>
       <c r="B252" s="3" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
     </row>
     <row r="253" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -37357,23 +37357,23 @@
         <v>131</v>
       </c>
       <c r="B253" s="3" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
     </row>
     <row r="254" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A254" s="2" t="s">
+        <v>961</v>
+      </c>
+      <c r="B254" s="3" t="s">
         <v>962</v>
-      </c>
-      <c r="B254" s="3" t="s">
-        <v>963</v>
       </c>
     </row>
     <row r="255" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A255" s="2" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="B255" s="3" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
     </row>
     <row r="256" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -37381,7 +37381,7 @@
         <v>132</v>
       </c>
       <c r="B256" s="3" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="257" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -37389,15 +37389,15 @@
         <v>133</v>
       </c>
       <c r="B257" s="3" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="258" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A258" s="2" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="B258" s="3" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="259" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37405,23 +37405,23 @@
         <v>134</v>
       </c>
       <c r="B259" s="3" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="260" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A260" s="2" t="s">
+        <v>1016</v>
+      </c>
+      <c r="B260" s="3" t="s">
         <v>1017</v>
-      </c>
-      <c r="B260" s="3" t="s">
-        <v>1018</v>
       </c>
     </row>
     <row r="261" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A261" s="2" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B261" s="3" t="s">
         <v>1019</v>
-      </c>
-      <c r="B261" s="3" t="s">
-        <v>1020</v>
       </c>
     </row>
     <row r="262" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -37429,15 +37429,15 @@
         <v>135</v>
       </c>
       <c r="B262" s="3" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="263" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A263" s="2" t="s">
+        <v>1021</v>
+      </c>
+      <c r="B263" s="3" t="s">
         <v>1022</v>
-      </c>
-      <c r="B263" s="3" t="s">
-        <v>1023</v>
       </c>
     </row>
     <row r="264" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -37445,7 +37445,7 @@
         <v>136</v>
       </c>
       <c r="B264" s="3" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="265" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -37469,7 +37469,7 @@
         <v>233</v>
       </c>
       <c r="B267" s="3" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
     </row>
     <row r="268" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -37477,7 +37477,7 @@
         <v>138</v>
       </c>
       <c r="B268" s="3" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
     </row>
     <row r="269" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37485,7 +37485,7 @@
         <v>234</v>
       </c>
       <c r="B269" s="3" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
     </row>
     <row r="270" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37493,7 +37493,7 @@
         <v>235</v>
       </c>
       <c r="B270" s="3" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="271" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -37501,7 +37501,7 @@
         <v>139</v>
       </c>
       <c r="B271" s="3" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="272" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -37509,7 +37509,7 @@
         <v>239</v>
       </c>
       <c r="B272" s="3" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
     </row>
     <row r="273" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37517,7 +37517,7 @@
         <v>240</v>
       </c>
       <c r="B273" s="3" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="274" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37525,7 +37525,7 @@
         <v>241</v>
       </c>
       <c r="B274" s="3" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="275" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37533,7 +37533,7 @@
         <v>140</v>
       </c>
       <c r="B275" s="3" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="276" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -37541,7 +37541,7 @@
         <v>236</v>
       </c>
       <c r="B276" s="3" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="277" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37549,7 +37549,7 @@
         <v>237</v>
       </c>
       <c r="B277" s="3" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="278" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37557,7 +37557,7 @@
         <v>238</v>
       </c>
       <c r="B278" s="3" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="279" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -37565,7 +37565,7 @@
         <v>141</v>
       </c>
       <c r="B279" s="3" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="280" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -37573,7 +37573,7 @@
         <v>142</v>
       </c>
       <c r="B280" s="3" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="281" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -37581,7 +37581,7 @@
         <v>143</v>
       </c>
       <c r="B281" s="3" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="282" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -37589,7 +37589,7 @@
         <v>144</v>
       </c>
       <c r="B282" s="3" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="283" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -37597,7 +37597,7 @@
         <v>242</v>
       </c>
       <c r="B283" s="3" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="284" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37605,7 +37605,7 @@
         <v>145</v>
       </c>
       <c r="B284" s="3" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="285" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -37613,7 +37613,7 @@
         <v>146</v>
       </c>
       <c r="B285" s="3" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="286" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37621,7 +37621,7 @@
         <v>147</v>
       </c>
       <c r="B286" s="3" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="287" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -37629,7 +37629,7 @@
         <v>148</v>
       </c>
       <c r="B287" s="3" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="288" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -37637,31 +37637,31 @@
         <v>149</v>
       </c>
       <c r="B288" s="3" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="289" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A289" s="2" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="B289" s="3" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="290" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A290" s="2" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="B290" s="3" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="291" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A291" s="2" t="s">
+        <v>1092</v>
+      </c>
+      <c r="B291" s="3" t="s">
         <v>1093</v>
-      </c>
-      <c r="B291" s="3" t="s">
-        <v>1094</v>
       </c>
     </row>
     <row r="292" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37669,15 +37669,15 @@
         <v>150</v>
       </c>
       <c r="B292" s="3" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="293" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A293" s="2" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="B293" s="3" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="294" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -37685,7 +37685,7 @@
         <v>151</v>
       </c>
       <c r="B294" s="3" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
     </row>
     <row r="295" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37693,7 +37693,7 @@
         <v>243</v>
       </c>
       <c r="B295" s="3" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="296" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37701,7 +37701,7 @@
         <v>244</v>
       </c>
       <c r="B296" s="3" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
     </row>
     <row r="297" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37709,7 +37709,7 @@
         <v>245</v>
       </c>
       <c r="B297" s="3" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
     </row>
     <row r="298" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37717,7 +37717,7 @@
         <v>152</v>
       </c>
       <c r="B298" s="3" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
     </row>
     <row r="299" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -37725,7 +37725,7 @@
         <v>153</v>
       </c>
       <c r="B299" s="3" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="300" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37733,7 +37733,7 @@
         <v>154</v>
       </c>
       <c r="B300" s="3" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
     </row>
     <row r="301" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -37741,7 +37741,7 @@
         <v>155</v>
       </c>
       <c r="B301" s="3" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="302" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37749,7 +37749,7 @@
         <v>156</v>
       </c>
       <c r="B302" s="3" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
     </row>
     <row r="303" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -37757,7 +37757,7 @@
         <v>157</v>
       </c>
       <c r="B303" s="3" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="304" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -37765,7 +37765,7 @@
         <v>246</v>
       </c>
       <c r="B304" s="3" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
     </row>
     <row r="305" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37773,7 +37773,7 @@
         <v>247</v>
       </c>
       <c r="B305" s="3" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
     </row>
     <row r="306" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37781,7 +37781,7 @@
         <v>248</v>
       </c>
       <c r="B306" s="3" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
     </row>
     <row r="307" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37789,7 +37789,7 @@
         <v>158</v>
       </c>
       <c r="B307" s="3" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
     </row>
     <row r="308" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -37797,7 +37797,7 @@
         <v>159</v>
       </c>
       <c r="B308" s="3" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
     </row>
     <row r="309" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37805,7 +37805,7 @@
         <v>160</v>
       </c>
       <c r="B309" s="3" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="310" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -37813,7 +37813,7 @@
         <v>161</v>
       </c>
       <c r="B310" s="3" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="311" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37821,31 +37821,31 @@
         <v>162</v>
       </c>
       <c r="B311" s="3" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="312" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A312" s="2" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="B312" s="3" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="313" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A313" s="2" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="B313" s="3" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="314" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A314" s="2" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="B314" s="3" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="315" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37853,7 +37853,7 @@
         <v>163</v>
       </c>
       <c r="B315" s="3" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="316" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -37861,7 +37861,7 @@
         <v>164</v>
       </c>
       <c r="B316" s="3" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="317" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37869,7 +37869,7 @@
         <v>175</v>
       </c>
       <c r="B317" s="3" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="318" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -37877,7 +37877,7 @@
         <v>176</v>
       </c>
       <c r="B318" s="3" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="319" spans="1:2" ht="390" x14ac:dyDescent="0.25">
@@ -37885,7 +37885,7 @@
         <v>177</v>
       </c>
       <c r="B319" s="3" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="320" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -37893,7 +37893,7 @@
         <v>527</v>
       </c>
       <c r="B320" s="3" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="321" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37901,7 +37901,7 @@
         <v>528</v>
       </c>
       <c r="B321" s="3" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="322" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37909,7 +37909,7 @@
         <v>529</v>
       </c>
       <c r="B322" s="3" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="323" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -37917,7 +37917,7 @@
         <v>530</v>
       </c>
       <c r="B323" s="3" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="324" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37925,7 +37925,7 @@
         <v>531</v>
       </c>
       <c r="B324" s="3" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="325" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37933,15 +37933,15 @@
         <v>532</v>
       </c>
       <c r="B325" s="3" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="326" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A326" s="2" t="s">
+        <v>1114</v>
+      </c>
+      <c r="B326" s="3" t="s">
         <v>1115</v>
-      </c>
-      <c r="B326" s="3" t="s">
-        <v>1116</v>
       </c>
     </row>
     <row r="327" spans="1:2" ht="390" x14ac:dyDescent="0.25">
@@ -37949,7 +37949,7 @@
         <v>178</v>
       </c>
       <c r="B327" s="3" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="328" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -37957,7 +37957,7 @@
         <v>500</v>
       </c>
       <c r="B328" s="3" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="329" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37965,7 +37965,7 @@
         <v>557</v>
       </c>
       <c r="B329" s="3" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="330" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37973,7 +37973,7 @@
         <v>558</v>
       </c>
       <c r="B330" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="331" spans="1:2" ht="315" x14ac:dyDescent="0.25">
@@ -37981,7 +37981,7 @@
         <v>179</v>
       </c>
       <c r="B331" s="3" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
     </row>
     <row r="332" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -37989,7 +37989,7 @@
         <v>249</v>
       </c>
       <c r="B332" s="3" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
     </row>
     <row r="333" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -37997,7 +37997,7 @@
         <v>250</v>
       </c>
       <c r="B333" s="3" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
     </row>
     <row r="334" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -38005,7 +38005,7 @@
         <v>251</v>
       </c>
       <c r="B334" s="3" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
     </row>
     <row r="335" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38013,7 +38013,7 @@
         <v>252</v>
       </c>
       <c r="B335" s="3" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="336" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -38021,23 +38021,23 @@
         <v>253</v>
       </c>
       <c r="B336" s="3" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
     </row>
     <row r="337" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A337" s="2" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="B337" s="3" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
     </row>
     <row r="338" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A338" s="2" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="B338" s="3" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
     </row>
     <row r="339" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -38045,7 +38045,7 @@
         <v>180</v>
       </c>
       <c r="B339" s="3" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="340" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38077,7 +38077,7 @@
         <v>183</v>
       </c>
       <c r="B343" s="3" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="344" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -38149,7 +38149,7 @@
         <v>461</v>
       </c>
       <c r="B352" s="3" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
     </row>
     <row r="353" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -38181,15 +38181,15 @@
         <v>192</v>
       </c>
       <c r="B356" s="3" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="357" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A357" s="2" t="s">
+        <v>626</v>
+      </c>
+      <c r="B357" s="3" t="s">
         <v>627</v>
-      </c>
-      <c r="B357" s="3" t="s">
-        <v>628</v>
       </c>
     </row>
     <row r="358" spans="1:2" ht="270" x14ac:dyDescent="0.25">
@@ -38197,7 +38197,7 @@
         <v>193</v>
       </c>
       <c r="B358" s="3" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="359" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -38213,7 +38213,7 @@
         <v>341</v>
       </c>
       <c r="B360" s="3" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="361" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -38221,7 +38221,7 @@
         <v>194</v>
       </c>
       <c r="B361" s="3" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
     </row>
     <row r="362" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -38229,7 +38229,7 @@
         <v>195</v>
       </c>
       <c r="B362" s="3" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
     </row>
     <row r="363" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -38237,7 +38237,7 @@
         <v>196</v>
       </c>
       <c r="B363" s="3" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
     </row>
     <row r="364" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -38245,7 +38245,7 @@
         <v>331</v>
       </c>
       <c r="B364" s="3" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
     </row>
     <row r="365" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -38253,15 +38253,15 @@
         <v>197</v>
       </c>
       <c r="B365" s="3" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="366" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A366" s="2" t="s">
+        <v>670</v>
+      </c>
+      <c r="B366" s="3" t="s">
         <v>671</v>
-      </c>
-      <c r="B366" s="3" t="s">
-        <v>672</v>
       </c>
     </row>
     <row r="367" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38269,7 +38269,7 @@
         <v>198</v>
       </c>
       <c r="B367" s="3" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
     </row>
     <row r="368" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38277,7 +38277,7 @@
         <v>199</v>
       </c>
       <c r="B368" s="3" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
     </row>
     <row r="369" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -38285,7 +38285,7 @@
         <v>200</v>
       </c>
       <c r="B369" s="3" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
     </row>
     <row r="370" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -38293,7 +38293,7 @@
         <v>201</v>
       </c>
       <c r="B370" s="3" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="371" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38301,7 +38301,7 @@
         <v>202</v>
       </c>
       <c r="B371" s="3" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="372" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -38309,47 +38309,47 @@
         <v>203</v>
       </c>
       <c r="B372" s="3" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
     </row>
     <row r="373" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A373" s="2" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="B373" s="3" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="374" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A374" s="2" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B374" s="3" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
     </row>
     <row r="375" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A375" s="2" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="B375" s="3" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="376" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A376" s="2" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="B376" s="3" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
     </row>
     <row r="377" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A377" s="2" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="B377" s="3" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="378" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -38357,55 +38357,55 @@
         <v>204</v>
       </c>
       <c r="B378" s="3" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="379" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A379" s="2" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="B379" s="3" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="380" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A380" s="2" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="B380" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="381" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A381" s="2" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="B381" s="3" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="382" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A382" s="2" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="B382" s="3" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
     </row>
     <row r="383" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A383" s="2" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="B383" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="384" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A384" s="2" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B384" s="3" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="385" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -38413,55 +38413,55 @@
         <v>205</v>
       </c>
       <c r="B385" s="3" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="386" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A386" s="2" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="B386" s="3" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="387" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A387" s="2" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="B387" s="3" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
     </row>
     <row r="388" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A388" s="2" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="B388" s="3" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
     </row>
     <row r="389" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A389" s="2" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="B389" s="3" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
     </row>
     <row r="390" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A390" s="2" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="B390" s="3" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="391" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A391" s="2" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="B391" s="3" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
     </row>
     <row r="392" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38469,7 +38469,7 @@
         <v>206</v>
       </c>
       <c r="B392" s="3" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="393" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -38477,7 +38477,7 @@
         <v>207</v>
       </c>
       <c r="B393" s="3" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="394" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -38485,7 +38485,7 @@
         <v>208</v>
       </c>
       <c r="B394" s="3" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="395" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -38493,55 +38493,55 @@
         <v>209</v>
       </c>
       <c r="B395" s="3" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
     </row>
     <row r="396" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A396" s="2" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="B396" s="3" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
     </row>
     <row r="397" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A397" s="2" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="B397" s="3" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="398" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A398" s="2" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="B398" s="3" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
     </row>
     <row r="399" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A399" s="2" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="B399" s="3" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="400" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A400" s="2" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="B400" s="4" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
     </row>
     <row r="401" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A401" s="2" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="B401" s="3" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
     </row>
     <row r="402" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -38549,63 +38549,63 @@
         <v>210</v>
       </c>
       <c r="B402" s="3" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="403" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A403" s="2" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="B403" s="3" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="404" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A404" s="2" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="B404" s="3" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
     </row>
     <row r="405" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A405" s="2" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="B405" s="3" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="406" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A406" s="2" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="B406" s="3" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="407" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A407" s="2" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="B407" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="408" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A408" s="2" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="B408" s="3" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
     <row r="409" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A409" s="2" t="s">
+        <v>648</v>
+      </c>
+      <c r="B409" s="3" t="s">
         <v>649</v>
-      </c>
-      <c r="B409" s="3" t="s">
-        <v>650</v>
       </c>
     </row>
     <row r="410" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -38613,7 +38613,7 @@
         <v>211</v>
       </c>
       <c r="B410" s="3" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="411" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -38661,7 +38661,7 @@
         <v>213</v>
       </c>
       <c r="B416" s="3" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
     </row>
     <row r="417" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -38669,7 +38669,7 @@
         <v>214</v>
       </c>
       <c r="B417" s="3" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
     </row>
     <row r="418" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -38677,7 +38677,7 @@
         <v>215</v>
       </c>
       <c r="B418" s="3" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="419" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38709,7 +38709,7 @@
         <v>219</v>
       </c>
       <c r="B422" s="3" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
     </row>
     <row r="423" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38717,7 +38717,7 @@
         <v>220</v>
       </c>
       <c r="B423" s="3" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
     </row>
     <row r="424" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -38725,7 +38725,7 @@
         <v>221</v>
       </c>
       <c r="B424" s="3" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="425" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -38733,7 +38733,7 @@
         <v>222</v>
       </c>
       <c r="B425" s="3" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="426" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -38741,7 +38741,7 @@
         <v>223</v>
       </c>
       <c r="B426" s="3" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="427" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -38749,7 +38749,7 @@
         <v>224</v>
       </c>
       <c r="B427" s="3" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="428" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -38757,7 +38757,7 @@
         <v>332</v>
       </c>
       <c r="B428" s="3" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="429" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -38773,7 +38773,7 @@
         <v>225</v>
       </c>
       <c r="B430" s="3" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
     </row>
     <row r="431" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -38837,7 +38837,7 @@
         <v>449</v>
       </c>
       <c r="B438" s="3" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="439" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -38845,31 +38845,31 @@
         <v>451</v>
       </c>
       <c r="B439" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="440" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A440" s="2" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="B440" s="3" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="441" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A441" s="2" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="B441" s="3" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
     </row>
     <row r="442" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A442" s="2" t="s">
+        <v>800</v>
+      </c>
+      <c r="B442" s="3" t="s">
         <v>801</v>
-      </c>
-      <c r="B442" s="3" t="s">
-        <v>802</v>
       </c>
     </row>
     <row r="443" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -38877,7 +38877,7 @@
         <v>319</v>
       </c>
       <c r="B443" s="3" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="444" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -38885,7 +38885,7 @@
         <v>320</v>
       </c>
       <c r="B444" s="3" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="445" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -38893,7 +38893,7 @@
         <v>321</v>
       </c>
       <c r="B445" s="3" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="446" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -38901,15 +38901,15 @@
         <v>318</v>
       </c>
       <c r="B446" s="3" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="447" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A447" s="2" t="s">
+        <v>1067</v>
+      </c>
+      <c r="B447" s="3" t="s">
         <v>1068</v>
-      </c>
-      <c r="B447" s="3" t="s">
-        <v>1069</v>
       </c>
     </row>
     <row r="448" spans="1:2" ht="255" x14ac:dyDescent="0.25">
@@ -38917,7 +38917,7 @@
         <v>322</v>
       </c>
       <c r="B448" s="3" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="449" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38981,7 +38981,7 @@
         <v>566</v>
       </c>
       <c r="B456" s="3" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="457" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -38997,7 +38997,7 @@
         <v>574</v>
       </c>
       <c r="B458" s="3" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
     </row>
     <row r="459" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39005,7 +39005,7 @@
         <v>575</v>
       </c>
       <c r="B459" s="3" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="460" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39029,7 +39029,7 @@
         <v>578</v>
       </c>
       <c r="B462" s="3" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="463" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -39037,7 +39037,7 @@
         <v>579</v>
       </c>
       <c r="B463" s="3" t="s">
-        <v>585</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="464" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -39045,7 +39045,7 @@
         <v>580</v>
       </c>
       <c r="B464" s="3" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="465" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -39053,7 +39053,7 @@
         <v>581</v>
       </c>
       <c r="B465" s="3" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="466" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -39061,215 +39061,215 @@
         <v>582</v>
       </c>
       <c r="B466" s="3" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="467" spans="1:2" ht="225" x14ac:dyDescent="0.25">
       <c r="A467" s="2" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="B467" s="3" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="468" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A468" s="2" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="B468" s="3" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
     </row>
     <row r="469" spans="1:2" ht="225" x14ac:dyDescent="0.25">
       <c r="A469" s="2" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="B469" s="3" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
     </row>
     <row r="470" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A470" s="2" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="B470" s="3" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
     </row>
     <row r="471" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A471" s="2" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="B471" s="3" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
     </row>
     <row r="472" spans="1:2" ht="225" x14ac:dyDescent="0.25">
       <c r="A472" s="2" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="B472" s="3" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
     </row>
     <row r="473" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A473" s="2" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="B473" s="3" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
     </row>
     <row r="474" spans="1:2" ht="255" x14ac:dyDescent="0.25">
       <c r="A474" s="2" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="B474" s="1" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
     </row>
     <row r="475" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A475" s="2" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="B475" s="1" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
     </row>
     <row r="476" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A476" s="2" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="B476" s="1" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="477" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A477" s="2" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="B477" s="1" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="478" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A478" s="2" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="B478" s="1" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="479" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A479" s="2" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="B479" s="1" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
     </row>
     <row r="480" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A480" s="2" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="B480" s="1" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
     </row>
     <row r="481" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A481" s="2" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="B481" s="1" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="482" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A482" s="2" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="B482" s="1" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="483" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A483" s="2" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="B483" s="1" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
     </row>
     <row r="484" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A484" s="2" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="B484" s="1" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
     </row>
     <row r="485" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A485" s="2" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="B485" s="1" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
     </row>
     <row r="486" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A486" s="2" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="B486" s="1" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
     </row>
     <row r="487" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A487" s="2" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="B487" s="1" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
     </row>
     <row r="488" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A488" s="2" t="s">
+        <v>699</v>
+      </c>
+      <c r="B488" s="1" t="s">
         <v>700</v>
-      </c>
-      <c r="B488" s="1" t="s">
-        <v>701</v>
       </c>
     </row>
     <row r="489" spans="1:2" ht="255" x14ac:dyDescent="0.25">
       <c r="A489" s="2" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="B489" s="1" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="490" spans="1:2" ht="92.25" x14ac:dyDescent="0.25">
       <c r="A490" s="2" t="s">
+        <v>1047</v>
+      </c>
+      <c r="B490" s="1" t="s">
         <v>1048</v>
-      </c>
-      <c r="B490" s="1" t="s">
-        <v>1049</v>
       </c>
     </row>
     <row r="491" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A491" s="2" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="B491" s="1" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
     </row>
     <row r="492" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A492" s="2" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="B492" s="3" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="493" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -39277,7 +39277,7 @@
         <v>552</v>
       </c>
       <c r="B493" s="3" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
     </row>
     <row r="494" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -39285,7 +39285,7 @@
         <v>553</v>
       </c>
       <c r="B494" s="3" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
     </row>
     <row r="495" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -39293,7 +39293,7 @@
         <v>554</v>
       </c>
       <c r="B495" s="3" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
     </row>
     <row r="496" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39365,7 +39365,7 @@
         <v>275</v>
       </c>
       <c r="B504" s="1" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="505" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39373,7 +39373,7 @@
         <v>276</v>
       </c>
       <c r="B505" s="1" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="506" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39381,7 +39381,7 @@
         <v>277</v>
       </c>
       <c r="B506" s="1" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="507" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -39429,7 +39429,7 @@
         <v>260</v>
       </c>
       <c r="B512" s="3" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="513" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39437,7 +39437,7 @@
         <v>480</v>
       </c>
       <c r="B513" s="3" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
     </row>
     <row r="514" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -39445,15 +39445,15 @@
         <v>481</v>
       </c>
       <c r="B514" s="1" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
     </row>
     <row r="515" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A515" s="2" t="s">
+        <v>808</v>
+      </c>
+      <c r="B515" s="3" t="s">
         <v>809</v>
-      </c>
-      <c r="B515" s="3" t="s">
-        <v>810</v>
       </c>
     </row>
     <row r="516" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39501,7 +39501,7 @@
         <v>285</v>
       </c>
       <c r="B521" s="1" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
     </row>
     <row r="522" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -39509,7 +39509,7 @@
         <v>286</v>
       </c>
       <c r="B522" s="1" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
     </row>
     <row r="523" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -39589,7 +39589,7 @@
         <v>296</v>
       </c>
       <c r="B532" s="1" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
     </row>
     <row r="533" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -39597,7 +39597,7 @@
         <v>297</v>
       </c>
       <c r="B533" s="1" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
     </row>
     <row r="534" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -39629,7 +39629,7 @@
         <v>298</v>
       </c>
       <c r="B537" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
     </row>
     <row r="538" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -39645,7 +39645,7 @@
         <v>299</v>
       </c>
       <c r="B539" s="1" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
     </row>
     <row r="540" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -39669,7 +39669,7 @@
         <v>300</v>
       </c>
       <c r="B542" s="1" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
     </row>
     <row r="543" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -39677,7 +39677,7 @@
         <v>301</v>
       </c>
       <c r="B543" s="1" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
     </row>
     <row r="544" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -39717,7 +39717,7 @@
         <v>396</v>
       </c>
       <c r="B548" s="1" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
     </row>
     <row r="549" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -39730,10 +39730,10 @@
     </row>
     <row r="550" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A550" s="2" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="B550" s="1" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
     </row>
     <row r="551" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -39741,7 +39741,7 @@
         <v>305</v>
       </c>
       <c r="B551" s="1" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="552" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -39770,10 +39770,10 @@
     </row>
     <row r="555" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A555" s="2" t="s">
+        <v>748</v>
+      </c>
+      <c r="B555" s="1" t="s">
         <v>749</v>
-      </c>
-      <c r="B555" s="1" t="s">
-        <v>750</v>
       </c>
     </row>
     <row r="556" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -39781,7 +39781,7 @@
         <v>306</v>
       </c>
       <c r="B556" s="1" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
     </row>
     <row r="557" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -39805,7 +39805,7 @@
         <v>307</v>
       </c>
       <c r="B559" s="1" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="560" spans="1:2" ht="375" x14ac:dyDescent="0.25">
@@ -39813,7 +39813,7 @@
         <v>311</v>
       </c>
       <c r="B560" s="1" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
     </row>
     <row r="561" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39837,15 +39837,15 @@
         <v>376</v>
       </c>
       <c r="B563" s="3" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="564" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A564" s="2" t="s">
+        <v>752</v>
+      </c>
+      <c r="B564" s="3" t="s">
         <v>753</v>
-      </c>
-      <c r="B564" s="3" t="s">
-        <v>754</v>
       </c>
     </row>
     <row r="565" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -39853,7 +39853,7 @@
         <v>329</v>
       </c>
       <c r="B565" s="3" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Started adding path details
</commit_message>
<xml_diff>
--- a/Documentation/Events.xlsx
+++ b/Documentation/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\happysulla\BarbarianPrince\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9B4D98F4-CE59-46A7-9B42-6CCD61243726}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{93AB987B-673F-4C1D-96B8-0DAF39C11289}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -9666,59 +9666,6 @@
   </si>
   <si>
     <r>
-      <t>&lt;Bold&gt;e209h Buy Valuable Information&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;If you buy it, roll one die:  &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>dieRoll</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.gif' Name='</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>DieRoll</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>' Height='21' Width='21'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt; 
-&lt;LineBreak/&gt;   1 - Bogus secrets prove worthless
-&lt;LineBreak/&gt;   2 - &lt;InlineUIContainer&gt;&lt;Button Content='e147' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;   3 - &lt;InlineUIContainer&gt;&lt;Button Content='e143' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;   4 - &lt;InlineUIContainer&gt;&lt;Button Content='e144' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;   5 - &lt;InlineUIContainer&gt;&lt;Button Content='e145' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;   6 - &lt;InlineUIContainer&gt;&lt;Button Content='e146' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>&lt;Bold&gt;e016 Magician's Home&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;You spot a magician home. Choose the approach strategy.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
@@ -33923,56 +33870,6 @@
   </si>
   <si>
     <r>
-      <t>&lt;Bold&gt;e134 Unstable Ruins&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;In the ruins are many unstable walls and rocks making your search very dangerous. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Image Name='ShakeyWallsEnd' Source='../../Images/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Campfire2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.gif' Height='75'  Width='75'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;Click the campfire to abandon search.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Image Name='ShakeyWalls' Source='../../Images/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ShakyWalls</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">.gif' Height='75'  Width='75'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt; Click the shaking walls to continue. </t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>&lt;Bold&gt;e208 Searching a Ruin&lt;/Bold&gt; &lt;InlineUIContainer&gt;&lt;Button Content='r208' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;Spend the day searching a ruins with your party. To see what happens during the search, roll two dice:
  &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
@@ -34880,6 +34777,171 @@
         <scheme val="minor"/>
       </rPr>
       <t>.gif' Height='250'  Width='500'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;Bold&gt;e134 Unstable Ruins&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;In the ruins are many unstable walls and rocks making your search very dangerous. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Image Name='ShakeyWallsEnd' Source='../../Images/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Campfire2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.gif' Height='75'  Width='75'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;Click the campfire to abandon search.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Image Name='</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ShakeyWalls</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>' Source='../../Images/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ShakyWalls</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">.gif' Height='75'  Width='75'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt; Click the shaking walls to continue. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;Bold&gt;e209h Buy Valuable Information&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;If you buy it, roll one die:  &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dieRoll</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.gif' Name='</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DieRoll</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>' Height='21' Width='21'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt; 
+&lt;LineBreak/&gt;   1 - Bogus secrets prove worthless
+&lt;LineBreak/&gt;   2 - &lt;InlineUIContainer&gt;&lt;Button Content='e147' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;   3 - &lt;InlineUIContainer&gt;&lt;Button Content='e143' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;   4 - &lt;InlineUIContainer&gt;&lt;Button Content='e144' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;   5 - &lt;InlineUIContainer&gt;&lt;Button Content='e145' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;   6 - &lt;InlineUIContainer&gt;&lt;Button Content='e146' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;&lt;InlineUIContainer&gt;
+                                      &lt;InlineUIContainer&gt;&lt;Image Name='</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>BuyInfoEnd</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>' Source='../../Images/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Nothing</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.gif' Height='150' Width='150'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
     </r>
   </si>
 </sst>
@@ -35346,8 +35408,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B565"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A341" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B343" sqref="B343"/>
+    <sheetView tabSelected="1" topLeftCell="A456" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B457" sqref="B457"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -35361,7 +35423,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -35369,7 +35431,7 @@
         <v>254</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -35377,7 +35439,7 @@
         <v>255</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -35385,15 +35447,15 @@
         <v>256</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="390" x14ac:dyDescent="0.25">
@@ -35409,7 +35471,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35417,7 +35479,7 @@
         <v>22</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35449,7 +35511,7 @@
         <v>3</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -35457,7 +35519,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35465,7 +35527,7 @@
         <v>5</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35473,7 +35535,7 @@
         <v>6</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -35481,7 +35543,7 @@
         <v>7</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -35489,7 +35551,7 @@
         <v>8</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35497,7 +35559,7 @@
         <v>10</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35505,7 +35567,7 @@
         <v>9</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -35513,7 +35575,7 @@
         <v>11</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -35521,7 +35583,7 @@
         <v>12</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35529,7 +35591,7 @@
         <v>13</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35537,7 +35599,7 @@
         <v>14</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -35545,7 +35607,7 @@
         <v>15</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -35553,7 +35615,7 @@
         <v>16</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -35561,7 +35623,7 @@
         <v>17</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -35569,7 +35631,7 @@
         <v>18</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -35577,31 +35639,31 @@
         <v>261</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -35609,7 +35671,7 @@
         <v>19</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -35617,7 +35679,7 @@
         <v>20</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -35625,23 +35687,23 @@
         <v>21</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -35649,23 +35711,23 @@
         <v>25</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -35673,7 +35735,7 @@
         <v>26</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -35697,7 +35759,7 @@
         <v>27</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -35713,7 +35775,7 @@
         <v>29</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -35721,7 +35783,7 @@
         <v>30</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -35734,10 +35796,10 @@
     </row>
     <row r="48" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -35745,7 +35807,7 @@
         <v>31</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -35753,7 +35815,7 @@
         <v>32</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -35761,7 +35823,7 @@
         <v>33</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -35793,7 +35855,7 @@
         <v>501</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>1128</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -35817,7 +35879,7 @@
         <v>264</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35825,7 +35887,7 @@
         <v>265</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -35841,7 +35903,7 @@
         <v>563</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -35849,7 +35911,7 @@
         <v>35</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -35881,7 +35943,7 @@
         <v>37</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="285" x14ac:dyDescent="0.25">
@@ -35889,7 +35951,7 @@
         <v>38</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -35897,7 +35959,7 @@
         <v>43</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35905,23 +35967,23 @@
         <v>44</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
+        <v>720</v>
+      </c>
+      <c r="B71" s="3" t="s">
         <v>721</v>
-      </c>
-      <c r="B71" s="3" t="s">
-        <v>722</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35929,7 +35991,7 @@
         <v>39</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -35961,7 +36023,7 @@
         <v>42</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35969,7 +36031,7 @@
         <v>46</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -35993,7 +36055,7 @@
         <v>49</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -36033,7 +36095,7 @@
         <v>54</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -36041,7 +36103,7 @@
         <v>55</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -36049,7 +36111,7 @@
         <v>56</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -36057,7 +36119,7 @@
         <v>57</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -36065,31 +36127,31 @@
         <v>58</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
+        <v>801</v>
+      </c>
+      <c r="B92" s="3" t="s">
         <v>802</v>
-      </c>
-      <c r="B92" s="3" t="s">
-        <v>803</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -36097,15 +36159,15 @@
         <v>59</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
+        <v>916</v>
+      </c>
+      <c r="B94" s="3" t="s">
         <v>917</v>
-      </c>
-      <c r="B94" s="3" t="s">
-        <v>918</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -36113,15 +36175,15 @@
         <v>60</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>1124</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -36129,7 +36191,7 @@
         <v>61</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -36137,7 +36199,7 @@
         <v>62</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -36169,7 +36231,7 @@
         <v>65</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -36177,7 +36239,7 @@
         <v>66</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -36257,7 +36319,7 @@
         <v>70</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -36289,7 +36351,7 @@
         <v>72</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
     </row>
     <row r="118" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -36297,7 +36359,7 @@
         <v>73</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="119" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -36345,7 +36407,7 @@
         <v>77</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
     </row>
     <row r="125" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -36358,10 +36420,10 @@
     </row>
     <row r="126" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
+        <v>968</v>
+      </c>
+      <c r="B126" s="3" t="s">
         <v>969</v>
-      </c>
-      <c r="B126" s="3" t="s">
-        <v>970</v>
       </c>
     </row>
     <row r="127" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -36369,7 +36431,7 @@
         <v>78</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
     </row>
     <row r="128" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -36377,7 +36439,7 @@
         <v>377</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
     </row>
     <row r="129" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -36417,7 +36479,7 @@
         <v>80</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
     </row>
     <row r="134" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -36425,87 +36487,87 @@
         <v>81</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
     </row>
     <row r="135" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
     </row>
     <row r="136" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
     </row>
     <row r="137" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
     </row>
     <row r="138" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="139" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="B139" s="3" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
     </row>
     <row r="140" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
     </row>
     <row r="141" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
     </row>
     <row r="142" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
     </row>
     <row r="143" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
+        <v>984</v>
+      </c>
+      <c r="B143" s="3" t="s">
         <v>985</v>
-      </c>
-      <c r="B143" s="3" t="s">
-        <v>986</v>
       </c>
     </row>
     <row r="144" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
     </row>
     <row r="145" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -36513,7 +36575,7 @@
         <v>82</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
     </row>
     <row r="146" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -36521,12 +36583,12 @@
         <v>83</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
     </row>
     <row r="147" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
-        <v>1125</v>
+        <v>1123</v>
       </c>
       <c r="B147" s="3" t="s">
         <v>559</v>
@@ -36561,7 +36623,7 @@
         <v>558</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
     </row>
     <row r="152" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -36569,7 +36631,7 @@
         <v>86</v>
       </c>
       <c r="B152" s="3" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="153" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -36625,7 +36687,7 @@
         <v>346</v>
       </c>
       <c r="B159" s="3" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="160" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -36633,7 +36695,7 @@
         <v>348</v>
       </c>
       <c r="B160" s="3" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="161" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -36662,10 +36724,10 @@
     </row>
     <row r="164" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
+        <v>729</v>
+      </c>
+      <c r="B164" s="3" t="s">
         <v>730</v>
-      </c>
-      <c r="B164" s="3" t="s">
-        <v>731</v>
       </c>
     </row>
     <row r="165" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -36681,7 +36743,7 @@
         <v>445</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
     </row>
     <row r="167" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -36705,23 +36767,23 @@
         <v>90</v>
       </c>
       <c r="B169" s="3" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
     <row r="170" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="B170" s="3" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
     </row>
     <row r="171" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="B171" s="3" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
     </row>
     <row r="172" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -36753,7 +36815,7 @@
         <v>93</v>
       </c>
       <c r="B175" s="3" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
     </row>
     <row r="176" spans="1:2" ht="270" x14ac:dyDescent="0.25">
@@ -36761,7 +36823,7 @@
         <v>94</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
     </row>
     <row r="177" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -36769,7 +36831,7 @@
         <v>95</v>
       </c>
       <c r="B177" s="3" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
     </row>
     <row r="178" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -36777,55 +36839,55 @@
         <v>96</v>
       </c>
       <c r="B178" s="3" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
     </row>
     <row r="179" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A179" s="2" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="B179" s="3" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="180" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A180" s="2" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="B180" s="3" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
     </row>
     <row r="181" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
     </row>
     <row r="182" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="B182" s="3" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
     </row>
     <row r="183" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="B183" s="3" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="184" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A184" s="2" t="s">
+        <v>887</v>
+      </c>
+      <c r="B184" s="3" t="s">
         <v>888</v>
-      </c>
-      <c r="B184" s="3" t="s">
-        <v>889</v>
       </c>
     </row>
     <row r="185" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -36833,7 +36895,7 @@
         <v>97</v>
       </c>
       <c r="B185" s="3" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
     </row>
     <row r="186" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -36841,7 +36903,7 @@
         <v>98</v>
       </c>
       <c r="B186" s="3" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="187" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -36849,7 +36911,7 @@
         <v>99</v>
       </c>
       <c r="B187" s="3" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="188" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -36865,7 +36927,7 @@
         <v>100</v>
       </c>
       <c r="B189" s="3" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
     </row>
     <row r="190" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -36873,7 +36935,7 @@
         <v>102</v>
       </c>
       <c r="B190" s="3" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="191" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -36881,7 +36943,7 @@
         <v>103</v>
       </c>
       <c r="B191" s="3" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="192" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -36889,7 +36951,7 @@
         <v>104</v>
       </c>
       <c r="B192" s="3" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
     </row>
     <row r="193" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -36897,23 +36959,23 @@
         <v>105</v>
       </c>
       <c r="B193" s="3" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="194" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A194" s="2" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="B194" s="3" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="195" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A195" s="2" t="s">
+        <v>702</v>
+      </c>
+      <c r="B195" s="3" t="s">
         <v>703</v>
-      </c>
-      <c r="B195" s="3" t="s">
-        <v>704</v>
       </c>
     </row>
     <row r="196" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -36921,7 +36983,7 @@
         <v>106</v>
       </c>
       <c r="B196" s="3" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
     </row>
     <row r="197" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -36929,7 +36991,7 @@
         <v>107</v>
       </c>
       <c r="B197" s="3" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
     </row>
     <row r="198" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -36937,15 +36999,15 @@
         <v>165</v>
       </c>
       <c r="B198" s="3" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
     </row>
     <row r="199" spans="1:2" ht="225" x14ac:dyDescent="0.25">
       <c r="A199" s="2" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="B199" s="3" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
     </row>
     <row r="200" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -36953,7 +37015,7 @@
         <v>108</v>
       </c>
       <c r="B200" s="3" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="201" spans="1:2" ht="285" x14ac:dyDescent="0.25">
@@ -36961,7 +37023,7 @@
         <v>109</v>
       </c>
       <c r="B201" s="3" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
     </row>
     <row r="202" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -36969,7 +37031,7 @@
         <v>110</v>
       </c>
       <c r="B202" s="3" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
     </row>
     <row r="203" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -36977,7 +37039,7 @@
         <v>166</v>
       </c>
       <c r="B203" s="3" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="204" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -36985,7 +37047,7 @@
         <v>167</v>
       </c>
       <c r="B204" s="3" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="205" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -36993,23 +37055,23 @@
         <v>168</v>
       </c>
       <c r="B205" s="3" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
     </row>
     <row r="206" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A206" s="2" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="B206" s="3" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
     </row>
     <row r="207" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A207" s="2" t="s">
+        <v>902</v>
+      </c>
+      <c r="B207" s="3" t="s">
         <v>903</v>
-      </c>
-      <c r="B207" s="3" t="s">
-        <v>904</v>
       </c>
     </row>
     <row r="208" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37017,39 +37079,39 @@
         <v>111</v>
       </c>
       <c r="B208" s="3" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
     </row>
     <row r="209" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A209" s="2" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="B209" s="3" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
     </row>
     <row r="210" spans="1:2" ht="225" x14ac:dyDescent="0.25">
       <c r="A210" s="2" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="B210" s="3" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
     </row>
     <row r="211" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A211" s="2" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="B211" s="3" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
     </row>
     <row r="212" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A212" s="2" t="s">
+        <v>737</v>
+      </c>
+      <c r="B212" s="3" t="s">
         <v>738</v>
-      </c>
-      <c r="B212" s="3" t="s">
-        <v>739</v>
       </c>
     </row>
     <row r="213" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37057,7 +37119,7 @@
         <v>112</v>
       </c>
       <c r="B213" s="3" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="214" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37065,7 +37127,7 @@
         <v>169</v>
       </c>
       <c r="B214" s="3" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
     </row>
     <row r="215" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -37073,7 +37135,7 @@
         <v>170</v>
       </c>
       <c r="B215" s="3" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="216" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -37081,7 +37143,7 @@
         <v>171</v>
       </c>
       <c r="B216" s="3" t="s">
-        <v>1117</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="217" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37089,7 +37151,7 @@
         <v>113</v>
       </c>
       <c r="B217" s="3" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="218" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -37097,7 +37159,7 @@
         <v>114</v>
       </c>
       <c r="B218" s="3" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
     </row>
     <row r="219" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -37105,15 +37167,15 @@
         <v>266</v>
       </c>
       <c r="B219" s="3" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
     </row>
     <row r="220" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A220" s="2" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="B220" s="3" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
     </row>
     <row r="221" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37121,15 +37183,15 @@
         <v>115</v>
       </c>
       <c r="B221" s="3" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
     </row>
     <row r="222" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A222" s="2" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="B222" s="3" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
     </row>
     <row r="223" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37137,15 +37199,15 @@
         <v>116</v>
       </c>
       <c r="B223" s="3" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="224" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A224" s="2" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="B224" s="3" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
     </row>
     <row r="225" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -37153,31 +37215,31 @@
         <v>117</v>
       </c>
       <c r="B225" s="4" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
     </row>
     <row r="226" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A226" s="2" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="B226" s="4" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
     </row>
     <row r="227" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A227" s="2" t="s">
+        <v>761</v>
+      </c>
+      <c r="B227" s="4" t="s">
         <v>762</v>
-      </c>
-      <c r="B227" s="4" t="s">
-        <v>763</v>
       </c>
     </row>
     <row r="228" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A228" s="2" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="B228" s="4" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
     </row>
     <row r="229" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -37185,23 +37247,23 @@
         <v>118</v>
       </c>
       <c r="B229" s="3" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
     </row>
     <row r="230" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A230" s="2" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="B230" s="3" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
     </row>
     <row r="231" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A231" s="2" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="B231" s="3" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="232" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -37209,23 +37271,23 @@
         <v>119</v>
       </c>
       <c r="B232" s="3" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="233" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A233" s="2" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="B233" s="3" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
     </row>
     <row r="234" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A234" s="2" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="B234" s="3" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
     </row>
     <row r="235" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -37233,7 +37295,7 @@
         <v>120</v>
       </c>
       <c r="B235" s="3" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
     </row>
     <row r="236" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -37241,7 +37303,7 @@
         <v>172</v>
       </c>
       <c r="B236" s="3" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
     </row>
     <row r="237" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37249,7 +37311,7 @@
         <v>173</v>
       </c>
       <c r="B237" s="3" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
     </row>
     <row r="238" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37257,7 +37319,7 @@
         <v>174</v>
       </c>
       <c r="B238" s="3" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
     </row>
     <row r="239" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37273,15 +37335,15 @@
         <v>122</v>
       </c>
       <c r="B240" s="3" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="241" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A241" s="2" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="B241" s="3" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="242" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -37289,23 +37351,23 @@
         <v>123</v>
       </c>
       <c r="B242" s="3" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
     </row>
     <row r="243" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A243" s="2" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="B243" s="3" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
     </row>
     <row r="244" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A244" s="2" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="B244" s="3" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
     </row>
     <row r="245" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37313,7 +37375,7 @@
         <v>124</v>
       </c>
       <c r="B245" s="3" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
     </row>
     <row r="246" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37321,15 +37383,15 @@
         <v>125</v>
       </c>
       <c r="B246" s="3" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="247" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A247" s="2" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="B247" s="3" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="248" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37337,7 +37399,7 @@
         <v>126</v>
       </c>
       <c r="B248" s="3" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="249" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37345,7 +37407,7 @@
         <v>127</v>
       </c>
       <c r="B249" s="3" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
     </row>
     <row r="250" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37353,7 +37415,7 @@
         <v>128</v>
       </c>
       <c r="B250" s="3" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
     </row>
     <row r="251" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -37361,7 +37423,7 @@
         <v>129</v>
       </c>
       <c r="B251" s="3" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="252" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37369,7 +37431,7 @@
         <v>130</v>
       </c>
       <c r="B252" s="3" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
     </row>
     <row r="253" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -37377,23 +37439,23 @@
         <v>131</v>
       </c>
       <c r="B253" s="3" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
     </row>
     <row r="254" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A254" s="2" t="s">
+        <v>958</v>
+      </c>
+      <c r="B254" s="3" t="s">
         <v>959</v>
-      </c>
-      <c r="B254" s="3" t="s">
-        <v>960</v>
       </c>
     </row>
     <row r="255" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A255" s="2" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="B255" s="3" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
     </row>
     <row r="256" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -37401,7 +37463,7 @@
         <v>132</v>
       </c>
       <c r="B256" s="3" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="257" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -37409,15 +37471,15 @@
         <v>133</v>
       </c>
       <c r="B257" s="3" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="258" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A258" s="2" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="B258" s="3" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="259" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37425,23 +37487,23 @@
         <v>134</v>
       </c>
       <c r="B259" s="3" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="260" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A260" s="2" t="s">
+        <v>1013</v>
+      </c>
+      <c r="B260" s="3" t="s">
         <v>1014</v>
-      </c>
-      <c r="B260" s="3" t="s">
-        <v>1015</v>
       </c>
     </row>
     <row r="261" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A261" s="2" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B261" s="3" t="s">
         <v>1016</v>
-      </c>
-      <c r="B261" s="3" t="s">
-        <v>1017</v>
       </c>
     </row>
     <row r="262" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -37449,15 +37511,15 @@
         <v>135</v>
       </c>
       <c r="B262" s="3" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="263" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A263" s="2" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B263" s="3" t="s">
         <v>1019</v>
-      </c>
-      <c r="B263" s="3" t="s">
-        <v>1020</v>
       </c>
     </row>
     <row r="264" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -37465,7 +37527,7 @@
         <v>136</v>
       </c>
       <c r="B264" s="3" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="265" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -37489,7 +37551,7 @@
         <v>233</v>
       </c>
       <c r="B267" s="3" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
     </row>
     <row r="268" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -37497,7 +37559,7 @@
         <v>138</v>
       </c>
       <c r="B268" s="3" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="269" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37505,7 +37567,7 @@
         <v>234</v>
       </c>
       <c r="B269" s="3" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
     </row>
     <row r="270" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37513,7 +37575,7 @@
         <v>235</v>
       </c>
       <c r="B270" s="3" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
     </row>
     <row r="271" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -37521,7 +37583,7 @@
         <v>139</v>
       </c>
       <c r="B271" s="3" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
     </row>
     <row r="272" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -37529,7 +37591,7 @@
         <v>239</v>
       </c>
       <c r="B272" s="3" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="273" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37537,7 +37599,7 @@
         <v>240</v>
       </c>
       <c r="B273" s="3" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="274" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37545,7 +37607,7 @@
         <v>241</v>
       </c>
       <c r="B274" s="3" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
     </row>
     <row r="275" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37553,7 +37615,7 @@
         <v>140</v>
       </c>
       <c r="B275" s="3" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="276" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -37561,7 +37623,7 @@
         <v>236</v>
       </c>
       <c r="B276" s="3" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="277" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37569,7 +37631,7 @@
         <v>237</v>
       </c>
       <c r="B277" s="3" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="278" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37577,7 +37639,7 @@
         <v>238</v>
       </c>
       <c r="B278" s="3" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="279" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -37585,7 +37647,7 @@
         <v>141</v>
       </c>
       <c r="B279" s="3" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="280" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -37593,7 +37655,7 @@
         <v>142</v>
       </c>
       <c r="B280" s="3" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="281" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -37601,7 +37663,7 @@
         <v>143</v>
       </c>
       <c r="B281" s="3" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="282" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -37609,7 +37671,7 @@
         <v>144</v>
       </c>
       <c r="B282" s="3" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="283" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -37617,7 +37679,7 @@
         <v>242</v>
       </c>
       <c r="B283" s="3" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="284" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37625,7 +37687,7 @@
         <v>145</v>
       </c>
       <c r="B284" s="3" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="285" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -37633,7 +37695,7 @@
         <v>146</v>
       </c>
       <c r="B285" s="3" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="286" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37641,7 +37703,7 @@
         <v>147</v>
       </c>
       <c r="B286" s="3" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="287" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -37649,7 +37711,7 @@
         <v>148</v>
       </c>
       <c r="B287" s="3" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="288" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -37657,31 +37719,31 @@
         <v>149</v>
       </c>
       <c r="B288" s="3" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="289" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A289" s="2" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="B289" s="3" t="s">
-        <v>1118</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="290" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A290" s="2" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="B290" s="3" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="291" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A291" s="2" t="s">
+        <v>1089</v>
+      </c>
+      <c r="B291" s="3" t="s">
         <v>1090</v>
-      </c>
-      <c r="B291" s="3" t="s">
-        <v>1091</v>
       </c>
     </row>
     <row r="292" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37689,15 +37751,15 @@
         <v>150</v>
       </c>
       <c r="B292" s="3" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="293" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A293" s="2" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="B293" s="3" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="294" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -37705,7 +37767,7 @@
         <v>151</v>
       </c>
       <c r="B294" s="3" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="295" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37713,7 +37775,7 @@
         <v>243</v>
       </c>
       <c r="B295" s="3" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
     </row>
     <row r="296" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37721,7 +37783,7 @@
         <v>244</v>
       </c>
       <c r="B296" s="3" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="297" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37729,7 +37791,7 @@
         <v>245</v>
       </c>
       <c r="B297" s="3" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
     </row>
     <row r="298" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37737,7 +37799,7 @@
         <v>152</v>
       </c>
       <c r="B298" s="3" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
     </row>
     <row r="299" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -37745,7 +37807,7 @@
         <v>153</v>
       </c>
       <c r="B299" s="3" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="300" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37753,7 +37815,7 @@
         <v>154</v>
       </c>
       <c r="B300" s="3" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
     </row>
     <row r="301" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -37761,7 +37823,7 @@
         <v>155</v>
       </c>
       <c r="B301" s="3" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="302" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37769,7 +37831,7 @@
         <v>156</v>
       </c>
       <c r="B302" s="3" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
     </row>
     <row r="303" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -37777,7 +37839,7 @@
         <v>157</v>
       </c>
       <c r="B303" s="3" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
     </row>
     <row r="304" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -37785,7 +37847,7 @@
         <v>246</v>
       </c>
       <c r="B304" s="3" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
     </row>
     <row r="305" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37793,7 +37855,7 @@
         <v>247</v>
       </c>
       <c r="B305" s="3" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
     </row>
     <row r="306" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37801,7 +37863,7 @@
         <v>248</v>
       </c>
       <c r="B306" s="3" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
     </row>
     <row r="307" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37809,7 +37871,7 @@
         <v>158</v>
       </c>
       <c r="B307" s="3" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
     </row>
     <row r="308" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -37817,7 +37879,7 @@
         <v>159</v>
       </c>
       <c r="B308" s="3" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
     </row>
     <row r="309" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37825,7 +37887,7 @@
         <v>160</v>
       </c>
       <c r="B309" s="3" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="310" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -37833,7 +37895,7 @@
         <v>161</v>
       </c>
       <c r="B310" s="3" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="311" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37841,31 +37903,31 @@
         <v>162</v>
       </c>
       <c r="B311" s="3" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="312" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A312" s="2" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="B312" s="3" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="313" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A313" s="2" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="B313" s="3" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="314" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A314" s="2" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="B314" s="3" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="315" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37873,7 +37935,7 @@
         <v>163</v>
       </c>
       <c r="B315" s="3" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="316" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -37881,7 +37943,7 @@
         <v>164</v>
       </c>
       <c r="B316" s="3" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="317" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37889,7 +37951,7 @@
         <v>175</v>
       </c>
       <c r="B317" s="3" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="318" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -37897,7 +37959,7 @@
         <v>176</v>
       </c>
       <c r="B318" s="3" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="319" spans="1:2" ht="390" x14ac:dyDescent="0.25">
@@ -37905,7 +37967,7 @@
         <v>177</v>
       </c>
       <c r="B319" s="3" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="320" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -37913,7 +37975,7 @@
         <v>525</v>
       </c>
       <c r="B320" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="321" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37921,7 +37983,7 @@
         <v>526</v>
       </c>
       <c r="B321" s="3" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="322" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37929,7 +37991,7 @@
         <v>527</v>
       </c>
       <c r="B322" s="3" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="323" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -37937,7 +37999,7 @@
         <v>528</v>
       </c>
       <c r="B323" s="3" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="324" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37945,7 +38007,7 @@
         <v>529</v>
       </c>
       <c r="B324" s="3" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="325" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37953,15 +38015,15 @@
         <v>530</v>
       </c>
       <c r="B325" s="3" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="326" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A326" s="2" t="s">
+        <v>1111</v>
+      </c>
+      <c r="B326" s="3" t="s">
         <v>1112</v>
-      </c>
-      <c r="B326" s="3" t="s">
-        <v>1113</v>
       </c>
     </row>
     <row r="327" spans="1:2" ht="390" x14ac:dyDescent="0.25">
@@ -37969,7 +38031,7 @@
         <v>178</v>
       </c>
       <c r="B327" s="3" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="328" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -37977,7 +38039,7 @@
         <v>499</v>
       </c>
       <c r="B328" s="3" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="329" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37985,7 +38047,7 @@
         <v>555</v>
       </c>
       <c r="B329" s="3" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="330" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37993,7 +38055,7 @@
         <v>556</v>
       </c>
       <c r="B330" s="3" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="331" spans="1:2" ht="315" x14ac:dyDescent="0.25">
@@ -38001,7 +38063,7 @@
         <v>179</v>
       </c>
       <c r="B331" s="3" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
     </row>
     <row r="332" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -38009,7 +38071,7 @@
         <v>249</v>
       </c>
       <c r="B332" s="3" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
     </row>
     <row r="333" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -38017,7 +38079,7 @@
         <v>250</v>
       </c>
       <c r="B333" s="3" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
     </row>
     <row r="334" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -38025,7 +38087,7 @@
         <v>251</v>
       </c>
       <c r="B334" s="3" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
     </row>
     <row r="335" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38033,7 +38095,7 @@
         <v>252</v>
       </c>
       <c r="B335" s="3" t="s">
-        <v>1126</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="336" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -38041,23 +38103,23 @@
         <v>253</v>
       </c>
       <c r="B336" s="3" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
     </row>
     <row r="337" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A337" s="2" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="B337" s="3" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
     </row>
     <row r="338" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A338" s="2" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="B338" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="339" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -38065,7 +38127,7 @@
         <v>180</v>
       </c>
       <c r="B339" s="3" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="340" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38097,7 +38159,7 @@
         <v>183</v>
       </c>
       <c r="B343" s="3" t="s">
-        <v>1115</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="344" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -38105,7 +38167,7 @@
         <v>184</v>
       </c>
       <c r="B344" s="3" t="s">
-        <v>1129</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="345" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -38169,7 +38231,7 @@
         <v>461</v>
       </c>
       <c r="B352" s="3" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
     </row>
     <row r="353" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -38201,15 +38263,15 @@
         <v>192</v>
       </c>
       <c r="B356" s="3" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="357" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A357" s="2" t="s">
+        <v>623</v>
+      </c>
+      <c r="B357" s="3" t="s">
         <v>624</v>
-      </c>
-      <c r="B357" s="3" t="s">
-        <v>625</v>
       </c>
     </row>
     <row r="358" spans="1:2" ht="270" x14ac:dyDescent="0.25">
@@ -38217,7 +38279,7 @@
         <v>193</v>
       </c>
       <c r="B358" s="3" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
     </row>
     <row r="359" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -38233,7 +38295,7 @@
         <v>341</v>
       </c>
       <c r="B360" s="3" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
     </row>
     <row r="361" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -38241,7 +38303,7 @@
         <v>194</v>
       </c>
       <c r="B361" s="3" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
     </row>
     <row r="362" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -38249,7 +38311,7 @@
         <v>195</v>
       </c>
       <c r="B362" s="3" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
     </row>
     <row r="363" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -38257,7 +38319,7 @@
         <v>196</v>
       </c>
       <c r="B363" s="3" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
     </row>
     <row r="364" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -38265,7 +38327,7 @@
         <v>331</v>
       </c>
       <c r="B364" s="3" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
     </row>
     <row r="365" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -38273,15 +38335,15 @@
         <v>197</v>
       </c>
       <c r="B365" s="3" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
     </row>
     <row r="366" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A366" s="2" t="s">
+        <v>667</v>
+      </c>
+      <c r="B366" s="3" t="s">
         <v>668</v>
-      </c>
-      <c r="B366" s="3" t="s">
-        <v>669</v>
       </c>
     </row>
     <row r="367" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38289,7 +38351,7 @@
         <v>198</v>
       </c>
       <c r="B367" s="3" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="368" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38297,7 +38359,7 @@
         <v>199</v>
       </c>
       <c r="B368" s="3" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
     </row>
     <row r="369" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -38305,7 +38367,7 @@
         <v>200</v>
       </c>
       <c r="B369" s="3" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
     </row>
     <row r="370" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -38313,7 +38375,7 @@
         <v>201</v>
       </c>
       <c r="B370" s="3" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
     </row>
     <row r="371" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38321,7 +38383,7 @@
         <v>202</v>
       </c>
       <c r="B371" s="3" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
     </row>
     <row r="372" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -38329,47 +38391,47 @@
         <v>203</v>
       </c>
       <c r="B372" s="3" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
     </row>
     <row r="373" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A373" s="2" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="B373" s="3" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
     </row>
     <row r="374" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A374" s="2" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="B374" s="3" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
     </row>
     <row r="375" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A375" s="2" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B375" s="3" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
     </row>
     <row r="376" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A376" s="2" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="B376" s="3" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="377" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A377" s="2" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B377" s="3" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="378" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -38377,55 +38439,55 @@
         <v>204</v>
       </c>
       <c r="B378" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="379" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A379" s="2" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="B379" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="380" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A380" s="2" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="B380" s="3" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row r="381" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A381" s="2" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="B381" s="3" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="382" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A382" s="2" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="B382" s="3" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="383" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A383" s="2" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="B383" s="3" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="384" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A384" s="2" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="B384" s="3" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
     <row r="385" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -38433,55 +38495,55 @@
         <v>205</v>
       </c>
       <c r="B385" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="386" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A386" s="2" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B386" s="3" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
     </row>
     <row r="387" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A387" s="2" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="B387" s="3" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
     </row>
     <row r="388" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A388" s="2" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="B388" s="3" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
     </row>
     <row r="389" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A389" s="2" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="B389" s="3" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
     </row>
     <row r="390" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A390" s="2" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="B390" s="3" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="391" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A391" s="2" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="B391" s="3" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
     </row>
     <row r="392" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38489,7 +38551,7 @@
         <v>206</v>
       </c>
       <c r="B392" s="3" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="393" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -38497,7 +38559,7 @@
         <v>207</v>
       </c>
       <c r="B393" s="3" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
     </row>
     <row r="394" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -38505,7 +38567,7 @@
         <v>208</v>
       </c>
       <c r="B394" s="3" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="395" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -38513,55 +38575,55 @@
         <v>209</v>
       </c>
       <c r="B395" s="3" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
     </row>
     <row r="396" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A396" s="2" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="B396" s="3" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
     </row>
     <row r="397" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A397" s="2" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="B397" s="3" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
     </row>
     <row r="398" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A398" s="2" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="B398" s="3" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
     </row>
     <row r="399" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A399" s="2" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="B399" s="3" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
     </row>
     <row r="400" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A400" s="2" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="B400" s="4" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
     </row>
     <row r="401" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A401" s="2" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="B401" s="3" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="402" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -38569,63 +38631,63 @@
         <v>210</v>
       </c>
       <c r="B402" s="3" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
     </row>
     <row r="403" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A403" s="2" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="B403" s="3" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="404" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A404" s="2" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="B404" s="3" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
     </row>
     <row r="405" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A405" s="2" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="B405" s="3" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="406" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A406" s="2" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="B406" s="3" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="407" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A407" s="2" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="B407" s="3" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="408" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A408" s="2" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="B408" s="3" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="409" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A409" s="2" t="s">
+        <v>645</v>
+      </c>
+      <c r="B409" s="3" t="s">
         <v>646</v>
-      </c>
-      <c r="B409" s="3" t="s">
-        <v>647</v>
       </c>
     </row>
     <row r="410" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -38633,7 +38695,7 @@
         <v>211</v>
       </c>
       <c r="B410" s="3" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="411" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -38681,7 +38743,7 @@
         <v>213</v>
       </c>
       <c r="B416" s="3" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
     </row>
     <row r="417" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -38689,7 +38751,7 @@
         <v>214</v>
       </c>
       <c r="B417" s="3" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
     </row>
     <row r="418" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -38697,7 +38759,7 @@
         <v>215</v>
       </c>
       <c r="B418" s="3" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="419" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38729,7 +38791,7 @@
         <v>219</v>
       </c>
       <c r="B422" s="3" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
     </row>
     <row r="423" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38737,7 +38799,7 @@
         <v>220</v>
       </c>
       <c r="B423" s="3" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
     </row>
     <row r="424" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -38745,7 +38807,7 @@
         <v>221</v>
       </c>
       <c r="B424" s="3" t="s">
-        <v>1122</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="425" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -38753,7 +38815,7 @@
         <v>222</v>
       </c>
       <c r="B425" s="3" t="s">
-        <v>1121</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="426" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -38761,7 +38823,7 @@
         <v>223</v>
       </c>
       <c r="B426" s="3" t="s">
-        <v>1120</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="427" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -38769,7 +38831,7 @@
         <v>224</v>
       </c>
       <c r="B427" s="3" t="s">
-        <v>1119</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="428" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -38777,7 +38839,7 @@
         <v>332</v>
       </c>
       <c r="B428" s="3" t="s">
-        <v>1123</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="429" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -38793,7 +38855,7 @@
         <v>225</v>
       </c>
       <c r="B430" s="3" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
     </row>
     <row r="431" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -38857,7 +38919,7 @@
         <v>449</v>
       </c>
       <c r="B438" s="3" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="439" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -38865,31 +38927,31 @@
         <v>451</v>
       </c>
       <c r="B439" s="3" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="440" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A440" s="2" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="B440" s="3" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="441" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A441" s="2" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="B441" s="3" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
     </row>
     <row r="442" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A442" s="2" t="s">
+        <v>797</v>
+      </c>
+      <c r="B442" s="3" t="s">
         <v>798</v>
-      </c>
-      <c r="B442" s="3" t="s">
-        <v>799</v>
       </c>
     </row>
     <row r="443" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -38897,7 +38959,7 @@
         <v>319</v>
       </c>
       <c r="B443" s="3" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="444" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -38905,7 +38967,7 @@
         <v>320</v>
       </c>
       <c r="B444" s="3" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="445" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -38913,7 +38975,7 @@
         <v>321</v>
       </c>
       <c r="B445" s="3" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="446" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -38921,15 +38983,15 @@
         <v>318</v>
       </c>
       <c r="B446" s="3" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="447" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A447" s="2" t="s">
+        <v>1064</v>
+      </c>
+      <c r="B447" s="3" t="s">
         <v>1065</v>
-      </c>
-      <c r="B447" s="3" t="s">
-        <v>1066</v>
       </c>
     </row>
     <row r="448" spans="1:2" ht="255" x14ac:dyDescent="0.25">
@@ -38937,7 +38999,7 @@
         <v>322</v>
       </c>
       <c r="B448" s="3" t="s">
-        <v>1116</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="449" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38953,7 +39015,7 @@
         <v>490</v>
       </c>
       <c r="B450" s="3" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="451" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -39001,295 +39063,295 @@
         <v>564</v>
       </c>
       <c r="B456" s="3" t="s">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="457" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="457" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A457" s="2" t="s">
         <v>568</v>
       </c>
       <c r="B457" s="3" t="s">
-        <v>569</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="458" spans="1:2" ht="225" x14ac:dyDescent="0.25">
       <c r="A458" s="2" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="B458" s="3" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
     <row r="459" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A459" s="2" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B459" s="3" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="460" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A460" s="2" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="B460" s="3" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="461" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A461" s="2" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="B461" s="3" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="462" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A462" s="2" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="B462" s="3" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="463" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A463" s="2" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B463" s="3" t="s">
-        <v>1127</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="464" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A464" s="2" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="B464" s="3" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="465" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A465" s="2" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="B465" s="3" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="466" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A466" s="2" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="B466" s="3" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="467" spans="1:2" ht="225" x14ac:dyDescent="0.25">
       <c r="A467" s="2" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="B467" s="3" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="468" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A468" s="2" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="B468" s="3" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
     </row>
     <row r="469" spans="1:2" ht="225" x14ac:dyDescent="0.25">
       <c r="A469" s="2" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="B469" s="3" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
     </row>
     <row r="470" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A470" s="2" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="B470" s="3" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
     </row>
     <row r="471" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A471" s="2" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="B471" s="3" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
     </row>
     <row r="472" spans="1:2" ht="225" x14ac:dyDescent="0.25">
       <c r="A472" s="2" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="B472" s="3" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
     </row>
     <row r="473" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A473" s="2" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="B473" s="3" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
     </row>
     <row r="474" spans="1:2" ht="255" x14ac:dyDescent="0.25">
       <c r="A474" s="2" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="B474" s="1" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="475" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A475" s="2" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="B475" s="1" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="476" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A476" s="2" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="B476" s="1" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
     </row>
     <row r="477" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A477" s="2" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="B477" s="1" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="478" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A478" s="2" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="B478" s="1" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="479" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A479" s="2" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="B479" s="1" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
     </row>
     <row r="480" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A480" s="2" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="B480" s="1" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
     </row>
     <row r="481" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A481" s="2" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="B481" s="1" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="482" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A482" s="2" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="B482" s="1" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="483" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A483" s="2" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="B483" s="1" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
     </row>
     <row r="484" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A484" s="2" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="B484" s="1" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="485" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A485" s="2" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="B485" s="1" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
     </row>
     <row r="486" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A486" s="2" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="B486" s="1" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
     </row>
     <row r="487" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A487" s="2" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="B487" s="1" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
     </row>
     <row r="488" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A488" s="2" t="s">
+        <v>696</v>
+      </c>
+      <c r="B488" s="1" t="s">
         <v>697</v>
-      </c>
-      <c r="B488" s="1" t="s">
-        <v>698</v>
       </c>
     </row>
     <row r="489" spans="1:2" ht="255" x14ac:dyDescent="0.25">
       <c r="A489" s="2" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="B489" s="1" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="490" spans="1:2" ht="92.25" x14ac:dyDescent="0.25">
       <c r="A490" s="2" t="s">
+        <v>1044</v>
+      </c>
+      <c r="B490" s="1" t="s">
         <v>1045</v>
-      </c>
-      <c r="B490" s="1" t="s">
-        <v>1046</v>
       </c>
     </row>
     <row r="491" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A491" s="2" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="B491" s="1" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
     </row>
     <row r="492" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A492" s="2" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="B492" s="3" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="493" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -39297,7 +39359,7 @@
         <v>550</v>
       </c>
       <c r="B493" s="3" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
     </row>
     <row r="494" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -39305,7 +39367,7 @@
         <v>551</v>
       </c>
       <c r="B494" s="3" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
     </row>
     <row r="495" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -39313,7 +39375,7 @@
         <v>552</v>
       </c>
       <c r="B495" s="3" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
     </row>
     <row r="496" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39385,7 +39447,7 @@
         <v>275</v>
       </c>
       <c r="B504" s="1" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="505" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39393,7 +39455,7 @@
         <v>276</v>
       </c>
       <c r="B505" s="1" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="506" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39401,7 +39463,7 @@
         <v>277</v>
       </c>
       <c r="B506" s="1" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="507" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -39449,7 +39511,7 @@
         <v>260</v>
       </c>
       <c r="B512" s="3" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="513" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39457,7 +39519,7 @@
         <v>480</v>
       </c>
       <c r="B513" s="3" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
     </row>
     <row r="514" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -39465,15 +39527,15 @@
         <v>481</v>
       </c>
       <c r="B514" s="1" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
     </row>
     <row r="515" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A515" s="2" t="s">
+        <v>805</v>
+      </c>
+      <c r="B515" s="3" t="s">
         <v>806</v>
-      </c>
-      <c r="B515" s="3" t="s">
-        <v>807</v>
       </c>
     </row>
     <row r="516" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39521,7 +39583,7 @@
         <v>285</v>
       </c>
       <c r="B521" s="1" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
     </row>
     <row r="522" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -39529,7 +39591,7 @@
         <v>286</v>
       </c>
       <c r="B522" s="1" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
     </row>
     <row r="523" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -39609,7 +39671,7 @@
         <v>296</v>
       </c>
       <c r="B532" s="1" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
     </row>
     <row r="533" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -39617,7 +39679,7 @@
         <v>297</v>
       </c>
       <c r="B533" s="1" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
     </row>
     <row r="534" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -39649,7 +39711,7 @@
         <v>298</v>
       </c>
       <c r="B537" s="1" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
     </row>
     <row r="538" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -39665,7 +39727,7 @@
         <v>299</v>
       </c>
       <c r="B539" s="1" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
     </row>
     <row r="540" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -39689,7 +39751,7 @@
         <v>300</v>
       </c>
       <c r="B542" s="1" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
     </row>
     <row r="543" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -39697,7 +39759,7 @@
         <v>301</v>
       </c>
       <c r="B543" s="1" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
     </row>
     <row r="544" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -39737,7 +39799,7 @@
         <v>396</v>
       </c>
       <c r="B548" s="1" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="549" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -39750,10 +39812,10 @@
     </row>
     <row r="550" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A550" s="2" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="B550" s="1" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
     </row>
     <row r="551" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -39761,7 +39823,7 @@
         <v>305</v>
       </c>
       <c r="B551" s="1" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
     </row>
     <row r="552" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -39790,10 +39852,10 @@
     </row>
     <row r="555" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A555" s="2" t="s">
+        <v>745</v>
+      </c>
+      <c r="B555" s="1" t="s">
         <v>746</v>
-      </c>
-      <c r="B555" s="1" t="s">
-        <v>747</v>
       </c>
     </row>
     <row r="556" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -39801,7 +39863,7 @@
         <v>306</v>
       </c>
       <c r="B556" s="1" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
     </row>
     <row r="557" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -39825,7 +39887,7 @@
         <v>307</v>
       </c>
       <c r="B559" s="1" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="560" spans="1:2" ht="375" x14ac:dyDescent="0.25">
@@ -39833,7 +39895,7 @@
         <v>311</v>
       </c>
       <c r="B560" s="1" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="561" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39857,15 +39919,15 @@
         <v>376</v>
       </c>
       <c r="B563" s="3" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="564" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A564" s="2" t="s">
+        <v>749</v>
+      </c>
+      <c r="B564" s="3" t="s">
         <v>750</v>
-      </c>
-      <c r="B564" s="3" t="s">
-        <v>751</v>
       </c>
     </row>
     <row r="565" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -39873,7 +39935,7 @@
         <v>329</v>
       </c>
       <c r="B565" s="3" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Show Title for Events in Ellipses. Fix issue with e086 after redistribute. Fix issue with escape/follow removing raft.
</commit_message>
<xml_diff>
--- a/Documentation/Events.xlsx
+++ b/Documentation/Events.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\happysulla\BarbarianPrince\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{93AB987B-673F-4C1D-96B8-0DAF39C11289}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{606C653B-432B-45CB-A649-B16508CC3093}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" r:id="rId1"/>
@@ -27786,63 +27786,6 @@
   </si>
   <si>
     <r>
-      <t>&lt;Bold&gt;e086a High Pass Travels&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;When you travel the high pass,  roll for the effects of high winds, sub-freezing temperatures, snow, etc. Roll two die for the entire party: &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>dieRoll</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.gif' Name='</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>DiceRoll</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>' Height='21' Width='21' &gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;
-&lt;LineBreak/&gt;8 = Characters suffers wound
-&lt;LineBreak/&gt;9 = Characters suffer 2 wounds
-&lt;LineBreak/&gt;10 = Characters suffer 3 wounds
-&lt;LineBreak/&gt;11 = Characters suffer 4 wounds
-&lt;LineBreak/&gt;12 = Characters suffer 4 wounds plus poison wound
-&lt;LineBreak/&gt;Additionally, if greater than 8, all mounts die
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-No caches are allowed. Due to terrible conditions, if your transport ability
- &lt;InlineUIContainer&gt;&lt;Button Content='r206' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
- is reduced due to loss of characters or mounts, you cannot cache spare wealth and possessions. They must be abandoned in the snows and lost entirely.</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>&lt;Bold&gt;e210a Freeman Available&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;A freeman joins your party at no cost (except food and lodging). He has a combat skill 3 and endurance 4. 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;Click to not allow him to join:
@@ -34942,6 +34885,63 @@
         <scheme val="minor"/>
       </rPr>
       <t>.gif' Height='150' Width='150'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;Bold&gt;e086a High Pass Travels&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;When you travel the high pass, roll for the effects of high winds, sub-freezing temperatures, snow, etc. Roll two die for the entire party: &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dieRoll</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.gif' Name='</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DiceRoll</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>' Height='21' Width='21' &gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;
+&lt;LineBreak/&gt;8 = Characters suffers wound
+&lt;LineBreak/&gt;9 = Characters suffer 2 wounds
+&lt;LineBreak/&gt;10 = Characters suffer 3 wounds
+&lt;LineBreak/&gt;11 = Characters suffer 4 wounds
+&lt;LineBreak/&gt;12 = Characters suffer 4 wounds plus poison wound
+&lt;LineBreak/&gt;Additionally, if greater than 8, all mounts die
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+No caches are allowed. Due to terrible conditions, if your transport ability
+ &lt;InlineUIContainer&gt;&lt;Button Content='r206' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+ is reduced due to loss of characters or mounts, you cannot cache spare wealth and possessions. They must be abandoned in the snows and lost entirely.</t>
     </r>
   </si>
 </sst>
@@ -35408,8 +35408,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B565"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A456" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B457" sqref="B457"/>
+    <sheetView tabSelected="1" topLeftCell="A244" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B247" sqref="B247"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -35423,7 +35423,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -35431,7 +35431,7 @@
         <v>254</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -35439,7 +35439,7 @@
         <v>255</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -35447,15 +35447,15 @@
         <v>256</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="390" x14ac:dyDescent="0.25">
@@ -35479,7 +35479,7 @@
         <v>22</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35511,7 +35511,7 @@
         <v>3</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -35711,7 +35711,7 @@
         <v>25</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -35735,7 +35735,7 @@
         <v>26</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -35775,7 +35775,7 @@
         <v>29</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -35799,7 +35799,7 @@
         <v>715</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -35807,7 +35807,7 @@
         <v>31</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -35855,7 +35855,7 @@
         <v>501</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -35879,7 +35879,7 @@
         <v>264</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35887,7 +35887,7 @@
         <v>265</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -36023,7 +36023,7 @@
         <v>42</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -36031,7 +36031,7 @@
         <v>46</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -36183,7 +36183,7 @@
         <v>791</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -36319,7 +36319,7 @@
         <v>70</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -36588,7 +36588,7 @@
     </row>
     <row r="147" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="B147" s="3" t="s">
         <v>559</v>
@@ -36943,7 +36943,7 @@
         <v>103</v>
       </c>
       <c r="B191" s="3" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="192" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37015,7 +37015,7 @@
         <v>108</v>
       </c>
       <c r="B200" s="3" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="201" spans="1:2" ht="285" x14ac:dyDescent="0.25">
@@ -37039,7 +37039,7 @@
         <v>166</v>
       </c>
       <c r="B203" s="3" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="204" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -37047,7 +37047,7 @@
         <v>167</v>
       </c>
       <c r="B204" s="3" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="205" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -37143,7 +37143,7 @@
         <v>171</v>
       </c>
       <c r="B216" s="3" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="217" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37151,7 +37151,7 @@
         <v>113</v>
       </c>
       <c r="B217" s="3" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="218" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -37199,7 +37199,7 @@
         <v>116</v>
       </c>
       <c r="B223" s="3" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="224" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -37263,7 +37263,7 @@
         <v>941</v>
       </c>
       <c r="B231" s="3" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="232" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -37391,7 +37391,7 @@
         <v>1002</v>
       </c>
       <c r="B247" s="3" t="s">
-        <v>1004</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="248" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37399,7 +37399,7 @@
         <v>126</v>
       </c>
       <c r="B248" s="3" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="249" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37423,7 +37423,7 @@
         <v>129</v>
       </c>
       <c r="B251" s="3" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="252" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37463,7 +37463,7 @@
         <v>132</v>
       </c>
       <c r="B256" s="3" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="257" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -37471,7 +37471,7 @@
         <v>133</v>
       </c>
       <c r="B257" s="3" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="258" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -37479,7 +37479,7 @@
         <v>954</v>
       </c>
       <c r="B258" s="3" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="259" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37487,23 +37487,23 @@
         <v>134</v>
       </c>
       <c r="B259" s="3" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="260" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A260" s="2" t="s">
+        <v>1012</v>
+      </c>
+      <c r="B260" s="3" t="s">
         <v>1013</v>
-      </c>
-      <c r="B260" s="3" t="s">
-        <v>1014</v>
       </c>
     </row>
     <row r="261" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A261" s="2" t="s">
+        <v>1014</v>
+      </c>
+      <c r="B261" s="3" t="s">
         <v>1015</v>
-      </c>
-      <c r="B261" s="3" t="s">
-        <v>1016</v>
       </c>
     </row>
     <row r="262" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -37511,15 +37511,15 @@
         <v>135</v>
       </c>
       <c r="B262" s="3" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="263" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A263" s="2" t="s">
+        <v>1017</v>
+      </c>
+      <c r="B263" s="3" t="s">
         <v>1018</v>
-      </c>
-      <c r="B263" s="3" t="s">
-        <v>1019</v>
       </c>
     </row>
     <row r="264" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -37527,7 +37527,7 @@
         <v>136</v>
       </c>
       <c r="B264" s="3" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="265" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -37615,7 +37615,7 @@
         <v>140</v>
       </c>
       <c r="B275" s="3" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="276" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -37623,7 +37623,7 @@
         <v>236</v>
       </c>
       <c r="B276" s="3" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="277" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37631,7 +37631,7 @@
         <v>237</v>
       </c>
       <c r="B277" s="3" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="278" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37639,7 +37639,7 @@
         <v>238</v>
       </c>
       <c r="B278" s="3" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="279" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -37647,7 +37647,7 @@
         <v>141</v>
       </c>
       <c r="B279" s="3" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="280" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -37655,7 +37655,7 @@
         <v>142</v>
       </c>
       <c r="B280" s="3" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="281" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -37663,7 +37663,7 @@
         <v>143</v>
       </c>
       <c r="B281" s="3" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="282" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -37671,7 +37671,7 @@
         <v>144</v>
       </c>
       <c r="B282" s="3" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="283" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -37679,7 +37679,7 @@
         <v>242</v>
       </c>
       <c r="B283" s="3" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="284" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37687,7 +37687,7 @@
         <v>145</v>
       </c>
       <c r="B284" s="3" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="285" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -37695,7 +37695,7 @@
         <v>146</v>
       </c>
       <c r="B285" s="3" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="286" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37703,7 +37703,7 @@
         <v>147</v>
       </c>
       <c r="B286" s="3" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="287" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -37711,7 +37711,7 @@
         <v>148</v>
       </c>
       <c r="B287" s="3" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="288" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -37719,31 +37719,31 @@
         <v>149</v>
       </c>
       <c r="B288" s="3" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="289" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A289" s="2" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="B289" s="3" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="290" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A290" s="2" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="B290" s="3" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="291" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A291" s="2" t="s">
+        <v>1088</v>
+      </c>
+      <c r="B291" s="3" t="s">
         <v>1089</v>
-      </c>
-      <c r="B291" s="3" t="s">
-        <v>1090</v>
       </c>
     </row>
     <row r="292" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37751,15 +37751,15 @@
         <v>150</v>
       </c>
       <c r="B292" s="3" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="293" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A293" s="2" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="B293" s="3" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="294" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -37807,7 +37807,7 @@
         <v>153</v>
       </c>
       <c r="B299" s="3" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="300" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37887,7 +37887,7 @@
         <v>160</v>
       </c>
       <c r="B309" s="3" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="310" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -37895,7 +37895,7 @@
         <v>161</v>
       </c>
       <c r="B310" s="3" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="311" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37903,31 +37903,31 @@
         <v>162</v>
       </c>
       <c r="B311" s="3" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="312" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A312" s="2" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="B312" s="3" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="313" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A313" s="2" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="B313" s="3" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="314" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A314" s="2" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="B314" s="3" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="315" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37935,7 +37935,7 @@
         <v>163</v>
       </c>
       <c r="B315" s="3" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="316" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -37943,7 +37943,7 @@
         <v>164</v>
       </c>
       <c r="B316" s="3" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="317" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37951,7 +37951,7 @@
         <v>175</v>
       </c>
       <c r="B317" s="3" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="318" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -37959,7 +37959,7 @@
         <v>176</v>
       </c>
       <c r="B318" s="3" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="319" spans="1:2" ht="390" x14ac:dyDescent="0.25">
@@ -37967,7 +37967,7 @@
         <v>177</v>
       </c>
       <c r="B319" s="3" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="320" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -37975,7 +37975,7 @@
         <v>525</v>
       </c>
       <c r="B320" s="3" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="321" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37983,7 +37983,7 @@
         <v>526</v>
       </c>
       <c r="B321" s="3" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="322" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37991,7 +37991,7 @@
         <v>527</v>
       </c>
       <c r="B322" s="3" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="323" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -37999,7 +37999,7 @@
         <v>528</v>
       </c>
       <c r="B323" s="3" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="324" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -38007,7 +38007,7 @@
         <v>529</v>
       </c>
       <c r="B324" s="3" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="325" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -38015,15 +38015,15 @@
         <v>530</v>
       </c>
       <c r="B325" s="3" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="326" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A326" s="2" t="s">
+        <v>1110</v>
+      </c>
+      <c r="B326" s="3" t="s">
         <v>1111</v>
-      </c>
-      <c r="B326" s="3" t="s">
-        <v>1112</v>
       </c>
     </row>
     <row r="327" spans="1:2" ht="390" x14ac:dyDescent="0.25">
@@ -38031,7 +38031,7 @@
         <v>178</v>
       </c>
       <c r="B327" s="3" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="328" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -38039,7 +38039,7 @@
         <v>499</v>
       </c>
       <c r="B328" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="329" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -38047,7 +38047,7 @@
         <v>555</v>
       </c>
       <c r="B329" s="3" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="330" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -38055,7 +38055,7 @@
         <v>556</v>
       </c>
       <c r="B330" s="3" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="331" spans="1:2" ht="315" x14ac:dyDescent="0.25">
@@ -38095,7 +38095,7 @@
         <v>252</v>
       </c>
       <c r="B335" s="3" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="336" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -38127,7 +38127,7 @@
         <v>180</v>
       </c>
       <c r="B339" s="3" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="340" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38159,7 +38159,7 @@
         <v>183</v>
       </c>
       <c r="B343" s="3" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="344" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -38167,7 +38167,7 @@
         <v>184</v>
       </c>
       <c r="B344" s="3" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="345" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -38759,7 +38759,7 @@
         <v>215</v>
       </c>
       <c r="B418" s="3" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="419" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38807,7 +38807,7 @@
         <v>221</v>
       </c>
       <c r="B424" s="3" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="425" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -38815,7 +38815,7 @@
         <v>222</v>
       </c>
       <c r="B425" s="3" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="426" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -38823,7 +38823,7 @@
         <v>223</v>
       </c>
       <c r="B426" s="3" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="427" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -38831,7 +38831,7 @@
         <v>224</v>
       </c>
       <c r="B427" s="3" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="428" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -38839,7 +38839,7 @@
         <v>332</v>
       </c>
       <c r="B428" s="3" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="429" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -38919,7 +38919,7 @@
         <v>449</v>
       </c>
       <c r="B438" s="3" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="439" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -38959,7 +38959,7 @@
         <v>319</v>
       </c>
       <c r="B443" s="3" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="444" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -38967,7 +38967,7 @@
         <v>320</v>
       </c>
       <c r="B444" s="3" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="445" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -38975,7 +38975,7 @@
         <v>321</v>
       </c>
       <c r="B445" s="3" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="446" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -38983,15 +38983,15 @@
         <v>318</v>
       </c>
       <c r="B446" s="3" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="447" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A447" s="2" t="s">
+        <v>1063</v>
+      </c>
+      <c r="B447" s="3" t="s">
         <v>1064</v>
-      </c>
-      <c r="B447" s="3" t="s">
-        <v>1065</v>
       </c>
     </row>
     <row r="448" spans="1:2" ht="255" x14ac:dyDescent="0.25">
@@ -38999,7 +38999,7 @@
         <v>322</v>
       </c>
       <c r="B448" s="3" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="449" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39071,7 +39071,7 @@
         <v>568</v>
       </c>
       <c r="B457" s="3" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="458" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -39087,7 +39087,7 @@
         <v>572</v>
       </c>
       <c r="B459" s="3" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="460" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39119,7 +39119,7 @@
         <v>576</v>
       </c>
       <c r="B463" s="3" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="464" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -39324,18 +39324,18 @@
     </row>
     <row r="489" spans="1:2" ht="255" x14ac:dyDescent="0.25">
       <c r="A489" s="2" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="B489" s="1" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="490" spans="1:2" ht="92.25" x14ac:dyDescent="0.25">
       <c r="A490" s="2" t="s">
+        <v>1043</v>
+      </c>
+      <c r="B490" s="1" t="s">
         <v>1044</v>
-      </c>
-      <c r="B490" s="1" t="s">
-        <v>1045</v>
       </c>
     </row>
     <row r="491" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -39351,7 +39351,7 @@
         <v>735</v>
       </c>
       <c r="B492" s="3" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="493" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -39447,7 +39447,7 @@
         <v>275</v>
       </c>
       <c r="B504" s="1" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="505" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39455,7 +39455,7 @@
         <v>276</v>
       </c>
       <c r="B505" s="1" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="506" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39463,7 +39463,7 @@
         <v>277</v>
       </c>
       <c r="B506" s="1" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="507" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -39511,7 +39511,7 @@
         <v>260</v>
       </c>
       <c r="B512" s="3" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="513" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39887,7 +39887,7 @@
         <v>307</v>
       </c>
       <c r="B559" s="1" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="560" spans="1:2" ht="375" x14ac:dyDescent="0.25">
@@ -39919,7 +39919,7 @@
         <v>376</v>
       </c>
       <c r="B563" s="3" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="564" spans="1:2" ht="60" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fix issue in Events.xls related to e20xh. Undo fixes rafting. Chanaged title of RuleListingDialog if showing events.
</commit_message>
<xml_diff>
--- a/Documentation/Events.xlsx
+++ b/Documentation/Events.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\happysulla\BarbarianPrince\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{420C7E61-F201-4F5F-BFBC-25516A08D876}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{77CCEDD2-C4BA-4D76-AFEC-68D2136BBF29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" r:id="rId1"/>
@@ -14642,63 +14642,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t>&lt;Bold&gt;e005 Amazons&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;You see a group of amazon warriors approaching all on foot. The number in the group is one die roll plus one.
- &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>dieRoll</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.gif' Name='</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>DieRoll</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;All have a combat skill 6, endurance 5, and wealth 4. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;They are blood-sisters and will always hire out together and serve together. If any are abandoned or left behind, all will desert you. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;Your options are:
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
- &lt;InlineUIContainer&gt;&lt;Button FontFamily='Courier New'  FontSize='12'  Content='Talk ' Name='e005a'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   -&gt;  
-&lt;InlineUIContainer&gt;&lt;Button FontFamily='Courier New'  FontSize='12' Content='e005a'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;&lt;LineBreak/&gt;
- &lt;InlineUIContainer&gt;&lt;Button FontFamily='Courier New'  FontSize='12' Content='Evade' Name='e005b'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   -&gt;  
-&lt;InlineUIContainer&gt;&lt;Button FontFamily='Courier New'  FontSize='12' Content='e005b'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;*&lt;LineBreak/&gt;
- &lt;InlineUIContainer&gt;&lt;Button FontFamily='Courier New'  FontSize='12' Content='Fight' Name='e005c'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   -&gt;  
-&lt;InlineUIContainer&gt;&lt;Button FontFamily='Courier New'  FontSize='12' Content='e005c'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;</t>
-    </r>
-  </si>
-  <si>
     <t>e338c</t>
   </si>
   <si>
@@ -31075,116 +31018,6 @@
   </si>
   <si>
     <r>
-      <t>&lt;LineBreak/&gt;&lt;Bold&gt;Game Events Shown Here&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;Active events show a green background. The game may only advance when a green background is displayed. However, the game lets you explore what may happen by showing inactive events. Inactive events have a gray background. To return to the current active event, select the active event button in the status bar per the image.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                     &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Tutorial0</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.gif' Height='70'  Width='370'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Name='</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Read_Rules</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>' Content='</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Read Rules</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>' FontFamily='Courier New'  FontSize='12'&gt; &lt;/Button&gt;&lt;/InlineUIContainer&gt; or &lt;InlineUIContainer&gt;&lt;Button Name='</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Begin</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>' Content='</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Begin Game</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>' FontFamily='Courier New'  FontSize='12'&gt; &lt;/Button&gt;&lt;/InlineUIContainer&gt;</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>&lt;Bold&gt;e218 Escape&lt;/Bold&gt; &lt;InlineUIContainer&gt;&lt;Button Content='r218a' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt; Managed to find an escape path. Click image to continue.
 &lt;LineBreak/&gt; &lt;LineBreak/&gt; 
@@ -32380,101 +32213,6 @@
   </si>
   <si>
     <r>
-      <t>&lt;Bold&gt;e209h Buy Valuable Information&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;If you buy it, roll one die:  &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>dieRoll</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.gif' Name='</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>DieRoll</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>' Height='21' Width='21'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt; 
-&lt;LineBreak/&gt;   1 - Bogus secrets prove worthless
-&lt;LineBreak/&gt;   2 - &lt;InlineUIContainer&gt;&lt;Button Content='e147' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;   3 - &lt;InlineUIContainer&gt;&lt;Button Content='e143' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;   4 - &lt;InlineUIContainer&gt;&lt;Button Content='e144' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;   5 - &lt;InlineUIContainer&gt;&lt;Button Content='e145' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;   6 - &lt;InlineUIContainer&gt;&lt;Button Content='e146' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;&lt;InlineUIContainer&gt;
-                                      &lt;InlineUIContainer&gt;&lt;Image Name='</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>BuyInfoEnd</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>' Source='../../Images/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Nothing</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.gif' Height='150' Width='150'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>&lt;Bold&gt;e086a High Pass Travels&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;When you travel the high pass, roll for the effects of high winds, sub-freezing temperatures, snow, etc. Roll two die for the entire party: &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
     </r>
@@ -34942,6 +34680,268 @@
         <scheme val="minor"/>
       </rPr>
       <t>' Height='300' Width='300'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;Bold&gt;e005 Amazons&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;You see a group of amazon warriors approaching all on foot. The number in the group is one die roll plus one. Die Roll=
+ &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dieRoll</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.gif' Name='</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DieRoll</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;All have a combat skill 6, endurance 5, and wealth 4. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;They are blood-sisters and will always hire out together and serve together. If any are abandoned or left behind, all will desert you. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;Your options are:
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+ &lt;InlineUIContainer&gt;&lt;Button FontFamily='Courier New'  FontSize='12'  Content='Talk ' Name='e005a'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   -&gt;  
+&lt;InlineUIContainer&gt;&lt;Button FontFamily='Courier New'  FontSize='12' Content='e005a'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;&lt;LineBreak/&gt;
+ &lt;InlineUIContainer&gt;&lt;Button FontFamily='Courier New'  FontSize='12' Content='Evade' Name='e005b'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   -&gt;  
+&lt;InlineUIContainer&gt;&lt;Button FontFamily='Courier New'  FontSize='12' Content='e005b'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;*&lt;LineBreak/&gt;
+ &lt;InlineUIContainer&gt;&lt;Button FontFamily='Courier New'  FontSize='12' Content='Fight' Name='e005c'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   -&gt;  
+&lt;InlineUIContainer&gt;&lt;Button FontFamily='Courier New'  FontSize='12' Content='e005c'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;LineBreak/&gt;&lt;Bold&gt;e000 Game Events Shown Here&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;Active events show a green background. The game may only advance when a green background is displayed. However, the game lets you explore what may happen by showing inactive events. Inactive events have a gray background. To return to the current active event, select the active event button in the status bar per the image.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                     &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Tutorial0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.gif' Height='70'  Width='370'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Name='</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Read_Rules</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>' Content='</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Read Rules</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>' FontFamily='Courier New'  FontSize='12'&gt; &lt;/Button&gt;&lt;/InlineUIContainer&gt; or &lt;InlineUIContainer&gt;&lt;Button Name='</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Begin</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>' Content='</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Begin Game</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>' FontFamily='Courier New'  FontSize='12'&gt; &lt;/Button&gt;&lt;/InlineUIContainer&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;Bold&gt;e209h Buy Valuable Information&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;If you buy it, roll one die:  &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dieRoll</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.gif' Name='</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DieRoll</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>' Height='21' Width='21'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt; 
+&lt;LineBreak/&gt;   1 - Bogus secrets prove worthless
+&lt;LineBreak/&gt;   2 - &lt;InlineUIContainer&gt;&lt;Button Content='e147' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;   3 - &lt;InlineUIContainer&gt;&lt;Button Content='e143' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;   4 - &lt;InlineUIContainer&gt;&lt;Button Content='e144' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;   5 - &lt;InlineUIContainer&gt;&lt;Button Content='e145' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;   6 - &lt;InlineUIContainer&gt;&lt;Button Content='e146' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                      &lt;InlineUIContainer&gt;&lt;Image Name='</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>BuyInfoEnd</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>' Source='../../Images/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Nothing</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.gif' Height='150' Width='150'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
     </r>
   </si>
 </sst>
@@ -35408,8 +35408,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B565"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView tabSelected="1" topLeftCell="A454" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B455" sqref="B455"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -35423,7 +35423,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1065</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -35431,7 +35431,7 @@
         <v>254</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -35439,7 +35439,7 @@
         <v>255</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -35447,15 +35447,15 @@
         <v>256</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="390" x14ac:dyDescent="0.25">
@@ -35471,7 +35471,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35479,7 +35479,7 @@
         <v>22</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>1067</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35511,7 +35511,7 @@
         <v>3</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -35519,7 +35519,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35543,7 +35543,7 @@
         <v>7</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -35551,7 +35551,7 @@
         <v>8</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35559,7 +35559,7 @@
         <v>10</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35567,7 +35567,7 @@
         <v>9</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -35575,7 +35575,7 @@
         <v>11</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>732</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -35583,7 +35583,7 @@
         <v>12</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35591,7 +35591,7 @@
         <v>13</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35599,7 +35599,7 @@
         <v>14</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -35607,7 +35607,7 @@
         <v>15</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -35615,7 +35615,7 @@
         <v>16</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -35623,7 +35623,7 @@
         <v>17</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -35631,7 +35631,7 @@
         <v>18</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -35639,31 +35639,31 @@
         <v>261</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -35671,7 +35671,7 @@
         <v>19</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -35679,7 +35679,7 @@
         <v>20</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -35687,23 +35687,23 @@
         <v>21</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>1119</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>1121</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>1120</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -35711,23 +35711,23 @@
         <v>25</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -35735,7 +35735,7 @@
         <v>26</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -35759,7 +35759,7 @@
         <v>27</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>1123</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -35767,7 +35767,7 @@
         <v>28</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>1127</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -35775,7 +35775,7 @@
         <v>29</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>1124</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -35783,7 +35783,7 @@
         <v>30</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>1128</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -35799,7 +35799,7 @@
         <v>707</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>1122</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -35807,7 +35807,7 @@
         <v>31</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>1125</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -35815,7 +35815,7 @@
         <v>32</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>1129</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -35823,7 +35823,7 @@
         <v>33</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>1126</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -35855,7 +35855,7 @@
         <v>497</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>1087</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -35879,7 +35879,7 @@
         <v>264</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35887,7 +35887,7 @@
         <v>265</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -35911,7 +35911,7 @@
         <v>35</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -35943,7 +35943,7 @@
         <v>37</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="285" x14ac:dyDescent="0.25">
@@ -35951,7 +35951,7 @@
         <v>38</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -35967,7 +35967,7 @@
         <v>44</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -35975,7 +35975,7 @@
         <v>710</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -36023,7 +36023,7 @@
         <v>42</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -36031,7 +36031,7 @@
         <v>46</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -36055,7 +36055,7 @@
         <v>49</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -36095,7 +36095,7 @@
         <v>54</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -36103,7 +36103,7 @@
         <v>55</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -36111,7 +36111,7 @@
         <v>56</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -36119,7 +36119,7 @@
         <v>57</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -36127,31 +36127,31 @@
         <v>58</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>1092</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -36159,15 +36159,15 @@
         <v>59</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
+        <v>891</v>
+      </c>
+      <c r="B94" s="3" t="s">
         <v>892</v>
-      </c>
-      <c r="B94" s="3" t="s">
-        <v>893</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -36175,15 +36175,15 @@
         <v>60</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>1093</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -36191,7 +36191,7 @@
         <v>61</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -36199,7 +36199,7 @@
         <v>62</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -36231,7 +36231,7 @@
         <v>65</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -36239,7 +36239,7 @@
         <v>66</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -36287,7 +36287,7 @@
         <v>475</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>1094</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -36319,7 +36319,7 @@
         <v>70</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -36407,7 +36407,7 @@
         <v>77</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
     </row>
     <row r="125" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -36420,10 +36420,10 @@
     </row>
     <row r="126" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>1095</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="127" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -36431,7 +36431,7 @@
         <v>78</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
     </row>
     <row r="128" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -36439,7 +36439,7 @@
         <v>376</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
     </row>
     <row r="129" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -36479,7 +36479,7 @@
         <v>80</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
     </row>
     <row r="134" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -36487,87 +36487,87 @@
         <v>81</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
     </row>
     <row r="135" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
     </row>
     <row r="136" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
     </row>
     <row r="137" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
     </row>
     <row r="138" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="139" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="B139" s="3" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
     </row>
     <row r="140" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
     </row>
     <row r="141" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
     </row>
     <row r="142" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
     </row>
     <row r="143" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
+        <v>953</v>
+      </c>
+      <c r="B143" s="3" t="s">
         <v>954</v>
-      </c>
-      <c r="B143" s="3" t="s">
-        <v>955</v>
       </c>
     </row>
     <row r="144" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
     </row>
     <row r="145" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -36575,7 +36575,7 @@
         <v>82</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
     </row>
     <row r="146" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -36583,12 +36583,12 @@
         <v>83</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
     </row>
     <row r="147" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
-        <v>1084</v>
+        <v>1082</v>
       </c>
       <c r="B147" s="3" t="s">
         <v>553</v>
@@ -36623,7 +36623,7 @@
         <v>552</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
     </row>
     <row r="152" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -36631,7 +36631,7 @@
         <v>86</v>
       </c>
       <c r="B152" s="3" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
     <row r="153" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -36743,7 +36743,7 @@
         <v>444</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
     </row>
     <row r="167" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -36767,23 +36767,23 @@
         <v>90</v>
       </c>
       <c r="B169" s="3" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
     </row>
     <row r="170" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="B170" s="3" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
     </row>
     <row r="171" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="B171" s="3" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
     </row>
     <row r="172" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -36815,7 +36815,7 @@
         <v>93</v>
       </c>
       <c r="B175" s="3" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="176" spans="1:2" ht="270" x14ac:dyDescent="0.25">
@@ -36823,7 +36823,7 @@
         <v>94</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
     </row>
     <row r="177" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -36831,7 +36831,7 @@
         <v>95</v>
       </c>
       <c r="B177" s="3" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
     </row>
     <row r="178" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -36839,55 +36839,55 @@
         <v>96</v>
       </c>
       <c r="B178" s="3" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="179" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A179" s="2" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="B179" s="3" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
     </row>
     <row r="180" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A180" s="2" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="B180" s="3" t="s">
-        <v>1096</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="181" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>1097</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="182" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="B182" s="3" t="s">
-        <v>1098</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="183" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="B183" s="3" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
     </row>
     <row r="184" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A184" s="2" t="s">
+        <v>867</v>
+      </c>
+      <c r="B184" s="3" t="s">
         <v>868</v>
-      </c>
-      <c r="B184" s="3" t="s">
-        <v>869</v>
       </c>
     </row>
     <row r="185" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -36895,7 +36895,7 @@
         <v>97</v>
       </c>
       <c r="B185" s="3" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
     </row>
     <row r="186" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -36927,7 +36927,7 @@
         <v>100</v>
       </c>
       <c r="B189" s="3" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
     </row>
     <row r="190" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -36943,7 +36943,7 @@
         <v>103</v>
       </c>
       <c r="B191" s="3" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
     </row>
     <row r="192" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -36951,7 +36951,7 @@
         <v>104</v>
       </c>
       <c r="B192" s="3" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
     </row>
     <row r="193" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -36967,7 +36967,7 @@
         <v>694</v>
       </c>
       <c r="B194" s="3" t="s">
-        <v>1099</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="195" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -36983,7 +36983,7 @@
         <v>106</v>
       </c>
       <c r="B196" s="3" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
     </row>
     <row r="197" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -36991,7 +36991,7 @@
         <v>107</v>
       </c>
       <c r="B197" s="3" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
     </row>
     <row r="198" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -36999,15 +36999,15 @@
         <v>165</v>
       </c>
       <c r="B198" s="3" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
     </row>
     <row r="199" spans="1:2" ht="225" x14ac:dyDescent="0.25">
       <c r="A199" s="2" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="B199" s="3" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
     </row>
     <row r="200" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37015,7 +37015,7 @@
         <v>108</v>
       </c>
       <c r="B200" s="3" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="201" spans="1:2" ht="285" x14ac:dyDescent="0.25">
@@ -37023,7 +37023,7 @@
         <v>109</v>
       </c>
       <c r="B201" s="3" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
     </row>
     <row r="202" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -37031,7 +37031,7 @@
         <v>110</v>
       </c>
       <c r="B202" s="3" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
     </row>
     <row r="203" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -37039,7 +37039,7 @@
         <v>166</v>
       </c>
       <c r="B203" s="3" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="204" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -37047,7 +37047,7 @@
         <v>167</v>
       </c>
       <c r="B204" s="3" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="205" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -37055,23 +37055,23 @@
         <v>168</v>
       </c>
       <c r="B205" s="3" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="206" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A206" s="2" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="B206" s="3" t="s">
-        <v>1100</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="207" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A207" s="2" t="s">
+        <v>882</v>
+      </c>
+      <c r="B207" s="3" t="s">
         <v>883</v>
-      </c>
-      <c r="B207" s="3" t="s">
-        <v>884</v>
       </c>
     </row>
     <row r="208" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37119,7 +37119,7 @@
         <v>112</v>
       </c>
       <c r="B213" s="3" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="214" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37127,7 +37127,7 @@
         <v>169</v>
       </c>
       <c r="B214" s="3" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
     </row>
     <row r="215" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -37135,7 +37135,7 @@
         <v>170</v>
       </c>
       <c r="B215" s="3" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="216" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -37143,7 +37143,7 @@
         <v>171</v>
       </c>
       <c r="B216" s="3" t="s">
-        <v>1077</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="217" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37151,7 +37151,7 @@
         <v>113</v>
       </c>
       <c r="B217" s="3" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="218" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -37159,7 +37159,7 @@
         <v>114</v>
       </c>
       <c r="B218" s="3" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="219" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -37167,15 +37167,15 @@
         <v>266</v>
       </c>
       <c r="B219" s="3" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
     </row>
     <row r="220" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A220" s="2" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="B220" s="3" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
     </row>
     <row r="221" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37183,15 +37183,15 @@
         <v>115</v>
       </c>
       <c r="B221" s="3" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
     </row>
     <row r="222" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A222" s="2" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="B222" s="3" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="223" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37199,15 +37199,15 @@
         <v>116</v>
       </c>
       <c r="B223" s="3" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="224" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A224" s="2" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="B224" s="3" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="225" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -37215,31 +37215,31 @@
         <v>117</v>
       </c>
       <c r="B225" s="4" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
     </row>
     <row r="226" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A226" s="2" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="B226" s="4" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
     </row>
     <row r="227" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A227" s="2" t="s">
+        <v>749</v>
+      </c>
+      <c r="B227" s="4" t="s">
         <v>750</v>
-      </c>
-      <c r="B227" s="4" t="s">
-        <v>751</v>
       </c>
     </row>
     <row r="228" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A228" s="2" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="B228" s="4" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
     </row>
     <row r="229" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -37247,23 +37247,23 @@
         <v>118</v>
       </c>
       <c r="B229" s="3" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
     </row>
     <row r="230" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A230" s="2" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="B230" s="3" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="231" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A231" s="2" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="B231" s="3" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="232" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -37271,23 +37271,23 @@
         <v>119</v>
       </c>
       <c r="B232" s="3" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
     </row>
     <row r="233" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A233" s="2" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="B233" s="3" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
     </row>
     <row r="234" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A234" s="2" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="B234" s="3" t="s">
-        <v>1101</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="235" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -37295,7 +37295,7 @@
         <v>120</v>
       </c>
       <c r="B235" s="3" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
     </row>
     <row r="236" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -37303,7 +37303,7 @@
         <v>172</v>
       </c>
       <c r="B236" s="3" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
     </row>
     <row r="237" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37311,7 +37311,7 @@
         <v>173</v>
       </c>
       <c r="B237" s="3" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
     </row>
     <row r="238" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37319,7 +37319,7 @@
         <v>174</v>
       </c>
       <c r="B238" s="3" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
     </row>
     <row r="239" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37335,15 +37335,15 @@
         <v>122</v>
       </c>
       <c r="B240" s="3" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
     </row>
     <row r="241" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A241" s="2" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="B241" s="3" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
     </row>
     <row r="242" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -37351,23 +37351,23 @@
         <v>123</v>
       </c>
       <c r="B242" s="3" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
     </row>
     <row r="243" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A243" s="2" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="B243" s="3" t="s">
-        <v>1102</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="244" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A244" s="2" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="B244" s="3" t="s">
-        <v>1103</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="245" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37375,7 +37375,7 @@
         <v>124</v>
       </c>
       <c r="B245" s="3" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
     </row>
     <row r="246" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37383,15 +37383,15 @@
         <v>125</v>
       </c>
       <c r="B246" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="247" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A247" s="2" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="B247" s="3" t="s">
-        <v>1091</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="248" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37399,7 +37399,7 @@
         <v>126</v>
       </c>
       <c r="B248" s="3" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
     </row>
     <row r="249" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37407,7 +37407,7 @@
         <v>127</v>
       </c>
       <c r="B249" s="3" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
     </row>
     <row r="250" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37415,7 +37415,7 @@
         <v>128</v>
       </c>
       <c r="B250" s="3" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
     </row>
     <row r="251" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -37423,7 +37423,7 @@
         <v>129</v>
       </c>
       <c r="B251" s="3" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="252" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37431,7 +37431,7 @@
         <v>130</v>
       </c>
       <c r="B252" s="3" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
     </row>
     <row r="253" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -37439,23 +37439,23 @@
         <v>131</v>
       </c>
       <c r="B253" s="3" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
     </row>
     <row r="254" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A254" s="2" t="s">
+        <v>929</v>
+      </c>
+      <c r="B254" s="3" t="s">
         <v>930</v>
-      </c>
-      <c r="B254" s="3" t="s">
-        <v>931</v>
       </c>
     </row>
     <row r="255" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A255" s="2" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="B255" s="3" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
     </row>
     <row r="256" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -37463,7 +37463,7 @@
         <v>132</v>
       </c>
       <c r="B256" s="3" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
     </row>
     <row r="257" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -37471,15 +37471,15 @@
         <v>133</v>
       </c>
       <c r="B257" s="3" t="s">
-        <v>1104</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="258" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A258" s="2" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="B258" s="3" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="259" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37487,23 +37487,23 @@
         <v>134</v>
       </c>
       <c r="B259" s="3" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
     </row>
     <row r="260" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A260" s="2" t="s">
+        <v>981</v>
+      </c>
+      <c r="B260" s="3" t="s">
         <v>982</v>
-      </c>
-      <c r="B260" s="3" t="s">
-        <v>983</v>
       </c>
     </row>
     <row r="261" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A261" s="2" t="s">
+        <v>983</v>
+      </c>
+      <c r="B261" s="3" t="s">
         <v>984</v>
-      </c>
-      <c r="B261" s="3" t="s">
-        <v>985</v>
       </c>
     </row>
     <row r="262" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -37511,15 +37511,15 @@
         <v>135</v>
       </c>
       <c r="B262" s="3" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
     </row>
     <row r="263" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A263" s="2" t="s">
+        <v>986</v>
+      </c>
+      <c r="B263" s="3" t="s">
         <v>987</v>
-      </c>
-      <c r="B263" s="3" t="s">
-        <v>988</v>
       </c>
     </row>
     <row r="264" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -37527,7 +37527,7 @@
         <v>136</v>
       </c>
       <c r="B264" s="3" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
     </row>
     <row r="265" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -37551,7 +37551,7 @@
         <v>233</v>
       </c>
       <c r="B267" s="3" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
     </row>
     <row r="268" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -37567,7 +37567,7 @@
         <v>234</v>
       </c>
       <c r="B269" s="3" t="s">
-        <v>1105</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="270" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37575,7 +37575,7 @@
         <v>235</v>
       </c>
       <c r="B270" s="3" t="s">
-        <v>1106</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="271" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -37583,7 +37583,7 @@
         <v>139</v>
       </c>
       <c r="B271" s="3" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
     </row>
     <row r="272" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -37591,7 +37591,7 @@
         <v>239</v>
       </c>
       <c r="B272" s="3" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
     </row>
     <row r="273" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37599,7 +37599,7 @@
         <v>240</v>
       </c>
       <c r="B273" s="3" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
     </row>
     <row r="274" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37607,7 +37607,7 @@
         <v>241</v>
       </c>
       <c r="B274" s="3" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
     </row>
     <row r="275" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37615,7 +37615,7 @@
         <v>140</v>
       </c>
       <c r="B275" s="3" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="276" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -37623,7 +37623,7 @@
         <v>236</v>
       </c>
       <c r="B276" s="3" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="277" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37631,7 +37631,7 @@
         <v>237</v>
       </c>
       <c r="B277" s="3" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="278" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37639,7 +37639,7 @@
         <v>238</v>
       </c>
       <c r="B278" s="3" t="s">
-        <v>1107</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="279" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -37647,7 +37647,7 @@
         <v>141</v>
       </c>
       <c r="B279" s="3" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="280" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -37655,7 +37655,7 @@
         <v>142</v>
       </c>
       <c r="B280" s="3" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="281" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -37663,7 +37663,7 @@
         <v>143</v>
       </c>
       <c r="B281" s="3" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="282" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -37671,7 +37671,7 @@
         <v>144</v>
       </c>
       <c r="B282" s="3" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="283" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -37679,7 +37679,7 @@
         <v>242</v>
       </c>
       <c r="B283" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="284" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37687,7 +37687,7 @@
         <v>145</v>
       </c>
       <c r="B284" s="3" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="285" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -37695,7 +37695,7 @@
         <v>146</v>
       </c>
       <c r="B285" s="3" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="286" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37703,7 +37703,7 @@
         <v>147</v>
       </c>
       <c r="B286" s="3" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="287" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -37711,7 +37711,7 @@
         <v>148</v>
       </c>
       <c r="B287" s="3" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="288" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -37719,31 +37719,31 @@
         <v>149</v>
       </c>
       <c r="B288" s="3" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="289" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A289" s="2" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="B289" s="3" t="s">
-        <v>1078</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="290" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A290" s="2" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="B290" s="3" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="291" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A291" s="2" t="s">
+        <v>1051</v>
+      </c>
+      <c r="B291" s="3" t="s">
         <v>1052</v>
-      </c>
-      <c r="B291" s="3" t="s">
-        <v>1053</v>
       </c>
     </row>
     <row r="292" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37751,15 +37751,15 @@
         <v>150</v>
       </c>
       <c r="B292" s="3" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="293" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A293" s="2" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="B293" s="3" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="294" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -37767,7 +37767,7 @@
         <v>151</v>
       </c>
       <c r="B294" s="3" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
     </row>
     <row r="295" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37775,7 +37775,7 @@
         <v>243</v>
       </c>
       <c r="B295" s="3" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
     </row>
     <row r="296" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37783,7 +37783,7 @@
         <v>244</v>
       </c>
       <c r="B296" s="3" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
     </row>
     <row r="297" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37791,7 +37791,7 @@
         <v>245</v>
       </c>
       <c r="B297" s="3" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="298" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37799,7 +37799,7 @@
         <v>152</v>
       </c>
       <c r="B298" s="3" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
     </row>
     <row r="299" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -37807,7 +37807,7 @@
         <v>153</v>
       </c>
       <c r="B299" s="3" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="300" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37815,7 +37815,7 @@
         <v>154</v>
       </c>
       <c r="B300" s="3" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
     </row>
     <row r="301" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -37823,7 +37823,7 @@
         <v>155</v>
       </c>
       <c r="B301" s="3" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
     </row>
     <row r="302" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37831,7 +37831,7 @@
         <v>156</v>
       </c>
       <c r="B302" s="3" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
     </row>
     <row r="303" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -37839,7 +37839,7 @@
         <v>157</v>
       </c>
       <c r="B303" s="3" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
     </row>
     <row r="304" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -37847,7 +37847,7 @@
         <v>246</v>
       </c>
       <c r="B304" s="3" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="305" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37855,7 +37855,7 @@
         <v>247</v>
       </c>
       <c r="B305" s="3" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="306" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37863,7 +37863,7 @@
         <v>248</v>
       </c>
       <c r="B306" s="3" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
     </row>
     <row r="307" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37871,7 +37871,7 @@
         <v>158</v>
       </c>
       <c r="B307" s="3" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
     </row>
     <row r="308" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -37879,7 +37879,7 @@
         <v>159</v>
       </c>
       <c r="B308" s="3" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
     </row>
     <row r="309" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37887,7 +37887,7 @@
         <v>160</v>
       </c>
       <c r="B309" s="3" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
     </row>
     <row r="310" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -37895,7 +37895,7 @@
         <v>161</v>
       </c>
       <c r="B310" s="3" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="311" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37903,31 +37903,31 @@
         <v>162</v>
       </c>
       <c r="B311" s="3" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="312" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A312" s="2" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="B312" s="3" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="313" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A313" s="2" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="B313" s="3" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="314" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A314" s="2" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="B314" s="3" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="315" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37935,7 +37935,7 @@
         <v>163</v>
       </c>
       <c r="B315" s="3" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="316" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -37943,7 +37943,7 @@
         <v>164</v>
       </c>
       <c r="B316" s="3" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="317" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37951,7 +37951,7 @@
         <v>175</v>
       </c>
       <c r="B317" s="3" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="318" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -37959,7 +37959,7 @@
         <v>176</v>
       </c>
       <c r="B318" s="3" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="319" spans="1:2" ht="390" x14ac:dyDescent="0.25">
@@ -37967,7 +37967,7 @@
         <v>177</v>
       </c>
       <c r="B319" s="3" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
     </row>
     <row r="320" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -37975,7 +37975,7 @@
         <v>520</v>
       </c>
       <c r="B320" s="3" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="321" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37983,7 +37983,7 @@
         <v>521</v>
       </c>
       <c r="B321" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="322" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37991,7 +37991,7 @@
         <v>522</v>
       </c>
       <c r="B322" s="3" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="323" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -37999,7 +37999,7 @@
         <v>523</v>
       </c>
       <c r="B323" s="3" t="s">
-        <v>1075</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="324" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -38007,7 +38007,7 @@
         <v>524</v>
       </c>
       <c r="B324" s="3" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="325" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -38015,15 +38015,15 @@
         <v>525</v>
       </c>
       <c r="B325" s="3" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
     </row>
     <row r="326" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A326" s="2" t="s">
-        <v>1074</v>
+        <v>1072</v>
       </c>
       <c r="B326" s="3" t="s">
-        <v>1108</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="327" spans="1:2" ht="390" x14ac:dyDescent="0.25">
@@ -38031,7 +38031,7 @@
         <v>178</v>
       </c>
       <c r="B327" s="3" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
     </row>
     <row r="328" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -38039,7 +38039,7 @@
         <v>495</v>
       </c>
       <c r="B328" s="3" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="329" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -38047,7 +38047,7 @@
         <v>549</v>
       </c>
       <c r="B329" s="3" t="s">
-        <v>1109</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="330" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -38055,7 +38055,7 @@
         <v>550</v>
       </c>
       <c r="B330" s="3" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="331" spans="1:2" ht="315" x14ac:dyDescent="0.25">
@@ -38063,7 +38063,7 @@
         <v>179</v>
       </c>
       <c r="B331" s="3" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
     </row>
     <row r="332" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -38071,7 +38071,7 @@
         <v>249</v>
       </c>
       <c r="B332" s="3" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
     <row r="333" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -38079,7 +38079,7 @@
         <v>250</v>
       </c>
       <c r="B333" s="3" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
     </row>
     <row r="334" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -38087,7 +38087,7 @@
         <v>251</v>
       </c>
       <c r="B334" s="3" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
     </row>
     <row r="335" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38095,7 +38095,7 @@
         <v>252</v>
       </c>
       <c r="B335" s="3" t="s">
-        <v>1085</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="336" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -38103,23 +38103,23 @@
         <v>253</v>
       </c>
       <c r="B336" s="3" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
     </row>
     <row r="337" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A337" s="2" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="B337" s="3" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
     </row>
     <row r="338" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A338" s="2" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="B338" s="3" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
     </row>
     <row r="339" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -38127,7 +38127,7 @@
         <v>180</v>
       </c>
       <c r="B339" s="3" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
     </row>
     <row r="340" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38159,7 +38159,7 @@
         <v>183</v>
       </c>
       <c r="B343" s="3" t="s">
-        <v>1089</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="344" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -38167,7 +38167,7 @@
         <v>184</v>
       </c>
       <c r="B344" s="3" t="s">
-        <v>1088</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="345" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -38207,7 +38207,7 @@
         <v>470</v>
       </c>
       <c r="B349" s="3" t="s">
-        <v>1110</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="350" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -38231,7 +38231,7 @@
         <v>460</v>
       </c>
       <c r="B352" s="3" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
     </row>
     <row r="353" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -38287,7 +38287,7 @@
         <v>340</v>
       </c>
       <c r="B359" s="3" t="s">
-        <v>1111</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="360" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -38295,7 +38295,7 @@
         <v>341</v>
       </c>
       <c r="B360" s="3" t="s">
-        <v>1112</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="361" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -38319,7 +38319,7 @@
         <v>196</v>
       </c>
       <c r="B363" s="3" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
     </row>
     <row r="364" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -38327,7 +38327,7 @@
         <v>331</v>
       </c>
       <c r="B364" s="3" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
     </row>
     <row r="365" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -38343,7 +38343,7 @@
         <v>661</v>
       </c>
       <c r="B366" s="3" t="s">
-        <v>1113</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="367" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38383,7 +38383,7 @@
         <v>202</v>
       </c>
       <c r="B371" s="3" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
     </row>
     <row r="372" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -38503,7 +38503,7 @@
         <v>588</v>
       </c>
       <c r="B386" s="3" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
     </row>
     <row r="387" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -38511,7 +38511,7 @@
         <v>589</v>
       </c>
       <c r="B387" s="3" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
     </row>
     <row r="388" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -38519,7 +38519,7 @@
         <v>590</v>
       </c>
       <c r="B388" s="3" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
     </row>
     <row r="389" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -38527,7 +38527,7 @@
         <v>591</v>
       </c>
       <c r="B389" s="3" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
     </row>
     <row r="390" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38543,7 +38543,7 @@
         <v>593</v>
       </c>
       <c r="B391" s="3" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
     </row>
     <row r="392" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38559,7 +38559,7 @@
         <v>207</v>
       </c>
       <c r="B393" s="3" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
     </row>
     <row r="394" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -38583,7 +38583,7 @@
         <v>643</v>
       </c>
       <c r="B396" s="3" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
     </row>
     <row r="397" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -38711,7 +38711,7 @@
         <v>538</v>
       </c>
       <c r="B412" s="3" t="s">
-        <v>1114</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="413" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -38743,7 +38743,7 @@
         <v>213</v>
       </c>
       <c r="B416" s="3" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
     </row>
     <row r="417" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -38759,7 +38759,7 @@
         <v>215</v>
       </c>
       <c r="B418" s="3" t="s">
-        <v>1072</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="419" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38799,7 +38799,7 @@
         <v>220</v>
       </c>
       <c r="B423" s="3" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="424" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -38807,7 +38807,7 @@
         <v>221</v>
       </c>
       <c r="B424" s="3" t="s">
-        <v>1082</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="425" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -38815,7 +38815,7 @@
         <v>222</v>
       </c>
       <c r="B425" s="3" t="s">
-        <v>1081</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="426" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -38823,7 +38823,7 @@
         <v>223</v>
       </c>
       <c r="B426" s="3" t="s">
-        <v>1080</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="427" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -38831,7 +38831,7 @@
         <v>224</v>
       </c>
       <c r="B427" s="3" t="s">
-        <v>1079</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="428" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -38839,7 +38839,7 @@
         <v>332</v>
       </c>
       <c r="B428" s="3" t="s">
-        <v>1083</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="429" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -38855,7 +38855,7 @@
         <v>225</v>
       </c>
       <c r="B430" s="3" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
     </row>
     <row r="431" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -38919,7 +38919,7 @@
         <v>448</v>
       </c>
       <c r="B438" s="3" t="s">
-        <v>1073</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="439" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -38943,15 +38943,15 @@
         <v>582</v>
       </c>
       <c r="B441" s="3" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="442" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A442" s="2" t="s">
+        <v>785</v>
+      </c>
+      <c r="B442" s="3" t="s">
         <v>786</v>
-      </c>
-      <c r="B442" s="3" t="s">
-        <v>787</v>
       </c>
     </row>
     <row r="443" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -38959,7 +38959,7 @@
         <v>319</v>
       </c>
       <c r="B443" s="3" t="s">
-        <v>1068</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="444" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -38967,7 +38967,7 @@
         <v>320</v>
       </c>
       <c r="B444" s="3" t="s">
-        <v>1071</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="445" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -38975,7 +38975,7 @@
         <v>321</v>
       </c>
       <c r="B445" s="3" t="s">
-        <v>1069</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="446" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -38983,15 +38983,15 @@
         <v>318</v>
       </c>
       <c r="B446" s="3" t="s">
-        <v>1070</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="447" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A447" s="2" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B447" s="3" t="s">
         <v>1028</v>
-      </c>
-      <c r="B447" s="3" t="s">
-        <v>1029</v>
       </c>
     </row>
     <row r="448" spans="1:2" ht="255" x14ac:dyDescent="0.25">
@@ -38999,7 +38999,7 @@
         <v>322</v>
       </c>
       <c r="B448" s="3" t="s">
-        <v>1076</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="449" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39023,7 +39023,7 @@
         <v>489</v>
       </c>
       <c r="B451" s="3" t="s">
-        <v>1115</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="452" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -39063,7 +39063,7 @@
         <v>558</v>
       </c>
       <c r="B456" s="3" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
     </row>
     <row r="457" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -39071,7 +39071,7 @@
         <v>562</v>
       </c>
       <c r="B457" s="3" t="s">
-        <v>1090</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="458" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -39087,7 +39087,7 @@
         <v>566</v>
       </c>
       <c r="B459" s="3" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
     </row>
     <row r="460" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39111,7 +39111,7 @@
         <v>569</v>
       </c>
       <c r="B462" s="3" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
     </row>
     <row r="463" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -39119,7 +39119,7 @@
         <v>570</v>
       </c>
       <c r="B463" s="3" t="s">
-        <v>1086</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="464" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -39135,7 +39135,7 @@
         <v>572</v>
       </c>
       <c r="B465" s="3" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
     </row>
     <row r="466" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -39159,7 +39159,7 @@
         <v>580</v>
       </c>
       <c r="B468" s="3" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
     </row>
     <row r="469" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -39167,7 +39167,7 @@
         <v>602</v>
       </c>
       <c r="B469" s="3" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
     </row>
     <row r="470" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -39175,7 +39175,7 @@
         <v>620</v>
       </c>
       <c r="B470" s="3" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
     </row>
     <row r="471" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -39183,7 +39183,7 @@
         <v>621</v>
       </c>
       <c r="B471" s="3" t="s">
-        <v>1116</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="472" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -39191,15 +39191,15 @@
         <v>622</v>
       </c>
       <c r="B472" s="3" t="s">
-        <v>1117</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="473" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A473" s="2" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="B473" s="3" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
     </row>
     <row r="474" spans="1:2" ht="255" x14ac:dyDescent="0.25">
@@ -39207,7 +39207,7 @@
         <v>662</v>
       </c>
       <c r="B474" s="1" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
     </row>
     <row r="475" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -39255,7 +39255,7 @@
         <v>668</v>
       </c>
       <c r="B480" s="1" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
     </row>
     <row r="481" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -39295,7 +39295,7 @@
         <v>673</v>
       </c>
       <c r="B485" s="1" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
     </row>
     <row r="486" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -39324,18 +39324,18 @@
     </row>
     <row r="489" spans="1:2" ht="255" x14ac:dyDescent="0.25">
       <c r="A489" s="2" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="B489" s="1" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="490" spans="1:2" ht="92.25" x14ac:dyDescent="0.25">
       <c r="A490" s="2" t="s">
+        <v>1009</v>
+      </c>
+      <c r="B490" s="1" t="s">
         <v>1010</v>
-      </c>
-      <c r="B490" s="1" t="s">
-        <v>1011</v>
       </c>
     </row>
     <row r="491" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -39343,7 +39343,7 @@
         <v>692</v>
       </c>
       <c r="B491" s="1" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
     </row>
     <row r="492" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -39351,7 +39351,7 @@
         <v>724</v>
       </c>
       <c r="B492" s="3" t="s">
-        <v>1066</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="493" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -39367,7 +39367,7 @@
         <v>545</v>
       </c>
       <c r="B494" s="3" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
     </row>
     <row r="495" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -39375,7 +39375,7 @@
         <v>546</v>
       </c>
       <c r="B495" s="3" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
     </row>
     <row r="496" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39447,7 +39447,7 @@
         <v>275</v>
       </c>
       <c r="B504" s="1" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="505" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39455,7 +39455,7 @@
         <v>276</v>
       </c>
       <c r="B505" s="1" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="506" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39463,7 +39463,7 @@
         <v>277</v>
       </c>
       <c r="B506" s="1" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="507" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -39511,7 +39511,7 @@
         <v>260</v>
       </c>
       <c r="B512" s="3" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
     </row>
     <row r="513" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39519,7 +39519,7 @@
         <v>477</v>
       </c>
       <c r="B513" s="3" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
     </row>
     <row r="514" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -39527,15 +39527,15 @@
         <v>478</v>
       </c>
       <c r="B514" s="1" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
     </row>
     <row r="515" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A515" s="2" t="s">
+        <v>792</v>
+      </c>
+      <c r="B515" s="3" t="s">
         <v>793</v>
-      </c>
-      <c r="B515" s="3" t="s">
-        <v>794</v>
       </c>
     </row>
     <row r="516" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39583,7 +39583,7 @@
         <v>285</v>
       </c>
       <c r="B521" s="1" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
     </row>
     <row r="522" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -39591,7 +39591,7 @@
         <v>286</v>
       </c>
       <c r="B522" s="1" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
     </row>
     <row r="523" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -39671,7 +39671,7 @@
         <v>296</v>
       </c>
       <c r="B532" s="1" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
     </row>
     <row r="533" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -39711,7 +39711,7 @@
         <v>298</v>
       </c>
       <c r="B537" s="1" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
     </row>
     <row r="538" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -39751,7 +39751,7 @@
         <v>300</v>
       </c>
       <c r="B542" s="1" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
     </row>
     <row r="543" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -39759,7 +39759,7 @@
         <v>301</v>
       </c>
       <c r="B543" s="1" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="544" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -39799,7 +39799,7 @@
         <v>395</v>
       </c>
       <c r="B548" s="1" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="549" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -39812,10 +39812,10 @@
     </row>
     <row r="550" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A550" s="2" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="B550" s="1" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="551" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -39852,10 +39852,10 @@
     </row>
     <row r="555" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A555" s="2" t="s">
+        <v>733</v>
+      </c>
+      <c r="B555" s="1" t="s">
         <v>734</v>
-      </c>
-      <c r="B555" s="1" t="s">
-        <v>735</v>
       </c>
     </row>
     <row r="556" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -39887,7 +39887,7 @@
         <v>307</v>
       </c>
       <c r="B559" s="1" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
     </row>
     <row r="560" spans="1:2" ht="375" x14ac:dyDescent="0.25">
@@ -39919,15 +39919,15 @@
         <v>375</v>
       </c>
       <c r="B563" s="3" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
     </row>
     <row r="564" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A564" s="2" t="s">
+        <v>737</v>
+      </c>
+      <c r="B564" s="3" t="s">
         <v>738</v>
-      </c>
-      <c r="B564" s="3" t="s">
-        <v>739</v>
       </c>
     </row>
     <row r="565" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -39935,7 +39935,7 @@
         <v>329</v>
       </c>
       <c r="B565" s="3" t="s">
-        <v>1118</v>
+        <v>1115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fox issue with nerve gas not showing up for surprise when rolled
</commit_message>
<xml_diff>
--- a/Documentation/Events.xlsx
+++ b/Documentation/Events.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\happysulla\BarbarianPrince\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C6F9579C-6DCF-400C-9381-ED0D04FD6C67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{780BC9CE-139D-452B-AF16-248A83713217}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" r:id="rId1"/>
@@ -15975,82 +15975,6 @@
   </si>
   <si>
     <r>
-      <t>&lt;Bold&gt;e112b Evade to Eagle Clan&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt; Roll one die: 
- &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>dieRoll</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.gif' Name='</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>DieRoll</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>' Height='21'  Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
- &lt;InlineUIContainer&gt;&lt;Button Content='e325' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; - 1 Pass&lt;LineBreak/&gt;
- &lt;InlineUIContainer&gt;&lt;Button Content='e325' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; - 2 Pass&lt;LineBreak/&gt;
- &lt;InlineUIContainer&gt;&lt;Button Content='e326' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; - 3 Pass&lt;LineBreak/&gt;
- &lt;InlineUIContainer&gt;&lt;Button Content='e326' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; - 4 Pass&lt;LineBreak/&gt;
- &lt;InlineUIContainer&gt;&lt;Button Content='e341' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; - 5 Conversation&lt;LineBreak/&gt;
- &lt;InlineUIContainer&gt;&lt;Button Content='e342' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; - 6 Inquiry
-&lt;LineBreak/&gt; &lt;LineBreak/&gt;
-                &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Eagle</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.gif' Height='210' Width='400'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>&lt;Bold&gt;e112c Fight Eagle Clan&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt; Roll one die: 
  &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
@@ -34993,6 +34917,82 @@
         <scheme val="minor"/>
       </rPr>
       <t>.gif' Height='250'  Width='500'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;Bold&gt;e112b Evade Eagle Clan&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt; Roll one die: 
+ &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dieRoll</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.gif' Name='</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DieRoll</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>' Height='21'  Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+ &lt;InlineUIContainer&gt;&lt;Button Content='e325' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; - 1 Pass&lt;LineBreak/&gt;
+ &lt;InlineUIContainer&gt;&lt;Button Content='e325' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; - 2 Pass&lt;LineBreak/&gt;
+ &lt;InlineUIContainer&gt;&lt;Button Content='e326' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; - 3 Pass&lt;LineBreak/&gt;
+ &lt;InlineUIContainer&gt;&lt;Button Content='e326' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; - 4 Pass&lt;LineBreak/&gt;
+ &lt;InlineUIContainer&gt;&lt;Button Content='e341' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; - 5 Conversation&lt;LineBreak/&gt;
+ &lt;InlineUIContainer&gt;&lt;Button Content='e342' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; - 6 Inquiry
+&lt;LineBreak/&gt; &lt;LineBreak/&gt;
+                &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Eagle</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.gif' Height='210' Width='400'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
     </r>
   </si>
 </sst>
@@ -35459,8 +35459,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B566"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A242" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B246" sqref="B246"/>
+    <sheetView tabSelected="1" topLeftCell="A296" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B297" sqref="B297"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -35474,7 +35474,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -35482,7 +35482,7 @@
         <v>254</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -35490,7 +35490,7 @@
         <v>255</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -35498,15 +35498,15 @@
         <v>256</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="390" x14ac:dyDescent="0.25">
@@ -35522,7 +35522,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35530,7 +35530,7 @@
         <v>22</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35546,7 +35546,7 @@
         <v>23</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -35562,7 +35562,7 @@
         <v>3</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -35570,7 +35570,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35594,7 +35594,7 @@
         <v>7</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -35602,7 +35602,7 @@
         <v>8</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35610,7 +35610,7 @@
         <v>10</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35618,7 +35618,7 @@
         <v>9</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -35626,7 +35626,7 @@
         <v>11</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -35658,7 +35658,7 @@
         <v>15</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -35666,7 +35666,7 @@
         <v>16</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -35674,7 +35674,7 @@
         <v>17</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -35682,7 +35682,7 @@
         <v>18</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -35690,31 +35690,31 @@
         <v>261</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -35722,7 +35722,7 @@
         <v>19</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -35730,7 +35730,7 @@
         <v>20</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -35738,23 +35738,23 @@
         <v>21</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -35762,23 +35762,23 @@
         <v>25</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -35786,7 +35786,7 @@
         <v>26</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -35810,7 +35810,7 @@
         <v>27</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -35818,7 +35818,7 @@
         <v>28</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -35826,7 +35826,7 @@
         <v>29</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -35834,7 +35834,7 @@
         <v>30</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -35850,7 +35850,7 @@
         <v>706</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -35858,7 +35858,7 @@
         <v>31</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -35866,7 +35866,7 @@
         <v>32</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -35874,7 +35874,7 @@
         <v>33</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -35906,7 +35906,7 @@
         <v>496</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -35930,7 +35930,7 @@
         <v>264</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35938,7 +35938,7 @@
         <v>265</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -35962,7 +35962,7 @@
         <v>35</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -36002,7 +36002,7 @@
         <v>38</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -36026,7 +36026,7 @@
         <v>709</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -36074,7 +36074,7 @@
         <v>42</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -36082,7 +36082,7 @@
         <v>46</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -36106,7 +36106,7 @@
         <v>49</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -36146,7 +36146,7 @@
         <v>54</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -36154,7 +36154,7 @@
         <v>55</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -36162,7 +36162,7 @@
         <v>56</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -36170,7 +36170,7 @@
         <v>57</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -36178,31 +36178,31 @@
         <v>58</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -36210,15 +36210,15 @@
         <v>59</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
+        <v>889</v>
+      </c>
+      <c r="B94" s="3" t="s">
         <v>890</v>
-      </c>
-      <c r="B94" s="3" t="s">
-        <v>891</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -36226,15 +36226,15 @@
         <v>60</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -36242,7 +36242,7 @@
         <v>61</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -36250,7 +36250,7 @@
         <v>62</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -36282,7 +36282,7 @@
         <v>65</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -36290,7 +36290,7 @@
         <v>66</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -36338,7 +36338,7 @@
         <v>474</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -36370,7 +36370,7 @@
         <v>70</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -36458,7 +36458,7 @@
         <v>77</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
     </row>
     <row r="125" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -36471,10 +36471,10 @@
     </row>
     <row r="126" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="127" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -36482,7 +36482,7 @@
         <v>78</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
     </row>
     <row r="128" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -36490,7 +36490,7 @@
         <v>376</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
     </row>
     <row r="129" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -36530,7 +36530,7 @@
         <v>80</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
     </row>
     <row r="134" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -36538,87 +36538,87 @@
         <v>81</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
     </row>
     <row r="135" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
     </row>
     <row r="136" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
     </row>
     <row r="137" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
     </row>
     <row r="138" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
     </row>
     <row r="139" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="B139" s="3" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
     </row>
     <row r="140" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
     </row>
     <row r="141" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="142" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
     </row>
     <row r="143" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
+        <v>950</v>
+      </c>
+      <c r="B143" s="3" t="s">
         <v>951</v>
-      </c>
-      <c r="B143" s="3" t="s">
-        <v>952</v>
       </c>
     </row>
     <row r="144" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
     </row>
     <row r="145" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -36626,7 +36626,7 @@
         <v>82</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
     </row>
     <row r="146" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -36634,12 +36634,12 @@
         <v>83</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
     </row>
     <row r="147" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="B147" s="3" t="s">
         <v>552</v>
@@ -36674,7 +36674,7 @@
         <v>551</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
     </row>
     <row r="152" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -36682,7 +36682,7 @@
         <v>86</v>
       </c>
       <c r="B152" s="3" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
     </row>
     <row r="153" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -36794,7 +36794,7 @@
         <v>443</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
     </row>
     <row r="167" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -36818,23 +36818,23 @@
         <v>90</v>
       </c>
       <c r="B169" s="3" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
     </row>
     <row r="170" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="B170" s="3" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="171" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="B171" s="3" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
     </row>
     <row r="172" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -36866,7 +36866,7 @@
         <v>93</v>
       </c>
       <c r="B175" s="3" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
     </row>
     <row r="176" spans="1:2" ht="270" x14ac:dyDescent="0.25">
@@ -36874,7 +36874,7 @@
         <v>94</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="177" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -36882,7 +36882,7 @@
         <v>95</v>
       </c>
       <c r="B177" s="3" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
     </row>
     <row r="178" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -36890,55 +36890,55 @@
         <v>96</v>
       </c>
       <c r="B178" s="3" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="179" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A179" s="2" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="B179" s="3" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
     </row>
     <row r="180" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A180" s="2" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="B180" s="3" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="181" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="182" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="B182" s="3" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="183" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="B183" s="3" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="184" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A184" s="2" t="s">
+        <v>865</v>
+      </c>
+      <c r="B184" s="3" t="s">
         <v>866</v>
-      </c>
-      <c r="B184" s="3" t="s">
-        <v>867</v>
       </c>
     </row>
     <row r="185" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -36946,7 +36946,7 @@
         <v>97</v>
       </c>
       <c r="B185" s="3" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
     </row>
     <row r="186" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -36978,7 +36978,7 @@
         <v>100</v>
       </c>
       <c r="B189" s="3" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
     </row>
     <row r="190" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -36994,7 +36994,7 @@
         <v>103</v>
       </c>
       <c r="B191" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="192" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37002,7 +37002,7 @@
         <v>104</v>
       </c>
       <c r="B192" s="3" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
     </row>
     <row r="193" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37018,7 +37018,7 @@
         <v>693</v>
       </c>
       <c r="B194" s="3" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="195" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37034,7 +37034,7 @@
         <v>106</v>
       </c>
       <c r="B196" s="3" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
     </row>
     <row r="197" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37042,7 +37042,7 @@
         <v>107</v>
       </c>
       <c r="B197" s="3" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
     </row>
     <row r="198" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -37050,15 +37050,15 @@
         <v>165</v>
       </c>
       <c r="B198" s="3" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
     </row>
     <row r="199" spans="1:2" ht="225" x14ac:dyDescent="0.25">
       <c r="A199" s="2" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="B199" s="3" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
     </row>
     <row r="200" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37066,7 +37066,7 @@
         <v>108</v>
       </c>
       <c r="B200" s="3" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
     </row>
     <row r="201" spans="1:2" ht="285" x14ac:dyDescent="0.25">
@@ -37074,7 +37074,7 @@
         <v>109</v>
       </c>
       <c r="B201" s="3" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
     </row>
     <row r="202" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -37082,7 +37082,7 @@
         <v>110</v>
       </c>
       <c r="B202" s="3" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
     </row>
     <row r="203" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -37090,7 +37090,7 @@
         <v>166</v>
       </c>
       <c r="B203" s="3" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="204" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -37098,7 +37098,7 @@
         <v>167</v>
       </c>
       <c r="B204" s="3" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="205" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -37106,23 +37106,23 @@
         <v>168</v>
       </c>
       <c r="B205" s="3" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
     </row>
     <row r="206" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A206" s="2" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="B206" s="3" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="207" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A207" s="2" t="s">
+        <v>880</v>
+      </c>
+      <c r="B207" s="3" t="s">
         <v>881</v>
-      </c>
-      <c r="B207" s="3" t="s">
-        <v>882</v>
       </c>
     </row>
     <row r="208" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37170,7 +37170,7 @@
         <v>112</v>
       </c>
       <c r="B213" s="3" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
     </row>
     <row r="214" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37178,7 +37178,7 @@
         <v>169</v>
       </c>
       <c r="B214" s="3" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="215" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -37186,7 +37186,7 @@
         <v>170</v>
       </c>
       <c r="B215" s="3" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
     </row>
     <row r="216" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -37194,7 +37194,7 @@
         <v>171</v>
       </c>
       <c r="B216" s="3" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="217" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37202,7 +37202,7 @@
         <v>113</v>
       </c>
       <c r="B217" s="3" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="218" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -37210,7 +37210,7 @@
         <v>114</v>
       </c>
       <c r="B218" s="3" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
     </row>
     <row r="219" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -37218,15 +37218,15 @@
         <v>266</v>
       </c>
       <c r="B219" s="3" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
     </row>
     <row r="220" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A220" s="2" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="B220" s="3" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="221" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37234,7 +37234,7 @@
         <v>115</v>
       </c>
       <c r="B221" s="3" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
     </row>
     <row r="222" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -37250,7 +37250,7 @@
         <v>116</v>
       </c>
       <c r="B223" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="224" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -37266,7 +37266,7 @@
         <v>117</v>
       </c>
       <c r="B225" s="4" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
     </row>
     <row r="226" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -37290,7 +37290,7 @@
         <v>751</v>
       </c>
       <c r="B228" s="4" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
     </row>
     <row r="229" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -37298,23 +37298,23 @@
         <v>118</v>
       </c>
       <c r="B229" s="3" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
     </row>
     <row r="230" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A230" s="2" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="B230" s="3" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
     </row>
     <row r="231" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A231" s="2" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="B231" s="3" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="232" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -37322,23 +37322,23 @@
         <v>119</v>
       </c>
       <c r="B232" s="3" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
     </row>
     <row r="233" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A233" s="2" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="B233" s="3" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
     </row>
     <row r="234" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A234" s="2" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="B234" s="3" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="235" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -37346,7 +37346,7 @@
         <v>120</v>
       </c>
       <c r="B235" s="3" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
     </row>
     <row r="236" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -37354,7 +37354,7 @@
         <v>172</v>
       </c>
       <c r="B236" s="3" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
     </row>
     <row r="237" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37362,7 +37362,7 @@
         <v>173</v>
       </c>
       <c r="B237" s="3" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
     </row>
     <row r="238" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37370,7 +37370,7 @@
         <v>174</v>
       </c>
       <c r="B238" s="3" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
     </row>
     <row r="239" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37402,23 +37402,23 @@
         <v>123</v>
       </c>
       <c r="B242" s="3" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
     </row>
     <row r="243" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A243" s="2" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="B243" s="3" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="244" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A244" s="2" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="B244" s="3" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="245" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37431,10 +37431,10 @@
     </row>
     <row r="246" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A246" s="2" t="s">
+        <v>1129</v>
+      </c>
+      <c r="B246" s="3" t="s">
         <v>1130</v>
-      </c>
-      <c r="B246" s="3" t="s">
-        <v>1131</v>
       </c>
     </row>
     <row r="247" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37442,15 +37442,15 @@
         <v>125</v>
       </c>
       <c r="B247" s="3" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
     </row>
     <row r="248" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A248" s="2" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="B248" s="3" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="249" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37458,7 +37458,7 @@
         <v>126</v>
       </c>
       <c r="B249" s="3" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
     </row>
     <row r="250" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37466,7 +37466,7 @@
         <v>127</v>
       </c>
       <c r="B250" s="3" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
     </row>
     <row r="251" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37482,7 +37482,7 @@
         <v>129</v>
       </c>
       <c r="B252" s="3" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
     </row>
     <row r="253" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37490,7 +37490,7 @@
         <v>130</v>
       </c>
       <c r="B253" s="3" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
     </row>
     <row r="254" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -37498,23 +37498,23 @@
         <v>131</v>
       </c>
       <c r="B254" s="3" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
     </row>
     <row r="255" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A255" s="2" t="s">
+        <v>926</v>
+      </c>
+      <c r="B255" s="3" t="s">
         <v>927</v>
-      </c>
-      <c r="B255" s="3" t="s">
-        <v>928</v>
       </c>
     </row>
     <row r="256" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A256" s="2" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="B256" s="3" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
     </row>
     <row r="257" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -37522,7 +37522,7 @@
         <v>132</v>
       </c>
       <c r="B257" s="3" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
     </row>
     <row r="258" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -37530,15 +37530,15 @@
         <v>133</v>
       </c>
       <c r="B258" s="3" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="259" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A259" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="B259" s="3" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="260" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37546,23 +37546,23 @@
         <v>134</v>
       </c>
       <c r="B260" s="3" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="261" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A261" s="2" t="s">
+        <v>978</v>
+      </c>
+      <c r="B261" s="3" t="s">
         <v>979</v>
-      </c>
-      <c r="B261" s="3" t="s">
-        <v>980</v>
       </c>
     </row>
     <row r="262" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A262" s="2" t="s">
+        <v>980</v>
+      </c>
+      <c r="B262" s="3" t="s">
         <v>981</v>
-      </c>
-      <c r="B262" s="3" t="s">
-        <v>982</v>
       </c>
     </row>
     <row r="263" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -37570,15 +37570,15 @@
         <v>135</v>
       </c>
       <c r="B263" s="3" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
     </row>
     <row r="264" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A264" s="2" t="s">
+        <v>983</v>
+      </c>
+      <c r="B264" s="3" t="s">
         <v>984</v>
-      </c>
-      <c r="B264" s="3" t="s">
-        <v>985</v>
       </c>
     </row>
     <row r="265" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -37586,7 +37586,7 @@
         <v>136</v>
       </c>
       <c r="B265" s="3" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
     </row>
     <row r="266" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -37610,7 +37610,7 @@
         <v>233</v>
       </c>
       <c r="B268" s="3" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="269" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -37626,7 +37626,7 @@
         <v>234</v>
       </c>
       <c r="B270" s="3" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="271" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37634,7 +37634,7 @@
         <v>235</v>
       </c>
       <c r="B271" s="3" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="272" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -37642,7 +37642,7 @@
         <v>139</v>
       </c>
       <c r="B272" s="3" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
     </row>
     <row r="273" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -37650,7 +37650,7 @@
         <v>239</v>
       </c>
       <c r="B273" s="3" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
     </row>
     <row r="274" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37658,7 +37658,7 @@
         <v>240</v>
       </c>
       <c r="B274" s="3" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
     </row>
     <row r="275" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37666,7 +37666,7 @@
         <v>241</v>
       </c>
       <c r="B275" s="3" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
     </row>
     <row r="276" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37674,7 +37674,7 @@
         <v>140</v>
       </c>
       <c r="B276" s="3" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="277" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -37682,7 +37682,7 @@
         <v>236</v>
       </c>
       <c r="B277" s="3" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="278" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37690,7 +37690,7 @@
         <v>237</v>
       </c>
       <c r="B278" s="3" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="279" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37698,7 +37698,7 @@
         <v>238</v>
       </c>
       <c r="B279" s="3" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="280" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -37706,7 +37706,7 @@
         <v>141</v>
       </c>
       <c r="B280" s="3" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="281" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -37714,7 +37714,7 @@
         <v>142</v>
       </c>
       <c r="B281" s="3" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="282" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -37722,7 +37722,7 @@
         <v>143</v>
       </c>
       <c r="B282" s="3" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="283" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -37730,7 +37730,7 @@
         <v>144</v>
       </c>
       <c r="B283" s="3" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="284" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -37738,7 +37738,7 @@
         <v>242</v>
       </c>
       <c r="B284" s="3" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="285" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37746,7 +37746,7 @@
         <v>145</v>
       </c>
       <c r="B285" s="3" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="286" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -37754,7 +37754,7 @@
         <v>146</v>
       </c>
       <c r="B286" s="3" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="287" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37762,7 +37762,7 @@
         <v>147</v>
       </c>
       <c r="B287" s="3" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="288" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -37770,7 +37770,7 @@
         <v>148</v>
       </c>
       <c r="B288" s="3" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="289" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -37778,31 +37778,31 @@
         <v>149</v>
       </c>
       <c r="B289" s="3" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="290" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A290" s="2" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="B290" s="3" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="291" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A291" s="2" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="B291" s="3" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="292" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A292" s="2" t="s">
+        <v>1048</v>
+      </c>
+      <c r="B292" s="3" t="s">
         <v>1049</v>
-      </c>
-      <c r="B292" s="3" t="s">
-        <v>1050</v>
       </c>
     </row>
     <row r="293" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37810,15 +37810,15 @@
         <v>150</v>
       </c>
       <c r="B293" s="3" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="294" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A294" s="2" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="B294" s="3" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="295" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -37834,7 +37834,7 @@
         <v>243</v>
       </c>
       <c r="B296" s="3" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
     </row>
     <row r="297" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37842,7 +37842,7 @@
         <v>244</v>
       </c>
       <c r="B297" s="3" t="s">
-        <v>762</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="298" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37850,7 +37850,7 @@
         <v>245</v>
       </c>
       <c r="B298" s="3" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
     </row>
     <row r="299" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37858,7 +37858,7 @@
         <v>152</v>
       </c>
       <c r="B299" s="3" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="300" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -37866,7 +37866,7 @@
         <v>153</v>
       </c>
       <c r="B300" s="3" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="301" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37874,7 +37874,7 @@
         <v>154</v>
       </c>
       <c r="B301" s="3" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
     </row>
     <row r="302" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -37882,7 +37882,7 @@
         <v>155</v>
       </c>
       <c r="B302" s="3" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
     </row>
     <row r="303" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37890,7 +37890,7 @@
         <v>156</v>
       </c>
       <c r="B303" s="3" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
     </row>
     <row r="304" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -37930,7 +37930,7 @@
         <v>158</v>
       </c>
       <c r="B308" s="3" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
     </row>
     <row r="309" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -37938,7 +37938,7 @@
         <v>159</v>
       </c>
       <c r="B309" s="3" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
     </row>
     <row r="310" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37946,7 +37946,7 @@
         <v>160</v>
       </c>
       <c r="B310" s="3" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
     </row>
     <row r="311" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -37954,7 +37954,7 @@
         <v>161</v>
       </c>
       <c r="B311" s="3" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="312" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37962,31 +37962,31 @@
         <v>162</v>
       </c>
       <c r="B312" s="3" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="313" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A313" s="2" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="B313" s="3" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="314" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A314" s="2" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="B314" s="3" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="315" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A315" s="2" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="B315" s="3" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="316" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37994,7 +37994,7 @@
         <v>163</v>
       </c>
       <c r="B316" s="3" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="317" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -38002,7 +38002,7 @@
         <v>164</v>
       </c>
       <c r="B317" s="3" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="318" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -38010,7 +38010,7 @@
         <v>175</v>
       </c>
       <c r="B318" s="3" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="319" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -38018,7 +38018,7 @@
         <v>176</v>
       </c>
       <c r="B319" s="3" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="320" spans="1:2" ht="390" x14ac:dyDescent="0.25">
@@ -38026,7 +38026,7 @@
         <v>177</v>
       </c>
       <c r="B320" s="3" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
     </row>
     <row r="321" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -38034,7 +38034,7 @@
         <v>519</v>
       </c>
       <c r="B321" s="3" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="322" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -38042,7 +38042,7 @@
         <v>520</v>
       </c>
       <c r="B322" s="3" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
     </row>
     <row r="323" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -38050,7 +38050,7 @@
         <v>521</v>
       </c>
       <c r="B323" s="3" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
     </row>
     <row r="324" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -38058,7 +38058,7 @@
         <v>522</v>
       </c>
       <c r="B324" s="3" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="325" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -38066,7 +38066,7 @@
         <v>523</v>
       </c>
       <c r="B325" s="3" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
     </row>
     <row r="326" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -38074,15 +38074,15 @@
         <v>524</v>
       </c>
       <c r="B326" s="3" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
     </row>
     <row r="327" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A327" s="2" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="B327" s="3" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="328" spans="1:2" ht="390" x14ac:dyDescent="0.25">
@@ -38090,7 +38090,7 @@
         <v>178</v>
       </c>
       <c r="B328" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="329" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -38098,7 +38098,7 @@
         <v>494</v>
       </c>
       <c r="B329" s="3" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="330" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -38106,7 +38106,7 @@
         <v>548</v>
       </c>
       <c r="B330" s="3" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="331" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -38114,7 +38114,7 @@
         <v>549</v>
       </c>
       <c r="B331" s="3" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
     </row>
     <row r="332" spans="1:2" ht="315" x14ac:dyDescent="0.25">
@@ -38122,7 +38122,7 @@
         <v>179</v>
       </c>
       <c r="B332" s="3" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
     </row>
     <row r="333" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -38130,7 +38130,7 @@
         <v>249</v>
       </c>
       <c r="B333" s="3" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
     <row r="334" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -38138,7 +38138,7 @@
         <v>250</v>
       </c>
       <c r="B334" s="3" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
     </row>
     <row r="335" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -38146,7 +38146,7 @@
         <v>251</v>
       </c>
       <c r="B335" s="3" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
     </row>
     <row r="336" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38154,7 +38154,7 @@
         <v>252</v>
       </c>
       <c r="B336" s="3" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="337" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -38162,23 +38162,23 @@
         <v>253</v>
       </c>
       <c r="B337" s="3" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="338" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A338" s="2" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="B338" s="3" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
     <row r="339" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A339" s="2" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="B339" s="3" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
     </row>
     <row r="340" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -38186,7 +38186,7 @@
         <v>180</v>
       </c>
       <c r="B340" s="3" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
     </row>
     <row r="341" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38218,7 +38218,7 @@
         <v>183</v>
       </c>
       <c r="B344" s="3" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="345" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -38226,7 +38226,7 @@
         <v>184</v>
       </c>
       <c r="B345" s="3" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="346" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -38266,7 +38266,7 @@
         <v>469</v>
       </c>
       <c r="B350" s="3" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="351" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -38290,7 +38290,7 @@
         <v>459</v>
       </c>
       <c r="B353" s="3" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
     </row>
     <row r="354" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -38346,7 +38346,7 @@
         <v>340</v>
       </c>
       <c r="B360" s="3" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="361" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -38354,7 +38354,7 @@
         <v>341</v>
       </c>
       <c r="B361" s="3" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="362" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -38378,7 +38378,7 @@
         <v>196</v>
       </c>
       <c r="B364" s="3" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="365" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -38386,7 +38386,7 @@
         <v>331</v>
       </c>
       <c r="B365" s="3" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
     </row>
     <row r="366" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -38402,7 +38402,7 @@
         <v>660</v>
       </c>
       <c r="B367" s="3" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="368" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38442,7 +38442,7 @@
         <v>202</v>
       </c>
       <c r="B372" s="3" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
     </row>
     <row r="373" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -38562,7 +38562,7 @@
         <v>587</v>
       </c>
       <c r="B387" s="3" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
     </row>
     <row r="388" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -38570,7 +38570,7 @@
         <v>588</v>
       </c>
       <c r="B388" s="3" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
     </row>
     <row r="389" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -38578,7 +38578,7 @@
         <v>589</v>
       </c>
       <c r="B389" s="3" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
     </row>
     <row r="390" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -38586,7 +38586,7 @@
         <v>590</v>
       </c>
       <c r="B390" s="3" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
     </row>
     <row r="391" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38602,7 +38602,7 @@
         <v>592</v>
       </c>
       <c r="B392" s="3" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
     </row>
     <row r="393" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38618,7 +38618,7 @@
         <v>207</v>
       </c>
       <c r="B394" s="3" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
     </row>
     <row r="395" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -38642,7 +38642,7 @@
         <v>642</v>
       </c>
       <c r="B397" s="3" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
     </row>
     <row r="398" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -38770,7 +38770,7 @@
         <v>537</v>
       </c>
       <c r="B413" s="3" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="414" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -38802,7 +38802,7 @@
         <v>213</v>
       </c>
       <c r="B417" s="3" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
     </row>
     <row r="418" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -38818,7 +38818,7 @@
         <v>215</v>
       </c>
       <c r="B419" s="3" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="420" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38858,7 +38858,7 @@
         <v>220</v>
       </c>
       <c r="B424" s="3" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
     </row>
     <row r="425" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -38866,7 +38866,7 @@
         <v>221</v>
       </c>
       <c r="B425" s="3" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="426" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -38874,7 +38874,7 @@
         <v>222</v>
       </c>
       <c r="B426" s="3" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="427" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -38882,7 +38882,7 @@
         <v>223</v>
       </c>
       <c r="B427" s="3" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="428" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -38890,7 +38890,7 @@
         <v>224</v>
       </c>
       <c r="B428" s="3" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="429" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -38898,7 +38898,7 @@
         <v>332</v>
       </c>
       <c r="B429" s="3" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="430" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -38914,7 +38914,7 @@
         <v>225</v>
       </c>
       <c r="B431" s="3" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
     </row>
     <row r="432" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -38978,7 +38978,7 @@
         <v>447</v>
       </c>
       <c r="B439" s="3" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="440" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -39002,15 +39002,15 @@
         <v>581</v>
       </c>
       <c r="B442" s="3" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="443" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A443" s="2" t="s">
+        <v>783</v>
+      </c>
+      <c r="B443" s="3" t="s">
         <v>784</v>
-      </c>
-      <c r="B443" s="3" t="s">
-        <v>785</v>
       </c>
     </row>
     <row r="444" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -39018,7 +39018,7 @@
         <v>319</v>
       </c>
       <c r="B444" s="3" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="445" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -39026,7 +39026,7 @@
         <v>320</v>
       </c>
       <c r="B445" s="3" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="446" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -39034,7 +39034,7 @@
         <v>321</v>
       </c>
       <c r="B446" s="3" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="447" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -39042,15 +39042,15 @@
         <v>318</v>
       </c>
       <c r="B447" s="3" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="448" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A448" s="2" t="s">
+        <v>1024</v>
+      </c>
+      <c r="B448" s="3" t="s">
         <v>1025</v>
-      </c>
-      <c r="B448" s="3" t="s">
-        <v>1026</v>
       </c>
     </row>
     <row r="449" spans="1:2" ht="255" x14ac:dyDescent="0.25">
@@ -39058,7 +39058,7 @@
         <v>322</v>
       </c>
       <c r="B449" s="3" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="450" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39082,7 +39082,7 @@
         <v>488</v>
       </c>
       <c r="B452" s="3" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="453" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -39122,7 +39122,7 @@
         <v>557</v>
       </c>
       <c r="B457" s="3" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
     </row>
     <row r="458" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -39130,7 +39130,7 @@
         <v>561</v>
       </c>
       <c r="B458" s="3" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="459" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -39146,7 +39146,7 @@
         <v>565</v>
       </c>
       <c r="B460" s="3" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
     </row>
     <row r="461" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39170,7 +39170,7 @@
         <v>568</v>
       </c>
       <c r="B463" s="3" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
     </row>
     <row r="464" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -39178,7 +39178,7 @@
         <v>569</v>
       </c>
       <c r="B464" s="3" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="465" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -39194,7 +39194,7 @@
         <v>571</v>
       </c>
       <c r="B466" s="3" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
     </row>
     <row r="467" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -39218,7 +39218,7 @@
         <v>579</v>
       </c>
       <c r="B469" s="3" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
     </row>
     <row r="470" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -39226,7 +39226,7 @@
         <v>601</v>
       </c>
       <c r="B470" s="3" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="471" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -39234,7 +39234,7 @@
         <v>619</v>
       </c>
       <c r="B471" s="3" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
     </row>
     <row r="472" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -39242,7 +39242,7 @@
         <v>620</v>
       </c>
       <c r="B472" s="3" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="473" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -39250,15 +39250,15 @@
         <v>621</v>
       </c>
       <c r="B473" s="3" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="474" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A474" s="2" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="B474" s="3" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
     </row>
     <row r="475" spans="1:2" ht="255" x14ac:dyDescent="0.25">
@@ -39266,7 +39266,7 @@
         <v>661</v>
       </c>
       <c r="B475" s="1" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
     </row>
     <row r="476" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -39314,7 +39314,7 @@
         <v>667</v>
       </c>
       <c r="B481" s="1" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
     </row>
     <row r="482" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -39354,7 +39354,7 @@
         <v>672</v>
       </c>
       <c r="B486" s="1" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
     </row>
     <row r="487" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -39383,18 +39383,18 @@
     </row>
     <row r="490" spans="1:2" ht="255" x14ac:dyDescent="0.25">
       <c r="A490" s="2" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="B490" s="1" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="491" spans="1:2" ht="92.25" x14ac:dyDescent="0.25">
       <c r="A491" s="2" t="s">
+        <v>1006</v>
+      </c>
+      <c r="B491" s="1" t="s">
         <v>1007</v>
-      </c>
-      <c r="B491" s="1" t="s">
-        <v>1008</v>
       </c>
     </row>
     <row r="492" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -39402,7 +39402,7 @@
         <v>691</v>
       </c>
       <c r="B492" s="1" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
     </row>
     <row r="493" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -39410,7 +39410,7 @@
         <v>723</v>
       </c>
       <c r="B493" s="3" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="494" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -39426,7 +39426,7 @@
         <v>544</v>
       </c>
       <c r="B495" s="3" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
     </row>
     <row r="496" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -39434,7 +39434,7 @@
         <v>545</v>
       </c>
       <c r="B496" s="3" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
     </row>
     <row r="497" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39506,7 +39506,7 @@
         <v>275</v>
       </c>
       <c r="B505" s="1" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="506" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39514,7 +39514,7 @@
         <v>276</v>
       </c>
       <c r="B506" s="1" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="507" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39522,7 +39522,7 @@
         <v>277</v>
       </c>
       <c r="B507" s="1" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="508" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -39570,7 +39570,7 @@
         <v>260</v>
       </c>
       <c r="B513" s="3" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="514" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39578,7 +39578,7 @@
         <v>476</v>
       </c>
       <c r="B514" s="3" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
     </row>
     <row r="515" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -39586,15 +39586,15 @@
         <v>477</v>
       </c>
       <c r="B515" s="1" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
     </row>
     <row r="516" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A516" s="2" t="s">
+        <v>790</v>
+      </c>
+      <c r="B516" s="3" t="s">
         <v>791</v>
-      </c>
-      <c r="B516" s="3" t="s">
-        <v>792</v>
       </c>
     </row>
     <row r="517" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39642,7 +39642,7 @@
         <v>285</v>
       </c>
       <c r="B522" s="1" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
     </row>
     <row r="523" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -39650,7 +39650,7 @@
         <v>286</v>
       </c>
       <c r="B523" s="1" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
     </row>
     <row r="524" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -39730,7 +39730,7 @@
         <v>296</v>
       </c>
       <c r="B533" s="1" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
     </row>
     <row r="534" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -39770,7 +39770,7 @@
         <v>298</v>
       </c>
       <c r="B538" s="1" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
     </row>
     <row r="539" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -39810,7 +39810,7 @@
         <v>300</v>
       </c>
       <c r="B543" s="1" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
     </row>
     <row r="544" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -39818,7 +39818,7 @@
         <v>301</v>
       </c>
       <c r="B544" s="1" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
     </row>
     <row r="545" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -39946,7 +39946,7 @@
         <v>307</v>
       </c>
       <c r="B560" s="1" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
     </row>
     <row r="561" spans="1:2" ht="375" x14ac:dyDescent="0.25">
@@ -39978,7 +39978,7 @@
         <v>375</v>
       </c>
       <c r="B564" s="3" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
     </row>
     <row r="565" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -39994,7 +39994,7 @@
         <v>329</v>
       </c>
       <c r="B566" s="3" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix issue with No buying food when in a Temple Hex. Add Prince options for Nerve Gas and Necklass
</commit_message>
<xml_diff>
--- a/Documentation/Events.xlsx
+++ b/Documentation/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\happysulla\BarbarianPrince\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{780BC9CE-139D-452B-AF16-248A83713217}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4C80C65A-0484-4D2B-9692-F03B6C07A64C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -11542,60 +11542,6 @@
   </si>
   <si>
     <r>
-      <t>&lt;Bold&gt;e160 Audience with Lady Aeravir&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-You are allowed a semi-private interview with the rule of Aeravir Castle. Roll one die for the results:  &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>dieRoll</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.gif' Name='</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>DieRoll</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='e160a' FontFamily='Courier New' FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; - 1 - Shows No Interest&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='e160b' FontFamily='Courier New' FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; - 2 -Distracted &lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='e160c' FontFamily='Courier New' FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; - 3 - Shows Pity&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='e160d' FontFamily='Courier New' FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; - 4 - Finds Virtue &lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='e160e' FontFamily='Courier New' FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; - 5 - Seduction&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='e160f' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; - 6 - Shows Support</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>&lt;Bold&gt;e160c Lady Aeravir Pity&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 She takes pity on you and gives you a gift of wealth 60 to help in your quest but decrees that you cannot seek another audience with her. Click image to continue.
@@ -34107,78 +34053,6 @@
   </si>
   <si>
     <r>
-      <t>&lt;Bold&gt;e012a Farmer with Protector Friendly Approach&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;&lt;Italic&gt;Friendly Approach:&lt;/Italic&gt;The farmer warns you off his land, but he will sell you food in any quantity you desire. 
-Regardless of whether you buy or not, the event will end and you continue on your way.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt; 
-                                                     &lt;InlineUIContainer&gt;&lt;Button Content='  -  ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-&lt;InlineUIContainer&gt;&lt;Image Source='../../Images/Food.gif' Name='</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFFC000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Food</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>'  Height='50' Width='50'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt; 
-&lt;InlineUIContainer&gt;&lt;Button Content='  +  ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;         &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Farmland</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.gif' Name='</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>FarmlandEnd</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>'  Height='250' Width='500'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>&lt;Bold&gt;e013a Rich Peasant Family Friendly Approach&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;&lt;Italic&gt;Friendly Approach:&lt;/Italic&gt;The family provides food
  &lt;InlineUIContainer&gt;&lt;Button Content='r215' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; and lodging
@@ -34993,6 +34867,132 @@
         <scheme val="minor"/>
       </rPr>
       <t>.gif' Height='210' Width='400'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;Bold&gt;e012a Farmer with Protector Friendly Approach&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;&lt;Italic&gt;Friendly Approach:&lt;/Italic&gt; The farmer warns you off his land, but he will sell you food in any quantity you desire. 
+Regardless of whether you buy or not, the event will end and you continue on your way.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt; 
+                                                     &lt;InlineUIContainer&gt;&lt;Button Content='  -  ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+&lt;InlineUIContainer&gt;&lt;Image Source='../../Images/Food.gif' Name='</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Food</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'  Height='50' Width='50'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='  +  ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;         &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Farmland</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.gif' Name='</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>FarmlandEnd</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'  Height='250' Width='500'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;Bold&gt;e160 Audience with Lady Aeravir&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+You are allowed a semi-private interview with the ruler of Aeravir Castle. Roll one die for the results:  &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dieRoll</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.gif' Name='</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DieRoll</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='e160a' FontFamily='Courier New' FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; - 1 - Shows No Interest&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='e160b' FontFamily='Courier New' FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; - 2 -Distracted &lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='e160c' FontFamily='Courier New' FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; - 3 - Shows Pity&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='e160d' FontFamily='Courier New' FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; - 4 - Finds Virtue &lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='e160e' FontFamily='Courier New' FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; - 5 - Seduction&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='e160f' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; - 6 - Shows Support</t>
     </r>
   </si>
 </sst>
@@ -35459,8 +35459,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B566"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A296" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B297" sqref="B297"/>
+    <sheetView tabSelected="1" topLeftCell="A395" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B395" sqref="B395"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -35474,7 +35474,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1124</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -35482,7 +35482,7 @@
         <v>254</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -35490,7 +35490,7 @@
         <v>255</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -35498,15 +35498,15 @@
         <v>256</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="390" x14ac:dyDescent="0.25">
@@ -35522,7 +35522,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35530,7 +35530,7 @@
         <v>22</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35546,7 +35546,7 @@
         <v>23</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>1126</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -35562,7 +35562,7 @@
         <v>3</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -35570,7 +35570,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35578,7 +35578,7 @@
         <v>5</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35586,7 +35586,7 @@
         <v>6</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -35594,7 +35594,7 @@
         <v>7</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -35602,7 +35602,7 @@
         <v>8</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35610,7 +35610,7 @@
         <v>10</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35618,7 +35618,7 @@
         <v>9</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -35626,7 +35626,7 @@
         <v>11</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>1123</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -35634,7 +35634,7 @@
         <v>12</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35642,7 +35642,7 @@
         <v>13</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35650,7 +35650,7 @@
         <v>14</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -35658,7 +35658,7 @@
         <v>15</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -35666,7 +35666,7 @@
         <v>16</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -35674,7 +35674,7 @@
         <v>17</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -35682,7 +35682,7 @@
         <v>18</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -35690,31 +35690,31 @@
         <v>261</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -35722,7 +35722,7 @@
         <v>19</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -35730,7 +35730,7 @@
         <v>20</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -35738,23 +35738,23 @@
         <v>21</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -35762,23 +35762,23 @@
         <v>25</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -35786,7 +35786,7 @@
         <v>26</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -35810,7 +35810,7 @@
         <v>27</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -35818,7 +35818,7 @@
         <v>28</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>1120</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -35826,7 +35826,7 @@
         <v>29</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -35834,7 +35834,7 @@
         <v>30</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>1121</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -35847,10 +35847,10 @@
     </row>
     <row r="48" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -35858,7 +35858,7 @@
         <v>31</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>1118</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -35866,7 +35866,7 @@
         <v>32</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>1122</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -35874,7 +35874,7 @@
         <v>33</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>1119</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -35906,7 +35906,7 @@
         <v>496</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -35930,7 +35930,7 @@
         <v>264</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35938,7 +35938,7 @@
         <v>265</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -35962,7 +35962,7 @@
         <v>35</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -35994,7 +35994,7 @@
         <v>37</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="285" x14ac:dyDescent="0.25">
@@ -36002,7 +36002,7 @@
         <v>38</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -36010,7 +36010,7 @@
         <v>43</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -36018,23 +36018,23 @@
         <v>44</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
+        <v>709</v>
+      </c>
+      <c r="B71" s="3" t="s">
         <v>710</v>
-      </c>
-      <c r="B71" s="3" t="s">
-        <v>711</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -36042,7 +36042,7 @@
         <v>39</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -36074,7 +36074,7 @@
         <v>42</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -36082,7 +36082,7 @@
         <v>46</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -36106,7 +36106,7 @@
         <v>49</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -36146,7 +36146,7 @@
         <v>54</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -36154,7 +36154,7 @@
         <v>55</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -36162,7 +36162,7 @@
         <v>56</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -36170,7 +36170,7 @@
         <v>57</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -36178,31 +36178,31 @@
         <v>58</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -36210,15 +36210,15 @@
         <v>59</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
+        <v>888</v>
+      </c>
+      <c r="B94" s="3" t="s">
         <v>889</v>
-      </c>
-      <c r="B94" s="3" t="s">
-        <v>890</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -36226,15 +36226,15 @@
         <v>60</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -36242,7 +36242,7 @@
         <v>61</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -36250,7 +36250,7 @@
         <v>62</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -36282,7 +36282,7 @@
         <v>65</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -36290,7 +36290,7 @@
         <v>66</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -36338,7 +36338,7 @@
         <v>474</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -36370,7 +36370,7 @@
         <v>70</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -36402,7 +36402,7 @@
         <v>72</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="118" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -36410,7 +36410,7 @@
         <v>73</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
     </row>
     <row r="119" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -36458,7 +36458,7 @@
         <v>77</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
     </row>
     <row r="125" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -36471,10 +36471,10 @@
     </row>
     <row r="126" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="127" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -36482,7 +36482,7 @@
         <v>78</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
     </row>
     <row r="128" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -36490,7 +36490,7 @@
         <v>376</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
     </row>
     <row r="129" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -36530,7 +36530,7 @@
         <v>80</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
     </row>
     <row r="134" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -36538,87 +36538,87 @@
         <v>81</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
     </row>
     <row r="135" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
     </row>
     <row r="136" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
     </row>
     <row r="137" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
     </row>
     <row r="138" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
     </row>
     <row r="139" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="B139" s="3" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
     </row>
     <row r="140" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
     </row>
     <row r="141" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
     </row>
     <row r="142" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
     </row>
     <row r="143" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
+        <v>949</v>
+      </c>
+      <c r="B143" s="3" t="s">
         <v>950</v>
-      </c>
-      <c r="B143" s="3" t="s">
-        <v>951</v>
       </c>
     </row>
     <row r="144" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
     </row>
     <row r="145" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -36626,7 +36626,7 @@
         <v>82</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
     </row>
     <row r="146" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -36634,12 +36634,12 @@
         <v>83</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
     </row>
     <row r="147" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="B147" s="3" t="s">
         <v>552</v>
@@ -36674,7 +36674,7 @@
         <v>551</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
     </row>
     <row r="152" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -36682,7 +36682,7 @@
         <v>86</v>
       </c>
       <c r="B152" s="3" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
     </row>
     <row r="153" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -36738,7 +36738,7 @@
         <v>345</v>
       </c>
       <c r="B159" s="3" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
     </row>
     <row r="160" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -36746,7 +36746,7 @@
         <v>347</v>
       </c>
       <c r="B160" s="3" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
     </row>
     <row r="161" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -36775,10 +36775,10 @@
     </row>
     <row r="164" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
+        <v>716</v>
+      </c>
+      <c r="B164" s="3" t="s">
         <v>717</v>
-      </c>
-      <c r="B164" s="3" t="s">
-        <v>718</v>
       </c>
     </row>
     <row r="165" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -36794,7 +36794,7 @@
         <v>443</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
     </row>
     <row r="167" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -36818,23 +36818,23 @@
         <v>90</v>
       </c>
       <c r="B169" s="3" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
     </row>
     <row r="170" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="B170" s="3" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
     </row>
     <row r="171" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="B171" s="3" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="172" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -36866,7 +36866,7 @@
         <v>93</v>
       </c>
       <c r="B175" s="3" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="176" spans="1:2" ht="270" x14ac:dyDescent="0.25">
@@ -36874,7 +36874,7 @@
         <v>94</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
     </row>
     <row r="177" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -36882,7 +36882,7 @@
         <v>95</v>
       </c>
       <c r="B177" s="3" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
     </row>
     <row r="178" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -36890,55 +36890,55 @@
         <v>96</v>
       </c>
       <c r="B178" s="3" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
     </row>
     <row r="179" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A179" s="2" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="B179" s="3" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="180" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A180" s="2" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="B180" s="3" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="181" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="182" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="B182" s="3" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="183" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="B183" s="3" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
     </row>
     <row r="184" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A184" s="2" t="s">
+        <v>864</v>
+      </c>
+      <c r="B184" s="3" t="s">
         <v>865</v>
-      </c>
-      <c r="B184" s="3" t="s">
-        <v>866</v>
       </c>
     </row>
     <row r="185" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -36946,7 +36946,7 @@
         <v>97</v>
       </c>
       <c r="B185" s="3" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="186" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -36978,7 +36978,7 @@
         <v>100</v>
       </c>
       <c r="B189" s="3" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
     </row>
     <row r="190" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -36994,7 +36994,7 @@
         <v>103</v>
       </c>
       <c r="B191" s="3" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
     </row>
     <row r="192" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37002,7 +37002,7 @@
         <v>104</v>
       </c>
       <c r="B192" s="3" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
     </row>
     <row r="193" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37010,23 +37010,23 @@
         <v>105</v>
       </c>
       <c r="B193" s="3" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="194" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A194" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="B194" s="3" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="195" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A195" s="2" t="s">
+        <v>693</v>
+      </c>
+      <c r="B195" s="3" t="s">
         <v>694</v>
-      </c>
-      <c r="B195" s="3" t="s">
-        <v>695</v>
       </c>
     </row>
     <row r="196" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -37034,7 +37034,7 @@
         <v>106</v>
       </c>
       <c r="B196" s="3" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
     </row>
     <row r="197" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37042,7 +37042,7 @@
         <v>107</v>
       </c>
       <c r="B197" s="3" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
     </row>
     <row r="198" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -37050,15 +37050,15 @@
         <v>165</v>
       </c>
       <c r="B198" s="3" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
     </row>
     <row r="199" spans="1:2" ht="225" x14ac:dyDescent="0.25">
       <c r="A199" s="2" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="B199" s="3" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
     </row>
     <row r="200" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37066,7 +37066,7 @@
         <v>108</v>
       </c>
       <c r="B200" s="3" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
     </row>
     <row r="201" spans="1:2" ht="285" x14ac:dyDescent="0.25">
@@ -37074,7 +37074,7 @@
         <v>109</v>
       </c>
       <c r="B201" s="3" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
     </row>
     <row r="202" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -37082,7 +37082,7 @@
         <v>110</v>
       </c>
       <c r="B202" s="3" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
     </row>
     <row r="203" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -37090,7 +37090,7 @@
         <v>166</v>
       </c>
       <c r="B203" s="3" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="204" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -37098,7 +37098,7 @@
         <v>167</v>
       </c>
       <c r="B204" s="3" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="205" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -37106,23 +37106,23 @@
         <v>168</v>
       </c>
       <c r="B205" s="3" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
     </row>
     <row r="206" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A206" s="2" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="B206" s="3" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="207" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A207" s="2" t="s">
+        <v>879</v>
+      </c>
+      <c r="B207" s="3" t="s">
         <v>880</v>
-      </c>
-      <c r="B207" s="3" t="s">
-        <v>881</v>
       </c>
     </row>
     <row r="208" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37130,39 +37130,39 @@
         <v>111</v>
       </c>
       <c r="B208" s="3" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="209" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A209" s="2" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="B209" s="3" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="210" spans="1:2" ht="225" x14ac:dyDescent="0.25">
       <c r="A210" s="2" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="B210" s="3" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="211" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A211" s="2" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="B211" s="3" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="212" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A212" s="2" t="s">
+        <v>724</v>
+      </c>
+      <c r="B212" s="3" t="s">
         <v>725</v>
-      </c>
-      <c r="B212" s="3" t="s">
-        <v>726</v>
       </c>
     </row>
     <row r="213" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37170,7 +37170,7 @@
         <v>112</v>
       </c>
       <c r="B213" s="3" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
     </row>
     <row r="214" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37178,7 +37178,7 @@
         <v>169</v>
       </c>
       <c r="B214" s="3" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
     </row>
     <row r="215" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -37186,7 +37186,7 @@
         <v>170</v>
       </c>
       <c r="B215" s="3" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
     </row>
     <row r="216" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -37194,7 +37194,7 @@
         <v>171</v>
       </c>
       <c r="B216" s="3" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="217" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37202,7 +37202,7 @@
         <v>113</v>
       </c>
       <c r="B217" s="3" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="218" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -37210,7 +37210,7 @@
         <v>114</v>
       </c>
       <c r="B218" s="3" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
     </row>
     <row r="219" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -37218,15 +37218,15 @@
         <v>266</v>
       </c>
       <c r="B219" s="3" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
     </row>
     <row r="220" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A220" s="2" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="B220" s="3" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
     </row>
     <row r="221" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37234,15 +37234,15 @@
         <v>115</v>
       </c>
       <c r="B221" s="3" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
     </row>
     <row r="222" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A222" s="2" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="B222" s="3" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
     </row>
     <row r="223" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37250,15 +37250,15 @@
         <v>116</v>
       </c>
       <c r="B223" s="3" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="224" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A224" s="2" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="B224" s="3" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
     </row>
     <row r="225" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -37266,31 +37266,31 @@
         <v>117</v>
       </c>
       <c r="B225" s="4" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
     </row>
     <row r="226" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A226" s="2" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="B226" s="4" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
     </row>
     <row r="227" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A227" s="2" t="s">
+        <v>747</v>
+      </c>
+      <c r="B227" s="4" t="s">
         <v>748</v>
-      </c>
-      <c r="B227" s="4" t="s">
-        <v>749</v>
       </c>
     </row>
     <row r="228" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A228" s="2" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="B228" s="4" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
     </row>
     <row r="229" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -37298,23 +37298,23 @@
         <v>118</v>
       </c>
       <c r="B229" s="3" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
     </row>
     <row r="230" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A230" s="2" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="B230" s="3" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
     </row>
     <row r="231" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A231" s="2" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="B231" s="3" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="232" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -37322,23 +37322,23 @@
         <v>119</v>
       </c>
       <c r="B232" s="3" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="233" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A233" s="2" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="B233" s="3" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
     </row>
     <row r="234" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A234" s="2" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="B234" s="3" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="235" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -37346,7 +37346,7 @@
         <v>120</v>
       </c>
       <c r="B235" s="3" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
     </row>
     <row r="236" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -37354,7 +37354,7 @@
         <v>172</v>
       </c>
       <c r="B236" s="3" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
     </row>
     <row r="237" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37362,7 +37362,7 @@
         <v>173</v>
       </c>
       <c r="B237" s="3" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
     </row>
     <row r="238" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37370,7 +37370,7 @@
         <v>174</v>
       </c>
       <c r="B238" s="3" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
     </row>
     <row r="239" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37386,15 +37386,15 @@
         <v>122</v>
       </c>
       <c r="B240" s="3" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
     <row r="241" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A241" s="2" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B241" s="3" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
     </row>
     <row r="242" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -37402,23 +37402,23 @@
         <v>123</v>
       </c>
       <c r="B242" s="3" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
     </row>
     <row r="243" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A243" s="2" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="B243" s="3" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="244" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A244" s="2" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="B244" s="3" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="245" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37426,15 +37426,15 @@
         <v>124</v>
       </c>
       <c r="B245" s="3" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
     </row>
     <row r="246" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A246" s="2" t="s">
-        <v>1129</v>
+        <v>1127</v>
       </c>
       <c r="B246" s="3" t="s">
-        <v>1130</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="247" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37442,15 +37442,15 @@
         <v>125</v>
       </c>
       <c r="B247" s="3" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
     </row>
     <row r="248" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A248" s="2" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="B248" s="3" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="249" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37458,7 +37458,7 @@
         <v>126</v>
       </c>
       <c r="B249" s="3" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
     </row>
     <row r="250" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37466,7 +37466,7 @@
         <v>127</v>
       </c>
       <c r="B250" s="3" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
     </row>
     <row r="251" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37474,7 +37474,7 @@
         <v>128</v>
       </c>
       <c r="B251" s="3" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
     </row>
     <row r="252" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -37482,7 +37482,7 @@
         <v>129</v>
       </c>
       <c r="B252" s="3" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
     </row>
     <row r="253" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37490,7 +37490,7 @@
         <v>130</v>
       </c>
       <c r="B253" s="3" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
     </row>
     <row r="254" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -37498,23 +37498,23 @@
         <v>131</v>
       </c>
       <c r="B254" s="3" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
     </row>
     <row r="255" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A255" s="2" t="s">
+        <v>925</v>
+      </c>
+      <c r="B255" s="3" t="s">
         <v>926</v>
-      </c>
-      <c r="B255" s="3" t="s">
-        <v>927</v>
       </c>
     </row>
     <row r="256" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A256" s="2" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="B256" s="3" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
     </row>
     <row r="257" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -37522,7 +37522,7 @@
         <v>132</v>
       </c>
       <c r="B257" s="3" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
     </row>
     <row r="258" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -37530,15 +37530,15 @@
         <v>133</v>
       </c>
       <c r="B258" s="3" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="259" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A259" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="B259" s="3" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="260" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37546,23 +37546,23 @@
         <v>134</v>
       </c>
       <c r="B260" s="3" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
     </row>
     <row r="261" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A261" s="2" t="s">
+        <v>977</v>
+      </c>
+      <c r="B261" s="3" t="s">
         <v>978</v>
-      </c>
-      <c r="B261" s="3" t="s">
-        <v>979</v>
       </c>
     </row>
     <row r="262" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A262" s="2" t="s">
+        <v>979</v>
+      </c>
+      <c r="B262" s="3" t="s">
         <v>980</v>
-      </c>
-      <c r="B262" s="3" t="s">
-        <v>981</v>
       </c>
     </row>
     <row r="263" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -37570,15 +37570,15 @@
         <v>135</v>
       </c>
       <c r="B263" s="3" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
     </row>
     <row r="264" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A264" s="2" t="s">
+        <v>982</v>
+      </c>
+      <c r="B264" s="3" t="s">
         <v>983</v>
-      </c>
-      <c r="B264" s="3" t="s">
-        <v>984</v>
       </c>
     </row>
     <row r="265" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -37586,7 +37586,7 @@
         <v>136</v>
       </c>
       <c r="B265" s="3" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
     </row>
     <row r="266" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -37610,7 +37610,7 @@
         <v>233</v>
       </c>
       <c r="B268" s="3" t="s">
-        <v>1128</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="269" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -37618,7 +37618,7 @@
         <v>138</v>
       </c>
       <c r="B269" s="3" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
     </row>
     <row r="270" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37626,7 +37626,7 @@
         <v>234</v>
       </c>
       <c r="B270" s="3" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="271" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37634,7 +37634,7 @@
         <v>235</v>
       </c>
       <c r="B271" s="3" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="272" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -37642,7 +37642,7 @@
         <v>139</v>
       </c>
       <c r="B272" s="3" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
     </row>
     <row r="273" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -37650,7 +37650,7 @@
         <v>239</v>
       </c>
       <c r="B273" s="3" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
     </row>
     <row r="274" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37658,7 +37658,7 @@
         <v>240</v>
       </c>
       <c r="B274" s="3" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
     </row>
     <row r="275" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37666,7 +37666,7 @@
         <v>241</v>
       </c>
       <c r="B275" s="3" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
     </row>
     <row r="276" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37674,7 +37674,7 @@
         <v>140</v>
       </c>
       <c r="B276" s="3" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="277" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -37682,7 +37682,7 @@
         <v>236</v>
       </c>
       <c r="B277" s="3" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="278" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37690,7 +37690,7 @@
         <v>237</v>
       </c>
       <c r="B278" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="279" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37698,7 +37698,7 @@
         <v>238</v>
       </c>
       <c r="B279" s="3" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="280" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -37706,7 +37706,7 @@
         <v>141</v>
       </c>
       <c r="B280" s="3" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="281" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -37714,7 +37714,7 @@
         <v>142</v>
       </c>
       <c r="B281" s="3" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="282" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -37722,7 +37722,7 @@
         <v>143</v>
       </c>
       <c r="B282" s="3" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="283" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -37730,7 +37730,7 @@
         <v>144</v>
       </c>
       <c r="B283" s="3" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="284" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -37738,7 +37738,7 @@
         <v>242</v>
       </c>
       <c r="B284" s="3" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="285" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37746,7 +37746,7 @@
         <v>145</v>
       </c>
       <c r="B285" s="3" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="286" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -37754,7 +37754,7 @@
         <v>146</v>
       </c>
       <c r="B286" s="3" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="287" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37762,7 +37762,7 @@
         <v>147</v>
       </c>
       <c r="B287" s="3" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="288" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -37770,7 +37770,7 @@
         <v>148</v>
       </c>
       <c r="B288" s="3" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="289" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -37778,31 +37778,31 @@
         <v>149</v>
       </c>
       <c r="B289" s="3" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="290" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A290" s="2" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="B290" s="3" t="s">
-        <v>1127</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="291" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A291" s="2" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="B291" s="3" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="292" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A292" s="2" t="s">
+        <v>1047</v>
+      </c>
+      <c r="B292" s="3" t="s">
         <v>1048</v>
-      </c>
-      <c r="B292" s="3" t="s">
-        <v>1049</v>
       </c>
     </row>
     <row r="293" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37810,15 +37810,15 @@
         <v>150</v>
       </c>
       <c r="B293" s="3" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="294" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A294" s="2" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="B294" s="3" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="295" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -37826,7 +37826,7 @@
         <v>151</v>
       </c>
       <c r="B295" s="3" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
     </row>
     <row r="296" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37834,7 +37834,7 @@
         <v>243</v>
       </c>
       <c r="B296" s="3" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
     </row>
     <row r="297" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37842,7 +37842,7 @@
         <v>244</v>
       </c>
       <c r="B297" s="3" t="s">
-        <v>1131</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="298" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37850,7 +37850,7 @@
         <v>245</v>
       </c>
       <c r="B298" s="3" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
     </row>
     <row r="299" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37858,7 +37858,7 @@
         <v>152</v>
       </c>
       <c r="B299" s="3" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
     </row>
     <row r="300" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -37866,7 +37866,7 @@
         <v>153</v>
       </c>
       <c r="B300" s="3" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="301" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37874,7 +37874,7 @@
         <v>154</v>
       </c>
       <c r="B301" s="3" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="302" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -37882,7 +37882,7 @@
         <v>155</v>
       </c>
       <c r="B302" s="3" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
     </row>
     <row r="303" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37890,7 +37890,7 @@
         <v>156</v>
       </c>
       <c r="B303" s="3" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
     </row>
     <row r="304" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -37898,7 +37898,7 @@
         <v>157</v>
       </c>
       <c r="B304" s="3" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="305" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -37906,7 +37906,7 @@
         <v>246</v>
       </c>
       <c r="B305" s="3" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
     </row>
     <row r="306" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37914,7 +37914,7 @@
         <v>247</v>
       </c>
       <c r="B306" s="3" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
     </row>
     <row r="307" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37922,7 +37922,7 @@
         <v>248</v>
       </c>
       <c r="B307" s="3" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="308" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37930,7 +37930,7 @@
         <v>158</v>
       </c>
       <c r="B308" s="3" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
     </row>
     <row r="309" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -37938,7 +37938,7 @@
         <v>159</v>
       </c>
       <c r="B309" s="3" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
     </row>
     <row r="310" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37946,7 +37946,7 @@
         <v>160</v>
       </c>
       <c r="B310" s="3" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
     </row>
     <row r="311" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -37954,7 +37954,7 @@
         <v>161</v>
       </c>
       <c r="B311" s="3" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="312" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37962,31 +37962,31 @@
         <v>162</v>
       </c>
       <c r="B312" s="3" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="313" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A313" s="2" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="B313" s="3" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="314" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A314" s="2" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="B314" s="3" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="315" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A315" s="2" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="B315" s="3" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="316" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37994,7 +37994,7 @@
         <v>163</v>
       </c>
       <c r="B316" s="3" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="317" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -38002,7 +38002,7 @@
         <v>164</v>
       </c>
       <c r="B317" s="3" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="318" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -38010,7 +38010,7 @@
         <v>175</v>
       </c>
       <c r="B318" s="3" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="319" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -38018,7 +38018,7 @@
         <v>176</v>
       </c>
       <c r="B319" s="3" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="320" spans="1:2" ht="390" x14ac:dyDescent="0.25">
@@ -38026,7 +38026,7 @@
         <v>177</v>
       </c>
       <c r="B320" s="3" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="321" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -38034,7 +38034,7 @@
         <v>519</v>
       </c>
       <c r="B321" s="3" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
     </row>
     <row r="322" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -38042,7 +38042,7 @@
         <v>520</v>
       </c>
       <c r="B322" s="3" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
     </row>
     <row r="323" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -38050,7 +38050,7 @@
         <v>521</v>
       </c>
       <c r="B323" s="3" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
     </row>
     <row r="324" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -38058,7 +38058,7 @@
         <v>522</v>
       </c>
       <c r="B324" s="3" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="325" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -38066,7 +38066,7 @@
         <v>523</v>
       </c>
       <c r="B325" s="3" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
     </row>
     <row r="326" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -38074,15 +38074,15 @@
         <v>524</v>
       </c>
       <c r="B326" s="3" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
     </row>
     <row r="327" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A327" s="2" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="B327" s="3" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="328" spans="1:2" ht="390" x14ac:dyDescent="0.25">
@@ -38090,7 +38090,7 @@
         <v>178</v>
       </c>
       <c r="B328" s="3" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
     </row>
     <row r="329" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -38098,7 +38098,7 @@
         <v>494</v>
       </c>
       <c r="B329" s="3" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="330" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -38106,7 +38106,7 @@
         <v>548</v>
       </c>
       <c r="B330" s="3" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="331" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -38114,7 +38114,7 @@
         <v>549</v>
       </c>
       <c r="B331" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="332" spans="1:2" ht="315" x14ac:dyDescent="0.25">
@@ -38122,7 +38122,7 @@
         <v>179</v>
       </c>
       <c r="B332" s="3" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
     </row>
     <row r="333" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -38130,7 +38130,7 @@
         <v>249</v>
       </c>
       <c r="B333" s="3" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
     </row>
     <row r="334" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -38138,7 +38138,7 @@
         <v>250</v>
       </c>
       <c r="B334" s="3" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
     </row>
     <row r="335" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -38146,7 +38146,7 @@
         <v>251</v>
       </c>
       <c r="B335" s="3" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
     </row>
     <row r="336" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38154,7 +38154,7 @@
         <v>252</v>
       </c>
       <c r="B336" s="3" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="337" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -38162,23 +38162,23 @@
         <v>253</v>
       </c>
       <c r="B337" s="3" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
     <row r="338" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A338" s="2" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="B338" s="3" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="339" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A339" s="2" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="B339" s="3" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
     </row>
     <row r="340" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -38186,7 +38186,7 @@
         <v>180</v>
       </c>
       <c r="B340" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="341" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38218,7 +38218,7 @@
         <v>183</v>
       </c>
       <c r="B344" s="3" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="345" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -38226,7 +38226,7 @@
         <v>184</v>
       </c>
       <c r="B345" s="3" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="346" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -38266,7 +38266,7 @@
         <v>469</v>
       </c>
       <c r="B350" s="3" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="351" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -38290,7 +38290,7 @@
         <v>459</v>
       </c>
       <c r="B353" s="3" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
     </row>
     <row r="354" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -38338,7 +38338,7 @@
         <v>193</v>
       </c>
       <c r="B359" s="3" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="360" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -38346,7 +38346,7 @@
         <v>340</v>
       </c>
       <c r="B360" s="3" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="361" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -38354,7 +38354,7 @@
         <v>341</v>
       </c>
       <c r="B361" s="3" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="362" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -38362,7 +38362,7 @@
         <v>194</v>
       </c>
       <c r="B362" s="3" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="363" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -38370,7 +38370,7 @@
         <v>195</v>
       </c>
       <c r="B363" s="3" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
     </row>
     <row r="364" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -38378,7 +38378,7 @@
         <v>196</v>
       </c>
       <c r="B364" s="3" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
     </row>
     <row r="365" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -38386,7 +38386,7 @@
         <v>331</v>
       </c>
       <c r="B365" s="3" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="366" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -38394,15 +38394,15 @@
         <v>197</v>
       </c>
       <c r="B366" s="3" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
     </row>
     <row r="367" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A367" s="2" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="B367" s="3" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="368" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38442,7 +38442,7 @@
         <v>202</v>
       </c>
       <c r="B372" s="3" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
     </row>
     <row r="373" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -38458,7 +38458,7 @@
         <v>596</v>
       </c>
       <c r="B374" s="3" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
     </row>
     <row r="375" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -38466,7 +38466,7 @@
         <v>597</v>
       </c>
       <c r="B375" s="3" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
     </row>
     <row r="376" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -38474,7 +38474,7 @@
         <v>598</v>
       </c>
       <c r="B376" s="3" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
     </row>
     <row r="377" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -38482,7 +38482,7 @@
         <v>599</v>
       </c>
       <c r="B377" s="3" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
     </row>
     <row r="378" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -38490,7 +38490,7 @@
         <v>600</v>
       </c>
       <c r="B378" s="3" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
     </row>
     <row r="379" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -38562,7 +38562,7 @@
         <v>587</v>
       </c>
       <c r="B387" s="3" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
     </row>
     <row r="388" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -38570,7 +38570,7 @@
         <v>588</v>
       </c>
       <c r="B388" s="3" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
     </row>
     <row r="389" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -38578,7 +38578,7 @@
         <v>589</v>
       </c>
       <c r="B389" s="3" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
     </row>
     <row r="390" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -38586,7 +38586,7 @@
         <v>590</v>
       </c>
       <c r="B390" s="3" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
     </row>
     <row r="391" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38602,7 +38602,7 @@
         <v>592</v>
       </c>
       <c r="B392" s="3" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
     </row>
     <row r="393" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38618,7 +38618,7 @@
         <v>207</v>
       </c>
       <c r="B394" s="3" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
     </row>
     <row r="395" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -38634,7 +38634,7 @@
         <v>209</v>
       </c>
       <c r="B396" s="3" t="s">
-        <v>648</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="397" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -38642,7 +38642,7 @@
         <v>642</v>
       </c>
       <c r="B397" s="3" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
     <row r="398" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -38650,7 +38650,7 @@
         <v>643</v>
       </c>
       <c r="B398" s="3" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
     </row>
     <row r="399" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -38658,7 +38658,7 @@
         <v>644</v>
       </c>
       <c r="B399" s="3" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="400" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -38666,7 +38666,7 @@
         <v>645</v>
       </c>
       <c r="B400" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="401" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -38674,7 +38674,7 @@
         <v>646</v>
       </c>
       <c r="B401" s="4" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
     <row r="402" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -38682,7 +38682,7 @@
         <v>647</v>
       </c>
       <c r="B402" s="3" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="403" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -38754,7 +38754,7 @@
         <v>211</v>
       </c>
       <c r="B411" s="3" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
     </row>
     <row r="412" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -38770,7 +38770,7 @@
         <v>537</v>
       </c>
       <c r="B413" s="3" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="414" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -38802,7 +38802,7 @@
         <v>213</v>
       </c>
       <c r="B417" s="3" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
     </row>
     <row r="418" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -38810,7 +38810,7 @@
         <v>214</v>
       </c>
       <c r="B418" s="3" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="419" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -38818,7 +38818,7 @@
         <v>215</v>
       </c>
       <c r="B419" s="3" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="420" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38850,7 +38850,7 @@
         <v>219</v>
       </c>
       <c r="B423" s="3" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
     </row>
     <row r="424" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38858,7 +38858,7 @@
         <v>220</v>
       </c>
       <c r="B424" s="3" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="425" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -38866,7 +38866,7 @@
         <v>221</v>
       </c>
       <c r="B425" s="3" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="426" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -38874,7 +38874,7 @@
         <v>222</v>
       </c>
       <c r="B426" s="3" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="427" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -38882,7 +38882,7 @@
         <v>223</v>
       </c>
       <c r="B427" s="3" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="428" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -38890,7 +38890,7 @@
         <v>224</v>
       </c>
       <c r="B428" s="3" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="429" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -38898,7 +38898,7 @@
         <v>332</v>
       </c>
       <c r="B429" s="3" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="430" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -38914,7 +38914,7 @@
         <v>225</v>
       </c>
       <c r="B431" s="3" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
     </row>
     <row r="432" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -38978,7 +38978,7 @@
         <v>447</v>
       </c>
       <c r="B439" s="3" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="440" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -39002,15 +39002,15 @@
         <v>581</v>
       </c>
       <c r="B442" s="3" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
     </row>
     <row r="443" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A443" s="2" t="s">
+        <v>782</v>
+      </c>
+      <c r="B443" s="3" t="s">
         <v>783</v>
-      </c>
-      <c r="B443" s="3" t="s">
-        <v>784</v>
       </c>
     </row>
     <row r="444" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -39018,7 +39018,7 @@
         <v>319</v>
       </c>
       <c r="B444" s="3" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="445" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -39026,7 +39026,7 @@
         <v>320</v>
       </c>
       <c r="B445" s="3" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="446" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -39034,7 +39034,7 @@
         <v>321</v>
       </c>
       <c r="B446" s="3" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="447" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -39042,15 +39042,15 @@
         <v>318</v>
       </c>
       <c r="B447" s="3" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="448" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A448" s="2" t="s">
+        <v>1023</v>
+      </c>
+      <c r="B448" s="3" t="s">
         <v>1024</v>
-      </c>
-      <c r="B448" s="3" t="s">
-        <v>1025</v>
       </c>
     </row>
     <row r="449" spans="1:2" ht="255" x14ac:dyDescent="0.25">
@@ -39058,7 +39058,7 @@
         <v>322</v>
       </c>
       <c r="B449" s="3" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="450" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39082,7 +39082,7 @@
         <v>488</v>
       </c>
       <c r="B452" s="3" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="453" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -39122,7 +39122,7 @@
         <v>557</v>
       </c>
       <c r="B457" s="3" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
     </row>
     <row r="458" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -39130,7 +39130,7 @@
         <v>561</v>
       </c>
       <c r="B458" s="3" t="s">
-        <v>1125</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="459" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -39138,7 +39138,7 @@
         <v>564</v>
       </c>
       <c r="B459" s="3" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="460" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39146,7 +39146,7 @@
         <v>565</v>
       </c>
       <c r="B460" s="3" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
     </row>
     <row r="461" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39170,7 +39170,7 @@
         <v>568</v>
       </c>
       <c r="B463" s="3" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
     </row>
     <row r="464" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -39178,7 +39178,7 @@
         <v>569</v>
       </c>
       <c r="B464" s="3" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="465" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -39194,7 +39194,7 @@
         <v>571</v>
       </c>
       <c r="B466" s="3" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
     </row>
     <row r="467" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -39218,7 +39218,7 @@
         <v>579</v>
       </c>
       <c r="B469" s="3" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
     </row>
     <row r="470" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -39226,7 +39226,7 @@
         <v>601</v>
       </c>
       <c r="B470" s="3" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
     </row>
     <row r="471" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -39234,7 +39234,7 @@
         <v>619</v>
       </c>
       <c r="B471" s="3" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="472" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -39242,7 +39242,7 @@
         <v>620</v>
       </c>
       <c r="B472" s="3" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="473" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -39250,167 +39250,167 @@
         <v>621</v>
       </c>
       <c r="B473" s="3" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="474" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A474" s="2" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="B474" s="3" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
     </row>
     <row r="475" spans="1:2" ht="255" x14ac:dyDescent="0.25">
       <c r="A475" s="2" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="B475" s="1" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
     </row>
     <row r="476" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A476" s="2" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="B476" s="1" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
     </row>
     <row r="477" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A477" s="2" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="B477" s="1" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
     </row>
     <row r="478" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A478" s="2" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="B478" s="1" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
     </row>
     <row r="479" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A479" s="2" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="B479" s="1" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
     </row>
     <row r="480" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A480" s="2" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="B480" s="1" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
     <row r="481" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A481" s="2" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="B481" s="1" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
     </row>
     <row r="482" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A482" s="2" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="B482" s="1" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
     </row>
     <row r="483" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A483" s="2" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="B483" s="1" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
     </row>
     <row r="484" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A484" s="2" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="B484" s="1" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="485" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A485" s="2" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="B485" s="1" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="486" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A486" s="2" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="B486" s="1" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
     </row>
     <row r="487" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A487" s="2" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="B487" s="1" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
     </row>
     <row r="488" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A488" s="2" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="B488" s="1" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="489" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A489" s="2" t="s">
+        <v>687</v>
+      </c>
+      <c r="B489" s="1" t="s">
         <v>688</v>
-      </c>
-      <c r="B489" s="1" t="s">
-        <v>689</v>
       </c>
     </row>
     <row r="490" spans="1:2" ht="255" x14ac:dyDescent="0.25">
       <c r="A490" s="2" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="B490" s="1" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="491" spans="1:2" ht="92.25" x14ac:dyDescent="0.25">
       <c r="A491" s="2" t="s">
+        <v>1005</v>
+      </c>
+      <c r="B491" s="1" t="s">
         <v>1006</v>
-      </c>
-      <c r="B491" s="1" t="s">
-        <v>1007</v>
       </c>
     </row>
     <row r="492" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A492" s="2" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="B492" s="1" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
     </row>
     <row r="493" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A493" s="2" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="B493" s="3" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="494" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -39418,7 +39418,7 @@
         <v>543</v>
       </c>
       <c r="B494" s="3" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="495" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -39426,7 +39426,7 @@
         <v>544</v>
       </c>
       <c r="B495" s="3" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
     </row>
     <row r="496" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -39434,7 +39434,7 @@
         <v>545</v>
       </c>
       <c r="B496" s="3" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
     </row>
     <row r="497" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39506,7 +39506,7 @@
         <v>275</v>
       </c>
       <c r="B505" s="1" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="506" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39514,7 +39514,7 @@
         <v>276</v>
       </c>
       <c r="B506" s="1" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="507" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39522,7 +39522,7 @@
         <v>277</v>
       </c>
       <c r="B507" s="1" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="508" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -39570,7 +39570,7 @@
         <v>260</v>
       </c>
       <c r="B513" s="3" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
     </row>
     <row r="514" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39578,7 +39578,7 @@
         <v>476</v>
       </c>
       <c r="B514" s="3" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
     </row>
     <row r="515" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -39586,15 +39586,15 @@
         <v>477</v>
       </c>
       <c r="B515" s="1" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
     </row>
     <row r="516" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A516" s="2" t="s">
+        <v>789</v>
+      </c>
+      <c r="B516" s="3" t="s">
         <v>790</v>
-      </c>
-      <c r="B516" s="3" t="s">
-        <v>791</v>
       </c>
     </row>
     <row r="517" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39642,7 +39642,7 @@
         <v>285</v>
       </c>
       <c r="B522" s="1" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
     </row>
     <row r="523" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -39650,7 +39650,7 @@
         <v>286</v>
       </c>
       <c r="B523" s="1" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
     </row>
     <row r="524" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -39730,7 +39730,7 @@
         <v>296</v>
       </c>
       <c r="B533" s="1" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
     </row>
     <row r="534" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -39738,7 +39738,7 @@
         <v>297</v>
       </c>
       <c r="B534" s="1" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
     </row>
     <row r="535" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -39770,7 +39770,7 @@
         <v>298</v>
       </c>
       <c r="B538" s="1" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
     </row>
     <row r="539" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -39786,7 +39786,7 @@
         <v>299</v>
       </c>
       <c r="B540" s="1" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
     </row>
     <row r="541" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -39810,7 +39810,7 @@
         <v>300</v>
       </c>
       <c r="B543" s="1" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
     </row>
     <row r="544" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -39818,7 +39818,7 @@
         <v>301</v>
       </c>
       <c r="B544" s="1" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
     </row>
     <row r="545" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -39858,7 +39858,7 @@
         <v>395</v>
       </c>
       <c r="B549" s="1" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
     </row>
     <row r="550" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -39871,10 +39871,10 @@
     </row>
     <row r="551" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A551" s="2" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="B551" s="1" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
     </row>
     <row r="552" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -39882,7 +39882,7 @@
         <v>305</v>
       </c>
       <c r="B552" s="1" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
     </row>
     <row r="553" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -39911,10 +39911,10 @@
     </row>
     <row r="556" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A556" s="2" t="s">
+        <v>731</v>
+      </c>
+      <c r="B556" s="1" t="s">
         <v>732</v>
-      </c>
-      <c r="B556" s="1" t="s">
-        <v>733</v>
       </c>
     </row>
     <row r="557" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -39922,7 +39922,7 @@
         <v>306</v>
       </c>
       <c r="B557" s="1" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="558" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -39946,7 +39946,7 @@
         <v>307</v>
       </c>
       <c r="B560" s="1" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
     </row>
     <row r="561" spans="1:2" ht="375" x14ac:dyDescent="0.25">
@@ -39954,7 +39954,7 @@
         <v>311</v>
       </c>
       <c r="B561" s="1" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
     </row>
     <row r="562" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39978,15 +39978,15 @@
         <v>375</v>
       </c>
       <c r="B564" s="3" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
     </row>
     <row r="565" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A565" s="2" t="s">
+        <v>735</v>
+      </c>
+      <c r="B565" s="3" t="s">
         <v>736</v>
-      </c>
-      <c r="B565" s="3" t="s">
-        <v>737</v>
       </c>
     </row>
     <row r="566" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -39994,7 +39994,7 @@
         <v>329</v>
       </c>
       <c r="B566" s="3" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished Count Drogat Secret processing and FoulBane
</commit_message>
<xml_diff>
--- a/Documentation/Events.xlsx
+++ b/Documentation/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\happysulla\BarbarianPrince\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8A98CFF1-52E0-4CBF-AD7C-CE6B1714C557}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{08D4A4BD-B4A9-4FA0-9958-145BF8D4FE7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -35105,57 +35105,6 @@
   </si>
   <si>
     <r>
-      <t>&lt;Bold&gt;e146a Stealing Count Drogat Jewels&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;Using the foulbane in Drogat Castle, you can spend a day instead of a normal daily action in arranging for a special theft of the Count's personnel jewels.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;At the end of the day, you escape from the hex
- &lt;InlineUIContainer&gt;&lt;Button Content='r218' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
- with wealth 110. However, you can never return to the castle hex due to the Count's anger. In the process of the theft, you might acquire magic items as part of the wealth 110 check. Click image to continue.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                     &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>FoulBane</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.gif' Name='</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>EncounterEnd</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>' Height='250' Width='200'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>&lt;Bold&gt;e146 Secret of Count Drogat&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;You learn that Count Drogat, lord of Drogat Castle, is acutally an undead creature who enjoys the suffering, pain, and death of others. This explains why he so often tortures and dismembers felons in his realm.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;He often goes into rages that leave his lands in a reign of terror. 
@@ -35207,6 +35156,57 @@
         <scheme val="minor"/>
       </rPr>
       <t>' Height='250' Width='200'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;Bold&gt;e146a Stealing Count Drogat Jewels&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;Using the foulbane in Drogat Castle, you can spend a day instead of a normal daily action in arranging for a special theft of the Count's personnel jewels.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;At the end of the day, you escape from the hex
+ &lt;InlineUIContainer&gt;&lt;Button Content='r218' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+ with wealth 110. However, you can never return to the castle hex due to the Count's anger. In the process of the theft, you might acquire magic items as part of the wealth 110 check. Click image to continue.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                           &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CountDrogatJewels</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.gif' Name='</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CountDrogatJewels</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>' Height='300' Width='300'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
     </r>
   </si>
 </sst>
@@ -35673,7 +35673,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B569"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A362" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A363" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B364" sqref="B364"/>
     </sheetView>
   </sheetViews>
@@ -38584,7 +38584,7 @@
         <v>195</v>
       </c>
       <c r="B363" s="3" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
     </row>
     <row r="364" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -38592,7 +38592,7 @@
         <v>1131</v>
       </c>
       <c r="B364" s="3" t="s">
-        <v>1136</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="365" spans="1:2" ht="150" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Very minor fix. Remove extra space
</commit_message>
<xml_diff>
--- a/Documentation/Events.xlsx
+++ b/Documentation/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\happysulla\BarbarianPrince\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{8E54EA9A-E7DB-44D2-8E50-1A912CE65BED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BB42C8EB-999A-4ED2-B1E2-1A9B4DE1FE7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -18030,62 +18030,6 @@
   </si>
   <si>
     <r>
-      <t>&lt;Bold&gt;e050f  Mercenary Royal Guardsmen&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;Since you are within three hexes of Ogon
-  &lt;InlineUIContainer&gt;&lt;Button Content='0101' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
- or Weshor
-  &lt;InlineUIContainer&gt;&lt;Button Content='1501' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;,
- you do not encounter local constabulary. Instead, you may encounter the mercenary royal guardsmen. You see mercenary royal guardsmen attempting to find you. Roll one die, subtract three, then add one if you are in Ogon or Weshor.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-If the results is 1 plus, encounter the guardsmen
- &lt;InlineUIContainer&gt;&lt;Button Content='e002a' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-If the result is zero or less, no event occurs:
- &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>dieRoll</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">.gif' </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Name='DieRoll'</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Height='21'  Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>&lt;Bold&gt;e078 Bad Going For Horses&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;Terrain is difficult on horses. You must either &lt;InlineUIContainer&gt;&lt;Button Content='Halt' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; for the day to explore alternate routes or you risk injuries.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;If you continue normal travel today, roll one die and subtract three. If the result is 1 plus, that many horses have broken legs or thrown shoes. They are lost as mounts after the move.  Die Roll = &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
@@ -35325,6 +35269,62 @@
         <scheme val="minor"/>
       </rPr>
       <t>.gif' Height='200' Width='200'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;Bold&gt;e050f Mercenary Royal Guardsmen&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;Since you are within three hexes of Ogon
+  &lt;InlineUIContainer&gt;&lt;Button Content='0101' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+ or Weshor
+  &lt;InlineUIContainer&gt;&lt;Button Content='1501' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;,
+ you do not encounter local constabulary. Instead, you may encounter the mercenary royal guardsmen. You see mercenary royal guardsmen attempting to find you. Roll one die, subtract three, then add one if you are in Ogon or Weshor.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+If the results is 1 plus, encounter the guardsmen
+ &lt;InlineUIContainer&gt;&lt;Button Content='e002a' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+If the result is zero or less, no event occurs:
+ &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dieRoll</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">.gif' </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Name='DieRoll'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Height='21'  Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
     </r>
   </si>
 </sst>
@@ -35791,8 +35791,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B571"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A414" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B416" sqref="B416"/>
+    <sheetView tabSelected="1" topLeftCell="A150" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B151" sqref="B151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -35806,7 +35806,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -35814,7 +35814,7 @@
         <v>254</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -35822,7 +35822,7 @@
         <v>255</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -35830,15 +35830,15 @@
         <v>256</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="390" x14ac:dyDescent="0.25">
@@ -35862,7 +35862,7 @@
         <v>22</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35878,7 +35878,7 @@
         <v>23</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -35894,7 +35894,7 @@
         <v>3</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -35902,7 +35902,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35926,7 +35926,7 @@
         <v>7</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -35934,7 +35934,7 @@
         <v>8</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35942,7 +35942,7 @@
         <v>10</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -35950,7 +35950,7 @@
         <v>9</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -35958,7 +35958,7 @@
         <v>11</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -35990,7 +35990,7 @@
         <v>15</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -35998,7 +35998,7 @@
         <v>16</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -36006,7 +36006,7 @@
         <v>17</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -36014,7 +36014,7 @@
         <v>18</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -36022,31 +36022,31 @@
         <v>261</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -36054,7 +36054,7 @@
         <v>19</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -36062,7 +36062,7 @@
         <v>20</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -36070,23 +36070,23 @@
         <v>21</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -36094,23 +36094,23 @@
         <v>25</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -36118,7 +36118,7 @@
         <v>26</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -36142,7 +36142,7 @@
         <v>27</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -36150,7 +36150,7 @@
         <v>28</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -36158,7 +36158,7 @@
         <v>29</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -36166,7 +36166,7 @@
         <v>30</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -36182,7 +36182,7 @@
         <v>697</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -36190,7 +36190,7 @@
         <v>31</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -36198,7 +36198,7 @@
         <v>32</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -36206,7 +36206,7 @@
         <v>33</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -36238,7 +36238,7 @@
         <v>493</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -36262,7 +36262,7 @@
         <v>264</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -36270,7 +36270,7 @@
         <v>265</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -36294,7 +36294,7 @@
         <v>35</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -36406,7 +36406,7 @@
         <v>42</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -36414,7 +36414,7 @@
         <v>46</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -36478,7 +36478,7 @@
         <v>54</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -36534,7 +36534,7 @@
         <v>778</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -36542,15 +36542,15 @@
         <v>59</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
+        <v>878</v>
+      </c>
+      <c r="B94" s="3" t="s">
         <v>879</v>
-      </c>
-      <c r="B94" s="3" t="s">
-        <v>880</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -36566,7 +36566,7 @@
         <v>768</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -36622,7 +36622,7 @@
         <v>66</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -36670,7 +36670,7 @@
         <v>471</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -36702,7 +36702,7 @@
         <v>70</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -36790,7 +36790,7 @@
         <v>77</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
     </row>
     <row r="125" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -36803,10 +36803,10 @@
     </row>
     <row r="126" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="127" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -36814,7 +36814,7 @@
         <v>78</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
     </row>
     <row r="128" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -36822,7 +36822,7 @@
         <v>374</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
     </row>
     <row r="129" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -36870,87 +36870,87 @@
         <v>81</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
     </row>
     <row r="135" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
     </row>
     <row r="136" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
     </row>
     <row r="137" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
     </row>
     <row r="138" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
     </row>
     <row r="139" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="B139" s="3" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
     </row>
     <row r="140" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
     </row>
     <row r="141" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
     </row>
     <row r="142" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
     </row>
     <row r="143" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
+        <v>939</v>
+      </c>
+      <c r="B143" s="3" t="s">
         <v>940</v>
-      </c>
-      <c r="B143" s="3" t="s">
-        <v>941</v>
       </c>
     </row>
     <row r="144" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
     </row>
     <row r="145" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -36958,7 +36958,7 @@
         <v>82</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
     </row>
     <row r="146" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -36971,7 +36971,7 @@
     </row>
     <row r="147" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="B147" s="3" t="s">
         <v>547</v>
@@ -37006,7 +37006,7 @@
         <v>546</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>803</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="152" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37014,7 +37014,7 @@
         <v>86</v>
       </c>
       <c r="B152" s="3" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
     </row>
     <row r="153" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -37094,7 +37094,7 @@
         <v>346</v>
       </c>
       <c r="B162" s="3" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="163" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -37126,7 +37126,7 @@
         <v>440</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
     </row>
     <row r="167" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37150,23 +37150,23 @@
         <v>90</v>
       </c>
       <c r="B169" s="3" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
     </row>
     <row r="170" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="B170" s="3" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
     </row>
     <row r="171" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="B171" s="3" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
     </row>
     <row r="172" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -37198,7 +37198,7 @@
         <v>93</v>
       </c>
       <c r="B175" s="3" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
     </row>
     <row r="176" spans="1:2" ht="270" x14ac:dyDescent="0.25">
@@ -37206,7 +37206,7 @@
         <v>94</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
     </row>
     <row r="177" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37214,7 +37214,7 @@
         <v>95</v>
       </c>
       <c r="B177" s="3" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
     </row>
     <row r="178" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37222,55 +37222,55 @@
         <v>96</v>
       </c>
       <c r="B178" s="3" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
     <row r="179" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A179" s="2" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="B179" s="3" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="180" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A180" s="2" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="B180" s="3" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="181" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="182" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="B182" s="3" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="183" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="B183" s="3" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
     </row>
     <row r="184" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A184" s="2" t="s">
+        <v>855</v>
+      </c>
+      <c r="B184" s="3" t="s">
         <v>856</v>
-      </c>
-      <c r="B184" s="3" t="s">
-        <v>857</v>
       </c>
     </row>
     <row r="185" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -37278,7 +37278,7 @@
         <v>97</v>
       </c>
       <c r="B185" s="3" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
     </row>
     <row r="186" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -37326,7 +37326,7 @@
         <v>103</v>
       </c>
       <c r="B191" s="3" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
     </row>
     <row r="192" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37334,7 +37334,7 @@
         <v>104</v>
       </c>
       <c r="B192" s="3" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
     </row>
     <row r="193" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37350,7 +37350,7 @@
         <v>684</v>
       </c>
       <c r="B194" s="3" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="195" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37366,7 +37366,7 @@
         <v>106</v>
       </c>
       <c r="B196" s="3" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
     </row>
     <row r="197" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37374,7 +37374,7 @@
         <v>107</v>
       </c>
       <c r="B197" s="3" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
     </row>
     <row r="198" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -37382,15 +37382,15 @@
         <v>165</v>
       </c>
       <c r="B198" s="3" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
     </row>
     <row r="199" spans="1:2" ht="225" x14ac:dyDescent="0.25">
       <c r="A199" s="2" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="B199" s="3" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
     </row>
     <row r="200" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37398,7 +37398,7 @@
         <v>108</v>
       </c>
       <c r="B200" s="3" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
     </row>
     <row r="201" spans="1:2" ht="285" x14ac:dyDescent="0.25">
@@ -37406,7 +37406,7 @@
         <v>109</v>
       </c>
       <c r="B201" s="3" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
     </row>
     <row r="202" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -37422,7 +37422,7 @@
         <v>166</v>
       </c>
       <c r="B203" s="3" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="204" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -37430,7 +37430,7 @@
         <v>167</v>
       </c>
       <c r="B204" s="3" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="205" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -37438,23 +37438,23 @@
         <v>168</v>
       </c>
       <c r="B205" s="3" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
     </row>
     <row r="206" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A206" s="2" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="B206" s="3" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="207" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A207" s="2" t="s">
+        <v>869</v>
+      </c>
+      <c r="B207" s="3" t="s">
         <v>870</v>
-      </c>
-      <c r="B207" s="3" t="s">
-        <v>871</v>
       </c>
     </row>
     <row r="208" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37526,7 +37526,7 @@
         <v>171</v>
       </c>
       <c r="B216" s="3" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="217" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37534,7 +37534,7 @@
         <v>113</v>
       </c>
       <c r="B217" s="3" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
     </row>
     <row r="218" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -37542,7 +37542,7 @@
         <v>114</v>
       </c>
       <c r="B218" s="3" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
     </row>
     <row r="219" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -37550,15 +37550,15 @@
         <v>266</v>
       </c>
       <c r="B219" s="3" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
     </row>
     <row r="220" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A220" s="2" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="B220" s="3" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
     </row>
     <row r="221" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37566,7 +37566,7 @@
         <v>115</v>
       </c>
       <c r="B221" s="3" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
     </row>
     <row r="222" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -37582,7 +37582,7 @@
         <v>116</v>
       </c>
       <c r="B223" s="3" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="224" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -37598,7 +37598,7 @@
         <v>117</v>
       </c>
       <c r="B225" s="4" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
     </row>
     <row r="226" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -37622,7 +37622,7 @@
         <v>742</v>
       </c>
       <c r="B228" s="4" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
     </row>
     <row r="229" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -37630,23 +37630,23 @@
         <v>118</v>
       </c>
       <c r="B229" s="3" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
     </row>
     <row r="230" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A230" s="2" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="B230" s="3" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
     </row>
     <row r="231" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A231" s="2" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="B231" s="3" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="232" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -37654,23 +37654,23 @@
         <v>119</v>
       </c>
       <c r="B232" s="3" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
     </row>
     <row r="233" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A233" s="2" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="B233" s="3" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
     </row>
     <row r="234" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A234" s="2" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="B234" s="3" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="235" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -37678,7 +37678,7 @@
         <v>120</v>
       </c>
       <c r="B235" s="3" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
     </row>
     <row r="236" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -37686,7 +37686,7 @@
         <v>172</v>
       </c>
       <c r="B236" s="3" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
     </row>
     <row r="237" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37694,7 +37694,7 @@
         <v>173</v>
       </c>
       <c r="B237" s="3" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
     </row>
     <row r="238" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37702,7 +37702,7 @@
         <v>174</v>
       </c>
       <c r="B238" s="3" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
     </row>
     <row r="239" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37734,23 +37734,23 @@
         <v>123</v>
       </c>
       <c r="B242" s="3" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
     </row>
     <row r="243" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A243" s="2" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="B243" s="3" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="244" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A244" s="2" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="B244" s="3" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="245" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37763,10 +37763,10 @@
     </row>
     <row r="246" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A246" s="2" t="s">
+        <v>1114</v>
+      </c>
+      <c r="B246" s="3" t="s">
         <v>1115</v>
-      </c>
-      <c r="B246" s="3" t="s">
-        <v>1116</v>
       </c>
     </row>
     <row r="247" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37774,15 +37774,15 @@
         <v>125</v>
       </c>
       <c r="B247" s="3" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
     </row>
     <row r="248" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A248" s="2" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="B248" s="3" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="249" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37790,7 +37790,7 @@
         <v>126</v>
       </c>
       <c r="B249" s="3" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
     </row>
     <row r="250" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37798,7 +37798,7 @@
         <v>127</v>
       </c>
       <c r="B250" s="3" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
     </row>
     <row r="251" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37814,7 +37814,7 @@
         <v>129</v>
       </c>
       <c r="B252" s="3" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
     </row>
     <row r="253" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37822,7 +37822,7 @@
         <v>130</v>
       </c>
       <c r="B253" s="3" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
     </row>
     <row r="254" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -37830,23 +37830,23 @@
         <v>131</v>
       </c>
       <c r="B254" s="3" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
     </row>
     <row r="255" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A255" s="2" t="s">
+        <v>915</v>
+      </c>
+      <c r="B255" s="3" t="s">
         <v>916</v>
-      </c>
-      <c r="B255" s="3" t="s">
-        <v>917</v>
       </c>
     </row>
     <row r="256" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A256" s="2" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="B256" s="3" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
     </row>
     <row r="257" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -37854,7 +37854,7 @@
         <v>132</v>
       </c>
       <c r="B257" s="3" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
     </row>
     <row r="258" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -37862,15 +37862,15 @@
         <v>133</v>
       </c>
       <c r="B258" s="3" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="259" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A259" s="2" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="B259" s="3" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="260" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37878,23 +37878,23 @@
         <v>134</v>
       </c>
       <c r="B260" s="3" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
     </row>
     <row r="261" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A261" s="2" t="s">
+        <v>967</v>
+      </c>
+      <c r="B261" s="3" t="s">
         <v>968</v>
-      </c>
-      <c r="B261" s="3" t="s">
-        <v>969</v>
       </c>
     </row>
     <row r="262" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A262" s="2" t="s">
+        <v>969</v>
+      </c>
+      <c r="B262" s="3" t="s">
         <v>970</v>
-      </c>
-      <c r="B262" s="3" t="s">
-        <v>971</v>
       </c>
     </row>
     <row r="263" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -37902,15 +37902,15 @@
         <v>135</v>
       </c>
       <c r="B263" s="3" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
     </row>
     <row r="264" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A264" s="2" t="s">
+        <v>972</v>
+      </c>
+      <c r="B264" s="3" t="s">
         <v>973</v>
-      </c>
-      <c r="B264" s="3" t="s">
-        <v>974</v>
       </c>
     </row>
     <row r="265" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -37918,7 +37918,7 @@
         <v>136</v>
       </c>
       <c r="B265" s="3" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
     </row>
     <row r="266" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -37942,7 +37942,7 @@
         <v>233</v>
       </c>
       <c r="B268" s="3" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="269" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -37958,7 +37958,7 @@
         <v>234</v>
       </c>
       <c r="B270" s="3" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="271" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37966,7 +37966,7 @@
         <v>235</v>
       </c>
       <c r="B271" s="3" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="272" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -38006,7 +38006,7 @@
         <v>140</v>
       </c>
       <c r="B276" s="3" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="277" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -38014,7 +38014,7 @@
         <v>236</v>
       </c>
       <c r="B277" s="3" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="278" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -38022,7 +38022,7 @@
         <v>237</v>
       </c>
       <c r="B278" s="3" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="279" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -38030,7 +38030,7 @@
         <v>238</v>
       </c>
       <c r="B279" s="3" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="280" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -38038,7 +38038,7 @@
         <v>141</v>
       </c>
       <c r="B280" s="3" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="281" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -38046,7 +38046,7 @@
         <v>142</v>
       </c>
       <c r="B281" s="3" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="282" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38054,7 +38054,7 @@
         <v>143</v>
       </c>
       <c r="B282" s="3" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="283" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -38062,7 +38062,7 @@
         <v>144</v>
       </c>
       <c r="B283" s="3" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="284" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -38070,7 +38070,7 @@
         <v>242</v>
       </c>
       <c r="B284" s="3" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="285" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -38078,7 +38078,7 @@
         <v>145</v>
       </c>
       <c r="B285" s="3" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="286" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -38086,7 +38086,7 @@
         <v>146</v>
       </c>
       <c r="B286" s="3" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="287" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -38094,7 +38094,7 @@
         <v>147</v>
       </c>
       <c r="B287" s="3" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="288" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38102,7 +38102,7 @@
         <v>148</v>
       </c>
       <c r="B288" s="3" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="289" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -38110,31 +38110,31 @@
         <v>149</v>
       </c>
       <c r="B289" s="3" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="290" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A290" s="2" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="B290" s="3" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="291" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A291" s="2" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="B291" s="3" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="292" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A292" s="2" t="s">
+        <v>1037</v>
+      </c>
+      <c r="B292" s="3" t="s">
         <v>1038</v>
-      </c>
-      <c r="B292" s="3" t="s">
-        <v>1039</v>
       </c>
     </row>
     <row r="293" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -38142,15 +38142,15 @@
         <v>150</v>
       </c>
       <c r="B293" s="3" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="294" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A294" s="2" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="B294" s="3" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="295" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -38174,7 +38174,7 @@
         <v>244</v>
       </c>
       <c r="B297" s="3" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="298" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -38198,7 +38198,7 @@
         <v>153</v>
       </c>
       <c r="B300" s="3" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="301" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -38270,7 +38270,7 @@
         <v>159</v>
       </c>
       <c r="B309" s="3" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
     </row>
     <row r="310" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -38278,7 +38278,7 @@
         <v>160</v>
       </c>
       <c r="B310" s="3" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
     </row>
     <row r="311" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -38286,7 +38286,7 @@
         <v>161</v>
       </c>
       <c r="B311" s="3" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
     </row>
     <row r="312" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -38294,31 +38294,31 @@
         <v>162</v>
       </c>
       <c r="B312" s="3" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="313" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A313" s="2" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="B313" s="3" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="314" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A314" s="2" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="B314" s="3" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="315" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A315" s="2" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="B315" s="3" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="316" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -38326,7 +38326,7 @@
         <v>163</v>
       </c>
       <c r="B316" s="3" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="317" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -38334,7 +38334,7 @@
         <v>164</v>
       </c>
       <c r="B317" s="3" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
     </row>
     <row r="318" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -38342,7 +38342,7 @@
         <v>175</v>
       </c>
       <c r="B318" s="3" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
     </row>
     <row r="319" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -38350,7 +38350,7 @@
         <v>176</v>
       </c>
       <c r="B319" s="3" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
     </row>
     <row r="320" spans="1:2" ht="390" x14ac:dyDescent="0.25">
@@ -38358,7 +38358,7 @@
         <v>177</v>
       </c>
       <c r="B320" s="3" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
     </row>
     <row r="321" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -38366,7 +38366,7 @@
         <v>516</v>
       </c>
       <c r="B321" s="3" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
     </row>
     <row r="322" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -38374,7 +38374,7 @@
         <v>517</v>
       </c>
       <c r="B322" s="3" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
     </row>
     <row r="323" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -38382,7 +38382,7 @@
         <v>518</v>
       </c>
       <c r="B323" s="3" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
     </row>
     <row r="324" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -38390,7 +38390,7 @@
         <v>519</v>
       </c>
       <c r="B324" s="3" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="325" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -38398,7 +38398,7 @@
         <v>520</v>
       </c>
       <c r="B325" s="3" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
     </row>
     <row r="326" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -38406,15 +38406,15 @@
         <v>521</v>
       </c>
       <c r="B326" s="3" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
     </row>
     <row r="327" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A327" s="2" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="B327" s="3" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="328" spans="1:2" ht="390" x14ac:dyDescent="0.25">
@@ -38422,7 +38422,7 @@
         <v>178</v>
       </c>
       <c r="B328" s="3" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
     </row>
     <row r="329" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -38430,7 +38430,7 @@
         <v>491</v>
       </c>
       <c r="B329" s="3" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="330" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -38438,7 +38438,7 @@
         <v>543</v>
       </c>
       <c r="B330" s="3" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="331" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -38446,7 +38446,7 @@
         <v>544</v>
       </c>
       <c r="B331" s="3" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
     </row>
     <row r="332" spans="1:2" ht="315" x14ac:dyDescent="0.25">
@@ -38454,7 +38454,7 @@
         <v>179</v>
       </c>
       <c r="B332" s="3" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
     </row>
     <row r="333" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -38462,7 +38462,7 @@
         <v>249</v>
       </c>
       <c r="B333" s="3" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
     </row>
     <row r="334" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -38470,7 +38470,7 @@
         <v>250</v>
       </c>
       <c r="B334" s="3" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
     </row>
     <row r="335" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -38478,7 +38478,7 @@
         <v>251</v>
       </c>
       <c r="B335" s="3" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
     </row>
     <row r="336" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38486,7 +38486,7 @@
         <v>252</v>
       </c>
       <c r="B336" s="3" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="337" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -38494,23 +38494,23 @@
         <v>253</v>
       </c>
       <c r="B337" s="3" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
     </row>
     <row r="338" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A338" s="2" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="B338" s="3" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
     </row>
     <row r="339" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A339" s="2" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B339" s="3" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
     </row>
     <row r="340" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -38518,7 +38518,7 @@
         <v>180</v>
       </c>
       <c r="B340" s="3" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
     </row>
     <row r="341" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38542,15 +38542,15 @@
         <v>182</v>
       </c>
       <c r="B343" s="3" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="344" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A344" s="2" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="B344" s="3" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="345" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38558,7 +38558,7 @@
         <v>183</v>
       </c>
       <c r="B345" s="3" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="346" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -38566,7 +38566,7 @@
         <v>184</v>
       </c>
       <c r="B346" s="3" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="347" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -38582,7 +38582,7 @@
         <v>185</v>
       </c>
       <c r="B348" s="3" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
     </row>
     <row r="349" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -38606,7 +38606,7 @@
         <v>466</v>
       </c>
       <c r="B351" s="3" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="352" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -38686,7 +38686,7 @@
         <v>338</v>
       </c>
       <c r="B361" s="3" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="362" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -38694,7 +38694,7 @@
         <v>339</v>
       </c>
       <c r="B362" s="3" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="363" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -38710,15 +38710,15 @@
         <v>195</v>
       </c>
       <c r="B364" s="3" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="365" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A365" s="2" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="B365" s="3" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="366" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -38726,7 +38726,7 @@
         <v>196</v>
       </c>
       <c r="B366" s="3" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
     </row>
     <row r="367" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -38734,7 +38734,7 @@
         <v>330</v>
       </c>
       <c r="B367" s="3" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="368" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -38750,7 +38750,7 @@
         <v>652</v>
       </c>
       <c r="B369" s="3" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="370" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38774,7 +38774,7 @@
         <v>200</v>
       </c>
       <c r="B372" s="3" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="373" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -38790,7 +38790,7 @@
         <v>202</v>
       </c>
       <c r="B374" s="3" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
     </row>
     <row r="375" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -38910,7 +38910,7 @@
         <v>582</v>
       </c>
       <c r="B389" s="3" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="390" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -38918,7 +38918,7 @@
         <v>583</v>
       </c>
       <c r="B390" s="3" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
     </row>
     <row r="391" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -38926,7 +38926,7 @@
         <v>584</v>
       </c>
       <c r="B391" s="3" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
     </row>
     <row r="392" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -38934,7 +38934,7 @@
         <v>585</v>
       </c>
       <c r="B392" s="3" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
     </row>
     <row r="393" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38950,7 +38950,7 @@
         <v>587</v>
       </c>
       <c r="B394" s="3" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="395" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38966,7 +38966,7 @@
         <v>207</v>
       </c>
       <c r="B396" s="3" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
     </row>
     <row r="397" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -38982,7 +38982,7 @@
         <v>209</v>
       </c>
       <c r="B398" s="3" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="399" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -38990,7 +38990,7 @@
         <v>635</v>
       </c>
       <c r="B399" s="3" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
     <row r="400" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -39035,10 +39035,10 @@
     </row>
     <row r="405" spans="1:2" ht="240" x14ac:dyDescent="0.25">
       <c r="A405" s="2" t="s">
+        <v>1134</v>
+      </c>
+      <c r="B405" s="3" t="s">
         <v>1135</v>
-      </c>
-      <c r="B405" s="3" t="s">
-        <v>1136</v>
       </c>
     </row>
     <row r="406" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -39046,7 +39046,7 @@
         <v>210</v>
       </c>
       <c r="B406" s="3" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="407" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -39107,10 +39107,10 @@
     </row>
     <row r="414" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A414" s="2" t="s">
+        <v>1124</v>
+      </c>
+      <c r="B414" s="3" t="s">
         <v>1125</v>
-      </c>
-      <c r="B414" s="3" t="s">
-        <v>1126</v>
       </c>
     </row>
     <row r="415" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -39134,7 +39134,7 @@
         <v>532</v>
       </c>
       <c r="B417" s="3" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="418" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -39166,7 +39166,7 @@
         <v>213</v>
       </c>
       <c r="B421" s="3" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="422" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -39182,7 +39182,7 @@
         <v>215</v>
       </c>
       <c r="B423" s="3" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="424" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39230,7 +39230,7 @@
         <v>221</v>
       </c>
       <c r="B429" s="3" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="430" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -39238,7 +39238,7 @@
         <v>222</v>
       </c>
       <c r="B430" s="3" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="431" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -39246,7 +39246,7 @@
         <v>223</v>
       </c>
       <c r="B431" s="3" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="432" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -39254,7 +39254,7 @@
         <v>224</v>
       </c>
       <c r="B432" s="3" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="433" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -39262,7 +39262,7 @@
         <v>331</v>
       </c>
       <c r="B433" s="3" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="434" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -39278,7 +39278,7 @@
         <v>225</v>
       </c>
       <c r="B435" s="3" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
     </row>
     <row r="436" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -39302,15 +39302,15 @@
         <v>228</v>
       </c>
       <c r="B438" s="3" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="439" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A439" s="2" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="B439" s="3" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="440" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -39350,7 +39350,7 @@
         <v>444</v>
       </c>
       <c r="B444" s="3" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="445" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -39390,7 +39390,7 @@
         <v>319</v>
       </c>
       <c r="B449" s="3" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="450" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -39398,7 +39398,7 @@
         <v>320</v>
       </c>
       <c r="B450" s="3" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="451" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -39406,7 +39406,7 @@
         <v>321</v>
       </c>
       <c r="B451" s="3" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="452" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -39414,15 +39414,15 @@
         <v>318</v>
       </c>
       <c r="B452" s="3" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="453" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A453" s="2" t="s">
+        <v>1013</v>
+      </c>
+      <c r="B453" s="3" t="s">
         <v>1014</v>
-      </c>
-      <c r="B453" s="3" t="s">
-        <v>1015</v>
       </c>
     </row>
     <row r="454" spans="1:2" ht="255" x14ac:dyDescent="0.25">
@@ -39430,7 +39430,7 @@
         <v>322</v>
       </c>
       <c r="B454" s="3" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="455" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39454,7 +39454,7 @@
         <v>485</v>
       </c>
       <c r="B457" s="3" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="458" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -39462,7 +39462,7 @@
         <v>486</v>
       </c>
       <c r="B458" s="3" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="459" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39494,7 +39494,7 @@
         <v>552</v>
       </c>
       <c r="B462" s="3" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
     </row>
     <row r="463" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -39502,7 +39502,7 @@
         <v>556</v>
       </c>
       <c r="B463" s="3" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="464" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -39518,7 +39518,7 @@
         <v>560</v>
       </c>
       <c r="B465" s="3" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="466" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39542,7 +39542,7 @@
         <v>563</v>
       </c>
       <c r="B468" s="3" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
     </row>
     <row r="469" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -39550,7 +39550,7 @@
         <v>564</v>
       </c>
       <c r="B469" s="3" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="470" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -39566,7 +39566,7 @@
         <v>566</v>
       </c>
       <c r="B471" s="3" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
     </row>
     <row r="472" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -39598,7 +39598,7 @@
         <v>596</v>
       </c>
       <c r="B475" s="3" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
     </row>
     <row r="476" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -39606,7 +39606,7 @@
         <v>614</v>
       </c>
       <c r="B476" s="3" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="477" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -39614,7 +39614,7 @@
         <v>615</v>
       </c>
       <c r="B477" s="3" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="478" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -39622,15 +39622,15 @@
         <v>616</v>
       </c>
       <c r="B478" s="3" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="479" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A479" s="2" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="B479" s="3" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="480" spans="1:2" ht="255" x14ac:dyDescent="0.25">
@@ -39686,7 +39686,7 @@
         <v>659</v>
       </c>
       <c r="B486" s="1" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
     </row>
     <row r="487" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -39726,7 +39726,7 @@
         <v>664</v>
       </c>
       <c r="B491" s="1" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
     </row>
     <row r="492" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -39755,18 +39755,18 @@
     </row>
     <row r="495" spans="1:2" ht="255" x14ac:dyDescent="0.25">
       <c r="A495" s="2" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="B495" s="1" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="496" spans="1:2" ht="92.25" x14ac:dyDescent="0.25">
       <c r="A496" s="2" t="s">
+        <v>995</v>
+      </c>
+      <c r="B496" s="1" t="s">
         <v>996</v>
-      </c>
-      <c r="B496" s="1" t="s">
-        <v>997</v>
       </c>
     </row>
     <row r="497" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -39774,7 +39774,7 @@
         <v>682</v>
       </c>
       <c r="B497" s="1" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
     </row>
     <row r="498" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -39782,7 +39782,7 @@
         <v>714</v>
       </c>
       <c r="B498" s="3" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="499" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -39878,7 +39878,7 @@
         <v>275</v>
       </c>
       <c r="B510" s="1" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="511" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39886,7 +39886,7 @@
         <v>276</v>
       </c>
       <c r="B511" s="1" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="512" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39894,7 +39894,7 @@
         <v>277</v>
       </c>
       <c r="B512" s="1" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="513" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -39942,7 +39942,7 @@
         <v>260</v>
       </c>
       <c r="B518" s="3" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="519" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -40014,7 +40014,7 @@
         <v>285</v>
       </c>
       <c r="B527" s="1" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
     </row>
     <row r="528" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -40022,7 +40022,7 @@
         <v>286</v>
       </c>
       <c r="B528" s="1" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
     </row>
     <row r="529" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -40142,7 +40142,7 @@
         <v>298</v>
       </c>
       <c r="B543" s="1" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
     </row>
     <row r="544" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -40182,7 +40182,7 @@
         <v>300</v>
       </c>
       <c r="B548" s="1" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
     </row>
     <row r="549" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -40190,7 +40190,7 @@
         <v>301</v>
       </c>
       <c r="B549" s="1" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
     </row>
     <row r="550" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -40318,7 +40318,7 @@
         <v>307</v>
       </c>
       <c r="B565" s="1" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
     </row>
     <row r="566" spans="1:2" ht="375" x14ac:dyDescent="0.25">
@@ -40350,7 +40350,7 @@
         <v>373</v>
       </c>
       <c r="B569" s="3" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="570" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -40366,7 +40366,7 @@
         <v>328</v>
       </c>
       <c r="B571" s="3" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Still have problem with gi.DieResults[key][0] returned to no roll
</commit_message>
<xml_diff>
--- a/Documentation/Events.xlsx
+++ b/Documentation/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\happysulla\BarbarianPrince\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BB42C8EB-999A-4ED2-B1E2-1A9B4DE1FE7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0A8CC11D-7F67-41AE-916C-D5447A63BC0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -35005,11 +35005,274 @@
   </si>
   <si>
     <r>
+      <t>&lt;Bold&gt;e136 Hidden Treasures&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;You uncover the remains of a palace treasure room. Roll one die for the contents:
+ &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dieRoll</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.gif' Name='</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DieRoll</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+1 - &lt;InlineUIContainer&gt;&lt;Button Content='e037' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;&lt;LineBreak/&gt;
+2 - &lt;InlineUIContainer&gt;&lt;Button Content='e038' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;&lt;LineBreak/&gt;
+3 - &lt;InlineUIContainer&gt;&lt;Button Content='e039' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;&lt;LineBreak/&gt;
+4 - &lt;InlineUIContainer&gt;&lt;Button Content='e044' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;&lt;LineBreak/&gt;
+5 - 500 gold pieces&lt;LineBreak/&gt;
+6 - Nothing&lt;LineBreak/&gt;
+&lt;LineBreak/&gt;
+                         &lt;InlineUIContainer&gt;&lt;Image Name='</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TreasureRoomDoor</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>' Source='../../Images/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TreasureRoomDoor.gif</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>' Height='220'  Width='300'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;Bold&gt;e209c Feel at Home&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;Feel at home, learning nothing, but in the future always add one whenever resolving this action in this hex or when Seeking to Hire in this hex
+  &lt;InlineUIContainer&gt;&lt;Button Content='r210' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. Click image to continue.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                              &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>HappyFace</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.gif' Name='</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>EncounterEnd</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>' Height='300' Width='300'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t>e133a</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e133 Plague&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;After considerable searching during the day, you and your party find a variety of items worth 50 gold pieces amoung may skeletons. Tonight, just before you start to eat
+ &lt;InlineUIContainer&gt;&lt;Button Content='r215' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;,
+ a plague of mind-madness begins to affect your party due to an ancient curse on this place. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;Roll one die for each character in the party, a 3+ means madness has destroyed the mind and the character crumples into a heap and soon dies, foaming at the mouth. All surviving members of the party immediately ecape from the hex per &lt;InlineUIContainer&gt;&lt;Button Content='r218' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; and camp elsewhere for the night per &lt;InlineUIContainer&gt;&lt;Button Content='r215' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;Mounts are not affected, so survivors can bring mounts, possessions, and wealth of the entire party with them.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;If the Prince is affected by the plague, see  &lt;InlineUIContainer&gt;&lt;Button Content='e133a' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Click anywhere to continue.</t>
+  </si>
+  <si>
+    <r>
+      <t>&lt;Bold&gt;e133a Plague Affects Prince&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;If the you are affected by the plague, your Northern blood helps you to survive. You awake the next morning, having gone without food &lt;InlineUIContainer&gt;&lt;Button Content='r216' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;, and find all your surviving followers dead or escaped with all your wealth and possessioins. You can now deicde what action to take for the new day per &lt;InlineUIContainer&gt;&lt;Button Content='r203' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Click image to continue.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                  &lt;InlineUIContainer&gt;&lt;Image Name='</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>PlaguePrinceEnd</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>' Source='../../Images/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Nothing</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.gif' Height='200' Width='200'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;Bold&gt;e050f Mercenary Royal Guardsmen&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;Since you are within three hexes of Ogon
+  &lt;InlineUIContainer&gt;&lt;Button Content='0101' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+ or Weshor
+  &lt;InlineUIContainer&gt;&lt;Button Content='1501' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;,
+ you do not encounter local constabulary. Instead, you may encounter the mercenary royal guardsmen. You see mercenary royal guardsmen attempting to find you. Roll one die, subtract three, then add one if you are in Ogon or Weshor.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+If the results is 1 plus, encounter the guardsmen
+ &lt;InlineUIContainer&gt;&lt;Button Content='e002a' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+If the result is zero or less, no event occurs:
+ &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dieRoll</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">.gif' </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Name='DieRoll'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Height='21'  Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <t>&lt;Bold&gt;e160g Audience with Lady Aeravir Knowing Her Secret&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 You are allowed a semi-private interview with the ruler of Aeravir Castle. Since you know her secret, see  &lt;InlineUIContainer&gt;&lt;Button Content='e145' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. You roll twice and pick the result you want.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Roll one die for the results:  &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/dieRoll.gif' Name='DieRoll' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 &lt;InlineUIContainer&gt;&lt;Button Content='e160a' FontFamily='Courier New' FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; - 1 - Shows No Interest&lt;LineBreak/&gt;
 &lt;InlineUIContainer&gt;&lt;Button Content='e160b' FontFamily='Courier New' FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; - 2 -Distracted &lt;LineBreak/&gt;
@@ -35060,271 +35323,6 @@
         <scheme val="minor"/>
       </rPr>
       <t>' Height='21'  Width='21'  Visibility='Hidden'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>&lt;Bold&gt;e136 Hidden Treasures&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;You uncover the remains of a palace treasure room. Roll one die for the contents:
- &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>dieRoll</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.gif' Name='</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>DieRoll</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-1 - &lt;InlineUIContainer&gt;&lt;Button Content='e037' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;&lt;LineBreak/&gt;
-2 - &lt;InlineUIContainer&gt;&lt;Button Content='e038' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;&lt;LineBreak/&gt;
-3 - &lt;InlineUIContainer&gt;&lt;Button Content='e039' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;&lt;LineBreak/&gt;
-4 - &lt;InlineUIContainer&gt;&lt;Button Content='e044' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;&lt;LineBreak/&gt;
-5 - 500 gold pieces&lt;LineBreak/&gt;
-6 - Nothing&lt;LineBreak/&gt;
-&lt;LineBreak/&gt;
-                         &lt;InlineUIContainer&gt;&lt;Image Name='</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>TreasureRoomDoor</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>' Source='../../Images/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>TreasureRoomDoor.gif</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>' Height='220'  Width='300'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>&lt;Bold&gt;e209c Feel at Home&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;Feel at home, learning nothing, but in the future always add one whenever resolving this action in this hex or when Seeking to Hire in this hex
-  &lt;InlineUIContainer&gt;&lt;Button Content='r210' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. Click image to continue.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                              &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>HappyFace</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.gif' Name='</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>EncounterEnd</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>' Height='300' Width='300'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-    </r>
-  </si>
-  <si>
-    <t>e133a</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e133 Plague&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;After considerable searching during the day, you and your party find a variety of items worth 50 gold pieces amoung may skeletons. Tonight, just before you start to eat
- &lt;InlineUIContainer&gt;&lt;Button Content='r215' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;,
- a plague of mind-madness begins to affect your party due to an ancient curse on this place. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;Roll one die for each character in the party, a 3+ means madness has destroyed the mind and the character crumples into a heap and soon dies, foaming at the mouth. All surviving members of the party immediately ecape from the hex per &lt;InlineUIContainer&gt;&lt;Button Content='r218' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; and camp elsewhere for the night per &lt;InlineUIContainer&gt;&lt;Button Content='r215' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;Mounts are not affected, so survivors can bring mounts, possessions, and wealth of the entire party with them.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;If the Prince is affected by the plague, see  &lt;InlineUIContainer&gt;&lt;Button Content='e133a' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Click anywhere to continue.</t>
-  </si>
-  <si>
-    <r>
-      <t>&lt;Bold&gt;e133a Plague Affects Prince&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;If the you are affected by the plague, your Northern blood helps you to survive. You awake the next morning, having gone without food &lt;InlineUIContainer&gt;&lt;Button Content='r216' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;, and find all your surviving followers dead or escaped with all your wealth and possessioins. You can now deicde what action to take for the new day per &lt;InlineUIContainer&gt;&lt;Button Content='r203' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Click image to continue.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                  &lt;InlineUIContainer&gt;&lt;Image Name='</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>PlaguePrinceEnd</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>' Source='../../Images/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Nothing</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.gif' Height='200' Width='200'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>&lt;Bold&gt;e050f Mercenary Royal Guardsmen&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;Since you are within three hexes of Ogon
-  &lt;InlineUIContainer&gt;&lt;Button Content='0101' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
- or Weshor
-  &lt;InlineUIContainer&gt;&lt;Button Content='1501' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;,
- you do not encounter local constabulary. Instead, you may encounter the mercenary royal guardsmen. You see mercenary royal guardsmen attempting to find you. Roll one die, subtract three, then add one if you are in Ogon or Weshor.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-If the results is 1 plus, encounter the guardsmen
- &lt;InlineUIContainer&gt;&lt;Button Content='e002a' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-If the result is zero or less, no event occurs:
- &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>dieRoll</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">.gif' </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Name='DieRoll'</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Height='21'  Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
     </r>
   </si>
 </sst>
@@ -35791,8 +35789,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B571"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A150" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B151" sqref="B151"/>
+    <sheetView tabSelected="1" topLeftCell="A403" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B405" sqref="B405"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -37006,7 +37004,7 @@
         <v>546</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="152" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -38542,15 +38540,15 @@
         <v>182</v>
       </c>
       <c r="B343" s="3" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="344" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A344" s="2" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
       <c r="B344" s="3" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="345" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38582,7 +38580,7 @@
         <v>185</v>
       </c>
       <c r="B348" s="3" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
     </row>
     <row r="349" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -39033,12 +39031,12 @@
         <v>645</v>
       </c>
     </row>
-    <row r="405" spans="1:2" ht="240" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A405" s="2" t="s">
         <v>1134</v>
       </c>
       <c r="B405" s="3" t="s">
-        <v>1135</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="406" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -39462,7 +39460,7 @@
         <v>486</v>
       </c>
       <c r="B458" s="3" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
     </row>
     <row r="459" spans="1:2" ht="90" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Finished on path of e144 to restore the heir to his throne
</commit_message>
<xml_diff>
--- a/Documentation/Events.xlsx
+++ b/Documentation/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\happysulla\BarbarianPrince\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{958D2371-A893-4DC9-AA0C-D3BBC60BE9A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1490400D-635A-4ABA-AD4B-079ABFAFDC1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1148" uniqueCount="1148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1158" uniqueCount="1158">
   <si>
     <t>e001</t>
   </si>
@@ -35234,207 +35234,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t>&lt;Bold&gt;e144d Travel with Heir to Huldra Castle&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-You travel with the heir. If you reach Huldra Castle, your party and the heir have two options.&lt;LineBreak/&gt;
-1.) You can seek an audience with the current Baron
- &lt;InlineUIContainer&gt;&lt;Button Content='r211' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
- If you roll a 10 plus, you can reveal the true heir at the audience and despose the current Baron instantly. 
-&lt;LineBreak/&gt;
-2.)You can make a sneak attack on the Baron at night suprising his traditional six bodyguards
- &lt;InlineUIContainer&gt; &lt;Button Content='r220' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
- Each has combat skill 6 and endurance 6. After killing bodyguards, you can attack the Baron who has combat skill 6 and endurance 8. The Baron strikes first in combat.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-If you succeed in disposing the original Baron, the heir will take the throne and will return the favor by marching his army with you back to the Northlands to help you regain your throne. You win the game due to the aide of the new Baron Huldra! Click image to continue.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                     &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>BaronHuldra1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.gif' Name='</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>BaronHuldraFight</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>' Height='250' Width='200'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>&lt;Bold&gt;e144b Fight Guards to Rescue Heir of Huldra Castle&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;You can attempt to rescue the heir by fighting through guards using a suprise attack per &lt;InlineUIContainer&gt;&lt;Button Content='r220' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.  If you succeed, see &lt;InlineUIContainer&gt;&lt;Button Content='e144c' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; for the next steps to dispose Baron Huldra.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;Each guard has a combat skill 4 and endurance 5.  Roll three die and add one for the number of guards.  Die Roll = &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>dieRoll</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.gif' Name='</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Die3Roll</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                   &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>CrossedSwords</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.gif' Name='</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>HeirRescue</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>' Height='400' Width='400'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>&lt;Bold&gt;e144c Escape with True Heir to Huldra Castle&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;After either using the an item or killing the guards, you can escape
- &lt;InlineUIContainer&gt;&lt;Button Content='r218' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
- from the hill tribe in
- &lt;InlineUIContainer&gt;&lt;Button Content='1611' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. You escape
- with the true heir who has combat skill 5 and endurance 7.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Next, take the heir to the Huldra castle.  See  &lt;InlineUIContainer&gt;&lt;Button Content='e144d' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; when you get there. Click the image to continue.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                     &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>WarriorBoy</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.gif' Name='</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>HeirEscape</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>' Height='250' Width='200'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-    </r>
-  </si>
-  <si>
     <t>&lt;Bold&gt;e144a Rescue True Heir of Huldra Castle&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;You can attempt to rescue the heir and install him as the rightful Baron at Huldra if you wish. This requires that you have:
 &lt;LineBreak/&gt;
@@ -35452,10 +35251,475 @@
   </si>
   <si>
     <r>
+      <t>&lt;Bold&gt;e144c Escape with True Heir to Huldra Castle&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;After either using the an item or killing the guards, you can escape
+ &lt;InlineUIContainer&gt;&lt;Button Content='r218' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+ from the hill tribe in
+ &lt;InlineUIContainer&gt;&lt;Button Content='1611' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. You escape
+ with the true heir who has combat skill 5 and endurance 7.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Next, take the heir to the Huldra castle.  See  &lt;InlineUIContainer&gt;&lt;Button Content='e144d' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; when you get there. Click the image to continue.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                     &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>WarriorBoy</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.gif' Name='</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>EncounterEnd</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>' Height='250' Width='200'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;Bold&gt;e144b Fight Guards to Rescue Heir of Huldra Castle&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;You can attempt to rescue the heir by fighting through guards using a suprise attack per &lt;InlineUIContainer&gt;&lt;Button Content='r220' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.  If you succeed, see &lt;InlineUIContainer&gt;&lt;Button Content='e144c' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; for the next steps to dispose Baron Huldra.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;Each guard has a combat skill 4 and endurance 5.  Roll three die and add one for the number of guards.  
+Die Roll=&lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dieRoll</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.gif' Name='</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Die3Roll</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                   &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CrossedSwords</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.gif' Name='</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>HeirRescue</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>' Height='400' Width='400'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t>e144f</t>
+  </si>
+  <si>
+    <t>e144g</t>
+  </si>
+  <si>
+    <t>e144h</t>
+  </si>
+  <si>
+    <r>
+      <t>&lt;Bold&gt;e144h Baron Hauldra Exposed as Fraud&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+After seeking an audience with Baron Hauldra with the true heir in tow, you attempted and succeeded to expose Baron Hauldra as a fraud. The heir takes the throne and returns the favor by marching his army with you back to the Northlands to help you regain your throne. You win the game due to the aide of the new Baron Huldra! Click image to continue.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                             &lt;InlineUIContainer&gt;&lt;Image Name='</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>AllyNoble</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>' Source='../../Images/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>AllyNoble</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.gif' Height='200' Width='300'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t>e144i</t>
+  </si>
+  <si>
+    <t>e144j</t>
+  </si>
+  <si>
+    <r>
+      <t>&lt;Bold&gt;e144i Baron Hauldra Sneak Attack&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+You can make a sneak attack on the Baron at night suprising his traditional six bodyguards &lt;InlineUIContainer&gt; &lt;Button Content='r220' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. Each has combat skill 6 and endurance 6. Once you kill the bodyguards, you can attack the Baron who has combat skill 6 and endurance 8. The Baron strikes first in combat. Click image to continue.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                           &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>BodyGuard</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.gif' Name='</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>HuldraGuardFight</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>' Height='350' Width='350'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;Bold&gt;e144i Baron Hauldra Sneak Attack&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Once you have killed all the Baron Huldra's bodyguards, you now come face-to-face with Huldra and must kill him to restore the heir to the throne. Click image to continue.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                      &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>BaronHuldra1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.gif' Name='</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>HuldraFight</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>' Height='350' Width='350'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;Bold&gt;e144g Baron Hauldra Banished You&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+After seeking an audience with Baron Hauldra with the true heir in tow, you attempted but failed to expose Baron Hauldra as a fraud. You are banished from the castle and may no longer seek an audience with the Baron Huldra.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>BaronHuldra1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.gif' Name='</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>HuldraExposeFails</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>' Height='250' Width='200'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;Bold&gt;e144f Baron Hauldra Exposed as a Fraud&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+After seeking an audience with Baron Hauldra with the true heir in tow, you attempt to expose Baron Hauldra as a fraud. If you roll a 10 plus, you can reveal the true heir at the audience and despose the current Baron instantly. 
+Die Roll= &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dieRoll</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.gif' Name='</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DiceRoll</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>BaronHuldra1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.gif' Name='</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>HuldraExposeAttempt</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>' Height='250' Width='200'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <t>&lt;Bold&gt;e144e Heir to Huldra Castle Killed&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;You freed the Heir to Huldra Castle, but he was killed or disappeared before you could restore him to the throne. Such a sad day. Click image to continue.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                       &lt;InlineUIContainer&gt;&lt;Image Name='</t>
+                                  &lt;InlineUIContainer&gt;&lt;Image Name='</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>BaronHuldra1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>' Source='../../Images/</t>
     </r>
     <r>
       <rPr>
@@ -35475,27 +35739,45 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>' Source='../../Images/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Nothing</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>.gif' Height='200' Width='200'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;Bold&gt;e144d Travel with Heir to Huldra Castle&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+You travel with the heir. If you reach Huldra Castle, your party and the heir have two options.&lt;LineBreak/&gt;
+1.) You can seek an audience with the current Baron
+ &lt;InlineUIContainer&gt;&lt;Button Content='r211' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
+ If you roll a 10 plus, you can reveal the true heir at the audience and despose the current Baron instantly. 
+&lt;LineBreak/&gt;
+2.)You can make a sneak attack on the Baron at night suprising his traditional six bodyguards
+ &lt;InlineUIContainer&gt; &lt;Button Content='r220' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
+ Each has combat skill 6 and endurance 6. After killing bodyguards, you can attack the Baron who has combat skill 6 and endurance 8. The Baron strikes first in combat.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+If you succeed in disposing the original Baron, the heir will take the throne and will return the favor by marching his army with you back to the Northlands to help you regain your throne. You win the game due to the aide of the new Baron Huldra! Click image to continue.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>BaronHuldra1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.gif' Height='250' Width='200'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
     </r>
   </si>
 </sst>
@@ -35960,10 +36242,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
-  <dimension ref="A1:B574"/>
+  <dimension ref="A1:B579"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A363" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B365" sqref="B365"/>
+    <sheetView tabSelected="1" topLeftCell="A371" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B364" sqref="B364"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -38857,7 +39139,7 @@
         <v>338</v>
       </c>
       <c r="B361" s="3" t="s">
-        <v>1145</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="362" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -38865,7 +39147,7 @@
         <v>339</v>
       </c>
       <c r="B362" s="3" t="s">
-        <v>1143</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="363" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -38881,1692 +39163,1732 @@
         <v>1140</v>
       </c>
       <c r="B364" s="3" t="s">
-        <v>1142</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="365" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A365" s="2" t="s">
+        <v>1143</v>
+      </c>
+      <c r="B365" s="3" t="s">
+        <v>1156</v>
+      </c>
+    </row>
+    <row r="366" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A366" s="2" t="s">
         <v>1146</v>
       </c>
-      <c r="B365" s="3" t="s">
+      <c r="B366" s="3" t="s">
+        <v>1155</v>
+      </c>
+    </row>
+    <row r="367" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A367" s="2" t="s">
         <v>1147</v>
       </c>
-    </row>
-    <row r="366" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A366" s="2" t="s">
+      <c r="B367" s="3" t="s">
+        <v>1154</v>
+      </c>
+    </row>
+    <row r="368" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A368" s="2" t="s">
+        <v>1148</v>
+      </c>
+      <c r="B368" s="3" t="s">
+        <v>1149</v>
+      </c>
+    </row>
+    <row r="369" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A369" s="2" t="s">
+        <v>1150</v>
+      </c>
+      <c r="B369" s="3" t="s">
+        <v>1152</v>
+      </c>
+    </row>
+    <row r="370" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A370" s="2" t="s">
+        <v>1151</v>
+      </c>
+      <c r="B370" s="3" t="s">
+        <v>1153</v>
+      </c>
+    </row>
+    <row r="371" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A371" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="B366" s="3" t="s">
+      <c r="B371" s="3" t="s">
         <v>677</v>
       </c>
     </row>
-    <row r="367" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A367" s="2" t="s">
+    <row r="372" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A372" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="B367" s="3" t="s">
+      <c r="B372" s="3" t="s">
         <v>1129</v>
       </c>
     </row>
-    <row r="368" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A368" s="2" t="s">
+    <row r="373" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A373" s="2" t="s">
         <v>1124</v>
       </c>
-      <c r="B368" s="3" t="s">
+      <c r="B373" s="3" t="s">
         <v>1130</v>
       </c>
     </row>
-    <row r="369" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A369" s="2" t="s">
+    <row r="374" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A374" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="B369" s="3" t="s">
+      <c r="B374" s="3" t="s">
         <v>887</v>
       </c>
     </row>
-    <row r="370" spans="1:2" ht="240" x14ac:dyDescent="0.25">
-      <c r="A370" s="2" t="s">
+    <row r="375" spans="1:2" ht="240" x14ac:dyDescent="0.25">
+      <c r="A375" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="B370" s="3" t="s">
+      <c r="B375" s="3" t="s">
         <v>888</v>
       </c>
     </row>
-    <row r="371" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A371" s="2" t="s">
+    <row r="376" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A376" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="B371" s="3" t="s">
+      <c r="B376" s="3" t="s">
         <v>651</v>
       </c>
     </row>
-    <row r="372" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A372" s="2" t="s">
+    <row r="377" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A377" s="2" t="s">
         <v>652</v>
       </c>
-      <c r="B372" s="3" t="s">
+      <c r="B377" s="3" t="s">
         <v>1091</v>
       </c>
     </row>
-    <row r="373" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A373" s="2" t="s">
+    <row r="378" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A378" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="B373" s="3" t="s">
+      <c r="B378" s="3" t="s">
         <v>617</v>
       </c>
     </row>
-    <row r="374" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A374" s="2" t="s">
+    <row r="379" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A379" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="B374" s="3" t="s">
+      <c r="B379" s="3" t="s">
         <v>618</v>
       </c>
     </row>
-    <row r="375" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A375" s="2" t="s">
+    <row r="380" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A380" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="B375" s="3" t="s">
+      <c r="B380" s="3" t="s">
         <v>1123</v>
       </c>
     </row>
-    <row r="376" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A376" s="2" t="s">
+    <row r="381" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A381" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="B376" s="3" t="s">
+      <c r="B381" s="3" t="s">
         <v>619</v>
       </c>
     </row>
-    <row r="377" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A377" s="2" t="s">
+    <row r="382" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A382" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="B377" s="3" t="s">
+      <c r="B382" s="3" t="s">
         <v>951</v>
-      </c>
-    </row>
-    <row r="378" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A378" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="B378" s="3" t="s">
-        <v>620</v>
-      </c>
-    </row>
-    <row r="379" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A379" s="2" t="s">
-        <v>591</v>
-      </c>
-      <c r="B379" s="3" t="s">
-        <v>649</v>
-      </c>
-    </row>
-    <row r="380" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A380" s="2" t="s">
-        <v>592</v>
-      </c>
-      <c r="B380" s="3" t="s">
-        <v>648</v>
-      </c>
-    </row>
-    <row r="381" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A381" s="2" t="s">
-        <v>593</v>
-      </c>
-      <c r="B381" s="3" t="s">
-        <v>647</v>
-      </c>
-    </row>
-    <row r="382" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A382" s="2" t="s">
-        <v>594</v>
-      </c>
-      <c r="B382" s="3" t="s">
-        <v>646</v>
       </c>
     </row>
     <row r="383" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A383" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="B383" s="3" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="384" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A384" s="2" t="s">
+        <v>591</v>
+      </c>
+      <c r="B384" s="3" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="385" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A385" s="2" t="s">
+        <v>592</v>
+      </c>
+      <c r="B385" s="3" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="386" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A386" s="2" t="s">
+        <v>593</v>
+      </c>
+      <c r="B386" s="3" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="387" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A387" s="2" t="s">
+        <v>594</v>
+      </c>
+      <c r="B387" s="3" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="388" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A388" s="2" t="s">
         <v>595</v>
       </c>
-      <c r="B383" s="3" t="s">
+      <c r="B388" s="3" t="s">
         <v>650</v>
       </c>
     </row>
-    <row r="384" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A384" s="2" t="s">
+    <row r="389" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A389" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="B384" s="3" t="s">
+      <c r="B389" s="3" t="s">
         <v>610</v>
-      </c>
-    </row>
-    <row r="385" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A385" s="2" t="s">
-        <v>599</v>
-      </c>
-      <c r="B385" s="3" t="s">
-        <v>602</v>
-      </c>
-    </row>
-    <row r="386" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A386" s="2" t="s">
-        <v>600</v>
-      </c>
-      <c r="B386" s="3" t="s">
-        <v>607</v>
-      </c>
-    </row>
-    <row r="387" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A387" s="2" t="s">
-        <v>601</v>
-      </c>
-      <c r="B387" s="3" t="s">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="388" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A388" s="2" t="s">
-        <v>603</v>
-      </c>
-      <c r="B388" s="3" t="s">
-        <v>609</v>
-      </c>
-    </row>
-    <row r="389" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A389" s="2" t="s">
-        <v>604</v>
-      </c>
-      <c r="B389" s="3" t="s">
-        <v>613</v>
       </c>
     </row>
     <row r="390" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A390" s="2" t="s">
+        <v>599</v>
+      </c>
+      <c r="B390" s="3" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="391" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A391" s="2" t="s">
+        <v>600</v>
+      </c>
+      <c r="B391" s="3" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="392" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A392" s="2" t="s">
+        <v>601</v>
+      </c>
+      <c r="B392" s="3" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="393" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A393" s="2" t="s">
+        <v>603</v>
+      </c>
+      <c r="B393" s="3" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="394" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A394" s="2" t="s">
+        <v>604</v>
+      </c>
+      <c r="B394" s="3" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="395" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A395" s="2" t="s">
         <v>605</v>
       </c>
-      <c r="B390" s="3" t="s">
+      <c r="B395" s="3" t="s">
         <v>608</v>
       </c>
     </row>
-    <row r="391" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A391" s="2" t="s">
+    <row r="396" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A396" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="B391" s="3" t="s">
+      <c r="B396" s="3" t="s">
         <v>588</v>
       </c>
     </row>
-    <row r="392" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A392" s="2" t="s">
+    <row r="397" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A397" s="2" t="s">
         <v>582</v>
       </c>
-      <c r="B392" s="3" t="s">
+      <c r="B397" s="3" t="s">
         <v>863</v>
       </c>
     </row>
-    <row r="393" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A393" s="2" t="s">
+    <row r="398" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A398" s="2" t="s">
         <v>583</v>
       </c>
-      <c r="B393" s="3" t="s">
+      <c r="B398" s="3" t="s">
         <v>864</v>
       </c>
     </row>
-    <row r="394" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A394" s="2" t="s">
+    <row r="399" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A399" s="2" t="s">
         <v>584</v>
       </c>
-      <c r="B394" s="3" t="s">
+      <c r="B399" s="3" t="s">
         <v>861</v>
       </c>
     </row>
-    <row r="395" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A395" s="2" t="s">
+    <row r="400" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A400" s="2" t="s">
         <v>585</v>
       </c>
-      <c r="B395" s="3" t="s">
+      <c r="B400" s="3" t="s">
         <v>862</v>
       </c>
     </row>
-    <row r="396" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A396" s="2" t="s">
+    <row r="401" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A401" s="2" t="s">
         <v>586</v>
       </c>
-      <c r="B396" s="3" t="s">
+      <c r="B401" s="3" t="s">
         <v>590</v>
       </c>
     </row>
-    <row r="397" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A397" s="2" t="s">
+    <row r="402" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A402" s="2" t="s">
         <v>587</v>
       </c>
-      <c r="B397" s="3" t="s">
+      <c r="B402" s="3" t="s">
         <v>1117</v>
       </c>
     </row>
-    <row r="398" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A398" s="2" t="s">
+    <row r="403" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A403" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="B398" s="3" t="s">
+      <c r="B403" s="3" t="s">
         <v>589</v>
       </c>
     </row>
-    <row r="399" spans="1:2" ht="195" x14ac:dyDescent="0.25">
-      <c r="A399" s="2" t="s">
+    <row r="404" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+      <c r="A404" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="B399" s="3" t="s">
+      <c r="B404" s="3" t="s">
         <v>952</v>
       </c>
     </row>
-    <row r="400" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A400" s="2" t="s">
+    <row r="405" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A405" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="B400" s="3" t="s">
+      <c r="B405" s="3" t="s">
         <v>598</v>
       </c>
     </row>
-    <row r="401" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A401" s="2" t="s">
+    <row r="406" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A406" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="B401" s="3" t="s">
+      <c r="B406" s="3" t="s">
         <v>1115</v>
       </c>
     </row>
-    <row r="402" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A402" s="2" t="s">
+    <row r="407" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A407" s="2" t="s">
         <v>635</v>
       </c>
-      <c r="B402" s="3" t="s">
+      <c r="B407" s="3" t="s">
         <v>826</v>
       </c>
     </row>
-    <row r="403" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A403" s="2" t="s">
+    <row r="408" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A408" s="2" t="s">
         <v>636</v>
       </c>
-      <c r="B403" s="3" t="s">
+      <c r="B408" s="3" t="s">
         <v>642</v>
       </c>
     </row>
-    <row r="404" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A404" s="2" t="s">
+    <row r="409" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A409" s="2" t="s">
         <v>637</v>
       </c>
-      <c r="B404" s="3" t="s">
+      <c r="B409" s="3" t="s">
         <v>641</v>
       </c>
     </row>
-    <row r="405" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A405" s="2" t="s">
+    <row r="410" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A410" s="2" t="s">
         <v>638</v>
       </c>
-      <c r="B405" s="3" t="s">
+      <c r="B410" s="3" t="s">
         <v>643</v>
       </c>
     </row>
-    <row r="406" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A406" s="2" t="s">
+    <row r="411" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A411" s="2" t="s">
         <v>639</v>
       </c>
-      <c r="B406" s="4" t="s">
+      <c r="B411" s="4" t="s">
         <v>644</v>
       </c>
     </row>
-    <row r="407" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A407" s="2" t="s">
+    <row r="412" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A412" s="2" t="s">
         <v>640</v>
       </c>
-      <c r="B407" s="3" t="s">
+      <c r="B412" s="3" t="s">
         <v>645</v>
       </c>
     </row>
-    <row r="408" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A408" s="2" t="s">
+    <row r="413" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+      <c r="A413" s="2" t="s">
         <v>1131</v>
       </c>
-      <c r="B408" s="3" t="s">
+      <c r="B413" s="3" t="s">
         <v>1138</v>
       </c>
     </row>
-    <row r="409" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A409" s="2" t="s">
+    <row r="414" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A414" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="B409" s="3" t="s">
+      <c r="B414" s="3" t="s">
         <v>1128</v>
       </c>
     </row>
-    <row r="410" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A410" s="2" t="s">
+    <row r="415" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A415" s="2" t="s">
         <v>621</v>
       </c>
-      <c r="B410" s="3" t="s">
+      <c r="B415" s="3" t="s">
         <v>627</v>
-      </c>
-    </row>
-    <row r="411" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A411" s="2" t="s">
-        <v>622</v>
-      </c>
-      <c r="B411" s="3" t="s">
-        <v>628</v>
-      </c>
-    </row>
-    <row r="412" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A412" s="2" t="s">
-        <v>623</v>
-      </c>
-      <c r="B412" s="3" t="s">
-        <v>629</v>
-      </c>
-    </row>
-    <row r="413" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A413" s="2" t="s">
-        <v>624</v>
-      </c>
-      <c r="B413" s="3" t="s">
-        <v>630</v>
-      </c>
-    </row>
-    <row r="414" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A414" s="2" t="s">
-        <v>625</v>
-      </c>
-      <c r="B414" s="3" t="s">
-        <v>633</v>
-      </c>
-    </row>
-    <row r="415" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A415" s="2" t="s">
-        <v>626</v>
-      </c>
-      <c r="B415" s="3" t="s">
-        <v>634</v>
       </c>
     </row>
     <row r="416" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A416" s="2" t="s">
+        <v>622</v>
+      </c>
+      <c r="B416" s="3" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="417" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A417" s="2" t="s">
+        <v>623</v>
+      </c>
+      <c r="B417" s="3" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="418" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A418" s="2" t="s">
+        <v>624</v>
+      </c>
+      <c r="B418" s="3" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="419" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A419" s="2" t="s">
+        <v>625</v>
+      </c>
+      <c r="B419" s="3" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="420" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A420" s="2" t="s">
+        <v>626</v>
+      </c>
+      <c r="B420" s="3" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="421" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A421" s="2" t="s">
         <v>631</v>
       </c>
-      <c r="B416" s="3" t="s">
+      <c r="B421" s="3" t="s">
         <v>632</v>
       </c>
     </row>
-    <row r="417" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A417" s="2" t="s">
+    <row r="422" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A422" s="2" t="s">
         <v>1121</v>
       </c>
-      <c r="B417" s="3" t="s">
+      <c r="B422" s="3" t="s">
         <v>1122</v>
       </c>
     </row>
-    <row r="418" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A418" s="2" t="s">
+    <row r="423" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A423" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="B418" s="3" t="s">
+      <c r="B423" s="3" t="s">
         <v>686</v>
       </c>
     </row>
-    <row r="419" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A419" s="2" t="s">
+    <row r="424" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A424" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="B419" s="3" t="s">
+      <c r="B424" s="3" t="s">
         <v>536</v>
       </c>
     </row>
-    <row r="420" spans="1:2" ht="300" x14ac:dyDescent="0.25">
-      <c r="A420" s="2" t="s">
+    <row r="425" spans="1:2" ht="300" x14ac:dyDescent="0.25">
+      <c r="A425" s="2" t="s">
         <v>532</v>
       </c>
-      <c r="B420" s="3" t="s">
+      <c r="B425" s="3" t="s">
         <v>1092</v>
       </c>
     </row>
-    <row r="421" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A421" s="2" t="s">
+    <row r="426" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A426" s="2" t="s">
         <v>533</v>
       </c>
-      <c r="B421" s="3" t="s">
+      <c r="B426" s="3" t="s">
         <v>537</v>
       </c>
     </row>
-    <row r="422" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A422" s="2" t="s">
+    <row r="427" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A427" s="2" t="s">
         <v>534</v>
       </c>
-      <c r="B422" s="3" t="s">
+      <c r="B427" s="3" t="s">
         <v>541</v>
       </c>
     </row>
-    <row r="423" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A423" s="2" t="s">
+    <row r="428" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A428" s="2" t="s">
         <v>535</v>
       </c>
-      <c r="B423" s="3" t="s">
+      <c r="B428" s="3" t="s">
         <v>542</v>
       </c>
     </row>
-    <row r="424" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A424" s="2" t="s">
+    <row r="429" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A429" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="B424" s="3" t="s">
+      <c r="B429" s="3" t="s">
         <v>843</v>
       </c>
     </row>
-    <row r="425" spans="1:2" ht="240" x14ac:dyDescent="0.25">
-      <c r="A425" s="2" t="s">
+    <row r="430" spans="1:2" ht="240" x14ac:dyDescent="0.25">
+      <c r="A430" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="B425" s="3" t="s">
+      <c r="B430" s="3" t="s">
         <v>719</v>
       </c>
     </row>
-    <row r="426" spans="1:2" ht="240" x14ac:dyDescent="0.25">
-      <c r="A426" s="2" t="s">
+    <row r="431" spans="1:2" ht="240" x14ac:dyDescent="0.25">
+      <c r="A431" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="B426" s="3" t="s">
+      <c r="B431" s="3" t="s">
         <v>1055</v>
       </c>
     </row>
-    <row r="427" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A427" s="2" t="s">
+    <row r="432" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A432" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="B427" s="3" t="s">
+      <c r="B432" s="3" t="s">
         <v>525</v>
       </c>
     </row>
-    <row r="428" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A428" s="2" t="s">
+    <row r="433" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A433" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="B428" s="3" t="s">
+      <c r="B433" s="3" t="s">
         <v>526</v>
       </c>
     </row>
-    <row r="429" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A429" s="2" t="s">
+    <row r="434" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A434" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="B429" s="3" t="s">
+      <c r="B434" s="3" t="s">
         <v>527</v>
       </c>
     </row>
-    <row r="430" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A430" s="2" t="s">
+    <row r="435" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A435" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="B430" s="3" t="s">
+      <c r="B435" s="3" t="s">
         <v>687</v>
       </c>
     </row>
-    <row r="431" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A431" s="5" t="s">
+    <row r="436" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A436" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="B431" s="3" t="s">
+      <c r="B436" s="3" t="s">
         <v>778</v>
-      </c>
-    </row>
-    <row r="432" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A432" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="B432" s="3" t="s">
-        <v>1063</v>
-      </c>
-    </row>
-    <row r="433" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A433" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="B433" s="3" t="s">
-        <v>1062</v>
-      </c>
-    </row>
-    <row r="434" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A434" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="B434" s="3" t="s">
-        <v>1061</v>
-      </c>
-    </row>
-    <row r="435" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A435" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="B435" s="3" t="s">
-        <v>1060</v>
-      </c>
-    </row>
-    <row r="436" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A436" s="2" t="s">
-        <v>331</v>
-      </c>
-      <c r="B436" s="3" t="s">
-        <v>1064</v>
       </c>
     </row>
     <row r="437" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A437" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="B437" s="3" t="s">
+        <v>1063</v>
+      </c>
+    </row>
+    <row r="438" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A438" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="B438" s="3" t="s">
+        <v>1062</v>
+      </c>
+    </row>
+    <row r="439" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A439" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="B439" s="3" t="s">
+        <v>1061</v>
+      </c>
+    </row>
+    <row r="440" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+      <c r="A440" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="B440" s="3" t="s">
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="441" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A441" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="B441" s="3" t="s">
+        <v>1064</v>
+      </c>
+    </row>
+    <row r="442" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A442" s="2" t="s">
         <v>461</v>
       </c>
-      <c r="B437" s="3" t="s">
+      <c r="B442" s="3" t="s">
         <v>463</v>
       </c>
     </row>
-    <row r="438" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A438" s="2" t="s">
+    <row r="443" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A443" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="B438" s="3" t="s">
+      <c r="B443" s="3" t="s">
         <v>881</v>
       </c>
     </row>
-    <row r="439" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A439" s="2" t="s">
+    <row r="444" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+      <c r="A444" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="B439" s="3" t="s">
+      <c r="B444" s="3" t="s">
         <v>528</v>
       </c>
     </row>
-    <row r="440" spans="1:2" ht="195" x14ac:dyDescent="0.25">
-      <c r="A440" s="2" t="s">
+    <row r="445" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+      <c r="A445" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="B440" s="3" t="s">
+      <c r="B445" s="3" t="s">
         <v>529</v>
       </c>
     </row>
-    <row r="441" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A441" s="2" t="s">
+    <row r="446" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A446" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="B441" s="3" t="s">
+      <c r="B446" s="3" t="s">
         <v>1120</v>
-      </c>
-    </row>
-    <row r="442" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A442" s="2" t="s">
-        <v>1119</v>
-      </c>
-      <c r="B442" s="3" t="s">
-        <v>1125</v>
-      </c>
-    </row>
-    <row r="443" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A443" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="B443" s="3" t="s">
-        <v>530</v>
-      </c>
-    </row>
-    <row r="444" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A444" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="B444" s="3" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="445" spans="1:2" ht="225" x14ac:dyDescent="0.25">
-      <c r="A445" s="2" t="s">
-        <v>231</v>
-      </c>
-      <c r="B445" s="3" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="446" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A446" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="B446" s="3" t="s">
-        <v>479</v>
       </c>
     </row>
     <row r="447" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A447" s="2" t="s">
+        <v>1119</v>
+      </c>
+      <c r="B447" s="3" t="s">
+        <v>1125</v>
+      </c>
+    </row>
+    <row r="448" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A448" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="B448" s="3" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="449" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A449" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="B449" s="3" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="450" spans="1:2" ht="225" x14ac:dyDescent="0.25">
+      <c r="A450" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="B450" s="3" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="451" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A451" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="B451" s="3" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="452" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A452" s="2" t="s">
         <v>444</v>
       </c>
-      <c r="B447" s="3" t="s">
+      <c r="B452" s="3" t="s">
         <v>1056</v>
       </c>
     </row>
-    <row r="448" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A448" s="2" t="s">
+    <row r="453" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A453" s="2" t="s">
         <v>446</v>
       </c>
-      <c r="B448" s="3" t="s">
+      <c r="B453" s="3" t="s">
         <v>579</v>
       </c>
     </row>
-    <row r="449" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A449" s="2" t="s">
+    <row r="454" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A454" s="2" t="s">
         <v>575</v>
       </c>
-      <c r="B449" s="3" t="s">
+      <c r="B454" s="3" t="s">
         <v>577</v>
       </c>
     </row>
-    <row r="450" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A450" s="2" t="s">
+    <row r="455" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A455" s="2" t="s">
         <v>576</v>
       </c>
-      <c r="B450" s="3" t="s">
+      <c r="B455" s="3" t="s">
         <v>775</v>
       </c>
     </row>
-    <row r="451" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A451" s="2" t="s">
+    <row r="456" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A456" s="2" t="s">
         <v>773</v>
       </c>
-      <c r="B451" s="3" t="s">
+      <c r="B456" s="3" t="s">
         <v>774</v>
       </c>
     </row>
-    <row r="452" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A452" s="2" t="s">
+    <row r="457" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A457" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="B452" s="3" t="s">
+      <c r="B457" s="3" t="s">
         <v>1051</v>
       </c>
     </row>
-    <row r="453" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A453" s="2" t="s">
+    <row r="458" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A458" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="B453" s="3" t="s">
+      <c r="B458" s="3" t="s">
         <v>1054</v>
       </c>
     </row>
-    <row r="454" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A454" s="2" t="s">
+    <row r="459" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A459" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="B454" s="3" t="s">
+      <c r="B459" s="3" t="s">
         <v>1052</v>
-      </c>
-    </row>
-    <row r="455" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A455" s="2" t="s">
-        <v>318</v>
-      </c>
-      <c r="B455" s="3" t="s">
-        <v>1053</v>
-      </c>
-    </row>
-    <row r="456" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A456" s="2" t="s">
-        <v>1012</v>
-      </c>
-      <c r="B456" s="3" t="s">
-        <v>1013</v>
-      </c>
-    </row>
-    <row r="457" spans="1:2" ht="255" x14ac:dyDescent="0.25">
-      <c r="A457" s="2" t="s">
-        <v>322</v>
-      </c>
-      <c r="B457" s="3" t="s">
-        <v>1058</v>
-      </c>
-    </row>
-    <row r="458" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A458" s="2" t="s">
-        <v>484</v>
-      </c>
-      <c r="B458" s="3" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="459" spans="1:2" ht="240" x14ac:dyDescent="0.25">
-      <c r="A459" s="2" t="s">
-        <v>483</v>
-      </c>
-      <c r="B459" s="3" t="s">
-        <v>558</v>
       </c>
     </row>
     <row r="460" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A460" s="2" t="s">
-        <v>485</v>
+        <v>318</v>
       </c>
       <c r="B460" s="3" t="s">
-        <v>1093</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="461" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A461" s="2" t="s">
-        <v>486</v>
+        <v>1012</v>
       </c>
       <c r="B461" s="3" t="s">
-        <v>1133</v>
-      </c>
-    </row>
-    <row r="462" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="462" spans="1:2" ht="255" x14ac:dyDescent="0.25">
       <c r="A462" s="2" t="s">
-        <v>487</v>
+        <v>322</v>
       </c>
       <c r="B462" s="3" t="s">
-        <v>523</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="463" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A463" s="2" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="B463" s="3" t="s">
-        <v>555</v>
-      </c>
-    </row>
-    <row r="464" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="464" spans="1:2" ht="240" x14ac:dyDescent="0.25">
       <c r="A464" s="2" t="s">
-        <v>489</v>
+        <v>483</v>
       </c>
       <c r="B464" s="3" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="465" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="465" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A465" s="2" t="s">
-        <v>552</v>
+        <v>485</v>
       </c>
       <c r="B465" s="3" t="s">
-        <v>953</v>
-      </c>
-    </row>
-    <row r="466" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+        <v>1093</v>
+      </c>
+    </row>
+    <row r="466" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A466" s="2" t="s">
-        <v>556</v>
+        <v>486</v>
       </c>
       <c r="B466" s="3" t="s">
-        <v>1107</v>
-      </c>
-    </row>
-    <row r="467" spans="1:2" ht="225" x14ac:dyDescent="0.25">
+        <v>1133</v>
+      </c>
+    </row>
+    <row r="467" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A467" s="2" t="s">
-        <v>559</v>
+        <v>487</v>
       </c>
       <c r="B467" s="3" t="s">
-        <v>720</v>
+        <v>523</v>
       </c>
     </row>
     <row r="468" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A468" s="2" t="s">
+        <v>488</v>
+      </c>
+      <c r="B468" s="3" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="469" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A469" s="2" t="s">
+        <v>489</v>
+      </c>
+      <c r="B469" s="3" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="470" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A470" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="B470" s="3" t="s">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="471" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A471" s="2" t="s">
+        <v>556</v>
+      </c>
+      <c r="B471" s="3" t="s">
+        <v>1107</v>
+      </c>
+    </row>
+    <row r="472" spans="1:2" ht="225" x14ac:dyDescent="0.25">
+      <c r="A472" s="2" t="s">
+        <v>559</v>
+      </c>
+      <c r="B472" s="3" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="473" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A473" s="2" t="s">
         <v>560</v>
       </c>
-      <c r="B468" s="3" t="s">
+      <c r="B473" s="3" t="s">
         <v>958</v>
       </c>
     </row>
-    <row r="469" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A469" s="2" t="s">
+    <row r="474" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A474" s="2" t="s">
         <v>561</v>
       </c>
-      <c r="B469" s="3" t="s">
+      <c r="B474" s="3" t="s">
         <v>569</v>
       </c>
     </row>
-    <row r="470" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A470" s="2" t="s">
+    <row r="475" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A475" s="2" t="s">
         <v>562</v>
       </c>
-      <c r="B470" s="3" t="s">
+      <c r="B475" s="3" t="s">
         <v>568</v>
       </c>
     </row>
-    <row r="471" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A471" s="2" t="s">
+    <row r="476" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A476" s="2" t="s">
         <v>563</v>
       </c>
-      <c r="B471" s="3" t="s">
+      <c r="B476" s="3" t="s">
         <v>954</v>
       </c>
     </row>
-    <row r="472" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A472" s="2" t="s">
+    <row r="477" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A477" s="2" t="s">
         <v>564</v>
       </c>
-      <c r="B472" s="3" t="s">
+      <c r="B477" s="3" t="s">
         <v>1067</v>
       </c>
     </row>
-    <row r="473" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A473" s="2" t="s">
+    <row r="478" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A478" s="2" t="s">
         <v>565</v>
       </c>
-      <c r="B473" s="3" t="s">
+      <c r="B478" s="3" t="s">
         <v>572</v>
       </c>
     </row>
-    <row r="474" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A474" s="2" t="s">
+    <row r="479" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A479" s="2" t="s">
         <v>566</v>
       </c>
-      <c r="B474" s="3" t="s">
+      <c r="B479" s="3" t="s">
         <v>955</v>
       </c>
     </row>
-    <row r="475" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A475" s="2" t="s">
+    <row r="480" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A480" s="2" t="s">
         <v>567</v>
       </c>
-      <c r="B475" s="3" t="s">
+      <c r="B480" s="3" t="s">
         <v>571</v>
-      </c>
-    </row>
-    <row r="476" spans="1:2" ht="225" x14ac:dyDescent="0.25">
-      <c r="A476" s="2" t="s">
-        <v>570</v>
-      </c>
-      <c r="B476" s="3" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="477" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A477" s="2" t="s">
-        <v>574</v>
-      </c>
-      <c r="B477" s="3" t="s">
-        <v>790</v>
-      </c>
-    </row>
-    <row r="478" spans="1:2" ht="225" x14ac:dyDescent="0.25">
-      <c r="A478" s="2" t="s">
-        <v>596</v>
-      </c>
-      <c r="B478" s="3" t="s">
-        <v>903</v>
-      </c>
-    </row>
-    <row r="479" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A479" s="2" t="s">
-        <v>614</v>
-      </c>
-      <c r="B479" s="3" t="s">
-        <v>904</v>
-      </c>
-    </row>
-    <row r="480" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A480" s="2" t="s">
-        <v>615</v>
-      </c>
-      <c r="B480" s="3" t="s">
-        <v>1126</v>
       </c>
     </row>
     <row r="481" spans="1:2" ht="225" x14ac:dyDescent="0.25">
       <c r="A481" s="2" t="s">
+        <v>570</v>
+      </c>
+      <c r="B481" s="3" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="482" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A482" s="2" t="s">
+        <v>574</v>
+      </c>
+      <c r="B482" s="3" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="483" spans="1:2" ht="225" x14ac:dyDescent="0.25">
+      <c r="A483" s="2" t="s">
+        <v>596</v>
+      </c>
+      <c r="B483" s="3" t="s">
+        <v>903</v>
+      </c>
+    </row>
+    <row r="484" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+      <c r="A484" s="2" t="s">
+        <v>614</v>
+      </c>
+      <c r="B484" s="3" t="s">
+        <v>904</v>
+      </c>
+    </row>
+    <row r="485" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+      <c r="A485" s="2" t="s">
+        <v>615</v>
+      </c>
+      <c r="B485" s="3" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="486" spans="1:2" ht="225" x14ac:dyDescent="0.25">
+      <c r="A486" s="2" t="s">
         <v>616</v>
       </c>
-      <c r="B481" s="3" t="s">
+      <c r="B486" s="3" t="s">
         <v>1127</v>
       </c>
     </row>
-    <row r="482" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A482" s="2" t="s">
+    <row r="487" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+      <c r="A487" s="2" t="s">
         <v>838</v>
       </c>
-      <c r="B482" s="3" t="s">
+      <c r="B487" s="3" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="483" spans="1:2" ht="255" x14ac:dyDescent="0.25">
-      <c r="A483" s="2" t="s">
+    <row r="488" spans="1:2" ht="255" x14ac:dyDescent="0.25">
+      <c r="A488" s="2" t="s">
         <v>653</v>
       </c>
-      <c r="B483" s="1" t="s">
+      <c r="B488" s="1" t="s">
         <v>791</v>
       </c>
     </row>
-    <row r="484" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A484" s="2" t="s">
+    <row r="489" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A489" s="2" t="s">
         <v>654</v>
       </c>
-      <c r="B484" s="1" t="s">
+      <c r="B489" s="1" t="s">
         <v>671</v>
-      </c>
-    </row>
-    <row r="485" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A485" s="2" t="s">
-        <v>655</v>
-      </c>
-      <c r="B485" s="1" t="s">
-        <v>670</v>
-      </c>
-    </row>
-    <row r="486" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A486" s="2" t="s">
-        <v>656</v>
-      </c>
-      <c r="B486" s="1" t="s">
-        <v>669</v>
-      </c>
-    </row>
-    <row r="487" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A487" s="2" t="s">
-        <v>657</v>
-      </c>
-      <c r="B487" s="1" t="s">
-        <v>668</v>
-      </c>
-    </row>
-    <row r="488" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A488" s="2" t="s">
-        <v>658</v>
-      </c>
-      <c r="B488" s="1" t="s">
-        <v>667</v>
-      </c>
-    </row>
-    <row r="489" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A489" s="2" t="s">
-        <v>659</v>
-      </c>
-      <c r="B489" s="1" t="s">
-        <v>906</v>
       </c>
     </row>
     <row r="490" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A490" s="2" t="s">
-        <v>660</v>
+        <v>655</v>
       </c>
       <c r="B490" s="1" t="s">
-        <v>666</v>
+        <v>670</v>
       </c>
     </row>
     <row r="491" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A491" s="2" t="s">
+        <v>656</v>
+      </c>
+      <c r="B491" s="1" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="492" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A492" s="2" t="s">
+        <v>657</v>
+      </c>
+      <c r="B492" s="1" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="493" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A493" s="2" t="s">
+        <v>658</v>
+      </c>
+      <c r="B493" s="1" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="494" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A494" s="2" t="s">
+        <v>659</v>
+      </c>
+      <c r="B494" s="1" t="s">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="495" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A495" s="2" t="s">
+        <v>660</v>
+      </c>
+      <c r="B495" s="1" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="496" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A496" s="2" t="s">
         <v>661</v>
       </c>
-      <c r="B491" s="1" t="s">
+      <c r="B496" s="1" t="s">
         <v>672</v>
       </c>
     </row>
-    <row r="492" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A492" s="2" t="s">
+    <row r="497" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A497" s="2" t="s">
         <v>662</v>
       </c>
-      <c r="B492" s="1" t="s">
+      <c r="B497" s="1" t="s">
         <v>674</v>
       </c>
     </row>
-    <row r="493" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A493" s="2" t="s">
+    <row r="498" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A498" s="2" t="s">
         <v>663</v>
       </c>
-      <c r="B493" s="1" t="s">
+      <c r="B498" s="1" t="s">
         <v>673</v>
       </c>
     </row>
-    <row r="494" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A494" s="2" t="s">
+    <row r="499" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A499" s="2" t="s">
         <v>664</v>
       </c>
-      <c r="B494" s="1" t="s">
+      <c r="B499" s="1" t="s">
         <v>907</v>
       </c>
     </row>
-    <row r="495" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A495" s="2" t="s">
+    <row r="500" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A500" s="2" t="s">
         <v>665</v>
       </c>
-      <c r="B495" s="1" t="s">
+      <c r="B500" s="1" t="s">
         <v>676</v>
       </c>
     </row>
-    <row r="496" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A496" s="2" t="s">
+    <row r="501" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A501" s="2" t="s">
         <v>675</v>
       </c>
-      <c r="B496" s="1" t="s">
+      <c r="B501" s="1" t="s">
         <v>680</v>
       </c>
     </row>
-    <row r="497" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A497" s="2" t="s">
+    <row r="502" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A502" s="2" t="s">
         <v>678</v>
       </c>
-      <c r="B497" s="1" t="s">
+      <c r="B502" s="1" t="s">
         <v>679</v>
       </c>
     </row>
-    <row r="498" spans="1:2" ht="255" x14ac:dyDescent="0.25">
-      <c r="A498" s="2" t="s">
+    <row r="503" spans="1:2" ht="255" x14ac:dyDescent="0.25">
+      <c r="A503" s="2" t="s">
         <v>991</v>
       </c>
-      <c r="B498" s="1" t="s">
+      <c r="B503" s="1" t="s">
         <v>999</v>
       </c>
     </row>
-    <row r="499" spans="1:2" ht="92.25" x14ac:dyDescent="0.25">
-      <c r="A499" s="2" t="s">
+    <row r="504" spans="1:2" ht="92.25" x14ac:dyDescent="0.25">
+      <c r="A504" s="2" t="s">
         <v>994</v>
       </c>
-      <c r="B499" s="1" t="s">
+      <c r="B504" s="1" t="s">
         <v>995</v>
       </c>
     </row>
-    <row r="500" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A500" s="2" t="s">
+    <row r="505" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A505" s="2" t="s">
         <v>681</v>
       </c>
-      <c r="B500" s="1" t="s">
+      <c r="B505" s="1" t="s">
         <v>908</v>
       </c>
     </row>
-    <row r="501" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A501" s="2" t="s">
+    <row r="506" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A506" s="2" t="s">
         <v>713</v>
       </c>
-      <c r="B501" s="3" t="s">
+      <c r="B506" s="3" t="s">
         <v>1049</v>
       </c>
     </row>
-    <row r="502" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A502" s="2" t="s">
+    <row r="507" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A507" s="2" t="s">
         <v>538</v>
       </c>
-      <c r="B502" s="3" t="s">
+      <c r="B507" s="3" t="s">
         <v>682</v>
       </c>
     </row>
-    <row r="503" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A503" s="2" t="s">
+    <row r="508" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A508" s="2" t="s">
         <v>539</v>
       </c>
-      <c r="B503" s="3" t="s">
+      <c r="B508" s="3" t="s">
         <v>792</v>
       </c>
     </row>
-    <row r="504" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A504" s="2" t="s">
+    <row r="509" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A509" s="2" t="s">
         <v>540</v>
       </c>
-      <c r="B504" s="3" t="s">
+      <c r="B509" s="3" t="s">
         <v>793</v>
-      </c>
-    </row>
-    <row r="505" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A505" s="2" t="s">
-        <v>267</v>
-      </c>
-      <c r="B505" s="1" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="506" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A506" s="2" t="s">
-        <v>268</v>
-      </c>
-      <c r="B506" s="1" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="507" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A507" s="2" t="s">
-        <v>269</v>
-      </c>
-      <c r="B507" s="1" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="508" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A508" s="2" t="s">
-        <v>270</v>
-      </c>
-      <c r="B508" s="1" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="509" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A509" s="2" t="s">
-        <v>271</v>
-      </c>
-      <c r="B509" s="1" t="s">
-        <v>353</v>
       </c>
     </row>
     <row r="510" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A510" s="2" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="B510" s="1" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
     </row>
     <row r="511" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A511" s="2" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="B511" s="1" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
     </row>
     <row r="512" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A512" s="2" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="B512" s="1" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
     </row>
     <row r="513" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A513" s="2" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="B513" s="1" t="s">
-        <v>1028</v>
+        <v>352</v>
       </c>
     </row>
     <row r="514" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A514" s="2" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="B514" s="1" t="s">
-        <v>1029</v>
+        <v>353</v>
       </c>
     </row>
     <row r="515" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A515" s="2" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="B515" s="1" t="s">
-        <v>1030</v>
-      </c>
-    </row>
-    <row r="516" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="516" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A516" s="2" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="B516" s="1" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="517" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="517" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A517" s="2" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="B517" s="1" t="s">
-        <v>426</v>
+        <v>356</v>
       </c>
     </row>
     <row r="518" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A518" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="B518" s="1" t="s">
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="519" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A519" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="B519" s="1" t="s">
+        <v>1029</v>
+      </c>
+    </row>
+    <row r="520" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A520" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="B520" s="1" t="s">
+        <v>1030</v>
+      </c>
+    </row>
+    <row r="521" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A521" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="B521" s="1" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="522" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A522" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="B522" s="1" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="523" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A523" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="B518" s="1" t="s">
+      <c r="B523" s="1" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="519" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A519" s="2" t="s">
+    <row r="524" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A524" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="B519" s="1" t="s">
+      <c r="B524" s="1" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="520" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A520" s="2" t="s">
+    <row r="525" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A525" s="2" t="s">
         <v>427</v>
       </c>
-      <c r="B520" s="1" t="s">
+      <c r="B525" s="1" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="521" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A521" s="2" t="s">
+    <row r="526" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A526" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="B521" s="3" t="s">
+      <c r="B526" s="3" t="s">
         <v>978</v>
       </c>
     </row>
-    <row r="522" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A522" s="2" t="s">
+    <row r="527" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A527" s="2" t="s">
         <v>473</v>
       </c>
-      <c r="B522" s="3" t="s">
+      <c r="B527" s="3" t="s">
         <v>779</v>
       </c>
     </row>
-    <row r="523" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A523" s="2" t="s">
+    <row r="528" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A528" s="2" t="s">
         <v>474</v>
       </c>
-      <c r="B523" s="1" t="s">
+      <c r="B528" s="1" t="s">
         <v>782</v>
       </c>
     </row>
-    <row r="524" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A524" s="2" t="s">
+    <row r="529" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A529" s="2" t="s">
         <v>780</v>
       </c>
-      <c r="B524" s="3" t="s">
+      <c r="B529" s="3" t="s">
         <v>781</v>
       </c>
     </row>
-    <row r="525" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A525" s="2" t="s">
+    <row r="530" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A530" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="B525" s="1" t="s">
+      <c r="B530" s="1" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="526" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A526" s="2" t="s">
+    <row r="531" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A531" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="B526" s="1" t="s">
+      <c r="B531" s="1" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="527" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A527" s="2" t="s">
+    <row r="532" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A532" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="B527" s="1" t="s">
+      <c r="B532" s="1" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="528" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A528" s="2" t="s">
+    <row r="533" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A533" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="B528" s="1" t="s">
+      <c r="B533" s="1" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="529" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A529" s="2" t="s">
+    <row r="534" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A534" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B529" s="1" t="s">
+      <c r="B534" s="1" t="s">
         <v>433</v>
       </c>
     </row>
-    <row r="530" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A530" s="2" t="s">
+    <row r="535" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A535" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="B530" s="1" t="s">
+      <c r="B535" s="1" t="s">
         <v>840</v>
       </c>
     </row>
-    <row r="531" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A531" s="2" t="s">
+    <row r="536" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A536" s="2" t="s">
         <v>286</v>
       </c>
-      <c r="B531" s="1" t="s">
+      <c r="B536" s="1" t="s">
         <v>841</v>
       </c>
     </row>
-    <row r="532" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A532" s="2" t="s">
+    <row r="537" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A537" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="B532" s="1" t="s">
+      <c r="B537" s="1" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="533" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A533" s="2" t="s">
+    <row r="538" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A538" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="B533" s="1" t="s">
+      <c r="B538" s="1" t="s">
         <v>405</v>
-      </c>
-    </row>
-    <row r="534" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A534" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="B534" s="1" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="535" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A535" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="B535" s="1" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="536" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A536" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="B536" s="1" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="537" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A537" s="2" t="s">
-        <v>292</v>
-      </c>
-      <c r="B537" s="1" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="538" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A538" s="2" t="s">
-        <v>293</v>
-      </c>
-      <c r="B538" s="1" t="s">
-        <v>416</v>
       </c>
     </row>
     <row r="539" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A539" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="B539" s="1" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="540" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A540" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="B540" s="1" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="541" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A541" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="B541" s="1" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="542" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A542" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="B542" s="1" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="543" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A543" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="B543" s="1" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="544" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A544" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="B539" s="1" t="s">
+      <c r="B544" s="1" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="540" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A540" s="2" t="s">
+    <row r="545" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A545" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="B540" s="1" t="s">
+      <c r="B545" s="1" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="541" spans="1:2" ht="240" x14ac:dyDescent="0.25">
-      <c r="A541" s="2" t="s">
+    <row r="546" spans="1:2" ht="240" x14ac:dyDescent="0.25">
+      <c r="A546" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="B541" s="1" t="s">
+      <c r="B546" s="1" t="s">
         <v>794</v>
       </c>
     </row>
-    <row r="542" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A542" s="2" t="s">
+    <row r="547" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A547" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="B542" s="1" t="s">
+      <c r="B547" s="1" t="s">
         <v>690</v>
       </c>
     </row>
-    <row r="543" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A543" s="2" t="s">
+    <row r="548" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A548" s="2" t="s">
         <v>381</v>
       </c>
-      <c r="B543" s="1" t="s">
+      <c r="B548" s="1" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="544" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A544" s="2" t="s">
+    <row r="549" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A549" s="2" t="s">
         <v>400</v>
       </c>
-      <c r="B544" s="3" t="s">
+      <c r="B549" s="3" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="545" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A545" s="2" t="s">
+    <row r="550" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A550" s="2" t="s">
         <v>401</v>
       </c>
-      <c r="B545" s="1" t="s">
+      <c r="B550" s="1" t="s">
         <v>554</v>
       </c>
     </row>
-    <row r="546" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A546" s="2" t="s">
+    <row r="551" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A551" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="B546" s="1" t="s">
+      <c r="B551" s="1" t="s">
         <v>909</v>
       </c>
     </row>
-    <row r="547" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A547" s="2" t="s">
+    <row r="552" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A552" s="2" t="s">
         <v>398</v>
       </c>
-      <c r="B547" s="1" t="s">
+      <c r="B552" s="1" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="548" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A548" s="2" t="s">
+    <row r="553" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A553" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="B548" s="1" t="s">
+      <c r="B553" s="1" t="s">
         <v>692</v>
       </c>
     </row>
-    <row r="549" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A549" s="2" t="s">
+    <row r="554" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A554" s="2" t="s">
         <v>383</v>
       </c>
-      <c r="B549" s="1" t="s">
+      <c r="B554" s="1" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="550" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A550" s="2" t="s">
+    <row r="555" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A555" s="2" t="s">
         <v>388</v>
       </c>
-      <c r="B550" s="1" t="s">
+      <c r="B555" s="1" t="s">
         <v>425</v>
-      </c>
-    </row>
-    <row r="551" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A551" s="2" t="s">
-        <v>300</v>
-      </c>
-      <c r="B551" s="1" t="s">
-        <v>858</v>
-      </c>
-    </row>
-    <row r="552" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A552" s="2" t="s">
-        <v>301</v>
-      </c>
-      <c r="B552" s="1" t="s">
-        <v>872</v>
-      </c>
-    </row>
-    <row r="553" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A553" s="2" t="s">
-        <v>302</v>
-      </c>
-      <c r="B553" s="1" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="554" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A554" s="2" t="s">
-        <v>303</v>
-      </c>
-      <c r="B554" s="1" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="555" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A555" s="2" t="s">
-        <v>397</v>
-      </c>
-      <c r="B555" s="1" t="s">
-        <v>409</v>
       </c>
     </row>
     <row r="556" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A556" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="B556" s="1" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="557" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A557" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="B557" s="1" t="s">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="558" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A558" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="B558" s="1" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="559" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A559" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="B559" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="560" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A560" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="B560" s="1" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="561" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A561" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="B556" s="1" t="s">
+      <c r="B561" s="1" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="557" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A557" s="2" t="s">
+    <row r="562" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A562" s="2" t="s">
         <v>392</v>
       </c>
-      <c r="B557" s="1" t="s">
+      <c r="B562" s="1" t="s">
         <v>724</v>
-      </c>
-    </row>
-    <row r="558" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A558" s="2" t="s">
-        <v>393</v>
-      </c>
-      <c r="B558" s="1" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="559" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A559" s="2" t="s">
-        <v>721</v>
-      </c>
-      <c r="B559" s="1" t="s">
-        <v>725</v>
-      </c>
-    </row>
-    <row r="560" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A560" s="2" t="s">
-        <v>305</v>
-      </c>
-      <c r="B560" s="1" t="s">
-        <v>691</v>
-      </c>
-    </row>
-    <row r="561" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A561" s="2" t="s">
-        <v>389</v>
-      </c>
-      <c r="B561" s="1" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="562" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A562" s="2" t="s">
-        <v>390</v>
-      </c>
-      <c r="B562" s="1" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="563" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A563" s="2" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="B563" s="1" t="s">
-        <v>497</v>
+        <v>429</v>
       </c>
     </row>
     <row r="564" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A564" s="2" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="B564" s="1" t="s">
-        <v>723</v>
+        <v>725</v>
       </c>
     </row>
     <row r="565" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A565" s="2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B565" s="1" t="s">
-        <v>693</v>
-      </c>
-    </row>
-    <row r="566" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="566" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A566" s="2" t="s">
-        <v>380</v>
+        <v>389</v>
       </c>
       <c r="B566" s="1" t="s">
-        <v>384</v>
+        <v>396</v>
       </c>
     </row>
     <row r="567" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A567" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="B567" s="1" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="568" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A568" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="B568" s="1" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="569" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A569" s="2" t="s">
+        <v>722</v>
+      </c>
+      <c r="B569" s="1" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="570" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A570" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="B570" s="1" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="571" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A571" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="B571" s="1" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="572" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A572" s="2" t="s">
         <v>385</v>
       </c>
-      <c r="B567" s="3" t="s">
+      <c r="B572" s="3" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="568" spans="1:2" ht="405" x14ac:dyDescent="0.25">
-      <c r="A568" s="2" t="s">
+    <row r="573" spans="1:2" ht="405" x14ac:dyDescent="0.25">
+      <c r="A573" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="B568" s="1" t="s">
+      <c r="B573" s="1" t="s">
         <v>983</v>
       </c>
     </row>
-    <row r="569" spans="1:2" ht="375" x14ac:dyDescent="0.25">
-      <c r="A569" s="2" t="s">
+    <row r="574" spans="1:2" ht="375" x14ac:dyDescent="0.25">
+      <c r="A574" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="B569" s="1" t="s">
+      <c r="B574" s="1" t="s">
         <v>706</v>
       </c>
     </row>
-    <row r="570" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A570" s="2" t="s">
+    <row r="575" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A575" s="2" t="s">
         <v>386</v>
       </c>
-      <c r="B570" s="1" t="s">
+      <c r="B575" s="1" t="s">
         <v>498</v>
       </c>
     </row>
-    <row r="571" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A571" s="2" t="s">
+    <row r="576" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A576" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="B571" s="1" t="s">
+      <c r="B576" s="1" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="572" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A572" s="2" t="s">
+    <row r="577" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A577" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="B572" s="3" t="s">
+      <c r="B577" s="3" t="s">
         <v>976</v>
       </c>
     </row>
-    <row r="573" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A573" s="2" t="s">
+    <row r="578" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A578" s="2" t="s">
         <v>726</v>
       </c>
-      <c r="B573" s="3" t="s">
+      <c r="B578" s="3" t="s">
         <v>727</v>
       </c>
     </row>
-    <row r="574" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A574" s="2" t="s">
+    <row r="579" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A579" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="B574" s="3" t="s">
+      <c r="B579" s="3" t="s">
         <v>1094</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:B571">
-    <sortCondition ref="A1:A571"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:B576">
+    <sortCondition ref="A1:A576"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
almost done with e144
</commit_message>
<xml_diff>
--- a/Documentation/Events.xlsx
+++ b/Documentation/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\happysulla\BarbarianPrince\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1490400D-635A-4ABA-AD4B-079ABFAFDC1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{2DB0CBAF-5F5E-4364-B673-3980B95E5B2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1158" uniqueCount="1158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1160" uniqueCount="1160">
   <si>
     <t>e001</t>
   </si>
@@ -22980,22 +22980,6 @@
 &lt;LineBreak/&gt;  &lt;InlineUIContainer&gt;&lt;Button Content='e155' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  11 plus - Audience permitted</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e211c Seeking an Audience with the Baron of Huldra Castle&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;As a daily action, you spend the day trying to gain admission to see the Baron Huldra. Roll two die and consult the list below for results: 
- &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/dieRoll.gif' Name='DiceRoll' Height='21' Width='21'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-           2 Audience permantently refused. You cannot try again&lt;LineBreak/&gt;
-  &lt;InlineUIContainer&gt;&lt;Button Content='e154' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 3 Meet Baron's Daughter&lt;LineBreak/&gt;
-  &lt;InlineUIContainer&gt;&lt;Button Content='e149' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 4 Must learn court manners&lt;LineBreak/&gt;
-  &lt;InlineUIContainer&gt;&lt;Button Content='e158' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 5 Confonted by hostile guards&lt;LineBreak/&gt;
-           6,7  Audience refused today. You may try again Tomorrow&lt;LineBreak/&gt;
-  &lt;InlineUIContainer&gt;&lt;Button Content='e153' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 8 Encounter the Master of the Household&lt;LineBreak/&gt;
-  &lt;InlineUIContainer&gt;&lt;Button Content='e148' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 9 Seneschal requires a bribe&lt;LineBreak/&gt;
-  &lt;InlineUIContainer&gt;&lt;Button Content='e150' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 10,11 Pay your respects to the Baron&lt;LineBreak/&gt;
-  &lt;InlineUIContainer&gt;&lt;Button Content='e151' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 12 Find favor in the eyes of the Baron&lt;LineBreak/&gt;
-  &lt;InlineUIContainer&gt;&lt;Button Content='e152' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 13 plus - Baron becomes your Noble ally&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;e211f Seeking an Audience with the Dwarven King&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;As a daily action, you spend the day trying to gain admission to see the Dwarven King. Roll two die and consult the list below for results: 
  &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/dieRoll.gif' Name='DiceRoll' Height='21' Width='21'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
@@ -35758,6 +35742,117 @@
 If you succeed in disposing the original Baron, the heir will take the throne and will return the favor by marching his army with you back to the Northlands to help you regain your throne. You win the game due to the aide of the new Baron Huldra! Click image to continue.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
                                 &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>BaronHuldra1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.gif' Height='250' Width='200'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e211c Seeking an Audience with the Baron of Huldra Castle&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;As a daily action, you spend the day trying to gain admission to see the Baron Huldra. Roll two die and consult the list below for results: 
+ &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/dieRoll.gif' Name='DiceRoll' Height='21' Width='21'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+           2 Audience permanently refused. You cannot try again&lt;LineBreak/&gt;
+  &lt;InlineUIContainer&gt;&lt;Button Content='e154' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 3 Meet Baron's Daughter&lt;LineBreak/&gt;
+  &lt;InlineUIContainer&gt;&lt;Button Content='e149' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 4 Must learn court manners&lt;LineBreak/&gt;
+  &lt;InlineUIContainer&gt;&lt;Button Content='e158' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 5 Confonted by hostile guards&lt;LineBreak/&gt;
+           6,7  Audience refused today. You may try again Tomorrow&lt;LineBreak/&gt;
+  &lt;InlineUIContainer&gt;&lt;Button Content='e153' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 8 Encounter the Master of the Household&lt;LineBreak/&gt;
+  &lt;InlineUIContainer&gt;&lt;Button Content='e148' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 9 Seneschal requires a bribe&lt;LineBreak/&gt;
+  &lt;InlineUIContainer&gt;&lt;Button Content='e150' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 10,11 Pay your respects to the Baron&lt;LineBreak/&gt;
+  &lt;InlineUIContainer&gt;&lt;Button Content='e151' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 12 Find favor in the eyes of the Baron&lt;LineBreak/&gt;
+  &lt;InlineUIContainer&gt;&lt;Button Content='e152' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 13 plus - Baron becomes your Noble ally&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>e211g</t>
+  </si>
+  <si>
+    <r>
+      <t>&lt;Bold&gt;e211g Seeking an Audience with Real Heir in Party&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;As a daily action, you spend the day trying to gain admission to see the Baron Huldra. You have the real Huldra's heir in your party, and you want to restore him to the throne.  Choose one option:
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='Continue' FontFamily='Courier New' FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; to seek normal audience per &lt;InlineUIContainer&gt;&lt;Button Content='e211c' FontFamily='Courier New' FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;Alternatively, you can despose Baron Huldra if 10 plus rolled. Die Roll=
+&lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dieRoll</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.gif' Name='</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DiceRoll</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>' Height='21' Width='21'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                     &lt;InlineUIContainer&gt;&lt;Image Name='</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>HuldraAudience</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>' Source='../../Images/</t>
     </r>
     <r>
       <rPr>
@@ -36242,10 +36337,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
-  <dimension ref="A1:B579"/>
+  <dimension ref="A1:B580"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A371" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B364" sqref="B364"/>
+    <sheetView tabSelected="1" topLeftCell="A487" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B488" sqref="B488"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -36259,7 +36354,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -36267,7 +36362,7 @@
         <v>254</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -36275,7 +36370,7 @@
         <v>255</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -36283,15 +36378,15 @@
         <v>256</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="390" x14ac:dyDescent="0.25">
@@ -36315,7 +36410,7 @@
         <v>22</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -36331,7 +36426,7 @@
         <v>23</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -36347,7 +36442,7 @@
         <v>3</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -36411,7 +36506,7 @@
         <v>11</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -36523,7 +36618,7 @@
         <v>21</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -36531,7 +36626,7 @@
         <v>865</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -36539,7 +36634,7 @@
         <v>866</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -36547,7 +36642,7 @@
         <v>25</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -36571,7 +36666,7 @@
         <v>26</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -36595,7 +36690,7 @@
         <v>27</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -36603,7 +36698,7 @@
         <v>28</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -36611,7 +36706,7 @@
         <v>29</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -36619,7 +36714,7 @@
         <v>30</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -36635,7 +36730,7 @@
         <v>696</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -36643,7 +36738,7 @@
         <v>31</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -36651,7 +36746,7 @@
         <v>32</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -36659,7 +36754,7 @@
         <v>33</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -36691,7 +36786,7 @@
         <v>493</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -36715,7 +36810,7 @@
         <v>264</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -36723,7 +36818,7 @@
         <v>265</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -36859,7 +36954,7 @@
         <v>42</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -36867,7 +36962,7 @@
         <v>46</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -36987,7 +37082,7 @@
         <v>777</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -37019,7 +37114,7 @@
         <v>767</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -37075,7 +37170,7 @@
         <v>66</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37123,7 +37218,7 @@
         <v>471</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -37155,7 +37250,7 @@
         <v>70</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -37243,7 +37338,7 @@
         <v>77</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
     </row>
     <row r="125" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -37256,10 +37351,10 @@
     </row>
     <row r="126" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="127" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37323,87 +37418,87 @@
         <v>81</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
     </row>
     <row r="135" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
     </row>
     <row r="136" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
     </row>
     <row r="137" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
     </row>
     <row r="138" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
     </row>
     <row r="139" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="B139" s="3" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
     </row>
     <row r="140" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
     </row>
     <row r="141" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
     </row>
     <row r="142" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
     </row>
     <row r="143" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
+        <v>937</v>
+      </c>
+      <c r="B143" s="3" t="s">
         <v>938</v>
-      </c>
-      <c r="B143" s="3" t="s">
-        <v>939</v>
       </c>
     </row>
     <row r="144" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
     </row>
     <row r="145" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37411,7 +37506,7 @@
         <v>82</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
     </row>
     <row r="146" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -37424,7 +37519,7 @@
     </row>
     <row r="147" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="B147" s="3" t="s">
         <v>547</v>
@@ -37459,7 +37554,7 @@
         <v>546</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
     </row>
     <row r="152" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37547,7 +37642,7 @@
         <v>346</v>
       </c>
       <c r="B162" s="3" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="163" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -37691,7 +37786,7 @@
         <v>831</v>
       </c>
       <c r="B180" s="3" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="181" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37699,7 +37794,7 @@
         <v>832</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="182" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37707,7 +37802,7 @@
         <v>835</v>
       </c>
       <c r="B182" s="3" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="183" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -37779,7 +37874,7 @@
         <v>103</v>
       </c>
       <c r="B191" s="3" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="192" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37787,7 +37882,7 @@
         <v>104</v>
       </c>
       <c r="B192" s="3" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
     </row>
     <row r="193" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37803,7 +37898,7 @@
         <v>683</v>
       </c>
       <c r="B194" s="3" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="195" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37819,7 +37914,7 @@
         <v>106</v>
       </c>
       <c r="B196" s="3" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
     </row>
     <row r="197" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37851,7 +37946,7 @@
         <v>108</v>
       </c>
       <c r="B200" s="3" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
     </row>
     <row r="201" spans="1:2" ht="285" x14ac:dyDescent="0.25">
@@ -37875,7 +37970,7 @@
         <v>166</v>
       </c>
       <c r="B203" s="3" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="204" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -37883,7 +37978,7 @@
         <v>167</v>
       </c>
       <c r="B204" s="3" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="205" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -37899,7 +37994,7 @@
         <v>867</v>
       </c>
       <c r="B206" s="3" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="207" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37979,7 +38074,7 @@
         <v>171</v>
       </c>
       <c r="B216" s="3" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="217" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37987,7 +38082,7 @@
         <v>113</v>
       </c>
       <c r="B217" s="3" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
     </row>
     <row r="218" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -38019,7 +38114,7 @@
         <v>115</v>
       </c>
       <c r="B221" s="3" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
     </row>
     <row r="222" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -38035,7 +38130,7 @@
         <v>116</v>
       </c>
       <c r="B223" s="3" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="224" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -38099,7 +38194,7 @@
         <v>899</v>
       </c>
       <c r="B231" s="3" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="232" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38123,7 +38218,7 @@
         <v>874</v>
       </c>
       <c r="B234" s="3" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="235" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -38131,7 +38226,7 @@
         <v>120</v>
       </c>
       <c r="B235" s="3" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
     </row>
     <row r="236" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -38139,7 +38234,7 @@
         <v>172</v>
       </c>
       <c r="B236" s="3" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
     </row>
     <row r="237" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -38147,7 +38242,7 @@
         <v>173</v>
       </c>
       <c r="B237" s="3" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
     </row>
     <row r="238" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -38155,7 +38250,7 @@
         <v>174</v>
       </c>
       <c r="B238" s="3" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
     </row>
     <row r="239" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -38195,7 +38290,7 @@
         <v>894</v>
       </c>
       <c r="B243" s="3" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="244" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -38203,7 +38298,7 @@
         <v>895</v>
       </c>
       <c r="B244" s="3" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="245" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -38216,10 +38311,10 @@
     </row>
     <row r="246" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A246" s="2" t="s">
+        <v>1110</v>
+      </c>
+      <c r="B246" s="3" t="s">
         <v>1111</v>
-      </c>
-      <c r="B246" s="3" t="s">
-        <v>1112</v>
       </c>
     </row>
     <row r="247" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -38227,15 +38322,15 @@
         <v>125</v>
       </c>
       <c r="B247" s="3" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
     </row>
     <row r="248" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A248" s="2" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="B248" s="3" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="249" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -38243,7 +38338,7 @@
         <v>126</v>
       </c>
       <c r="B249" s="3" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
     </row>
     <row r="250" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -38251,7 +38346,7 @@
         <v>127</v>
       </c>
       <c r="B250" s="3" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
     </row>
     <row r="251" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -38267,7 +38362,7 @@
         <v>129</v>
       </c>
       <c r="B252" s="3" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
     </row>
     <row r="253" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -38275,7 +38370,7 @@
         <v>130</v>
       </c>
       <c r="B253" s="3" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
     </row>
     <row r="254" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -38283,23 +38378,23 @@
         <v>131</v>
       </c>
       <c r="B254" s="3" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
     </row>
     <row r="255" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A255" s="2" t="s">
+        <v>913</v>
+      </c>
+      <c r="B255" s="3" t="s">
         <v>914</v>
-      </c>
-      <c r="B255" s="3" t="s">
-        <v>915</v>
       </c>
     </row>
     <row r="256" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A256" s="2" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="B256" s="3" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
     </row>
     <row r="257" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -38307,7 +38402,7 @@
         <v>132</v>
       </c>
       <c r="B257" s="3" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
     </row>
     <row r="258" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38315,15 +38410,15 @@
         <v>133</v>
       </c>
       <c r="B258" s="3" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="259" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A259" s="2" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="B259" s="3" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="260" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -38331,23 +38426,23 @@
         <v>134</v>
       </c>
       <c r="B260" s="3" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
     </row>
     <row r="261" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A261" s="2" t="s">
+        <v>965</v>
+      </c>
+      <c r="B261" s="3" t="s">
         <v>966</v>
-      </c>
-      <c r="B261" s="3" t="s">
-        <v>967</v>
       </c>
     </row>
     <row r="262" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A262" s="2" t="s">
+        <v>967</v>
+      </c>
+      <c r="B262" s="3" t="s">
         <v>968</v>
-      </c>
-      <c r="B262" s="3" t="s">
-        <v>969</v>
       </c>
     </row>
     <row r="263" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -38355,15 +38450,15 @@
         <v>135</v>
       </c>
       <c r="B263" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="264" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A264" s="2" t="s">
+        <v>970</v>
+      </c>
+      <c r="B264" s="3" t="s">
         <v>971</v>
-      </c>
-      <c r="B264" s="3" t="s">
-        <v>972</v>
       </c>
     </row>
     <row r="265" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38371,7 +38466,7 @@
         <v>136</v>
       </c>
       <c r="B265" s="3" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
     </row>
     <row r="266" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -38395,7 +38490,7 @@
         <v>233</v>
       </c>
       <c r="B268" s="3" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="269" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -38411,7 +38506,7 @@
         <v>234</v>
       </c>
       <c r="B270" s="3" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="271" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -38419,7 +38514,7 @@
         <v>235</v>
       </c>
       <c r="B271" s="3" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="272" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -38459,7 +38554,7 @@
         <v>140</v>
       </c>
       <c r="B276" s="3" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="277" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -38467,7 +38562,7 @@
         <v>236</v>
       </c>
       <c r="B277" s="3" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="278" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -38475,7 +38570,7 @@
         <v>237</v>
       </c>
       <c r="B278" s="3" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="279" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -38483,7 +38578,7 @@
         <v>238</v>
       </c>
       <c r="B279" s="3" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="280" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -38491,7 +38586,7 @@
         <v>141</v>
       </c>
       <c r="B280" s="3" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="281" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -38499,7 +38594,7 @@
         <v>142</v>
       </c>
       <c r="B281" s="3" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="282" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38507,7 +38602,7 @@
         <v>143</v>
       </c>
       <c r="B282" s="3" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="283" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -38515,7 +38610,7 @@
         <v>144</v>
       </c>
       <c r="B283" s="3" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="284" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -38523,7 +38618,7 @@
         <v>242</v>
       </c>
       <c r="B284" s="3" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="285" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -38531,7 +38626,7 @@
         <v>145</v>
       </c>
       <c r="B285" s="3" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="286" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -38539,7 +38634,7 @@
         <v>146</v>
       </c>
       <c r="B286" s="3" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="287" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -38547,7 +38642,7 @@
         <v>147</v>
       </c>
       <c r="B287" s="3" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="288" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38555,7 +38650,7 @@
         <v>148</v>
       </c>
       <c r="B288" s="3" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="289" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -38563,31 +38658,31 @@
         <v>149</v>
       </c>
       <c r="B289" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="290" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A290" s="2" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="B290" s="3" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="291" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A291" s="2" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="B291" s="3" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="292" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A292" s="2" t="s">
+        <v>1035</v>
+      </c>
+      <c r="B292" s="3" t="s">
         <v>1036</v>
-      </c>
-      <c r="B292" s="3" t="s">
-        <v>1037</v>
       </c>
     </row>
     <row r="293" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -38595,15 +38690,15 @@
         <v>150</v>
       </c>
       <c r="B293" s="3" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="294" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A294" s="2" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="B294" s="3" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="295" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -38627,7 +38722,7 @@
         <v>244</v>
       </c>
       <c r="B297" s="3" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="298" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -38651,7 +38746,7 @@
         <v>153</v>
       </c>
       <c r="B300" s="3" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="301" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -38731,7 +38826,7 @@
         <v>160</v>
       </c>
       <c r="B310" s="3" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
     </row>
     <row r="311" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -38739,7 +38834,7 @@
         <v>161</v>
       </c>
       <c r="B311" s="3" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
     </row>
     <row r="312" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -38747,31 +38842,31 @@
         <v>162</v>
       </c>
       <c r="B312" s="3" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="313" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A313" s="2" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="B313" s="3" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="314" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A314" s="2" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="B314" s="3" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="315" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A315" s="2" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="B315" s="3" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="316" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -38779,7 +38874,7 @@
         <v>163</v>
       </c>
       <c r="B316" s="3" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="317" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -38787,7 +38882,7 @@
         <v>164</v>
       </c>
       <c r="B317" s="3" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
     </row>
     <row r="318" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -38795,7 +38890,7 @@
         <v>175</v>
       </c>
       <c r="B318" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="319" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -38803,7 +38898,7 @@
         <v>176</v>
       </c>
       <c r="B319" s="3" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
     </row>
     <row r="320" spans="1:2" ht="390" x14ac:dyDescent="0.25">
@@ -38811,7 +38906,7 @@
         <v>177</v>
       </c>
       <c r="B320" s="3" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
     </row>
     <row r="321" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -38819,7 +38914,7 @@
         <v>516</v>
       </c>
       <c r="B321" s="3" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
     </row>
     <row r="322" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -38827,7 +38922,7 @@
         <v>517</v>
       </c>
       <c r="B322" s="3" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
     </row>
     <row r="323" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -38835,7 +38930,7 @@
         <v>518</v>
       </c>
       <c r="B323" s="3" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
     </row>
     <row r="324" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -38843,7 +38938,7 @@
         <v>519</v>
       </c>
       <c r="B324" s="3" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="325" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -38851,7 +38946,7 @@
         <v>520</v>
       </c>
       <c r="B325" s="3" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
     </row>
     <row r="326" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -38859,15 +38954,15 @@
         <v>521</v>
       </c>
       <c r="B326" s="3" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="327" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A327" s="2" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="B327" s="3" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="328" spans="1:2" ht="390" x14ac:dyDescent="0.25">
@@ -38875,7 +38970,7 @@
         <v>178</v>
       </c>
       <c r="B328" s="3" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
     </row>
     <row r="329" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -38883,7 +38978,7 @@
         <v>491</v>
       </c>
       <c r="B329" s="3" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
     </row>
     <row r="330" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -38891,7 +38986,7 @@
         <v>543</v>
       </c>
       <c r="B330" s="3" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="331" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -38899,7 +38994,7 @@
         <v>544</v>
       </c>
       <c r="B331" s="3" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
     </row>
     <row r="332" spans="1:2" ht="315" x14ac:dyDescent="0.25">
@@ -38939,7 +39034,7 @@
         <v>252</v>
       </c>
       <c r="B336" s="3" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="337" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -38963,7 +39058,7 @@
         <v>822</v>
       </c>
       <c r="B339" s="3" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
     </row>
     <row r="340" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -38971,7 +39066,7 @@
         <v>180</v>
       </c>
       <c r="B340" s="3" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
     </row>
     <row r="341" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38995,15 +39090,15 @@
         <v>182</v>
       </c>
       <c r="B343" s="3" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="344" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A344" s="2" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
       <c r="B344" s="3" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
     </row>
     <row r="345" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39011,7 +39106,7 @@
         <v>183</v>
       </c>
       <c r="B345" s="3" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="346" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -39019,7 +39114,7 @@
         <v>184</v>
       </c>
       <c r="B346" s="3" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="347" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -39035,7 +39130,7 @@
         <v>185</v>
       </c>
       <c r="B348" s="3" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="349" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -39059,7 +39154,7 @@
         <v>466</v>
       </c>
       <c r="B351" s="3" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="352" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -39131,7 +39226,7 @@
         <v>193</v>
       </c>
       <c r="B360" s="3" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="361" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -39139,7 +39234,7 @@
         <v>338</v>
       </c>
       <c r="B361" s="3" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="362" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -39147,71 +39242,71 @@
         <v>339</v>
       </c>
       <c r="B362" s="3" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="363" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A363" s="2" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="B363" s="3" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="364" spans="1:2" ht="225" x14ac:dyDescent="0.25">
       <c r="A364" s="2" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="B364" s="3" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="365" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A365" s="2" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="B365" s="3" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="366" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A366" s="2" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="B366" s="3" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="367" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A367" s="2" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="B367" s="3" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="368" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A368" s="2" t="s">
+        <v>1147</v>
+      </c>
+      <c r="B368" s="3" t="s">
         <v>1148</v>
-      </c>
-      <c r="B368" s="3" t="s">
-        <v>1149</v>
       </c>
     </row>
     <row r="369" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A369" s="2" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="B369" s="3" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="370" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A370" s="2" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="B370" s="3" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="371" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -39227,15 +39322,15 @@
         <v>195</v>
       </c>
       <c r="B372" s="3" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="373" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A373" s="2" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="B373" s="3" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="374" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -39267,7 +39362,7 @@
         <v>652</v>
       </c>
       <c r="B377" s="3" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="378" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39291,7 +39386,7 @@
         <v>200</v>
       </c>
       <c r="B380" s="3" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="381" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -39307,7 +39402,7 @@
         <v>202</v>
       </c>
       <c r="B382" s="3" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
     </row>
     <row r="383" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -39467,7 +39562,7 @@
         <v>587</v>
       </c>
       <c r="B402" s="3" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="403" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39483,7 +39578,7 @@
         <v>207</v>
       </c>
       <c r="B404" s="3" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
     </row>
     <row r="405" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -39499,7 +39594,7 @@
         <v>209</v>
       </c>
       <c r="B406" s="3" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="407" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -39552,10 +39647,10 @@
     </row>
     <row r="413" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A413" s="2" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
       <c r="B413" s="3" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="414" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -39563,7 +39658,7 @@
         <v>210</v>
       </c>
       <c r="B414" s="3" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="415" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -39624,10 +39719,10 @@
     </row>
     <row r="422" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A422" s="2" t="s">
+        <v>1120</v>
+      </c>
+      <c r="B422" s="3" t="s">
         <v>1121</v>
-      </c>
-      <c r="B422" s="3" t="s">
-        <v>1122</v>
       </c>
     </row>
     <row r="423" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -39651,7 +39746,7 @@
         <v>532</v>
       </c>
       <c r="B425" s="3" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="426" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -39699,7 +39794,7 @@
         <v>215</v>
       </c>
       <c r="B431" s="3" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="432" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39747,7 +39842,7 @@
         <v>221</v>
       </c>
       <c r="B437" s="3" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="438" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -39755,7 +39850,7 @@
         <v>222</v>
       </c>
       <c r="B438" s="3" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="439" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -39763,7 +39858,7 @@
         <v>223</v>
       </c>
       <c r="B439" s="3" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="440" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -39771,7 +39866,7 @@
         <v>224</v>
       </c>
       <c r="B440" s="3" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="441" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -39779,7 +39874,7 @@
         <v>331</v>
       </c>
       <c r="B441" s="3" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="442" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -39819,15 +39914,15 @@
         <v>228</v>
       </c>
       <c r="B446" s="3" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="447" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A447" s="2" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="B447" s="3" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="448" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -39867,7 +39962,7 @@
         <v>444</v>
       </c>
       <c r="B452" s="3" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="453" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -39907,7 +40002,7 @@
         <v>319</v>
       </c>
       <c r="B457" s="3" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="458" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -39915,7 +40010,7 @@
         <v>320</v>
       </c>
       <c r="B458" s="3" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="459" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -39923,7 +40018,7 @@
         <v>321</v>
       </c>
       <c r="B459" s="3" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="460" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -39931,15 +40026,15 @@
         <v>318</v>
       </c>
       <c r="B460" s="3" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="461" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A461" s="2" t="s">
+        <v>1011</v>
+      </c>
+      <c r="B461" s="3" t="s">
         <v>1012</v>
-      </c>
-      <c r="B461" s="3" t="s">
-        <v>1013</v>
       </c>
     </row>
     <row r="462" spans="1:2" ht="255" x14ac:dyDescent="0.25">
@@ -39947,7 +40042,7 @@
         <v>322</v>
       </c>
       <c r="B462" s="3" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="463" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39971,7 +40066,7 @@
         <v>485</v>
       </c>
       <c r="B465" s="3" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="466" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -39979,7 +40074,7 @@
         <v>486</v>
       </c>
       <c r="B466" s="3" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="467" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -40011,7 +40106,7 @@
         <v>552</v>
       </c>
       <c r="B470" s="3" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
     </row>
     <row r="471" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -40019,7 +40114,7 @@
         <v>556</v>
       </c>
       <c r="B471" s="3" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="472" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -40035,7 +40130,7 @@
         <v>560</v>
       </c>
       <c r="B473" s="3" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
     </row>
     <row r="474" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -40059,7 +40154,7 @@
         <v>563</v>
       </c>
       <c r="B476" s="3" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
     </row>
     <row r="477" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -40067,7 +40162,7 @@
         <v>564</v>
       </c>
       <c r="B477" s="3" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="478" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -40083,7 +40178,7 @@
         <v>566</v>
       </c>
       <c r="B479" s="3" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
     </row>
     <row r="480" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -40123,7 +40218,7 @@
         <v>614</v>
       </c>
       <c r="B484" s="3" t="s">
-        <v>904</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="485" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -40131,7 +40226,7 @@
         <v>615</v>
       </c>
       <c r="B485" s="3" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="486" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -40139,7 +40234,7 @@
         <v>616</v>
       </c>
       <c r="B486" s="3" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="487" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -40147,748 +40242,756 @@
         <v>838</v>
       </c>
       <c r="B487" s="3" t="s">
-        <v>905</v>
-      </c>
-    </row>
-    <row r="488" spans="1:2" ht="255" x14ac:dyDescent="0.25">
+        <v>904</v>
+      </c>
+    </row>
+    <row r="488" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A488" s="2" t="s">
+        <v>1158</v>
+      </c>
+      <c r="B488" s="3" t="s">
+        <v>1159</v>
+      </c>
+    </row>
+    <row r="489" spans="1:2" ht="255" x14ac:dyDescent="0.25">
+      <c r="A489" s="2" t="s">
         <v>653</v>
       </c>
-      <c r="B488" s="1" t="s">
+      <c r="B489" s="1" t="s">
         <v>791</v>
       </c>
     </row>
-    <row r="489" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A489" s="2" t="s">
+    <row r="490" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A490" s="2" t="s">
         <v>654</v>
       </c>
-      <c r="B489" s="1" t="s">
+      <c r="B490" s="1" t="s">
         <v>671</v>
       </c>
     </row>
-    <row r="490" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A490" s="2" t="s">
+    <row r="491" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A491" s="2" t="s">
         <v>655</v>
       </c>
-      <c r="B490" s="1" t="s">
+      <c r="B491" s="1" t="s">
         <v>670</v>
-      </c>
-    </row>
-    <row r="491" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A491" s="2" t="s">
-        <v>656</v>
-      </c>
-      <c r="B491" s="1" t="s">
-        <v>669</v>
       </c>
     </row>
     <row r="492" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A492" s="2" t="s">
+        <v>656</v>
+      </c>
+      <c r="B492" s="1" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="493" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A493" s="2" t="s">
         <v>657</v>
       </c>
-      <c r="B492" s="1" t="s">
+      <c r="B493" s="1" t="s">
         <v>668</v>
       </c>
     </row>
-    <row r="493" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A493" s="2" t="s">
+    <row r="494" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A494" s="2" t="s">
         <v>658</v>
       </c>
-      <c r="B493" s="1" t="s">
+      <c r="B494" s="1" t="s">
         <v>667</v>
-      </c>
-    </row>
-    <row r="494" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A494" s="2" t="s">
-        <v>659</v>
-      </c>
-      <c r="B494" s="1" t="s">
-        <v>906</v>
       </c>
     </row>
     <row r="495" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A495" s="2" t="s">
+        <v>659</v>
+      </c>
+      <c r="B495" s="1" t="s">
+        <v>905</v>
+      </c>
+    </row>
+    <row r="496" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A496" s="2" t="s">
         <v>660</v>
       </c>
-      <c r="B495" s="1" t="s">
+      <c r="B496" s="1" t="s">
         <v>666</v>
       </c>
     </row>
-    <row r="496" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A496" s="2" t="s">
+    <row r="497" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A497" s="2" t="s">
         <v>661</v>
       </c>
-      <c r="B496" s="1" t="s">
+      <c r="B497" s="1" t="s">
         <v>672</v>
       </c>
     </row>
-    <row r="497" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A497" s="2" t="s">
+    <row r="498" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A498" s="2" t="s">
         <v>662</v>
       </c>
-      <c r="B497" s="1" t="s">
+      <c r="B498" s="1" t="s">
         <v>674</v>
       </c>
     </row>
-    <row r="498" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A498" s="2" t="s">
+    <row r="499" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A499" s="2" t="s">
         <v>663</v>
       </c>
-      <c r="B498" s="1" t="s">
+      <c r="B499" s="1" t="s">
         <v>673</v>
       </c>
     </row>
-    <row r="499" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A499" s="2" t="s">
+    <row r="500" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A500" s="2" t="s">
         <v>664</v>
       </c>
-      <c r="B499" s="1" t="s">
-        <v>907</v>
-      </c>
-    </row>
-    <row r="500" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A500" s="2" t="s">
+      <c r="B500" s="1" t="s">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="501" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A501" s="2" t="s">
         <v>665</v>
       </c>
-      <c r="B500" s="1" t="s">
+      <c r="B501" s="1" t="s">
         <v>676</v>
-      </c>
-    </row>
-    <row r="501" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A501" s="2" t="s">
-        <v>675</v>
-      </c>
-      <c r="B501" s="1" t="s">
-        <v>680</v>
       </c>
     </row>
     <row r="502" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A502" s="2" t="s">
+        <v>675</v>
+      </c>
+      <c r="B502" s="1" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="503" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A503" s="2" t="s">
         <v>678</v>
       </c>
-      <c r="B502" s="1" t="s">
+      <c r="B503" s="1" t="s">
         <v>679</v>
       </c>
     </row>
-    <row r="503" spans="1:2" ht="255" x14ac:dyDescent="0.25">
-      <c r="A503" s="2" t="s">
-        <v>991</v>
-      </c>
-      <c r="B503" s="1" t="s">
-        <v>999</v>
-      </c>
-    </row>
-    <row r="504" spans="1:2" ht="92.25" x14ac:dyDescent="0.25">
+    <row r="504" spans="1:2" ht="255" x14ac:dyDescent="0.25">
       <c r="A504" s="2" t="s">
+        <v>990</v>
+      </c>
+      <c r="B504" s="1" t="s">
+        <v>998</v>
+      </c>
+    </row>
+    <row r="505" spans="1:2" ht="92.25" x14ac:dyDescent="0.25">
+      <c r="A505" s="2" t="s">
+        <v>993</v>
+      </c>
+      <c r="B505" s="1" t="s">
         <v>994</v>
       </c>
-      <c r="B504" s="1" t="s">
-        <v>995</v>
-      </c>
-    </row>
-    <row r="505" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A505" s="2" t="s">
+    </row>
+    <row r="506" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A506" s="2" t="s">
         <v>681</v>
       </c>
-      <c r="B505" s="1" t="s">
-        <v>908</v>
-      </c>
-    </row>
-    <row r="506" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A506" s="2" t="s">
+      <c r="B506" s="1" t="s">
+        <v>907</v>
+      </c>
+    </row>
+    <row r="507" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A507" s="2" t="s">
         <v>713</v>
       </c>
-      <c r="B506" s="3" t="s">
-        <v>1049</v>
-      </c>
-    </row>
-    <row r="507" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A507" s="2" t="s">
+      <c r="B507" s="3" t="s">
+        <v>1048</v>
+      </c>
+    </row>
+    <row r="508" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A508" s="2" t="s">
         <v>538</v>
       </c>
-      <c r="B507" s="3" t="s">
+      <c r="B508" s="3" t="s">
         <v>682</v>
       </c>
     </row>
-    <row r="508" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A508" s="2" t="s">
+    <row r="509" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A509" s="2" t="s">
         <v>539</v>
       </c>
-      <c r="B508" s="3" t="s">
+      <c r="B509" s="3" t="s">
         <v>792</v>
       </c>
     </row>
-    <row r="509" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A509" s="2" t="s">
+    <row r="510" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A510" s="2" t="s">
         <v>540</v>
       </c>
-      <c r="B509" s="3" t="s">
+      <c r="B510" s="3" t="s">
         <v>793</v>
-      </c>
-    </row>
-    <row r="510" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A510" s="2" t="s">
-        <v>267</v>
-      </c>
-      <c r="B510" s="1" t="s">
-        <v>349</v>
       </c>
     </row>
     <row r="511" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A511" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B511" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="512" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A512" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B512" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="513" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A513" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B513" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="514" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A514" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B514" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="515" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A515" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B515" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="516" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A516" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B516" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="517" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A517" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B517" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="518" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A518" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B518" s="1" t="s">
-        <v>1028</v>
+        <v>356</v>
       </c>
     </row>
     <row r="519" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A519" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B519" s="1" t="s">
-        <v>1029</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="520" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A520" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="B520" s="1" t="s">
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="521" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A521" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="B520" s="1" t="s">
-        <v>1030</v>
-      </c>
-    </row>
-    <row r="521" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A521" s="2" t="s">
-        <v>278</v>
-      </c>
       <c r="B521" s="1" t="s">
-        <v>312</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="522" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A522" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="B522" s="1" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="523" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A523" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="B522" s="1" t="s">
+      <c r="B523" s="1" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="523" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A523" s="2" t="s">
+    <row r="524" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A524" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="B523" s="1" t="s">
+      <c r="B524" s="1" t="s">
         <v>316</v>
-      </c>
-    </row>
-    <row r="524" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A524" s="2" t="s">
-        <v>315</v>
-      </c>
-      <c r="B524" s="1" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="525" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A525" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="B525" s="1" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="526" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A526" s="2" t="s">
         <v>427</v>
       </c>
-      <c r="B525" s="1" t="s">
+      <c r="B526" s="1" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="526" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A526" s="2" t="s">
+    <row r="527" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A527" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="B526" s="3" t="s">
-        <v>978</v>
-      </c>
-    </row>
-    <row r="527" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A527" s="2" t="s">
+      <c r="B527" s="3" t="s">
+        <v>977</v>
+      </c>
+    </row>
+    <row r="528" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A528" s="2" t="s">
         <v>473</v>
       </c>
-      <c r="B527" s="3" t="s">
+      <c r="B528" s="3" t="s">
         <v>779</v>
       </c>
     </row>
-    <row r="528" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A528" s="2" t="s">
+    <row r="529" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A529" s="2" t="s">
         <v>474</v>
       </c>
-      <c r="B528" s="1" t="s">
+      <c r="B529" s="1" t="s">
         <v>782</v>
       </c>
     </row>
-    <row r="529" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A529" s="2" t="s">
+    <row r="530" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A530" s="2" t="s">
         <v>780</v>
       </c>
-      <c r="B529" s="3" t="s">
+      <c r="B530" s="3" t="s">
         <v>781</v>
-      </c>
-    </row>
-    <row r="530" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A530" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="B530" s="1" t="s">
-        <v>432</v>
       </c>
     </row>
     <row r="531" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A531" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="B531" s="1" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="532" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A532" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="B531" s="1" t="s">
+      <c r="B532" s="1" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="532" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A532" s="2" t="s">
+    <row r="533" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A533" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="B532" s="1" t="s">
+      <c r="B533" s="1" t="s">
         <v>310</v>
-      </c>
-    </row>
-    <row r="533" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A533" s="2" t="s">
-        <v>283</v>
-      </c>
-      <c r="B533" s="1" t="s">
-        <v>430</v>
       </c>
     </row>
     <row r="534" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A534" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="B534" s="1" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="535" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A535" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B534" s="1" t="s">
+      <c r="B535" s="1" t="s">
         <v>433</v>
-      </c>
-    </row>
-    <row r="535" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A535" s="2" t="s">
-        <v>285</v>
-      </c>
-      <c r="B535" s="1" t="s">
-        <v>840</v>
       </c>
     </row>
     <row r="536" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A536" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="B536" s="1" t="s">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="537" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A537" s="2" t="s">
         <v>286</v>
       </c>
-      <c r="B536" s="1" t="s">
+      <c r="B537" s="1" t="s">
         <v>841</v>
-      </c>
-    </row>
-    <row r="537" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A537" s="2" t="s">
-        <v>287</v>
-      </c>
-      <c r="B537" s="1" t="s">
-        <v>406</v>
       </c>
     </row>
     <row r="538" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A538" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B538" s="1" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
     </row>
     <row r="539" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A539" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B539" s="1" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
     </row>
     <row r="540" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A540" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="B540" s="1" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="541" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A541" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="B540" s="1" t="s">
+      <c r="B541" s="1" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="541" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A541" s="2" t="s">
+    <row r="542" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A542" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B541" s="1" t="s">
+      <c r="B542" s="1" t="s">
         <v>314</v>
-      </c>
-    </row>
-    <row r="542" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A542" s="2" t="s">
-        <v>292</v>
-      </c>
-      <c r="B542" s="1" t="s">
-        <v>413</v>
       </c>
     </row>
     <row r="543" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A543" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="B543" s="1" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="544" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A544" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="B543" s="1" t="s">
+      <c r="B544" s="1" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="544" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A544" s="2" t="s">
+    <row r="545" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A545" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="B544" s="1" t="s">
+      <c r="B545" s="1" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="545" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A545" s="2" t="s">
+    <row r="546" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A546" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="B545" s="1" t="s">
+      <c r="B546" s="1" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="546" spans="1:2" ht="240" x14ac:dyDescent="0.25">
-      <c r="A546" s="2" t="s">
+    <row r="547" spans="1:2" ht="240" x14ac:dyDescent="0.25">
+      <c r="A547" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="B546" s="1" t="s">
+      <c r="B547" s="1" t="s">
         <v>794</v>
       </c>
     </row>
-    <row r="547" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A547" s="2" t="s">
+    <row r="548" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A548" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="B547" s="1" t="s">
+      <c r="B548" s="1" t="s">
         <v>690</v>
       </c>
     </row>
-    <row r="548" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A548" s="2" t="s">
+    <row r="549" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A549" s="2" t="s">
         <v>381</v>
       </c>
-      <c r="B548" s="1" t="s">
+      <c r="B549" s="1" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="549" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A549" s="2" t="s">
+    <row r="550" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A550" s="2" t="s">
         <v>400</v>
       </c>
-      <c r="B549" s="3" t="s">
+      <c r="B550" s="3" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="550" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A550" s="2" t="s">
+    <row r="551" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A551" s="2" t="s">
         <v>401</v>
       </c>
-      <c r="B550" s="1" t="s">
+      <c r="B551" s="1" t="s">
         <v>554</v>
       </c>
     </row>
-    <row r="551" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A551" s="2" t="s">
+    <row r="552" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A552" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="B551" s="1" t="s">
-        <v>909</v>
-      </c>
-    </row>
-    <row r="552" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A552" s="2" t="s">
+      <c r="B552" s="1" t="s">
+        <v>908</v>
+      </c>
+    </row>
+    <row r="553" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A553" s="2" t="s">
         <v>398</v>
       </c>
-      <c r="B552" s="1" t="s">
+      <c r="B553" s="1" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="553" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A553" s="2" t="s">
+    <row r="554" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A554" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="B553" s="1" t="s">
+      <c r="B554" s="1" t="s">
         <v>692</v>
       </c>
     </row>
-    <row r="554" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A554" s="2" t="s">
+    <row r="555" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A555" s="2" t="s">
         <v>383</v>
       </c>
-      <c r="B554" s="1" t="s">
+      <c r="B555" s="1" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="555" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A555" s="2" t="s">
+    <row r="556" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A556" s="2" t="s">
         <v>388</v>
       </c>
-      <c r="B555" s="1" t="s">
+      <c r="B556" s="1" t="s">
         <v>425</v>
-      </c>
-    </row>
-    <row r="556" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A556" s="2" t="s">
-        <v>300</v>
-      </c>
-      <c r="B556" s="1" t="s">
-        <v>858</v>
       </c>
     </row>
     <row r="557" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A557" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="B557" s="1" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="558" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A558" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="B557" s="1" t="s">
+      <c r="B558" s="1" t="s">
         <v>872</v>
       </c>
     </row>
-    <row r="558" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A558" s="2" t="s">
+    <row r="559" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A559" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="B558" s="1" t="s">
+      <c r="B559" s="1" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="559" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A559" s="2" t="s">
+    <row r="560" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A560" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="B559" s="1" t="s">
+      <c r="B560" s="1" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="560" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A560" s="2" t="s">
+    <row r="561" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A561" s="2" t="s">
         <v>397</v>
       </c>
-      <c r="B560" s="1" t="s">
+      <c r="B561" s="1" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="561" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A561" s="2" t="s">
+    <row r="562" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A562" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="B561" s="1" t="s">
+      <c r="B562" s="1" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="562" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A562" s="2" t="s">
+    <row r="563" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A563" s="2" t="s">
         <v>392</v>
       </c>
-      <c r="B562" s="1" t="s">
+      <c r="B563" s="1" t="s">
         <v>724</v>
       </c>
     </row>
-    <row r="563" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A563" s="2" t="s">
+    <row r="564" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A564" s="2" t="s">
         <v>393</v>
       </c>
-      <c r="B563" s="1" t="s">
+      <c r="B564" s="1" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="564" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A564" s="2" t="s">
+    <row r="565" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A565" s="2" t="s">
         <v>721</v>
       </c>
-      <c r="B564" s="1" t="s">
+      <c r="B565" s="1" t="s">
         <v>725</v>
       </c>
     </row>
-    <row r="565" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A565" s="2" t="s">
+    <row r="566" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A566" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="B565" s="1" t="s">
+      <c r="B566" s="1" t="s">
         <v>691</v>
       </c>
     </row>
-    <row r="566" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A566" s="2" t="s">
+    <row r="567" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A567" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="B566" s="1" t="s">
+      <c r="B567" s="1" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="567" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A567" s="2" t="s">
+    <row r="568" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A568" s="2" t="s">
         <v>390</v>
       </c>
-      <c r="B567" s="1" t="s">
+      <c r="B568" s="1" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="568" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A568" s="2" t="s">
+    <row r="569" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A569" s="2" t="s">
         <v>391</v>
       </c>
-      <c r="B568" s="1" t="s">
+      <c r="B569" s="1" t="s">
         <v>497</v>
       </c>
     </row>
-    <row r="569" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A569" s="2" t="s">
+    <row r="570" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A570" s="2" t="s">
         <v>722</v>
       </c>
-      <c r="B569" s="1" t="s">
+      <c r="B570" s="1" t="s">
         <v>723</v>
-      </c>
-    </row>
-    <row r="570" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A570" s="2" t="s">
-        <v>306</v>
-      </c>
-      <c r="B570" s="1" t="s">
-        <v>693</v>
       </c>
     </row>
     <row r="571" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A571" s="2" t="s">
-        <v>380</v>
+        <v>306</v>
       </c>
       <c r="B571" s="1" t="s">
-        <v>384</v>
+        <v>693</v>
       </c>
     </row>
     <row r="572" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A572" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="B572" s="1" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="573" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A573" s="2" t="s">
         <v>385</v>
       </c>
-      <c r="B572" s="3" t="s">
+      <c r="B573" s="3" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="573" spans="1:2" ht="405" x14ac:dyDescent="0.25">
-      <c r="A573" s="2" t="s">
+    <row r="574" spans="1:2" ht="405" x14ac:dyDescent="0.25">
+      <c r="A574" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="B573" s="1" t="s">
-        <v>983</v>
-      </c>
-    </row>
-    <row r="574" spans="1:2" ht="375" x14ac:dyDescent="0.25">
-      <c r="A574" s="2" t="s">
+      <c r="B574" s="1" t="s">
+        <v>982</v>
+      </c>
+    </row>
+    <row r="575" spans="1:2" ht="375" x14ac:dyDescent="0.25">
+      <c r="A575" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="B574" s="1" t="s">
+      <c r="B575" s="1" t="s">
         <v>706</v>
       </c>
     </row>
-    <row r="575" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A575" s="2" t="s">
+    <row r="576" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A576" s="2" t="s">
         <v>386</v>
       </c>
-      <c r="B575" s="1" t="s">
+      <c r="B576" s="1" t="s">
         <v>498</v>
-      </c>
-    </row>
-    <row r="576" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A576" s="2" t="s">
-        <v>308</v>
-      </c>
-      <c r="B576" s="1" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="577" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A577" s="2" t="s">
-        <v>373</v>
-      </c>
-      <c r="B577" s="3" t="s">
-        <v>976</v>
+        <v>308</v>
+      </c>
+      <c r="B577" s="1" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="578" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A578" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="B578" s="3" t="s">
+        <v>975</v>
+      </c>
+    </row>
+    <row r="579" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A579" s="2" t="s">
         <v>726</v>
       </c>
-      <c r="B578" s="3" t="s">
+      <c r="B579" s="3" t="s">
         <v>727</v>
       </c>
     </row>
-    <row r="579" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A579" s="2" t="s">
+    <row r="580" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A580" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="B579" s="3" t="s">
-        <v>1094</v>
+      <c r="B580" s="3" t="s">
+        <v>1093</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:B576">
-    <sortCondition ref="A1:A576"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:B577">
+    <sortCondition ref="A1:A577"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Finished e144 - Huldra secret
</commit_message>
<xml_diff>
--- a/Documentation/Events.xlsx
+++ b/Documentation/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\happysulla\BarbarianPrince\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{2DB0CBAF-5F5E-4364-B673-3980B95E5B2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{69F82AE2-1079-490A-8AF0-A89299FDAC1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -35765,10 +35765,11 @@
     </r>
   </si>
   <si>
+    <t>e211g</t>
+  </si>
+  <si>
     <t>&lt;Bold&gt;e211c Seeking an Audience with the Baron of Huldra Castle&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;As a daily action, you spend the day trying to gain admission to see the Baron Huldra. Roll two die and consult the list below for results: 
- &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/dieRoll.gif' Name='DiceRoll' Height='21' Width='21'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;As a daily action, you spend the day trying to gain admission to see the Baron Huldra.&lt;LineBreak/&gt;&lt;LineBreak/&gt;
            2 Audience permanently refused. You cannot try again&lt;LineBreak/&gt;
   &lt;InlineUIContainer&gt;&lt;Button Content='e154' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 3 Meet Baron's Daughter&lt;LineBreak/&gt;
   &lt;InlineUIContainer&gt;&lt;Button Content='e149' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 4 Must learn court manners&lt;LineBreak/&gt;
@@ -35778,19 +35779,65 @@
   &lt;InlineUIContainer&gt;&lt;Button Content='e148' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 9 Seneschal requires a bribe&lt;LineBreak/&gt;
   &lt;InlineUIContainer&gt;&lt;Button Content='e150' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 10,11 Pay your respects to the Baron&lt;LineBreak/&gt;
   &lt;InlineUIContainer&gt;&lt;Button Content='e151' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 12 Find favor in the eyes of the Baron&lt;LineBreak/&gt;
-  &lt;InlineUIContainer&gt;&lt;Button Content='e152' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 13 plus - Baron becomes your Noble ally&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
-    <t>e211g</t>
+  &lt;InlineUIContainer&gt;&lt;Button Content='e152' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 13 plus - Baron becomes your Noble ally
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='Dismiss' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; a random magic user from party to add one to die roll.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Roll two die and consult list for results:  &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/dieRoll.gif' Name='DiceRoll' Height='21' Width='21'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
     <r>
       <t>&lt;Bold&gt;e211g Seeking an Audience with Real Heir in Party&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;As a daily action, you spend the day trying to gain admission to see the Baron Huldra. You have the real Huldra's heir in your party, and you want to restore him to the throne.  Choose one option:
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='Continue' FontFamily='Courier New' FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; to seek normal audience per &lt;InlineUIContainer&gt;&lt;Button Content='e211c' FontFamily='Courier New' FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;Alternatively, you can despose Baron Huldra if 10 plus rolled. Die Roll=
-&lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;As a daily action, you spend the day trying to gain admission to see the Baron Huldra. You have the real Huldra's heir in your party, and you want to restore him to the throne. You will despose Baron Huldra if a 10 plus is rolled. If you fail, you will be expelled from the kingdom and may never return. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;Alternately, you can 
+&lt;InlineUIContainer&gt;&lt;Button Name='Continue' Content='Continue' FontFamily='Courier New' FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+to seek normal audience per &lt;InlineUIContainer&gt;&lt;Button Content='e211c' FontFamily='Courier New' FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                     &lt;InlineUIContainer&gt;&lt;Image Name='</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>HuldraAudience</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>' Source='../../Images/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>BaronHuldra1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.gif' Height='250' Width='200'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='Dismiss' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; a random magic user from party to add one to die roll.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Roll two die and consult list for results:  &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
     </r>
     <r>
       <rPr>
@@ -35830,49 +35877,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>' Height='21' Width='21'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                     &lt;InlineUIContainer&gt;&lt;Image Name='</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>HuldraAudience</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>' Source='../../Images/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>BaronHuldra1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.gif' Height='250' Width='200'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+      <t>' Height='21' Width='21'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
     </r>
   </si>
 </sst>
@@ -36339,8 +36344,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B580"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A487" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B488" sqref="B488"/>
+    <sheetView tabSelected="1" topLeftCell="A483" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B487" sqref="B487"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -40213,12 +40218,12 @@
         <v>903</v>
       </c>
     </row>
-    <row r="484" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+    <row r="484" spans="1:2" ht="240" x14ac:dyDescent="0.25">
       <c r="A484" s="2" t="s">
         <v>614</v>
       </c>
       <c r="B484" s="3" t="s">
-        <v>1157</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="485" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -40245,9 +40250,9 @@
         <v>904</v>
       </c>
     </row>
-    <row r="488" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+    <row r="488" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A488" s="2" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
       <c r="B488" s="3" t="s">
         <v>1159</v>

</xml_diff>

<commit_message>
Fixed problem with meeting high lords on the travels
</commit_message>
<xml_diff>
--- a/Documentation/Events.xlsx
+++ b/Documentation/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\happysulla\BarbarianPrince\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4F0AD85A-745B-457E-83E8-BC190E353FA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C6C12BD6-98A5-4E28-BE4D-5AA6BC131ECC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -19160,164 +19160,6 @@
   </si>
   <si>
     <r>
-      <t>&lt;Bold&gt;e130a Talk to High Lord&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
- &lt;InlineUIContainer&gt;&lt;Button Content='e327' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; - 1 Pass&lt;LineBreak/&gt;
- &lt;InlineUIContainer&gt;&lt;Button Content='e329' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; - 2 Pass&lt;LineBreak/&gt;
- &lt;InlineUIContainer&gt;&lt;Button Content='e130d' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; - 3 Arrested&lt;LineBreak/&gt;
- &lt;InlineUIContainer&gt;&lt;Button Content='e130e' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; - 4 Audience&lt;LineBreak/&gt;
- &lt;InlineUIContainer&gt;&lt;Button Content='e130g' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; - 5 Inquiry&lt;LineBreak/&gt;
- &lt;InlineUIContainer&gt;&lt;Button Content='e307' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; - 6 Attacked
-&lt;LineBreak/&gt;Roll die:
- &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>dieRoll</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.gif' Name='</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>DieRoll</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>' Height='21'  Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
- &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>dieRoll</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.gif' Name='</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>DieRoll1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>' Height='21'  Width='21'  Visibility='Hidden'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
- &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>dieRoll</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.gif' Name='</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>DieRoll2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>' Height='21'  Width='21' Visibility='Hidden'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;
-                   &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>HighLords</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.gif' Height='200'  Width='400' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>&lt;Bold&gt;e130e Audience With High Lord on Travels&lt;/Bold&gt;
 &lt;LineBreak/&gt;
 &lt;LineBreak/&gt;If you gain an audence with Baron Huldra, see &lt;InlineUIContainer&gt;&lt;Button Content='e130f' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
@@ -24608,55 +24450,6 @@
         <scheme val="minor"/>
       </rPr>
       <t>.gif' Height='210' Width='300'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>&lt;Bold&gt;e130g High Lord Inquiry Bribe/Robbery&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-You may bribe the bodyguard for an audience. If you pay this, see &lt;InlineUIContainer&gt;&lt;Button Content='e130d' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. However, you must still suffer any adverse results from the audience. Presumably, this is due to additional guards in the area, magic protection, or power of the Lord/Lady. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;Alternatively, instead of an audience, you can rob the Lord/Lady who has wealth 100. However, if you rob Baron Huldra, Count Drogat, or Lady Aeravir; you can never enter the castle hex where they rule.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;Robbery: &lt;LineBreak/&gt;&lt;InlineUIContainer&gt;&lt;Image Name='</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>GuardRob</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>' Source='../../Images/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>CoinsStackedDeny</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">.gif' Height='75'  Width='75'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt; </t>
     </r>
   </si>
   <si>
@@ -35929,6 +35722,258 @@
         <scheme val="minor"/>
       </rPr>
       <t>' Height='350' Width='300'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;Bold&gt;e130g High Lord Inquiry Bribe/Robbery&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+You may bribe the bodyguard for an audience. If you pay this, see &lt;InlineUIContainer&gt;&lt;Button Content='e130e' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. However, you must still suffer any adverse results from the audience. Presumably, this is due to additional guards in the area, magic protection, or power of the Lord/Lady. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;Alternatively, instead of an audience, you can rob the Lord/Lady who has wealth 100. However, if you rob Baron Huldra, Count Drogat, or Lady Aeravir; you can never enter the castle hex where they rule.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;Do nothing and event ends: 
+&lt;LineBreak/&gt;&lt;InlineUIContainer&gt;&lt;Image Name='</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>EncounterEnd</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>' Source='../../Images/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CoinsStackedDeny</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.gif' Height='100'  Width='100'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt; 
+&lt;LineBreak/&gt;Robbery: 
+&lt;LineBreak/&gt;&lt;InlineUIContainer&gt;&lt;Image Name='</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>GuardRob</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>' Source='../../Images/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Robbery</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">.gif' Height='100'  Width='100'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt; </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;Bold&gt;e130a Talk to High Lord&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+ &lt;InlineUIContainer&gt;&lt;Button Content='e327' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; - 1 Pass&lt;LineBreak/&gt;
+ &lt;InlineUIContainer&gt;&lt;Button Content='e329' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; - 2 Pass&lt;LineBreak/&gt;
+ &lt;InlineUIContainer&gt;&lt;Button Content='e130d' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; - 3 Arrested&lt;LineBreak/&gt;
+ &lt;InlineUIContainer&gt;&lt;Button Content='e130e' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; - 4 Audience&lt;LineBreak/&gt;
+ &lt;InlineUIContainer&gt;&lt;Button Content='r342' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; - 5 Inquiry*&lt;LineBreak/&gt;
+ &lt;InlineUIContainer&gt;&lt;Button Content='e307' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; - 6 Attacked
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+&lt;Italic&gt;*Note:&lt;/Italic&gt; Any inquiry result that normally allows hiring a character instead permits you to bribe the bodyguards with 10gp for an audience. If you do not pay, encounter ends. Aternatively, you can perform a robbery for wealth class 100.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;Roll die:
+ &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dieRoll</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.gif' Name='</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DieRoll</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>' Height='21'  Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
+ &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dieRoll</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.gif' Name='</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DieRoll1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>' Height='21'  Width='21'  Visibility='Hidden'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
+ &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dieRoll</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.gif' Name='</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DieRoll2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>' Height='21'  Width='21' Visibility='Hidden'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;
+                   &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>HighLords</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.gif' Height='200'  Width='400' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
     </r>
   </si>
 </sst>
@@ -36395,8 +36440,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B581"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A414" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B414" sqref="B414"/>
+    <sheetView tabSelected="1" topLeftCell="A333" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B334" sqref="B334"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -36410,7 +36455,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1102</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -36418,7 +36463,7 @@
         <v>254</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1044</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -36426,7 +36471,7 @@
         <v>255</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>1043</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -36434,15 +36479,15 @@
         <v>256</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>1041</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>1038</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>1040</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>1042</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="390" x14ac:dyDescent="0.25">
@@ -36466,7 +36511,7 @@
         <v>22</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>1046</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -36482,7 +36527,7 @@
         <v>23</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>1104</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -36498,7 +36543,7 @@
         <v>3</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>973</v>
+        <v>971</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -36562,7 +36607,7 @@
         <v>11</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>1101</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -36594,7 +36639,7 @@
         <v>15</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -36602,7 +36647,7 @@
         <v>16</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -36610,7 +36655,7 @@
         <v>17</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -36618,7 +36663,7 @@
         <v>18</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -36626,31 +36671,31 @@
         <v>261</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -36658,7 +36703,7 @@
         <v>19</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -36666,7 +36711,7 @@
         <v>20</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -36674,23 +36719,23 @@
         <v>21</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>1091</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>1093</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>1092</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -36698,23 +36743,23 @@
         <v>25</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -36722,7 +36767,7 @@
         <v>26</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>988</v>
+        <v>986</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -36746,7 +36791,7 @@
         <v>27</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>1095</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -36754,7 +36799,7 @@
         <v>28</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>1098</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -36762,7 +36807,7 @@
         <v>29</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>1096</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -36770,7 +36815,7 @@
         <v>30</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>1099</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -36786,7 +36831,7 @@
         <v>693</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>1094</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -36794,7 +36839,7 @@
         <v>31</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>1110</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -36802,7 +36847,7 @@
         <v>32</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>1100</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -36810,7 +36855,7 @@
         <v>33</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>1097</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -36842,7 +36887,7 @@
         <v>491</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>1064</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -36866,7 +36911,7 @@
         <v>264</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>998</v>
+        <v>996</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -36874,7 +36919,7 @@
         <v>265</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>997</v>
+        <v>995</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37010,7 +37055,7 @@
         <v>42</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>971</v>
+        <v>969</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37018,7 +37063,7 @@
         <v>46</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>1027</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -37138,7 +37183,7 @@
         <v>774</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>1068</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -37146,15 +37191,15 @@
         <v>59</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
+        <v>873</v>
+      </c>
+      <c r="B94" s="3" t="s">
         <v>874</v>
-      </c>
-      <c r="B94" s="3" t="s">
-        <v>875</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -37170,7 +37215,7 @@
         <v>764</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>1069</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -37226,7 +37271,7 @@
         <v>66</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37274,7 +37319,7 @@
         <v>469</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>1070</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -37306,7 +37351,7 @@
         <v>70</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>978</v>
+        <v>976</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -37370,7 +37415,7 @@
         <v>75</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="122" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -37378,15 +37423,15 @@
         <v>325</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>1158</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="123" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
-        <v>1157</v>
+        <v>1155</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>1160</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="124" spans="1:2" ht="270" x14ac:dyDescent="0.25">
@@ -37402,7 +37447,7 @@
         <v>77</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
     </row>
     <row r="126" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -37415,10 +37460,10 @@
     </row>
     <row r="127" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>1071</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="128" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37426,7 +37471,7 @@
         <v>78</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
     </row>
     <row r="129" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -37434,7 +37479,7 @@
         <v>372</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
     </row>
     <row r="130" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37482,87 +37527,87 @@
         <v>81</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
     </row>
     <row r="136" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
     </row>
     <row r="137" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
     </row>
     <row r="138" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
     </row>
     <row r="139" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="B139" s="3" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
     </row>
     <row r="140" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
     </row>
     <row r="141" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
     </row>
     <row r="142" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
     </row>
     <row r="143" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="B143" s="3" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
     </row>
     <row r="144" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
+        <v>933</v>
+      </c>
+      <c r="B144" s="3" t="s">
         <v>934</v>
-      </c>
-      <c r="B144" s="3" t="s">
-        <v>935</v>
       </c>
     </row>
     <row r="145" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
     </row>
     <row r="146" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37570,7 +37615,7 @@
         <v>82</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
     </row>
     <row r="147" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -37583,7 +37628,7 @@
     </row>
     <row r="148" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
-        <v>1061</v>
+        <v>1059</v>
       </c>
       <c r="B148" s="3" t="s">
         <v>545</v>
@@ -37618,7 +37663,7 @@
         <v>544</v>
       </c>
       <c r="B152" s="3" t="s">
-        <v>1133</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="153" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37706,7 +37751,7 @@
         <v>344</v>
       </c>
       <c r="B163" s="3" t="s">
-        <v>1114</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="164" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -37738,7 +37783,7 @@
         <v>438</v>
       </c>
       <c r="B167" s="3" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
     </row>
     <row r="168" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37810,7 +37855,7 @@
         <v>93</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
     </row>
     <row r="177" spans="1:2" ht="270" x14ac:dyDescent="0.25">
@@ -37818,7 +37863,7 @@
         <v>94</v>
       </c>
       <c r="B177" s="3" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
     </row>
     <row r="178" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37826,7 +37871,7 @@
         <v>95</v>
       </c>
       <c r="B178" s="3" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
     </row>
     <row r="179" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37834,55 +37879,55 @@
         <v>96</v>
       </c>
       <c r="B179" s="3" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
     </row>
     <row r="180" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A180" s="2" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="B180" s="3" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
     </row>
     <row r="181" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>1072</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="182" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="B182" s="3" t="s">
-        <v>1073</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="183" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="B183" s="3" t="s">
-        <v>1074</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="184" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A184" s="2" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="B184" s="3" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="185" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A185" s="2" t="s">
+        <v>850</v>
+      </c>
+      <c r="B185" s="3" t="s">
         <v>851</v>
-      </c>
-      <c r="B185" s="3" t="s">
-        <v>852</v>
       </c>
     </row>
     <row r="186" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -37890,7 +37935,7 @@
         <v>97</v>
       </c>
       <c r="B186" s="3" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="187" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -37938,7 +37983,7 @@
         <v>103</v>
       </c>
       <c r="B192" s="3" t="s">
-        <v>956</v>
+        <v>954</v>
       </c>
     </row>
     <row r="193" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37946,7 +37991,7 @@
         <v>104</v>
       </c>
       <c r="B193" s="3" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
     </row>
     <row r="194" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37962,7 +38007,7 @@
         <v>680</v>
       </c>
       <c r="B195" s="3" t="s">
-        <v>1075</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="196" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37978,7 +38023,7 @@
         <v>106</v>
       </c>
       <c r="B197" s="3" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
     </row>
     <row r="198" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -38010,7 +38055,7 @@
         <v>108</v>
       </c>
       <c r="B201" s="3" t="s">
-        <v>960</v>
+        <v>958</v>
       </c>
     </row>
     <row r="202" spans="1:2" ht="285" x14ac:dyDescent="0.25">
@@ -38018,7 +38063,7 @@
         <v>109</v>
       </c>
       <c r="B202" s="3" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
     </row>
     <row r="203" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -38034,7 +38079,7 @@
         <v>166</v>
       </c>
       <c r="B204" s="3" t="s">
-        <v>1028</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="205" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -38042,7 +38087,7 @@
         <v>167</v>
       </c>
       <c r="B205" s="3" t="s">
-        <v>1039</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="206" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -38050,23 +38095,23 @@
         <v>168</v>
       </c>
       <c r="B206" s="3" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
     </row>
     <row r="207" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A207" s="2" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="B207" s="3" t="s">
-        <v>1076</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="208" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A208" s="2" t="s">
+        <v>864</v>
+      </c>
+      <c r="B208" s="3" t="s">
         <v>865</v>
-      </c>
-      <c r="B208" s="3" t="s">
-        <v>866</v>
       </c>
     </row>
     <row r="209" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -38138,7 +38183,7 @@
         <v>171</v>
       </c>
       <c r="B217" s="3" t="s">
-        <v>1055</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="218" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -38146,7 +38191,7 @@
         <v>113</v>
       </c>
       <c r="B218" s="3" t="s">
-        <v>989</v>
+        <v>987</v>
       </c>
     </row>
     <row r="219" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -38154,7 +38199,7 @@
         <v>114</v>
       </c>
       <c r="B219" s="3" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="220" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -38162,15 +38207,15 @@
         <v>266</v>
       </c>
       <c r="B220" s="3" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
     </row>
     <row r="221" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A221" s="2" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="B221" s="3" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="222" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -38178,7 +38223,7 @@
         <v>115</v>
       </c>
       <c r="B222" s="3" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
     </row>
     <row r="223" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -38194,7 +38239,7 @@
         <v>116</v>
       </c>
       <c r="B224" s="3" t="s">
-        <v>1021</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="225" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -38234,7 +38279,7 @@
         <v>738</v>
       </c>
       <c r="B229" s="4" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
     </row>
     <row r="230" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38242,23 +38287,23 @@
         <v>118</v>
       </c>
       <c r="B230" s="3" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
     </row>
     <row r="231" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A231" s="2" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="B231" s="3" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
     </row>
     <row r="232" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A232" s="2" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="B232" s="3" t="s">
-        <v>1017</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="233" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38266,23 +38311,23 @@
         <v>119</v>
       </c>
       <c r="B233" s="3" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
     </row>
     <row r="234" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A234" s="2" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="B234" s="3" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
     </row>
     <row r="235" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A235" s="2" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="B235" s="3" t="s">
-        <v>1077</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="236" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -38290,7 +38335,7 @@
         <v>120</v>
       </c>
       <c r="B236" s="3" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
     </row>
     <row r="237" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -38298,7 +38343,7 @@
         <v>172</v>
       </c>
       <c r="B237" s="3" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="238" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -38306,7 +38351,7 @@
         <v>173</v>
       </c>
       <c r="B238" s="3" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
     </row>
     <row r="239" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -38314,7 +38359,7 @@
         <v>174</v>
       </c>
       <c r="B239" s="3" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
     </row>
     <row r="240" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -38346,23 +38391,23 @@
         <v>123</v>
       </c>
       <c r="B243" s="3" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
     </row>
     <row r="244" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A244" s="2" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="B244" s="3" t="s">
-        <v>1078</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="245" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A245" s="2" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="B245" s="3" t="s">
-        <v>1079</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="246" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -38375,10 +38420,10 @@
     </row>
     <row r="247" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A247" s="2" t="s">
-        <v>1107</v>
+        <v>1105</v>
       </c>
       <c r="B247" s="3" t="s">
-        <v>1108</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="248" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -38386,15 +38431,15 @@
         <v>125</v>
       </c>
       <c r="B248" s="3" t="s">
-        <v>953</v>
+        <v>951</v>
       </c>
     </row>
     <row r="249" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A249" s="2" t="s">
-        <v>952</v>
+        <v>950</v>
       </c>
       <c r="B249" s="3" t="s">
-        <v>1067</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="250" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -38402,7 +38447,7 @@
         <v>126</v>
       </c>
       <c r="B250" s="3" t="s">
-        <v>959</v>
+        <v>957</v>
       </c>
     </row>
     <row r="251" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -38410,7 +38455,7 @@
         <v>127</v>
       </c>
       <c r="B251" s="3" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
     </row>
     <row r="252" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -38426,7 +38471,7 @@
         <v>129</v>
       </c>
       <c r="B253" s="3" t="s">
-        <v>958</v>
+        <v>956</v>
       </c>
     </row>
     <row r="254" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -38434,7 +38479,7 @@
         <v>130</v>
       </c>
       <c r="B254" s="3" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="255" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -38442,23 +38487,23 @@
         <v>131</v>
       </c>
       <c r="B255" s="3" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
     </row>
     <row r="256" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A256" s="2" t="s">
+        <v>909</v>
+      </c>
+      <c r="B256" s="3" t="s">
         <v>910</v>
-      </c>
-      <c r="B256" s="3" t="s">
-        <v>911</v>
       </c>
     </row>
     <row r="257" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A257" s="2" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="B257" s="3" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
     </row>
     <row r="258" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -38466,7 +38511,7 @@
         <v>132</v>
       </c>
       <c r="B258" s="3" t="s">
-        <v>966</v>
+        <v>964</v>
       </c>
     </row>
     <row r="259" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38474,15 +38519,15 @@
         <v>133</v>
       </c>
       <c r="B259" s="3" t="s">
-        <v>1080</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="260" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A260" s="2" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="B260" s="3" t="s">
-        <v>1007</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="261" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -38490,23 +38535,23 @@
         <v>134</v>
       </c>
       <c r="B261" s="3" t="s">
-        <v>961</v>
+        <v>959</v>
       </c>
     </row>
     <row r="262" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A262" s="2" t="s">
-        <v>962</v>
+        <v>960</v>
       </c>
       <c r="B262" s="3" t="s">
-        <v>963</v>
+        <v>961</v>
       </c>
     </row>
     <row r="263" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A263" s="2" t="s">
-        <v>964</v>
+        <v>962</v>
       </c>
       <c r="B263" s="3" t="s">
-        <v>965</v>
+        <v>963</v>
       </c>
     </row>
     <row r="264" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -38514,15 +38559,15 @@
         <v>135</v>
       </c>
       <c r="B264" s="3" t="s">
-        <v>969</v>
+        <v>967</v>
       </c>
     </row>
     <row r="265" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A265" s="2" t="s">
-        <v>967</v>
+        <v>965</v>
       </c>
       <c r="B265" s="3" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
     </row>
     <row r="266" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38530,7 +38575,7 @@
         <v>136</v>
       </c>
       <c r="B266" s="3" t="s">
-        <v>970</v>
+        <v>968</v>
       </c>
     </row>
     <row r="267" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -38554,7 +38599,7 @@
         <v>233</v>
       </c>
       <c r="B269" s="3" t="s">
-        <v>1106</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="270" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -38570,7 +38615,7 @@
         <v>234</v>
       </c>
       <c r="B271" s="3" t="s">
-        <v>1081</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="272" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -38578,7 +38623,7 @@
         <v>235</v>
       </c>
       <c r="B272" s="3" t="s">
-        <v>1082</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="273" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -38618,7 +38663,7 @@
         <v>140</v>
       </c>
       <c r="B277" s="3" t="s">
-        <v>1023</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="278" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -38626,7 +38671,7 @@
         <v>236</v>
       </c>
       <c r="B278" s="3" t="s">
-        <v>1029</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="279" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -38634,7 +38679,7 @@
         <v>237</v>
       </c>
       <c r="B279" s="3" t="s">
-        <v>1022</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="280" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -38642,7 +38687,7 @@
         <v>238</v>
       </c>
       <c r="B280" s="3" t="s">
-        <v>1083</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="281" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -38650,7 +38695,7 @@
         <v>141</v>
       </c>
       <c r="B281" s="3" t="s">
-        <v>1010</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="282" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -38658,7 +38703,7 @@
         <v>142</v>
       </c>
       <c r="B282" s="3" t="s">
-        <v>1011</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="283" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38666,7 +38711,7 @@
         <v>143</v>
       </c>
       <c r="B283" s="3" t="s">
-        <v>1012</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="284" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -38674,7 +38719,7 @@
         <v>144</v>
       </c>
       <c r="B284" s="3" t="s">
-        <v>1016</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="285" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -38682,7 +38727,7 @@
         <v>242</v>
       </c>
       <c r="B285" s="3" t="s">
-        <v>1018</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="286" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -38690,7 +38735,7 @@
         <v>145</v>
       </c>
       <c r="B286" s="3" t="s">
-        <v>1015</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="287" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -38698,7 +38743,7 @@
         <v>146</v>
       </c>
       <c r="B287" s="3" t="s">
-        <v>1019</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="288" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -38706,7 +38751,7 @@
         <v>147</v>
       </c>
       <c r="B288" s="3" t="s">
-        <v>1014</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="289" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38714,7 +38759,7 @@
         <v>148</v>
       </c>
       <c r="B289" s="3" t="s">
-        <v>1020</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="290" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -38722,31 +38767,31 @@
         <v>149</v>
       </c>
       <c r="B290" s="3" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="291" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A291" s="2" t="s">
-        <v>1031</v>
+        <v>1029</v>
       </c>
       <c r="B291" s="3" t="s">
-        <v>1105</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="292" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A292" s="2" t="s">
-        <v>1030</v>
+        <v>1028</v>
       </c>
       <c r="B292" s="3" t="s">
-        <v>1035</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="293" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A293" s="2" t="s">
-        <v>1032</v>
+        <v>1030</v>
       </c>
       <c r="B293" s="3" t="s">
-        <v>1033</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="294" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -38754,15 +38799,15 @@
         <v>150</v>
       </c>
       <c r="B294" s="3" t="s">
-        <v>1037</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="295" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A295" s="2" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B295" s="3" t="s">
         <v>1036</v>
-      </c>
-      <c r="B295" s="3" t="s">
-        <v>1038</v>
       </c>
     </row>
     <row r="296" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -38786,7 +38831,7 @@
         <v>244</v>
       </c>
       <c r="B298" s="3" t="s">
-        <v>1109</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="299" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -38810,7 +38855,7 @@
         <v>153</v>
       </c>
       <c r="B301" s="3" t="s">
-        <v>1013</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="302" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -38882,7 +38927,7 @@
         <v>159</v>
       </c>
       <c r="B310" s="3" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
     </row>
     <row r="311" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -38890,7 +38935,7 @@
         <v>160</v>
       </c>
       <c r="B311" s="3" t="s">
-        <v>955</v>
+        <v>953</v>
       </c>
     </row>
     <row r="312" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -38898,7 +38943,7 @@
         <v>161</v>
       </c>
       <c r="B312" s="3" t="s">
-        <v>986</v>
+        <v>984</v>
       </c>
     </row>
     <row r="313" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -38906,31 +38951,31 @@
         <v>162</v>
       </c>
       <c r="B313" s="3" t="s">
-        <v>1001</v>
+        <v>999</v>
       </c>
     </row>
     <row r="314" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A314" s="2" t="s">
-        <v>999</v>
+        <v>997</v>
       </c>
       <c r="B314" s="3" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="315" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A315" s="2" t="s">
-        <v>1000</v>
+        <v>998</v>
       </c>
       <c r="B315" s="3" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="316" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A316" s="2" t="s">
+        <v>1001</v>
+      </c>
+      <c r="B316" s="3" t="s">
         <v>1003</v>
-      </c>
-      <c r="B316" s="3" t="s">
-        <v>1005</v>
       </c>
     </row>
     <row r="317" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -38938,7 +38983,7 @@
         <v>163</v>
       </c>
       <c r="B317" s="3" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="318" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -38946,7 +38991,7 @@
         <v>164</v>
       </c>
       <c r="B318" s="3" t="s">
-        <v>994</v>
+        <v>992</v>
       </c>
     </row>
     <row r="319" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -38954,7 +38999,7 @@
         <v>175</v>
       </c>
       <c r="B319" s="3" t="s">
-        <v>993</v>
+        <v>991</v>
       </c>
     </row>
     <row r="320" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -38962,7 +39007,7 @@
         <v>176</v>
       </c>
       <c r="B320" s="3" t="s">
-        <v>992</v>
+        <v>990</v>
       </c>
     </row>
     <row r="321" spans="1:2" ht="390" x14ac:dyDescent="0.25">
@@ -38970,7 +39015,7 @@
         <v>177</v>
       </c>
       <c r="B321" s="3" t="s">
-        <v>975</v>
+        <v>973</v>
       </c>
     </row>
     <row r="322" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -38978,7 +39023,7 @@
         <v>514</v>
       </c>
       <c r="B322" s="3" t="s">
-        <v>984</v>
+        <v>982</v>
       </c>
     </row>
     <row r="323" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -38986,7 +39031,7 @@
         <v>515</v>
       </c>
       <c r="B323" s="3" t="s">
-        <v>977</v>
+        <v>975</v>
       </c>
     </row>
     <row r="324" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -38994,7 +39039,7 @@
         <v>516</v>
       </c>
       <c r="B324" s="3" t="s">
-        <v>983</v>
+        <v>981</v>
       </c>
     </row>
     <row r="325" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -39002,7 +39047,7 @@
         <v>517</v>
       </c>
       <c r="B325" s="3" t="s">
-        <v>1112</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="326" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -39010,7 +39055,7 @@
         <v>518</v>
       </c>
       <c r="B326" s="3" t="s">
-        <v>982</v>
+        <v>980</v>
       </c>
     </row>
     <row r="327" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -39018,15 +39063,15 @@
         <v>519</v>
       </c>
       <c r="B327" s="3" t="s">
-        <v>976</v>
+        <v>974</v>
       </c>
     </row>
     <row r="328" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A328" s="2" t="s">
-        <v>1053</v>
+        <v>1051</v>
       </c>
       <c r="B328" s="3" t="s">
-        <v>1084</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="329" spans="1:2" ht="390" x14ac:dyDescent="0.25">
@@ -39034,7 +39079,7 @@
         <v>178</v>
       </c>
       <c r="B329" s="3" t="s">
-        <v>980</v>
+        <v>978</v>
       </c>
     </row>
     <row r="330" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -39042,7 +39087,7 @@
         <v>489</v>
       </c>
       <c r="B330" s="3" t="s">
-        <v>985</v>
+        <v>983</v>
       </c>
     </row>
     <row r="331" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -39050,7 +39095,7 @@
         <v>541</v>
       </c>
       <c r="B331" s="3" t="s">
-        <v>1085</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="332" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -39058,7 +39103,7 @@
         <v>542</v>
       </c>
       <c r="B332" s="3" t="s">
-        <v>981</v>
+        <v>979</v>
       </c>
     </row>
     <row r="333" spans="1:2" ht="315" x14ac:dyDescent="0.25">
@@ -39069,12 +39114,12 @@
         <v>817</v>
       </c>
     </row>
-    <row r="334" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:2" ht="240" x14ac:dyDescent="0.25">
       <c r="A334" s="2" t="s">
         <v>249</v>
       </c>
       <c r="B334" s="3" t="s">
-        <v>820</v>
+        <v>1161</v>
       </c>
     </row>
     <row r="335" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -39082,7 +39127,7 @@
         <v>250</v>
       </c>
       <c r="B335" s="3" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
     </row>
     <row r="336" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -39090,7 +39135,7 @@
         <v>251</v>
       </c>
       <c r="B336" s="3" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
     </row>
     <row r="337" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39098,7 +39143,7 @@
         <v>252</v>
       </c>
       <c r="B337" s="3" t="s">
-        <v>1062</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="338" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -39106,7 +39151,7 @@
         <v>253</v>
       </c>
       <c r="B338" s="3" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
     </row>
     <row r="339" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -39114,15 +39159,15 @@
         <v>818</v>
       </c>
       <c r="B339" s="3" t="s">
-        <v>822</v>
-      </c>
-    </row>
-    <row r="340" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="340" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A340" s="2" t="s">
         <v>819</v>
       </c>
       <c r="B340" s="3" t="s">
-        <v>946</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="341" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -39130,7 +39175,7 @@
         <v>180</v>
       </c>
       <c r="B341" s="3" t="s">
-        <v>957</v>
+        <v>955</v>
       </c>
     </row>
     <row r="342" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39154,15 +39199,15 @@
         <v>182</v>
       </c>
       <c r="B344" s="3" t="s">
-        <v>1131</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="345" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A345" s="2" t="s">
+        <v>1128</v>
+      </c>
+      <c r="B345" s="3" t="s">
         <v>1130</v>
-      </c>
-      <c r="B345" s="3" t="s">
-        <v>1132</v>
       </c>
     </row>
     <row r="346" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39170,7 +39215,7 @@
         <v>183</v>
       </c>
       <c r="B346" s="3" t="s">
-        <v>1066</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="347" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -39178,7 +39223,7 @@
         <v>184</v>
       </c>
       <c r="B347" s="3" t="s">
-        <v>1065</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="348" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -39194,7 +39239,7 @@
         <v>185</v>
       </c>
       <c r="B349" s="3" t="s">
-        <v>1128</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="350" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -39218,7 +39263,7 @@
         <v>464</v>
       </c>
       <c r="B352" s="3" t="s">
-        <v>1086</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="353" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -39290,7 +39335,7 @@
         <v>193</v>
       </c>
       <c r="B361" s="3" t="s">
-        <v>1137</v>
+        <v>1135</v>
       </c>
     </row>
     <row r="362" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -39298,7 +39343,7 @@
         <v>336</v>
       </c>
       <c r="B362" s="3" t="s">
-        <v>1138</v>
+        <v>1136</v>
       </c>
     </row>
     <row r="363" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -39306,71 +39351,71 @@
         <v>337</v>
       </c>
       <c r="B363" s="3" t="s">
-        <v>1141</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="364" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A364" s="2" t="s">
-        <v>1135</v>
+        <v>1133</v>
       </c>
       <c r="B364" s="3" t="s">
-        <v>1140</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="365" spans="1:2" ht="225" x14ac:dyDescent="0.25">
       <c r="A365" s="2" t="s">
-        <v>1136</v>
+        <v>1134</v>
       </c>
       <c r="B365" s="3" t="s">
-        <v>1153</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="366" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A366" s="2" t="s">
-        <v>1139</v>
+        <v>1137</v>
       </c>
       <c r="B366" s="3" t="s">
-        <v>1152</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="367" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A367" s="2" t="s">
-        <v>1142</v>
+        <v>1140</v>
       </c>
       <c r="B367" s="3" t="s">
-        <v>1151</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="368" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A368" s="2" t="s">
-        <v>1143</v>
+        <v>1141</v>
       </c>
       <c r="B368" s="3" t="s">
-        <v>1150</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="369" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A369" s="2" t="s">
-        <v>1144</v>
+        <v>1142</v>
       </c>
       <c r="B369" s="3" t="s">
-        <v>1145</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="370" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A370" s="2" t="s">
+        <v>1144</v>
+      </c>
+      <c r="B370" s="3" t="s">
         <v>1146</v>
-      </c>
-      <c r="B370" s="3" t="s">
-        <v>1148</v>
       </c>
     </row>
     <row r="371" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A371" s="2" t="s">
+        <v>1145</v>
+      </c>
+      <c r="B371" s="3" t="s">
         <v>1147</v>
-      </c>
-      <c r="B371" s="3" t="s">
-        <v>1149</v>
       </c>
     </row>
     <row r="372" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -39386,15 +39431,15 @@
         <v>195</v>
       </c>
       <c r="B373" s="3" t="s">
-        <v>1125</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="374" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A374" s="2" t="s">
-        <v>1120</v>
+        <v>1118</v>
       </c>
       <c r="B374" s="3" t="s">
-        <v>1126</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="375" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -39402,7 +39447,7 @@
         <v>196</v>
       </c>
       <c r="B375" s="3" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
     </row>
     <row r="376" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -39410,7 +39455,7 @@
         <v>328</v>
       </c>
       <c r="B376" s="3" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
     </row>
     <row r="377" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -39426,7 +39471,7 @@
         <v>649</v>
       </c>
       <c r="B378" s="3" t="s">
-        <v>1087</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="379" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39450,7 +39495,7 @@
         <v>200</v>
       </c>
       <c r="B381" s="3" t="s">
-        <v>1119</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="382" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -39466,7 +39511,7 @@
         <v>202</v>
       </c>
       <c r="B383" s="3" t="s">
-        <v>947</v>
+        <v>945</v>
       </c>
     </row>
     <row r="384" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -39586,7 +39631,7 @@
         <v>580</v>
       </c>
       <c r="B398" s="3" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
     </row>
     <row r="399" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -39594,7 +39639,7 @@
         <v>581</v>
       </c>
       <c r="B399" s="3" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
     </row>
     <row r="400" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -39602,7 +39647,7 @@
         <v>582</v>
       </c>
       <c r="B400" s="3" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
     </row>
     <row r="401" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -39610,7 +39655,7 @@
         <v>583</v>
       </c>
       <c r="B401" s="3" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
     </row>
     <row r="402" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39626,7 +39671,7 @@
         <v>585</v>
       </c>
       <c r="B403" s="3" t="s">
-        <v>1113</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="404" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39642,7 +39687,7 @@
         <v>207</v>
       </c>
       <c r="B405" s="3" t="s">
-        <v>948</v>
+        <v>946</v>
       </c>
     </row>
     <row r="406" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -39658,7 +39703,7 @@
         <v>209</v>
       </c>
       <c r="B407" s="3" t="s">
-        <v>1111</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="408" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -39666,7 +39711,7 @@
         <v>632</v>
       </c>
       <c r="B408" s="3" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
     </row>
     <row r="409" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -39711,10 +39756,10 @@
     </row>
     <row r="414" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A414" s="2" t="s">
-        <v>1127</v>
+        <v>1125</v>
       </c>
       <c r="B414" s="3" t="s">
-        <v>1134</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="415" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -39722,7 +39767,7 @@
         <v>210</v>
       </c>
       <c r="B415" s="3" t="s">
-        <v>1124</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="416" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -39730,7 +39775,7 @@
         <v>619</v>
       </c>
       <c r="B416" s="3" t="s">
-        <v>1161</v>
+        <v>1159</v>
       </c>
     </row>
     <row r="417" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -39783,10 +39828,10 @@
     </row>
     <row r="423" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A423" s="2" t="s">
-        <v>1117</v>
+        <v>1115</v>
       </c>
       <c r="B423" s="3" t="s">
-        <v>1118</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="424" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -39810,7 +39855,7 @@
         <v>530</v>
       </c>
       <c r="B426" s="3" t="s">
-        <v>1088</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="427" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -39842,7 +39887,7 @@
         <v>213</v>
       </c>
       <c r="B430" s="3" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
     </row>
     <row r="431" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -39858,7 +39903,7 @@
         <v>215</v>
       </c>
       <c r="B432" s="3" t="s">
-        <v>1051</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="433" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39906,7 +39951,7 @@
         <v>221</v>
       </c>
       <c r="B438" s="3" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="439" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -39914,7 +39959,7 @@
         <v>222</v>
       </c>
       <c r="B439" s="3" t="s">
-        <v>1058</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="440" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -39922,7 +39967,7 @@
         <v>223</v>
       </c>
       <c r="B440" s="3" t="s">
-        <v>1057</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="441" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -39930,7 +39975,7 @@
         <v>224</v>
       </c>
       <c r="B441" s="3" t="s">
-        <v>1056</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="442" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -39938,7 +39983,7 @@
         <v>329</v>
       </c>
       <c r="B442" s="3" t="s">
-        <v>1060</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="443" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -39954,7 +39999,7 @@
         <v>225</v>
       </c>
       <c r="B444" s="3" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
     </row>
     <row r="445" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -39978,15 +40023,15 @@
         <v>228</v>
       </c>
       <c r="B447" s="3" t="s">
-        <v>1116</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="448" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A448" s="2" t="s">
-        <v>1115</v>
+        <v>1113</v>
       </c>
       <c r="B448" s="3" t="s">
-        <v>1121</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="449" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -40026,7 +40071,7 @@
         <v>442</v>
       </c>
       <c r="B453" s="3" t="s">
-        <v>1052</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="454" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -40066,7 +40111,7 @@
         <v>319</v>
       </c>
       <c r="B458" s="3" t="s">
-        <v>1047</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="459" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -40074,7 +40119,7 @@
         <v>320</v>
       </c>
       <c r="B459" s="3" t="s">
-        <v>1050</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="460" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -40082,7 +40127,7 @@
         <v>321</v>
       </c>
       <c r="B460" s="3" t="s">
-        <v>1048</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="461" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -40090,15 +40135,15 @@
         <v>318</v>
       </c>
       <c r="B461" s="3" t="s">
-        <v>1049</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="462" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A462" s="2" t="s">
-        <v>1008</v>
+        <v>1006</v>
       </c>
       <c r="B462" s="3" t="s">
-        <v>1009</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="463" spans="1:2" ht="255" x14ac:dyDescent="0.25">
@@ -40106,7 +40151,7 @@
         <v>322</v>
       </c>
       <c r="B463" s="3" t="s">
-        <v>1054</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="464" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -40130,7 +40175,7 @@
         <v>483</v>
       </c>
       <c r="B466" s="3" t="s">
-        <v>1089</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="467" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -40138,7 +40183,7 @@
         <v>484</v>
       </c>
       <c r="B467" s="3" t="s">
-        <v>1129</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="468" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -40170,7 +40215,7 @@
         <v>550</v>
       </c>
       <c r="B471" s="3" t="s">
-        <v>949</v>
+        <v>947</v>
       </c>
     </row>
     <row r="472" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -40178,7 +40223,7 @@
         <v>554</v>
       </c>
       <c r="B472" s="3" t="s">
-        <v>1103</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="473" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -40194,7 +40239,7 @@
         <v>558</v>
       </c>
       <c r="B474" s="3" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
     </row>
     <row r="475" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -40218,7 +40263,7 @@
         <v>561</v>
       </c>
       <c r="B477" s="3" t="s">
-        <v>950</v>
+        <v>948</v>
       </c>
     </row>
     <row r="478" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -40226,7 +40271,7 @@
         <v>562</v>
       </c>
       <c r="B478" s="3" t="s">
-        <v>1063</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="479" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -40242,7 +40287,7 @@
         <v>564</v>
       </c>
       <c r="B480" s="3" t="s">
-        <v>951</v>
+        <v>949</v>
       </c>
     </row>
     <row r="481" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -40274,7 +40319,7 @@
         <v>594</v>
       </c>
       <c r="B484" s="3" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="485" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -40282,7 +40327,7 @@
         <v>612</v>
       </c>
       <c r="B485" s="3" t="s">
-        <v>1155</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="486" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -40290,7 +40335,7 @@
         <v>613</v>
       </c>
       <c r="B486" s="3" t="s">
-        <v>1122</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="487" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -40298,23 +40343,23 @@
         <v>614</v>
       </c>
       <c r="B487" s="3" t="s">
-        <v>1123</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="488" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A488" s="2" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="B488" s="3" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
     </row>
     <row r="489" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A489" s="2" t="s">
+        <v>1152</v>
+      </c>
+      <c r="B489" s="3" t="s">
         <v>1154</v>
-      </c>
-      <c r="B489" s="3" t="s">
-        <v>1156</v>
       </c>
     </row>
     <row r="490" spans="1:2" ht="255" x14ac:dyDescent="0.25">
@@ -40370,7 +40415,7 @@
         <v>656</v>
       </c>
       <c r="B496" s="1" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
     </row>
     <row r="497" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -40410,7 +40455,7 @@
         <v>661</v>
       </c>
       <c r="B501" s="1" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
     </row>
     <row r="502" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -40439,18 +40484,18 @@
     </row>
     <row r="505" spans="1:2" ht="255" x14ac:dyDescent="0.25">
       <c r="A505" s="2" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
       <c r="B505" s="1" t="s">
-        <v>995</v>
+        <v>993</v>
       </c>
     </row>
     <row r="506" spans="1:2" ht="92.25" x14ac:dyDescent="0.25">
       <c r="A506" s="2" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
       <c r="B506" s="1" t="s">
-        <v>991</v>
+        <v>989</v>
       </c>
     </row>
     <row r="507" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -40458,7 +40503,7 @@
         <v>678</v>
       </c>
       <c r="B507" s="1" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
     </row>
     <row r="508" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -40466,7 +40511,7 @@
         <v>710</v>
       </c>
       <c r="B508" s="3" t="s">
-        <v>1045</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="509" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -40562,7 +40607,7 @@
         <v>275</v>
       </c>
       <c r="B520" s="1" t="s">
-        <v>1024</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="521" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -40570,7 +40615,7 @@
         <v>276</v>
       </c>
       <c r="B521" s="1" t="s">
-        <v>1025</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="522" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -40578,7 +40623,7 @@
         <v>277</v>
       </c>
       <c r="B522" s="1" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="523" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -40626,7 +40671,7 @@
         <v>260</v>
       </c>
       <c r="B528" s="3" t="s">
-        <v>974</v>
+        <v>972</v>
       </c>
     </row>
     <row r="529" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -40698,7 +40743,7 @@
         <v>285</v>
       </c>
       <c r="B537" s="1" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
     <row r="538" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -40706,7 +40751,7 @@
         <v>286</v>
       </c>
       <c r="B538" s="1" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
     </row>
     <row r="539" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -40826,7 +40871,7 @@
         <v>298</v>
       </c>
       <c r="B553" s="1" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
     </row>
     <row r="554" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -40866,7 +40911,7 @@
         <v>300</v>
       </c>
       <c r="B558" s="1" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
     </row>
     <row r="559" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -40874,7 +40919,7 @@
         <v>301</v>
       </c>
       <c r="B559" s="1" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
     </row>
     <row r="560" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -41002,7 +41047,7 @@
         <v>307</v>
       </c>
       <c r="B575" s="1" t="s">
-        <v>979</v>
+        <v>977</v>
       </c>
     </row>
     <row r="576" spans="1:2" ht="375" x14ac:dyDescent="0.25">
@@ -41034,7 +41079,7 @@
         <v>371</v>
       </c>
       <c r="B579" s="3" t="s">
-        <v>972</v>
+        <v>970</v>
       </c>
     </row>
     <row r="580" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -41050,7 +41095,7 @@
         <v>326</v>
       </c>
       <c r="B581" s="3" t="s">
-        <v>1090</v>
+        <v>1088</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix issue with Dwarven Mines
</commit_message>
<xml_diff>
--- a/Documentation/Events.xlsx
+++ b/Documentation/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\happysulla\BarbarianPrince\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C6C12BD6-98A5-4E28-BE4D-5AA6BC131ECC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5709F30C-00C8-4261-A8C5-C1EF232808FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -19876,61 +19876,6 @@
   </si>
   <si>
     <r>
-      <t>&lt;Bold&gt;e059 Dwarf Mines&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;You see a great underground castle inhabited by dwarves. Dwarven constables and patrols intercept your party. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;Roll one die. If the die roll exceeds your wit and wiles, you and your party are arrested immediately, see
- &lt;InlineUIContainer&gt;&lt;Button Content='e060' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;Otherwise, you may pass and enter the castle mines. There you can undertake any actions and activities normally allowed in a castle
- &lt;InlineUIContainer&gt;&lt;Button Content='r203' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
- This includes seeking an audence with the Dwarf King who rules there. See 
- &lt;InlineUIContainer&gt;&lt;Button Content='r211' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;Like any castle, you must spend the normal amounts for food &lt;InlineUIContainer&gt;&lt;Button Content='r215' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
- and lodgings &lt;InlineUIContainer&gt;&lt;Button Content='r217' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. Any hired help in this hex are dwarves.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;Die Roll = &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>dieRoll</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.gif' Name='</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>DieRoll</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>&lt;Bold&gt;e319 Easy Group Hide&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;You look around for enough cover to hide your party. 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;If the number of characters in your party is equal or less than the die roll, your party hides in the hex
@@ -35974,6 +35919,61 @@
         <scheme val="minor"/>
       </rPr>
       <t>.gif' Height='200'  Width='400' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;Bold&gt;e059 Dwarf Mines&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;You see a great underground castle inhabited by dwarves. Dwarven constables and patrols intercept your party. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;Roll one die. If the die roll exceeds your wit and wiles, you and your party are arrested immediately, see
+ &lt;InlineUIContainer&gt;&lt;Button Content='e060' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;Otherwise, you may pass and enter the castle mines. There you can undertake any actions and activities normally allowed in a castle.
+ &lt;InlineUIContainer&gt;&lt;Button Content='r203' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
+ This includes seeking an audence with the Dwarf King who rules there. See 
+ &lt;InlineUIContainer&gt;&lt;Button Content='r211' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;Like any castle, you must spend the normal amounts for food &lt;InlineUIContainer&gt;&lt;Button Content='r215' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+ and lodgings &lt;InlineUIContainer&gt;&lt;Button Content='r217' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. Any hired help in this hex are dwarves.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;Die Roll =  &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dieRoll</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.gif' Name='</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DieRoll</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
     </r>
   </si>
 </sst>
@@ -36440,8 +36440,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B581"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A333" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B334" sqref="B334"/>
+    <sheetView tabSelected="1" topLeftCell="A184" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B186" sqref="B186"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -36455,7 +36455,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -36463,7 +36463,7 @@
         <v>254</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -36471,7 +36471,7 @@
         <v>255</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -36479,15 +36479,15 @@
         <v>256</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="390" x14ac:dyDescent="0.25">
@@ -36511,7 +36511,7 @@
         <v>22</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -36527,7 +36527,7 @@
         <v>23</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -36543,7 +36543,7 @@
         <v>3</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -36607,7 +36607,7 @@
         <v>11</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -36639,7 +36639,7 @@
         <v>15</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -36647,7 +36647,7 @@
         <v>16</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -36655,7 +36655,7 @@
         <v>17</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -36663,7 +36663,7 @@
         <v>18</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -36671,31 +36671,31 @@
         <v>261</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -36703,7 +36703,7 @@
         <v>19</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -36711,7 +36711,7 @@
         <v>20</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -36719,23 +36719,23 @@
         <v>21</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -36743,23 +36743,23 @@
         <v>25</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -36767,7 +36767,7 @@
         <v>26</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -36791,7 +36791,7 @@
         <v>27</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -36799,7 +36799,7 @@
         <v>28</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -36807,7 +36807,7 @@
         <v>29</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -36815,7 +36815,7 @@
         <v>30</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -36831,7 +36831,7 @@
         <v>693</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -36839,7 +36839,7 @@
         <v>31</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -36847,7 +36847,7 @@
         <v>32</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -36855,7 +36855,7 @@
         <v>33</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -36887,7 +36887,7 @@
         <v>491</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -36911,7 +36911,7 @@
         <v>264</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -36919,7 +36919,7 @@
         <v>265</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37055,7 +37055,7 @@
         <v>42</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37063,7 +37063,7 @@
         <v>46</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -37183,7 +37183,7 @@
         <v>774</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -37191,15 +37191,15 @@
         <v>59</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
+        <v>872</v>
+      </c>
+      <c r="B94" s="3" t="s">
         <v>873</v>
-      </c>
-      <c r="B94" s="3" t="s">
-        <v>874</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -37215,7 +37215,7 @@
         <v>764</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -37271,7 +37271,7 @@
         <v>66</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37319,7 +37319,7 @@
         <v>469</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -37351,7 +37351,7 @@
         <v>70</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -37415,7 +37415,7 @@
         <v>75</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="122" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -37423,15 +37423,15 @@
         <v>325</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="123" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="124" spans="1:2" ht="270" x14ac:dyDescent="0.25">
@@ -37447,7 +37447,7 @@
         <v>77</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
     </row>
     <row r="126" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -37460,10 +37460,10 @@
     </row>
     <row r="127" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="128" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37471,7 +37471,7 @@
         <v>78</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
     </row>
     <row r="129" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -37479,7 +37479,7 @@
         <v>372</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
     </row>
     <row r="130" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37527,87 +37527,87 @@
         <v>81</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
     </row>
     <row r="136" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
     </row>
     <row r="137" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
     </row>
     <row r="138" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
     </row>
     <row r="139" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="B139" s="3" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
     </row>
     <row r="140" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
     </row>
     <row r="141" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
     </row>
     <row r="142" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
     </row>
     <row r="143" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="B143" s="3" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
     </row>
     <row r="144" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
+        <v>932</v>
+      </c>
+      <c r="B144" s="3" t="s">
         <v>933</v>
-      </c>
-      <c r="B144" s="3" t="s">
-        <v>934</v>
       </c>
     </row>
     <row r="145" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
     </row>
     <row r="146" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37615,7 +37615,7 @@
         <v>82</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
     </row>
     <row r="147" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -37628,7 +37628,7 @@
     </row>
     <row r="148" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="B148" s="3" t="s">
         <v>545</v>
@@ -37663,7 +37663,7 @@
         <v>544</v>
       </c>
       <c r="B152" s="3" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="153" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37751,7 +37751,7 @@
         <v>344</v>
       </c>
       <c r="B163" s="3" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="164" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -37783,7 +37783,7 @@
         <v>438</v>
       </c>
       <c r="B167" s="3" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
     </row>
     <row r="168" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37871,7 +37871,7 @@
         <v>95</v>
       </c>
       <c r="B178" s="3" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
     </row>
     <row r="179" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37895,7 +37895,7 @@
         <v>827</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="182" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37903,7 +37903,7 @@
         <v>828</v>
       </c>
       <c r="B182" s="3" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="183" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37911,23 +37911,23 @@
         <v>831</v>
       </c>
       <c r="B183" s="3" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="184" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A184" s="2" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="B184" s="3" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="185" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A185" s="2" t="s">
+        <v>849</v>
+      </c>
+      <c r="B185" s="3" t="s">
         <v>850</v>
-      </c>
-      <c r="B185" s="3" t="s">
-        <v>851</v>
       </c>
     </row>
     <row r="186" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -37935,7 +37935,7 @@
         <v>97</v>
       </c>
       <c r="B186" s="3" t="s">
-        <v>835</v>
+        <v>1161</v>
       </c>
     </row>
     <row r="187" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -37983,7 +37983,7 @@
         <v>103</v>
       </c>
       <c r="B192" s="3" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
     </row>
     <row r="193" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37991,7 +37991,7 @@
         <v>104</v>
       </c>
       <c r="B193" s="3" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
     </row>
     <row r="194" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -38007,7 +38007,7 @@
         <v>680</v>
       </c>
       <c r="B195" s="3" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="196" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -38023,7 +38023,7 @@
         <v>106</v>
       </c>
       <c r="B197" s="3" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
     </row>
     <row r="198" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -38055,7 +38055,7 @@
         <v>108</v>
       </c>
       <c r="B201" s="3" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
     </row>
     <row r="202" spans="1:2" ht="285" x14ac:dyDescent="0.25">
@@ -38063,7 +38063,7 @@
         <v>109</v>
       </c>
       <c r="B202" s="3" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
     </row>
     <row r="203" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -38079,7 +38079,7 @@
         <v>166</v>
       </c>
       <c r="B204" s="3" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="205" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -38087,7 +38087,7 @@
         <v>167</v>
       </c>
       <c r="B205" s="3" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="206" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -38095,23 +38095,23 @@
         <v>168</v>
       </c>
       <c r="B206" s="3" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
     </row>
     <row r="207" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A207" s="2" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="B207" s="3" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="208" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A208" s="2" t="s">
+        <v>863</v>
+      </c>
+      <c r="B208" s="3" t="s">
         <v>864</v>
-      </c>
-      <c r="B208" s="3" t="s">
-        <v>865</v>
       </c>
     </row>
     <row r="209" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -38183,7 +38183,7 @@
         <v>171</v>
       </c>
       <c r="B217" s="3" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="218" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -38191,7 +38191,7 @@
         <v>113</v>
       </c>
       <c r="B218" s="3" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
     </row>
     <row r="219" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -38199,7 +38199,7 @@
         <v>114</v>
       </c>
       <c r="B219" s="3" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="220" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -38207,15 +38207,15 @@
         <v>266</v>
       </c>
       <c r="B220" s="3" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="221" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A221" s="2" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="B221" s="3" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
     </row>
     <row r="222" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -38223,7 +38223,7 @@
         <v>115</v>
       </c>
       <c r="B222" s="3" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="223" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -38239,7 +38239,7 @@
         <v>116</v>
       </c>
       <c r="B224" s="3" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="225" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -38279,7 +38279,7 @@
         <v>738</v>
       </c>
       <c r="B229" s="4" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
     </row>
     <row r="230" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38287,23 +38287,23 @@
         <v>118</v>
       </c>
       <c r="B230" s="3" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
     </row>
     <row r="231" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A231" s="2" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="B231" s="3" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
     </row>
     <row r="232" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A232" s="2" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="B232" s="3" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="233" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38311,23 +38311,23 @@
         <v>119</v>
       </c>
       <c r="B233" s="3" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
     </row>
     <row r="234" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A234" s="2" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="B234" s="3" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
     </row>
     <row r="235" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A235" s="2" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="B235" s="3" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="236" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -38335,7 +38335,7 @@
         <v>120</v>
       </c>
       <c r="B236" s="3" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
     </row>
     <row r="237" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -38343,7 +38343,7 @@
         <v>172</v>
       </c>
       <c r="B237" s="3" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
     </row>
     <row r="238" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -38351,7 +38351,7 @@
         <v>173</v>
       </c>
       <c r="B238" s="3" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
     </row>
     <row r="239" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -38359,7 +38359,7 @@
         <v>174</v>
       </c>
       <c r="B239" s="3" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="240" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -38391,23 +38391,23 @@
         <v>123</v>
       </c>
       <c r="B243" s="3" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
     </row>
     <row r="244" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A244" s="2" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="B244" s="3" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="245" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A245" s="2" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="B245" s="3" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="246" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -38420,10 +38420,10 @@
     </row>
     <row r="247" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A247" s="2" t="s">
+        <v>1104</v>
+      </c>
+      <c r="B247" s="3" t="s">
         <v>1105</v>
-      </c>
-      <c r="B247" s="3" t="s">
-        <v>1106</v>
       </c>
     </row>
     <row r="248" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -38431,15 +38431,15 @@
         <v>125</v>
       </c>
       <c r="B248" s="3" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
     </row>
     <row r="249" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A249" s="2" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="B249" s="3" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="250" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -38447,7 +38447,7 @@
         <v>126</v>
       </c>
       <c r="B250" s="3" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
     </row>
     <row r="251" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -38455,7 +38455,7 @@
         <v>127</v>
       </c>
       <c r="B251" s="3" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
     </row>
     <row r="252" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -38471,7 +38471,7 @@
         <v>129</v>
       </c>
       <c r="B253" s="3" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
     </row>
     <row r="254" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -38479,7 +38479,7 @@
         <v>130</v>
       </c>
       <c r="B254" s="3" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="255" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -38487,23 +38487,23 @@
         <v>131</v>
       </c>
       <c r="B255" s="3" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
     </row>
     <row r="256" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A256" s="2" t="s">
+        <v>908</v>
+      </c>
+      <c r="B256" s="3" t="s">
         <v>909</v>
-      </c>
-      <c r="B256" s="3" t="s">
-        <v>910</v>
       </c>
     </row>
     <row r="257" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A257" s="2" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="B257" s="3" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
     </row>
     <row r="258" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -38511,7 +38511,7 @@
         <v>132</v>
       </c>
       <c r="B258" s="3" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
     </row>
     <row r="259" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38519,15 +38519,15 @@
         <v>133</v>
       </c>
       <c r="B259" s="3" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="260" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A260" s="2" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="B260" s="3" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="261" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -38535,23 +38535,23 @@
         <v>134</v>
       </c>
       <c r="B261" s="3" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
     </row>
     <row r="262" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A262" s="2" t="s">
+        <v>959</v>
+      </c>
+      <c r="B262" s="3" t="s">
         <v>960</v>
-      </c>
-      <c r="B262" s="3" t="s">
-        <v>961</v>
       </c>
     </row>
     <row r="263" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A263" s="2" t="s">
+        <v>961</v>
+      </c>
+      <c r="B263" s="3" t="s">
         <v>962</v>
-      </c>
-      <c r="B263" s="3" t="s">
-        <v>963</v>
       </c>
     </row>
     <row r="264" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -38559,15 +38559,15 @@
         <v>135</v>
       </c>
       <c r="B264" s="3" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
     </row>
     <row r="265" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A265" s="2" t="s">
+        <v>964</v>
+      </c>
+      <c r="B265" s="3" t="s">
         <v>965</v>
-      </c>
-      <c r="B265" s="3" t="s">
-        <v>966</v>
       </c>
     </row>
     <row r="266" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38575,7 +38575,7 @@
         <v>136</v>
       </c>
       <c r="B266" s="3" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
     </row>
     <row r="267" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -38599,7 +38599,7 @@
         <v>233</v>
       </c>
       <c r="B269" s="3" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="270" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -38615,7 +38615,7 @@
         <v>234</v>
       </c>
       <c r="B271" s="3" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="272" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -38623,7 +38623,7 @@
         <v>235</v>
       </c>
       <c r="B272" s="3" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="273" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -38663,7 +38663,7 @@
         <v>140</v>
       </c>
       <c r="B277" s="3" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="278" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -38671,7 +38671,7 @@
         <v>236</v>
       </c>
       <c r="B278" s="3" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="279" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -38679,7 +38679,7 @@
         <v>237</v>
       </c>
       <c r="B279" s="3" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="280" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -38687,7 +38687,7 @@
         <v>238</v>
       </c>
       <c r="B280" s="3" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="281" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -38695,7 +38695,7 @@
         <v>141</v>
       </c>
       <c r="B281" s="3" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="282" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -38703,7 +38703,7 @@
         <v>142</v>
       </c>
       <c r="B282" s="3" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="283" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38711,7 +38711,7 @@
         <v>143</v>
       </c>
       <c r="B283" s="3" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="284" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -38719,7 +38719,7 @@
         <v>144</v>
       </c>
       <c r="B284" s="3" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="285" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -38727,7 +38727,7 @@
         <v>242</v>
       </c>
       <c r="B285" s="3" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="286" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -38735,7 +38735,7 @@
         <v>145</v>
       </c>
       <c r="B286" s="3" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="287" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -38743,7 +38743,7 @@
         <v>146</v>
       </c>
       <c r="B287" s="3" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="288" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -38751,7 +38751,7 @@
         <v>147</v>
       </c>
       <c r="B288" s="3" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="289" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38759,7 +38759,7 @@
         <v>148</v>
       </c>
       <c r="B289" s="3" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="290" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -38767,31 +38767,31 @@
         <v>149</v>
       </c>
       <c r="B290" s="3" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="291" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A291" s="2" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="B291" s="3" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="292" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A292" s="2" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="B292" s="3" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="293" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A293" s="2" t="s">
+        <v>1029</v>
+      </c>
+      <c r="B293" s="3" t="s">
         <v>1030</v>
-      </c>
-      <c r="B293" s="3" t="s">
-        <v>1031</v>
       </c>
     </row>
     <row r="294" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -38799,15 +38799,15 @@
         <v>150</v>
       </c>
       <c r="B294" s="3" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="295" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A295" s="2" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="B295" s="3" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="296" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -38831,7 +38831,7 @@
         <v>244</v>
       </c>
       <c r="B298" s="3" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="299" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -38855,7 +38855,7 @@
         <v>153</v>
       </c>
       <c r="B301" s="3" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="302" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -38935,7 +38935,7 @@
         <v>160</v>
       </c>
       <c r="B311" s="3" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
     </row>
     <row r="312" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -38943,7 +38943,7 @@
         <v>161</v>
       </c>
       <c r="B312" s="3" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
     </row>
     <row r="313" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -38951,31 +38951,31 @@
         <v>162</v>
       </c>
       <c r="B313" s="3" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
     </row>
     <row r="314" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A314" s="2" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="B314" s="3" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
     </row>
     <row r="315" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A315" s="2" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="B315" s="3" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="316" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A316" s="2" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="B316" s="3" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="317" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -38983,7 +38983,7 @@
         <v>163</v>
       </c>
       <c r="B317" s="3" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="318" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -38991,7 +38991,7 @@
         <v>164</v>
       </c>
       <c r="B318" s="3" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
     </row>
     <row r="319" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -38999,7 +38999,7 @@
         <v>175</v>
       </c>
       <c r="B319" s="3" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="320" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -39007,7 +39007,7 @@
         <v>176</v>
       </c>
       <c r="B320" s="3" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
     </row>
     <row r="321" spans="1:2" ht="390" x14ac:dyDescent="0.25">
@@ -39015,7 +39015,7 @@
         <v>177</v>
       </c>
       <c r="B321" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="322" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -39023,7 +39023,7 @@
         <v>514</v>
       </c>
       <c r="B322" s="3" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
     </row>
     <row r="323" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -39031,7 +39031,7 @@
         <v>515</v>
       </c>
       <c r="B323" s="3" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
     </row>
     <row r="324" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -39039,7 +39039,7 @@
         <v>516</v>
       </c>
       <c r="B324" s="3" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
     </row>
     <row r="325" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -39047,7 +39047,7 @@
         <v>517</v>
       </c>
       <c r="B325" s="3" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="326" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -39055,7 +39055,7 @@
         <v>518</v>
       </c>
       <c r="B326" s="3" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="327" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -39063,15 +39063,15 @@
         <v>519</v>
       </c>
       <c r="B327" s="3" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
     </row>
     <row r="328" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A328" s="2" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="B328" s="3" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="329" spans="1:2" ht="390" x14ac:dyDescent="0.25">
@@ -39079,7 +39079,7 @@
         <v>178</v>
       </c>
       <c r="B329" s="3" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="330" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -39087,7 +39087,7 @@
         <v>489</v>
       </c>
       <c r="B330" s="3" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
     </row>
     <row r="331" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -39095,7 +39095,7 @@
         <v>541</v>
       </c>
       <c r="B331" s="3" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="332" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -39103,7 +39103,7 @@
         <v>542</v>
       </c>
       <c r="B332" s="3" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
     </row>
     <row r="333" spans="1:2" ht="315" x14ac:dyDescent="0.25">
@@ -39119,7 +39119,7 @@
         <v>249</v>
       </c>
       <c r="B334" s="3" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="335" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -39143,7 +39143,7 @@
         <v>252</v>
       </c>
       <c r="B337" s="3" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="338" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -39167,7 +39167,7 @@
         <v>819</v>
       </c>
       <c r="B340" s="3" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
     </row>
     <row r="341" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -39175,7 +39175,7 @@
         <v>180</v>
       </c>
       <c r="B341" s="3" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
     </row>
     <row r="342" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39199,15 +39199,15 @@
         <v>182</v>
       </c>
       <c r="B344" s="3" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="345" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A345" s="2" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="B345" s="3" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="346" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39215,7 +39215,7 @@
         <v>183</v>
       </c>
       <c r="B346" s="3" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="347" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -39223,7 +39223,7 @@
         <v>184</v>
       </c>
       <c r="B347" s="3" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="348" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -39239,7 +39239,7 @@
         <v>185</v>
       </c>
       <c r="B349" s="3" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="350" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -39263,7 +39263,7 @@
         <v>464</v>
       </c>
       <c r="B352" s="3" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="353" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -39335,7 +39335,7 @@
         <v>193</v>
       </c>
       <c r="B361" s="3" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="362" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -39343,7 +39343,7 @@
         <v>336</v>
       </c>
       <c r="B362" s="3" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
     </row>
     <row r="363" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -39351,71 +39351,71 @@
         <v>337</v>
       </c>
       <c r="B363" s="3" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="364" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A364" s="2" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
       <c r="B364" s="3" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="365" spans="1:2" ht="225" x14ac:dyDescent="0.25">
       <c r="A365" s="2" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
       <c r="B365" s="3" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="366" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A366" s="2" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="B366" s="3" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="367" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A367" s="2" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="B367" s="3" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="368" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A368" s="2" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="B368" s="3" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="369" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A369" s="2" t="s">
+        <v>1141</v>
+      </c>
+      <c r="B369" s="3" t="s">
         <v>1142</v>
-      </c>
-      <c r="B369" s="3" t="s">
-        <v>1143</v>
       </c>
     </row>
     <row r="370" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A370" s="2" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="B370" s="3" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="371" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A371" s="2" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="B371" s="3" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="372" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -39431,15 +39431,15 @@
         <v>195</v>
       </c>
       <c r="B373" s="3" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="374" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A374" s="2" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
       <c r="B374" s="3" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="375" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -39447,7 +39447,7 @@
         <v>196</v>
       </c>
       <c r="B375" s="3" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
     </row>
     <row r="376" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -39455,7 +39455,7 @@
         <v>328</v>
       </c>
       <c r="B376" s="3" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
     </row>
     <row r="377" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -39471,7 +39471,7 @@
         <v>649</v>
       </c>
       <c r="B378" s="3" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="379" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39495,7 +39495,7 @@
         <v>200</v>
       </c>
       <c r="B381" s="3" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="382" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -39511,7 +39511,7 @@
         <v>202</v>
       </c>
       <c r="B383" s="3" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
     </row>
     <row r="384" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -39631,7 +39631,7 @@
         <v>580</v>
       </c>
       <c r="B398" s="3" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
     </row>
     <row r="399" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -39639,7 +39639,7 @@
         <v>581</v>
       </c>
       <c r="B399" s="3" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
     </row>
     <row r="400" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -39647,7 +39647,7 @@
         <v>582</v>
       </c>
       <c r="B400" s="3" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
     </row>
     <row r="401" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -39655,7 +39655,7 @@
         <v>583</v>
       </c>
       <c r="B401" s="3" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
     </row>
     <row r="402" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39671,7 +39671,7 @@
         <v>585</v>
       </c>
       <c r="B403" s="3" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="404" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39687,7 +39687,7 @@
         <v>207</v>
       </c>
       <c r="B405" s="3" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
     </row>
     <row r="406" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -39703,7 +39703,7 @@
         <v>209</v>
       </c>
       <c r="B407" s="3" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="408" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -39756,10 +39756,10 @@
     </row>
     <row r="414" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A414" s="2" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="B414" s="3" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="415" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -39767,7 +39767,7 @@
         <v>210</v>
       </c>
       <c r="B415" s="3" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="416" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -39775,7 +39775,7 @@
         <v>619</v>
       </c>
       <c r="B416" s="3" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="417" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -39828,10 +39828,10 @@
     </row>
     <row r="423" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A423" s="2" t="s">
+        <v>1114</v>
+      </c>
+      <c r="B423" s="3" t="s">
         <v>1115</v>
-      </c>
-      <c r="B423" s="3" t="s">
-        <v>1116</v>
       </c>
     </row>
     <row r="424" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -39855,7 +39855,7 @@
         <v>530</v>
       </c>
       <c r="B426" s="3" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="427" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -39887,7 +39887,7 @@
         <v>213</v>
       </c>
       <c r="B430" s="3" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
     </row>
     <row r="431" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -39903,7 +39903,7 @@
         <v>215</v>
       </c>
       <c r="B432" s="3" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="433" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39951,7 +39951,7 @@
         <v>221</v>
       </c>
       <c r="B438" s="3" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="439" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -39959,7 +39959,7 @@
         <v>222</v>
       </c>
       <c r="B439" s="3" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="440" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -39967,7 +39967,7 @@
         <v>223</v>
       </c>
       <c r="B440" s="3" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="441" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -39975,7 +39975,7 @@
         <v>224</v>
       </c>
       <c r="B441" s="3" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="442" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -39983,7 +39983,7 @@
         <v>329</v>
       </c>
       <c r="B442" s="3" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="443" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -39999,7 +39999,7 @@
         <v>225</v>
       </c>
       <c r="B444" s="3" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
     </row>
     <row r="445" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -40023,15 +40023,15 @@
         <v>228</v>
       </c>
       <c r="B447" s="3" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="448" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A448" s="2" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="B448" s="3" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="449" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -40071,7 +40071,7 @@
         <v>442</v>
       </c>
       <c r="B453" s="3" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="454" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -40111,7 +40111,7 @@
         <v>319</v>
       </c>
       <c r="B458" s="3" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="459" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -40119,7 +40119,7 @@
         <v>320</v>
       </c>
       <c r="B459" s="3" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="460" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -40127,7 +40127,7 @@
         <v>321</v>
       </c>
       <c r="B460" s="3" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="461" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -40135,15 +40135,15 @@
         <v>318</v>
       </c>
       <c r="B461" s="3" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="462" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A462" s="2" t="s">
+        <v>1005</v>
+      </c>
+      <c r="B462" s="3" t="s">
         <v>1006</v>
-      </c>
-      <c r="B462" s="3" t="s">
-        <v>1007</v>
       </c>
     </row>
     <row r="463" spans="1:2" ht="255" x14ac:dyDescent="0.25">
@@ -40151,7 +40151,7 @@
         <v>322</v>
       </c>
       <c r="B463" s="3" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="464" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -40175,7 +40175,7 @@
         <v>483</v>
       </c>
       <c r="B466" s="3" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="467" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -40183,7 +40183,7 @@
         <v>484</v>
       </c>
       <c r="B467" s="3" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="468" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -40215,7 +40215,7 @@
         <v>550</v>
       </c>
       <c r="B471" s="3" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
     </row>
     <row r="472" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -40223,7 +40223,7 @@
         <v>554</v>
       </c>
       <c r="B472" s="3" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="473" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -40239,7 +40239,7 @@
         <v>558</v>
       </c>
       <c r="B474" s="3" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
     </row>
     <row r="475" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -40263,7 +40263,7 @@
         <v>561</v>
       </c>
       <c r="B477" s="3" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
     </row>
     <row r="478" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -40271,7 +40271,7 @@
         <v>562</v>
       </c>
       <c r="B478" s="3" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="479" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -40287,7 +40287,7 @@
         <v>564</v>
       </c>
       <c r="B480" s="3" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
     </row>
     <row r="481" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -40319,7 +40319,7 @@
         <v>594</v>
       </c>
       <c r="B484" s="3" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
     </row>
     <row r="485" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -40327,7 +40327,7 @@
         <v>612</v>
       </c>
       <c r="B485" s="3" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="486" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -40335,7 +40335,7 @@
         <v>613</v>
       </c>
       <c r="B486" s="3" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="487" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -40343,7 +40343,7 @@
         <v>614</v>
       </c>
       <c r="B487" s="3" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="488" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -40351,15 +40351,15 @@
         <v>834</v>
       </c>
       <c r="B488" s="3" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="489" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A489" s="2" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="B489" s="3" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="490" spans="1:2" ht="255" x14ac:dyDescent="0.25">
@@ -40415,7 +40415,7 @@
         <v>656</v>
       </c>
       <c r="B496" s="1" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
     </row>
     <row r="497" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -40455,7 +40455,7 @@
         <v>661</v>
       </c>
       <c r="B501" s="1" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
     </row>
     <row r="502" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -40484,18 +40484,18 @@
     </row>
     <row r="505" spans="1:2" ht="255" x14ac:dyDescent="0.25">
       <c r="A505" s="2" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="B505" s="1" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
     </row>
     <row r="506" spans="1:2" ht="92.25" x14ac:dyDescent="0.25">
       <c r="A506" s="2" t="s">
+        <v>987</v>
+      </c>
+      <c r="B506" s="1" t="s">
         <v>988</v>
-      </c>
-      <c r="B506" s="1" t="s">
-        <v>989</v>
       </c>
     </row>
     <row r="507" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -40503,7 +40503,7 @@
         <v>678</v>
       </c>
       <c r="B507" s="1" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
     </row>
     <row r="508" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -40511,7 +40511,7 @@
         <v>710</v>
       </c>
       <c r="B508" s="3" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="509" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -40607,7 +40607,7 @@
         <v>275</v>
       </c>
       <c r="B520" s="1" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="521" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -40615,7 +40615,7 @@
         <v>276</v>
       </c>
       <c r="B521" s="1" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="522" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -40623,7 +40623,7 @@
         <v>277</v>
       </c>
       <c r="B522" s="1" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="523" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -40671,7 +40671,7 @@
         <v>260</v>
       </c>
       <c r="B528" s="3" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
     </row>
     <row r="529" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -40743,7 +40743,7 @@
         <v>285</v>
       </c>
       <c r="B537" s="1" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="538" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -40751,7 +40751,7 @@
         <v>286</v>
       </c>
       <c r="B538" s="1" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
     <row r="539" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -40871,7 +40871,7 @@
         <v>298</v>
       </c>
       <c r="B553" s="1" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
     </row>
     <row r="554" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -40911,7 +40911,7 @@
         <v>300</v>
       </c>
       <c r="B558" s="1" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
     </row>
     <row r="559" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -40919,7 +40919,7 @@
         <v>301</v>
       </c>
       <c r="B559" s="1" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
     </row>
     <row r="560" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -41047,7 +41047,7 @@
         <v>307</v>
       </c>
       <c r="B575" s="1" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
     </row>
     <row r="576" spans="1:2" ht="375" x14ac:dyDescent="0.25">
@@ -41079,7 +41079,7 @@
         <v>371</v>
       </c>
       <c r="B579" s="3" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
     </row>
     <row r="580" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -41095,7 +41095,7 @@
         <v>326</v>
       </c>
       <c r="B581" s="3" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert to previous working version without images created in EventViewer
</commit_message>
<xml_diff>
--- a/Documentation/Events.xlsx
+++ b/Documentation/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\happysulla\BarbarianPrince\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{1E801356-D03B-4768-8B4C-4FC6DE77085D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1559771E-7CF8-4C1E-99BB-D94844D46CB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Events" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20938,29 +20937,6 @@
     </r>
   </si>
   <si>
-    <t>&lt;Bold&gt;e156c Town Mayor Favor&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-He hears your story with favor. He gives you a letter or recommendation &lt;InlineUIContainer&gt;&lt;Button Content='r212' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
- to the Lord at the nearest castle. You cannot seek another audience with him for at least a week. Click image to continue.</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e156d Town Mayor Interest&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-He hears your story with interest. He gives you a letter of recommendation to the Lord of the nearest castle
- &lt;InlineUIContainer&gt;&lt;Button Content='e157' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
- and gives you 50 gold for expenses. You cannot seek another audience with him until you have used the letter. Click image to continue.</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e156a Town Mayor Stone Faced&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-He hears your story but remains stone-faced and unwilling or unable to help. However, you are free to seek audiences with him again any day. Select image to continue.</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e156b Town Mayor Free Food and Lodging&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-He hears your story and gives you free food and lodging for tonight as a distinguished if dispossessed visitor from the north. You are free to seek audiences with him again any day. Click image to continue.</t>
-  </si>
-  <si>
     <t>e007d</t>
   </si>
   <si>
@@ -35819,11 +35795,6 @@
     <t>e156g</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e156f Town Mayor Religious Interest Thwarted&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Since your party does not includes a monk or priest, he dismisses you and refuses any further audiences until you have such a character in your party. When you do have a monk or priest, he will provide a letter of recommendation to any castle or temple you request, gives you wealth 100, and his trusted assistant becomes a member of your party. Click image to continue.</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;e156e Town Mayor Religious Interest Stoked&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 Since your party includes a monk or priest, he will support your cause for religious reasons. 
@@ -35988,6 +35959,34 @@
       </rPr>
       <t>' Height='300' Width='300'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
     </r>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e156a Town Mayor Stone Faced&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+He hears your story but remains stone-faced and unwilling or unable to help. However, you are free to seek audiences with him again any day.</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e156b Town Mayor Free Food and Lodging&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+He hears your story and gives you free food and lodging for tonight as a distinguished if dispossessed visitor from the north. You are free to seek audiences with him again any day.</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e156c Town Mayor Favor&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+He hears your story with favor. He gives you a letter or recommendation &lt;InlineUIContainer&gt;&lt;Button Content='r212' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+ to the Lord at the nearest castle. You cannot seek another audience with him for at least a week.</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e156d Town Mayor Interest&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+He hears your story with interest. He gives you a letter of recommendation to the Lord of the nearest castle
+ &lt;InlineUIContainer&gt;&lt;Button Content='e157' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+ and gives you 50 gold for expenses. You cannot seek another audience with him until you have used the letter.</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e156f Town Mayor Religious Interest Thwarted&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Since your party does not includes a monk or priest, he dismisses you and refuses any further audiences until you have such a character in your party. When you do have a monk or priest, he will provide a letter of recommendation to any castle or temple you request, gives you wealth 100, and his trusted assistant becomes a member of your party.</t>
   </si>
 </sst>
 </file>
@@ -36453,8 +36452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B582"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A372" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A375" sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A532" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A536" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -36468,7 +36467,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1096</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -36476,7 +36475,7 @@
         <v>254</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1039</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -36484,7 +36483,7 @@
         <v>255</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>1038</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -36492,15 +36491,15 @@
         <v>256</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>1036</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>1035</v>
+        <v>1031</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>1037</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="390" x14ac:dyDescent="0.25">
@@ -36524,7 +36523,7 @@
         <v>22</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>1041</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -36540,7 +36539,7 @@
         <v>23</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>1098</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -36556,7 +36555,7 @@
         <v>3</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>968</v>
+        <v>964</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -36620,7 +36619,7 @@
         <v>11</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>1095</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -36716,7 +36715,7 @@
         <v>19</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>863</v>
+        <v>859</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -36724,7 +36723,7 @@
         <v>20</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>864</v>
+        <v>860</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -36732,23 +36731,23 @@
         <v>21</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>1085</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>858</v>
+        <v>854</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>1087</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>859</v>
+        <v>855</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>1086</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -36756,23 +36755,23 @@
         <v>25</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>991</v>
+        <v>987</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
+        <v>871</v>
+      </c>
+      <c r="B38" s="3" t="s">
         <v>875</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>879</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>876</v>
+        <v>872</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>878</v>
+        <v>874</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -36780,7 +36779,7 @@
         <v>26</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>983</v>
+        <v>979</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -36804,7 +36803,7 @@
         <v>27</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>1089</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -36812,7 +36811,7 @@
         <v>28</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>1092</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -36820,7 +36819,7 @@
         <v>29</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>1090</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -36828,7 +36827,7 @@
         <v>30</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>1093</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -36844,7 +36843,7 @@
         <v>691</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>1088</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -36852,7 +36851,7 @@
         <v>31</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>1104</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -36860,7 +36859,7 @@
         <v>32</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>1094</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -36868,7 +36867,7 @@
         <v>33</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>1091</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -36900,7 +36899,7 @@
         <v>491</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>1058</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -36924,7 +36923,7 @@
         <v>264</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>993</v>
+        <v>989</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -36932,7 +36931,7 @@
         <v>265</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>992</v>
+        <v>988</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37068,7 +37067,7 @@
         <v>42</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>966</v>
+        <v>962</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37076,7 +37075,7 @@
         <v>46</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>1022</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -37196,7 +37195,7 @@
         <v>772</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>1062</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -37209,10 +37208,10 @@
     </row>
     <row r="94" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
-        <v>870</v>
+        <v>866</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>871</v>
+        <v>867</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -37228,7 +37227,7 @@
         <v>762</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>1063</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -37284,7 +37283,7 @@
         <v>66</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>940</v>
+        <v>936</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37332,7 +37331,7 @@
         <v>469</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>1064</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -37364,7 +37363,7 @@
         <v>70</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>973</v>
+        <v>969</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -37428,7 +37427,7 @@
         <v>75</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>1151</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="122" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -37436,15 +37435,15 @@
         <v>325</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>1150</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="123" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
-        <v>1149</v>
+        <v>1145</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>1152</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="124" spans="1:2" ht="270" x14ac:dyDescent="0.25">
@@ -37460,7 +37459,7 @@
         <v>77</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>917</v>
+        <v>913</v>
       </c>
     </row>
     <row r="126" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -37473,10 +37472,10 @@
     </row>
     <row r="127" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
-        <v>916</v>
+        <v>912</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>1065</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="128" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -37484,7 +37483,7 @@
         <v>78</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>872</v>
+        <v>868</v>
       </c>
     </row>
     <row r="129" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -37492,7 +37491,7 @@
         <v>372</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>873</v>
+        <v>869</v>
       </c>
     </row>
     <row r="130" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37540,87 +37539,87 @@
         <v>81</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>920</v>
+        <v>916</v>
       </c>
     </row>
     <row r="136" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
-        <v>918</v>
+        <v>914</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>929</v>
+        <v>925</v>
       </c>
     </row>
     <row r="137" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
-        <v>919</v>
+        <v>915</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>928</v>
+        <v>924</v>
       </c>
     </row>
     <row r="138" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
-        <v>921</v>
+        <v>917</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>935</v>
+        <v>931</v>
       </c>
     </row>
     <row r="139" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
-        <v>922</v>
+        <v>918</v>
       </c>
       <c r="B139" s="3" t="s">
-        <v>936</v>
+        <v>932</v>
       </c>
     </row>
     <row r="140" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
-        <v>923</v>
+        <v>919</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>937</v>
+        <v>933</v>
       </c>
     </row>
     <row r="141" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
-        <v>924</v>
+        <v>920</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>927</v>
+        <v>923</v>
       </c>
     </row>
     <row r="142" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
-        <v>925</v>
+        <v>921</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>939</v>
+        <v>935</v>
       </c>
     </row>
     <row r="143" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
-        <v>926</v>
+        <v>922</v>
       </c>
       <c r="B143" s="3" t="s">
-        <v>938</v>
+        <v>934</v>
       </c>
     </row>
     <row r="144" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
-        <v>930</v>
+        <v>926</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>931</v>
+        <v>927</v>
       </c>
     </row>
     <row r="145" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
-        <v>932</v>
+        <v>928</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>934</v>
+        <v>930</v>
       </c>
     </row>
     <row r="146" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37628,7 +37627,7 @@
         <v>82</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>933</v>
+        <v>929</v>
       </c>
     </row>
     <row r="147" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -37641,7 +37640,7 @@
     </row>
     <row r="148" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
-        <v>1055</v>
+        <v>1051</v>
       </c>
       <c r="B148" s="3" t="s">
         <v>545</v>
@@ -37676,7 +37675,7 @@
         <v>544</v>
       </c>
       <c r="B152" s="3" t="s">
-        <v>1126</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="153" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -37764,7 +37763,7 @@
         <v>344</v>
       </c>
       <c r="B163" s="3" t="s">
-        <v>1107</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="164" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -37796,7 +37795,7 @@
         <v>438</v>
       </c>
       <c r="B167" s="3" t="s">
-        <v>882</v>
+        <v>878</v>
       </c>
     </row>
     <row r="168" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -37908,7 +37907,7 @@
         <v>825</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>1066</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="182" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37916,7 +37915,7 @@
         <v>826</v>
       </c>
       <c r="B182" s="3" t="s">
-        <v>1067</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="183" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -37924,7 +37923,7 @@
         <v>829</v>
       </c>
       <c r="B183" s="3" t="s">
-        <v>1068</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="184" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -37948,7 +37947,7 @@
         <v>97</v>
       </c>
       <c r="B186" s="3" t="s">
-        <v>1156</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="187" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -37996,7 +37995,7 @@
         <v>103</v>
       </c>
       <c r="B192" s="3" t="s">
-        <v>951</v>
+        <v>947</v>
       </c>
     </row>
     <row r="193" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -38004,7 +38003,7 @@
         <v>104</v>
       </c>
       <c r="B193" s="3" t="s">
-        <v>915</v>
+        <v>911</v>
       </c>
     </row>
     <row r="194" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -38020,7 +38019,7 @@
         <v>678</v>
       </c>
       <c r="B195" s="3" t="s">
-        <v>1069</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="196" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -38036,7 +38035,7 @@
         <v>106</v>
       </c>
       <c r="B197" s="3" t="s">
-        <v>941</v>
+        <v>937</v>
       </c>
     </row>
     <row r="198" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -38068,7 +38067,7 @@
         <v>108</v>
       </c>
       <c r="B201" s="3" t="s">
-        <v>955</v>
+        <v>951</v>
       </c>
     </row>
     <row r="202" spans="1:2" ht="285" x14ac:dyDescent="0.25">
@@ -38076,7 +38075,7 @@
         <v>109</v>
       </c>
       <c r="B202" s="3" t="s">
-        <v>890</v>
+        <v>886</v>
       </c>
     </row>
     <row r="203" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -38092,7 +38091,7 @@
         <v>166</v>
       </c>
       <c r="B204" s="3" t="s">
-        <v>1023</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="205" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -38100,7 +38099,7 @@
         <v>167</v>
       </c>
       <c r="B205" s="3" t="s">
-        <v>1034</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="206" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -38108,23 +38107,23 @@
         <v>168</v>
       </c>
       <c r="B206" s="3" t="s">
-        <v>866</v>
+        <v>862</v>
       </c>
     </row>
     <row r="207" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A207" s="2" t="s">
-        <v>860</v>
+        <v>856</v>
       </c>
       <c r="B207" s="3" t="s">
-        <v>1070</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="208" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A208" s="2" t="s">
-        <v>861</v>
+        <v>857</v>
       </c>
       <c r="B208" s="3" t="s">
-        <v>862</v>
+        <v>858</v>
       </c>
     </row>
     <row r="209" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -38196,7 +38195,7 @@
         <v>171</v>
       </c>
       <c r="B217" s="3" t="s">
-        <v>1050</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="218" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -38204,7 +38203,7 @@
         <v>113</v>
       </c>
       <c r="B218" s="3" t="s">
-        <v>984</v>
+        <v>980</v>
       </c>
     </row>
     <row r="219" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -38212,7 +38211,7 @@
         <v>114</v>
       </c>
       <c r="B219" s="3" t="s">
-        <v>884</v>
+        <v>880</v>
       </c>
     </row>
     <row r="220" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -38220,15 +38219,15 @@
         <v>266</v>
       </c>
       <c r="B220" s="3" t="s">
-        <v>885</v>
+        <v>881</v>
       </c>
     </row>
     <row r="221" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A221" s="2" t="s">
-        <v>883</v>
+        <v>879</v>
       </c>
       <c r="B221" s="3" t="s">
-        <v>886</v>
+        <v>882</v>
       </c>
     </row>
     <row r="222" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -38236,7 +38235,7 @@
         <v>115</v>
       </c>
       <c r="B222" s="3" t="s">
-        <v>904</v>
+        <v>900</v>
       </c>
     </row>
     <row r="223" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -38252,7 +38251,7 @@
         <v>116</v>
       </c>
       <c r="B224" s="3" t="s">
-        <v>1016</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="225" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -38292,7 +38291,7 @@
         <v>736</v>
       </c>
       <c r="B229" s="4" t="s">
-        <v>894</v>
+        <v>890</v>
       </c>
     </row>
     <row r="230" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38300,23 +38299,23 @@
         <v>118</v>
       </c>
       <c r="B230" s="3" t="s">
-        <v>895</v>
+        <v>891</v>
       </c>
     </row>
     <row r="231" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A231" s="2" t="s">
-        <v>891</v>
+        <v>887</v>
       </c>
       <c r="B231" s="3" t="s">
-        <v>893</v>
+        <v>889</v>
       </c>
     </row>
     <row r="232" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A232" s="2" t="s">
-        <v>892</v>
+        <v>888</v>
       </c>
       <c r="B232" s="3" t="s">
-        <v>1012</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="233" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38324,23 +38323,23 @@
         <v>119</v>
       </c>
       <c r="B233" s="3" t="s">
-        <v>869</v>
+        <v>865</v>
       </c>
     </row>
     <row r="234" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A234" s="2" t="s">
-        <v>868</v>
+        <v>864</v>
       </c>
       <c r="B234" s="3" t="s">
-        <v>877</v>
+        <v>873</v>
       </c>
     </row>
     <row r="235" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A235" s="2" t="s">
-        <v>867</v>
+        <v>863</v>
       </c>
       <c r="B235" s="3" t="s">
-        <v>1071</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="236" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -38348,7 +38347,7 @@
         <v>120</v>
       </c>
       <c r="B236" s="3" t="s">
-        <v>914</v>
+        <v>910</v>
       </c>
     </row>
     <row r="237" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -38356,7 +38355,7 @@
         <v>172</v>
       </c>
       <c r="B237" s="3" t="s">
-        <v>912</v>
+        <v>908</v>
       </c>
     </row>
     <row r="238" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -38364,7 +38363,7 @@
         <v>173</v>
       </c>
       <c r="B238" s="3" t="s">
-        <v>911</v>
+        <v>907</v>
       </c>
     </row>
     <row r="239" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -38372,7 +38371,7 @@
         <v>174</v>
       </c>
       <c r="B239" s="3" t="s">
-        <v>913</v>
+        <v>909</v>
       </c>
     </row>
     <row r="240" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -38404,23 +38403,23 @@
         <v>123</v>
       </c>
       <c r="B243" s="3" t="s">
-        <v>889</v>
+        <v>885</v>
       </c>
     </row>
     <row r="244" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A244" s="2" t="s">
-        <v>887</v>
+        <v>883</v>
       </c>
       <c r="B244" s="3" t="s">
-        <v>1072</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="245" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A245" s="2" t="s">
-        <v>888</v>
+        <v>884</v>
       </c>
       <c r="B245" s="3" t="s">
-        <v>1073</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="246" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -38433,10 +38432,10 @@
     </row>
     <row r="247" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A247" s="2" t="s">
-        <v>1101</v>
+        <v>1097</v>
       </c>
       <c r="B247" s="3" t="s">
-        <v>1102</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="248" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -38444,15 +38443,15 @@
         <v>125</v>
       </c>
       <c r="B248" s="3" t="s">
-        <v>948</v>
+        <v>944</v>
       </c>
     </row>
     <row r="249" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A249" s="2" t="s">
-        <v>947</v>
+        <v>943</v>
       </c>
       <c r="B249" s="3" t="s">
-        <v>1061</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="250" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -38460,7 +38459,7 @@
         <v>126</v>
       </c>
       <c r="B250" s="3" t="s">
-        <v>954</v>
+        <v>950</v>
       </c>
     </row>
     <row r="251" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -38468,7 +38467,7 @@
         <v>127</v>
       </c>
       <c r="B251" s="3" t="s">
-        <v>905</v>
+        <v>901</v>
       </c>
     </row>
     <row r="252" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -38484,7 +38483,7 @@
         <v>129</v>
       </c>
       <c r="B253" s="3" t="s">
-        <v>953</v>
+        <v>949</v>
       </c>
     </row>
     <row r="254" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -38492,7 +38491,7 @@
         <v>130</v>
       </c>
       <c r="B254" s="3" t="s">
-        <v>903</v>
+        <v>899</v>
       </c>
     </row>
     <row r="255" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -38500,23 +38499,23 @@
         <v>131</v>
       </c>
       <c r="B255" s="3" t="s">
-        <v>909</v>
+        <v>905</v>
       </c>
     </row>
     <row r="256" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A256" s="2" t="s">
-        <v>906</v>
+        <v>902</v>
       </c>
       <c r="B256" s="3" t="s">
-        <v>907</v>
+        <v>903</v>
       </c>
     </row>
     <row r="257" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A257" s="2" t="s">
-        <v>908</v>
+        <v>904</v>
       </c>
       <c r="B257" s="3" t="s">
-        <v>910</v>
+        <v>906</v>
       </c>
     </row>
     <row r="258" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -38524,7 +38523,7 @@
         <v>132</v>
       </c>
       <c r="B258" s="3" t="s">
-        <v>961</v>
+        <v>957</v>
       </c>
     </row>
     <row r="259" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38532,15 +38531,15 @@
         <v>133</v>
       </c>
       <c r="B259" s="3" t="s">
-        <v>1074</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="260" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A260" s="2" t="s">
-        <v>902</v>
+        <v>898</v>
       </c>
       <c r="B260" s="3" t="s">
-        <v>1002</v>
+        <v>998</v>
       </c>
     </row>
     <row r="261" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -38548,23 +38547,23 @@
         <v>134</v>
       </c>
       <c r="B261" s="3" t="s">
-        <v>956</v>
+        <v>952</v>
       </c>
     </row>
     <row r="262" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A262" s="2" t="s">
-        <v>957</v>
+        <v>953</v>
       </c>
       <c r="B262" s="3" t="s">
-        <v>958</v>
+        <v>954</v>
       </c>
     </row>
     <row r="263" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A263" s="2" t="s">
-        <v>959</v>
+        <v>955</v>
       </c>
       <c r="B263" s="3" t="s">
-        <v>960</v>
+        <v>956</v>
       </c>
     </row>
     <row r="264" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -38572,15 +38571,15 @@
         <v>135</v>
       </c>
       <c r="B264" s="3" t="s">
-        <v>964</v>
+        <v>960</v>
       </c>
     </row>
     <row r="265" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A265" s="2" t="s">
-        <v>962</v>
+        <v>958</v>
       </c>
       <c r="B265" s="3" t="s">
-        <v>963</v>
+        <v>959</v>
       </c>
     </row>
     <row r="266" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38588,7 +38587,7 @@
         <v>136</v>
       </c>
       <c r="B266" s="3" t="s">
-        <v>965</v>
+        <v>961</v>
       </c>
     </row>
     <row r="267" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -38612,7 +38611,7 @@
         <v>233</v>
       </c>
       <c r="B269" s="3" t="s">
-        <v>1100</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="270" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -38628,7 +38627,7 @@
         <v>234</v>
       </c>
       <c r="B271" s="3" t="s">
-        <v>1075</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="272" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -38636,7 +38635,7 @@
         <v>235</v>
       </c>
       <c r="B272" s="3" t="s">
-        <v>1076</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="273" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -38676,7 +38675,7 @@
         <v>140</v>
       </c>
       <c r="B277" s="3" t="s">
-        <v>1018</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="278" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -38684,7 +38683,7 @@
         <v>236</v>
       </c>
       <c r="B278" s="3" t="s">
-        <v>1024</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="279" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -38692,7 +38691,7 @@
         <v>237</v>
       </c>
       <c r="B279" s="3" t="s">
-        <v>1017</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="280" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -38700,7 +38699,7 @@
         <v>238</v>
       </c>
       <c r="B280" s="3" t="s">
-        <v>1077</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="281" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -38708,7 +38707,7 @@
         <v>141</v>
       </c>
       <c r="B281" s="3" t="s">
-        <v>1005</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="282" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -38716,7 +38715,7 @@
         <v>142</v>
       </c>
       <c r="B282" s="3" t="s">
-        <v>1006</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="283" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38724,7 +38723,7 @@
         <v>143</v>
       </c>
       <c r="B283" s="3" t="s">
-        <v>1007</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="284" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -38732,7 +38731,7 @@
         <v>144</v>
       </c>
       <c r="B284" s="3" t="s">
-        <v>1011</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="285" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -38740,7 +38739,7 @@
         <v>242</v>
       </c>
       <c r="B285" s="3" t="s">
-        <v>1013</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="286" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -38748,7 +38747,7 @@
         <v>145</v>
       </c>
       <c r="B286" s="3" t="s">
-        <v>1010</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="287" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -38756,7 +38755,7 @@
         <v>146</v>
       </c>
       <c r="B287" s="3" t="s">
-        <v>1014</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="288" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -38764,7 +38763,7 @@
         <v>147</v>
       </c>
       <c r="B288" s="3" t="s">
-        <v>1009</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="289" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -38772,7 +38771,7 @@
         <v>148</v>
       </c>
       <c r="B289" s="3" t="s">
-        <v>1015</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="290" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -38780,31 +38779,31 @@
         <v>149</v>
       </c>
       <c r="B290" s="3" t="s">
-        <v>1029</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="291" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A291" s="2" t="s">
-        <v>1026</v>
+        <v>1022</v>
       </c>
       <c r="B291" s="3" t="s">
-        <v>1099</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="292" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A292" s="2" t="s">
-        <v>1025</v>
+        <v>1021</v>
       </c>
       <c r="B292" s="3" t="s">
-        <v>1030</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="293" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A293" s="2" t="s">
-        <v>1027</v>
+        <v>1023</v>
       </c>
       <c r="B293" s="3" t="s">
-        <v>1028</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="294" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -38812,15 +38811,15 @@
         <v>150</v>
       </c>
       <c r="B294" s="3" t="s">
-        <v>1032</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="295" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A295" s="2" t="s">
-        <v>1031</v>
+        <v>1027</v>
       </c>
       <c r="B295" s="3" t="s">
-        <v>1033</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="296" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -38844,7 +38843,7 @@
         <v>244</v>
       </c>
       <c r="B298" s="3" t="s">
-        <v>1103</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="299" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -38868,7 +38867,7 @@
         <v>153</v>
       </c>
       <c r="B301" s="3" t="s">
-        <v>1008</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="302" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -38948,7 +38947,7 @@
         <v>160</v>
       </c>
       <c r="B311" s="3" t="s">
-        <v>950</v>
+        <v>946</v>
       </c>
     </row>
     <row r="312" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -38956,7 +38955,7 @@
         <v>161</v>
       </c>
       <c r="B312" s="3" t="s">
-        <v>981</v>
+        <v>977</v>
       </c>
     </row>
     <row r="313" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -38964,31 +38963,31 @@
         <v>162</v>
       </c>
       <c r="B313" s="3" t="s">
-        <v>996</v>
+        <v>992</v>
       </c>
     </row>
     <row r="314" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A314" s="2" t="s">
-        <v>994</v>
+        <v>990</v>
       </c>
       <c r="B314" s="3" t="s">
-        <v>997</v>
+        <v>993</v>
       </c>
     </row>
     <row r="315" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A315" s="2" t="s">
+        <v>991</v>
+      </c>
+      <c r="B315" s="3" t="s">
         <v>995</v>
-      </c>
-      <c r="B315" s="3" t="s">
-        <v>999</v>
       </c>
     </row>
     <row r="316" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A316" s="2" t="s">
-        <v>998</v>
+        <v>994</v>
       </c>
       <c r="B316" s="3" t="s">
-        <v>1000</v>
+        <v>996</v>
       </c>
     </row>
     <row r="317" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -38996,7 +38995,7 @@
         <v>163</v>
       </c>
       <c r="B317" s="3" t="s">
-        <v>1001</v>
+        <v>997</v>
       </c>
     </row>
     <row r="318" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -39004,7 +39003,7 @@
         <v>164</v>
       </c>
       <c r="B318" s="3" t="s">
-        <v>989</v>
+        <v>985</v>
       </c>
     </row>
     <row r="319" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -39012,7 +39011,7 @@
         <v>175</v>
       </c>
       <c r="B319" s="3" t="s">
-        <v>988</v>
+        <v>984</v>
       </c>
     </row>
     <row r="320" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -39020,7 +39019,7 @@
         <v>176</v>
       </c>
       <c r="B320" s="3" t="s">
-        <v>987</v>
+        <v>983</v>
       </c>
     </row>
     <row r="321" spans="1:2" ht="390" x14ac:dyDescent="0.25">
@@ -39028,7 +39027,7 @@
         <v>177</v>
       </c>
       <c r="B321" s="3" t="s">
-        <v>970</v>
+        <v>966</v>
       </c>
     </row>
     <row r="322" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -39036,7 +39035,7 @@
         <v>514</v>
       </c>
       <c r="B322" s="3" t="s">
-        <v>979</v>
+        <v>975</v>
       </c>
     </row>
     <row r="323" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -39044,7 +39043,7 @@
         <v>515</v>
       </c>
       <c r="B323" s="3" t="s">
-        <v>972</v>
+        <v>968</v>
       </c>
     </row>
     <row r="324" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -39052,7 +39051,7 @@
         <v>516</v>
       </c>
       <c r="B324" s="3" t="s">
-        <v>978</v>
+        <v>974</v>
       </c>
     </row>
     <row r="325" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -39060,7 +39059,7 @@
         <v>517</v>
       </c>
       <c r="B325" s="3" t="s">
-        <v>1106</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="326" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -39068,7 +39067,7 @@
         <v>518</v>
       </c>
       <c r="B326" s="3" t="s">
-        <v>977</v>
+        <v>973</v>
       </c>
     </row>
     <row r="327" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -39076,15 +39075,15 @@
         <v>519</v>
       </c>
       <c r="B327" s="3" t="s">
-        <v>971</v>
+        <v>967</v>
       </c>
     </row>
     <row r="328" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A328" s="2" t="s">
-        <v>1048</v>
+        <v>1044</v>
       </c>
       <c r="B328" s="3" t="s">
-        <v>1078</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="329" spans="1:2" ht="390" x14ac:dyDescent="0.25">
@@ -39092,7 +39091,7 @@
         <v>178</v>
       </c>
       <c r="B329" s="3" t="s">
-        <v>975</v>
+        <v>971</v>
       </c>
     </row>
     <row r="330" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -39100,7 +39099,7 @@
         <v>489</v>
       </c>
       <c r="B330" s="3" t="s">
-        <v>980</v>
+        <v>976</v>
       </c>
     </row>
     <row r="331" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -39108,7 +39107,7 @@
         <v>541</v>
       </c>
       <c r="B331" s="3" t="s">
-        <v>1079</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="332" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -39116,7 +39115,7 @@
         <v>542</v>
       </c>
       <c r="B332" s="3" t="s">
-        <v>976</v>
+        <v>972</v>
       </c>
     </row>
     <row r="333" spans="1:2" ht="315" x14ac:dyDescent="0.25">
@@ -39132,7 +39131,7 @@
         <v>249</v>
       </c>
       <c r="B334" s="3" t="s">
-        <v>1155</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="335" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -39156,7 +39155,7 @@
         <v>252</v>
       </c>
       <c r="B337" s="3" t="s">
-        <v>1056</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="338" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -39180,7 +39179,7 @@
         <v>817</v>
       </c>
       <c r="B340" s="3" t="s">
-        <v>1154</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="341" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -39188,7 +39187,7 @@
         <v>180</v>
       </c>
       <c r="B341" s="3" t="s">
-        <v>952</v>
+        <v>948</v>
       </c>
     </row>
     <row r="342" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39212,15 +39211,15 @@
         <v>182</v>
       </c>
       <c r="B344" s="3" t="s">
-        <v>1124</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="345" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A345" s="2" t="s">
-        <v>1123</v>
+        <v>1119</v>
       </c>
       <c r="B345" s="3" t="s">
-        <v>1125</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="346" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39228,7 +39227,7 @@
         <v>183</v>
       </c>
       <c r="B346" s="3" t="s">
-        <v>1060</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="347" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -39236,7 +39235,7 @@
         <v>184</v>
       </c>
       <c r="B347" s="3" t="s">
-        <v>1059</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="348" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -39252,7 +39251,7 @@
         <v>185</v>
       </c>
       <c r="B349" s="3" t="s">
-        <v>1121</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="350" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -39276,7 +39275,7 @@
         <v>464</v>
       </c>
       <c r="B352" s="3" t="s">
-        <v>1080</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="353" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -39348,7 +39347,7 @@
         <v>193</v>
       </c>
       <c r="B361" s="3" t="s">
-        <v>1130</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="362" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -39356,7 +39355,7 @@
         <v>336</v>
       </c>
       <c r="B362" s="3" t="s">
-        <v>1131</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="363" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -39364,71 +39363,71 @@
         <v>337</v>
       </c>
       <c r="B363" s="3" t="s">
-        <v>1134</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="364" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A364" s="2" t="s">
-        <v>1128</v>
+        <v>1124</v>
       </c>
       <c r="B364" s="3" t="s">
-        <v>1133</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="365" spans="1:2" ht="225" x14ac:dyDescent="0.25">
       <c r="A365" s="2" t="s">
-        <v>1129</v>
+        <v>1125</v>
       </c>
       <c r="B365" s="3" t="s">
-        <v>1145</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="366" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A366" s="2" t="s">
-        <v>1132</v>
+        <v>1128</v>
       </c>
       <c r="B366" s="3" t="s">
-        <v>1144</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="367" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A367" s="2" t="s">
-        <v>1135</v>
+        <v>1131</v>
       </c>
       <c r="B367" s="3" t="s">
-        <v>1143</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="368" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A368" s="2" t="s">
-        <v>1136</v>
+        <v>1132</v>
       </c>
       <c r="B368" s="3" t="s">
-        <v>1142</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="369" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A369" s="2" t="s">
-        <v>1137</v>
+        <v>1133</v>
       </c>
       <c r="B369" s="3" t="s">
-        <v>1138</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="370" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A370" s="2" t="s">
-        <v>1139</v>
+        <v>1135</v>
       </c>
       <c r="B370" s="3" t="s">
-        <v>1141</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="371" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A371" s="2" t="s">
-        <v>1140</v>
+        <v>1136</v>
       </c>
       <c r="B371" s="3" t="s">
-        <v>1160</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="372" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -39444,15 +39443,15 @@
         <v>195</v>
       </c>
       <c r="B373" s="3" t="s">
-        <v>1118</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="374" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A374" s="2" t="s">
-        <v>1113</v>
+        <v>1109</v>
       </c>
       <c r="B374" s="3" t="s">
-        <v>1119</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="375" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -39460,7 +39459,7 @@
         <v>196</v>
       </c>
       <c r="B375" s="3" t="s">
-        <v>880</v>
+        <v>876</v>
       </c>
     </row>
     <row r="376" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -39468,7 +39467,7 @@
         <v>328</v>
       </c>
       <c r="B376" s="3" t="s">
-        <v>881</v>
+        <v>877</v>
       </c>
     </row>
     <row r="377" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -39484,7 +39483,7 @@
         <v>648</v>
       </c>
       <c r="B378" s="3" t="s">
-        <v>1081</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="379" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39508,7 +39507,7 @@
         <v>200</v>
       </c>
       <c r="B381" s="3" t="s">
-        <v>1112</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="382" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -39524,7 +39523,7 @@
         <v>202</v>
       </c>
       <c r="B383" s="3" t="s">
-        <v>942</v>
+        <v>938</v>
       </c>
     </row>
     <row r="384" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -39644,7 +39643,7 @@
         <v>580</v>
       </c>
       <c r="B398" s="3" t="s">
-        <v>856</v>
+        <v>1159</v>
       </c>
     </row>
     <row r="399" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -39652,7 +39651,7 @@
         <v>581</v>
       </c>
       <c r="B399" s="3" t="s">
-        <v>857</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="400" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -39660,7 +39659,7 @@
         <v>582</v>
       </c>
       <c r="B400" s="3" t="s">
-        <v>854</v>
+        <v>1161</v>
       </c>
     </row>
     <row r="401" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -39668,7 +39667,7 @@
         <v>583</v>
       </c>
       <c r="B401" s="3" t="s">
-        <v>855</v>
+        <v>1162</v>
       </c>
     </row>
     <row r="402" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39676,7 +39675,7 @@
         <v>584</v>
       </c>
       <c r="B402" s="3" t="s">
-        <v>1159</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="403" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -39684,15 +39683,15 @@
         <v>585</v>
       </c>
       <c r="B403" s="3" t="s">
-        <v>1158</v>
+        <v>1163</v>
       </c>
     </row>
     <row r="404" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A404" s="2" t="s">
-        <v>1157</v>
+        <v>1153</v>
       </c>
       <c r="B404" s="3" t="s">
-        <v>1161</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="405" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39708,7 +39707,7 @@
         <v>207</v>
       </c>
       <c r="B406" s="3" t="s">
-        <v>943</v>
+        <v>939</v>
       </c>
     </row>
     <row r="407" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -39724,7 +39723,7 @@
         <v>209</v>
       </c>
       <c r="B408" s="3" t="s">
-        <v>1105</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="409" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -39777,10 +39776,10 @@
     </row>
     <row r="415" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A415" s="2" t="s">
-        <v>1120</v>
+        <v>1116</v>
       </c>
       <c r="B415" s="3" t="s">
-        <v>1127</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="416" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -39788,7 +39787,7 @@
         <v>210</v>
       </c>
       <c r="B416" s="3" t="s">
-        <v>1117</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="417" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -39796,7 +39795,7 @@
         <v>618</v>
       </c>
       <c r="B417" s="3" t="s">
-        <v>1153</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="418" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -39849,10 +39848,10 @@
     </row>
     <row r="424" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A424" s="2" t="s">
-        <v>1110</v>
+        <v>1106</v>
       </c>
       <c r="B424" s="3" t="s">
-        <v>1111</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="425" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -39876,7 +39875,7 @@
         <v>530</v>
       </c>
       <c r="B427" s="3" t="s">
-        <v>1082</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="428" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -39924,7 +39923,7 @@
         <v>215</v>
       </c>
       <c r="B433" s="3" t="s">
-        <v>1046</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="434" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -39972,7 +39971,7 @@
         <v>221</v>
       </c>
       <c r="B439" s="3" t="s">
-        <v>1163</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="440" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -39980,7 +39979,7 @@
         <v>222</v>
       </c>
       <c r="B440" s="3" t="s">
-        <v>1053</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="441" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -39988,7 +39987,7 @@
         <v>223</v>
       </c>
       <c r="B441" s="3" t="s">
-        <v>1052</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="442" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -39996,7 +39995,7 @@
         <v>224</v>
       </c>
       <c r="B442" s="3" t="s">
-        <v>1051</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="443" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -40004,7 +40003,7 @@
         <v>329</v>
       </c>
       <c r="B443" s="3" t="s">
-        <v>1054</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="444" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -40020,7 +40019,7 @@
         <v>225</v>
       </c>
       <c r="B445" s="3" t="s">
-        <v>874</v>
+        <v>870</v>
       </c>
     </row>
     <row r="446" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -40044,15 +40043,15 @@
         <v>228</v>
       </c>
       <c r="B448" s="3" t="s">
-        <v>1109</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="449" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A449" s="2" t="s">
-        <v>1108</v>
+        <v>1104</v>
       </c>
       <c r="B449" s="3" t="s">
-        <v>1114</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="450" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -40092,7 +40091,7 @@
         <v>442</v>
       </c>
       <c r="B454" s="3" t="s">
-        <v>1047</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="455" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -40132,7 +40131,7 @@
         <v>319</v>
       </c>
       <c r="B459" s="3" t="s">
-        <v>1042</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="460" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -40140,7 +40139,7 @@
         <v>320</v>
       </c>
       <c r="B460" s="3" t="s">
-        <v>1045</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="461" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -40148,7 +40147,7 @@
         <v>321</v>
       </c>
       <c r="B461" s="3" t="s">
-        <v>1043</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="462" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -40156,15 +40155,15 @@
         <v>318</v>
       </c>
       <c r="B462" s="3" t="s">
-        <v>1044</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="463" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A463" s="2" t="s">
-        <v>1003</v>
+        <v>999</v>
       </c>
       <c r="B463" s="3" t="s">
-        <v>1004</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="464" spans="1:2" ht="255" x14ac:dyDescent="0.25">
@@ -40172,7 +40171,7 @@
         <v>322</v>
       </c>
       <c r="B464" s="3" t="s">
-        <v>1049</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="465" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -40196,7 +40195,7 @@
         <v>483</v>
       </c>
       <c r="B467" s="3" t="s">
-        <v>1083</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="468" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -40204,7 +40203,7 @@
         <v>484</v>
       </c>
       <c r="B468" s="3" t="s">
-        <v>1122</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="469" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -40236,7 +40235,7 @@
         <v>550</v>
       </c>
       <c r="B472" s="3" t="s">
-        <v>944</v>
+        <v>940</v>
       </c>
     </row>
     <row r="473" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -40244,7 +40243,7 @@
         <v>554</v>
       </c>
       <c r="B473" s="3" t="s">
-        <v>1097</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="474" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -40260,7 +40259,7 @@
         <v>558</v>
       </c>
       <c r="B475" s="3" t="s">
-        <v>949</v>
+        <v>945</v>
       </c>
     </row>
     <row r="476" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -40284,7 +40283,7 @@
         <v>561</v>
       </c>
       <c r="B478" s="3" t="s">
-        <v>945</v>
+        <v>941</v>
       </c>
     </row>
     <row r="479" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -40292,7 +40291,7 @@
         <v>562</v>
       </c>
       <c r="B479" s="3" t="s">
-        <v>1057</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="480" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -40308,7 +40307,7 @@
         <v>564</v>
       </c>
       <c r="B481" s="3" t="s">
-        <v>946</v>
+        <v>942</v>
       </c>
     </row>
     <row r="482" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -40340,7 +40339,7 @@
         <v>593</v>
       </c>
       <c r="B485" s="3" t="s">
-        <v>896</v>
+        <v>892</v>
       </c>
     </row>
     <row r="486" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -40348,7 +40347,7 @@
         <v>611</v>
       </c>
       <c r="B486" s="3" t="s">
-        <v>1147</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="487" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -40356,7 +40355,7 @@
         <v>612</v>
       </c>
       <c r="B487" s="3" t="s">
-        <v>1115</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="488" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -40364,7 +40363,7 @@
         <v>613</v>
       </c>
       <c r="B488" s="3" t="s">
-        <v>1116</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="489" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -40372,15 +40371,15 @@
         <v>832</v>
       </c>
       <c r="B489" s="3" t="s">
-        <v>897</v>
+        <v>893</v>
       </c>
     </row>
     <row r="490" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A490" s="2" t="s">
-        <v>1146</v>
+        <v>1142</v>
       </c>
       <c r="B490" s="3" t="s">
-        <v>1148</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="491" spans="1:2" ht="255" x14ac:dyDescent="0.25">
@@ -40436,7 +40435,7 @@
         <v>655</v>
       </c>
       <c r="B497" s="1" t="s">
-        <v>898</v>
+        <v>894</v>
       </c>
     </row>
     <row r="498" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -40452,7 +40451,7 @@
         <v>657</v>
       </c>
       <c r="B499" s="1" t="s">
-        <v>1162</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="500" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -40476,7 +40475,7 @@
         <v>660</v>
       </c>
       <c r="B502" s="1" t="s">
-        <v>899</v>
+        <v>895</v>
       </c>
     </row>
     <row r="503" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -40505,18 +40504,18 @@
     </row>
     <row r="506" spans="1:2" ht="255" x14ac:dyDescent="0.25">
       <c r="A506" s="2" t="s">
-        <v>982</v>
+        <v>978</v>
       </c>
       <c r="B506" s="1" t="s">
-        <v>990</v>
+        <v>986</v>
       </c>
     </row>
     <row r="507" spans="1:2" ht="92.25" x14ac:dyDescent="0.25">
       <c r="A507" s="2" t="s">
-        <v>985</v>
+        <v>981</v>
       </c>
       <c r="B507" s="1" t="s">
-        <v>986</v>
+        <v>982</v>
       </c>
     </row>
     <row r="508" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -40524,7 +40523,7 @@
         <v>676</v>
       </c>
       <c r="B508" s="1" t="s">
-        <v>900</v>
+        <v>896</v>
       </c>
     </row>
     <row r="509" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -40532,7 +40531,7 @@
         <v>708</v>
       </c>
       <c r="B509" s="3" t="s">
-        <v>1040</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="510" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -40628,7 +40627,7 @@
         <v>275</v>
       </c>
       <c r="B521" s="1" t="s">
-        <v>1019</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="522" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -40636,7 +40635,7 @@
         <v>276</v>
       </c>
       <c r="B522" s="1" t="s">
-        <v>1020</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="523" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -40644,7 +40643,7 @@
         <v>277</v>
       </c>
       <c r="B523" s="1" t="s">
-        <v>1021</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="524" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -40692,7 +40691,7 @@
         <v>260</v>
       </c>
       <c r="B529" s="3" t="s">
-        <v>969</v>
+        <v>965</v>
       </c>
     </row>
     <row r="530" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -40892,7 +40891,7 @@
         <v>298</v>
       </c>
       <c r="B554" s="1" t="s">
-        <v>901</v>
+        <v>897</v>
       </c>
     </row>
     <row r="555" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -40940,7 +40939,7 @@
         <v>301</v>
       </c>
       <c r="B560" s="1" t="s">
-        <v>865</v>
+        <v>861</v>
       </c>
     </row>
     <row r="561" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -41068,7 +41067,7 @@
         <v>307</v>
       </c>
       <c r="B576" s="1" t="s">
-        <v>974</v>
+        <v>970</v>
       </c>
     </row>
     <row r="577" spans="1:2" ht="375" x14ac:dyDescent="0.25">
@@ -41100,7 +41099,7 @@
         <v>371</v>
       </c>
       <c r="B580" s="3" t="s">
-        <v>967</v>
+        <v>963</v>
       </c>
     </row>
     <row r="581" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -41116,7 +41115,7 @@
         <v>326</v>
       </c>
       <c r="B582" s="3" t="s">
-        <v>1084</v>
+        <v>1080</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Lots of fixes. I think I fixed image problem by using UriEnum=Absolute. Fixed issue with e081a causing hangup.  Fixed issue with e027 not rolling for wealth.
</commit_message>
<xml_diff>
--- a/Documentation/Events.xlsx
+++ b/Documentation/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\happysulla\BarbarianPrince\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{07E1B478-8C33-4832-B598-4D60303D2DBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{A1278F85-69E2-46F4-904E-564ED6AF2301}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -3575,13 +3575,6 @@
 See &lt;InlineUIContainer&gt;&lt;Button Content='e026' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; when you arrive.</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;Bold&gt;e027 Ancient Treasure&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;You find an ancient treasure that was long lost. It has wealth code 110. See
- &lt;InlineUIContainer&gt;&lt;Button Content='r225' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.  Click image to continue.
-&lt;LineBreak/&gt;
-                   &lt;InlineUIContainer&gt;&lt;Image Name='EncounterEnd' Source='../bin/Images/CoinsStacked.gif' Height='400'  Width='400'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt; </t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;e028 Cave Tombs Entrance&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;Amid the howling winds on a craggy cliff, you find caves. Within the caves, you find the tombs of an ancient race. You can decide to avoid them which ends this event. Or, you can continue inward and investigate the tombs. See
  &lt;InlineUIContainer&gt;&lt;Button Content='e028a' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.&lt;LineBreak/&gt;
@@ -8021,6 +8014,13 @@
   <si>
     <t>&lt;Bold&gt;&gt;e500 Click Horde to continue&lt;/Bold&gt;&lt;LineBreak/&gt;
 &lt;InlineUIContainer&gt;&lt;Image Source='../bin/Images/CoinsFalling.gif' Name='Horde' Height='550' Width='550'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;Bold&gt;e027 Ancient Treasure&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;You find an ancient treasure that was long lost. It has wealth code 110. See
+ &lt;InlineUIContainer&gt;&lt;Button Content='r225' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.  Click image to continue.
+&lt;LineBreak/&gt;
+                   &lt;InlineUIContainer&gt;&lt;Image Name='AncientTreasure' Source='../bin/Images/CoinsStacked.gif' Height='400'  Width='400'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt; </t>
   </si>
 </sst>
 </file>
@@ -8409,8 +8409,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B582"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A532" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B534" sqref="B534"/>
+    <sheetView tabSelected="1" topLeftCell="A235" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B236" sqref="B236"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9192,7 +9192,7 @@
         <v>61</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>738</v>
+        <v>1163</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -9200,7 +9200,7 @@
         <v>62</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -9208,7 +9208,7 @@
         <v>342</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -9216,7 +9216,7 @@
         <v>63</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -9224,7 +9224,7 @@
         <v>64</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -9232,7 +9232,7 @@
         <v>65</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -9240,7 +9240,7 @@
         <v>66</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -9248,7 +9248,7 @@
         <v>330</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -9256,7 +9256,7 @@
         <v>67</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -9264,7 +9264,7 @@
         <v>388</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -9272,7 +9272,7 @@
         <v>68</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -9280,7 +9280,7 @@
         <v>343</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -9288,7 +9288,7 @@
         <v>389</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -9296,7 +9296,7 @@
         <v>69</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
     </row>
     <row r="111" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -9304,7 +9304,7 @@
         <v>392</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -9312,7 +9312,7 @@
         <v>393</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
     </row>
     <row r="113" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -9320,7 +9320,7 @@
         <v>70</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -9328,7 +9328,7 @@
         <v>344</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
     </row>
     <row r="115" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -9336,7 +9336,7 @@
         <v>259</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
     </row>
     <row r="116" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -9344,7 +9344,7 @@
         <v>71</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="117" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -9352,7 +9352,7 @@
         <v>72</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="118" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -9360,7 +9360,7 @@
         <v>73</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
     </row>
     <row r="119" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -9376,7 +9376,7 @@
         <v>74</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
     </row>
     <row r="121" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -9392,7 +9392,7 @@
         <v>325</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
     </row>
     <row r="123" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -9400,7 +9400,7 @@
         <v>634</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
     </row>
     <row r="124" spans="1:2" ht="270" x14ac:dyDescent="0.25">
@@ -9408,7 +9408,7 @@
         <v>76</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
     </row>
     <row r="125" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -9416,7 +9416,7 @@
         <v>77</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
     </row>
     <row r="126" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -9440,7 +9440,7 @@
         <v>78</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="129" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -9448,7 +9448,7 @@
         <v>350</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
     </row>
     <row r="130" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -9456,7 +9456,7 @@
         <v>351</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
     </row>
     <row r="131" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -9464,7 +9464,7 @@
         <v>79</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
     </row>
     <row r="132" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -9472,7 +9472,7 @@
         <v>347</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
     </row>
     <row r="133" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -9480,7 +9480,7 @@
         <v>348</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
     </row>
     <row r="134" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -9488,7 +9488,7 @@
         <v>80</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
     </row>
     <row r="135" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -9496,7 +9496,7 @@
         <v>81</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
     </row>
     <row r="136" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -9504,7 +9504,7 @@
         <v>579</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
     </row>
     <row r="137" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -9512,7 +9512,7 @@
         <v>580</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
     </row>
     <row r="138" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -9520,7 +9520,7 @@
         <v>581</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="139" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -9528,7 +9528,7 @@
         <v>582</v>
       </c>
       <c r="B139" s="3" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="140" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -9536,7 +9536,7 @@
         <v>583</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
     </row>
     <row r="141" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -9544,7 +9544,7 @@
         <v>584</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
     </row>
     <row r="142" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -9552,7 +9552,7 @@
         <v>585</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
     </row>
     <row r="143" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -9560,7 +9560,7 @@
         <v>586</v>
       </c>
       <c r="B143" s="3" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
     </row>
     <row r="144" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -9568,7 +9568,7 @@
         <v>587</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="145" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -9576,7 +9576,7 @@
         <v>588</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
     </row>
     <row r="146" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -9584,7 +9584,7 @@
         <v>82</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
     </row>
     <row r="147" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -9592,7 +9592,7 @@
         <v>83</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="148" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -9600,7 +9600,7 @@
         <v>614</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
     </row>
     <row r="149" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -9608,7 +9608,7 @@
         <v>84</v>
       </c>
       <c r="B149" s="3" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="150" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -9616,7 +9616,7 @@
         <v>85</v>
       </c>
       <c r="B150" s="3" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="151" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -9624,7 +9624,7 @@
         <v>428</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="152" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -9632,7 +9632,7 @@
         <v>429</v>
       </c>
       <c r="B152" s="3" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
     </row>
     <row r="153" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -9640,7 +9640,7 @@
         <v>86</v>
       </c>
       <c r="B153" s="3" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
     </row>
     <row r="154" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -9648,7 +9648,7 @@
         <v>87</v>
       </c>
       <c r="B154" s="3" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="155" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -9656,7 +9656,7 @@
         <v>334</v>
       </c>
       <c r="B155" s="3" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
     </row>
     <row r="156" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -9664,7 +9664,7 @@
         <v>371</v>
       </c>
       <c r="B156" s="3" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
     </row>
     <row r="157" spans="1:2" ht="345" x14ac:dyDescent="0.25">
@@ -9672,7 +9672,7 @@
         <v>88</v>
       </c>
       <c r="B157" s="3" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
     </row>
     <row r="158" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -9680,7 +9680,7 @@
         <v>335</v>
       </c>
       <c r="B158" s="3" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
     </row>
     <row r="159" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -9688,7 +9688,7 @@
         <v>336</v>
       </c>
       <c r="B159" s="3" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
     </row>
     <row r="160" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -9696,7 +9696,7 @@
         <v>337</v>
       </c>
       <c r="B160" s="3" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
     </row>
     <row r="161" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -9704,7 +9704,7 @@
         <v>339</v>
       </c>
       <c r="B161" s="3" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
     </row>
     <row r="162" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -9712,7 +9712,7 @@
         <v>338</v>
       </c>
       <c r="B162" s="3" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
     </row>
     <row r="163" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -9720,7 +9720,7 @@
         <v>340</v>
       </c>
       <c r="B163" s="3" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
     </row>
     <row r="164" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -9728,7 +9728,7 @@
         <v>341</v>
       </c>
       <c r="B164" s="3" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
     </row>
     <row r="165" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -9736,7 +9736,7 @@
         <v>513</v>
       </c>
       <c r="B165" s="3" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
     </row>
     <row r="166" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -9744,7 +9744,7 @@
         <v>89</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
     </row>
     <row r="167" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -9752,7 +9752,7 @@
         <v>377</v>
       </c>
       <c r="B167" s="3" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
     </row>
     <row r="168" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -9760,7 +9760,7 @@
         <v>378</v>
       </c>
       <c r="B168" s="3" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
     </row>
     <row r="169" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -9768,7 +9768,7 @@
         <v>381</v>
       </c>
       <c r="B169" s="3" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
     </row>
     <row r="170" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -9776,7 +9776,7 @@
         <v>90</v>
       </c>
       <c r="B170" s="3" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
     </row>
     <row r="171" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -9784,7 +9784,7 @@
         <v>542</v>
       </c>
       <c r="B171" s="3" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
     </row>
     <row r="172" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -9792,7 +9792,7 @@
         <v>543</v>
       </c>
       <c r="B172" s="3" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
     </row>
     <row r="173" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -9800,7 +9800,7 @@
         <v>91</v>
       </c>
       <c r="B173" s="3" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
     </row>
     <row r="174" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -9808,7 +9808,7 @@
         <v>382</v>
       </c>
       <c r="B174" s="3" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
     </row>
     <row r="175" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -9816,7 +9816,7 @@
         <v>92</v>
       </c>
       <c r="B175" s="3" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
     </row>
     <row r="176" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -9824,7 +9824,7 @@
         <v>93</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
     </row>
     <row r="177" spans="1:2" ht="270" x14ac:dyDescent="0.25">
@@ -9848,7 +9848,7 @@
         <v>96</v>
       </c>
       <c r="B179" s="3" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
     </row>
     <row r="180" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -9856,7 +9856,7 @@
         <v>547</v>
       </c>
       <c r="B180" s="3" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
     </row>
     <row r="181" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -9864,7 +9864,7 @@
         <v>548</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
     </row>
     <row r="182" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -9872,7 +9872,7 @@
         <v>549</v>
       </c>
       <c r="B182" s="3" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
     </row>
     <row r="183" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -9880,7 +9880,7 @@
         <v>550</v>
       </c>
       <c r="B183" s="3" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
     </row>
     <row r="184" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -9888,7 +9888,7 @@
         <v>556</v>
       </c>
       <c r="B184" s="3" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="185" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -9904,7 +9904,7 @@
         <v>97</v>
       </c>
       <c r="B186" s="3" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
     </row>
     <row r="187" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -9912,7 +9912,7 @@
         <v>98</v>
       </c>
       <c r="B187" s="3" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
     </row>
     <row r="188" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -9920,7 +9920,7 @@
         <v>99</v>
       </c>
       <c r="B188" s="3" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
     </row>
     <row r="189" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -9928,7 +9928,7 @@
         <v>101</v>
       </c>
       <c r="B189" s="3" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
     </row>
     <row r="190" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -9936,7 +9936,7 @@
         <v>100</v>
       </c>
       <c r="B190" s="3" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
     </row>
     <row r="191" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -9944,7 +9944,7 @@
         <v>102</v>
       </c>
       <c r="B191" s="3" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
     </row>
     <row r="192" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -9952,7 +9952,7 @@
         <v>103</v>
       </c>
       <c r="B192" s="3" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
     </row>
     <row r="193" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -9960,7 +9960,7 @@
         <v>104</v>
       </c>
       <c r="B193" s="3" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
     </row>
     <row r="194" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -9968,7 +9968,7 @@
         <v>105</v>
       </c>
       <c r="B194" s="3" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
     <row r="195" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -9976,7 +9976,7 @@
         <v>504</v>
       </c>
       <c r="B195" s="3" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
     </row>
     <row r="196" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -9984,7 +9984,7 @@
         <v>505</v>
       </c>
       <c r="B196" s="3" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
     </row>
     <row r="197" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -9992,7 +9992,7 @@
         <v>106</v>
       </c>
       <c r="B197" s="3" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
     </row>
     <row r="198" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10000,7 +10000,7 @@
         <v>107</v>
       </c>
       <c r="B198" s="3" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
     </row>
     <row r="199" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -10008,7 +10008,7 @@
         <v>165</v>
       </c>
       <c r="B199" s="3" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
     </row>
     <row r="200" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -10016,7 +10016,7 @@
         <v>544</v>
       </c>
       <c r="B200" s="3" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
     </row>
     <row r="201" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -10024,7 +10024,7 @@
         <v>108</v>
       </c>
       <c r="B201" s="3" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
     <row r="202" spans="1:2" ht="285" x14ac:dyDescent="0.25">
@@ -10032,7 +10032,7 @@
         <v>109</v>
       </c>
       <c r="B202" s="3" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="203" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -10040,7 +10040,7 @@
         <v>110</v>
       </c>
       <c r="B203" s="3" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
     <row r="204" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -10048,7 +10048,7 @@
         <v>166</v>
       </c>
       <c r="B204" s="3" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
     </row>
     <row r="205" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -10056,7 +10056,7 @@
         <v>167</v>
       </c>
       <c r="B205" s="3" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
     </row>
     <row r="206" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -10064,7 +10064,7 @@
         <v>168</v>
       </c>
       <c r="B206" s="3" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
     </row>
     <row r="207" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -10072,7 +10072,7 @@
         <v>562</v>
       </c>
       <c r="B207" s="3" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
     </row>
     <row r="208" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10088,7 +10088,7 @@
         <v>111</v>
       </c>
       <c r="B209" s="3" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
     </row>
     <row r="210" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10096,7 +10096,7 @@
         <v>510</v>
       </c>
       <c r="B210" s="3" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
     </row>
     <row r="211" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -10104,7 +10104,7 @@
         <v>511</v>
       </c>
       <c r="B211" s="3" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
     </row>
     <row r="212" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -10120,7 +10120,7 @@
         <v>516</v>
       </c>
       <c r="B213" s="3" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="214" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10128,7 +10128,7 @@
         <v>112</v>
       </c>
       <c r="B214" s="3" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
     </row>
     <row r="215" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10136,7 +10136,7 @@
         <v>169</v>
       </c>
       <c r="B215" s="3" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="216" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10144,7 +10144,7 @@
         <v>170</v>
       </c>
       <c r="B216" s="3" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
     </row>
     <row r="217" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10152,7 +10152,7 @@
         <v>171</v>
       </c>
       <c r="B217" s="3" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="218" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -10160,7 +10160,7 @@
         <v>113</v>
       </c>
       <c r="B218" s="3" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="219" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -10168,7 +10168,7 @@
         <v>114</v>
       </c>
       <c r="B219" s="3" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
     </row>
     <row r="220" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10176,7 +10176,7 @@
         <v>266</v>
       </c>
       <c r="B220" s="3" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
     </row>
     <row r="221" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -10184,7 +10184,7 @@
         <v>570</v>
       </c>
       <c r="B221" s="3" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
     </row>
     <row r="222" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10192,7 +10192,7 @@
         <v>115</v>
       </c>
       <c r="B222" s="3" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
     </row>
     <row r="223" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10200,7 +10200,7 @@
         <v>522</v>
       </c>
       <c r="B223" s="3" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
     </row>
     <row r="224" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -10208,7 +10208,7 @@
         <v>116</v>
       </c>
       <c r="B224" s="3" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
     </row>
     <row r="225" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10216,7 +10216,7 @@
         <v>520</v>
       </c>
       <c r="B225" s="3" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
     </row>
     <row r="226" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10224,7 +10224,7 @@
         <v>117</v>
       </c>
       <c r="B226" s="4" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
     </row>
     <row r="227" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10232,7 +10232,7 @@
         <v>523</v>
       </c>
       <c r="B227" s="4" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
     </row>
     <row r="228" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10240,7 +10240,7 @@
         <v>524</v>
       </c>
       <c r="B228" s="4" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
     </row>
     <row r="229" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10248,7 +10248,7 @@
         <v>525</v>
       </c>
       <c r="B229" s="4" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
     </row>
     <row r="230" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10256,7 +10256,7 @@
         <v>118</v>
       </c>
       <c r="B230" s="3" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
     </row>
     <row r="231" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -10264,7 +10264,7 @@
         <v>573</v>
       </c>
       <c r="B231" s="3" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
     </row>
     <row r="232" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10272,7 +10272,7 @@
         <v>574</v>
       </c>
       <c r="B232" s="3" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
     </row>
     <row r="233" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10280,7 +10280,7 @@
         <v>119</v>
       </c>
       <c r="B233" s="3" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="234" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10288,7 +10288,7 @@
         <v>566</v>
       </c>
       <c r="B234" s="3" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
     </row>
     <row r="235" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10296,7 +10296,7 @@
         <v>565</v>
       </c>
       <c r="B235" s="3" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
     </row>
     <row r="236" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10304,7 +10304,7 @@
         <v>120</v>
       </c>
       <c r="B236" s="3" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
     </row>
     <row r="237" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -10312,7 +10312,7 @@
         <v>172</v>
       </c>
       <c r="B237" s="3" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
     </row>
     <row r="238" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10320,7 +10320,7 @@
         <v>173</v>
       </c>
       <c r="B238" s="3" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
     </row>
     <row r="239" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10328,7 +10328,7 @@
         <v>174</v>
       </c>
       <c r="B239" s="3" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
     </row>
     <row r="240" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -10336,7 +10336,7 @@
         <v>121</v>
       </c>
       <c r="B240" s="3" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
     </row>
     <row r="241" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10344,7 +10344,7 @@
         <v>122</v>
       </c>
       <c r="B241" s="3" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
     </row>
     <row r="242" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10352,7 +10352,7 @@
         <v>521</v>
       </c>
       <c r="B242" s="3" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
     </row>
     <row r="243" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -10360,7 +10360,7 @@
         <v>123</v>
       </c>
       <c r="B243" s="3" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
     </row>
     <row r="244" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10368,7 +10368,7 @@
         <v>571</v>
       </c>
       <c r="B244" s="3" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
     </row>
     <row r="245" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10376,7 +10376,7 @@
         <v>572</v>
       </c>
       <c r="B245" s="3" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
     </row>
     <row r="246" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10384,7 +10384,7 @@
         <v>124</v>
       </c>
       <c r="B246" s="3" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
     </row>
     <row r="247" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10392,7 +10392,7 @@
         <v>617</v>
       </c>
       <c r="B247" s="3" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
     </row>
     <row r="248" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10400,7 +10400,7 @@
         <v>125</v>
       </c>
       <c r="B248" s="3" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
     </row>
     <row r="249" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -10408,7 +10408,7 @@
         <v>589</v>
       </c>
       <c r="B249" s="3" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
     </row>
     <row r="250" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10416,7 +10416,7 @@
         <v>126</v>
       </c>
       <c r="B250" s="3" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
     </row>
     <row r="251" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -10424,7 +10424,7 @@
         <v>127</v>
       </c>
       <c r="B251" s="3" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
     </row>
     <row r="252" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10432,7 +10432,7 @@
         <v>128</v>
       </c>
       <c r="B252" s="3" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
     </row>
     <row r="253" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -10440,7 +10440,7 @@
         <v>129</v>
       </c>
       <c r="B253" s="3" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
     </row>
     <row r="254" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10448,7 +10448,7 @@
         <v>130</v>
       </c>
       <c r="B254" s="3" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
     </row>
     <row r="255" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -10456,7 +10456,7 @@
         <v>131</v>
       </c>
       <c r="B255" s="3" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="256" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -10464,7 +10464,7 @@
         <v>576</v>
       </c>
       <c r="B256" s="3" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="257" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10472,7 +10472,7 @@
         <v>577</v>
       </c>
       <c r="B257" s="3" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
     </row>
     <row r="258" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -10480,7 +10480,7 @@
         <v>132</v>
       </c>
       <c r="B258" s="3" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="259" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10488,7 +10488,7 @@
         <v>133</v>
       </c>
       <c r="B259" s="3" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
     </row>
     <row r="260" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10496,7 +10496,7 @@
         <v>575</v>
       </c>
       <c r="B260" s="3" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
     </row>
     <row r="261" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -10504,7 +10504,7 @@
         <v>134</v>
       </c>
       <c r="B261" s="3" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
     </row>
     <row r="262" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10512,7 +10512,7 @@
         <v>590</v>
       </c>
       <c r="B262" s="3" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
     </row>
     <row r="263" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10520,7 +10520,7 @@
         <v>591</v>
       </c>
       <c r="B263" s="3" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
     </row>
     <row r="264" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -10528,7 +10528,7 @@
         <v>135</v>
       </c>
       <c r="B264" s="3" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
     </row>
     <row r="265" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -10536,7 +10536,7 @@
         <v>592</v>
       </c>
       <c r="B265" s="3" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
     </row>
     <row r="266" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10544,7 +10544,7 @@
         <v>136</v>
       </c>
       <c r="B266" s="3" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
     </row>
     <row r="267" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -10552,7 +10552,7 @@
         <v>137</v>
       </c>
       <c r="B267" s="3" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
     </row>
     <row r="268" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10560,7 +10560,7 @@
         <v>232</v>
       </c>
       <c r="B268" s="3" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="269" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10568,7 +10568,7 @@
         <v>233</v>
       </c>
       <c r="B269" s="3" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
     </row>
     <row r="270" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -10584,7 +10584,7 @@
         <v>234</v>
       </c>
       <c r="B271" s="3" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
     </row>
     <row r="272" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10592,7 +10592,7 @@
         <v>235</v>
       </c>
       <c r="B272" s="3" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
     </row>
     <row r="273" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -10608,7 +10608,7 @@
         <v>239</v>
       </c>
       <c r="B274" s="3" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
     </row>
     <row r="275" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10616,7 +10616,7 @@
         <v>240</v>
       </c>
       <c r="B275" s="3" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
     </row>
     <row r="276" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10624,7 +10624,7 @@
         <v>241</v>
       </c>
       <c r="B276" s="3" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="277" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10640,7 +10640,7 @@
         <v>236</v>
       </c>
       <c r="B278" s="3" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="279" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10648,7 +10648,7 @@
         <v>237</v>
       </c>
       <c r="B279" s="3" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
     </row>
     <row r="280" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10656,7 +10656,7 @@
         <v>238</v>
       </c>
       <c r="B280" s="3" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
     </row>
     <row r="281" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10664,7 +10664,7 @@
         <v>141</v>
       </c>
       <c r="B281" s="3" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
     </row>
     <row r="282" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10672,7 +10672,7 @@
         <v>142</v>
       </c>
       <c r="B282" s="3" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
     </row>
     <row r="283" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10680,7 +10680,7 @@
         <v>143</v>
       </c>
       <c r="B283" s="3" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
     </row>
     <row r="284" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -10688,7 +10688,7 @@
         <v>144</v>
       </c>
       <c r="B284" s="3" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
     </row>
     <row r="285" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10696,7 +10696,7 @@
         <v>242</v>
       </c>
       <c r="B285" s="3" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
     </row>
     <row r="286" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10704,7 +10704,7 @@
         <v>145</v>
       </c>
       <c r="B286" s="3" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
     </row>
     <row r="287" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10712,7 +10712,7 @@
         <v>146</v>
       </c>
       <c r="B287" s="3" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="288" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10720,7 +10720,7 @@
         <v>147</v>
       </c>
       <c r="B288" s="3" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
     </row>
     <row r="289" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10728,7 +10728,7 @@
         <v>148</v>
       </c>
       <c r="B289" s="3" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
     </row>
     <row r="290" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10736,7 +10736,7 @@
         <v>149</v>
       </c>
       <c r="B290" s="3" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
     </row>
     <row r="291" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10744,7 +10744,7 @@
         <v>605</v>
       </c>
       <c r="B291" s="3" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
     </row>
     <row r="292" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10752,7 +10752,7 @@
         <v>604</v>
       </c>
       <c r="B292" s="3" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
     </row>
     <row r="293" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10760,7 +10760,7 @@
         <v>606</v>
       </c>
       <c r="B293" s="3" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
     </row>
     <row r="294" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10768,7 +10768,7 @@
         <v>150</v>
       </c>
       <c r="B294" s="3" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
     </row>
     <row r="295" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10776,7 +10776,7 @@
         <v>607</v>
       </c>
       <c r="B295" s="3" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
     </row>
     <row r="296" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -10784,7 +10784,7 @@
         <v>151</v>
       </c>
       <c r="B296" s="3" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
     </row>
     <row r="297" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10792,7 +10792,7 @@
         <v>243</v>
       </c>
       <c r="B297" s="3" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
     </row>
     <row r="298" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10800,7 +10800,7 @@
         <v>244</v>
       </c>
       <c r="B298" s="3" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
     </row>
     <row r="299" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10808,7 +10808,7 @@
         <v>245</v>
       </c>
       <c r="B299" s="3" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
     </row>
     <row r="300" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10816,7 +10816,7 @@
         <v>152</v>
       </c>
       <c r="B300" s="3" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
     </row>
     <row r="301" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10824,7 +10824,7 @@
         <v>153</v>
       </c>
       <c r="B301" s="3" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
     </row>
     <row r="302" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10832,7 +10832,7 @@
         <v>154</v>
       </c>
       <c r="B302" s="3" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
     </row>
     <row r="303" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -10840,7 +10840,7 @@
         <v>155</v>
       </c>
       <c r="B303" s="3" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
     </row>
     <row r="304" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10848,7 +10848,7 @@
         <v>156</v>
       </c>
       <c r="B304" s="3" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
     </row>
     <row r="305" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10864,7 +10864,7 @@
         <v>246</v>
       </c>
       <c r="B306" s="3" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
     </row>
     <row r="307" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10872,7 +10872,7 @@
         <v>247</v>
       </c>
       <c r="B307" s="3" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
     </row>
     <row r="308" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10880,7 +10880,7 @@
         <v>248</v>
       </c>
       <c r="B308" s="3" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
     </row>
     <row r="309" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10896,7 +10896,7 @@
         <v>159</v>
       </c>
       <c r="B310" s="3" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
     </row>
     <row r="311" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10904,7 +10904,7 @@
         <v>160</v>
       </c>
       <c r="B311" s="3" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
     </row>
     <row r="312" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -10912,7 +10912,7 @@
         <v>161</v>
       </c>
       <c r="B312" s="3" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
     </row>
     <row r="313" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -10920,7 +10920,7 @@
         <v>162</v>
       </c>
       <c r="B313" s="3" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
     </row>
     <row r="314" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -10928,7 +10928,7 @@
         <v>599</v>
       </c>
       <c r="B314" s="3" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
     </row>
     <row r="315" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10936,7 +10936,7 @@
         <v>600</v>
       </c>
       <c r="B315" s="3" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
     </row>
     <row r="316" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10944,7 +10944,7 @@
         <v>601</v>
       </c>
       <c r="B316" s="3" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
     </row>
     <row r="317" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10952,7 +10952,7 @@
         <v>163</v>
       </c>
       <c r="B317" s="3" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
     </row>
     <row r="318" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10960,7 +10960,7 @@
         <v>164</v>
       </c>
       <c r="B318" s="3" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
     </row>
     <row r="319" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10968,7 +10968,7 @@
         <v>175</v>
       </c>
       <c r="B319" s="3" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
     </row>
     <row r="320" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -10976,7 +10976,7 @@
         <v>176</v>
       </c>
       <c r="B320" s="3" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
     </row>
     <row r="321" spans="1:2" ht="390" x14ac:dyDescent="0.25">
@@ -10984,7 +10984,7 @@
         <v>177</v>
       </c>
       <c r="B321" s="3" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
     </row>
     <row r="322" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -11000,7 +11000,7 @@
         <v>414</v>
       </c>
       <c r="B323" s="3" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
     </row>
     <row r="324" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11008,7 +11008,7 @@
         <v>415</v>
       </c>
       <c r="B324" s="3" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
     </row>
     <row r="325" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -11016,7 +11016,7 @@
         <v>416</v>
       </c>
       <c r="B325" s="3" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
     </row>
     <row r="326" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -11024,7 +11024,7 @@
         <v>417</v>
       </c>
       <c r="B326" s="3" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
     </row>
     <row r="327" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11032,7 +11032,7 @@
         <v>418</v>
       </c>
       <c r="B327" s="3" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
     </row>
     <row r="328" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11040,7 +11040,7 @@
         <v>613</v>
       </c>
       <c r="B328" s="3" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
     </row>
     <row r="329" spans="1:2" ht="390" x14ac:dyDescent="0.25">
@@ -11048,7 +11048,7 @@
         <v>178</v>
       </c>
       <c r="B329" s="3" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
     </row>
     <row r="330" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -11064,7 +11064,7 @@
         <v>426</v>
       </c>
       <c r="B331" s="3" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
     </row>
     <row r="332" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11072,7 +11072,7 @@
         <v>427</v>
       </c>
       <c r="B332" s="3" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
     </row>
     <row r="333" spans="1:2" ht="315" x14ac:dyDescent="0.25">
@@ -11080,7 +11080,7 @@
         <v>179</v>
       </c>
       <c r="B333" s="3" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
     </row>
     <row r="334" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -11088,7 +11088,7 @@
         <v>249</v>
       </c>
       <c r="B334" s="3" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
     </row>
     <row r="335" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -11096,7 +11096,7 @@
         <v>250</v>
       </c>
       <c r="B335" s="3" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="336" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -11104,7 +11104,7 @@
         <v>251</v>
       </c>
       <c r="B336" s="3" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
     </row>
     <row r="337" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11112,7 +11112,7 @@
         <v>252</v>
       </c>
       <c r="B337" s="3" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
     </row>
     <row r="338" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -11120,7 +11120,7 @@
         <v>253</v>
       </c>
       <c r="B338" s="3" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
     </row>
     <row r="339" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -11128,7 +11128,7 @@
         <v>545</v>
       </c>
       <c r="B339" s="3" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
     </row>
     <row r="340" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -11136,7 +11136,7 @@
         <v>546</v>
       </c>
       <c r="B340" s="3" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
     </row>
     <row r="341" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11144,7 +11144,7 @@
         <v>180</v>
       </c>
       <c r="B341" s="3" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
     </row>
     <row r="342" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11152,7 +11152,7 @@
         <v>181</v>
       </c>
       <c r="B342" s="3" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
     </row>
     <row r="343" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11160,7 +11160,7 @@
         <v>386</v>
       </c>
       <c r="B343" s="3" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
     </row>
     <row r="344" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -11176,7 +11176,7 @@
         <v>622</v>
       </c>
       <c r="B345" s="3" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
     </row>
     <row r="346" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11184,7 +11184,7 @@
         <v>183</v>
       </c>
       <c r="B346" s="3" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
     </row>
     <row r="347" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -11192,7 +11192,7 @@
         <v>184</v>
       </c>
       <c r="B347" s="3" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
     </row>
     <row r="348" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -11208,7 +11208,7 @@
         <v>185</v>
       </c>
       <c r="B349" s="3" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
     </row>
     <row r="350" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -11216,7 +11216,7 @@
         <v>186</v>
       </c>
       <c r="B350" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="351" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -11224,7 +11224,7 @@
         <v>187</v>
       </c>
       <c r="B351" s="3" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
     </row>
     <row r="352" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11240,7 +11240,7 @@
         <v>188</v>
       </c>
       <c r="B353" s="3" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
     </row>
     <row r="354" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -11248,7 +11248,7 @@
         <v>189</v>
       </c>
       <c r="B354" s="3" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
     </row>
     <row r="355" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -11256,7 +11256,7 @@
         <v>383</v>
       </c>
       <c r="B355" s="3" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
     </row>
     <row r="356" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -11264,7 +11264,7 @@
         <v>384</v>
       </c>
       <c r="B356" s="3" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="357" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -11272,7 +11272,7 @@
         <v>190</v>
       </c>
       <c r="B357" s="3" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
     </row>
     <row r="358" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -11280,7 +11280,7 @@
         <v>191</v>
       </c>
       <c r="B358" s="3" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="359" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -11288,7 +11288,7 @@
         <v>192</v>
       </c>
       <c r="B359" s="3" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
     </row>
     <row r="360" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -11296,7 +11296,7 @@
         <v>465</v>
       </c>
       <c r="B360" s="3" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
     </row>
     <row r="361" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -11304,7 +11304,7 @@
         <v>193</v>
       </c>
       <c r="B361" s="3" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
     </row>
     <row r="362" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -11320,7 +11320,7 @@
         <v>333</v>
       </c>
       <c r="B363" s="3" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
     </row>
     <row r="364" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -11328,7 +11328,7 @@
         <v>624</v>
       </c>
       <c r="B364" s="3" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
     </row>
     <row r="365" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -11336,7 +11336,7 @@
         <v>625</v>
       </c>
       <c r="B365" s="3" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
     </row>
     <row r="366" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11344,7 +11344,7 @@
         <v>627</v>
       </c>
       <c r="B366" s="3" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
     </row>
     <row r="367" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11352,7 +11352,7 @@
         <v>628</v>
       </c>
       <c r="B367" s="3" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
     </row>
     <row r="368" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11360,7 +11360,7 @@
         <v>629</v>
       </c>
       <c r="B368" s="3" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
     </row>
     <row r="369" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11368,7 +11368,7 @@
         <v>630</v>
       </c>
       <c r="B369" s="3" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
     </row>
     <row r="370" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11376,7 +11376,7 @@
         <v>631</v>
       </c>
       <c r="B370" s="3" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="371" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11384,7 +11384,7 @@
         <v>632</v>
       </c>
       <c r="B371" s="3" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
     </row>
     <row r="372" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -11392,7 +11392,7 @@
         <v>194</v>
       </c>
       <c r="B372" s="3" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
     </row>
     <row r="373" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -11400,7 +11400,7 @@
         <v>195</v>
       </c>
       <c r="B373" s="3" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
     </row>
     <row r="374" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -11408,7 +11408,7 @@
         <v>620</v>
       </c>
       <c r="B374" s="3" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
     </row>
     <row r="375" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -11416,7 +11416,7 @@
         <v>196</v>
       </c>
       <c r="B375" s="3" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
     </row>
     <row r="376" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -11424,7 +11424,7 @@
         <v>328</v>
       </c>
       <c r="B376" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="377" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -11432,7 +11432,7 @@
         <v>197</v>
       </c>
       <c r="B377" s="3" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
     </row>
     <row r="378" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11440,7 +11440,7 @@
         <v>487</v>
       </c>
       <c r="B378" s="3" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
     </row>
     <row r="379" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11448,7 +11448,7 @@
         <v>198</v>
       </c>
       <c r="B379" s="3" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
     </row>
     <row r="380" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11456,7 +11456,7 @@
         <v>199</v>
       </c>
       <c r="B380" s="3" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="381" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -11464,7 +11464,7 @@
         <v>200</v>
       </c>
       <c r="B381" s="3" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="382" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11472,7 +11472,7 @@
         <v>201</v>
       </c>
       <c r="B382" s="3" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="383" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11480,7 +11480,7 @@
         <v>202</v>
       </c>
       <c r="B383" s="3" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="384" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -11488,7 +11488,7 @@
         <v>203</v>
       </c>
       <c r="B384" s="3" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="385" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -11536,7 +11536,7 @@
         <v>204</v>
       </c>
       <c r="B390" s="3" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="391" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11544,7 +11544,7 @@
         <v>459</v>
       </c>
       <c r="B391" s="3" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="392" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11552,7 +11552,7 @@
         <v>460</v>
       </c>
       <c r="B392" s="3" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="393" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11560,7 +11560,7 @@
         <v>461</v>
       </c>
       <c r="B393" s="3" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="394" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11568,7 +11568,7 @@
         <v>462</v>
       </c>
       <c r="B394" s="3" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="395" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11576,7 +11576,7 @@
         <v>463</v>
       </c>
       <c r="B395" s="3" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="396" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11584,7 +11584,7 @@
         <v>464</v>
       </c>
       <c r="B396" s="3" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="397" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -11592,7 +11592,7 @@
         <v>205</v>
       </c>
       <c r="B397" s="3" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="398" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -11664,7 +11664,7 @@
         <v>207</v>
       </c>
       <c r="B406" s="3" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="407" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -11672,7 +11672,7 @@
         <v>208</v>
       </c>
       <c r="B407" s="3" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="408" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -11680,7 +11680,7 @@
         <v>209</v>
       </c>
       <c r="B408" s="3" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="409" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11688,7 +11688,7 @@
         <v>476</v>
       </c>
       <c r="B409" s="3" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="410" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11696,7 +11696,7 @@
         <v>477</v>
       </c>
       <c r="B410" s="3" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="411" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11704,7 +11704,7 @@
         <v>478</v>
       </c>
       <c r="B411" s="3" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="412" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -11712,7 +11712,7 @@
         <v>479</v>
       </c>
       <c r="B412" s="3" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="413" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -11720,7 +11720,7 @@
         <v>480</v>
       </c>
       <c r="B413" s="4" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="414" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -11728,7 +11728,7 @@
         <v>481</v>
       </c>
       <c r="B414" s="3" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="415" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -11736,7 +11736,7 @@
         <v>621</v>
       </c>
       <c r="B415" s="3" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="416" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -11744,7 +11744,7 @@
         <v>210</v>
       </c>
       <c r="B416" s="3" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="417" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11752,7 +11752,7 @@
         <v>469</v>
       </c>
       <c r="B417" s="3" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="418" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11760,7 +11760,7 @@
         <v>470</v>
       </c>
       <c r="B418" s="3" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="419" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11768,7 +11768,7 @@
         <v>471</v>
       </c>
       <c r="B419" s="3" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="420" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11776,7 +11776,7 @@
         <v>472</v>
       </c>
       <c r="B420" s="3" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="421" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11784,7 +11784,7 @@
         <v>473</v>
       </c>
       <c r="B421" s="3" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="422" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11792,7 +11792,7 @@
         <v>474</v>
       </c>
       <c r="B422" s="3" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="423" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11800,7 +11800,7 @@
         <v>475</v>
       </c>
       <c r="B423" s="3" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="424" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11808,7 +11808,7 @@
         <v>619</v>
       </c>
       <c r="B424" s="3" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="425" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -11816,7 +11816,7 @@
         <v>211</v>
       </c>
       <c r="B425" s="3" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="426" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11824,7 +11824,7 @@
         <v>212</v>
       </c>
       <c r="B426" s="3" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="427" spans="1:2" ht="300" x14ac:dyDescent="0.25">
@@ -11832,7 +11832,7 @@
         <v>419</v>
       </c>
       <c r="B427" s="3" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="428" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11840,7 +11840,7 @@
         <v>420</v>
       </c>
       <c r="B428" s="3" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="429" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -11848,7 +11848,7 @@
         <v>421</v>
       </c>
       <c r="B429" s="3" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="430" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11856,7 +11856,7 @@
         <v>422</v>
       </c>
       <c r="B430" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="431" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -11864,7 +11864,7 @@
         <v>213</v>
       </c>
       <c r="B431" s="3" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="432" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -11872,7 +11872,7 @@
         <v>214</v>
       </c>
       <c r="B432" s="3" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="433" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -11880,7 +11880,7 @@
         <v>215</v>
       </c>
       <c r="B433" s="3" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="434" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11888,7 +11888,7 @@
         <v>216</v>
       </c>
       <c r="B434" s="3" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="435" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11896,7 +11896,7 @@
         <v>217</v>
       </c>
       <c r="B435" s="3" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="436" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11904,7 +11904,7 @@
         <v>218</v>
       </c>
       <c r="B436" s="3" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="437" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11912,7 +11912,7 @@
         <v>219</v>
       </c>
       <c r="B437" s="3" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="438" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11920,7 +11920,7 @@
         <v>220</v>
       </c>
       <c r="B438" s="3" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="439" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11928,7 +11928,7 @@
         <v>221</v>
       </c>
       <c r="B439" s="3" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="440" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11936,7 +11936,7 @@
         <v>222</v>
       </c>
       <c r="B440" s="3" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="441" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11944,7 +11944,7 @@
         <v>223</v>
       </c>
       <c r="B441" s="3" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="442" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -11952,7 +11952,7 @@
         <v>224</v>
       </c>
       <c r="B442" s="3" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="443" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -11960,7 +11960,7 @@
         <v>329</v>
       </c>
       <c r="B443" s="3" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="444" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11968,7 +11968,7 @@
         <v>385</v>
       </c>
       <c r="B444" s="3" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="445" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11976,7 +11976,7 @@
         <v>225</v>
       </c>
       <c r="B445" s="3" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="446" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -11984,7 +11984,7 @@
         <v>226</v>
       </c>
       <c r="B446" s="3" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="447" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -11992,7 +11992,7 @@
         <v>227</v>
       </c>
       <c r="B447" s="3" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="448" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -12000,7 +12000,7 @@
         <v>228</v>
       </c>
       <c r="B448" s="3" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="449" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -12008,7 +12008,7 @@
         <v>618</v>
       </c>
       <c r="B449" s="3" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="450" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12016,7 +12016,7 @@
         <v>229</v>
       </c>
       <c r="B450" s="3" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="451" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -12024,7 +12024,7 @@
         <v>230</v>
       </c>
       <c r="B451" s="3" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="452" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -12032,7 +12032,7 @@
         <v>231</v>
       </c>
       <c r="B452" s="3" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="453" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12040,7 +12040,7 @@
         <v>257</v>
       </c>
       <c r="B453" s="3" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="454" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -12048,7 +12048,7 @@
         <v>379</v>
       </c>
       <c r="B454" s="3" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="455" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12056,7 +12056,7 @@
         <v>380</v>
       </c>
       <c r="B455" s="3" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="456" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12064,7 +12064,7 @@
         <v>444</v>
       </c>
       <c r="B456" s="3" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="457" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12080,7 +12080,7 @@
         <v>531</v>
       </c>
       <c r="B458" s="3" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="459" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -12120,7 +12120,7 @@
         <v>602</v>
       </c>
       <c r="B463" s="3" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="464" spans="1:2" ht="255" x14ac:dyDescent="0.25">
@@ -12128,7 +12128,7 @@
         <v>322</v>
       </c>
       <c r="B464" s="3" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="465" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12136,7 +12136,7 @@
         <v>395</v>
       </c>
       <c r="B465" s="3" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="466" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -12144,7 +12144,7 @@
         <v>394</v>
       </c>
       <c r="B466" s="3" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="467" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12152,7 +12152,7 @@
         <v>396</v>
       </c>
       <c r="B467" s="3" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="468" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12160,7 +12160,7 @@
         <v>397</v>
       </c>
       <c r="B468" s="3" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="469" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12168,7 +12168,7 @@
         <v>398</v>
       </c>
       <c r="B469" s="3" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="470" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12176,7 +12176,7 @@
         <v>399</v>
       </c>
       <c r="B470" s="3" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="471" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12184,7 +12184,7 @@
         <v>400</v>
       </c>
       <c r="B471" s="3" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="472" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12192,7 +12192,7 @@
         <v>431</v>
       </c>
       <c r="B472" s="3" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="473" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -12200,7 +12200,7 @@
         <v>432</v>
       </c>
       <c r="B473" s="3" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="474" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -12208,7 +12208,7 @@
         <v>433</v>
       </c>
       <c r="B474" s="3" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="475" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12216,7 +12216,7 @@
         <v>434</v>
       </c>
       <c r="B475" s="3" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="476" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12224,7 +12224,7 @@
         <v>435</v>
       </c>
       <c r="B476" s="3" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="477" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12232,7 +12232,7 @@
         <v>436</v>
       </c>
       <c r="B477" s="3" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="478" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -12240,7 +12240,7 @@
         <v>437</v>
       </c>
       <c r="B478" s="3" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="479" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12248,7 +12248,7 @@
         <v>438</v>
       </c>
       <c r="B479" s="3" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="480" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12256,7 +12256,7 @@
         <v>439</v>
       </c>
       <c r="B480" s="3" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="481" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -12264,7 +12264,7 @@
         <v>440</v>
       </c>
       <c r="B481" s="3" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="482" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12272,7 +12272,7 @@
         <v>441</v>
       </c>
       <c r="B482" s="3" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="483" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -12280,7 +12280,7 @@
         <v>442</v>
       </c>
       <c r="B483" s="3" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="484" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -12288,7 +12288,7 @@
         <v>443</v>
       </c>
       <c r="B484" s="3" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="485" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -12296,7 +12296,7 @@
         <v>458</v>
       </c>
       <c r="B485" s="3" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="486" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -12304,7 +12304,7 @@
         <v>466</v>
       </c>
       <c r="B486" s="3" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="487" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -12312,7 +12312,7 @@
         <v>467</v>
       </c>
       <c r="B487" s="3" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="488" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -12320,7 +12320,7 @@
         <v>468</v>
       </c>
       <c r="B488" s="3" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="489" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -12328,7 +12328,7 @@
         <v>552</v>
       </c>
       <c r="B489" s="3" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="490" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -12336,7 +12336,7 @@
         <v>633</v>
       </c>
       <c r="B490" s="3" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="491" spans="1:2" ht="255" x14ac:dyDescent="0.25">
@@ -12344,7 +12344,7 @@
         <v>488</v>
       </c>
       <c r="B491" s="1" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="492" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12352,7 +12352,7 @@
         <v>489</v>
       </c>
       <c r="B492" s="1" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="493" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12360,7 +12360,7 @@
         <v>490</v>
       </c>
       <c r="B493" s="1" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="494" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12368,7 +12368,7 @@
         <v>491</v>
       </c>
       <c r="B494" s="1" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="495" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12376,7 +12376,7 @@
         <v>492</v>
       </c>
       <c r="B495" s="1" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="496" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12384,7 +12384,7 @@
         <v>493</v>
       </c>
       <c r="B496" s="1" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="497" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12392,7 +12392,7 @@
         <v>494</v>
       </c>
       <c r="B497" s="1" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="498" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12400,7 +12400,7 @@
         <v>495</v>
       </c>
       <c r="B498" s="1" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="499" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12408,7 +12408,7 @@
         <v>496</v>
       </c>
       <c r="B499" s="1" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="500" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -12416,7 +12416,7 @@
         <v>497</v>
       </c>
       <c r="B500" s="1" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="501" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12424,7 +12424,7 @@
         <v>498</v>
       </c>
       <c r="B501" s="1" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="502" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12432,7 +12432,7 @@
         <v>499</v>
       </c>
       <c r="B502" s="1" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="503" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -12440,7 +12440,7 @@
         <v>500</v>
       </c>
       <c r="B503" s="1" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="504" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12448,7 +12448,7 @@
         <v>501</v>
       </c>
       <c r="B504" s="1" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="505" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12456,7 +12456,7 @@
         <v>502</v>
       </c>
       <c r="B505" s="1" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="506" spans="1:2" ht="255" x14ac:dyDescent="0.25">
@@ -12464,7 +12464,7 @@
         <v>597</v>
       </c>
       <c r="B506" s="1" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="507" spans="1:2" ht="92.25" x14ac:dyDescent="0.25">
@@ -12472,7 +12472,7 @@
         <v>598</v>
       </c>
       <c r="B507" s="1" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="508" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12480,7 +12480,7 @@
         <v>503</v>
       </c>
       <c r="B508" s="1" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="509" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12488,7 +12488,7 @@
         <v>515</v>
       </c>
       <c r="B509" s="3" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="510" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -12496,7 +12496,7 @@
         <v>423</v>
       </c>
       <c r="B510" s="3" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="511" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12520,7 +12520,7 @@
         <v>267</v>
       </c>
       <c r="B513" s="1" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="514" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12528,7 +12528,7 @@
         <v>268</v>
       </c>
       <c r="B514" s="1" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="515" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12536,7 +12536,7 @@
         <v>269</v>
       </c>
       <c r="B515" s="1" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="516" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12544,7 +12544,7 @@
         <v>270</v>
       </c>
       <c r="B516" s="1" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="517" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12552,7 +12552,7 @@
         <v>271</v>
       </c>
       <c r="B517" s="1" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="518" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12560,7 +12560,7 @@
         <v>272</v>
       </c>
       <c r="B518" s="1" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="519" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12568,7 +12568,7 @@
         <v>273</v>
       </c>
       <c r="B519" s="1" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="520" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12576,7 +12576,7 @@
         <v>274</v>
       </c>
       <c r="B520" s="1" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="521" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12584,7 +12584,7 @@
         <v>275</v>
       </c>
       <c r="B521" s="1" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="522" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12592,7 +12592,7 @@
         <v>276</v>
       </c>
       <c r="B522" s="1" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="523" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12600,7 +12600,7 @@
         <v>277</v>
       </c>
       <c r="B523" s="1" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="524" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12680,7 +12680,7 @@
         <v>280</v>
       </c>
       <c r="B533" s="1" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="534" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12688,7 +12688,7 @@
         <v>281</v>
       </c>
       <c r="B534" s="1" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="535" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12704,7 +12704,7 @@
         <v>283</v>
       </c>
       <c r="B536" s="1" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="537" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12712,7 +12712,7 @@
         <v>284</v>
       </c>
       <c r="B537" s="1" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="538" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12720,7 +12720,7 @@
         <v>285</v>
       </c>
       <c r="B538" s="1" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="539" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12728,7 +12728,7 @@
         <v>286</v>
       </c>
       <c r="B539" s="1" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="540" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12776,7 +12776,7 @@
         <v>292</v>
       </c>
       <c r="B545" s="1" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="546" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12784,7 +12784,7 @@
         <v>293</v>
       </c>
       <c r="B546" s="1" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="547" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12792,7 +12792,7 @@
         <v>294</v>
       </c>
       <c r="B547" s="1" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="548" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12800,7 +12800,7 @@
         <v>295</v>
       </c>
       <c r="B548" s="1" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="549" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -12808,7 +12808,7 @@
         <v>296</v>
       </c>
       <c r="B549" s="1" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="550" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12816,7 +12816,7 @@
         <v>297</v>
       </c>
       <c r="B550" s="1" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
     </row>
     <row r="551" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -12824,7 +12824,7 @@
         <v>353</v>
       </c>
       <c r="B551" s="1" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
     </row>
     <row r="552" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12832,7 +12832,7 @@
         <v>365</v>
       </c>
       <c r="B552" s="3" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="553" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12840,7 +12840,7 @@
         <v>366</v>
       </c>
       <c r="B553" s="1" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="554" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12848,7 +12848,7 @@
         <v>298</v>
       </c>
       <c r="B554" s="1" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="555" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -12856,7 +12856,7 @@
         <v>364</v>
       </c>
       <c r="B555" s="1" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="556" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12864,7 +12864,7 @@
         <v>299</v>
       </c>
       <c r="B556" s="1" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="557" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -12872,7 +12872,7 @@
         <v>354</v>
       </c>
       <c r="B557" s="1" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="558" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -12888,7 +12888,7 @@
         <v>300</v>
       </c>
       <c r="B559" s="1" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="560" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12896,7 +12896,7 @@
         <v>301</v>
       </c>
       <c r="B560" s="1" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="561" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12904,7 +12904,7 @@
         <v>302</v>
       </c>
       <c r="B561" s="1" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="562" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12912,7 +12912,7 @@
         <v>303</v>
       </c>
       <c r="B562" s="1" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="563" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -12920,7 +12920,7 @@
         <v>363</v>
       </c>
       <c r="B563" s="1" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="564" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12928,7 +12928,7 @@
         <v>304</v>
       </c>
       <c r="B564" s="1" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="565" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12936,7 +12936,7 @@
         <v>361</v>
       </c>
       <c r="B565" s="1" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="566" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -12952,7 +12952,7 @@
         <v>517</v>
       </c>
       <c r="B567" s="1" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="568" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12960,7 +12960,7 @@
         <v>305</v>
       </c>
       <c r="B568" s="1" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="569" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12968,7 +12968,7 @@
         <v>358</v>
       </c>
       <c r="B569" s="1" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="570" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12976,7 +12976,7 @@
         <v>359</v>
       </c>
       <c r="B570" s="1" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="571" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -12992,7 +12992,7 @@
         <v>518</v>
       </c>
       <c r="B572" s="1" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="573" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -13000,7 +13000,7 @@
         <v>306</v>
       </c>
       <c r="B573" s="1" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="574" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -13008,7 +13008,7 @@
         <v>352</v>
       </c>
       <c r="B574" s="1" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="575" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -13016,7 +13016,7 @@
         <v>355</v>
       </c>
       <c r="B575" s="3" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="576" spans="1:2" ht="405" x14ac:dyDescent="0.25">
@@ -13024,7 +13024,7 @@
         <v>307</v>
       </c>
       <c r="B576" s="1" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="577" spans="1:2" ht="375" x14ac:dyDescent="0.25">
@@ -13032,7 +13032,7 @@
         <v>311</v>
       </c>
       <c r="B577" s="1" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
     </row>
     <row r="578" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -13056,7 +13056,7 @@
         <v>349</v>
       </c>
       <c r="B580" s="3" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="581" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -13064,7 +13064,7 @@
         <v>519</v>
       </c>
       <c r="B581" s="3" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
     </row>
     <row r="582" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -13072,7 +13072,7 @@
         <v>326</v>
       </c>
       <c r="B582" s="3" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix Rules.xlsx images. Fix time track when over 9 weeks. Fix wizard henchmen shooting fireballs. Removed delay by adding Random to MapItem. Add logging for caching. Turn on that logging.
</commit_message>
<xml_diff>
--- a/Documentation/Events.xlsx
+++ b/Documentation/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\happysulla\BarbarianPrince\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{A1278F85-69E2-46F4-904E-564ED6AF2301}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{00B6A5D9-892E-4CB9-8944-395CC78FF2EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -7468,15 +7468,6 @@
                    &lt;InlineUIContainer&gt;&lt;Image Source='../bin/Images/Temple.gif' Name='Temple' Height='300' Width='400'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e212k High Priest Encounter&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;The High Priest spends an afternoon talking with you.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;&lt;InlineUIContainer&gt;&lt;Button Content='Request' Name='e212l' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; clues for some secret information 
-&lt;InlineUIContainer&gt;&lt;Button Content='e212l' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;&lt;InlineUIContainer&gt;&lt;Button Content='  Use  ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; influence to add 3  in offering Tomorrow. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                   &lt;InlineUIContainer&gt;&lt;Image Source='../bin/Images/Temple.gif' Height='300' Width='400'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;e212l High Priest Provides Secrets&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;The High Priest spends an afternoon talking with you and provides you with clues to some secret information. Roll one die:
  &lt;InlineUIContainer&gt;&lt;Image Source='../bin/Images/dieRoll.gif' Name='DieRoll' Height='21' Width='21'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
@@ -8021,6 +8012,15 @@
  &lt;InlineUIContainer&gt;&lt;Button Content='r225' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.  Click image to continue.
 &lt;LineBreak/&gt;
                    &lt;InlineUIContainer&gt;&lt;Image Name='AncientTreasure' Source='../bin/Images/CoinsStacked.gif' Height='400'  Width='400'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt; </t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e212k High Priest Encounter&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;The High Priest spends an afternoon talking with you. Choose an option.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;&lt;InlineUIContainer&gt;&lt;Button Content='Request' Name='e212l' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; clues for some secret information 
+&lt;InlineUIContainer&gt;&lt;Button Content='e212l' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;&lt;InlineUIContainer&gt;&lt;Button Content='  Use  ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; influence to add 3  in offering Tomorrow. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                   &lt;InlineUIContainer&gt;&lt;Image Source='../bin/Images/Temple.gif' Height='300' Width='400'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
 </sst>
 </file>
@@ -8409,8 +8409,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B582"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A235" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B236" sqref="B236"/>
+    <sheetView tabSelected="1" topLeftCell="A500" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B502" sqref="B502"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9192,7 +9192,7 @@
         <v>61</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10715,7 +10715,7 @@
         <v>915</v>
       </c>
     </row>
-    <row r="288" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A288" s="2" t="s">
         <v>147</v>
       </c>
@@ -12432,7 +12432,7 @@
         <v>499</v>
       </c>
       <c r="B502" s="1" t="s">
-        <v>1104</v>
+        <v>1163</v>
       </c>
     </row>
     <row r="503" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -12440,7 +12440,7 @@
         <v>500</v>
       </c>
       <c r="B503" s="1" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="504" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12448,7 +12448,7 @@
         <v>501</v>
       </c>
       <c r="B504" s="1" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="505" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12456,7 +12456,7 @@
         <v>502</v>
       </c>
       <c r="B505" s="1" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="506" spans="1:2" ht="255" x14ac:dyDescent="0.25">
@@ -12464,15 +12464,15 @@
         <v>597</v>
       </c>
       <c r="B506" s="1" t="s">
-        <v>1108</v>
-      </c>
-    </row>
-    <row r="507" spans="1:2" ht="92.25" x14ac:dyDescent="0.25">
+        <v>1107</v>
+      </c>
+    </row>
+    <row r="507" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A507" s="2" t="s">
         <v>598</v>
       </c>
       <c r="B507" s="1" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="508" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12480,7 +12480,7 @@
         <v>503</v>
       </c>
       <c r="B508" s="1" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="509" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12488,7 +12488,7 @@
         <v>515</v>
       </c>
       <c r="B509" s="3" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="510" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -12496,7 +12496,7 @@
         <v>423</v>
       </c>
       <c r="B510" s="3" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="511" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12520,7 +12520,7 @@
         <v>267</v>
       </c>
       <c r="B513" s="1" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="514" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12528,7 +12528,7 @@
         <v>268</v>
       </c>
       <c r="B514" s="1" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="515" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12536,7 +12536,7 @@
         <v>269</v>
       </c>
       <c r="B515" s="1" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="516" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12544,7 +12544,7 @@
         <v>270</v>
       </c>
       <c r="B516" s="1" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="517" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12552,7 +12552,7 @@
         <v>271</v>
       </c>
       <c r="B517" s="1" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="518" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12560,7 +12560,7 @@
         <v>272</v>
       </c>
       <c r="B518" s="1" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="519" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12568,7 +12568,7 @@
         <v>273</v>
       </c>
       <c r="B519" s="1" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="520" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12576,7 +12576,7 @@
         <v>274</v>
       </c>
       <c r="B520" s="1" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="521" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12584,7 +12584,7 @@
         <v>275</v>
       </c>
       <c r="B521" s="1" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="522" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12592,7 +12592,7 @@
         <v>276</v>
       </c>
       <c r="B522" s="1" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="523" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12600,7 +12600,7 @@
         <v>277</v>
       </c>
       <c r="B523" s="1" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="524" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12680,7 +12680,7 @@
         <v>280</v>
       </c>
       <c r="B533" s="1" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="534" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12688,7 +12688,7 @@
         <v>281</v>
       </c>
       <c r="B534" s="1" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="535" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12704,7 +12704,7 @@
         <v>283</v>
       </c>
       <c r="B536" s="1" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="537" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12712,7 +12712,7 @@
         <v>284</v>
       </c>
       <c r="B537" s="1" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="538" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12720,7 +12720,7 @@
         <v>285</v>
       </c>
       <c r="B538" s="1" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="539" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12728,7 +12728,7 @@
         <v>286</v>
       </c>
       <c r="B539" s="1" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="540" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12776,7 +12776,7 @@
         <v>292</v>
       </c>
       <c r="B545" s="1" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="546" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12784,7 +12784,7 @@
         <v>293</v>
       </c>
       <c r="B546" s="1" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="547" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12792,7 +12792,7 @@
         <v>294</v>
       </c>
       <c r="B547" s="1" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="548" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12800,7 +12800,7 @@
         <v>295</v>
       </c>
       <c r="B548" s="1" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="549" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -12808,7 +12808,7 @@
         <v>296</v>
       </c>
       <c r="B549" s="1" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="550" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12816,7 +12816,7 @@
         <v>297</v>
       </c>
       <c r="B550" s="1" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="551" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -12824,7 +12824,7 @@
         <v>353</v>
       </c>
       <c r="B551" s="1" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
     </row>
     <row r="552" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12832,7 +12832,7 @@
         <v>365</v>
       </c>
       <c r="B552" s="3" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
     </row>
     <row r="553" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12840,7 +12840,7 @@
         <v>366</v>
       </c>
       <c r="B553" s="1" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="554" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12848,7 +12848,7 @@
         <v>298</v>
       </c>
       <c r="B554" s="1" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="555" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -12856,7 +12856,7 @@
         <v>364</v>
       </c>
       <c r="B555" s="1" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="556" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12864,7 +12864,7 @@
         <v>299</v>
       </c>
       <c r="B556" s="1" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="557" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -12872,7 +12872,7 @@
         <v>354</v>
       </c>
       <c r="B557" s="1" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="558" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -12888,7 +12888,7 @@
         <v>300</v>
       </c>
       <c r="B559" s="1" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="560" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12896,7 +12896,7 @@
         <v>301</v>
       </c>
       <c r="B560" s="1" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="561" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12904,7 +12904,7 @@
         <v>302</v>
       </c>
       <c r="B561" s="1" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="562" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12912,7 +12912,7 @@
         <v>303</v>
       </c>
       <c r="B562" s="1" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="563" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -12920,7 +12920,7 @@
         <v>363</v>
       </c>
       <c r="B563" s="1" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="564" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12928,7 +12928,7 @@
         <v>304</v>
       </c>
       <c r="B564" s="1" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="565" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12936,7 +12936,7 @@
         <v>361</v>
       </c>
       <c r="B565" s="1" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="566" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -12952,7 +12952,7 @@
         <v>517</v>
       </c>
       <c r="B567" s="1" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="568" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12960,7 +12960,7 @@
         <v>305</v>
       </c>
       <c r="B568" s="1" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="569" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12968,7 +12968,7 @@
         <v>358</v>
       </c>
       <c r="B569" s="1" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="570" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12976,7 +12976,7 @@
         <v>359</v>
       </c>
       <c r="B570" s="1" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="571" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -12992,7 +12992,7 @@
         <v>518</v>
       </c>
       <c r="B572" s="1" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="573" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -13000,7 +13000,7 @@
         <v>306</v>
       </c>
       <c r="B573" s="1" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="574" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -13008,7 +13008,7 @@
         <v>352</v>
       </c>
       <c r="B574" s="1" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="575" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -13016,7 +13016,7 @@
         <v>355</v>
       </c>
       <c r="B575" s="3" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="576" spans="1:2" ht="405" x14ac:dyDescent="0.25">
@@ -13024,7 +13024,7 @@
         <v>307</v>
       </c>
       <c r="B576" s="1" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="577" spans="1:2" ht="375" x14ac:dyDescent="0.25">
@@ -13032,7 +13032,7 @@
         <v>311</v>
       </c>
       <c r="B577" s="1" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="578" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -13056,7 +13056,7 @@
         <v>349</v>
       </c>
       <c r="B580" s="3" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
     </row>
     <row r="581" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -13064,7 +13064,7 @@
         <v>519</v>
       </c>
       <c r="B581" s="3" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="582" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -13072,7 +13072,7 @@
         <v>326</v>
       </c>
       <c r="B582" s="3" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix issue with Starvation with no rolls. Fix issue with Revert game to in jail
</commit_message>
<xml_diff>
--- a/Documentation/Events.xlsx
+++ b/Documentation/Events.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\happysulla\BarbarianPrince\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{00B6A5D9-892E-4CB9-8944-395CC78FF2EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{455EFE8E-AB41-4A37-9AD4-7F80BA0956C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1164" uniqueCount="1164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1166" uniqueCount="1166">
   <si>
     <t>e001</t>
   </si>
@@ -3871,12 +3871,6 @@
  for the effects of traveling through the arch.</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e045a Arch of Travel With Unknown Runes&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;You find a metal-banded archway inscribed with runes. Since your party does not have a magician, wizard, or witch; the runes are unknown.  Click image to continue.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                          &lt;InlineUIContainer&gt;&lt;Image Name='ArchSkip'  Source='../bin/Images/Arch.gif' Height='300' Width='220'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;e045b Arch of Travel Effects&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;As well as traveling great distances, time will advance on the time track by one die roll. Any travel events still occur, but you cannot get lost by traveling through the arch. Roll one die for number of lost days:
  &lt;InlineUIContainer&gt;&lt;Image Source='../bin/Images/dieRoll.gif' Name='DieRoll' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
@@ -4821,12 +4815,6 @@
                                       &lt;InlineUIContainer&gt;&lt;Image Name='WolvesEncounter' Source='../bin/Images/Wolves.gif' Height='300' Width='204'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e075a Wolves Howling&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;As you eat your evening meal, you hear wolves in the distant howling in hunger. You are glad you are safe. Click image to continue.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                         &lt;InlineUIContainer&gt;&lt;Image Name='EncounterEnd' Source='../bin/Images/WolvesHowling.gif' Height='300' Width='225'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;e075b Wolves Attack Campfire&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 At night, a hunting pack of wolves attacks your party. Each has a combat skill of 3 and endurance 3. Roll three die for the number of wolves: 
@@ -5159,22 +5147,6 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;Start of a new day! You remain stranded and are limited in your daily actions. Select action button from the Daily Actions panel. 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
           &lt;InlineUIContainer&gt;&lt;Image Source='../bin/Images/FloodContinues.gif' Height='155'  Width='500'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e093  Poison Plants&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;You notice poison plants around you today, often a sign of a greater evil. You cannot hunt for food
- &lt;InlineUIContainer&gt;&lt;Button Content='r215' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
- today. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Roll one die for an additional event:  &lt;InlineUIContainer&gt;&lt;Image Source='../bin/Images/dieRoll.gif' Name='DieRoll' Height='21' Width='21' &gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
- 1 - &lt;InlineUIContainer&gt;&lt;Button Content='e034' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;&lt;LineBreak/&gt;
- 2 - &lt;InlineUIContainer&gt;&lt;Button Content='e032' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;&lt;LineBreak/&gt;
- 3 - &lt;InlineUIContainer&gt;&lt;Button Content='e033' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;&lt;LineBreak/&gt;
- 4 - &lt;InlineUIContainer&gt;&lt;Button Content='e074' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;&lt;LineBreak/&gt;
- 5,6 - No additional events
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                               &lt;InlineUIContainer&gt;&lt;Image  Name='PoisonPlant' Source='../bin/Images/PoisonPlant.gif' Height='225' Width='300'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
     <t>&lt;Bold&gt;e094 Crocodiles in Swamp&lt;/Bold&gt;
@@ -8021,6 +7993,41 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;&lt;InlineUIContainer&gt;&lt;Button Content='  Use  ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; influence to add 3  in offering Tomorrow. 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
                    &lt;InlineUIContainer&gt;&lt;Image Source='../bin/Images/Temple.gif' Height='300' Width='400'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e075a Wolves Howling&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;As you eat your evening meal, you hear wolves in the distant howling in hunger. You are glad you are safe. Click image to continue.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                 &lt;InlineUIContainer&gt;&lt;Image Name='EncounterEnd' Source='../bin/Images/WolvesHowling.gif' Height='300' Width='225'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e045a Arch of Travel With Unknown Runes&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;You find a metal-banded archway inscribed with runes. Since your party does not have a magician, wizard, or witch; the runes are unknown.  When you add one to your party, this secret becomes known. Click image to continue.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                          &lt;InlineUIContainer&gt;&lt;Image Name='ArchSkip'  Source='../bin/Images/Arch.gif' Height='300' Width='220'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e093 Poison Plants&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;You notice poison plants around you today, often a sign of a greater evil. You cannot hunt for food
+ &lt;InlineUIContainer&gt;&lt;Button Content='r215' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+ today. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Roll one die for an additional event:  &lt;InlineUIContainer&gt;&lt;Image Source='../bin/Images/dieRoll.gif' Name='DieRoll' Height='21' Width='21' &gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+ 1 - &lt;InlineUIContainer&gt;&lt;Button Content='e034' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;&lt;LineBreak/&gt;
+ 2 - &lt;InlineUIContainer&gt;&lt;Button Content='e032' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;&lt;LineBreak/&gt;
+ 3 - &lt;InlineUIContainer&gt;&lt;Button Content='e033' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;&lt;LineBreak/&gt;
+ 4 - &lt;InlineUIContainer&gt;&lt;Button Content='e074' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;&lt;LineBreak/&gt;
+ 5,6 - No additional events
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                               &lt;InlineUIContainer&gt;&lt;Image  Name='PoisonPlant' Source='../bin/Images/PoisonPlant.gif' Height='225' Width='300'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>e203f</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e203f Wakeup in Bad Straights&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;The game is recovered with you in bad way. Click image to continue.</t>
   </si>
 </sst>
 </file>
@@ -8407,10 +8414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
-  <dimension ref="A1:B582"/>
+  <dimension ref="A1:B583"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A500" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B502" sqref="B502"/>
+    <sheetView tabSelected="1" topLeftCell="A455" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A459" sqref="A459"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9192,7 +9199,7 @@
         <v>61</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>1162</v>
+        <v>1159</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -9448,7 +9455,7 @@
         <v>350</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>765</v>
+        <v>1162</v>
       </c>
     </row>
     <row r="130" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -9456,7 +9463,7 @@
         <v>351</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
     </row>
     <row r="131" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -9464,7 +9471,7 @@
         <v>79</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
     </row>
     <row r="132" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -9472,7 +9479,7 @@
         <v>347</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
     </row>
     <row r="133" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -9480,7 +9487,7 @@
         <v>348</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
     </row>
     <row r="134" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -9488,7 +9495,7 @@
         <v>80</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
     </row>
     <row r="135" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -9496,7 +9503,7 @@
         <v>81</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
     </row>
     <row r="136" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -9504,7 +9511,7 @@
         <v>579</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
     </row>
     <row r="137" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -9512,7 +9519,7 @@
         <v>580</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
     </row>
     <row r="138" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -9520,7 +9527,7 @@
         <v>581</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
     </row>
     <row r="139" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -9528,7 +9535,7 @@
         <v>582</v>
       </c>
       <c r="B139" s="3" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="140" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -9536,7 +9543,7 @@
         <v>583</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="141" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -9544,7 +9551,7 @@
         <v>584</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
     </row>
     <row r="142" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -9552,7 +9559,7 @@
         <v>585</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
     </row>
     <row r="143" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -9560,7 +9567,7 @@
         <v>586</v>
       </c>
       <c r="B143" s="3" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
     </row>
     <row r="144" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -9568,7 +9575,7 @@
         <v>587</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
     </row>
     <row r="145" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -9576,7 +9583,7 @@
         <v>588</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="146" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -9584,7 +9591,7 @@
         <v>82</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
     </row>
     <row r="147" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -9592,7 +9599,7 @@
         <v>83</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
     </row>
     <row r="148" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -9600,7 +9607,7 @@
         <v>614</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="149" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -9608,7 +9615,7 @@
         <v>84</v>
       </c>
       <c r="B149" s="3" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
     </row>
     <row r="150" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -9616,7 +9623,7 @@
         <v>85</v>
       </c>
       <c r="B150" s="3" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="151" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -9624,7 +9631,7 @@
         <v>428</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="152" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -9632,7 +9639,7 @@
         <v>429</v>
       </c>
       <c r="B152" s="3" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="153" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -9640,7 +9647,7 @@
         <v>86</v>
       </c>
       <c r="B153" s="3" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
     </row>
     <row r="154" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -9648,7 +9655,7 @@
         <v>87</v>
       </c>
       <c r="B154" s="3" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
     </row>
     <row r="155" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -9656,7 +9663,7 @@
         <v>334</v>
       </c>
       <c r="B155" s="3" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="156" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -9664,7 +9671,7 @@
         <v>371</v>
       </c>
       <c r="B156" s="3" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
     </row>
     <row r="157" spans="1:2" ht="345" x14ac:dyDescent="0.25">
@@ -9672,7 +9679,7 @@
         <v>88</v>
       </c>
       <c r="B157" s="3" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
     </row>
     <row r="158" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -9680,7 +9687,7 @@
         <v>335</v>
       </c>
       <c r="B158" s="3" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
     </row>
     <row r="159" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -9688,7 +9695,7 @@
         <v>336</v>
       </c>
       <c r="B159" s="3" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
     </row>
     <row r="160" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -9696,7 +9703,7 @@
         <v>337</v>
       </c>
       <c r="B160" s="3" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
     </row>
     <row r="161" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -9704,7 +9711,7 @@
         <v>339</v>
       </c>
       <c r="B161" s="3" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
     </row>
     <row r="162" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -9712,7 +9719,7 @@
         <v>338</v>
       </c>
       <c r="B162" s="3" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
     </row>
     <row r="163" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -9720,7 +9727,7 @@
         <v>340</v>
       </c>
       <c r="B163" s="3" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
     </row>
     <row r="164" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -9728,7 +9735,7 @@
         <v>341</v>
       </c>
       <c r="B164" s="3" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
     </row>
     <row r="165" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -9736,7 +9743,7 @@
         <v>513</v>
       </c>
       <c r="B165" s="3" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
     </row>
     <row r="166" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -9744,7 +9751,7 @@
         <v>89</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
     </row>
     <row r="167" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -9752,7 +9759,7 @@
         <v>377</v>
       </c>
       <c r="B167" s="3" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
     </row>
     <row r="168" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -9760,7 +9767,7 @@
         <v>378</v>
       </c>
       <c r="B168" s="3" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
     </row>
     <row r="169" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -9768,7 +9775,7 @@
         <v>381</v>
       </c>
       <c r="B169" s="3" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
     </row>
     <row r="170" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -9776,7 +9783,7 @@
         <v>90</v>
       </c>
       <c r="B170" s="3" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
     </row>
     <row r="171" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -9784,7 +9791,7 @@
         <v>542</v>
       </c>
       <c r="B171" s="3" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
     </row>
     <row r="172" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -9792,7 +9799,7 @@
         <v>543</v>
       </c>
       <c r="B172" s="3" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
     </row>
     <row r="173" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -9800,7 +9807,7 @@
         <v>91</v>
       </c>
       <c r="B173" s="3" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
     </row>
     <row r="174" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -9808,7 +9815,7 @@
         <v>382</v>
       </c>
       <c r="B174" s="3" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
     </row>
     <row r="175" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -9816,7 +9823,7 @@
         <v>92</v>
       </c>
       <c r="B175" s="3" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
     </row>
     <row r="176" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -9824,7 +9831,7 @@
         <v>93</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
     </row>
     <row r="177" spans="1:2" ht="270" x14ac:dyDescent="0.25">
@@ -9848,7 +9855,7 @@
         <v>96</v>
       </c>
       <c r="B179" s="3" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
     </row>
     <row r="180" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -9856,7 +9863,7 @@
         <v>547</v>
       </c>
       <c r="B180" s="3" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
     </row>
     <row r="181" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -9864,7 +9871,7 @@
         <v>548</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
     </row>
     <row r="182" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -9872,7 +9879,7 @@
         <v>549</v>
       </c>
       <c r="B182" s="3" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
     </row>
     <row r="183" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -9880,7 +9887,7 @@
         <v>550</v>
       </c>
       <c r="B183" s="3" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
     </row>
     <row r="184" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -9888,7 +9895,7 @@
         <v>556</v>
       </c>
       <c r="B184" s="3" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
     </row>
     <row r="185" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -9904,7 +9911,7 @@
         <v>97</v>
       </c>
       <c r="B186" s="3" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="187" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -9912,7 +9919,7 @@
         <v>98</v>
       </c>
       <c r="B187" s="3" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
     </row>
     <row r="188" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -9920,7 +9927,7 @@
         <v>99</v>
       </c>
       <c r="B188" s="3" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
     </row>
     <row r="189" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -9928,7 +9935,7 @@
         <v>101</v>
       </c>
       <c r="B189" s="3" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
     </row>
     <row r="190" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -9936,7 +9943,7 @@
         <v>100</v>
       </c>
       <c r="B190" s="3" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
     </row>
     <row r="191" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -9944,7 +9951,7 @@
         <v>102</v>
       </c>
       <c r="B191" s="3" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
     </row>
     <row r="192" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -9952,7 +9959,7 @@
         <v>103</v>
       </c>
       <c r="B192" s="3" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
     </row>
     <row r="193" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -9960,7 +9967,7 @@
         <v>104</v>
       </c>
       <c r="B193" s="3" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
     </row>
     <row r="194" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -9968,7 +9975,7 @@
         <v>105</v>
       </c>
       <c r="B194" s="3" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
     </row>
     <row r="195" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -9976,7 +9983,7 @@
         <v>504</v>
       </c>
       <c r="B195" s="3" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
     <row r="196" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -9984,7 +9991,7 @@
         <v>505</v>
       </c>
       <c r="B196" s="3" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
     </row>
     <row r="197" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -9992,7 +9999,7 @@
         <v>106</v>
       </c>
       <c r="B197" s="3" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
     </row>
     <row r="198" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10000,7 +10007,7 @@
         <v>107</v>
       </c>
       <c r="B198" s="3" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
     </row>
     <row r="199" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -10008,7 +10015,7 @@
         <v>165</v>
       </c>
       <c r="B199" s="3" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
     </row>
     <row r="200" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -10016,7 +10023,7 @@
         <v>544</v>
       </c>
       <c r="B200" s="3" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
     </row>
     <row r="201" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -10024,7 +10031,7 @@
         <v>108</v>
       </c>
       <c r="B201" s="3" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
     </row>
     <row r="202" spans="1:2" ht="285" x14ac:dyDescent="0.25">
@@ -10032,7 +10039,7 @@
         <v>109</v>
       </c>
       <c r="B202" s="3" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
     <row r="203" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -10040,7 +10047,7 @@
         <v>110</v>
       </c>
       <c r="B203" s="3" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="204" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -10048,7 +10055,7 @@
         <v>166</v>
       </c>
       <c r="B204" s="3" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
     <row r="205" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -10056,7 +10063,7 @@
         <v>167</v>
       </c>
       <c r="B205" s="3" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
     </row>
     <row r="206" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -10064,7 +10071,7 @@
         <v>168</v>
       </c>
       <c r="B206" s="3" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
     </row>
     <row r="207" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -10072,7 +10079,7 @@
         <v>562</v>
       </c>
       <c r="B207" s="3" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
     </row>
     <row r="208" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10088,7 +10095,7 @@
         <v>111</v>
       </c>
       <c r="B209" s="3" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
     </row>
     <row r="210" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10096,7 +10103,7 @@
         <v>510</v>
       </c>
       <c r="B210" s="3" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
     </row>
     <row r="211" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -10104,7 +10111,7 @@
         <v>511</v>
       </c>
       <c r="B211" s="3" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
     </row>
     <row r="212" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -10120,7 +10127,7 @@
         <v>516</v>
       </c>
       <c r="B213" s="3" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
     </row>
     <row r="214" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10128,7 +10135,7 @@
         <v>112</v>
       </c>
       <c r="B214" s="3" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="215" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10136,7 +10143,7 @@
         <v>169</v>
       </c>
       <c r="B215" s="3" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
     </row>
     <row r="216" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10144,7 +10151,7 @@
         <v>170</v>
       </c>
       <c r="B216" s="3" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="217" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10152,7 +10159,7 @@
         <v>171</v>
       </c>
       <c r="B217" s="3" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
     </row>
     <row r="218" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -10160,7 +10167,7 @@
         <v>113</v>
       </c>
       <c r="B218" s="3" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="219" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -10168,7 +10175,7 @@
         <v>114</v>
       </c>
       <c r="B219" s="3" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="220" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10176,7 +10183,7 @@
         <v>266</v>
       </c>
       <c r="B220" s="3" t="s">
-        <v>851</v>
+        <v>1161</v>
       </c>
     </row>
     <row r="221" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -10184,7 +10191,7 @@
         <v>570</v>
       </c>
       <c r="B221" s="3" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
     </row>
     <row r="222" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10192,7 +10199,7 @@
         <v>115</v>
       </c>
       <c r="B222" s="3" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
     </row>
     <row r="223" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10200,7 +10207,7 @@
         <v>522</v>
       </c>
       <c r="B223" s="3" t="s">
-        <v>854</v>
+        <v>852</v>
       </c>
     </row>
     <row r="224" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -10208,7 +10215,7 @@
         <v>116</v>
       </c>
       <c r="B224" s="3" t="s">
-        <v>855</v>
+        <v>853</v>
       </c>
     </row>
     <row r="225" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10216,7 +10223,7 @@
         <v>520</v>
       </c>
       <c r="B225" s="3" t="s">
-        <v>856</v>
+        <v>854</v>
       </c>
     </row>
     <row r="226" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10224,7 +10231,7 @@
         <v>117</v>
       </c>
       <c r="B226" s="4" t="s">
-        <v>857</v>
+        <v>855</v>
       </c>
     </row>
     <row r="227" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10232,7 +10239,7 @@
         <v>523</v>
       </c>
       <c r="B227" s="4" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
     </row>
     <row r="228" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10240,7 +10247,7 @@
         <v>524</v>
       </c>
       <c r="B228" s="4" t="s">
-        <v>859</v>
+        <v>857</v>
       </c>
     </row>
     <row r="229" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10248,7 +10255,7 @@
         <v>525</v>
       </c>
       <c r="B229" s="4" t="s">
-        <v>860</v>
+        <v>858</v>
       </c>
     </row>
     <row r="230" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10256,7 +10263,7 @@
         <v>118</v>
       </c>
       <c r="B230" s="3" t="s">
-        <v>861</v>
+        <v>859</v>
       </c>
     </row>
     <row r="231" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -10264,7 +10271,7 @@
         <v>573</v>
       </c>
       <c r="B231" s="3" t="s">
-        <v>862</v>
+        <v>860</v>
       </c>
     </row>
     <row r="232" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10272,7 +10279,7 @@
         <v>574</v>
       </c>
       <c r="B232" s="3" t="s">
-        <v>863</v>
+        <v>861</v>
       </c>
     </row>
     <row r="233" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10280,7 +10287,7 @@
         <v>119</v>
       </c>
       <c r="B233" s="3" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
     </row>
     <row r="234" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10288,7 +10295,7 @@
         <v>566</v>
       </c>
       <c r="B234" s="3" t="s">
-        <v>865</v>
+        <v>863</v>
       </c>
     </row>
     <row r="235" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10296,7 +10303,7 @@
         <v>565</v>
       </c>
       <c r="B235" s="3" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
     </row>
     <row r="236" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10304,7 +10311,7 @@
         <v>120</v>
       </c>
       <c r="B236" s="3" t="s">
-        <v>867</v>
+        <v>865</v>
       </c>
     </row>
     <row r="237" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -10312,7 +10319,7 @@
         <v>172</v>
       </c>
       <c r="B237" s="3" t="s">
-        <v>868</v>
+        <v>866</v>
       </c>
     </row>
     <row r="238" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10320,7 +10327,7 @@
         <v>173</v>
       </c>
       <c r="B238" s="3" t="s">
-        <v>869</v>
+        <v>867</v>
       </c>
     </row>
     <row r="239" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10328,7 +10335,7 @@
         <v>174</v>
       </c>
       <c r="B239" s="3" t="s">
-        <v>870</v>
+        <v>868</v>
       </c>
     </row>
     <row r="240" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -10336,7 +10343,7 @@
         <v>121</v>
       </c>
       <c r="B240" s="3" t="s">
-        <v>871</v>
+        <v>869</v>
       </c>
     </row>
     <row r="241" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10344,7 +10351,7 @@
         <v>122</v>
       </c>
       <c r="B241" s="3" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
     </row>
     <row r="242" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10352,7 +10359,7 @@
         <v>521</v>
       </c>
       <c r="B242" s="3" t="s">
-        <v>873</v>
+        <v>871</v>
       </c>
     </row>
     <row r="243" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -10360,7 +10367,7 @@
         <v>123</v>
       </c>
       <c r="B243" s="3" t="s">
-        <v>874</v>
+        <v>872</v>
       </c>
     </row>
     <row r="244" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10368,7 +10375,7 @@
         <v>571</v>
       </c>
       <c r="B244" s="3" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
     </row>
     <row r="245" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10376,7 +10383,7 @@
         <v>572</v>
       </c>
       <c r="B245" s="3" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
     </row>
     <row r="246" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10384,7 +10391,7 @@
         <v>124</v>
       </c>
       <c r="B246" s="3" t="s">
-        <v>877</v>
+        <v>875</v>
       </c>
     </row>
     <row r="247" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10392,7 +10399,7 @@
         <v>617</v>
       </c>
       <c r="B247" s="3" t="s">
-        <v>878</v>
+        <v>876</v>
       </c>
     </row>
     <row r="248" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10400,7 +10407,7 @@
         <v>125</v>
       </c>
       <c r="B248" s="3" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
     </row>
     <row r="249" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -10408,7 +10415,7 @@
         <v>589</v>
       </c>
       <c r="B249" s="3" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
     </row>
     <row r="250" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10416,7 +10423,7 @@
         <v>126</v>
       </c>
       <c r="B250" s="3" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
     </row>
     <row r="251" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -10424,7 +10431,7 @@
         <v>127</v>
       </c>
       <c r="B251" s="3" t="s">
-        <v>882</v>
+        <v>880</v>
       </c>
     </row>
     <row r="252" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10432,7 +10439,7 @@
         <v>128</v>
       </c>
       <c r="B252" s="3" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
     </row>
     <row r="253" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -10440,7 +10447,7 @@
         <v>129</v>
       </c>
       <c r="B253" s="3" t="s">
-        <v>884</v>
+        <v>882</v>
       </c>
     </row>
     <row r="254" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10448,7 +10455,7 @@
         <v>130</v>
       </c>
       <c r="B254" s="3" t="s">
-        <v>885</v>
+        <v>883</v>
       </c>
     </row>
     <row r="255" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -10456,7 +10463,7 @@
         <v>131</v>
       </c>
       <c r="B255" s="3" t="s">
-        <v>886</v>
+        <v>884</v>
       </c>
     </row>
     <row r="256" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -10464,7 +10471,7 @@
         <v>576</v>
       </c>
       <c r="B256" s="3" t="s">
-        <v>887</v>
+        <v>885</v>
       </c>
     </row>
     <row r="257" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10472,7 +10479,7 @@
         <v>577</v>
       </c>
       <c r="B257" s="3" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
     </row>
     <row r="258" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -10480,7 +10487,7 @@
         <v>132</v>
       </c>
       <c r="B258" s="3" t="s">
-        <v>889</v>
+        <v>1163</v>
       </c>
     </row>
     <row r="259" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10488,7 +10495,7 @@
         <v>133</v>
       </c>
       <c r="B259" s="3" t="s">
-        <v>890</v>
+        <v>887</v>
       </c>
     </row>
     <row r="260" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10496,7 +10503,7 @@
         <v>575</v>
       </c>
       <c r="B260" s="3" t="s">
-        <v>891</v>
+        <v>888</v>
       </c>
     </row>
     <row r="261" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -10504,7 +10511,7 @@
         <v>134</v>
       </c>
       <c r="B261" s="3" t="s">
-        <v>892</v>
+        <v>889</v>
       </c>
     </row>
     <row r="262" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10512,7 +10519,7 @@
         <v>590</v>
       </c>
       <c r="B262" s="3" t="s">
-        <v>893</v>
+        <v>890</v>
       </c>
     </row>
     <row r="263" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10520,7 +10527,7 @@
         <v>591</v>
       </c>
       <c r="B263" s="3" t="s">
-        <v>894</v>
+        <v>891</v>
       </c>
     </row>
     <row r="264" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -10528,7 +10535,7 @@
         <v>135</v>
       </c>
       <c r="B264" s="3" t="s">
-        <v>895</v>
+        <v>892</v>
       </c>
     </row>
     <row r="265" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -10536,7 +10543,7 @@
         <v>592</v>
       </c>
       <c r="B265" s="3" t="s">
-        <v>896</v>
+        <v>893</v>
       </c>
     </row>
     <row r="266" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10544,7 +10551,7 @@
         <v>136</v>
       </c>
       <c r="B266" s="3" t="s">
-        <v>897</v>
+        <v>894</v>
       </c>
     </row>
     <row r="267" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -10552,7 +10559,7 @@
         <v>137</v>
       </c>
       <c r="B267" s="3" t="s">
-        <v>898</v>
+        <v>895</v>
       </c>
     </row>
     <row r="268" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10560,7 +10567,7 @@
         <v>232</v>
       </c>
       <c r="B268" s="3" t="s">
-        <v>899</v>
+        <v>896</v>
       </c>
     </row>
     <row r="269" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10568,7 +10575,7 @@
         <v>233</v>
       </c>
       <c r="B269" s="3" t="s">
-        <v>900</v>
+        <v>897</v>
       </c>
     </row>
     <row r="270" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -10584,7 +10591,7 @@
         <v>234</v>
       </c>
       <c r="B271" s="3" t="s">
-        <v>901</v>
+        <v>898</v>
       </c>
     </row>
     <row r="272" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10592,7 +10599,7 @@
         <v>235</v>
       </c>
       <c r="B272" s="3" t="s">
-        <v>902</v>
+        <v>899</v>
       </c>
     </row>
     <row r="273" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -10608,7 +10615,7 @@
         <v>239</v>
       </c>
       <c r="B274" s="3" t="s">
-        <v>903</v>
+        <v>900</v>
       </c>
     </row>
     <row r="275" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10616,7 +10623,7 @@
         <v>240</v>
       </c>
       <c r="B275" s="3" t="s">
-        <v>904</v>
+        <v>901</v>
       </c>
     </row>
     <row r="276" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10624,7 +10631,7 @@
         <v>241</v>
       </c>
       <c r="B276" s="3" t="s">
-        <v>905</v>
+        <v>902</v>
       </c>
     </row>
     <row r="277" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10640,7 +10647,7 @@
         <v>236</v>
       </c>
       <c r="B278" s="3" t="s">
-        <v>906</v>
+        <v>903</v>
       </c>
     </row>
     <row r="279" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10648,7 +10655,7 @@
         <v>237</v>
       </c>
       <c r="B279" s="3" t="s">
-        <v>907</v>
+        <v>904</v>
       </c>
     </row>
     <row r="280" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10656,7 +10663,7 @@
         <v>238</v>
       </c>
       <c r="B280" s="3" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
     </row>
     <row r="281" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10664,7 +10671,7 @@
         <v>141</v>
       </c>
       <c r="B281" s="3" t="s">
-        <v>909</v>
+        <v>906</v>
       </c>
     </row>
     <row r="282" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10672,7 +10679,7 @@
         <v>142</v>
       </c>
       <c r="B282" s="3" t="s">
-        <v>910</v>
+        <v>907</v>
       </c>
     </row>
     <row r="283" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10680,7 +10687,7 @@
         <v>143</v>
       </c>
       <c r="B283" s="3" t="s">
-        <v>911</v>
+        <v>908</v>
       </c>
     </row>
     <row r="284" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -10688,7 +10695,7 @@
         <v>144</v>
       </c>
       <c r="B284" s="3" t="s">
-        <v>912</v>
+        <v>909</v>
       </c>
     </row>
     <row r="285" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10696,7 +10703,7 @@
         <v>242</v>
       </c>
       <c r="B285" s="3" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
     </row>
     <row r="286" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10704,7 +10711,7 @@
         <v>145</v>
       </c>
       <c r="B286" s="3" t="s">
-        <v>914</v>
+        <v>911</v>
       </c>
     </row>
     <row r="287" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10712,7 +10719,7 @@
         <v>146</v>
       </c>
       <c r="B287" s="3" t="s">
-        <v>915</v>
+        <v>912</v>
       </c>
     </row>
     <row r="288" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10720,7 +10727,7 @@
         <v>147</v>
       </c>
       <c r="B288" s="3" t="s">
-        <v>916</v>
+        <v>913</v>
       </c>
     </row>
     <row r="289" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10728,7 +10735,7 @@
         <v>148</v>
       </c>
       <c r="B289" s="3" t="s">
-        <v>917</v>
+        <v>914</v>
       </c>
     </row>
     <row r="290" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10736,7 +10743,7 @@
         <v>149</v>
       </c>
       <c r="B290" s="3" t="s">
-        <v>918</v>
+        <v>915</v>
       </c>
     </row>
     <row r="291" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10744,7 +10751,7 @@
         <v>605</v>
       </c>
       <c r="B291" s="3" t="s">
-        <v>919</v>
+        <v>916</v>
       </c>
     </row>
     <row r="292" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10752,7 +10759,7 @@
         <v>604</v>
       </c>
       <c r="B292" s="3" t="s">
-        <v>920</v>
+        <v>917</v>
       </c>
     </row>
     <row r="293" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10760,7 +10767,7 @@
         <v>606</v>
       </c>
       <c r="B293" s="3" t="s">
-        <v>921</v>
+        <v>918</v>
       </c>
     </row>
     <row r="294" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10768,7 +10775,7 @@
         <v>150</v>
       </c>
       <c r="B294" s="3" t="s">
-        <v>922</v>
+        <v>919</v>
       </c>
     </row>
     <row r="295" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10776,7 +10783,7 @@
         <v>607</v>
       </c>
       <c r="B295" s="3" t="s">
-        <v>923</v>
+        <v>920</v>
       </c>
     </row>
     <row r="296" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -10784,7 +10791,7 @@
         <v>151</v>
       </c>
       <c r="B296" s="3" t="s">
-        <v>924</v>
+        <v>921</v>
       </c>
     </row>
     <row r="297" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10792,7 +10799,7 @@
         <v>243</v>
       </c>
       <c r="B297" s="3" t="s">
-        <v>925</v>
+        <v>922</v>
       </c>
     </row>
     <row r="298" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10800,7 +10807,7 @@
         <v>244</v>
       </c>
       <c r="B298" s="3" t="s">
-        <v>926</v>
+        <v>923</v>
       </c>
     </row>
     <row r="299" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10808,7 +10815,7 @@
         <v>245</v>
       </c>
       <c r="B299" s="3" t="s">
-        <v>927</v>
+        <v>924</v>
       </c>
     </row>
     <row r="300" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10816,7 +10823,7 @@
         <v>152</v>
       </c>
       <c r="B300" s="3" t="s">
-        <v>928</v>
+        <v>925</v>
       </c>
     </row>
     <row r="301" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10824,7 +10831,7 @@
         <v>153</v>
       </c>
       <c r="B301" s="3" t="s">
-        <v>929</v>
+        <v>926</v>
       </c>
     </row>
     <row r="302" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10832,7 +10839,7 @@
         <v>154</v>
       </c>
       <c r="B302" s="3" t="s">
-        <v>930</v>
+        <v>927</v>
       </c>
     </row>
     <row r="303" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -10840,7 +10847,7 @@
         <v>155</v>
       </c>
       <c r="B303" s="3" t="s">
-        <v>931</v>
+        <v>928</v>
       </c>
     </row>
     <row r="304" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10848,7 +10855,7 @@
         <v>156</v>
       </c>
       <c r="B304" s="3" t="s">
-        <v>932</v>
+        <v>929</v>
       </c>
     </row>
     <row r="305" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10864,7 +10871,7 @@
         <v>246</v>
       </c>
       <c r="B306" s="3" t="s">
-        <v>933</v>
+        <v>930</v>
       </c>
     </row>
     <row r="307" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10872,7 +10879,7 @@
         <v>247</v>
       </c>
       <c r="B307" s="3" t="s">
-        <v>934</v>
+        <v>931</v>
       </c>
     </row>
     <row r="308" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10880,7 +10887,7 @@
         <v>248</v>
       </c>
       <c r="B308" s="3" t="s">
-        <v>935</v>
+        <v>932</v>
       </c>
     </row>
     <row r="309" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10896,7 +10903,7 @@
         <v>159</v>
       </c>
       <c r="B310" s="3" t="s">
-        <v>936</v>
+        <v>933</v>
       </c>
     </row>
     <row r="311" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10904,7 +10911,7 @@
         <v>160</v>
       </c>
       <c r="B311" s="3" t="s">
-        <v>937</v>
+        <v>934</v>
       </c>
     </row>
     <row r="312" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -10912,7 +10919,7 @@
         <v>161</v>
       </c>
       <c r="B312" s="3" t="s">
-        <v>938</v>
+        <v>935</v>
       </c>
     </row>
     <row r="313" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -10920,7 +10927,7 @@
         <v>162</v>
       </c>
       <c r="B313" s="3" t="s">
-        <v>939</v>
+        <v>936</v>
       </c>
     </row>
     <row r="314" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -10928,7 +10935,7 @@
         <v>599</v>
       </c>
       <c r="B314" s="3" t="s">
-        <v>940</v>
+        <v>937</v>
       </c>
     </row>
     <row r="315" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10936,7 +10943,7 @@
         <v>600</v>
       </c>
       <c r="B315" s="3" t="s">
-        <v>941</v>
+        <v>938</v>
       </c>
     </row>
     <row r="316" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10944,7 +10951,7 @@
         <v>601</v>
       </c>
       <c r="B316" s="3" t="s">
-        <v>942</v>
+        <v>939</v>
       </c>
     </row>
     <row r="317" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10952,7 +10959,7 @@
         <v>163</v>
       </c>
       <c r="B317" s="3" t="s">
-        <v>943</v>
+        <v>940</v>
       </c>
     </row>
     <row r="318" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10960,7 +10967,7 @@
         <v>164</v>
       </c>
       <c r="B318" s="3" t="s">
-        <v>944</v>
+        <v>941</v>
       </c>
     </row>
     <row r="319" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10968,7 +10975,7 @@
         <v>175</v>
       </c>
       <c r="B319" s="3" t="s">
-        <v>945</v>
+        <v>942</v>
       </c>
     </row>
     <row r="320" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -10976,7 +10983,7 @@
         <v>176</v>
       </c>
       <c r="B320" s="3" t="s">
-        <v>946</v>
+        <v>943</v>
       </c>
     </row>
     <row r="321" spans="1:2" ht="390" x14ac:dyDescent="0.25">
@@ -10984,7 +10991,7 @@
         <v>177</v>
       </c>
       <c r="B321" s="3" t="s">
-        <v>947</v>
+        <v>944</v>
       </c>
     </row>
     <row r="322" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -11000,7 +11007,7 @@
         <v>414</v>
       </c>
       <c r="B323" s="3" t="s">
-        <v>948</v>
+        <v>945</v>
       </c>
     </row>
     <row r="324" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11008,7 +11015,7 @@
         <v>415</v>
       </c>
       <c r="B324" s="3" t="s">
-        <v>949</v>
+        <v>946</v>
       </c>
     </row>
     <row r="325" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -11016,7 +11023,7 @@
         <v>416</v>
       </c>
       <c r="B325" s="3" t="s">
-        <v>950</v>
+        <v>947</v>
       </c>
     </row>
     <row r="326" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -11024,7 +11031,7 @@
         <v>417</v>
       </c>
       <c r="B326" s="3" t="s">
-        <v>951</v>
+        <v>948</v>
       </c>
     </row>
     <row r="327" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11032,7 +11039,7 @@
         <v>418</v>
       </c>
       <c r="B327" s="3" t="s">
-        <v>952</v>
+        <v>949</v>
       </c>
     </row>
     <row r="328" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11040,7 +11047,7 @@
         <v>613</v>
       </c>
       <c r="B328" s="3" t="s">
-        <v>953</v>
+        <v>950</v>
       </c>
     </row>
     <row r="329" spans="1:2" ht="390" x14ac:dyDescent="0.25">
@@ -11048,7 +11055,7 @@
         <v>178</v>
       </c>
       <c r="B329" s="3" t="s">
-        <v>954</v>
+        <v>951</v>
       </c>
     </row>
     <row r="330" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -11064,7 +11071,7 @@
         <v>426</v>
       </c>
       <c r="B331" s="3" t="s">
-        <v>955</v>
+        <v>952</v>
       </c>
     </row>
     <row r="332" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11072,7 +11079,7 @@
         <v>427</v>
       </c>
       <c r="B332" s="3" t="s">
-        <v>956</v>
+        <v>953</v>
       </c>
     </row>
     <row r="333" spans="1:2" ht="315" x14ac:dyDescent="0.25">
@@ -11080,7 +11087,7 @@
         <v>179</v>
       </c>
       <c r="B333" s="3" t="s">
-        <v>957</v>
+        <v>954</v>
       </c>
     </row>
     <row r="334" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -11088,7 +11095,7 @@
         <v>249</v>
       </c>
       <c r="B334" s="3" t="s">
-        <v>958</v>
+        <v>955</v>
       </c>
     </row>
     <row r="335" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -11096,7 +11103,7 @@
         <v>250</v>
       </c>
       <c r="B335" s="3" t="s">
-        <v>959</v>
+        <v>956</v>
       </c>
     </row>
     <row r="336" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -11104,7 +11111,7 @@
         <v>251</v>
       </c>
       <c r="B336" s="3" t="s">
-        <v>960</v>
+        <v>957</v>
       </c>
     </row>
     <row r="337" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11112,7 +11119,7 @@
         <v>252</v>
       </c>
       <c r="B337" s="3" t="s">
-        <v>961</v>
+        <v>958</v>
       </c>
     </row>
     <row r="338" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -11120,7 +11127,7 @@
         <v>253</v>
       </c>
       <c r="B338" s="3" t="s">
-        <v>962</v>
+        <v>959</v>
       </c>
     </row>
     <row r="339" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -11128,7 +11135,7 @@
         <v>545</v>
       </c>
       <c r="B339" s="3" t="s">
-        <v>963</v>
+        <v>960</v>
       </c>
     </row>
     <row r="340" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -11136,7 +11143,7 @@
         <v>546</v>
       </c>
       <c r="B340" s="3" t="s">
-        <v>964</v>
+        <v>961</v>
       </c>
     </row>
     <row r="341" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11144,7 +11151,7 @@
         <v>180</v>
       </c>
       <c r="B341" s="3" t="s">
-        <v>965</v>
+        <v>962</v>
       </c>
     </row>
     <row r="342" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11152,7 +11159,7 @@
         <v>181</v>
       </c>
       <c r="B342" s="3" t="s">
-        <v>966</v>
+        <v>963</v>
       </c>
     </row>
     <row r="343" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11160,7 +11167,7 @@
         <v>386</v>
       </c>
       <c r="B343" s="3" t="s">
-        <v>967</v>
+        <v>964</v>
       </c>
     </row>
     <row r="344" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -11176,7 +11183,7 @@
         <v>622</v>
       </c>
       <c r="B345" s="3" t="s">
-        <v>968</v>
+        <v>965</v>
       </c>
     </row>
     <row r="346" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11184,7 +11191,7 @@
         <v>183</v>
       </c>
       <c r="B346" s="3" t="s">
-        <v>969</v>
+        <v>966</v>
       </c>
     </row>
     <row r="347" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -11192,7 +11199,7 @@
         <v>184</v>
       </c>
       <c r="B347" s="3" t="s">
-        <v>970</v>
+        <v>967</v>
       </c>
     </row>
     <row r="348" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -11208,7 +11215,7 @@
         <v>185</v>
       </c>
       <c r="B349" s="3" t="s">
-        <v>971</v>
+        <v>968</v>
       </c>
     </row>
     <row r="350" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -11216,7 +11223,7 @@
         <v>186</v>
       </c>
       <c r="B350" s="3" t="s">
-        <v>972</v>
+        <v>969</v>
       </c>
     </row>
     <row r="351" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -11224,7 +11231,7 @@
         <v>187</v>
       </c>
       <c r="B351" s="3" t="s">
-        <v>973</v>
+        <v>970</v>
       </c>
     </row>
     <row r="352" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11240,7 +11247,7 @@
         <v>188</v>
       </c>
       <c r="B353" s="3" t="s">
-        <v>974</v>
+        <v>971</v>
       </c>
     </row>
     <row r="354" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -11248,7 +11255,7 @@
         <v>189</v>
       </c>
       <c r="B354" s="3" t="s">
-        <v>975</v>
+        <v>972</v>
       </c>
     </row>
     <row r="355" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -11256,7 +11263,7 @@
         <v>383</v>
       </c>
       <c r="B355" s="3" t="s">
-        <v>976</v>
+        <v>973</v>
       </c>
     </row>
     <row r="356" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -11264,7 +11271,7 @@
         <v>384</v>
       </c>
       <c r="B356" s="3" t="s">
-        <v>977</v>
+        <v>974</v>
       </c>
     </row>
     <row r="357" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -11272,7 +11279,7 @@
         <v>190</v>
       </c>
       <c r="B357" s="3" t="s">
-        <v>978</v>
+        <v>975</v>
       </c>
     </row>
     <row r="358" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -11280,7 +11287,7 @@
         <v>191</v>
       </c>
       <c r="B358" s="3" t="s">
-        <v>979</v>
+        <v>976</v>
       </c>
     </row>
     <row r="359" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -11288,7 +11295,7 @@
         <v>192</v>
       </c>
       <c r="B359" s="3" t="s">
-        <v>980</v>
+        <v>977</v>
       </c>
     </row>
     <row r="360" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -11296,7 +11303,7 @@
         <v>465</v>
       </c>
       <c r="B360" s="3" t="s">
-        <v>981</v>
+        <v>978</v>
       </c>
     </row>
     <row r="361" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -11304,7 +11311,7 @@
         <v>193</v>
       </c>
       <c r="B361" s="3" t="s">
-        <v>982</v>
+        <v>979</v>
       </c>
     </row>
     <row r="362" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -11320,7 +11327,7 @@
         <v>333</v>
       </c>
       <c r="B363" s="3" t="s">
-        <v>983</v>
+        <v>980</v>
       </c>
     </row>
     <row r="364" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -11328,7 +11335,7 @@
         <v>624</v>
       </c>
       <c r="B364" s="3" t="s">
-        <v>984</v>
+        <v>981</v>
       </c>
     </row>
     <row r="365" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -11336,7 +11343,7 @@
         <v>625</v>
       </c>
       <c r="B365" s="3" t="s">
-        <v>985</v>
+        <v>982</v>
       </c>
     </row>
     <row r="366" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11344,7 +11351,7 @@
         <v>627</v>
       </c>
       <c r="B366" s="3" t="s">
-        <v>986</v>
+        <v>983</v>
       </c>
     </row>
     <row r="367" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11352,7 +11359,7 @@
         <v>628</v>
       </c>
       <c r="B367" s="3" t="s">
-        <v>987</v>
+        <v>984</v>
       </c>
     </row>
     <row r="368" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11360,7 +11367,7 @@
         <v>629</v>
       </c>
       <c r="B368" s="3" t="s">
-        <v>988</v>
+        <v>985</v>
       </c>
     </row>
     <row r="369" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11368,7 +11375,7 @@
         <v>630</v>
       </c>
       <c r="B369" s="3" t="s">
-        <v>989</v>
+        <v>986</v>
       </c>
     </row>
     <row r="370" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11376,7 +11383,7 @@
         <v>631</v>
       </c>
       <c r="B370" s="3" t="s">
-        <v>990</v>
+        <v>987</v>
       </c>
     </row>
     <row r="371" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11384,7 +11391,7 @@
         <v>632</v>
       </c>
       <c r="B371" s="3" t="s">
-        <v>991</v>
+        <v>988</v>
       </c>
     </row>
     <row r="372" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -11392,7 +11399,7 @@
         <v>194</v>
       </c>
       <c r="B372" s="3" t="s">
-        <v>992</v>
+        <v>989</v>
       </c>
     </row>
     <row r="373" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -11400,7 +11407,7 @@
         <v>195</v>
       </c>
       <c r="B373" s="3" t="s">
-        <v>993</v>
+        <v>990</v>
       </c>
     </row>
     <row r="374" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -11408,7 +11415,7 @@
         <v>620</v>
       </c>
       <c r="B374" s="3" t="s">
-        <v>994</v>
+        <v>991</v>
       </c>
     </row>
     <row r="375" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -11416,7 +11423,7 @@
         <v>196</v>
       </c>
       <c r="B375" s="3" t="s">
-        <v>995</v>
+        <v>992</v>
       </c>
     </row>
     <row r="376" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -11424,7 +11431,7 @@
         <v>328</v>
       </c>
       <c r="B376" s="3" t="s">
-        <v>996</v>
+        <v>993</v>
       </c>
     </row>
     <row r="377" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -11432,7 +11439,7 @@
         <v>197</v>
       </c>
       <c r="B377" s="3" t="s">
-        <v>997</v>
+        <v>994</v>
       </c>
     </row>
     <row r="378" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11440,7 +11447,7 @@
         <v>487</v>
       </c>
       <c r="B378" s="3" t="s">
-        <v>998</v>
+        <v>995</v>
       </c>
     </row>
     <row r="379" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11448,7 +11455,7 @@
         <v>198</v>
       </c>
       <c r="B379" s="3" t="s">
-        <v>999</v>
+        <v>996</v>
       </c>
     </row>
     <row r="380" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11456,7 +11463,7 @@
         <v>199</v>
       </c>
       <c r="B380" s="3" t="s">
-        <v>1000</v>
+        <v>997</v>
       </c>
     </row>
     <row r="381" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -11464,7 +11471,7 @@
         <v>200</v>
       </c>
       <c r="B381" s="3" t="s">
-        <v>1001</v>
+        <v>998</v>
       </c>
     </row>
     <row r="382" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11472,7 +11479,7 @@
         <v>201</v>
       </c>
       <c r="B382" s="3" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
     </row>
     <row r="383" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11480,7 +11487,7 @@
         <v>202</v>
       </c>
       <c r="B383" s="3" t="s">
-        <v>1003</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="384" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -11488,7 +11495,7 @@
         <v>203</v>
       </c>
       <c r="B384" s="3" t="s">
-        <v>1004</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="385" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -11536,7 +11543,7 @@
         <v>204</v>
       </c>
       <c r="B390" s="3" t="s">
-        <v>1005</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="391" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11544,7 +11551,7 @@
         <v>459</v>
       </c>
       <c r="B391" s="3" t="s">
-        <v>1006</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="392" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11552,7 +11559,7 @@
         <v>460</v>
       </c>
       <c r="B392" s="3" t="s">
-        <v>1007</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="393" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11560,7 +11567,7 @@
         <v>461</v>
       </c>
       <c r="B393" s="3" t="s">
-        <v>1008</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="394" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11568,7 +11575,7 @@
         <v>462</v>
       </c>
       <c r="B394" s="3" t="s">
-        <v>1009</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="395" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11576,7 +11583,7 @@
         <v>463</v>
       </c>
       <c r="B395" s="3" t="s">
-        <v>1010</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="396" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11584,7 +11591,7 @@
         <v>464</v>
       </c>
       <c r="B396" s="3" t="s">
-        <v>1011</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="397" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -11592,7 +11599,7 @@
         <v>205</v>
       </c>
       <c r="B397" s="3" t="s">
-        <v>1012</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="398" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -11664,7 +11671,7 @@
         <v>207</v>
       </c>
       <c r="B406" s="3" t="s">
-        <v>1013</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="407" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -11672,7 +11679,7 @@
         <v>208</v>
       </c>
       <c r="B407" s="3" t="s">
-        <v>1014</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="408" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -11680,7 +11687,7 @@
         <v>209</v>
       </c>
       <c r="B408" s="3" t="s">
-        <v>1015</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="409" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11688,7 +11695,7 @@
         <v>476</v>
       </c>
       <c r="B409" s="3" t="s">
-        <v>1016</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="410" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11696,7 +11703,7 @@
         <v>477</v>
       </c>
       <c r="B410" s="3" t="s">
-        <v>1017</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="411" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11704,7 +11711,7 @@
         <v>478</v>
       </c>
       <c r="B411" s="3" t="s">
-        <v>1018</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="412" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -11712,7 +11719,7 @@
         <v>479</v>
       </c>
       <c r="B412" s="3" t="s">
-        <v>1019</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="413" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -11720,7 +11727,7 @@
         <v>480</v>
       </c>
       <c r="B413" s="4" t="s">
-        <v>1020</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="414" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -11728,7 +11735,7 @@
         <v>481</v>
       </c>
       <c r="B414" s="3" t="s">
-        <v>1021</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="415" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -11736,7 +11743,7 @@
         <v>621</v>
       </c>
       <c r="B415" s="3" t="s">
-        <v>1022</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="416" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -11744,7 +11751,7 @@
         <v>210</v>
       </c>
       <c r="B416" s="3" t="s">
-        <v>1023</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="417" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11752,7 +11759,7 @@
         <v>469</v>
       </c>
       <c r="B417" s="3" t="s">
-        <v>1024</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="418" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11760,7 +11767,7 @@
         <v>470</v>
       </c>
       <c r="B418" s="3" t="s">
-        <v>1025</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="419" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11768,7 +11775,7 @@
         <v>471</v>
       </c>
       <c r="B419" s="3" t="s">
-        <v>1026</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="420" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11776,7 +11783,7 @@
         <v>472</v>
       </c>
       <c r="B420" s="3" t="s">
-        <v>1027</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="421" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11784,7 +11791,7 @@
         <v>473</v>
       </c>
       <c r="B421" s="3" t="s">
-        <v>1028</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="422" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11792,7 +11799,7 @@
         <v>474</v>
       </c>
       <c r="B422" s="3" t="s">
-        <v>1029</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="423" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11800,7 +11807,7 @@
         <v>475</v>
       </c>
       <c r="B423" s="3" t="s">
-        <v>1030</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="424" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11808,7 +11815,7 @@
         <v>619</v>
       </c>
       <c r="B424" s="3" t="s">
-        <v>1031</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="425" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -11816,7 +11823,7 @@
         <v>211</v>
       </c>
       <c r="B425" s="3" t="s">
-        <v>1032</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="426" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11824,7 +11831,7 @@
         <v>212</v>
       </c>
       <c r="B426" s="3" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="427" spans="1:2" ht="300" x14ac:dyDescent="0.25">
@@ -11832,7 +11839,7 @@
         <v>419</v>
       </c>
       <c r="B427" s="3" t="s">
-        <v>1034</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="428" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11840,7 +11847,7 @@
         <v>420</v>
       </c>
       <c r="B428" s="3" t="s">
-        <v>1035</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="429" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -11848,7 +11855,7 @@
         <v>421</v>
       </c>
       <c r="B429" s="3" t="s">
-        <v>1036</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="430" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11856,7 +11863,7 @@
         <v>422</v>
       </c>
       <c r="B430" s="3" t="s">
-        <v>1037</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="431" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -11864,7 +11871,7 @@
         <v>213</v>
       </c>
       <c r="B431" s="3" t="s">
-        <v>1038</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="432" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -11872,7 +11879,7 @@
         <v>214</v>
       </c>
       <c r="B432" s="3" t="s">
-        <v>1039</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="433" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -11880,7 +11887,7 @@
         <v>215</v>
       </c>
       <c r="B433" s="3" t="s">
-        <v>1040</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="434" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11888,7 +11895,7 @@
         <v>216</v>
       </c>
       <c r="B434" s="3" t="s">
-        <v>1041</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="435" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11896,7 +11903,7 @@
         <v>217</v>
       </c>
       <c r="B435" s="3" t="s">
-        <v>1042</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="436" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11904,7 +11911,7 @@
         <v>218</v>
       </c>
       <c r="B436" s="3" t="s">
-        <v>1043</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="437" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11912,7 +11919,7 @@
         <v>219</v>
       </c>
       <c r="B437" s="3" t="s">
-        <v>1044</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="438" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11920,7 +11927,7 @@
         <v>220</v>
       </c>
       <c r="B438" s="3" t="s">
-        <v>1045</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="439" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11928,7 +11935,7 @@
         <v>221</v>
       </c>
       <c r="B439" s="3" t="s">
-        <v>1046</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="440" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11936,7 +11943,7 @@
         <v>222</v>
       </c>
       <c r="B440" s="3" t="s">
-        <v>1047</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="441" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11944,7 +11951,7 @@
         <v>223</v>
       </c>
       <c r="B441" s="3" t="s">
-        <v>1048</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="442" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -11952,7 +11959,7 @@
         <v>224</v>
       </c>
       <c r="B442" s="3" t="s">
-        <v>1049</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="443" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -11960,7 +11967,7 @@
         <v>329</v>
       </c>
       <c r="B443" s="3" t="s">
-        <v>1050</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="444" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11968,7 +11975,7 @@
         <v>385</v>
       </c>
       <c r="B444" s="3" t="s">
-        <v>1051</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="445" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11976,7 +11983,7 @@
         <v>225</v>
       </c>
       <c r="B445" s="3" t="s">
-        <v>1052</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="446" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -11984,7 +11991,7 @@
         <v>226</v>
       </c>
       <c r="B446" s="3" t="s">
-        <v>1053</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="447" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -11992,7 +11999,7 @@
         <v>227</v>
       </c>
       <c r="B447" s="3" t="s">
-        <v>1054</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="448" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -12000,7 +12007,7 @@
         <v>228</v>
       </c>
       <c r="B448" s="3" t="s">
-        <v>1055</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="449" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -12008,7 +12015,7 @@
         <v>618</v>
       </c>
       <c r="B449" s="3" t="s">
-        <v>1056</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="450" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12016,7 +12023,7 @@
         <v>229</v>
       </c>
       <c r="B450" s="3" t="s">
-        <v>1057</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="451" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -12024,7 +12031,7 @@
         <v>230</v>
       </c>
       <c r="B451" s="3" t="s">
-        <v>1058</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="452" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -12032,7 +12039,7 @@
         <v>231</v>
       </c>
       <c r="B452" s="3" t="s">
-        <v>1059</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="453" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12040,7 +12047,7 @@
         <v>257</v>
       </c>
       <c r="B453" s="3" t="s">
-        <v>1060</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="454" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -12048,7 +12055,7 @@
         <v>379</v>
       </c>
       <c r="B454" s="3" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="455" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12056,7 +12063,7 @@
         <v>380</v>
       </c>
       <c r="B455" s="3" t="s">
-        <v>1062</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="456" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12064,7 +12071,7 @@
         <v>444</v>
       </c>
       <c r="B456" s="3" t="s">
-        <v>1063</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="457" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12080,1004 +12087,1012 @@
         <v>531</v>
       </c>
       <c r="B458" s="3" t="s">
-        <v>1064</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="459" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A459" s="2" t="s">
-        <v>319</v>
+        <v>1164</v>
       </c>
       <c r="B459" s="3" t="s">
-        <v>609</v>
+        <v>1165</v>
       </c>
     </row>
     <row r="460" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A460" s="2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B460" s="3" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
     </row>
     <row r="461" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A461" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="B461" s="3" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="462" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A462" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="B461" s="3" t="s">
+      <c r="B462" s="3" t="s">
         <v>610</v>
       </c>
     </row>
-    <row r="462" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A462" s="2" t="s">
+    <row r="463" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A463" s="2" t="s">
         <v>318</v>
       </c>
-      <c r="B462" s="3" t="s">
+      <c r="B463" s="3" t="s">
         <v>611</v>
       </c>
     </row>
-    <row r="463" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A463" s="2" t="s">
+    <row r="464" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A464" s="2" t="s">
         <v>602</v>
       </c>
-      <c r="B463" s="3" t="s">
+      <c r="B464" s="3" t="s">
+        <v>1062</v>
+      </c>
+    </row>
+    <row r="465" spans="1:2" ht="255" x14ac:dyDescent="0.25">
+      <c r="A465" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="B465" s="3" t="s">
+        <v>1063</v>
+      </c>
+    </row>
+    <row r="466" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A466" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="B466" s="3" t="s">
+        <v>1064</v>
+      </c>
+    </row>
+    <row r="467" spans="1:2" ht="240" x14ac:dyDescent="0.25">
+      <c r="A467" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="B467" s="3" t="s">
         <v>1065</v>
       </c>
     </row>
-    <row r="464" spans="1:2" ht="255" x14ac:dyDescent="0.25">
-      <c r="A464" s="2" t="s">
-        <v>322</v>
-      </c>
-      <c r="B464" s="3" t="s">
+    <row r="468" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A468" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="B468" s="3" t="s">
         <v>1066</v>
       </c>
     </row>
-    <row r="465" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A465" s="2" t="s">
-        <v>395</v>
-      </c>
-      <c r="B465" s="3" t="s">
+    <row r="469" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A469" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="B469" s="3" t="s">
         <v>1067</v>
-      </c>
-    </row>
-    <row r="466" spans="1:2" ht="240" x14ac:dyDescent="0.25">
-      <c r="A466" s="2" t="s">
-        <v>394</v>
-      </c>
-      <c r="B466" s="3" t="s">
-        <v>1068</v>
-      </c>
-    </row>
-    <row r="467" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A467" s="2" t="s">
-        <v>396</v>
-      </c>
-      <c r="B467" s="3" t="s">
-        <v>1069</v>
-      </c>
-    </row>
-    <row r="468" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A468" s="2" t="s">
-        <v>397</v>
-      </c>
-      <c r="B468" s="3" t="s">
-        <v>1070</v>
-      </c>
-    </row>
-    <row r="469" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A469" s="2" t="s">
-        <v>398</v>
-      </c>
-      <c r="B469" s="3" t="s">
-        <v>1071</v>
       </c>
     </row>
     <row r="470" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A470" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="B470" s="3" t="s">
+        <v>1068</v>
+      </c>
+    </row>
+    <row r="471" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A471" s="2" t="s">
         <v>399</v>
       </c>
-      <c r="B470" s="3" t="s">
+      <c r="B471" s="3" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="472" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A472" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="B472" s="3" t="s">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="473" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A473" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="B473" s="3" t="s">
+        <v>1071</v>
+      </c>
+    </row>
+    <row r="474" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A474" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="B474" s="3" t="s">
         <v>1072</v>
       </c>
     </row>
-    <row r="471" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A471" s="2" t="s">
-        <v>400</v>
-      </c>
-      <c r="B471" s="3" t="s">
+    <row r="475" spans="1:2" ht="225" x14ac:dyDescent="0.25">
+      <c r="A475" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="B475" s="3" t="s">
         <v>1073</v>
-      </c>
-    </row>
-    <row r="472" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A472" s="2" t="s">
-        <v>431</v>
-      </c>
-      <c r="B472" s="3" t="s">
-        <v>1074</v>
-      </c>
-    </row>
-    <row r="473" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A473" s="2" t="s">
-        <v>432</v>
-      </c>
-      <c r="B473" s="3" t="s">
-        <v>1075</v>
-      </c>
-    </row>
-    <row r="474" spans="1:2" ht="225" x14ac:dyDescent="0.25">
-      <c r="A474" s="2" t="s">
-        <v>433</v>
-      </c>
-      <c r="B474" s="3" t="s">
-        <v>1076</v>
-      </c>
-    </row>
-    <row r="475" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A475" s="2" t="s">
-        <v>434</v>
-      </c>
-      <c r="B475" s="3" t="s">
-        <v>1077</v>
       </c>
     </row>
     <row r="476" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A476" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="B476" s="3" t="s">
+        <v>1074</v>
+      </c>
+    </row>
+    <row r="477" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A477" s="2" t="s">
         <v>435</v>
       </c>
-      <c r="B476" s="3" t="s">
+      <c r="B477" s="3" t="s">
+        <v>1075</v>
+      </c>
+    </row>
+    <row r="478" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A478" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="B478" s="3" t="s">
+        <v>1076</v>
+      </c>
+    </row>
+    <row r="479" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A479" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="B479" s="3" t="s">
+        <v>1077</v>
+      </c>
+    </row>
+    <row r="480" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A480" s="2" t="s">
+        <v>438</v>
+      </c>
+      <c r="B480" s="3" t="s">
         <v>1078</v>
       </c>
     </row>
-    <row r="477" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A477" s="2" t="s">
-        <v>436</v>
-      </c>
-      <c r="B477" s="3" t="s">
+    <row r="481" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A481" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="B481" s="3" t="s">
         <v>1079</v>
       </c>
     </row>
-    <row r="478" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A478" s="2" t="s">
-        <v>437</v>
-      </c>
-      <c r="B478" s="3" t="s">
+    <row r="482" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A482" s="2" t="s">
+        <v>440</v>
+      </c>
+      <c r="B482" s="3" t="s">
         <v>1080</v>
       </c>
     </row>
-    <row r="479" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A479" s="2" t="s">
-        <v>438</v>
-      </c>
-      <c r="B479" s="3" t="s">
+    <row r="483" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A483" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="B483" s="3" t="s">
         <v>1081</v>
       </c>
     </row>
-    <row r="480" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A480" s="2" t="s">
-        <v>439</v>
-      </c>
-      <c r="B480" s="3" t="s">
+    <row r="484" spans="1:2" ht="225" x14ac:dyDescent="0.25">
+      <c r="A484" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="B484" s="3" t="s">
         <v>1082</v>
       </c>
     </row>
-    <row r="481" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A481" s="2" t="s">
-        <v>440</v>
-      </c>
-      <c r="B481" s="3" t="s">
+    <row r="485" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A485" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="B485" s="3" t="s">
         <v>1083</v>
       </c>
     </row>
-    <row r="482" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A482" s="2" t="s">
-        <v>441</v>
-      </c>
-      <c r="B482" s="3" t="s">
+    <row r="486" spans="1:2" ht="225" x14ac:dyDescent="0.25">
+      <c r="A486" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="B486" s="3" t="s">
         <v>1084</v>
       </c>
     </row>
-    <row r="483" spans="1:2" ht="225" x14ac:dyDescent="0.25">
-      <c r="A483" s="2" t="s">
-        <v>442</v>
-      </c>
-      <c r="B483" s="3" t="s">
+    <row r="487" spans="1:2" ht="240" x14ac:dyDescent="0.25">
+      <c r="A487" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="B487" s="3" t="s">
         <v>1085</v>
       </c>
     </row>
-    <row r="484" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A484" s="2" t="s">
-        <v>443</v>
-      </c>
-      <c r="B484" s="3" t="s">
+    <row r="488" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+      <c r="A488" s="2" t="s">
+        <v>467</v>
+      </c>
+      <c r="B488" s="3" t="s">
         <v>1086</v>
       </c>
     </row>
-    <row r="485" spans="1:2" ht="225" x14ac:dyDescent="0.25">
-      <c r="A485" s="2" t="s">
-        <v>458</v>
-      </c>
-      <c r="B485" s="3" t="s">
+    <row r="489" spans="1:2" ht="225" x14ac:dyDescent="0.25">
+      <c r="A489" s="2" t="s">
+        <v>468</v>
+      </c>
+      <c r="B489" s="3" t="s">
         <v>1087</v>
       </c>
     </row>
-    <row r="486" spans="1:2" ht="240" x14ac:dyDescent="0.25">
-      <c r="A486" s="2" t="s">
-        <v>466</v>
-      </c>
-      <c r="B486" s="3" t="s">
+    <row r="490" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+      <c r="A490" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="B490" s="3" t="s">
         <v>1088</v>
       </c>
     </row>
-    <row r="487" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A487" s="2" t="s">
-        <v>467</v>
-      </c>
-      <c r="B487" s="3" t="s">
+    <row r="491" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A491" s="2" t="s">
+        <v>633</v>
+      </c>
+      <c r="B491" s="3" t="s">
         <v>1089</v>
       </c>
     </row>
-    <row r="488" spans="1:2" ht="225" x14ac:dyDescent="0.25">
-      <c r="A488" s="2" t="s">
-        <v>468</v>
-      </c>
-      <c r="B488" s="3" t="s">
+    <row r="492" spans="1:2" ht="255" x14ac:dyDescent="0.25">
+      <c r="A492" s="2" t="s">
+        <v>488</v>
+      </c>
+      <c r="B492" s="1" t="s">
         <v>1090</v>
       </c>
     </row>
-    <row r="489" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A489" s="2" t="s">
-        <v>552</v>
-      </c>
-      <c r="B489" s="3" t="s">
+    <row r="493" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A493" s="2" t="s">
+        <v>489</v>
+      </c>
+      <c r="B493" s="1" t="s">
         <v>1091</v>
       </c>
     </row>
-    <row r="490" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A490" s="2" t="s">
-        <v>633</v>
-      </c>
-      <c r="B490" s="3" t="s">
+    <row r="494" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A494" s="2" t="s">
+        <v>490</v>
+      </c>
+      <c r="B494" s="1" t="s">
         <v>1092</v>
-      </c>
-    </row>
-    <row r="491" spans="1:2" ht="255" x14ac:dyDescent="0.25">
-      <c r="A491" s="2" t="s">
-        <v>488</v>
-      </c>
-      <c r="B491" s="1" t="s">
-        <v>1093</v>
-      </c>
-    </row>
-    <row r="492" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A492" s="2" t="s">
-        <v>489</v>
-      </c>
-      <c r="B492" s="1" t="s">
-        <v>1094</v>
-      </c>
-    </row>
-    <row r="493" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A493" s="2" t="s">
-        <v>490</v>
-      </c>
-      <c r="B493" s="1" t="s">
-        <v>1095</v>
-      </c>
-    </row>
-    <row r="494" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A494" s="2" t="s">
-        <v>491</v>
-      </c>
-      <c r="B494" s="1" t="s">
-        <v>1096</v>
       </c>
     </row>
     <row r="495" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A495" s="2" t="s">
+        <v>491</v>
+      </c>
+      <c r="B495" s="1" t="s">
+        <v>1093</v>
+      </c>
+    </row>
+    <row r="496" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A496" s="2" t="s">
         <v>492</v>
       </c>
-      <c r="B495" s="1" t="s">
-        <v>1097</v>
-      </c>
-    </row>
-    <row r="496" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A496" s="2" t="s">
+      <c r="B496" s="1" t="s">
+        <v>1094</v>
+      </c>
+    </row>
+    <row r="497" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A497" s="2" t="s">
         <v>493</v>
       </c>
-      <c r="B496" s="1" t="s">
-        <v>1098</v>
-      </c>
-    </row>
-    <row r="497" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A497" s="2" t="s">
-        <v>494</v>
-      </c>
       <c r="B497" s="1" t="s">
-        <v>1099</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="498" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A498" s="2" t="s">
+        <v>494</v>
+      </c>
+      <c r="B498" s="1" t="s">
+        <v>1096</v>
+      </c>
+    </row>
+    <row r="499" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A499" s="2" t="s">
         <v>495</v>
       </c>
-      <c r="B498" s="1" t="s">
+      <c r="B499" s="1" t="s">
+        <v>1097</v>
+      </c>
+    </row>
+    <row r="500" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A500" s="2" t="s">
+        <v>496</v>
+      </c>
+      <c r="B500" s="1" t="s">
+        <v>1098</v>
+      </c>
+    </row>
+    <row r="501" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A501" s="2" t="s">
+        <v>497</v>
+      </c>
+      <c r="B501" s="1" t="s">
+        <v>1099</v>
+      </c>
+    </row>
+    <row r="502" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A502" s="2" t="s">
+        <v>498</v>
+      </c>
+      <c r="B502" s="1" t="s">
         <v>1100</v>
       </c>
     </row>
-    <row r="499" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A499" s="2" t="s">
-        <v>496</v>
-      </c>
-      <c r="B499" s="1" t="s">
+    <row r="503" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A503" s="2" t="s">
+        <v>499</v>
+      </c>
+      <c r="B503" s="1" t="s">
+        <v>1160</v>
+      </c>
+    </row>
+    <row r="504" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A504" s="2" t="s">
+        <v>500</v>
+      </c>
+      <c r="B504" s="1" t="s">
         <v>1101</v>
-      </c>
-    </row>
-    <row r="500" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A500" s="2" t="s">
-        <v>497</v>
-      </c>
-      <c r="B500" s="1" t="s">
-        <v>1102</v>
-      </c>
-    </row>
-    <row r="501" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A501" s="2" t="s">
-        <v>498</v>
-      </c>
-      <c r="B501" s="1" t="s">
-        <v>1103</v>
-      </c>
-    </row>
-    <row r="502" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A502" s="2" t="s">
-        <v>499</v>
-      </c>
-      <c r="B502" s="1" t="s">
-        <v>1163</v>
-      </c>
-    </row>
-    <row r="503" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A503" s="2" t="s">
-        <v>500</v>
-      </c>
-      <c r="B503" s="1" t="s">
-        <v>1104</v>
-      </c>
-    </row>
-    <row r="504" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A504" s="2" t="s">
-        <v>501</v>
-      </c>
-      <c r="B504" s="1" t="s">
-        <v>1105</v>
       </c>
     </row>
     <row r="505" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A505" s="2" t="s">
+        <v>501</v>
+      </c>
+      <c r="B505" s="1" t="s">
+        <v>1102</v>
+      </c>
+    </row>
+    <row r="506" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A506" s="2" t="s">
         <v>502</v>
       </c>
-      <c r="B505" s="1" t="s">
+      <c r="B506" s="1" t="s">
+        <v>1103</v>
+      </c>
+    </row>
+    <row r="507" spans="1:2" ht="255" x14ac:dyDescent="0.25">
+      <c r="A507" s="2" t="s">
+        <v>597</v>
+      </c>
+      <c r="B507" s="1" t="s">
+        <v>1104</v>
+      </c>
+    </row>
+    <row r="508" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A508" s="2" t="s">
+        <v>598</v>
+      </c>
+      <c r="B508" s="1" t="s">
+        <v>1105</v>
+      </c>
+    </row>
+    <row r="509" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A509" s="2" t="s">
+        <v>503</v>
+      </c>
+      <c r="B509" s="1" t="s">
         <v>1106</v>
       </c>
     </row>
-    <row r="506" spans="1:2" ht="255" x14ac:dyDescent="0.25">
-      <c r="A506" s="2" t="s">
-        <v>597</v>
-      </c>
-      <c r="B506" s="1" t="s">
+    <row r="510" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A510" s="2" t="s">
+        <v>515</v>
+      </c>
+      <c r="B510" s="3" t="s">
         <v>1107</v>
       </c>
     </row>
-    <row r="507" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A507" s="2" t="s">
-        <v>598</v>
-      </c>
-      <c r="B507" s="1" t="s">
+    <row r="511" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A511" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="B511" s="3" t="s">
         <v>1108</v>
       </c>
     </row>
-    <row r="508" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A508" s="2" t="s">
-        <v>503</v>
-      </c>
-      <c r="B508" s="1" t="s">
-        <v>1109</v>
-      </c>
-    </row>
-    <row r="509" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A509" s="2" t="s">
-        <v>515</v>
-      </c>
-      <c r="B509" s="3" t="s">
-        <v>1110</v>
-      </c>
-    </row>
-    <row r="510" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A510" s="2" t="s">
-        <v>423</v>
-      </c>
-      <c r="B510" s="3" t="s">
-        <v>1111</v>
-      </c>
-    </row>
-    <row r="511" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A511" s="2" t="s">
+    <row r="512" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A512" s="2" t="s">
         <v>424</v>
       </c>
-      <c r="B511" s="3" t="s">
+      <c r="B512" s="3" t="s">
         <v>539</v>
       </c>
     </row>
-    <row r="512" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A512" s="2" t="s">
+    <row r="513" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A513" s="2" t="s">
         <v>425</v>
       </c>
-      <c r="B512" s="3" t="s">
+      <c r="B513" s="3" t="s">
         <v>540</v>
-      </c>
-    </row>
-    <row r="513" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A513" s="2" t="s">
-        <v>267</v>
-      </c>
-      <c r="B513" s="1" t="s">
-        <v>1112</v>
       </c>
     </row>
     <row r="514" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A514" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B514" s="1" t="s">
-        <v>1113</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="515" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A515" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B515" s="1" t="s">
-        <v>1114</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="516" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A516" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B516" s="1" t="s">
-        <v>1115</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="517" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A517" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B517" s="1" t="s">
-        <v>1116</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="518" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A518" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B518" s="1" t="s">
-        <v>1117</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="519" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A519" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B519" s="1" t="s">
-        <v>1118</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="520" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A520" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B520" s="1" t="s">
-        <v>1119</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="521" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A521" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B521" s="1" t="s">
-        <v>1120</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="522" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A522" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B522" s="1" t="s">
-        <v>1121</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="523" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A523" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="B523" s="1" t="s">
+        <v>1118</v>
+      </c>
+    </row>
+    <row r="524" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A524" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="B523" s="1" t="s">
-        <v>1122</v>
-      </c>
-    </row>
-    <row r="524" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A524" s="2" t="s">
-        <v>278</v>
-      </c>
       <c r="B524" s="1" t="s">
-        <v>312</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="525" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A525" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="B525" s="1" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="526" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A526" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="B525" s="1" t="s">
+      <c r="B526" s="1" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="526" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A526" s="2" t="s">
+    <row r="527" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A527" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="B526" s="1" t="s">
+      <c r="B527" s="1" t="s">
         <v>316</v>
-      </c>
-    </row>
-    <row r="527" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A527" s="2" t="s">
-        <v>315</v>
-      </c>
-      <c r="B527" s="1" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="528" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A528" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="B528" s="1" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="529" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A529" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="B528" s="1" t="s">
+      <c r="B529" s="1" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="529" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A529" s="2" t="s">
+    <row r="530" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A530" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="B529" s="3" t="s">
+      <c r="B530" s="3" t="s">
         <v>594</v>
       </c>
     </row>
-    <row r="530" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A530" s="2" t="s">
+    <row r="531" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A531" s="2" t="s">
         <v>390</v>
       </c>
-      <c r="B530" s="3" t="s">
+      <c r="B531" s="3" t="s">
         <v>534</v>
       </c>
     </row>
-    <row r="531" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A531" s="2" t="s">
+    <row r="532" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A532" s="2" t="s">
         <v>391</v>
       </c>
-      <c r="B531" s="1" t="s">
+      <c r="B532" s="1" t="s">
         <v>537</v>
       </c>
     </row>
-    <row r="532" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A532" s="2" t="s">
+    <row r="533" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A533" s="2" t="s">
         <v>535</v>
       </c>
-      <c r="B532" s="3" t="s">
+      <c r="B533" s="3" t="s">
         <v>536</v>
-      </c>
-    </row>
-    <row r="533" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A533" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="B533" s="1" t="s">
-        <v>1123</v>
       </c>
     </row>
     <row r="534" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A534" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="B534" s="1" t="s">
+        <v>1120</v>
+      </c>
+    </row>
+    <row r="535" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A535" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="B534" s="1" t="s">
-        <v>1124</v>
-      </c>
-    </row>
-    <row r="535" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A535" s="2" t="s">
+      <c r="B535" s="1" t="s">
+        <v>1121</v>
+      </c>
+    </row>
+    <row r="536" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A536" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="B535" s="1" t="s">
+      <c r="B536" s="1" t="s">
         <v>310</v>
-      </c>
-    </row>
-    <row r="536" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A536" s="2" t="s">
-        <v>283</v>
-      </c>
-      <c r="B536" s="1" t="s">
-        <v>1125</v>
       </c>
     </row>
     <row r="537" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A537" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="B537" s="1" t="s">
+        <v>1122</v>
+      </c>
+    </row>
+    <row r="538" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A538" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B537" s="1" t="s">
-        <v>1126</v>
-      </c>
-    </row>
-    <row r="538" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A538" s="2" t="s">
-        <v>285</v>
-      </c>
       <c r="B538" s="1" t="s">
-        <v>1127</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="539" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A539" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="B539" s="1" t="s">
+        <v>1124</v>
+      </c>
+    </row>
+    <row r="540" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A540" s="2" t="s">
         <v>286</v>
       </c>
-      <c r="B539" s="1" t="s">
-        <v>1128</v>
-      </c>
-    </row>
-    <row r="540" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A540" s="2" t="s">
-        <v>287</v>
-      </c>
       <c r="B540" s="1" t="s">
-        <v>370</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="541" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A541" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B541" s="1" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
     </row>
     <row r="542" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A542" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B542" s="1" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
     </row>
     <row r="543" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A543" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="B543" s="1" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="544" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A544" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="B543" s="1" t="s">
+      <c r="B544" s="1" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="544" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A544" s="2" t="s">
+    <row r="545" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A545" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B544" s="1" t="s">
+      <c r="B545" s="1" t="s">
         <v>314</v>
-      </c>
-    </row>
-    <row r="545" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A545" s="2" t="s">
-        <v>292</v>
-      </c>
-      <c r="B545" s="1" t="s">
-        <v>1129</v>
       </c>
     </row>
     <row r="546" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A546" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="B546" s="1" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="547" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A547" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="B546" s="1" t="s">
+      <c r="B547" s="1" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="548" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A548" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="B548" s="1" t="s">
+        <v>1128</v>
+      </c>
+    </row>
+    <row r="549" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A549" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="B549" s="1" t="s">
+        <v>1129</v>
+      </c>
+    </row>
+    <row r="550" spans="1:2" ht="240" x14ac:dyDescent="0.25">
+      <c r="A550" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="B550" s="1" t="s">
         <v>1130</v>
       </c>
     </row>
-    <row r="547" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A547" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="B547" s="1" t="s">
+    <row r="551" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A551" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="B551" s="1" t="s">
         <v>1131</v>
       </c>
     </row>
-    <row r="548" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A548" s="2" t="s">
-        <v>295</v>
-      </c>
-      <c r="B548" s="1" t="s">
+    <row r="552" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A552" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="B552" s="1" t="s">
         <v>1132</v>
       </c>
     </row>
-    <row r="549" spans="1:2" ht="240" x14ac:dyDescent="0.25">
-      <c r="A549" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="B549" s="1" t="s">
+    <row r="553" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A553" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="B553" s="3" t="s">
         <v>1133</v>
       </c>
     </row>
-    <row r="550" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A550" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="B550" s="1" t="s">
+    <row r="554" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A554" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="B554" s="1" t="s">
         <v>1134</v>
       </c>
     </row>
-    <row r="551" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A551" s="2" t="s">
-        <v>353</v>
-      </c>
-      <c r="B551" s="1" t="s">
+    <row r="555" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A555" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="B555" s="1" t="s">
         <v>1135</v>
       </c>
     </row>
-    <row r="552" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A552" s="2" t="s">
-        <v>365</v>
-      </c>
-      <c r="B552" s="3" t="s">
+    <row r="556" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A556" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="B556" s="1" t="s">
         <v>1136</v>
       </c>
     </row>
-    <row r="553" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A553" s="2" t="s">
-        <v>366</v>
-      </c>
-      <c r="B553" s="1" t="s">
+    <row r="557" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A557" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="B557" s="1" t="s">
         <v>1137</v>
       </c>
     </row>
-    <row r="554" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A554" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="B554" s="1" t="s">
+    <row r="558" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A558" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="B558" s="1" t="s">
         <v>1138</v>
       </c>
     </row>
-    <row r="555" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A555" s="2" t="s">
-        <v>364</v>
-      </c>
-      <c r="B555" s="1" t="s">
-        <v>1139</v>
-      </c>
-    </row>
-    <row r="556" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A556" s="2" t="s">
-        <v>299</v>
-      </c>
-      <c r="B556" s="1" t="s">
-        <v>1140</v>
-      </c>
-    </row>
-    <row r="557" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A557" s="2" t="s">
-        <v>354</v>
-      </c>
-      <c r="B557" s="1" t="s">
-        <v>1141</v>
-      </c>
-    </row>
-    <row r="558" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A558" s="2" t="s">
+    <row r="559" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A559" s="2" t="s">
         <v>357</v>
       </c>
-      <c r="B558" s="1" t="s">
+      <c r="B559" s="1" t="s">
         <v>372</v>
-      </c>
-    </row>
-    <row r="559" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A559" s="2" t="s">
-        <v>300</v>
-      </c>
-      <c r="B559" s="1" t="s">
-        <v>1142</v>
       </c>
     </row>
     <row r="560" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A560" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="B560" s="1" t="s">
+        <v>1139</v>
+      </c>
+    </row>
+    <row r="561" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A561" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="B560" s="1" t="s">
+      <c r="B561" s="1" t="s">
+        <v>1140</v>
+      </c>
+    </row>
+    <row r="562" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A562" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="B562" s="1" t="s">
+        <v>1141</v>
+      </c>
+    </row>
+    <row r="563" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A563" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="B563" s="1" t="s">
+        <v>1142</v>
+      </c>
+    </row>
+    <row r="564" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A564" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="B564" s="1" t="s">
         <v>1143</v>
       </c>
     </row>
-    <row r="561" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A561" s="2" t="s">
-        <v>302</v>
-      </c>
-      <c r="B561" s="1" t="s">
+    <row r="565" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A565" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="B565" s="1" t="s">
         <v>1144</v>
       </c>
     </row>
-    <row r="562" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A562" s="2" t="s">
-        <v>303</v>
-      </c>
-      <c r="B562" s="1" t="s">
+    <row r="566" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A566" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="B566" s="1" t="s">
         <v>1145</v>
       </c>
     </row>
-    <row r="563" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A563" s="2" t="s">
-        <v>363</v>
-      </c>
-      <c r="B563" s="1" t="s">
+    <row r="567" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A567" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="B567" s="1" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="568" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A568" s="2" t="s">
+        <v>517</v>
+      </c>
+      <c r="B568" s="1" t="s">
         <v>1146</v>
       </c>
     </row>
-    <row r="564" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A564" s="2" t="s">
-        <v>304</v>
-      </c>
-      <c r="B564" s="1" t="s">
+    <row r="569" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A569" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="B569" s="1" t="s">
         <v>1147</v>
       </c>
     </row>
-    <row r="565" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A565" s="2" t="s">
-        <v>361</v>
-      </c>
-      <c r="B565" s="1" t="s">
+    <row r="570" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A570" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="B570" s="1" t="s">
         <v>1148</v>
       </c>
     </row>
-    <row r="566" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A566" s="2" t="s">
-        <v>362</v>
-      </c>
-      <c r="B566" s="1" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="567" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A567" s="2" t="s">
-        <v>517</v>
-      </c>
-      <c r="B567" s="1" t="s">
+    <row r="571" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A571" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="B571" s="1" t="s">
         <v>1149</v>
       </c>
     </row>
-    <row r="568" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A568" s="2" t="s">
-        <v>305</v>
-      </c>
-      <c r="B568" s="1" t="s">
+    <row r="572" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A572" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="B572" s="1" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="573" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A573" s="2" t="s">
+        <v>518</v>
+      </c>
+      <c r="B573" s="1" t="s">
         <v>1150</v>
-      </c>
-    </row>
-    <row r="569" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A569" s="2" t="s">
-        <v>358</v>
-      </c>
-      <c r="B569" s="1" t="s">
-        <v>1151</v>
-      </c>
-    </row>
-    <row r="570" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A570" s="2" t="s">
-        <v>359</v>
-      </c>
-      <c r="B570" s="1" t="s">
-        <v>1152</v>
-      </c>
-    </row>
-    <row r="571" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A571" s="2" t="s">
-        <v>360</v>
-      </c>
-      <c r="B571" s="1" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="572" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A572" s="2" t="s">
-        <v>518</v>
-      </c>
-      <c r="B572" s="1" t="s">
-        <v>1153</v>
-      </c>
-    </row>
-    <row r="573" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A573" s="2" t="s">
-        <v>306</v>
-      </c>
-      <c r="B573" s="1" t="s">
-        <v>1154</v>
       </c>
     </row>
     <row r="574" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A574" s="2" t="s">
-        <v>352</v>
+        <v>306</v>
       </c>
       <c r="B574" s="1" t="s">
-        <v>1155</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="575" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A575" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="B575" s="1" t="s">
+        <v>1152</v>
+      </c>
+    </row>
+    <row r="576" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A576" s="2" t="s">
         <v>355</v>
       </c>
-      <c r="B575" s="3" t="s">
-        <v>1156</v>
-      </c>
-    </row>
-    <row r="576" spans="1:2" ht="405" x14ac:dyDescent="0.25">
-      <c r="A576" s="2" t="s">
+      <c r="B576" s="3" t="s">
+        <v>1153</v>
+      </c>
+    </row>
+    <row r="577" spans="1:2" ht="405" x14ac:dyDescent="0.25">
+      <c r="A577" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="B576" s="1" t="s">
-        <v>1157</v>
-      </c>
-    </row>
-    <row r="577" spans="1:2" ht="375" x14ac:dyDescent="0.25">
-      <c r="A577" s="2" t="s">
+      <c r="B577" s="1" t="s">
+        <v>1154</v>
+      </c>
+    </row>
+    <row r="578" spans="1:2" ht="375" x14ac:dyDescent="0.25">
+      <c r="A578" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="B577" s="1" t="s">
-        <v>1158</v>
-      </c>
-    </row>
-    <row r="578" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A578" s="2" t="s">
+      <c r="B578" s="1" t="s">
+        <v>1155</v>
+      </c>
+    </row>
+    <row r="579" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A579" s="2" t="s">
         <v>356</v>
       </c>
-      <c r="B578" s="1" t="s">
+      <c r="B579" s="1" t="s">
         <v>406</v>
-      </c>
-    </row>
-    <row r="579" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A579" s="2" t="s">
-        <v>308</v>
-      </c>
-      <c r="B579" s="1" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="580" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A580" s="2" t="s">
-        <v>349</v>
-      </c>
-      <c r="B580" s="3" t="s">
-        <v>1159</v>
+        <v>308</v>
+      </c>
+      <c r="B580" s="1" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="581" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A581" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="B581" s="3" t="s">
+        <v>1156</v>
+      </c>
+    </row>
+    <row r="582" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A582" s="2" t="s">
         <v>519</v>
       </c>
-      <c r="B581" s="3" t="s">
-        <v>1160</v>
-      </c>
-    </row>
-    <row r="582" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A582" s="2" t="s">
+      <c r="B582" s="3" t="s">
+        <v>1157</v>
+      </c>
+    </row>
+    <row r="583" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A583" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="B582" s="3" t="s">
-        <v>1161</v>
+      <c r="B583" s="3" t="s">
+        <v>1158</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:B579">
-    <sortCondition ref="A1:A579"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:B580">
+    <sortCondition ref="A1:A580"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fix mispelling of Dwarfs.
</commit_message>
<xml_diff>
--- a/Documentation/Events.xlsx
+++ b/Documentation/Events.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\happysulla\BarbarianPrince\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{455EFE8E-AB41-4A37-9AD4-7F80BA0956C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CC540120-483B-4B15-85E7-6947EE8C4525}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" r:id="rId1"/>
@@ -4748,16 +4748,6 @@
                 &lt;InlineUIContainer&gt;&lt;Image Name='DecisionShare' Source='../bin/Images/DecisionShare.gif'  Height='200' Width='200'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;&lt;InlineUIContainer&gt;&lt;Image Name='DecisionFight' Source='../bin/Images/DecisionFight.gif'  Height='200' Width='200'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e072d Follow an Elven Band&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;Roll one die to see where you end the day: &lt;InlineUIContainer&gt;&lt;Image Source='../bin/Images/dieRoll.gif' Name='DieRoll1' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
- &lt;InlineUIContainer&gt;&lt;Button Content='e165' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  1 - Eleven Town&lt;LineBreak/&gt;
- &lt;InlineUIContainer&gt;&lt;Button Content='e166' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  2 - Elven Castle&lt;LineBreak/&gt;
- &lt;InlineUIContainer&gt;&lt;Button Content='e053' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  3,4,5,6 - Campsite&lt;LineBreak/&gt;
-&lt;LineBreak/&gt; &lt;LineBreak/&gt;
-                                   &lt;InlineUIContainer&gt;&lt;Image Source='../bin/Images/Elf.gif' Height='300' Width='240'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;e073 Witch&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;You encounter a witch with combat skill 1, endurance 3, wealth 5.  
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
@@ -8028,6 +8018,16 @@
   <si>
     <t>&lt;Bold&gt;e203f Wakeup in Bad Straights&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;The game is recovered with you in bad way. Click image to continue.</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e072d Follow an Elven Band&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;Roll one die to see where you end the day: &lt;InlineUIContainer&gt;&lt;Image Source='../bin/Images/dieRoll.gif' Name='DieRoll1' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+ &lt;InlineUIContainer&gt;&lt;Button Content='e165' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  1 - Eleven Town&lt;LineBreak/&gt;
+ &lt;InlineUIContainer&gt;&lt;Button Content='e166' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  2 - Elven Fortress&lt;LineBreak/&gt;
+ &lt;InlineUIContainer&gt;&lt;Button Content='e053' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  3,4,5,6 - Campsite&lt;LineBreak/&gt;
+&lt;LineBreak/&gt; &lt;LineBreak/&gt;
+                                   &lt;InlineUIContainer&gt;&lt;Image Source='../bin/Images/Elf.gif' Height='300' Width='240'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
 </sst>
 </file>
@@ -8416,8 +8416,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B583"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A455" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A459" sqref="A459"/>
+    <sheetView tabSelected="1" topLeftCell="A211" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B213" sqref="B213"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9199,7 +9199,7 @@
         <v>61</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -9455,7 +9455,7 @@
         <v>350</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
     </row>
     <row r="130" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10127,7 +10127,7 @@
         <v>516</v>
       </c>
       <c r="B213" s="3" t="s">
-        <v>843</v>
+        <v>1165</v>
       </c>
     </row>
     <row r="214" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10135,7 +10135,7 @@
         <v>112</v>
       </c>
       <c r="B214" s="3" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
     </row>
     <row r="215" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10143,7 +10143,7 @@
         <v>169</v>
       </c>
       <c r="B215" s="3" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="216" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10151,7 +10151,7 @@
         <v>170</v>
       </c>
       <c r="B216" s="3" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
     </row>
     <row r="217" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10159,7 +10159,7 @@
         <v>171</v>
       </c>
       <c r="B217" s="3" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="218" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -10167,7 +10167,7 @@
         <v>113</v>
       </c>
       <c r="B218" s="3" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
     </row>
     <row r="219" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -10175,7 +10175,7 @@
         <v>114</v>
       </c>
       <c r="B219" s="3" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="220" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10183,7 +10183,7 @@
         <v>266</v>
       </c>
       <c r="B220" s="3" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="221" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -10191,7 +10191,7 @@
         <v>570</v>
       </c>
       <c r="B221" s="3" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="222" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10199,7 +10199,7 @@
         <v>115</v>
       </c>
       <c r="B222" s="3" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
     </row>
     <row r="223" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10207,7 +10207,7 @@
         <v>522</v>
       </c>
       <c r="B223" s="3" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
     </row>
     <row r="224" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -10215,7 +10215,7 @@
         <v>116</v>
       </c>
       <c r="B224" s="3" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
     </row>
     <row r="225" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10223,7 +10223,7 @@
         <v>520</v>
       </c>
       <c r="B225" s="3" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
     </row>
     <row r="226" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10231,7 +10231,7 @@
         <v>117</v>
       </c>
       <c r="B226" s="4" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
     </row>
     <row r="227" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10239,7 +10239,7 @@
         <v>523</v>
       </c>
       <c r="B227" s="4" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
     </row>
     <row r="228" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10247,7 +10247,7 @@
         <v>524</v>
       </c>
       <c r="B228" s="4" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
     </row>
     <row r="229" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10255,7 +10255,7 @@
         <v>525</v>
       </c>
       <c r="B229" s="4" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
     </row>
     <row r="230" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10263,7 +10263,7 @@
         <v>118</v>
       </c>
       <c r="B230" s="3" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
     </row>
     <row r="231" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -10271,7 +10271,7 @@
         <v>573</v>
       </c>
       <c r="B231" s="3" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
     </row>
     <row r="232" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10279,7 +10279,7 @@
         <v>574</v>
       </c>
       <c r="B232" s="3" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
     </row>
     <row r="233" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10287,7 +10287,7 @@
         <v>119</v>
       </c>
       <c r="B233" s="3" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
     </row>
     <row r="234" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10295,7 +10295,7 @@
         <v>566</v>
       </c>
       <c r="B234" s="3" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
     </row>
     <row r="235" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10303,7 +10303,7 @@
         <v>565</v>
       </c>
       <c r="B235" s="3" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
     </row>
     <row r="236" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10311,7 +10311,7 @@
         <v>120</v>
       </c>
       <c r="B236" s="3" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="237" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -10319,7 +10319,7 @@
         <v>172</v>
       </c>
       <c r="B237" s="3" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
     </row>
     <row r="238" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10327,7 +10327,7 @@
         <v>173</v>
       </c>
       <c r="B238" s="3" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
     </row>
     <row r="239" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10335,7 +10335,7 @@
         <v>174</v>
       </c>
       <c r="B239" s="3" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
     </row>
     <row r="240" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -10343,7 +10343,7 @@
         <v>121</v>
       </c>
       <c r="B240" s="3" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
     </row>
     <row r="241" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10351,7 +10351,7 @@
         <v>122</v>
       </c>
       <c r="B241" s="3" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
     </row>
     <row r="242" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10359,7 +10359,7 @@
         <v>521</v>
       </c>
       <c r="B242" s="3" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
     </row>
     <row r="243" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -10367,7 +10367,7 @@
         <v>123</v>
       </c>
       <c r="B243" s="3" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
     </row>
     <row r="244" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10375,7 +10375,7 @@
         <v>571</v>
       </c>
       <c r="B244" s="3" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
     </row>
     <row r="245" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10383,7 +10383,7 @@
         <v>572</v>
       </c>
       <c r="B245" s="3" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
     </row>
     <row r="246" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10391,7 +10391,7 @@
         <v>124</v>
       </c>
       <c r="B246" s="3" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
     </row>
     <row r="247" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10399,7 +10399,7 @@
         <v>617</v>
       </c>
       <c r="B247" s="3" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
     </row>
     <row r="248" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10407,7 +10407,7 @@
         <v>125</v>
       </c>
       <c r="B248" s="3" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
     </row>
     <row r="249" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -10415,7 +10415,7 @@
         <v>589</v>
       </c>
       <c r="B249" s="3" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
     </row>
     <row r="250" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10423,7 +10423,7 @@
         <v>126</v>
       </c>
       <c r="B250" s="3" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
     </row>
     <row r="251" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -10431,7 +10431,7 @@
         <v>127</v>
       </c>
       <c r="B251" s="3" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
     </row>
     <row r="252" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10439,7 +10439,7 @@
         <v>128</v>
       </c>
       <c r="B252" s="3" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
     </row>
     <row r="253" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -10447,7 +10447,7 @@
         <v>129</v>
       </c>
       <c r="B253" s="3" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
     </row>
     <row r="254" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10455,7 +10455,7 @@
         <v>130</v>
       </c>
       <c r="B254" s="3" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
     </row>
     <row r="255" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -10463,7 +10463,7 @@
         <v>131</v>
       </c>
       <c r="B255" s="3" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
     </row>
     <row r="256" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -10471,7 +10471,7 @@
         <v>576</v>
       </c>
       <c r="B256" s="3" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
     </row>
     <row r="257" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10479,7 +10479,7 @@
         <v>577</v>
       </c>
       <c r="B257" s="3" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
     </row>
     <row r="258" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -10487,7 +10487,7 @@
         <v>132</v>
       </c>
       <c r="B258" s="3" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
     </row>
     <row r="259" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10495,7 +10495,7 @@
         <v>133</v>
       </c>
       <c r="B259" s="3" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="260" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10503,7 +10503,7 @@
         <v>575</v>
       </c>
       <c r="B260" s="3" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="261" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -10511,7 +10511,7 @@
         <v>134</v>
       </c>
       <c r="B261" s="3" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
     </row>
     <row r="262" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10519,7 +10519,7 @@
         <v>590</v>
       </c>
       <c r="B262" s="3" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="263" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10527,7 +10527,7 @@
         <v>591</v>
       </c>
       <c r="B263" s="3" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
     </row>
     <row r="264" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -10535,7 +10535,7 @@
         <v>135</v>
       </c>
       <c r="B264" s="3" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
     </row>
     <row r="265" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -10543,7 +10543,7 @@
         <v>592</v>
       </c>
       <c r="B265" s="3" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
     </row>
     <row r="266" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10551,7 +10551,7 @@
         <v>136</v>
       </c>
       <c r="B266" s="3" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
     </row>
     <row r="267" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -10559,7 +10559,7 @@
         <v>137</v>
       </c>
       <c r="B267" s="3" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
     </row>
     <row r="268" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10567,7 +10567,7 @@
         <v>232</v>
       </c>
       <c r="B268" s="3" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
     </row>
     <row r="269" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10575,7 +10575,7 @@
         <v>233</v>
       </c>
       <c r="B269" s="3" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
     </row>
     <row r="270" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -10591,7 +10591,7 @@
         <v>234</v>
       </c>
       <c r="B271" s="3" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
     </row>
     <row r="272" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10599,7 +10599,7 @@
         <v>235</v>
       </c>
       <c r="B272" s="3" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
     </row>
     <row r="273" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -10615,7 +10615,7 @@
         <v>239</v>
       </c>
       <c r="B274" s="3" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="275" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10623,7 +10623,7 @@
         <v>240</v>
       </c>
       <c r="B275" s="3" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
     </row>
     <row r="276" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10631,7 +10631,7 @@
         <v>241</v>
       </c>
       <c r="B276" s="3" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
     </row>
     <row r="277" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10647,7 +10647,7 @@
         <v>236</v>
       </c>
       <c r="B278" s="3" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
     </row>
     <row r="279" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10655,7 +10655,7 @@
         <v>237</v>
       </c>
       <c r="B279" s="3" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
     </row>
     <row r="280" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10663,7 +10663,7 @@
         <v>238</v>
       </c>
       <c r="B280" s="3" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
     </row>
     <row r="281" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10671,7 +10671,7 @@
         <v>141</v>
       </c>
       <c r="B281" s="3" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="282" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10679,7 +10679,7 @@
         <v>142</v>
       </c>
       <c r="B282" s="3" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="283" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10687,7 +10687,7 @@
         <v>143</v>
       </c>
       <c r="B283" s="3" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
     </row>
     <row r="284" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -10695,7 +10695,7 @@
         <v>144</v>
       </c>
       <c r="B284" s="3" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
     </row>
     <row r="285" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10703,7 +10703,7 @@
         <v>242</v>
       </c>
       <c r="B285" s="3" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
     </row>
     <row r="286" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10711,7 +10711,7 @@
         <v>145</v>
       </c>
       <c r="B286" s="3" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
     </row>
     <row r="287" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10719,7 +10719,7 @@
         <v>146</v>
       </c>
       <c r="B287" s="3" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
     </row>
     <row r="288" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10727,7 +10727,7 @@
         <v>147</v>
       </c>
       <c r="B288" s="3" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
     </row>
     <row r="289" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10735,7 +10735,7 @@
         <v>148</v>
       </c>
       <c r="B289" s="3" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
     </row>
     <row r="290" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10743,7 +10743,7 @@
         <v>149</v>
       </c>
       <c r="B290" s="3" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
     </row>
     <row r="291" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10751,7 +10751,7 @@
         <v>605</v>
       </c>
       <c r="B291" s="3" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="292" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10759,7 +10759,7 @@
         <v>604</v>
       </c>
       <c r="B292" s="3" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
     </row>
     <row r="293" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10767,7 +10767,7 @@
         <v>606</v>
       </c>
       <c r="B293" s="3" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
     </row>
     <row r="294" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10775,7 +10775,7 @@
         <v>150</v>
       </c>
       <c r="B294" s="3" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
     </row>
     <row r="295" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10783,7 +10783,7 @@
         <v>607</v>
       </c>
       <c r="B295" s="3" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
     </row>
     <row r="296" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -10791,7 +10791,7 @@
         <v>151</v>
       </c>
       <c r="B296" s="3" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
     </row>
     <row r="297" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10799,7 +10799,7 @@
         <v>243</v>
       </c>
       <c r="B297" s="3" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
     </row>
     <row r="298" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10807,7 +10807,7 @@
         <v>244</v>
       </c>
       <c r="B298" s="3" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
     </row>
     <row r="299" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10815,7 +10815,7 @@
         <v>245</v>
       </c>
       <c r="B299" s="3" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
     </row>
     <row r="300" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10823,7 +10823,7 @@
         <v>152</v>
       </c>
       <c r="B300" s="3" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
     </row>
     <row r="301" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10831,7 +10831,7 @@
         <v>153</v>
       </c>
       <c r="B301" s="3" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
     </row>
     <row r="302" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10839,7 +10839,7 @@
         <v>154</v>
       </c>
       <c r="B302" s="3" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
     </row>
     <row r="303" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -10847,7 +10847,7 @@
         <v>155</v>
       </c>
       <c r="B303" s="3" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
     </row>
     <row r="304" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10855,7 +10855,7 @@
         <v>156</v>
       </c>
       <c r="B304" s="3" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
     </row>
     <row r="305" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10871,7 +10871,7 @@
         <v>246</v>
       </c>
       <c r="B306" s="3" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
     </row>
     <row r="307" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10879,7 +10879,7 @@
         <v>247</v>
       </c>
       <c r="B307" s="3" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
     </row>
     <row r="308" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10887,7 +10887,7 @@
         <v>248</v>
       </c>
       <c r="B308" s="3" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
     </row>
     <row r="309" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10903,7 +10903,7 @@
         <v>159</v>
       </c>
       <c r="B310" s="3" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
     </row>
     <row r="311" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10911,7 +10911,7 @@
         <v>160</v>
       </c>
       <c r="B311" s="3" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
     </row>
     <row r="312" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -10919,7 +10919,7 @@
         <v>161</v>
       </c>
       <c r="B312" s="3" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
     </row>
     <row r="313" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -10927,7 +10927,7 @@
         <v>162</v>
       </c>
       <c r="B313" s="3" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
     </row>
     <row r="314" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -10935,7 +10935,7 @@
         <v>599</v>
       </c>
       <c r="B314" s="3" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
     </row>
     <row r="315" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10943,7 +10943,7 @@
         <v>600</v>
       </c>
       <c r="B315" s="3" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
     </row>
     <row r="316" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10951,7 +10951,7 @@
         <v>601</v>
       </c>
       <c r="B316" s="3" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
     </row>
     <row r="317" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10959,7 +10959,7 @@
         <v>163</v>
       </c>
       <c r="B317" s="3" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
     </row>
     <row r="318" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10967,7 +10967,7 @@
         <v>164</v>
       </c>
       <c r="B318" s="3" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
     </row>
     <row r="319" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10975,7 +10975,7 @@
         <v>175</v>
       </c>
       <c r="B319" s="3" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
     </row>
     <row r="320" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -10983,7 +10983,7 @@
         <v>176</v>
       </c>
       <c r="B320" s="3" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
     </row>
     <row r="321" spans="1:2" ht="390" x14ac:dyDescent="0.25">
@@ -10991,7 +10991,7 @@
         <v>177</v>
       </c>
       <c r="B321" s="3" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
     </row>
     <row r="322" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -11007,7 +11007,7 @@
         <v>414</v>
       </c>
       <c r="B323" s="3" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
     </row>
     <row r="324" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11015,7 +11015,7 @@
         <v>415</v>
       </c>
       <c r="B324" s="3" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
     </row>
     <row r="325" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -11023,7 +11023,7 @@
         <v>416</v>
       </c>
       <c r="B325" s="3" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
     </row>
     <row r="326" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -11031,7 +11031,7 @@
         <v>417</v>
       </c>
       <c r="B326" s="3" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
     </row>
     <row r="327" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11039,7 +11039,7 @@
         <v>418</v>
       </c>
       <c r="B327" s="3" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
     </row>
     <row r="328" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11047,7 +11047,7 @@
         <v>613</v>
       </c>
       <c r="B328" s="3" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
     </row>
     <row r="329" spans="1:2" ht="390" x14ac:dyDescent="0.25">
@@ -11055,7 +11055,7 @@
         <v>178</v>
       </c>
       <c r="B329" s="3" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
     </row>
     <row r="330" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -11071,7 +11071,7 @@
         <v>426</v>
       </c>
       <c r="B331" s="3" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
     </row>
     <row r="332" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11079,7 +11079,7 @@
         <v>427</v>
       </c>
       <c r="B332" s="3" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
     </row>
     <row r="333" spans="1:2" ht="315" x14ac:dyDescent="0.25">
@@ -11087,7 +11087,7 @@
         <v>179</v>
       </c>
       <c r="B333" s="3" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
     </row>
     <row r="334" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -11095,7 +11095,7 @@
         <v>249</v>
       </c>
       <c r="B334" s="3" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
     </row>
     <row r="335" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -11103,7 +11103,7 @@
         <v>250</v>
       </c>
       <c r="B335" s="3" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
     </row>
     <row r="336" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -11111,7 +11111,7 @@
         <v>251</v>
       </c>
       <c r="B336" s="3" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
     </row>
     <row r="337" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11119,7 +11119,7 @@
         <v>252</v>
       </c>
       <c r="B337" s="3" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
     </row>
     <row r="338" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -11127,7 +11127,7 @@
         <v>253</v>
       </c>
       <c r="B338" s="3" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
     </row>
     <row r="339" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -11135,7 +11135,7 @@
         <v>545</v>
       </c>
       <c r="B339" s="3" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="340" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -11143,7 +11143,7 @@
         <v>546</v>
       </c>
       <c r="B340" s="3" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
     </row>
     <row r="341" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11151,7 +11151,7 @@
         <v>180</v>
       </c>
       <c r="B341" s="3" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
     </row>
     <row r="342" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11159,7 +11159,7 @@
         <v>181</v>
       </c>
       <c r="B342" s="3" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
     </row>
     <row r="343" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11167,7 +11167,7 @@
         <v>386</v>
       </c>
       <c r="B343" s="3" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
     </row>
     <row r="344" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -11183,7 +11183,7 @@
         <v>622</v>
       </c>
       <c r="B345" s="3" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
     </row>
     <row r="346" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11191,7 +11191,7 @@
         <v>183</v>
       </c>
       <c r="B346" s="3" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
     </row>
     <row r="347" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -11199,7 +11199,7 @@
         <v>184</v>
       </c>
       <c r="B347" s="3" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
     </row>
     <row r="348" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -11215,7 +11215,7 @@
         <v>185</v>
       </c>
       <c r="B349" s="3" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
     </row>
     <row r="350" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -11223,7 +11223,7 @@
         <v>186</v>
       </c>
       <c r="B350" s="3" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
     </row>
     <row r="351" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -11231,7 +11231,7 @@
         <v>187</v>
       </c>
       <c r="B351" s="3" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
     </row>
     <row r="352" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11247,7 +11247,7 @@
         <v>188</v>
       </c>
       <c r="B353" s="3" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
     </row>
     <row r="354" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -11255,7 +11255,7 @@
         <v>189</v>
       </c>
       <c r="B354" s="3" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
     </row>
     <row r="355" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -11263,7 +11263,7 @@
         <v>383</v>
       </c>
       <c r="B355" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="356" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -11271,7 +11271,7 @@
         <v>384</v>
       </c>
       <c r="B356" s="3" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
     </row>
     <row r="357" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -11279,7 +11279,7 @@
         <v>190</v>
       </c>
       <c r="B357" s="3" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
     </row>
     <row r="358" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -11287,7 +11287,7 @@
         <v>191</v>
       </c>
       <c r="B358" s="3" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
     </row>
     <row r="359" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -11295,7 +11295,7 @@
         <v>192</v>
       </c>
       <c r="B359" s="3" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
     </row>
     <row r="360" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -11303,7 +11303,7 @@
         <v>465</v>
       </c>
       <c r="B360" s="3" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="361" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -11311,7 +11311,7 @@
         <v>193</v>
       </c>
       <c r="B361" s="3" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
     </row>
     <row r="362" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -11327,7 +11327,7 @@
         <v>333</v>
       </c>
       <c r="B363" s="3" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="364" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -11335,7 +11335,7 @@
         <v>624</v>
       </c>
       <c r="B364" s="3" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
     </row>
     <row r="365" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -11343,7 +11343,7 @@
         <v>625</v>
       </c>
       <c r="B365" s="3" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
     </row>
     <row r="366" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11351,7 +11351,7 @@
         <v>627</v>
       </c>
       <c r="B366" s="3" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
     </row>
     <row r="367" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11359,7 +11359,7 @@
         <v>628</v>
       </c>
       <c r="B367" s="3" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
     </row>
     <row r="368" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11367,7 +11367,7 @@
         <v>629</v>
       </c>
       <c r="B368" s="3" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
     </row>
     <row r="369" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11375,7 +11375,7 @@
         <v>630</v>
       </c>
       <c r="B369" s="3" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
     </row>
     <row r="370" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11383,7 +11383,7 @@
         <v>631</v>
       </c>
       <c r="B370" s="3" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
     </row>
     <row r="371" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11391,7 +11391,7 @@
         <v>632</v>
       </c>
       <c r="B371" s="3" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
     </row>
     <row r="372" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -11399,7 +11399,7 @@
         <v>194</v>
       </c>
       <c r="B372" s="3" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
     </row>
     <row r="373" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -11407,7 +11407,7 @@
         <v>195</v>
       </c>
       <c r="B373" s="3" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
     </row>
     <row r="374" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -11415,7 +11415,7 @@
         <v>620</v>
       </c>
       <c r="B374" s="3" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="375" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -11423,7 +11423,7 @@
         <v>196</v>
       </c>
       <c r="B375" s="3" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
     </row>
     <row r="376" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -11431,7 +11431,7 @@
         <v>328</v>
       </c>
       <c r="B376" s="3" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
     </row>
     <row r="377" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -11439,7 +11439,7 @@
         <v>197</v>
       </c>
       <c r="B377" s="3" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
     </row>
     <row r="378" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11447,7 +11447,7 @@
         <v>487</v>
       </c>
       <c r="B378" s="3" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
     </row>
     <row r="379" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11455,7 +11455,7 @@
         <v>198</v>
       </c>
       <c r="B379" s="3" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
     </row>
     <row r="380" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11463,7 +11463,7 @@
         <v>199</v>
       </c>
       <c r="B380" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="381" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -11471,7 +11471,7 @@
         <v>200</v>
       </c>
       <c r="B381" s="3" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
     </row>
     <row r="382" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11479,7 +11479,7 @@
         <v>201</v>
       </c>
       <c r="B382" s="3" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
     </row>
     <row r="383" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11487,7 +11487,7 @@
         <v>202</v>
       </c>
       <c r="B383" s="3" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
     </row>
     <row r="384" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -11495,7 +11495,7 @@
         <v>203</v>
       </c>
       <c r="B384" s="3" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="385" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -11543,7 +11543,7 @@
         <v>204</v>
       </c>
       <c r="B390" s="3" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="391" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11551,7 +11551,7 @@
         <v>459</v>
       </c>
       <c r="B391" s="3" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="392" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11559,7 +11559,7 @@
         <v>460</v>
       </c>
       <c r="B392" s="3" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="393" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11567,7 +11567,7 @@
         <v>461</v>
       </c>
       <c r="B393" s="3" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="394" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11575,7 +11575,7 @@
         <v>462</v>
       </c>
       <c r="B394" s="3" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="395" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11583,7 +11583,7 @@
         <v>463</v>
       </c>
       <c r="B395" s="3" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="396" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11591,7 +11591,7 @@
         <v>464</v>
       </c>
       <c r="B396" s="3" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="397" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -11599,7 +11599,7 @@
         <v>205</v>
       </c>
       <c r="B397" s="3" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="398" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -11671,7 +11671,7 @@
         <v>207</v>
       </c>
       <c r="B406" s="3" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="407" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -11679,7 +11679,7 @@
         <v>208</v>
       </c>
       <c r="B407" s="3" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="408" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -11687,7 +11687,7 @@
         <v>209</v>
       </c>
       <c r="B408" s="3" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="409" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11695,7 +11695,7 @@
         <v>476</v>
       </c>
       <c r="B409" s="3" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="410" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11703,7 +11703,7 @@
         <v>477</v>
       </c>
       <c r="B410" s="3" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="411" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11711,7 +11711,7 @@
         <v>478</v>
       </c>
       <c r="B411" s="3" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="412" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -11719,7 +11719,7 @@
         <v>479</v>
       </c>
       <c r="B412" s="3" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="413" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -11727,7 +11727,7 @@
         <v>480</v>
       </c>
       <c r="B413" s="4" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="414" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -11735,7 +11735,7 @@
         <v>481</v>
       </c>
       <c r="B414" s="3" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="415" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -11743,7 +11743,7 @@
         <v>621</v>
       </c>
       <c r="B415" s="3" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="416" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -11751,7 +11751,7 @@
         <v>210</v>
       </c>
       <c r="B416" s="3" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="417" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11759,7 +11759,7 @@
         <v>469</v>
       </c>
       <c r="B417" s="3" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="418" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11767,7 +11767,7 @@
         <v>470</v>
       </c>
       <c r="B418" s="3" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="419" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11775,7 +11775,7 @@
         <v>471</v>
       </c>
       <c r="B419" s="3" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="420" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11783,7 +11783,7 @@
         <v>472</v>
       </c>
       <c r="B420" s="3" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="421" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11791,7 +11791,7 @@
         <v>473</v>
       </c>
       <c r="B421" s="3" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="422" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11799,7 +11799,7 @@
         <v>474</v>
       </c>
       <c r="B422" s="3" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="423" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11807,7 +11807,7 @@
         <v>475</v>
       </c>
       <c r="B423" s="3" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="424" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11815,7 +11815,7 @@
         <v>619</v>
       </c>
       <c r="B424" s="3" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="425" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -11823,7 +11823,7 @@
         <v>211</v>
       </c>
       <c r="B425" s="3" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="426" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11831,7 +11831,7 @@
         <v>212</v>
       </c>
       <c r="B426" s="3" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="427" spans="1:2" ht="300" x14ac:dyDescent="0.25">
@@ -11839,7 +11839,7 @@
         <v>419</v>
       </c>
       <c r="B427" s="3" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="428" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11847,7 +11847,7 @@
         <v>420</v>
       </c>
       <c r="B428" s="3" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="429" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -11855,7 +11855,7 @@
         <v>421</v>
       </c>
       <c r="B429" s="3" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="430" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11863,7 +11863,7 @@
         <v>422</v>
       </c>
       <c r="B430" s="3" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="431" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -11871,7 +11871,7 @@
         <v>213</v>
       </c>
       <c r="B431" s="3" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="432" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -11879,7 +11879,7 @@
         <v>214</v>
       </c>
       <c r="B432" s="3" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="433" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -11887,7 +11887,7 @@
         <v>215</v>
       </c>
       <c r="B433" s="3" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="434" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11895,7 +11895,7 @@
         <v>216</v>
       </c>
       <c r="B434" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="435" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11903,7 +11903,7 @@
         <v>217</v>
       </c>
       <c r="B435" s="3" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="436" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11911,7 +11911,7 @@
         <v>218</v>
       </c>
       <c r="B436" s="3" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="437" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11919,7 +11919,7 @@
         <v>219</v>
       </c>
       <c r="B437" s="3" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="438" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11927,7 +11927,7 @@
         <v>220</v>
       </c>
       <c r="B438" s="3" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="439" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11935,7 +11935,7 @@
         <v>221</v>
       </c>
       <c r="B439" s="3" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="440" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11943,7 +11943,7 @@
         <v>222</v>
       </c>
       <c r="B440" s="3" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="441" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11951,7 +11951,7 @@
         <v>223</v>
       </c>
       <c r="B441" s="3" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="442" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -11959,7 +11959,7 @@
         <v>224</v>
       </c>
       <c r="B442" s="3" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="443" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -11967,7 +11967,7 @@
         <v>329</v>
       </c>
       <c r="B443" s="3" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="444" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11975,7 +11975,7 @@
         <v>385</v>
       </c>
       <c r="B444" s="3" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="445" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11983,7 +11983,7 @@
         <v>225</v>
       </c>
       <c r="B445" s="3" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="446" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -11991,7 +11991,7 @@
         <v>226</v>
       </c>
       <c r="B446" s="3" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="447" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -11999,7 +11999,7 @@
         <v>227</v>
       </c>
       <c r="B447" s="3" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="448" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -12007,7 +12007,7 @@
         <v>228</v>
       </c>
       <c r="B448" s="3" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="449" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -12015,7 +12015,7 @@
         <v>618</v>
       </c>
       <c r="B449" s="3" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="450" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12023,7 +12023,7 @@
         <v>229</v>
       </c>
       <c r="B450" s="3" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="451" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -12031,7 +12031,7 @@
         <v>230</v>
       </c>
       <c r="B451" s="3" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="452" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -12039,7 +12039,7 @@
         <v>231</v>
       </c>
       <c r="B452" s="3" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="453" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12047,7 +12047,7 @@
         <v>257</v>
       </c>
       <c r="B453" s="3" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="454" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -12055,7 +12055,7 @@
         <v>379</v>
       </c>
       <c r="B454" s="3" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="455" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12063,7 +12063,7 @@
         <v>380</v>
       </c>
       <c r="B455" s="3" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="456" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12071,7 +12071,7 @@
         <v>444</v>
       </c>
       <c r="B456" s="3" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="457" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12087,15 +12087,15 @@
         <v>531</v>
       </c>
       <c r="B458" s="3" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="459" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A459" s="2" t="s">
+        <v>1163</v>
+      </c>
+      <c r="B459" s="3" t="s">
         <v>1164</v>
-      </c>
-      <c r="B459" s="3" t="s">
-        <v>1165</v>
       </c>
     </row>
     <row r="460" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -12135,7 +12135,7 @@
         <v>602</v>
       </c>
       <c r="B464" s="3" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="465" spans="1:2" ht="255" x14ac:dyDescent="0.25">
@@ -12143,7 +12143,7 @@
         <v>322</v>
       </c>
       <c r="B465" s="3" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="466" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12151,7 +12151,7 @@
         <v>395</v>
       </c>
       <c r="B466" s="3" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="467" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -12159,7 +12159,7 @@
         <v>394</v>
       </c>
       <c r="B467" s="3" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="468" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12167,7 +12167,7 @@
         <v>396</v>
       </c>
       <c r="B468" s="3" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="469" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12175,7 +12175,7 @@
         <v>397</v>
       </c>
       <c r="B469" s="3" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="470" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12183,7 +12183,7 @@
         <v>398</v>
       </c>
       <c r="B470" s="3" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="471" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12191,7 +12191,7 @@
         <v>399</v>
       </c>
       <c r="B471" s="3" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="472" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12199,7 +12199,7 @@
         <v>400</v>
       </c>
       <c r="B472" s="3" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="473" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12207,7 +12207,7 @@
         <v>431</v>
       </c>
       <c r="B473" s="3" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="474" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -12215,7 +12215,7 @@
         <v>432</v>
       </c>
       <c r="B474" s="3" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="475" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -12223,7 +12223,7 @@
         <v>433</v>
       </c>
       <c r="B475" s="3" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="476" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12231,7 +12231,7 @@
         <v>434</v>
       </c>
       <c r="B476" s="3" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="477" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12239,7 +12239,7 @@
         <v>435</v>
       </c>
       <c r="B477" s="3" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="478" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12247,7 +12247,7 @@
         <v>436</v>
       </c>
       <c r="B478" s="3" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="479" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -12255,7 +12255,7 @@
         <v>437</v>
       </c>
       <c r="B479" s="3" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="480" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12263,7 +12263,7 @@
         <v>438</v>
       </c>
       <c r="B480" s="3" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="481" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12271,7 +12271,7 @@
         <v>439</v>
       </c>
       <c r="B481" s="3" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="482" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -12279,7 +12279,7 @@
         <v>440</v>
       </c>
       <c r="B482" s="3" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="483" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12287,7 +12287,7 @@
         <v>441</v>
       </c>
       <c r="B483" s="3" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="484" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -12295,7 +12295,7 @@
         <v>442</v>
       </c>
       <c r="B484" s="3" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="485" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -12303,7 +12303,7 @@
         <v>443</v>
       </c>
       <c r="B485" s="3" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="486" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -12311,7 +12311,7 @@
         <v>458</v>
       </c>
       <c r="B486" s="3" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="487" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -12319,7 +12319,7 @@
         <v>466</v>
       </c>
       <c r="B487" s="3" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="488" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -12327,7 +12327,7 @@
         <v>467</v>
       </c>
       <c r="B488" s="3" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="489" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -12335,7 +12335,7 @@
         <v>468</v>
       </c>
       <c r="B489" s="3" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="490" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -12343,7 +12343,7 @@
         <v>552</v>
       </c>
       <c r="B490" s="3" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="491" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -12351,7 +12351,7 @@
         <v>633</v>
       </c>
       <c r="B491" s="3" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="492" spans="1:2" ht="255" x14ac:dyDescent="0.25">
@@ -12359,7 +12359,7 @@
         <v>488</v>
       </c>
       <c r="B492" s="1" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="493" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12367,7 +12367,7 @@
         <v>489</v>
       </c>
       <c r="B493" s="1" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="494" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12375,7 +12375,7 @@
         <v>490</v>
       </c>
       <c r="B494" s="1" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="495" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12383,7 +12383,7 @@
         <v>491</v>
       </c>
       <c r="B495" s="1" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="496" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12391,7 +12391,7 @@
         <v>492</v>
       </c>
       <c r="B496" s="1" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="497" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12399,7 +12399,7 @@
         <v>493</v>
       </c>
       <c r="B497" s="1" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="498" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12407,7 +12407,7 @@
         <v>494</v>
       </c>
       <c r="B498" s="1" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="499" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12415,7 +12415,7 @@
         <v>495</v>
       </c>
       <c r="B499" s="1" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="500" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12423,7 +12423,7 @@
         <v>496</v>
       </c>
       <c r="B500" s="1" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="501" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -12431,7 +12431,7 @@
         <v>497</v>
       </c>
       <c r="B501" s="1" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="502" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12439,7 +12439,7 @@
         <v>498</v>
       </c>
       <c r="B502" s="1" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="503" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12447,7 +12447,7 @@
         <v>499</v>
       </c>
       <c r="B503" s="1" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
     </row>
     <row r="504" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -12455,7 +12455,7 @@
         <v>500</v>
       </c>
       <c r="B504" s="1" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="505" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12463,7 +12463,7 @@
         <v>501</v>
       </c>
       <c r="B505" s="1" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="506" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12471,7 +12471,7 @@
         <v>502</v>
       </c>
       <c r="B506" s="1" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="507" spans="1:2" ht="255" x14ac:dyDescent="0.25">
@@ -12479,7 +12479,7 @@
         <v>597</v>
       </c>
       <c r="B507" s="1" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="508" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12487,7 +12487,7 @@
         <v>598</v>
       </c>
       <c r="B508" s="1" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="509" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12495,7 +12495,7 @@
         <v>503</v>
       </c>
       <c r="B509" s="1" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="510" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12503,7 +12503,7 @@
         <v>515</v>
       </c>
       <c r="B510" s="3" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="511" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -12511,7 +12511,7 @@
         <v>423</v>
       </c>
       <c r="B511" s="3" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="512" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12535,7 +12535,7 @@
         <v>267</v>
       </c>
       <c r="B514" s="1" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="515" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12543,7 +12543,7 @@
         <v>268</v>
       </c>
       <c r="B515" s="1" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="516" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12551,7 +12551,7 @@
         <v>269</v>
       </c>
       <c r="B516" s="1" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="517" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12559,7 +12559,7 @@
         <v>270</v>
       </c>
       <c r="B517" s="1" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="518" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12567,7 +12567,7 @@
         <v>271</v>
       </c>
       <c r="B518" s="1" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="519" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12575,7 +12575,7 @@
         <v>272</v>
       </c>
       <c r="B519" s="1" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="520" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12583,7 +12583,7 @@
         <v>273</v>
       </c>
       <c r="B520" s="1" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="521" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12591,7 +12591,7 @@
         <v>274</v>
       </c>
       <c r="B521" s="1" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="522" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12599,7 +12599,7 @@
         <v>275</v>
       </c>
       <c r="B522" s="1" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="523" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12607,7 +12607,7 @@
         <v>276</v>
       </c>
       <c r="B523" s="1" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="524" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12615,7 +12615,7 @@
         <v>277</v>
       </c>
       <c r="B524" s="1" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="525" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12695,7 +12695,7 @@
         <v>280</v>
       </c>
       <c r="B534" s="1" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="535" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12703,7 +12703,7 @@
         <v>281</v>
       </c>
       <c r="B535" s="1" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="536" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12719,7 +12719,7 @@
         <v>283</v>
       </c>
       <c r="B537" s="1" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="538" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12727,7 +12727,7 @@
         <v>284</v>
       </c>
       <c r="B538" s="1" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="539" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12735,7 +12735,7 @@
         <v>285</v>
       </c>
       <c r="B539" s="1" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="540" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12743,7 +12743,7 @@
         <v>286</v>
       </c>
       <c r="B540" s="1" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="541" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12791,7 +12791,7 @@
         <v>292</v>
       </c>
       <c r="B546" s="1" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="547" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12799,7 +12799,7 @@
         <v>293</v>
       </c>
       <c r="B547" s="1" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="548" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12807,7 +12807,7 @@
         <v>294</v>
       </c>
       <c r="B548" s="1" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="549" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12815,7 +12815,7 @@
         <v>295</v>
       </c>
       <c r="B549" s="1" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="550" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -12823,7 +12823,7 @@
         <v>296</v>
       </c>
       <c r="B550" s="1" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="551" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12831,7 +12831,7 @@
         <v>297</v>
       </c>
       <c r="B551" s="1" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="552" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -12839,7 +12839,7 @@
         <v>353</v>
       </c>
       <c r="B552" s="1" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="553" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12847,7 +12847,7 @@
         <v>365</v>
       </c>
       <c r="B553" s="3" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="554" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12855,7 +12855,7 @@
         <v>366</v>
       </c>
       <c r="B554" s="1" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="555" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12863,7 +12863,7 @@
         <v>298</v>
       </c>
       <c r="B555" s="1" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="556" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -12871,7 +12871,7 @@
         <v>364</v>
       </c>
       <c r="B556" s="1" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
     </row>
     <row r="557" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12879,7 +12879,7 @@
         <v>299</v>
       </c>
       <c r="B557" s="1" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
     </row>
     <row r="558" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -12887,7 +12887,7 @@
         <v>354</v>
       </c>
       <c r="B558" s="1" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="559" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -12903,7 +12903,7 @@
         <v>300</v>
       </c>
       <c r="B560" s="1" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="561" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12911,7 +12911,7 @@
         <v>301</v>
       </c>
       <c r="B561" s="1" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="562" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12919,7 +12919,7 @@
         <v>302</v>
       </c>
       <c r="B562" s="1" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="563" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12927,7 +12927,7 @@
         <v>303</v>
       </c>
       <c r="B563" s="1" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="564" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -12935,7 +12935,7 @@
         <v>363</v>
       </c>
       <c r="B564" s="1" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="565" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12943,7 +12943,7 @@
         <v>304</v>
       </c>
       <c r="B565" s="1" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="566" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12951,7 +12951,7 @@
         <v>361</v>
       </c>
       <c r="B566" s="1" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="567" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -12967,7 +12967,7 @@
         <v>517</v>
       </c>
       <c r="B568" s="1" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="569" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12975,7 +12975,7 @@
         <v>305</v>
       </c>
       <c r="B569" s="1" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="570" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12983,7 +12983,7 @@
         <v>358</v>
       </c>
       <c r="B570" s="1" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="571" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12991,7 +12991,7 @@
         <v>359</v>
       </c>
       <c r="B571" s="1" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="572" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -13007,7 +13007,7 @@
         <v>518</v>
       </c>
       <c r="B573" s="1" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="574" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -13015,7 +13015,7 @@
         <v>306</v>
       </c>
       <c r="B574" s="1" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="575" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -13023,7 +13023,7 @@
         <v>352</v>
       </c>
       <c r="B575" s="1" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="576" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -13031,7 +13031,7 @@
         <v>355</v>
       </c>
       <c r="B576" s="3" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="577" spans="1:2" ht="405" x14ac:dyDescent="0.25">
@@ -13039,7 +13039,7 @@
         <v>307</v>
       </c>
       <c r="B577" s="1" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="578" spans="1:2" ht="375" x14ac:dyDescent="0.25">
@@ -13047,7 +13047,7 @@
         <v>311</v>
       </c>
       <c r="B578" s="1" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="579" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -13071,7 +13071,7 @@
         <v>349</v>
       </c>
       <c r="B581" s="3" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="582" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -13079,7 +13079,7 @@
         <v>519</v>
       </c>
       <c r="B582" s="3" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="583" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -13087,7 +13087,7 @@
         <v>326</v>
       </c>
       <c r="B583" s="3" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix issue with Ancient Treasure E027. Update to indicate falcon cuases party to never get lost. Fixed name of Logs directory
</commit_message>
<xml_diff>
--- a/Documentation/Events.xlsx
+++ b/Documentation/Events.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\happysulla\BarbarianPrince\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstewa01\Documents\Visual Studio 2022\Projects\BarbarianPrince\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CC540120-483B-4B15-85E7-6947EE8C4525}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{811CD5D0-0C19-4EB6-93B5-BF2E610E87B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="-25320" yWindow="15" windowWidth="25440" windowHeight="15390" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" r:id="rId1"/>
@@ -5419,19 +5419,6 @@
           &lt;InlineUIContainer&gt;&lt;Image Name='AirOvercast' Source='../bin/Images/Overcast.gif' Height='220' Width='480'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e107 Falcon Scout&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;A friendly falcon joins your party if you &lt;InlineUIContainer&gt;&lt;Button Content='Feed' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; one unit of food
- &lt;InlineUIContainer&gt;&lt;Button Content='r215' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
- right now. For the rest of today, you cannot get lost.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;Tonight, at the evening meal
- &lt;InlineUIContainer&gt;&lt;Button Content='r215' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;,
- if you offer it a second food unit, roll the die. If you roll anyhing other than a six, the falcon will remain throughout tomorrow with your party as a guide.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;This can continue day after day provided you feed it a food unit at the evening meal and roll anything but a six.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;The falcon can only act as a guide. It has no combat skill or endurance value. Any wound will kill it. Click image to continue if not feeding.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                        &lt;InlineUIContainer&gt;&lt;Image Name='FalconNoFeed' Source='../bin/Images/Falcon.gif' Height='188' Width='250'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;e108 Hawkmen Attack&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;You encournter a group of hawkmen who swoop down on your party.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;Each has a combat skill 7, endurance 5, and wealth 7.  Roll one die for the number of hawkmen:  &lt;InlineUIContainer&gt;&lt;Image Source='../bin/Images/dieRoll.gif' Name='DieRoll' Height='21'  Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
@@ -8028,6 +8015,19 @@
  &lt;InlineUIContainer&gt;&lt;Button Content='e053' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  3,4,5,6 - Campsite&lt;LineBreak/&gt;
 &lt;LineBreak/&gt; &lt;LineBreak/&gt;
                                    &lt;InlineUIContainer&gt;&lt;Image Source='../bin/Images/Elf.gif' Height='300' Width='240'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e107 Falcon Scout&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;A friendly falcon joins your party if you &lt;InlineUIContainer&gt;&lt;Button Content='Feed' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; one unit of food
+ &lt;InlineUIContainer&gt;&lt;Button Content='r215' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+ right now. You cannot get lost when you have the falcon.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;Tonight, at the evening meal
+ &lt;InlineUIContainer&gt;&lt;Button Content='r215' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;,
+ if you offer it a second food unit, roll the die. If you roll anyhing other than a six, the falcon will remain throughout tomorrow with your party as a guide.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;This can continue day after day provided you feed it a food unit at the evening meal and roll anything but a six.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;The falcon can only act as a guide. It has no combat skill or endurance value. Any wound will kill it. Click image to continue if not feeding.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                        &lt;InlineUIContainer&gt;&lt;Image Name='FalconNoFeed' Source='../bin/Images/Falcon.gif' Height='188' Width='250'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
 </sst>
 </file>
@@ -8416,8 +8416,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B583"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A211" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B213" sqref="B213"/>
+    <sheetView tabSelected="1" topLeftCell="B284" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B287" sqref="B287"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9199,7 +9199,7 @@
         <v>61</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -9455,7 +9455,7 @@
         <v>350</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="130" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10127,7 +10127,7 @@
         <v>516</v>
       </c>
       <c r="B213" s="3" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="214" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10183,7 +10183,7 @@
         <v>266</v>
       </c>
       <c r="B220" s="3" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
     </row>
     <row r="221" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -10487,7 +10487,7 @@
         <v>132</v>
       </c>
       <c r="B258" s="3" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
     </row>
     <row r="259" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10719,7 +10719,7 @@
         <v>146</v>
       </c>
       <c r="B287" s="3" t="s">
-        <v>911</v>
+        <v>1165</v>
       </c>
     </row>
     <row r="288" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10727,7 +10727,7 @@
         <v>147</v>
       </c>
       <c r="B288" s="3" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
     </row>
     <row r="289" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10735,7 +10735,7 @@
         <v>148</v>
       </c>
       <c r="B289" s="3" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
     </row>
     <row r="290" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10743,7 +10743,7 @@
         <v>149</v>
       </c>
       <c r="B290" s="3" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
     </row>
     <row r="291" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10751,7 +10751,7 @@
         <v>605</v>
       </c>
       <c r="B291" s="3" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
     </row>
     <row r="292" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10759,7 +10759,7 @@
         <v>604</v>
       </c>
       <c r="B292" s="3" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="293" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10767,7 +10767,7 @@
         <v>606</v>
       </c>
       <c r="B293" s="3" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
     </row>
     <row r="294" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10775,7 +10775,7 @@
         <v>150</v>
       </c>
       <c r="B294" s="3" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
     </row>
     <row r="295" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10783,7 +10783,7 @@
         <v>607</v>
       </c>
       <c r="B295" s="3" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
     </row>
     <row r="296" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -10791,7 +10791,7 @@
         <v>151</v>
       </c>
       <c r="B296" s="3" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
     </row>
     <row r="297" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10799,7 +10799,7 @@
         <v>243</v>
       </c>
       <c r="B297" s="3" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
     </row>
     <row r="298" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10807,7 +10807,7 @@
         <v>244</v>
       </c>
       <c r="B298" s="3" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
     </row>
     <row r="299" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10815,7 +10815,7 @@
         <v>245</v>
       </c>
       <c r="B299" s="3" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
     </row>
     <row r="300" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10823,7 +10823,7 @@
         <v>152</v>
       </c>
       <c r="B300" s="3" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
     </row>
     <row r="301" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10831,7 +10831,7 @@
         <v>153</v>
       </c>
       <c r="B301" s="3" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
     </row>
     <row r="302" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10839,7 +10839,7 @@
         <v>154</v>
       </c>
       <c r="B302" s="3" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
     </row>
     <row r="303" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -10847,7 +10847,7 @@
         <v>155</v>
       </c>
       <c r="B303" s="3" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
     </row>
     <row r="304" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10855,7 +10855,7 @@
         <v>156</v>
       </c>
       <c r="B304" s="3" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
     </row>
     <row r="305" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10871,7 +10871,7 @@
         <v>246</v>
       </c>
       <c r="B306" s="3" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
     </row>
     <row r="307" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10879,7 +10879,7 @@
         <v>247</v>
       </c>
       <c r="B307" s="3" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
     </row>
     <row r="308" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10887,7 +10887,7 @@
         <v>248</v>
       </c>
       <c r="B308" s="3" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
     </row>
     <row r="309" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10903,7 +10903,7 @@
         <v>159</v>
       </c>
       <c r="B310" s="3" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
     </row>
     <row r="311" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10911,7 +10911,7 @@
         <v>160</v>
       </c>
       <c r="B311" s="3" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
     </row>
     <row r="312" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -10919,7 +10919,7 @@
         <v>161</v>
       </c>
       <c r="B312" s="3" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
     </row>
     <row r="313" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -10927,7 +10927,7 @@
         <v>162</v>
       </c>
       <c r="B313" s="3" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
     </row>
     <row r="314" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -10935,7 +10935,7 @@
         <v>599</v>
       </c>
       <c r="B314" s="3" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
     </row>
     <row r="315" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10943,7 +10943,7 @@
         <v>600</v>
       </c>
       <c r="B315" s="3" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
     </row>
     <row r="316" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10951,7 +10951,7 @@
         <v>601</v>
       </c>
       <c r="B316" s="3" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
     </row>
     <row r="317" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10959,7 +10959,7 @@
         <v>163</v>
       </c>
       <c r="B317" s="3" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
     </row>
     <row r="318" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10967,7 +10967,7 @@
         <v>164</v>
       </c>
       <c r="B318" s="3" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
     </row>
     <row r="319" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10975,7 +10975,7 @@
         <v>175</v>
       </c>
       <c r="B319" s="3" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
     </row>
     <row r="320" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -10983,7 +10983,7 @@
         <v>176</v>
       </c>
       <c r="B320" s="3" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
     </row>
     <row r="321" spans="1:2" ht="390" x14ac:dyDescent="0.25">
@@ -10991,7 +10991,7 @@
         <v>177</v>
       </c>
       <c r="B321" s="3" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
     </row>
     <row r="322" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -11007,7 +11007,7 @@
         <v>414</v>
       </c>
       <c r="B323" s="3" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
     </row>
     <row r="324" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11015,7 +11015,7 @@
         <v>415</v>
       </c>
       <c r="B324" s="3" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
     </row>
     <row r="325" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -11023,7 +11023,7 @@
         <v>416</v>
       </c>
       <c r="B325" s="3" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
     </row>
     <row r="326" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -11031,7 +11031,7 @@
         <v>417</v>
       </c>
       <c r="B326" s="3" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
     </row>
     <row r="327" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11039,7 +11039,7 @@
         <v>418</v>
       </c>
       <c r="B327" s="3" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
     </row>
     <row r="328" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11047,7 +11047,7 @@
         <v>613</v>
       </c>
       <c r="B328" s="3" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
     </row>
     <row r="329" spans="1:2" ht="390" x14ac:dyDescent="0.25">
@@ -11055,7 +11055,7 @@
         <v>178</v>
       </c>
       <c r="B329" s="3" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
     </row>
     <row r="330" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -11071,7 +11071,7 @@
         <v>426</v>
       </c>
       <c r="B331" s="3" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
     </row>
     <row r="332" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11079,7 +11079,7 @@
         <v>427</v>
       </c>
       <c r="B332" s="3" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
     </row>
     <row r="333" spans="1:2" ht="315" x14ac:dyDescent="0.25">
@@ -11087,7 +11087,7 @@
         <v>179</v>
       </c>
       <c r="B333" s="3" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
     </row>
     <row r="334" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -11095,7 +11095,7 @@
         <v>249</v>
       </c>
       <c r="B334" s="3" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
     </row>
     <row r="335" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -11103,7 +11103,7 @@
         <v>250</v>
       </c>
       <c r="B335" s="3" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
     </row>
     <row r="336" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -11111,7 +11111,7 @@
         <v>251</v>
       </c>
       <c r="B336" s="3" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
     </row>
     <row r="337" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11119,7 +11119,7 @@
         <v>252</v>
       </c>
       <c r="B337" s="3" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
     </row>
     <row r="338" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -11127,7 +11127,7 @@
         <v>253</v>
       </c>
       <c r="B338" s="3" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
     </row>
     <row r="339" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -11135,7 +11135,7 @@
         <v>545</v>
       </c>
       <c r="B339" s="3" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
     </row>
     <row r="340" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -11143,7 +11143,7 @@
         <v>546</v>
       </c>
       <c r="B340" s="3" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="341" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11151,7 +11151,7 @@
         <v>180</v>
       </c>
       <c r="B341" s="3" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
     </row>
     <row r="342" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11159,7 +11159,7 @@
         <v>181</v>
       </c>
       <c r="B342" s="3" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
     </row>
     <row r="343" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11167,7 +11167,7 @@
         <v>386</v>
       </c>
       <c r="B343" s="3" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
     </row>
     <row r="344" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -11183,7 +11183,7 @@
         <v>622</v>
       </c>
       <c r="B345" s="3" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
     </row>
     <row r="346" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11191,7 +11191,7 @@
         <v>183</v>
       </c>
       <c r="B346" s="3" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
     </row>
     <row r="347" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -11199,7 +11199,7 @@
         <v>184</v>
       </c>
       <c r="B347" s="3" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
     </row>
     <row r="348" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -11215,7 +11215,7 @@
         <v>185</v>
       </c>
       <c r="B349" s="3" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
     </row>
     <row r="350" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -11223,7 +11223,7 @@
         <v>186</v>
       </c>
       <c r="B350" s="3" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
     </row>
     <row r="351" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -11231,7 +11231,7 @@
         <v>187</v>
       </c>
       <c r="B351" s="3" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
     </row>
     <row r="352" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11247,7 +11247,7 @@
         <v>188</v>
       </c>
       <c r="B353" s="3" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
     </row>
     <row r="354" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -11255,7 +11255,7 @@
         <v>189</v>
       </c>
       <c r="B354" s="3" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
     </row>
     <row r="355" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -11263,7 +11263,7 @@
         <v>383</v>
       </c>
       <c r="B355" s="3" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
     </row>
     <row r="356" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -11271,7 +11271,7 @@
         <v>384</v>
       </c>
       <c r="B356" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="357" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -11279,7 +11279,7 @@
         <v>190</v>
       </c>
       <c r="B357" s="3" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
     </row>
     <row r="358" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -11287,7 +11287,7 @@
         <v>191</v>
       </c>
       <c r="B358" s="3" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
     </row>
     <row r="359" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -11295,7 +11295,7 @@
         <v>192</v>
       </c>
       <c r="B359" s="3" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
     </row>
     <row r="360" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -11303,7 +11303,7 @@
         <v>465</v>
       </c>
       <c r="B360" s="3" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
     </row>
     <row r="361" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -11311,7 +11311,7 @@
         <v>193</v>
       </c>
       <c r="B361" s="3" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="362" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -11327,7 +11327,7 @@
         <v>333</v>
       </c>
       <c r="B363" s="3" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
     </row>
     <row r="364" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -11335,7 +11335,7 @@
         <v>624</v>
       </c>
       <c r="B364" s="3" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="365" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -11343,7 +11343,7 @@
         <v>625</v>
       </c>
       <c r="B365" s="3" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
     </row>
     <row r="366" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11351,7 +11351,7 @@
         <v>627</v>
       </c>
       <c r="B366" s="3" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
     </row>
     <row r="367" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11359,7 +11359,7 @@
         <v>628</v>
       </c>
       <c r="B367" s="3" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
     </row>
     <row r="368" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11367,7 +11367,7 @@
         <v>629</v>
       </c>
       <c r="B368" s="3" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
     </row>
     <row r="369" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11375,7 +11375,7 @@
         <v>630</v>
       </c>
       <c r="B369" s="3" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
     </row>
     <row r="370" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11383,7 +11383,7 @@
         <v>631</v>
       </c>
       <c r="B370" s="3" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
     </row>
     <row r="371" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11391,7 +11391,7 @@
         <v>632</v>
       </c>
       <c r="B371" s="3" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
     </row>
     <row r="372" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -11399,7 +11399,7 @@
         <v>194</v>
       </c>
       <c r="B372" s="3" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
     </row>
     <row r="373" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -11407,7 +11407,7 @@
         <v>195</v>
       </c>
       <c r="B373" s="3" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
     </row>
     <row r="374" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -11415,7 +11415,7 @@
         <v>620</v>
       </c>
       <c r="B374" s="3" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
     </row>
     <row r="375" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -11423,7 +11423,7 @@
         <v>196</v>
       </c>
       <c r="B375" s="3" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="376" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -11431,7 +11431,7 @@
         <v>328</v>
       </c>
       <c r="B376" s="3" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
     </row>
     <row r="377" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -11439,7 +11439,7 @@
         <v>197</v>
       </c>
       <c r="B377" s="3" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
     </row>
     <row r="378" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11447,7 +11447,7 @@
         <v>487</v>
       </c>
       <c r="B378" s="3" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
     </row>
     <row r="379" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11455,7 +11455,7 @@
         <v>198</v>
       </c>
       <c r="B379" s="3" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
     </row>
     <row r="380" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11463,7 +11463,7 @@
         <v>199</v>
       </c>
       <c r="B380" s="3" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
     </row>
     <row r="381" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -11471,7 +11471,7 @@
         <v>200</v>
       </c>
       <c r="B381" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="382" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11479,7 +11479,7 @@
         <v>201</v>
       </c>
       <c r="B382" s="3" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
     </row>
     <row r="383" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11487,7 +11487,7 @@
         <v>202</v>
       </c>
       <c r="B383" s="3" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
     </row>
     <row r="384" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -11495,7 +11495,7 @@
         <v>203</v>
       </c>
       <c r="B384" s="3" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
     </row>
     <row r="385" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -11543,7 +11543,7 @@
         <v>204</v>
       </c>
       <c r="B390" s="3" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="391" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11551,7 +11551,7 @@
         <v>459</v>
       </c>
       <c r="B391" s="3" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="392" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11559,7 +11559,7 @@
         <v>460</v>
       </c>
       <c r="B392" s="3" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="393" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11567,7 +11567,7 @@
         <v>461</v>
       </c>
       <c r="B393" s="3" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="394" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11575,7 +11575,7 @@
         <v>462</v>
       </c>
       <c r="B394" s="3" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="395" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11583,7 +11583,7 @@
         <v>463</v>
       </c>
       <c r="B395" s="3" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="396" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11591,7 +11591,7 @@
         <v>464</v>
       </c>
       <c r="B396" s="3" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="397" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -11599,7 +11599,7 @@
         <v>205</v>
       </c>
       <c r="B397" s="3" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="398" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -11671,7 +11671,7 @@
         <v>207</v>
       </c>
       <c r="B406" s="3" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="407" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -11679,7 +11679,7 @@
         <v>208</v>
       </c>
       <c r="B407" s="3" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="408" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -11687,7 +11687,7 @@
         <v>209</v>
       </c>
       <c r="B408" s="3" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="409" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11695,7 +11695,7 @@
         <v>476</v>
       </c>
       <c r="B409" s="3" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="410" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11703,7 +11703,7 @@
         <v>477</v>
       </c>
       <c r="B410" s="3" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="411" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11711,7 +11711,7 @@
         <v>478</v>
       </c>
       <c r="B411" s="3" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="412" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -11719,7 +11719,7 @@
         <v>479</v>
       </c>
       <c r="B412" s="3" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="413" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -11727,7 +11727,7 @@
         <v>480</v>
       </c>
       <c r="B413" s="4" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="414" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -11735,7 +11735,7 @@
         <v>481</v>
       </c>
       <c r="B414" s="3" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="415" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -11743,7 +11743,7 @@
         <v>621</v>
       </c>
       <c r="B415" s="3" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="416" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -11751,7 +11751,7 @@
         <v>210</v>
       </c>
       <c r="B416" s="3" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="417" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11759,7 +11759,7 @@
         <v>469</v>
       </c>
       <c r="B417" s="3" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="418" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11767,7 +11767,7 @@
         <v>470</v>
       </c>
       <c r="B418" s="3" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="419" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11775,7 +11775,7 @@
         <v>471</v>
       </c>
       <c r="B419" s="3" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="420" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11783,7 +11783,7 @@
         <v>472</v>
       </c>
       <c r="B420" s="3" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="421" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11791,7 +11791,7 @@
         <v>473</v>
       </c>
       <c r="B421" s="3" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="422" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11799,7 +11799,7 @@
         <v>474</v>
       </c>
       <c r="B422" s="3" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="423" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11807,7 +11807,7 @@
         <v>475</v>
       </c>
       <c r="B423" s="3" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="424" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11815,7 +11815,7 @@
         <v>619</v>
       </c>
       <c r="B424" s="3" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="425" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -11823,7 +11823,7 @@
         <v>211</v>
       </c>
       <c r="B425" s="3" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="426" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11831,7 +11831,7 @@
         <v>212</v>
       </c>
       <c r="B426" s="3" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="427" spans="1:2" ht="300" x14ac:dyDescent="0.25">
@@ -11839,7 +11839,7 @@
         <v>419</v>
       </c>
       <c r="B427" s="3" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="428" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11847,7 +11847,7 @@
         <v>420</v>
       </c>
       <c r="B428" s="3" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="429" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -11855,7 +11855,7 @@
         <v>421</v>
       </c>
       <c r="B429" s="3" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="430" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11863,7 +11863,7 @@
         <v>422</v>
       </c>
       <c r="B430" s="3" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="431" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -11871,7 +11871,7 @@
         <v>213</v>
       </c>
       <c r="B431" s="3" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="432" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -11879,7 +11879,7 @@
         <v>214</v>
       </c>
       <c r="B432" s="3" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="433" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -11887,7 +11887,7 @@
         <v>215</v>
       </c>
       <c r="B433" s="3" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="434" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11895,7 +11895,7 @@
         <v>216</v>
       </c>
       <c r="B434" s="3" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="435" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11903,7 +11903,7 @@
         <v>217</v>
       </c>
       <c r="B435" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="436" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11911,7 +11911,7 @@
         <v>218</v>
       </c>
       <c r="B436" s="3" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="437" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11919,7 +11919,7 @@
         <v>219</v>
       </c>
       <c r="B437" s="3" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="438" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11927,7 +11927,7 @@
         <v>220</v>
       </c>
       <c r="B438" s="3" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="439" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11935,7 +11935,7 @@
         <v>221</v>
       </c>
       <c r="B439" s="3" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="440" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11943,7 +11943,7 @@
         <v>222</v>
       </c>
       <c r="B440" s="3" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="441" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11951,7 +11951,7 @@
         <v>223</v>
       </c>
       <c r="B441" s="3" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="442" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -11959,7 +11959,7 @@
         <v>224</v>
       </c>
       <c r="B442" s="3" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="443" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -11967,7 +11967,7 @@
         <v>329</v>
       </c>
       <c r="B443" s="3" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="444" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11975,7 +11975,7 @@
         <v>385</v>
       </c>
       <c r="B444" s="3" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="445" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11983,7 +11983,7 @@
         <v>225</v>
       </c>
       <c r="B445" s="3" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="446" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -11991,7 +11991,7 @@
         <v>226</v>
       </c>
       <c r="B446" s="3" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="447" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -11999,7 +11999,7 @@
         <v>227</v>
       </c>
       <c r="B447" s="3" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="448" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -12007,7 +12007,7 @@
         <v>228</v>
       </c>
       <c r="B448" s="3" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="449" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -12015,7 +12015,7 @@
         <v>618</v>
       </c>
       <c r="B449" s="3" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="450" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12023,7 +12023,7 @@
         <v>229</v>
       </c>
       <c r="B450" s="3" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="451" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -12031,7 +12031,7 @@
         <v>230</v>
       </c>
       <c r="B451" s="3" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="452" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -12039,7 +12039,7 @@
         <v>231</v>
       </c>
       <c r="B452" s="3" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="453" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12047,7 +12047,7 @@
         <v>257</v>
       </c>
       <c r="B453" s="3" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="454" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -12055,7 +12055,7 @@
         <v>379</v>
       </c>
       <c r="B454" s="3" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="455" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12063,7 +12063,7 @@
         <v>380</v>
       </c>
       <c r="B455" s="3" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="456" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12071,7 +12071,7 @@
         <v>444</v>
       </c>
       <c r="B456" s="3" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="457" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12087,15 +12087,15 @@
         <v>531</v>
       </c>
       <c r="B458" s="3" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="459" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A459" s="2" t="s">
+        <v>1162</v>
+      </c>
+      <c r="B459" s="3" t="s">
         <v>1163</v>
-      </c>
-      <c r="B459" s="3" t="s">
-        <v>1164</v>
       </c>
     </row>
     <row r="460" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -12135,7 +12135,7 @@
         <v>602</v>
       </c>
       <c r="B464" s="3" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="465" spans="1:2" ht="255" x14ac:dyDescent="0.25">
@@ -12143,7 +12143,7 @@
         <v>322</v>
       </c>
       <c r="B465" s="3" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="466" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12151,7 +12151,7 @@
         <v>395</v>
       </c>
       <c r="B466" s="3" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="467" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -12159,7 +12159,7 @@
         <v>394</v>
       </c>
       <c r="B467" s="3" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="468" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12167,7 +12167,7 @@
         <v>396</v>
       </c>
       <c r="B468" s="3" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="469" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12175,7 +12175,7 @@
         <v>397</v>
       </c>
       <c r="B469" s="3" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="470" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12183,7 +12183,7 @@
         <v>398</v>
       </c>
       <c r="B470" s="3" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="471" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12191,7 +12191,7 @@
         <v>399</v>
       </c>
       <c r="B471" s="3" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="472" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12199,7 +12199,7 @@
         <v>400</v>
       </c>
       <c r="B472" s="3" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="473" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12207,7 +12207,7 @@
         <v>431</v>
       </c>
       <c r="B473" s="3" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="474" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -12215,7 +12215,7 @@
         <v>432</v>
       </c>
       <c r="B474" s="3" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="475" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -12223,7 +12223,7 @@
         <v>433</v>
       </c>
       <c r="B475" s="3" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="476" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12231,7 +12231,7 @@
         <v>434</v>
       </c>
       <c r="B476" s="3" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="477" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12239,7 +12239,7 @@
         <v>435</v>
       </c>
       <c r="B477" s="3" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="478" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12247,7 +12247,7 @@
         <v>436</v>
       </c>
       <c r="B478" s="3" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="479" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -12255,7 +12255,7 @@
         <v>437</v>
       </c>
       <c r="B479" s="3" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="480" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12263,7 +12263,7 @@
         <v>438</v>
       </c>
       <c r="B480" s="3" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="481" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12271,7 +12271,7 @@
         <v>439</v>
       </c>
       <c r="B481" s="3" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="482" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -12279,7 +12279,7 @@
         <v>440</v>
       </c>
       <c r="B482" s="3" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="483" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12287,7 +12287,7 @@
         <v>441</v>
       </c>
       <c r="B483" s="3" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="484" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -12295,7 +12295,7 @@
         <v>442</v>
       </c>
       <c r="B484" s="3" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="485" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -12303,7 +12303,7 @@
         <v>443</v>
       </c>
       <c r="B485" s="3" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="486" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -12311,7 +12311,7 @@
         <v>458</v>
       </c>
       <c r="B486" s="3" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="487" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -12319,7 +12319,7 @@
         <v>466</v>
       </c>
       <c r="B487" s="3" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="488" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -12327,7 +12327,7 @@
         <v>467</v>
       </c>
       <c r="B488" s="3" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="489" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -12335,7 +12335,7 @@
         <v>468</v>
       </c>
       <c r="B489" s="3" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="490" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -12343,7 +12343,7 @@
         <v>552</v>
       </c>
       <c r="B490" s="3" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="491" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -12351,7 +12351,7 @@
         <v>633</v>
       </c>
       <c r="B491" s="3" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="492" spans="1:2" ht="255" x14ac:dyDescent="0.25">
@@ -12359,7 +12359,7 @@
         <v>488</v>
       </c>
       <c r="B492" s="1" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="493" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12367,7 +12367,7 @@
         <v>489</v>
       </c>
       <c r="B493" s="1" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="494" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12375,7 +12375,7 @@
         <v>490</v>
       </c>
       <c r="B494" s="1" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="495" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12383,7 +12383,7 @@
         <v>491</v>
       </c>
       <c r="B495" s="1" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="496" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12391,7 +12391,7 @@
         <v>492</v>
       </c>
       <c r="B496" s="1" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="497" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12399,7 +12399,7 @@
         <v>493</v>
       </c>
       <c r="B497" s="1" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="498" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12407,7 +12407,7 @@
         <v>494</v>
       </c>
       <c r="B498" s="1" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="499" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12415,7 +12415,7 @@
         <v>495</v>
       </c>
       <c r="B499" s="1" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="500" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12423,7 +12423,7 @@
         <v>496</v>
       </c>
       <c r="B500" s="1" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="501" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -12431,7 +12431,7 @@
         <v>497</v>
       </c>
       <c r="B501" s="1" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="502" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12439,7 +12439,7 @@
         <v>498</v>
       </c>
       <c r="B502" s="1" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="503" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12447,7 +12447,7 @@
         <v>499</v>
       </c>
       <c r="B503" s="1" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="504" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -12455,7 +12455,7 @@
         <v>500</v>
       </c>
       <c r="B504" s="1" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="505" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12463,7 +12463,7 @@
         <v>501</v>
       </c>
       <c r="B505" s="1" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="506" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12471,7 +12471,7 @@
         <v>502</v>
       </c>
       <c r="B506" s="1" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="507" spans="1:2" ht="255" x14ac:dyDescent="0.25">
@@ -12479,7 +12479,7 @@
         <v>597</v>
       </c>
       <c r="B507" s="1" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="508" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12487,7 +12487,7 @@
         <v>598</v>
       </c>
       <c r="B508" s="1" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="509" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12495,7 +12495,7 @@
         <v>503</v>
       </c>
       <c r="B509" s="1" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="510" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12503,7 +12503,7 @@
         <v>515</v>
       </c>
       <c r="B510" s="3" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="511" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -12511,7 +12511,7 @@
         <v>423</v>
       </c>
       <c r="B511" s="3" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="512" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12535,7 +12535,7 @@
         <v>267</v>
       </c>
       <c r="B514" s="1" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="515" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12543,7 +12543,7 @@
         <v>268</v>
       </c>
       <c r="B515" s="1" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="516" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12551,7 +12551,7 @@
         <v>269</v>
       </c>
       <c r="B516" s="1" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="517" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12559,7 +12559,7 @@
         <v>270</v>
       </c>
       <c r="B517" s="1" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="518" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12567,7 +12567,7 @@
         <v>271</v>
       </c>
       <c r="B518" s="1" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="519" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12575,7 +12575,7 @@
         <v>272</v>
       </c>
       <c r="B519" s="1" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="520" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12583,7 +12583,7 @@
         <v>273</v>
       </c>
       <c r="B520" s="1" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="521" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12591,7 +12591,7 @@
         <v>274</v>
       </c>
       <c r="B521" s="1" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="522" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12599,7 +12599,7 @@
         <v>275</v>
       </c>
       <c r="B522" s="1" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="523" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12607,7 +12607,7 @@
         <v>276</v>
       </c>
       <c r="B523" s="1" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="524" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12615,7 +12615,7 @@
         <v>277</v>
       </c>
       <c r="B524" s="1" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="525" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12695,7 +12695,7 @@
         <v>280</v>
       </c>
       <c r="B534" s="1" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="535" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12703,7 +12703,7 @@
         <v>281</v>
       </c>
       <c r="B535" s="1" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="536" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12719,7 +12719,7 @@
         <v>283</v>
       </c>
       <c r="B537" s="1" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="538" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12727,7 +12727,7 @@
         <v>284</v>
       </c>
       <c r="B538" s="1" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="539" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12735,7 +12735,7 @@
         <v>285</v>
       </c>
       <c r="B539" s="1" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="540" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12743,7 +12743,7 @@
         <v>286</v>
       </c>
       <c r="B540" s="1" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="541" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12791,7 +12791,7 @@
         <v>292</v>
       </c>
       <c r="B546" s="1" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="547" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12799,7 +12799,7 @@
         <v>293</v>
       </c>
       <c r="B547" s="1" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="548" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12807,7 +12807,7 @@
         <v>294</v>
       </c>
       <c r="B548" s="1" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="549" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12815,7 +12815,7 @@
         <v>295</v>
       </c>
       <c r="B549" s="1" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="550" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -12823,7 +12823,7 @@
         <v>296</v>
       </c>
       <c r="B550" s="1" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="551" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12831,7 +12831,7 @@
         <v>297</v>
       </c>
       <c r="B551" s="1" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="552" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -12839,7 +12839,7 @@
         <v>353</v>
       </c>
       <c r="B552" s="1" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="553" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12847,7 +12847,7 @@
         <v>365</v>
       </c>
       <c r="B553" s="3" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="554" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12855,7 +12855,7 @@
         <v>366</v>
       </c>
       <c r="B554" s="1" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="555" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12863,7 +12863,7 @@
         <v>298</v>
       </c>
       <c r="B555" s="1" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="556" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -12871,7 +12871,7 @@
         <v>364</v>
       </c>
       <c r="B556" s="1" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="557" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12879,7 +12879,7 @@
         <v>299</v>
       </c>
       <c r="B557" s="1" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
     </row>
     <row r="558" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -12887,7 +12887,7 @@
         <v>354</v>
       </c>
       <c r="B558" s="1" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
     </row>
     <row r="559" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -12903,7 +12903,7 @@
         <v>300</v>
       </c>
       <c r="B560" s="1" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="561" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12911,7 +12911,7 @@
         <v>301</v>
       </c>
       <c r="B561" s="1" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="562" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12919,7 +12919,7 @@
         <v>302</v>
       </c>
       <c r="B562" s="1" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="563" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12927,7 +12927,7 @@
         <v>303</v>
       </c>
       <c r="B563" s="1" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="564" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -12935,7 +12935,7 @@
         <v>363</v>
       </c>
       <c r="B564" s="1" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="565" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12943,7 +12943,7 @@
         <v>304</v>
       </c>
       <c r="B565" s="1" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="566" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12951,7 +12951,7 @@
         <v>361</v>
       </c>
       <c r="B566" s="1" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="567" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -12967,7 +12967,7 @@
         <v>517</v>
       </c>
       <c r="B568" s="1" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="569" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12975,7 +12975,7 @@
         <v>305</v>
       </c>
       <c r="B569" s="1" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="570" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12983,7 +12983,7 @@
         <v>358</v>
       </c>
       <c r="B570" s="1" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="571" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12991,7 +12991,7 @@
         <v>359</v>
       </c>
       <c r="B571" s="1" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="572" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -13007,7 +13007,7 @@
         <v>518</v>
       </c>
       <c r="B573" s="1" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="574" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -13015,7 +13015,7 @@
         <v>306</v>
       </c>
       <c r="B574" s="1" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="575" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -13023,7 +13023,7 @@
         <v>352</v>
       </c>
       <c r="B575" s="1" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="576" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -13031,7 +13031,7 @@
         <v>355</v>
       </c>
       <c r="B576" s="3" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="577" spans="1:2" ht="405" x14ac:dyDescent="0.25">
@@ -13039,7 +13039,7 @@
         <v>307</v>
       </c>
       <c r="B577" s="1" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="578" spans="1:2" ht="375" x14ac:dyDescent="0.25">
@@ -13047,7 +13047,7 @@
         <v>311</v>
       </c>
       <c r="B578" s="1" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="579" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -13071,7 +13071,7 @@
         <v>349</v>
       </c>
       <c r="B581" s="3" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="582" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -13079,7 +13079,7 @@
         <v>519</v>
       </c>
       <c r="B582" s="3" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="583" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -13087,7 +13087,7 @@
         <v>326</v>
       </c>
       <c r="B583" s="3" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Do not do an EncounterEnd after Search for Treasure (e026). EncounterEnd is performed when e026a is displayed
</commit_message>
<xml_diff>
--- a/Documentation/Events.xlsx
+++ b/Documentation/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstewa01\Documents\Visual Studio 2022\Projects\BarbarianPrince\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{811CD5D0-0C19-4EB6-93B5-BF2E610E87B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BB0B4EE8-A1D4-4340-980B-87E8E3D7414E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25320" yWindow="15" windowWidth="25440" windowHeight="15390" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -4719,19 +4719,6 @@
      &lt;InlineUIContainer&gt;&lt;Image Source='../bin/Images/Elves.gif' Height='250' Width='550'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e072a Follow an Elven Band&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt; Roll one die and add one for the number of elves in the band. Die Roll=
-&lt;InlineUIContainer&gt;&lt;Image Source='../bin/Images/dieRoll.gif' Name='DieRoll' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;Each elf has combat skill 5, endurance 4, and wealth 7. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;After making a follow move
- &lt;InlineUIContainer&gt;&lt;Button Content='e071' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
-, roll one die to see where you end the day: &lt;InlineUIContainer&gt;&lt;Image Source='../bin/Images/dieRoll.gif' Name='DieRoll1' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
- &lt;InlineUIContainer&gt;&lt;Button Content='e165' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  1 - Eleven Town&lt;LineBreak/&gt;
- &lt;InlineUIContainer&gt;&lt;Button Content='e166' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  2 - Elven Castle&lt;LineBreak/&gt;
- &lt;InlineUIContainer&gt;&lt;Button Content='e053' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  3,4,5,6 - Campsite</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;e072b Campsite Decision&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 You may peacefully share the campsite with the elves eating your own food or hunting where possible
@@ -8028,6 +8015,19 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;The falcon can only act as a guide. It has no combat skill or endurance value. Any wound will kill it. Click image to continue if not feeding.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
                                         &lt;InlineUIContainer&gt;&lt;Image Name='FalconNoFeed' Source='../bin/Images/Falcon.gif' Height='188' Width='250'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e072a Follow an Elven Band&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt; Roll one die and add one for the number of elves in the band. Die Roll=
+&lt;InlineUIContainer&gt;&lt;Image Source='../bin/Images/dieRoll.gif' Name='DieRoll' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;Each elf has combat skill 5, endurance 4, and wealth 7. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;After making a follow move
+ &lt;InlineUIContainer&gt;&lt;Button Content='e071' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+, roll one die to see where you end the day: &lt;InlineUIContainer&gt;&lt;Image Source='../bin/Images/dieRoll.gif' Name='DieRoll1' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+ &lt;InlineUIContainer&gt;&lt;Button Content='e165' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  1 - Eleven Town&lt;LineBreak/&gt;
+ &lt;InlineUIContainer&gt;&lt;Button Content='e166' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  2 - Elven Fortress&lt;LineBreak/&gt;
+ &lt;InlineUIContainer&gt;&lt;Button Content='e053' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  3,4,5,6 - Campsite</t>
   </si>
 </sst>
 </file>
@@ -8416,8 +8416,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B583"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B284" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B287" sqref="B287"/>
+    <sheetView tabSelected="1" topLeftCell="B209" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B210" sqref="B210"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9199,7 +9199,7 @@
         <v>61</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -9455,7 +9455,7 @@
         <v>350</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
     </row>
     <row r="130" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10103,7 +10103,7 @@
         <v>510</v>
       </c>
       <c r="B210" s="3" t="s">
-        <v>841</v>
+        <v>1165</v>
       </c>
     </row>
     <row r="211" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -10111,7 +10111,7 @@
         <v>511</v>
       </c>
       <c r="B211" s="3" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
     </row>
     <row r="212" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -10127,7 +10127,7 @@
         <v>516</v>
       </c>
       <c r="B213" s="3" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
     </row>
     <row r="214" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10135,7 +10135,7 @@
         <v>112</v>
       </c>
       <c r="B214" s="3" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
     </row>
     <row r="215" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10143,7 +10143,7 @@
         <v>169</v>
       </c>
       <c r="B215" s="3" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
     </row>
     <row r="216" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10151,7 +10151,7 @@
         <v>170</v>
       </c>
       <c r="B216" s="3" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="217" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10159,7 +10159,7 @@
         <v>171</v>
       </c>
       <c r="B217" s="3" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
     </row>
     <row r="218" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -10167,7 +10167,7 @@
         <v>113</v>
       </c>
       <c r="B218" s="3" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="219" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -10175,7 +10175,7 @@
         <v>114</v>
       </c>
       <c r="B219" s="3" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
     </row>
     <row r="220" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10183,7 +10183,7 @@
         <v>266</v>
       </c>
       <c r="B220" s="3" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="221" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -10191,7 +10191,7 @@
         <v>570</v>
       </c>
       <c r="B221" s="3" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="222" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10199,7 +10199,7 @@
         <v>115</v>
       </c>
       <c r="B222" s="3" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="223" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10207,7 +10207,7 @@
         <v>522</v>
       </c>
       <c r="B223" s="3" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
     </row>
     <row r="224" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -10215,7 +10215,7 @@
         <v>116</v>
       </c>
       <c r="B224" s="3" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
     </row>
     <row r="225" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10223,7 +10223,7 @@
         <v>520</v>
       </c>
       <c r="B225" s="3" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
     </row>
     <row r="226" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10231,7 +10231,7 @@
         <v>117</v>
       </c>
       <c r="B226" s="4" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
     </row>
     <row r="227" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10239,7 +10239,7 @@
         <v>523</v>
       </c>
       <c r="B227" s="4" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
     </row>
     <row r="228" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10247,7 +10247,7 @@
         <v>524</v>
       </c>
       <c r="B228" s="4" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
     </row>
     <row r="229" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10255,7 +10255,7 @@
         <v>525</v>
       </c>
       <c r="B229" s="4" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
     </row>
     <row r="230" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10263,7 +10263,7 @@
         <v>118</v>
       </c>
       <c r="B230" s="3" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
     </row>
     <row r="231" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -10271,7 +10271,7 @@
         <v>573</v>
       </c>
       <c r="B231" s="3" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
     </row>
     <row r="232" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10279,7 +10279,7 @@
         <v>574</v>
       </c>
       <c r="B232" s="3" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
     </row>
     <row r="233" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10287,7 +10287,7 @@
         <v>119</v>
       </c>
       <c r="B233" s="3" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
     </row>
     <row r="234" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10295,7 +10295,7 @@
         <v>566</v>
       </c>
       <c r="B234" s="3" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
     </row>
     <row r="235" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10303,7 +10303,7 @@
         <v>565</v>
       </c>
       <c r="B235" s="3" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
     </row>
     <row r="236" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10311,7 +10311,7 @@
         <v>120</v>
       </c>
       <c r="B236" s="3" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
     </row>
     <row r="237" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -10319,7 +10319,7 @@
         <v>172</v>
       </c>
       <c r="B237" s="3" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="238" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10327,7 +10327,7 @@
         <v>173</v>
       </c>
       <c r="B238" s="3" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
     </row>
     <row r="239" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10335,7 +10335,7 @@
         <v>174</v>
       </c>
       <c r="B239" s="3" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
     </row>
     <row r="240" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -10343,7 +10343,7 @@
         <v>121</v>
       </c>
       <c r="B240" s="3" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
     </row>
     <row r="241" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10351,7 +10351,7 @@
         <v>122</v>
       </c>
       <c r="B241" s="3" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
     </row>
     <row r="242" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10359,7 +10359,7 @@
         <v>521</v>
       </c>
       <c r="B242" s="3" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
     </row>
     <row r="243" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -10367,7 +10367,7 @@
         <v>123</v>
       </c>
       <c r="B243" s="3" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
     </row>
     <row r="244" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10375,7 +10375,7 @@
         <v>571</v>
       </c>
       <c r="B244" s="3" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
     </row>
     <row r="245" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10383,7 +10383,7 @@
         <v>572</v>
       </c>
       <c r="B245" s="3" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
     </row>
     <row r="246" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10391,7 +10391,7 @@
         <v>124</v>
       </c>
       <c r="B246" s="3" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
     </row>
     <row r="247" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10399,7 +10399,7 @@
         <v>617</v>
       </c>
       <c r="B247" s="3" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
     </row>
     <row r="248" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10407,7 +10407,7 @@
         <v>125</v>
       </c>
       <c r="B248" s="3" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
     </row>
     <row r="249" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -10415,7 +10415,7 @@
         <v>589</v>
       </c>
       <c r="B249" s="3" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
     </row>
     <row r="250" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10423,7 +10423,7 @@
         <v>126</v>
       </c>
       <c r="B250" s="3" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
     </row>
     <row r="251" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -10431,7 +10431,7 @@
         <v>127</v>
       </c>
       <c r="B251" s="3" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
     </row>
     <row r="252" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10439,7 +10439,7 @@
         <v>128</v>
       </c>
       <c r="B252" s="3" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
     </row>
     <row r="253" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -10447,7 +10447,7 @@
         <v>129</v>
       </c>
       <c r="B253" s="3" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
     </row>
     <row r="254" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10455,7 +10455,7 @@
         <v>130</v>
       </c>
       <c r="B254" s="3" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
     </row>
     <row r="255" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -10463,7 +10463,7 @@
         <v>131</v>
       </c>
       <c r="B255" s="3" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
     </row>
     <row r="256" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -10471,7 +10471,7 @@
         <v>576</v>
       </c>
       <c r="B256" s="3" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
     </row>
     <row r="257" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10479,7 +10479,7 @@
         <v>577</v>
       </c>
       <c r="B257" s="3" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
     </row>
     <row r="258" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -10487,7 +10487,7 @@
         <v>132</v>
       </c>
       <c r="B258" s="3" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="259" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10495,7 +10495,7 @@
         <v>133</v>
       </c>
       <c r="B259" s="3" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
     </row>
     <row r="260" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10503,7 +10503,7 @@
         <v>575</v>
       </c>
       <c r="B260" s="3" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="261" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -10511,7 +10511,7 @@
         <v>134</v>
       </c>
       <c r="B261" s="3" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="262" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10519,7 +10519,7 @@
         <v>590</v>
       </c>
       <c r="B262" s="3" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
     </row>
     <row r="263" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10527,7 +10527,7 @@
         <v>591</v>
       </c>
       <c r="B263" s="3" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="264" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -10535,7 +10535,7 @@
         <v>135</v>
       </c>
       <c r="B264" s="3" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
     </row>
     <row r="265" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -10543,7 +10543,7 @@
         <v>592</v>
       </c>
       <c r="B265" s="3" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
     </row>
     <row r="266" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10551,7 +10551,7 @@
         <v>136</v>
       </c>
       <c r="B266" s="3" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
     </row>
     <row r="267" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -10559,7 +10559,7 @@
         <v>137</v>
       </c>
       <c r="B267" s="3" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
     </row>
     <row r="268" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10567,7 +10567,7 @@
         <v>232</v>
       </c>
       <c r="B268" s="3" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
     </row>
     <row r="269" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10575,7 +10575,7 @@
         <v>233</v>
       </c>
       <c r="B269" s="3" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
     </row>
     <row r="270" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -10591,7 +10591,7 @@
         <v>234</v>
       </c>
       <c r="B271" s="3" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
     </row>
     <row r="272" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10599,7 +10599,7 @@
         <v>235</v>
       </c>
       <c r="B272" s="3" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
     </row>
     <row r="273" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -10615,7 +10615,7 @@
         <v>239</v>
       </c>
       <c r="B274" s="3" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
     </row>
     <row r="275" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10623,7 +10623,7 @@
         <v>240</v>
       </c>
       <c r="B275" s="3" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="276" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10631,7 +10631,7 @@
         <v>241</v>
       </c>
       <c r="B276" s="3" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
     </row>
     <row r="277" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10647,7 +10647,7 @@
         <v>236</v>
       </c>
       <c r="B278" s="3" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
     </row>
     <row r="279" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10655,7 +10655,7 @@
         <v>237</v>
       </c>
       <c r="B279" s="3" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
     </row>
     <row r="280" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10663,7 +10663,7 @@
         <v>238</v>
       </c>
       <c r="B280" s="3" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
     </row>
     <row r="281" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10671,7 +10671,7 @@
         <v>141</v>
       </c>
       <c r="B281" s="3" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
     </row>
     <row r="282" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10679,7 +10679,7 @@
         <v>142</v>
       </c>
       <c r="B282" s="3" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="283" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10687,7 +10687,7 @@
         <v>143</v>
       </c>
       <c r="B283" s="3" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="284" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -10695,7 +10695,7 @@
         <v>144</v>
       </c>
       <c r="B284" s="3" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
     </row>
     <row r="285" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10703,7 +10703,7 @@
         <v>242</v>
       </c>
       <c r="B285" s="3" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
     </row>
     <row r="286" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10711,7 +10711,7 @@
         <v>145</v>
       </c>
       <c r="B286" s="3" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
     </row>
     <row r="287" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10719,7 +10719,7 @@
         <v>146</v>
       </c>
       <c r="B287" s="3" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="288" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10727,7 +10727,7 @@
         <v>147</v>
       </c>
       <c r="B288" s="3" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
     </row>
     <row r="289" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10735,7 +10735,7 @@
         <v>148</v>
       </c>
       <c r="B289" s="3" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
     </row>
     <row r="290" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10743,7 +10743,7 @@
         <v>149</v>
       </c>
       <c r="B290" s="3" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
     </row>
     <row r="291" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10751,7 +10751,7 @@
         <v>605</v>
       </c>
       <c r="B291" s="3" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
     </row>
     <row r="292" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10759,7 +10759,7 @@
         <v>604</v>
       </c>
       <c r="B292" s="3" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
     </row>
     <row r="293" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10767,7 +10767,7 @@
         <v>606</v>
       </c>
       <c r="B293" s="3" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="294" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10775,7 +10775,7 @@
         <v>150</v>
       </c>
       <c r="B294" s="3" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
     </row>
     <row r="295" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10783,7 +10783,7 @@
         <v>607</v>
       </c>
       <c r="B295" s="3" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
     </row>
     <row r="296" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -10791,7 +10791,7 @@
         <v>151</v>
       </c>
       <c r="B296" s="3" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
     </row>
     <row r="297" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10799,7 +10799,7 @@
         <v>243</v>
       </c>
       <c r="B297" s="3" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
     </row>
     <row r="298" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10807,7 +10807,7 @@
         <v>244</v>
       </c>
       <c r="B298" s="3" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
     </row>
     <row r="299" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10815,7 +10815,7 @@
         <v>245</v>
       </c>
       <c r="B299" s="3" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
     </row>
     <row r="300" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10823,7 +10823,7 @@
         <v>152</v>
       </c>
       <c r="B300" s="3" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
     </row>
     <row r="301" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10831,7 +10831,7 @@
         <v>153</v>
       </c>
       <c r="B301" s="3" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
     </row>
     <row r="302" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10839,7 +10839,7 @@
         <v>154</v>
       </c>
       <c r="B302" s="3" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
     </row>
     <row r="303" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -10847,7 +10847,7 @@
         <v>155</v>
       </c>
       <c r="B303" s="3" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
     </row>
     <row r="304" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10855,7 +10855,7 @@
         <v>156</v>
       </c>
       <c r="B304" s="3" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
     </row>
     <row r="305" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10871,7 +10871,7 @@
         <v>246</v>
       </c>
       <c r="B306" s="3" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
     </row>
     <row r="307" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10879,7 +10879,7 @@
         <v>247</v>
       </c>
       <c r="B307" s="3" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
     </row>
     <row r="308" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10887,7 +10887,7 @@
         <v>248</v>
       </c>
       <c r="B308" s="3" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
     </row>
     <row r="309" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10903,7 +10903,7 @@
         <v>159</v>
       </c>
       <c r="B310" s="3" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
     </row>
     <row r="311" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10911,7 +10911,7 @@
         <v>160</v>
       </c>
       <c r="B311" s="3" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
     </row>
     <row r="312" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -10919,7 +10919,7 @@
         <v>161</v>
       </c>
       <c r="B312" s="3" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
     </row>
     <row r="313" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -10927,7 +10927,7 @@
         <v>162</v>
       </c>
       <c r="B313" s="3" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
     </row>
     <row r="314" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -10935,7 +10935,7 @@
         <v>599</v>
       </c>
       <c r="B314" s="3" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
     </row>
     <row r="315" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10943,7 +10943,7 @@
         <v>600</v>
       </c>
       <c r="B315" s="3" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
     </row>
     <row r="316" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10951,7 +10951,7 @@
         <v>601</v>
       </c>
       <c r="B316" s="3" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
     </row>
     <row r="317" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10959,7 +10959,7 @@
         <v>163</v>
       </c>
       <c r="B317" s="3" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
     </row>
     <row r="318" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10967,7 +10967,7 @@
         <v>164</v>
       </c>
       <c r="B318" s="3" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
     </row>
     <row r="319" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10975,7 +10975,7 @@
         <v>175</v>
       </c>
       <c r="B319" s="3" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
     </row>
     <row r="320" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -10983,7 +10983,7 @@
         <v>176</v>
       </c>
       <c r="B320" s="3" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
     </row>
     <row r="321" spans="1:2" ht="390" x14ac:dyDescent="0.25">
@@ -10991,7 +10991,7 @@
         <v>177</v>
       </c>
       <c r="B321" s="3" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
     </row>
     <row r="322" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -11007,7 +11007,7 @@
         <v>414</v>
       </c>
       <c r="B323" s="3" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
     </row>
     <row r="324" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11015,7 +11015,7 @@
         <v>415</v>
       </c>
       <c r="B324" s="3" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
     </row>
     <row r="325" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -11023,7 +11023,7 @@
         <v>416</v>
       </c>
       <c r="B325" s="3" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
     </row>
     <row r="326" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -11031,7 +11031,7 @@
         <v>417</v>
       </c>
       <c r="B326" s="3" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
     </row>
     <row r="327" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11039,7 +11039,7 @@
         <v>418</v>
       </c>
       <c r="B327" s="3" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
     </row>
     <row r="328" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11047,7 +11047,7 @@
         <v>613</v>
       </c>
       <c r="B328" s="3" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
     </row>
     <row r="329" spans="1:2" ht="390" x14ac:dyDescent="0.25">
@@ -11055,7 +11055,7 @@
         <v>178</v>
       </c>
       <c r="B329" s="3" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
     </row>
     <row r="330" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -11071,7 +11071,7 @@
         <v>426</v>
       </c>
       <c r="B331" s="3" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
     </row>
     <row r="332" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11079,7 +11079,7 @@
         <v>427</v>
       </c>
       <c r="B332" s="3" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
     </row>
     <row r="333" spans="1:2" ht="315" x14ac:dyDescent="0.25">
@@ -11087,7 +11087,7 @@
         <v>179</v>
       </c>
       <c r="B333" s="3" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
     </row>
     <row r="334" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -11095,7 +11095,7 @@
         <v>249</v>
       </c>
       <c r="B334" s="3" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
     </row>
     <row r="335" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -11103,7 +11103,7 @@
         <v>250</v>
       </c>
       <c r="B335" s="3" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
     </row>
     <row r="336" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -11111,7 +11111,7 @@
         <v>251</v>
       </c>
       <c r="B336" s="3" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
     </row>
     <row r="337" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11119,7 +11119,7 @@
         <v>252</v>
       </c>
       <c r="B337" s="3" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
     </row>
     <row r="338" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -11127,7 +11127,7 @@
         <v>253</v>
       </c>
       <c r="B338" s="3" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
     </row>
     <row r="339" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -11135,7 +11135,7 @@
         <v>545</v>
       </c>
       <c r="B339" s="3" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
     </row>
     <row r="340" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -11143,7 +11143,7 @@
         <v>546</v>
       </c>
       <c r="B340" s="3" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
     </row>
     <row r="341" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11151,7 +11151,7 @@
         <v>180</v>
       </c>
       <c r="B341" s="3" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="342" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11159,7 +11159,7 @@
         <v>181</v>
       </c>
       <c r="B342" s="3" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
     </row>
     <row r="343" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11167,7 +11167,7 @@
         <v>386</v>
       </c>
       <c r="B343" s="3" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
     </row>
     <row r="344" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -11183,7 +11183,7 @@
         <v>622</v>
       </c>
       <c r="B345" s="3" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
     </row>
     <row r="346" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11191,7 +11191,7 @@
         <v>183</v>
       </c>
       <c r="B346" s="3" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
     </row>
     <row r="347" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -11199,7 +11199,7 @@
         <v>184</v>
       </c>
       <c r="B347" s="3" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
     </row>
     <row r="348" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -11215,7 +11215,7 @@
         <v>185</v>
       </c>
       <c r="B349" s="3" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
     </row>
     <row r="350" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -11223,7 +11223,7 @@
         <v>186</v>
       </c>
       <c r="B350" s="3" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
     </row>
     <row r="351" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -11231,7 +11231,7 @@
         <v>187</v>
       </c>
       <c r="B351" s="3" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
     </row>
     <row r="352" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11247,7 +11247,7 @@
         <v>188</v>
       </c>
       <c r="B353" s="3" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
     </row>
     <row r="354" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -11255,7 +11255,7 @@
         <v>189</v>
       </c>
       <c r="B354" s="3" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
     </row>
     <row r="355" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -11263,7 +11263,7 @@
         <v>383</v>
       </c>
       <c r="B355" s="3" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
     </row>
     <row r="356" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -11271,7 +11271,7 @@
         <v>384</v>
       </c>
       <c r="B356" s="3" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
     </row>
     <row r="357" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -11279,7 +11279,7 @@
         <v>190</v>
       </c>
       <c r="B357" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="358" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -11287,7 +11287,7 @@
         <v>191</v>
       </c>
       <c r="B358" s="3" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
     </row>
     <row r="359" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -11295,7 +11295,7 @@
         <v>192</v>
       </c>
       <c r="B359" s="3" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
     </row>
     <row r="360" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -11303,7 +11303,7 @@
         <v>465</v>
       </c>
       <c r="B360" s="3" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
     </row>
     <row r="361" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -11311,7 +11311,7 @@
         <v>193</v>
       </c>
       <c r="B361" s="3" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
     </row>
     <row r="362" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -11327,7 +11327,7 @@
         <v>333</v>
       </c>
       <c r="B363" s="3" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="364" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -11335,7 +11335,7 @@
         <v>624</v>
       </c>
       <c r="B364" s="3" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
     </row>
     <row r="365" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -11343,7 +11343,7 @@
         <v>625</v>
       </c>
       <c r="B365" s="3" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="366" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11351,7 +11351,7 @@
         <v>627</v>
       </c>
       <c r="B366" s="3" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
     </row>
     <row r="367" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11359,7 +11359,7 @@
         <v>628</v>
       </c>
       <c r="B367" s="3" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
     </row>
     <row r="368" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11367,7 +11367,7 @@
         <v>629</v>
       </c>
       <c r="B368" s="3" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
     </row>
     <row r="369" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11375,7 +11375,7 @@
         <v>630</v>
       </c>
       <c r="B369" s="3" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
     </row>
     <row r="370" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11383,7 +11383,7 @@
         <v>631</v>
       </c>
       <c r="B370" s="3" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
     </row>
     <row r="371" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11391,7 +11391,7 @@
         <v>632</v>
       </c>
       <c r="B371" s="3" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
     </row>
     <row r="372" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -11399,7 +11399,7 @@
         <v>194</v>
       </c>
       <c r="B372" s="3" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
     </row>
     <row r="373" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -11407,7 +11407,7 @@
         <v>195</v>
       </c>
       <c r="B373" s="3" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
     </row>
     <row r="374" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -11415,7 +11415,7 @@
         <v>620</v>
       </c>
       <c r="B374" s="3" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
     </row>
     <row r="375" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -11423,7 +11423,7 @@
         <v>196</v>
       </c>
       <c r="B375" s="3" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
     </row>
     <row r="376" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -11431,7 +11431,7 @@
         <v>328</v>
       </c>
       <c r="B376" s="3" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="377" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -11439,7 +11439,7 @@
         <v>197</v>
       </c>
       <c r="B377" s="3" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
     </row>
     <row r="378" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11447,7 +11447,7 @@
         <v>487</v>
       </c>
       <c r="B378" s="3" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
     </row>
     <row r="379" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11455,7 +11455,7 @@
         <v>198</v>
       </c>
       <c r="B379" s="3" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
     </row>
     <row r="380" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11463,7 +11463,7 @@
         <v>199</v>
       </c>
       <c r="B380" s="3" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
     </row>
     <row r="381" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -11471,7 +11471,7 @@
         <v>200</v>
       </c>
       <c r="B381" s="3" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
     </row>
     <row r="382" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11479,7 +11479,7 @@
         <v>201</v>
       </c>
       <c r="B382" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="383" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11487,7 +11487,7 @@
         <v>202</v>
       </c>
       <c r="B383" s="3" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
     </row>
     <row r="384" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -11495,7 +11495,7 @@
         <v>203</v>
       </c>
       <c r="B384" s="3" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
     </row>
     <row r="385" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -11543,7 +11543,7 @@
         <v>204</v>
       </c>
       <c r="B390" s="3" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
     </row>
     <row r="391" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11551,7 +11551,7 @@
         <v>459</v>
       </c>
       <c r="B391" s="3" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="392" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11559,7 +11559,7 @@
         <v>460</v>
       </c>
       <c r="B392" s="3" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="393" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11567,7 +11567,7 @@
         <v>461</v>
       </c>
       <c r="B393" s="3" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="394" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11575,7 +11575,7 @@
         <v>462</v>
       </c>
       <c r="B394" s="3" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="395" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11583,7 +11583,7 @@
         <v>463</v>
       </c>
       <c r="B395" s="3" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="396" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11591,7 +11591,7 @@
         <v>464</v>
       </c>
       <c r="B396" s="3" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="397" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -11599,7 +11599,7 @@
         <v>205</v>
       </c>
       <c r="B397" s="3" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="398" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -11671,7 +11671,7 @@
         <v>207</v>
       </c>
       <c r="B406" s="3" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="407" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -11679,7 +11679,7 @@
         <v>208</v>
       </c>
       <c r="B407" s="3" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="408" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -11687,7 +11687,7 @@
         <v>209</v>
       </c>
       <c r="B408" s="3" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="409" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11695,7 +11695,7 @@
         <v>476</v>
       </c>
       <c r="B409" s="3" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="410" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11703,7 +11703,7 @@
         <v>477</v>
       </c>
       <c r="B410" s="3" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="411" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11711,7 +11711,7 @@
         <v>478</v>
       </c>
       <c r="B411" s="3" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="412" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -11719,7 +11719,7 @@
         <v>479</v>
       </c>
       <c r="B412" s="3" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="413" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -11727,7 +11727,7 @@
         <v>480</v>
       </c>
       <c r="B413" s="4" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="414" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -11735,7 +11735,7 @@
         <v>481</v>
       </c>
       <c r="B414" s="3" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="415" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -11743,7 +11743,7 @@
         <v>621</v>
       </c>
       <c r="B415" s="3" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="416" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -11751,7 +11751,7 @@
         <v>210</v>
       </c>
       <c r="B416" s="3" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="417" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11759,7 +11759,7 @@
         <v>469</v>
       </c>
       <c r="B417" s="3" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="418" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11767,7 +11767,7 @@
         <v>470</v>
       </c>
       <c r="B418" s="3" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="419" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11775,7 +11775,7 @@
         <v>471</v>
       </c>
       <c r="B419" s="3" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="420" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11783,7 +11783,7 @@
         <v>472</v>
       </c>
       <c r="B420" s="3" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="421" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11791,7 +11791,7 @@
         <v>473</v>
       </c>
       <c r="B421" s="3" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="422" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11799,7 +11799,7 @@
         <v>474</v>
       </c>
       <c r="B422" s="3" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="423" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11807,7 +11807,7 @@
         <v>475</v>
       </c>
       <c r="B423" s="3" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="424" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11815,7 +11815,7 @@
         <v>619</v>
       </c>
       <c r="B424" s="3" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="425" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -11823,7 +11823,7 @@
         <v>211</v>
       </c>
       <c r="B425" s="3" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="426" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11831,7 +11831,7 @@
         <v>212</v>
       </c>
       <c r="B426" s="3" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="427" spans="1:2" ht="300" x14ac:dyDescent="0.25">
@@ -11839,7 +11839,7 @@
         <v>419</v>
       </c>
       <c r="B427" s="3" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="428" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11847,7 +11847,7 @@
         <v>420</v>
       </c>
       <c r="B428" s="3" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="429" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -11855,7 +11855,7 @@
         <v>421</v>
       </c>
       <c r="B429" s="3" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="430" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11863,7 +11863,7 @@
         <v>422</v>
       </c>
       <c r="B430" s="3" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="431" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -11871,7 +11871,7 @@
         <v>213</v>
       </c>
       <c r="B431" s="3" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="432" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -11879,7 +11879,7 @@
         <v>214</v>
       </c>
       <c r="B432" s="3" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="433" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -11887,7 +11887,7 @@
         <v>215</v>
       </c>
       <c r="B433" s="3" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="434" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11895,7 +11895,7 @@
         <v>216</v>
       </c>
       <c r="B434" s="3" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="435" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11903,7 +11903,7 @@
         <v>217</v>
       </c>
       <c r="B435" s="3" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="436" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11911,7 +11911,7 @@
         <v>218</v>
       </c>
       <c r="B436" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="437" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11919,7 +11919,7 @@
         <v>219</v>
       </c>
       <c r="B437" s="3" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="438" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11927,7 +11927,7 @@
         <v>220</v>
       </c>
       <c r="B438" s="3" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="439" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11935,7 +11935,7 @@
         <v>221</v>
       </c>
       <c r="B439" s="3" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="440" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11943,7 +11943,7 @@
         <v>222</v>
       </c>
       <c r="B440" s="3" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="441" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11951,7 +11951,7 @@
         <v>223</v>
       </c>
       <c r="B441" s="3" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="442" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -11959,7 +11959,7 @@
         <v>224</v>
       </c>
       <c r="B442" s="3" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="443" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -11967,7 +11967,7 @@
         <v>329</v>
       </c>
       <c r="B443" s="3" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="444" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11975,7 +11975,7 @@
         <v>385</v>
       </c>
       <c r="B444" s="3" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="445" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11983,7 +11983,7 @@
         <v>225</v>
       </c>
       <c r="B445" s="3" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="446" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -11991,7 +11991,7 @@
         <v>226</v>
       </c>
       <c r="B446" s="3" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="447" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -11999,7 +11999,7 @@
         <v>227</v>
       </c>
       <c r="B447" s="3" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="448" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -12007,7 +12007,7 @@
         <v>228</v>
       </c>
       <c r="B448" s="3" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="449" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -12015,7 +12015,7 @@
         <v>618</v>
       </c>
       <c r="B449" s="3" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="450" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12023,7 +12023,7 @@
         <v>229</v>
       </c>
       <c r="B450" s="3" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="451" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -12031,7 +12031,7 @@
         <v>230</v>
       </c>
       <c r="B451" s="3" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="452" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -12039,7 +12039,7 @@
         <v>231</v>
       </c>
       <c r="B452" s="3" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="453" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12047,7 +12047,7 @@
         <v>257</v>
       </c>
       <c r="B453" s="3" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="454" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -12055,7 +12055,7 @@
         <v>379</v>
       </c>
       <c r="B454" s="3" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="455" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12063,7 +12063,7 @@
         <v>380</v>
       </c>
       <c r="B455" s="3" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="456" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12071,7 +12071,7 @@
         <v>444</v>
       </c>
       <c r="B456" s="3" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="457" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12087,15 +12087,15 @@
         <v>531</v>
       </c>
       <c r="B458" s="3" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="459" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A459" s="2" t="s">
+        <v>1161</v>
+      </c>
+      <c r="B459" s="3" t="s">
         <v>1162</v>
-      </c>
-      <c r="B459" s="3" t="s">
-        <v>1163</v>
       </c>
     </row>
     <row r="460" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -12135,7 +12135,7 @@
         <v>602</v>
       </c>
       <c r="B464" s="3" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="465" spans="1:2" ht="255" x14ac:dyDescent="0.25">
@@ -12143,7 +12143,7 @@
         <v>322</v>
       </c>
       <c r="B465" s="3" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="466" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12151,7 +12151,7 @@
         <v>395</v>
       </c>
       <c r="B466" s="3" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="467" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -12159,7 +12159,7 @@
         <v>394</v>
       </c>
       <c r="B467" s="3" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="468" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12167,7 +12167,7 @@
         <v>396</v>
       </c>
       <c r="B468" s="3" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="469" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12175,7 +12175,7 @@
         <v>397</v>
       </c>
       <c r="B469" s="3" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="470" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12183,7 +12183,7 @@
         <v>398</v>
       </c>
       <c r="B470" s="3" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="471" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12191,7 +12191,7 @@
         <v>399</v>
       </c>
       <c r="B471" s="3" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="472" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12199,7 +12199,7 @@
         <v>400</v>
       </c>
       <c r="B472" s="3" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="473" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12207,7 +12207,7 @@
         <v>431</v>
       </c>
       <c r="B473" s="3" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="474" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -12215,7 +12215,7 @@
         <v>432</v>
       </c>
       <c r="B474" s="3" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="475" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -12223,7 +12223,7 @@
         <v>433</v>
       </c>
       <c r="B475" s="3" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="476" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12231,7 +12231,7 @@
         <v>434</v>
       </c>
       <c r="B476" s="3" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="477" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12239,7 +12239,7 @@
         <v>435</v>
       </c>
       <c r="B477" s="3" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="478" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12247,7 +12247,7 @@
         <v>436</v>
       </c>
       <c r="B478" s="3" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="479" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -12255,7 +12255,7 @@
         <v>437</v>
       </c>
       <c r="B479" s="3" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="480" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12263,7 +12263,7 @@
         <v>438</v>
       </c>
       <c r="B480" s="3" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="481" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12271,7 +12271,7 @@
         <v>439</v>
       </c>
       <c r="B481" s="3" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="482" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -12279,7 +12279,7 @@
         <v>440</v>
       </c>
       <c r="B482" s="3" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="483" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12287,7 +12287,7 @@
         <v>441</v>
       </c>
       <c r="B483" s="3" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="484" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -12295,7 +12295,7 @@
         <v>442</v>
       </c>
       <c r="B484" s="3" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="485" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -12303,7 +12303,7 @@
         <v>443</v>
       </c>
       <c r="B485" s="3" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="486" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -12311,7 +12311,7 @@
         <v>458</v>
       </c>
       <c r="B486" s="3" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="487" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -12319,7 +12319,7 @@
         <v>466</v>
       </c>
       <c r="B487" s="3" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="488" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -12327,7 +12327,7 @@
         <v>467</v>
       </c>
       <c r="B488" s="3" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="489" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -12335,7 +12335,7 @@
         <v>468</v>
       </c>
       <c r="B489" s="3" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="490" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -12343,7 +12343,7 @@
         <v>552</v>
       </c>
       <c r="B490" s="3" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="491" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -12351,7 +12351,7 @@
         <v>633</v>
       </c>
       <c r="B491" s="3" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="492" spans="1:2" ht="255" x14ac:dyDescent="0.25">
@@ -12359,7 +12359,7 @@
         <v>488</v>
       </c>
       <c r="B492" s="1" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="493" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12367,7 +12367,7 @@
         <v>489</v>
       </c>
       <c r="B493" s="1" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="494" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12375,7 +12375,7 @@
         <v>490</v>
       </c>
       <c r="B494" s="1" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="495" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12383,7 +12383,7 @@
         <v>491</v>
       </c>
       <c r="B495" s="1" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="496" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12391,7 +12391,7 @@
         <v>492</v>
       </c>
       <c r="B496" s="1" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="497" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12399,7 +12399,7 @@
         <v>493</v>
       </c>
       <c r="B497" s="1" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="498" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12407,7 +12407,7 @@
         <v>494</v>
       </c>
       <c r="B498" s="1" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="499" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12415,7 +12415,7 @@
         <v>495</v>
       </c>
       <c r="B499" s="1" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="500" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12423,7 +12423,7 @@
         <v>496</v>
       </c>
       <c r="B500" s="1" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="501" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -12431,7 +12431,7 @@
         <v>497</v>
       </c>
       <c r="B501" s="1" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="502" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12439,7 +12439,7 @@
         <v>498</v>
       </c>
       <c r="B502" s="1" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="503" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12447,7 +12447,7 @@
         <v>499</v>
       </c>
       <c r="B503" s="1" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="504" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -12455,7 +12455,7 @@
         <v>500</v>
       </c>
       <c r="B504" s="1" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="505" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12463,7 +12463,7 @@
         <v>501</v>
       </c>
       <c r="B505" s="1" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="506" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12471,7 +12471,7 @@
         <v>502</v>
       </c>
       <c r="B506" s="1" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="507" spans="1:2" ht="255" x14ac:dyDescent="0.25">
@@ -12479,7 +12479,7 @@
         <v>597</v>
       </c>
       <c r="B507" s="1" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="508" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12487,7 +12487,7 @@
         <v>598</v>
       </c>
       <c r="B508" s="1" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="509" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12495,7 +12495,7 @@
         <v>503</v>
       </c>
       <c r="B509" s="1" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="510" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12503,7 +12503,7 @@
         <v>515</v>
       </c>
       <c r="B510" s="3" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="511" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -12511,7 +12511,7 @@
         <v>423</v>
       </c>
       <c r="B511" s="3" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="512" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12535,7 +12535,7 @@
         <v>267</v>
       </c>
       <c r="B514" s="1" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="515" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12543,7 +12543,7 @@
         <v>268</v>
       </c>
       <c r="B515" s="1" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="516" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12551,7 +12551,7 @@
         <v>269</v>
       </c>
       <c r="B516" s="1" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="517" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12559,7 +12559,7 @@
         <v>270</v>
       </c>
       <c r="B517" s="1" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="518" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12567,7 +12567,7 @@
         <v>271</v>
       </c>
       <c r="B518" s="1" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="519" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12575,7 +12575,7 @@
         <v>272</v>
       </c>
       <c r="B519" s="1" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="520" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12583,7 +12583,7 @@
         <v>273</v>
       </c>
       <c r="B520" s="1" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="521" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12591,7 +12591,7 @@
         <v>274</v>
       </c>
       <c r="B521" s="1" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="522" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12599,7 +12599,7 @@
         <v>275</v>
       </c>
       <c r="B522" s="1" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="523" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12607,7 +12607,7 @@
         <v>276</v>
       </c>
       <c r="B523" s="1" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="524" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12615,7 +12615,7 @@
         <v>277</v>
       </c>
       <c r="B524" s="1" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="525" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12695,7 +12695,7 @@
         <v>280</v>
       </c>
       <c r="B534" s="1" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="535" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12703,7 +12703,7 @@
         <v>281</v>
       </c>
       <c r="B535" s="1" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="536" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12719,7 +12719,7 @@
         <v>283</v>
       </c>
       <c r="B537" s="1" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="538" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12727,7 +12727,7 @@
         <v>284</v>
       </c>
       <c r="B538" s="1" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="539" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12735,7 +12735,7 @@
         <v>285</v>
       </c>
       <c r="B539" s="1" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="540" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12743,7 +12743,7 @@
         <v>286</v>
       </c>
       <c r="B540" s="1" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="541" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12791,7 +12791,7 @@
         <v>292</v>
       </c>
       <c r="B546" s="1" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="547" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12799,7 +12799,7 @@
         <v>293</v>
       </c>
       <c r="B547" s="1" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="548" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12807,7 +12807,7 @@
         <v>294</v>
       </c>
       <c r="B548" s="1" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="549" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12815,7 +12815,7 @@
         <v>295</v>
       </c>
       <c r="B549" s="1" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="550" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -12823,7 +12823,7 @@
         <v>296</v>
       </c>
       <c r="B550" s="1" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="551" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12831,7 +12831,7 @@
         <v>297</v>
       </c>
       <c r="B551" s="1" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="552" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -12839,7 +12839,7 @@
         <v>353</v>
       </c>
       <c r="B552" s="1" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="553" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12847,7 +12847,7 @@
         <v>365</v>
       </c>
       <c r="B553" s="3" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="554" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12855,7 +12855,7 @@
         <v>366</v>
       </c>
       <c r="B554" s="1" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="555" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12863,7 +12863,7 @@
         <v>298</v>
       </c>
       <c r="B555" s="1" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="556" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -12871,7 +12871,7 @@
         <v>364</v>
       </c>
       <c r="B556" s="1" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="557" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12879,7 +12879,7 @@
         <v>299</v>
       </c>
       <c r="B557" s="1" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="558" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -12887,7 +12887,7 @@
         <v>354</v>
       </c>
       <c r="B558" s="1" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
     </row>
     <row r="559" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -12903,7 +12903,7 @@
         <v>300</v>
       </c>
       <c r="B560" s="1" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
     </row>
     <row r="561" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12911,7 +12911,7 @@
         <v>301</v>
       </c>
       <c r="B561" s="1" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="562" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12919,7 +12919,7 @@
         <v>302</v>
       </c>
       <c r="B562" s="1" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="563" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12927,7 +12927,7 @@
         <v>303</v>
       </c>
       <c r="B563" s="1" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="564" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -12935,7 +12935,7 @@
         <v>363</v>
       </c>
       <c r="B564" s="1" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="565" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12943,7 +12943,7 @@
         <v>304</v>
       </c>
       <c r="B565" s="1" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="566" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12951,7 +12951,7 @@
         <v>361</v>
       </c>
       <c r="B566" s="1" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="567" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -12967,7 +12967,7 @@
         <v>517</v>
       </c>
       <c r="B568" s="1" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="569" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12975,7 +12975,7 @@
         <v>305</v>
       </c>
       <c r="B569" s="1" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="570" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12983,7 +12983,7 @@
         <v>358</v>
       </c>
       <c r="B570" s="1" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="571" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12991,7 +12991,7 @@
         <v>359</v>
       </c>
       <c r="B571" s="1" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="572" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -13007,7 +13007,7 @@
         <v>518</v>
       </c>
       <c r="B573" s="1" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="574" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -13015,7 +13015,7 @@
         <v>306</v>
       </c>
       <c r="B574" s="1" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="575" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -13023,7 +13023,7 @@
         <v>352</v>
       </c>
       <c r="B575" s="1" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="576" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -13031,7 +13031,7 @@
         <v>355</v>
       </c>
       <c r="B576" s="3" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="577" spans="1:2" ht="405" x14ac:dyDescent="0.25">
@@ -13039,7 +13039,7 @@
         <v>307</v>
       </c>
       <c r="B577" s="1" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="578" spans="1:2" ht="375" x14ac:dyDescent="0.25">
@@ -13047,7 +13047,7 @@
         <v>311</v>
       </c>
       <c r="B578" s="1" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="579" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -13071,7 +13071,7 @@
         <v>349</v>
       </c>
       <c r="B581" s="3" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="582" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -13079,7 +13079,7 @@
         <v>519</v>
       </c>
       <c r="B582" s="3" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="583" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -13087,7 +13087,7 @@
         <v>326</v>
       </c>
       <c r="B583" s="3" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change Elven Fortress to be audience as in town
</commit_message>
<xml_diff>
--- a/Documentation/Events.xlsx
+++ b/Documentation/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\happysulla\BarbarianPrince\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CC540120-483B-4B15-85E7-6947EE8C4525}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{DF19B41A-16B2-454F-8E6D-F48C4E98670C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -4719,19 +4719,6 @@
      &lt;InlineUIContainer&gt;&lt;Image Source='../bin/Images/Elves.gif' Height='250' Width='550'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e072a Follow an Elven Band&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt; Roll one die and add one for the number of elves in the band. Die Roll=
-&lt;InlineUIContainer&gt;&lt;Image Source='../bin/Images/dieRoll.gif' Name='DieRoll' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;Each elf has combat skill 5, endurance 4, and wealth 7. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;After making a follow move
- &lt;InlineUIContainer&gt;&lt;Button Content='e071' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
-, roll one die to see where you end the day: &lt;InlineUIContainer&gt;&lt;Image Source='../bin/Images/dieRoll.gif' Name='DieRoll1' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
- &lt;InlineUIContainer&gt;&lt;Button Content='e165' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  1 - Eleven Town&lt;LineBreak/&gt;
- &lt;InlineUIContainer&gt;&lt;Button Content='e166' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  2 - Elven Castle&lt;LineBreak/&gt;
- &lt;InlineUIContainer&gt;&lt;Button Content='e053' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  3,4,5,6 - Campsite</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;e072b Campsite Decision&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 You may peacefully share the campsite with the elves eating your own food or hunting where possible
@@ -8028,6 +8015,19 @@
  &lt;InlineUIContainer&gt;&lt;Button Content='e053' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  3,4,5,6 - Campsite&lt;LineBreak/&gt;
 &lt;LineBreak/&gt; &lt;LineBreak/&gt;
                                    &lt;InlineUIContainer&gt;&lt;Image Source='../bin/Images/Elf.gif' Height='300' Width='240'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e072a Follow an Elven Band&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt; Roll one die and add one for the number of elves in the band. Die Roll=
+&lt;InlineUIContainer&gt;&lt;Image Source='../bin/Images/dieRoll.gif' Name='DieRoll' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;Each elf has combat skill 5, endurance 4, and wealth 7. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;After making a follow move
+ &lt;InlineUIContainer&gt;&lt;Button Content='e071' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+, roll one die to see where you end the day: &lt;InlineUIContainer&gt;&lt;Image Source='../bin/Images/dieRoll.gif' Name='DieRoll1' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+ &lt;InlineUIContainer&gt;&lt;Button Content='e165' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  1 - Eleven Town&lt;LineBreak/&gt;
+ &lt;InlineUIContainer&gt;&lt;Button Content='e166' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  2 - Elven Fortress&lt;LineBreak/&gt;
+ &lt;InlineUIContainer&gt;&lt;Button Content='e053' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  3,4,5,6 - Campsite</t>
   </si>
 </sst>
 </file>
@@ -8416,8 +8416,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B583"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A211" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B213" sqref="B213"/>
+    <sheetView tabSelected="1" topLeftCell="A485" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B486" sqref="B486"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9199,7 +9199,7 @@
         <v>61</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -9455,7 +9455,7 @@
         <v>350</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="130" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10103,7 +10103,7 @@
         <v>510</v>
       </c>
       <c r="B210" s="3" t="s">
-        <v>841</v>
+        <v>1165</v>
       </c>
     </row>
     <row r="211" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -10111,7 +10111,7 @@
         <v>511</v>
       </c>
       <c r="B211" s="3" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
     </row>
     <row r="212" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -10127,7 +10127,7 @@
         <v>516</v>
       </c>
       <c r="B213" s="3" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="214" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10135,7 +10135,7 @@
         <v>112</v>
       </c>
       <c r="B214" s="3" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
     </row>
     <row r="215" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10143,7 +10143,7 @@
         <v>169</v>
       </c>
       <c r="B215" s="3" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
     </row>
     <row r="216" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10151,7 +10151,7 @@
         <v>170</v>
       </c>
       <c r="B216" s="3" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="217" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10159,7 +10159,7 @@
         <v>171</v>
       </c>
       <c r="B217" s="3" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
     </row>
     <row r="218" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -10167,7 +10167,7 @@
         <v>113</v>
       </c>
       <c r="B218" s="3" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="219" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -10175,7 +10175,7 @@
         <v>114</v>
       </c>
       <c r="B219" s="3" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
     </row>
     <row r="220" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10183,7 +10183,7 @@
         <v>266</v>
       </c>
       <c r="B220" s="3" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
     </row>
     <row r="221" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -10191,7 +10191,7 @@
         <v>570</v>
       </c>
       <c r="B221" s="3" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="222" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10199,7 +10199,7 @@
         <v>115</v>
       </c>
       <c r="B222" s="3" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="223" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10207,7 +10207,7 @@
         <v>522</v>
       </c>
       <c r="B223" s="3" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
     </row>
     <row r="224" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -10215,7 +10215,7 @@
         <v>116</v>
       </c>
       <c r="B224" s="3" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
     </row>
     <row r="225" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10223,7 +10223,7 @@
         <v>520</v>
       </c>
       <c r="B225" s="3" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
     </row>
     <row r="226" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10231,7 +10231,7 @@
         <v>117</v>
       </c>
       <c r="B226" s="4" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
     </row>
     <row r="227" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10239,7 +10239,7 @@
         <v>523</v>
       </c>
       <c r="B227" s="4" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
     </row>
     <row r="228" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10247,7 +10247,7 @@
         <v>524</v>
       </c>
       <c r="B228" s="4" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
     </row>
     <row r="229" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10255,7 +10255,7 @@
         <v>525</v>
       </c>
       <c r="B229" s="4" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
     </row>
     <row r="230" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10263,7 +10263,7 @@
         <v>118</v>
       </c>
       <c r="B230" s="3" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
     </row>
     <row r="231" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -10271,7 +10271,7 @@
         <v>573</v>
       </c>
       <c r="B231" s="3" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
     </row>
     <row r="232" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10279,7 +10279,7 @@
         <v>574</v>
       </c>
       <c r="B232" s="3" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
     </row>
     <row r="233" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10287,7 +10287,7 @@
         <v>119</v>
       </c>
       <c r="B233" s="3" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
     </row>
     <row r="234" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10295,7 +10295,7 @@
         <v>566</v>
       </c>
       <c r="B234" s="3" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
     </row>
     <row r="235" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10303,7 +10303,7 @@
         <v>565</v>
       </c>
       <c r="B235" s="3" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
     </row>
     <row r="236" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10311,7 +10311,7 @@
         <v>120</v>
       </c>
       <c r="B236" s="3" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
     </row>
     <row r="237" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -10319,7 +10319,7 @@
         <v>172</v>
       </c>
       <c r="B237" s="3" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="238" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10327,7 +10327,7 @@
         <v>173</v>
       </c>
       <c r="B238" s="3" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
     </row>
     <row r="239" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10335,7 +10335,7 @@
         <v>174</v>
       </c>
       <c r="B239" s="3" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
     </row>
     <row r="240" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -10343,7 +10343,7 @@
         <v>121</v>
       </c>
       <c r="B240" s="3" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
     </row>
     <row r="241" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10351,7 +10351,7 @@
         <v>122</v>
       </c>
       <c r="B241" s="3" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
     </row>
     <row r="242" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10359,7 +10359,7 @@
         <v>521</v>
       </c>
       <c r="B242" s="3" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
     </row>
     <row r="243" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -10367,7 +10367,7 @@
         <v>123</v>
       </c>
       <c r="B243" s="3" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
     </row>
     <row r="244" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10375,7 +10375,7 @@
         <v>571</v>
       </c>
       <c r="B244" s="3" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
     </row>
     <row r="245" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10383,7 +10383,7 @@
         <v>572</v>
       </c>
       <c r="B245" s="3" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
     </row>
     <row r="246" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10391,7 +10391,7 @@
         <v>124</v>
       </c>
       <c r="B246" s="3" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
     </row>
     <row r="247" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10399,7 +10399,7 @@
         <v>617</v>
       </c>
       <c r="B247" s="3" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
     </row>
     <row r="248" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10407,7 +10407,7 @@
         <v>125</v>
       </c>
       <c r="B248" s="3" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
     </row>
     <row r="249" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -10415,7 +10415,7 @@
         <v>589</v>
       </c>
       <c r="B249" s="3" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
     </row>
     <row r="250" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10423,7 +10423,7 @@
         <v>126</v>
       </c>
       <c r="B250" s="3" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
     </row>
     <row r="251" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -10431,7 +10431,7 @@
         <v>127</v>
       </c>
       <c r="B251" s="3" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
     </row>
     <row r="252" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10439,7 +10439,7 @@
         <v>128</v>
       </c>
       <c r="B252" s="3" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
     </row>
     <row r="253" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -10447,7 +10447,7 @@
         <v>129</v>
       </c>
       <c r="B253" s="3" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
     </row>
     <row r="254" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10455,7 +10455,7 @@
         <v>130</v>
       </c>
       <c r="B254" s="3" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
     </row>
     <row r="255" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -10463,7 +10463,7 @@
         <v>131</v>
       </c>
       <c r="B255" s="3" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
     </row>
     <row r="256" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -10471,7 +10471,7 @@
         <v>576</v>
       </c>
       <c r="B256" s="3" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
     </row>
     <row r="257" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10479,7 +10479,7 @@
         <v>577</v>
       </c>
       <c r="B257" s="3" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
     </row>
     <row r="258" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -10487,7 +10487,7 @@
         <v>132</v>
       </c>
       <c r="B258" s="3" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
     </row>
     <row r="259" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10495,7 +10495,7 @@
         <v>133</v>
       </c>
       <c r="B259" s="3" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
     </row>
     <row r="260" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10503,7 +10503,7 @@
         <v>575</v>
       </c>
       <c r="B260" s="3" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="261" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -10511,7 +10511,7 @@
         <v>134</v>
       </c>
       <c r="B261" s="3" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="262" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10519,7 +10519,7 @@
         <v>590</v>
       </c>
       <c r="B262" s="3" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
     </row>
     <row r="263" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10527,7 +10527,7 @@
         <v>591</v>
       </c>
       <c r="B263" s="3" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="264" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -10535,7 +10535,7 @@
         <v>135</v>
       </c>
       <c r="B264" s="3" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
     </row>
     <row r="265" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -10543,7 +10543,7 @@
         <v>592</v>
       </c>
       <c r="B265" s="3" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
     </row>
     <row r="266" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10551,7 +10551,7 @@
         <v>136</v>
       </c>
       <c r="B266" s="3" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
     </row>
     <row r="267" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -10559,7 +10559,7 @@
         <v>137</v>
       </c>
       <c r="B267" s="3" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
     </row>
     <row r="268" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10567,7 +10567,7 @@
         <v>232</v>
       </c>
       <c r="B268" s="3" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
     </row>
     <row r="269" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10575,7 +10575,7 @@
         <v>233</v>
       </c>
       <c r="B269" s="3" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
     </row>
     <row r="270" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -10591,7 +10591,7 @@
         <v>234</v>
       </c>
       <c r="B271" s="3" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
     </row>
     <row r="272" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10599,7 +10599,7 @@
         <v>235</v>
       </c>
       <c r="B272" s="3" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
     </row>
     <row r="273" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -10615,7 +10615,7 @@
         <v>239</v>
       </c>
       <c r="B274" s="3" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
     </row>
     <row r="275" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10623,7 +10623,7 @@
         <v>240</v>
       </c>
       <c r="B275" s="3" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="276" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10631,7 +10631,7 @@
         <v>241</v>
       </c>
       <c r="B276" s="3" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
     </row>
     <row r="277" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10647,7 +10647,7 @@
         <v>236</v>
       </c>
       <c r="B278" s="3" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
     </row>
     <row r="279" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10655,7 +10655,7 @@
         <v>237</v>
       </c>
       <c r="B279" s="3" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
     </row>
     <row r="280" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10663,7 +10663,7 @@
         <v>238</v>
       </c>
       <c r="B280" s="3" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
     </row>
     <row r="281" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10671,7 +10671,7 @@
         <v>141</v>
       </c>
       <c r="B281" s="3" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
     </row>
     <row r="282" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10679,7 +10679,7 @@
         <v>142</v>
       </c>
       <c r="B282" s="3" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="283" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10687,7 +10687,7 @@
         <v>143</v>
       </c>
       <c r="B283" s="3" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="284" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -10695,7 +10695,7 @@
         <v>144</v>
       </c>
       <c r="B284" s="3" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
     </row>
     <row r="285" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10703,7 +10703,7 @@
         <v>242</v>
       </c>
       <c r="B285" s="3" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
     </row>
     <row r="286" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10711,7 +10711,7 @@
         <v>145</v>
       </c>
       <c r="B286" s="3" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
     </row>
     <row r="287" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10719,7 +10719,7 @@
         <v>146</v>
       </c>
       <c r="B287" s="3" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
     </row>
     <row r="288" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10727,7 +10727,7 @@
         <v>147</v>
       </c>
       <c r="B288" s="3" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
     </row>
     <row r="289" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10735,7 +10735,7 @@
         <v>148</v>
       </c>
       <c r="B289" s="3" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
     </row>
     <row r="290" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10743,7 +10743,7 @@
         <v>149</v>
       </c>
       <c r="B290" s="3" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
     </row>
     <row r="291" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10751,7 +10751,7 @@
         <v>605</v>
       </c>
       <c r="B291" s="3" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
     </row>
     <row r="292" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10759,7 +10759,7 @@
         <v>604</v>
       </c>
       <c r="B292" s="3" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="293" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10767,7 +10767,7 @@
         <v>606</v>
       </c>
       <c r="B293" s="3" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
     </row>
     <row r="294" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10775,7 +10775,7 @@
         <v>150</v>
       </c>
       <c r="B294" s="3" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
     </row>
     <row r="295" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10783,7 +10783,7 @@
         <v>607</v>
       </c>
       <c r="B295" s="3" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
     </row>
     <row r="296" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -10791,7 +10791,7 @@
         <v>151</v>
       </c>
       <c r="B296" s="3" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
     </row>
     <row r="297" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10799,7 +10799,7 @@
         <v>243</v>
       </c>
       <c r="B297" s="3" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
     </row>
     <row r="298" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10807,7 +10807,7 @@
         <v>244</v>
       </c>
       <c r="B298" s="3" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
     </row>
     <row r="299" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10815,7 +10815,7 @@
         <v>245</v>
       </c>
       <c r="B299" s="3" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
     </row>
     <row r="300" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10823,7 +10823,7 @@
         <v>152</v>
       </c>
       <c r="B300" s="3" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
     </row>
     <row r="301" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10831,7 +10831,7 @@
         <v>153</v>
       </c>
       <c r="B301" s="3" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
     </row>
     <row r="302" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10839,7 +10839,7 @@
         <v>154</v>
       </c>
       <c r="B302" s="3" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
     </row>
     <row r="303" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -10847,7 +10847,7 @@
         <v>155</v>
       </c>
       <c r="B303" s="3" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
     </row>
     <row r="304" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10855,7 +10855,7 @@
         <v>156</v>
       </c>
       <c r="B304" s="3" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
     </row>
     <row r="305" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10871,7 +10871,7 @@
         <v>246</v>
       </c>
       <c r="B306" s="3" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
     </row>
     <row r="307" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10879,7 +10879,7 @@
         <v>247</v>
       </c>
       <c r="B307" s="3" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
     </row>
     <row r="308" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10887,7 +10887,7 @@
         <v>248</v>
       </c>
       <c r="B308" s="3" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
     </row>
     <row r="309" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10903,7 +10903,7 @@
         <v>159</v>
       </c>
       <c r="B310" s="3" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
     </row>
     <row r="311" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10911,7 +10911,7 @@
         <v>160</v>
       </c>
       <c r="B311" s="3" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
     </row>
     <row r="312" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -10919,7 +10919,7 @@
         <v>161</v>
       </c>
       <c r="B312" s="3" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
     </row>
     <row r="313" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -10927,7 +10927,7 @@
         <v>162</v>
       </c>
       <c r="B313" s="3" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
     </row>
     <row r="314" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -10935,7 +10935,7 @@
         <v>599</v>
       </c>
       <c r="B314" s="3" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
     </row>
     <row r="315" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10943,7 +10943,7 @@
         <v>600</v>
       </c>
       <c r="B315" s="3" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
     </row>
     <row r="316" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10951,7 +10951,7 @@
         <v>601</v>
       </c>
       <c r="B316" s="3" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
     </row>
     <row r="317" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10959,7 +10959,7 @@
         <v>163</v>
       </c>
       <c r="B317" s="3" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
     </row>
     <row r="318" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10967,7 +10967,7 @@
         <v>164</v>
       </c>
       <c r="B318" s="3" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
     </row>
     <row r="319" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10975,7 +10975,7 @@
         <v>175</v>
       </c>
       <c r="B319" s="3" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
     </row>
     <row r="320" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -10983,7 +10983,7 @@
         <v>176</v>
       </c>
       <c r="B320" s="3" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
     </row>
     <row r="321" spans="1:2" ht="390" x14ac:dyDescent="0.25">
@@ -10991,7 +10991,7 @@
         <v>177</v>
       </c>
       <c r="B321" s="3" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
     </row>
     <row r="322" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -11007,7 +11007,7 @@
         <v>414</v>
       </c>
       <c r="B323" s="3" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
     </row>
     <row r="324" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11015,7 +11015,7 @@
         <v>415</v>
       </c>
       <c r="B324" s="3" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
     </row>
     <row r="325" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -11023,7 +11023,7 @@
         <v>416</v>
       </c>
       <c r="B325" s="3" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
     </row>
     <row r="326" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -11031,7 +11031,7 @@
         <v>417</v>
       </c>
       <c r="B326" s="3" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
     </row>
     <row r="327" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11039,7 +11039,7 @@
         <v>418</v>
       </c>
       <c r="B327" s="3" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
     </row>
     <row r="328" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11047,7 +11047,7 @@
         <v>613</v>
       </c>
       <c r="B328" s="3" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
     </row>
     <row r="329" spans="1:2" ht="390" x14ac:dyDescent="0.25">
@@ -11055,7 +11055,7 @@
         <v>178</v>
       </c>
       <c r="B329" s="3" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
     </row>
     <row r="330" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -11071,7 +11071,7 @@
         <v>426</v>
       </c>
       <c r="B331" s="3" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
     </row>
     <row r="332" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11079,7 +11079,7 @@
         <v>427</v>
       </c>
       <c r="B332" s="3" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
     </row>
     <row r="333" spans="1:2" ht="315" x14ac:dyDescent="0.25">
@@ -11087,7 +11087,7 @@
         <v>179</v>
       </c>
       <c r="B333" s="3" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
     </row>
     <row r="334" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -11095,7 +11095,7 @@
         <v>249</v>
       </c>
       <c r="B334" s="3" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
     </row>
     <row r="335" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -11103,7 +11103,7 @@
         <v>250</v>
       </c>
       <c r="B335" s="3" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
     </row>
     <row r="336" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -11111,7 +11111,7 @@
         <v>251</v>
       </c>
       <c r="B336" s="3" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
     </row>
     <row r="337" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11119,7 +11119,7 @@
         <v>252</v>
       </c>
       <c r="B337" s="3" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
     </row>
     <row r="338" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -11127,7 +11127,7 @@
         <v>253</v>
       </c>
       <c r="B338" s="3" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
     </row>
     <row r="339" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -11135,7 +11135,7 @@
         <v>545</v>
       </c>
       <c r="B339" s="3" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
     </row>
     <row r="340" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -11143,7 +11143,7 @@
         <v>546</v>
       </c>
       <c r="B340" s="3" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="341" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11151,7 +11151,7 @@
         <v>180</v>
       </c>
       <c r="B341" s="3" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
     </row>
     <row r="342" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11159,7 +11159,7 @@
         <v>181</v>
       </c>
       <c r="B342" s="3" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
     </row>
     <row r="343" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11167,7 +11167,7 @@
         <v>386</v>
       </c>
       <c r="B343" s="3" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
     </row>
     <row r="344" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -11183,7 +11183,7 @@
         <v>622</v>
       </c>
       <c r="B345" s="3" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
     </row>
     <row r="346" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11191,7 +11191,7 @@
         <v>183</v>
       </c>
       <c r="B346" s="3" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
     </row>
     <row r="347" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -11199,7 +11199,7 @@
         <v>184</v>
       </c>
       <c r="B347" s="3" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
     </row>
     <row r="348" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -11215,7 +11215,7 @@
         <v>185</v>
       </c>
       <c r="B349" s="3" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
     </row>
     <row r="350" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -11223,7 +11223,7 @@
         <v>186</v>
       </c>
       <c r="B350" s="3" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
     </row>
     <row r="351" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -11231,7 +11231,7 @@
         <v>187</v>
       </c>
       <c r="B351" s="3" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
     </row>
     <row r="352" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11247,7 +11247,7 @@
         <v>188</v>
       </c>
       <c r="B353" s="3" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
     </row>
     <row r="354" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -11255,7 +11255,7 @@
         <v>189</v>
       </c>
       <c r="B354" s="3" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
     </row>
     <row r="355" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -11263,7 +11263,7 @@
         <v>383</v>
       </c>
       <c r="B355" s="3" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
     </row>
     <row r="356" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -11271,7 +11271,7 @@
         <v>384</v>
       </c>
       <c r="B356" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="357" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -11279,7 +11279,7 @@
         <v>190</v>
       </c>
       <c r="B357" s="3" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
     </row>
     <row r="358" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -11287,7 +11287,7 @@
         <v>191</v>
       </c>
       <c r="B358" s="3" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
     </row>
     <row r="359" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -11295,7 +11295,7 @@
         <v>192</v>
       </c>
       <c r="B359" s="3" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
     </row>
     <row r="360" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -11303,7 +11303,7 @@
         <v>465</v>
       </c>
       <c r="B360" s="3" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
     </row>
     <row r="361" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -11311,7 +11311,7 @@
         <v>193</v>
       </c>
       <c r="B361" s="3" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="362" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -11327,7 +11327,7 @@
         <v>333</v>
       </c>
       <c r="B363" s="3" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
     </row>
     <row r="364" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -11335,7 +11335,7 @@
         <v>624</v>
       </c>
       <c r="B364" s="3" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="365" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -11343,7 +11343,7 @@
         <v>625</v>
       </c>
       <c r="B365" s="3" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
     </row>
     <row r="366" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11351,7 +11351,7 @@
         <v>627</v>
       </c>
       <c r="B366" s="3" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
     </row>
     <row r="367" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11359,7 +11359,7 @@
         <v>628</v>
       </c>
       <c r="B367" s="3" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
     </row>
     <row r="368" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11367,7 +11367,7 @@
         <v>629</v>
       </c>
       <c r="B368" s="3" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
     </row>
     <row r="369" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11375,7 +11375,7 @@
         <v>630</v>
       </c>
       <c r="B369" s="3" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
     </row>
     <row r="370" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11383,7 +11383,7 @@
         <v>631</v>
       </c>
       <c r="B370" s="3" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
     </row>
     <row r="371" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11391,7 +11391,7 @@
         <v>632</v>
       </c>
       <c r="B371" s="3" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
     </row>
     <row r="372" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -11399,7 +11399,7 @@
         <v>194</v>
       </c>
       <c r="B372" s="3" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
     </row>
     <row r="373" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -11407,7 +11407,7 @@
         <v>195</v>
       </c>
       <c r="B373" s="3" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
     </row>
     <row r="374" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -11415,7 +11415,7 @@
         <v>620</v>
       </c>
       <c r="B374" s="3" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
     </row>
     <row r="375" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -11423,7 +11423,7 @@
         <v>196</v>
       </c>
       <c r="B375" s="3" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="376" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -11431,7 +11431,7 @@
         <v>328</v>
       </c>
       <c r="B376" s="3" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
     </row>
     <row r="377" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -11439,7 +11439,7 @@
         <v>197</v>
       </c>
       <c r="B377" s="3" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
     </row>
     <row r="378" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11447,7 +11447,7 @@
         <v>487</v>
       </c>
       <c r="B378" s="3" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
     </row>
     <row r="379" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11455,7 +11455,7 @@
         <v>198</v>
       </c>
       <c r="B379" s="3" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
     </row>
     <row r="380" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11463,7 +11463,7 @@
         <v>199</v>
       </c>
       <c r="B380" s="3" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
     </row>
     <row r="381" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -11471,7 +11471,7 @@
         <v>200</v>
       </c>
       <c r="B381" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="382" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11479,7 +11479,7 @@
         <v>201</v>
       </c>
       <c r="B382" s="3" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
     </row>
     <row r="383" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11487,7 +11487,7 @@
         <v>202</v>
       </c>
       <c r="B383" s="3" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
     </row>
     <row r="384" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -11495,7 +11495,7 @@
         <v>203</v>
       </c>
       <c r="B384" s="3" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
     </row>
     <row r="385" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -11543,7 +11543,7 @@
         <v>204</v>
       </c>
       <c r="B390" s="3" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="391" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11551,7 +11551,7 @@
         <v>459</v>
       </c>
       <c r="B391" s="3" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="392" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11559,7 +11559,7 @@
         <v>460</v>
       </c>
       <c r="B392" s="3" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="393" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11567,7 +11567,7 @@
         <v>461</v>
       </c>
       <c r="B393" s="3" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="394" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11575,7 +11575,7 @@
         <v>462</v>
       </c>
       <c r="B394" s="3" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="395" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11583,7 +11583,7 @@
         <v>463</v>
       </c>
       <c r="B395" s="3" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="396" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11591,7 +11591,7 @@
         <v>464</v>
       </c>
       <c r="B396" s="3" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="397" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -11599,7 +11599,7 @@
         <v>205</v>
       </c>
       <c r="B397" s="3" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="398" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -11671,7 +11671,7 @@
         <v>207</v>
       </c>
       <c r="B406" s="3" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="407" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -11679,7 +11679,7 @@
         <v>208</v>
       </c>
       <c r="B407" s="3" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="408" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -11687,7 +11687,7 @@
         <v>209</v>
       </c>
       <c r="B408" s="3" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="409" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11695,7 +11695,7 @@
         <v>476</v>
       </c>
       <c r="B409" s="3" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="410" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11703,7 +11703,7 @@
         <v>477</v>
       </c>
       <c r="B410" s="3" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="411" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11711,7 +11711,7 @@
         <v>478</v>
       </c>
       <c r="B411" s="3" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="412" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -11719,7 +11719,7 @@
         <v>479</v>
       </c>
       <c r="B412" s="3" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="413" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -11727,7 +11727,7 @@
         <v>480</v>
       </c>
       <c r="B413" s="4" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="414" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -11735,7 +11735,7 @@
         <v>481</v>
       </c>
       <c r="B414" s="3" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="415" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -11743,7 +11743,7 @@
         <v>621</v>
       </c>
       <c r="B415" s="3" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="416" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -11751,7 +11751,7 @@
         <v>210</v>
       </c>
       <c r="B416" s="3" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="417" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11759,7 +11759,7 @@
         <v>469</v>
       </c>
       <c r="B417" s="3" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="418" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11767,7 +11767,7 @@
         <v>470</v>
       </c>
       <c r="B418" s="3" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="419" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11775,7 +11775,7 @@
         <v>471</v>
       </c>
       <c r="B419" s="3" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="420" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11783,7 +11783,7 @@
         <v>472</v>
       </c>
       <c r="B420" s="3" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="421" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11791,7 +11791,7 @@
         <v>473</v>
       </c>
       <c r="B421" s="3" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="422" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11799,7 +11799,7 @@
         <v>474</v>
       </c>
       <c r="B422" s="3" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="423" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11807,7 +11807,7 @@
         <v>475</v>
       </c>
       <c r="B423" s="3" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="424" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11815,7 +11815,7 @@
         <v>619</v>
       </c>
       <c r="B424" s="3" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="425" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -11823,7 +11823,7 @@
         <v>211</v>
       </c>
       <c r="B425" s="3" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="426" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11831,7 +11831,7 @@
         <v>212</v>
       </c>
       <c r="B426" s="3" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="427" spans="1:2" ht="300" x14ac:dyDescent="0.25">
@@ -11839,7 +11839,7 @@
         <v>419</v>
       </c>
       <c r="B427" s="3" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="428" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11847,7 +11847,7 @@
         <v>420</v>
       </c>
       <c r="B428" s="3" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="429" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -11855,7 +11855,7 @@
         <v>421</v>
       </c>
       <c r="B429" s="3" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="430" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11863,7 +11863,7 @@
         <v>422</v>
       </c>
       <c r="B430" s="3" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="431" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -11871,7 +11871,7 @@
         <v>213</v>
       </c>
       <c r="B431" s="3" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="432" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -11879,7 +11879,7 @@
         <v>214</v>
       </c>
       <c r="B432" s="3" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="433" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -11887,7 +11887,7 @@
         <v>215</v>
       </c>
       <c r="B433" s="3" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="434" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11895,7 +11895,7 @@
         <v>216</v>
       </c>
       <c r="B434" s="3" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="435" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11903,7 +11903,7 @@
         <v>217</v>
       </c>
       <c r="B435" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="436" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11911,7 +11911,7 @@
         <v>218</v>
       </c>
       <c r="B436" s="3" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="437" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11919,7 +11919,7 @@
         <v>219</v>
       </c>
       <c r="B437" s="3" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="438" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11927,7 +11927,7 @@
         <v>220</v>
       </c>
       <c r="B438" s="3" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="439" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11935,7 +11935,7 @@
         <v>221</v>
       </c>
       <c r="B439" s="3" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="440" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11943,7 +11943,7 @@
         <v>222</v>
       </c>
       <c r="B440" s="3" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="441" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11951,7 +11951,7 @@
         <v>223</v>
       </c>
       <c r="B441" s="3" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="442" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -11959,7 +11959,7 @@
         <v>224</v>
       </c>
       <c r="B442" s="3" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="443" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -11967,7 +11967,7 @@
         <v>329</v>
       </c>
       <c r="B443" s="3" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="444" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11975,7 +11975,7 @@
         <v>385</v>
       </c>
       <c r="B444" s="3" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="445" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11983,7 +11983,7 @@
         <v>225</v>
       </c>
       <c r="B445" s="3" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="446" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -11991,7 +11991,7 @@
         <v>226</v>
       </c>
       <c r="B446" s="3" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="447" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -11999,7 +11999,7 @@
         <v>227</v>
       </c>
       <c r="B447" s="3" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="448" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -12007,7 +12007,7 @@
         <v>228</v>
       </c>
       <c r="B448" s="3" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="449" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -12015,7 +12015,7 @@
         <v>618</v>
       </c>
       <c r="B449" s="3" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="450" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12023,7 +12023,7 @@
         <v>229</v>
       </c>
       <c r="B450" s="3" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="451" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -12031,7 +12031,7 @@
         <v>230</v>
       </c>
       <c r="B451" s="3" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="452" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -12039,7 +12039,7 @@
         <v>231</v>
       </c>
       <c r="B452" s="3" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="453" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12047,7 +12047,7 @@
         <v>257</v>
       </c>
       <c r="B453" s="3" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="454" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -12055,7 +12055,7 @@
         <v>379</v>
       </c>
       <c r="B454" s="3" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="455" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12063,7 +12063,7 @@
         <v>380</v>
       </c>
       <c r="B455" s="3" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="456" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12071,7 +12071,7 @@
         <v>444</v>
       </c>
       <c r="B456" s="3" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="457" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12087,15 +12087,15 @@
         <v>531</v>
       </c>
       <c r="B458" s="3" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="459" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A459" s="2" t="s">
+        <v>1162</v>
+      </c>
+      <c r="B459" s="3" t="s">
         <v>1163</v>
-      </c>
-      <c r="B459" s="3" t="s">
-        <v>1164</v>
       </c>
     </row>
     <row r="460" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -12135,7 +12135,7 @@
         <v>602</v>
       </c>
       <c r="B464" s="3" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="465" spans="1:2" ht="255" x14ac:dyDescent="0.25">
@@ -12143,7 +12143,7 @@
         <v>322</v>
       </c>
       <c r="B465" s="3" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="466" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12151,7 +12151,7 @@
         <v>395</v>
       </c>
       <c r="B466" s="3" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="467" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -12159,7 +12159,7 @@
         <v>394</v>
       </c>
       <c r="B467" s="3" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="468" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12167,7 +12167,7 @@
         <v>396</v>
       </c>
       <c r="B468" s="3" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="469" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12175,7 +12175,7 @@
         <v>397</v>
       </c>
       <c r="B469" s="3" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="470" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12183,7 +12183,7 @@
         <v>398</v>
       </c>
       <c r="B470" s="3" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="471" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12191,7 +12191,7 @@
         <v>399</v>
       </c>
       <c r="B471" s="3" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="472" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12199,7 +12199,7 @@
         <v>400</v>
       </c>
       <c r="B472" s="3" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="473" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12207,7 +12207,7 @@
         <v>431</v>
       </c>
       <c r="B473" s="3" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="474" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -12215,7 +12215,7 @@
         <v>432</v>
       </c>
       <c r="B474" s="3" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="475" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -12223,7 +12223,7 @@
         <v>433</v>
       </c>
       <c r="B475" s="3" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="476" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12231,7 +12231,7 @@
         <v>434</v>
       </c>
       <c r="B476" s="3" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="477" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12239,7 +12239,7 @@
         <v>435</v>
       </c>
       <c r="B477" s="3" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="478" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12247,7 +12247,7 @@
         <v>436</v>
       </c>
       <c r="B478" s="3" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="479" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -12255,7 +12255,7 @@
         <v>437</v>
       </c>
       <c r="B479" s="3" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="480" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12263,7 +12263,7 @@
         <v>438</v>
       </c>
       <c r="B480" s="3" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="481" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12271,7 +12271,7 @@
         <v>439</v>
       </c>
       <c r="B481" s="3" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="482" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -12279,7 +12279,7 @@
         <v>440</v>
       </c>
       <c r="B482" s="3" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="483" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12287,7 +12287,7 @@
         <v>441</v>
       </c>
       <c r="B483" s="3" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="484" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -12295,7 +12295,7 @@
         <v>442</v>
       </c>
       <c r="B484" s="3" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="485" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -12303,7 +12303,7 @@
         <v>443</v>
       </c>
       <c r="B485" s="3" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="486" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -12311,7 +12311,7 @@
         <v>458</v>
       </c>
       <c r="B486" s="3" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="487" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -12319,7 +12319,7 @@
         <v>466</v>
       </c>
       <c r="B487" s="3" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="488" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -12327,7 +12327,7 @@
         <v>467</v>
       </c>
       <c r="B488" s="3" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="489" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -12335,7 +12335,7 @@
         <v>468</v>
       </c>
       <c r="B489" s="3" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="490" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -12343,7 +12343,7 @@
         <v>552</v>
       </c>
       <c r="B490" s="3" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="491" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -12351,7 +12351,7 @@
         <v>633</v>
       </c>
       <c r="B491" s="3" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="492" spans="1:2" ht="255" x14ac:dyDescent="0.25">
@@ -12359,7 +12359,7 @@
         <v>488</v>
       </c>
       <c r="B492" s="1" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="493" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12367,7 +12367,7 @@
         <v>489</v>
       </c>
       <c r="B493" s="1" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="494" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12375,7 +12375,7 @@
         <v>490</v>
       </c>
       <c r="B494" s="1" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="495" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12383,7 +12383,7 @@
         <v>491</v>
       </c>
       <c r="B495" s="1" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="496" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12391,7 +12391,7 @@
         <v>492</v>
       </c>
       <c r="B496" s="1" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="497" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12399,7 +12399,7 @@
         <v>493</v>
       </c>
       <c r="B497" s="1" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="498" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12407,7 +12407,7 @@
         <v>494</v>
       </c>
       <c r="B498" s="1" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="499" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12415,7 +12415,7 @@
         <v>495</v>
       </c>
       <c r="B499" s="1" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="500" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12423,7 +12423,7 @@
         <v>496</v>
       </c>
       <c r="B500" s="1" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="501" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -12431,7 +12431,7 @@
         <v>497</v>
       </c>
       <c r="B501" s="1" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="502" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12439,7 +12439,7 @@
         <v>498</v>
       </c>
       <c r="B502" s="1" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="503" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12447,7 +12447,7 @@
         <v>499</v>
       </c>
       <c r="B503" s="1" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="504" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -12455,7 +12455,7 @@
         <v>500</v>
       </c>
       <c r="B504" s="1" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="505" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12463,7 +12463,7 @@
         <v>501</v>
       </c>
       <c r="B505" s="1" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="506" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12471,7 +12471,7 @@
         <v>502</v>
       </c>
       <c r="B506" s="1" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="507" spans="1:2" ht="255" x14ac:dyDescent="0.25">
@@ -12479,7 +12479,7 @@
         <v>597</v>
       </c>
       <c r="B507" s="1" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="508" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12487,7 +12487,7 @@
         <v>598</v>
       </c>
       <c r="B508" s="1" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="509" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12495,7 +12495,7 @@
         <v>503</v>
       </c>
       <c r="B509" s="1" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="510" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12503,7 +12503,7 @@
         <v>515</v>
       </c>
       <c r="B510" s="3" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="511" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -12511,7 +12511,7 @@
         <v>423</v>
       </c>
       <c r="B511" s="3" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="512" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12535,7 +12535,7 @@
         <v>267</v>
       </c>
       <c r="B514" s="1" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="515" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12543,7 +12543,7 @@
         <v>268</v>
       </c>
       <c r="B515" s="1" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="516" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12551,7 +12551,7 @@
         <v>269</v>
       </c>
       <c r="B516" s="1" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="517" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12559,7 +12559,7 @@
         <v>270</v>
       </c>
       <c r="B517" s="1" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="518" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12567,7 +12567,7 @@
         <v>271</v>
       </c>
       <c r="B518" s="1" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="519" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12575,7 +12575,7 @@
         <v>272</v>
       </c>
       <c r="B519" s="1" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="520" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12583,7 +12583,7 @@
         <v>273</v>
       </c>
       <c r="B520" s="1" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="521" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12591,7 +12591,7 @@
         <v>274</v>
       </c>
       <c r="B521" s="1" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="522" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12599,7 +12599,7 @@
         <v>275</v>
       </c>
       <c r="B522" s="1" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="523" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12607,7 +12607,7 @@
         <v>276</v>
       </c>
       <c r="B523" s="1" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="524" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12615,7 +12615,7 @@
         <v>277</v>
       </c>
       <c r="B524" s="1" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="525" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12695,7 +12695,7 @@
         <v>280</v>
       </c>
       <c r="B534" s="1" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="535" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12703,7 +12703,7 @@
         <v>281</v>
       </c>
       <c r="B535" s="1" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="536" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12719,7 +12719,7 @@
         <v>283</v>
       </c>
       <c r="B537" s="1" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="538" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12727,7 +12727,7 @@
         <v>284</v>
       </c>
       <c r="B538" s="1" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="539" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12735,7 +12735,7 @@
         <v>285</v>
       </c>
       <c r="B539" s="1" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="540" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12743,7 +12743,7 @@
         <v>286</v>
       </c>
       <c r="B540" s="1" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="541" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12791,7 +12791,7 @@
         <v>292</v>
       </c>
       <c r="B546" s="1" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="547" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12799,7 +12799,7 @@
         <v>293</v>
       </c>
       <c r="B547" s="1" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="548" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12807,7 +12807,7 @@
         <v>294</v>
       </c>
       <c r="B548" s="1" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="549" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12815,7 +12815,7 @@
         <v>295</v>
       </c>
       <c r="B549" s="1" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="550" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -12823,7 +12823,7 @@
         <v>296</v>
       </c>
       <c r="B550" s="1" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="551" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12831,7 +12831,7 @@
         <v>297</v>
       </c>
       <c r="B551" s="1" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="552" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -12839,7 +12839,7 @@
         <v>353</v>
       </c>
       <c r="B552" s="1" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="553" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12847,7 +12847,7 @@
         <v>365</v>
       </c>
       <c r="B553" s="3" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="554" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12855,7 +12855,7 @@
         <v>366</v>
       </c>
       <c r="B554" s="1" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="555" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12863,7 +12863,7 @@
         <v>298</v>
       </c>
       <c r="B555" s="1" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="556" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -12871,7 +12871,7 @@
         <v>364</v>
       </c>
       <c r="B556" s="1" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="557" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12879,7 +12879,7 @@
         <v>299</v>
       </c>
       <c r="B557" s="1" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
     </row>
     <row r="558" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -12887,7 +12887,7 @@
         <v>354</v>
       </c>
       <c r="B558" s="1" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
     </row>
     <row r="559" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -12903,7 +12903,7 @@
         <v>300</v>
       </c>
       <c r="B560" s="1" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="561" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12911,7 +12911,7 @@
         <v>301</v>
       </c>
       <c r="B561" s="1" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="562" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12919,7 +12919,7 @@
         <v>302</v>
       </c>
       <c r="B562" s="1" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="563" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12927,7 +12927,7 @@
         <v>303</v>
       </c>
       <c r="B563" s="1" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="564" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -12935,7 +12935,7 @@
         <v>363</v>
       </c>
       <c r="B564" s="1" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="565" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12943,7 +12943,7 @@
         <v>304</v>
       </c>
       <c r="B565" s="1" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="566" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12951,7 +12951,7 @@
         <v>361</v>
       </c>
       <c r="B566" s="1" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="567" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -12967,7 +12967,7 @@
         <v>517</v>
       </c>
       <c r="B568" s="1" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="569" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12975,7 +12975,7 @@
         <v>305</v>
       </c>
       <c r="B569" s="1" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="570" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12983,7 +12983,7 @@
         <v>358</v>
       </c>
       <c r="B570" s="1" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="571" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12991,7 +12991,7 @@
         <v>359</v>
       </c>
       <c r="B571" s="1" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="572" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -13007,7 +13007,7 @@
         <v>518</v>
       </c>
       <c r="B573" s="1" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="574" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -13015,7 +13015,7 @@
         <v>306</v>
       </c>
       <c r="B574" s="1" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="575" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -13023,7 +13023,7 @@
         <v>352</v>
       </c>
       <c r="B575" s="1" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="576" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -13031,7 +13031,7 @@
         <v>355</v>
       </c>
       <c r="B576" s="3" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="577" spans="1:2" ht="405" x14ac:dyDescent="0.25">
@@ -13039,7 +13039,7 @@
         <v>307</v>
       </c>
       <c r="B577" s="1" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="578" spans="1:2" ht="375" x14ac:dyDescent="0.25">
@@ -13047,7 +13047,7 @@
         <v>311</v>
       </c>
       <c r="B578" s="1" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="579" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -13071,7 +13071,7 @@
         <v>349</v>
       </c>
       <c r="B581" s="3" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="582" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -13079,7 +13079,7 @@
         <v>519</v>
       </c>
       <c r="B582" s="3" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="583" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -13087,7 +13087,7 @@
         <v>326</v>
       </c>
       <c r="B583" s="3" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change text about falcon
</commit_message>
<xml_diff>
--- a/Documentation/Events.xlsx
+++ b/Documentation/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\happysulla\BarbarianPrince\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{DF19B41A-16B2-454F-8E6D-F48C4E98670C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4400EF6A-9D95-4150-BF11-AEEAA5F61C21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -5406,19 +5406,6 @@
           &lt;InlineUIContainer&gt;&lt;Image Name='AirOvercast' Source='../bin/Images/Overcast.gif' Height='220' Width='480'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e107 Falcon Scout&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;A friendly falcon joins your party if you &lt;InlineUIContainer&gt;&lt;Button Content='Feed' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; one unit of food
- &lt;InlineUIContainer&gt;&lt;Button Content='r215' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
- right now. For the rest of today, you cannot get lost.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;Tonight, at the evening meal
- &lt;InlineUIContainer&gt;&lt;Button Content='r215' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;,
- if you offer it a second food unit, roll the die. If you roll anyhing other than a six, the falcon will remain throughout tomorrow with your party as a guide.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;This can continue day after day provided you feed it a food unit at the evening meal and roll anything but a six.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;The falcon can only act as a guide. It has no combat skill or endurance value. Any wound will kill it. Click image to continue if not feeding.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                        &lt;InlineUIContainer&gt;&lt;Image Name='FalconNoFeed' Source='../bin/Images/Falcon.gif' Height='188' Width='250'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;e108 Hawkmen Attack&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;You encournter a group of hawkmen who swoop down on your party.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;Each has a combat skill 7, endurance 5, and wealth 7.  Roll one die for the number of hawkmen:  &lt;InlineUIContainer&gt;&lt;Image Source='../bin/Images/dieRoll.gif' Name='DieRoll' Height='21'  Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
@@ -8028,6 +8015,19 @@
  &lt;InlineUIContainer&gt;&lt;Button Content='e165' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  1 - Eleven Town&lt;LineBreak/&gt;
  &lt;InlineUIContainer&gt;&lt;Button Content='e166' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  2 - Elven Fortress&lt;LineBreak/&gt;
  &lt;InlineUIContainer&gt;&lt;Button Content='e053' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  3,4,5,6 - Campsite</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e107 Falcon Scout&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;A friendly falcon joins your party if you &lt;InlineUIContainer&gt;&lt;Button Content='Feed' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; one unit of food
+ &lt;InlineUIContainer&gt;&lt;Button Content='r215' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+ right now. You can never get lost with a falcon.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;Tonight, at the evening meal
+ &lt;InlineUIContainer&gt;&lt;Button Content='r215' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;,
+ if you offer it a second food unit, roll the die. If you roll anyhing other than a six, the falcon will remain throughout tomorrow with your party as a guide.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;This can continue day after day provided you feed it a food unit at the evening meal and roll anything but a six.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;The falcon can only act as a guide. It has no combat skill or endurance value. Any wound will kill it. Click image to continue if not feeding.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                        &lt;InlineUIContainer&gt;&lt;Image Name='FalconNoFeed' Source='../bin/Images/Falcon.gif' Height='188' Width='250'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
 </sst>
 </file>
@@ -8416,8 +8416,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B583"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A485" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B486" sqref="B486"/>
+    <sheetView tabSelected="1" topLeftCell="A285" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B287" sqref="B287"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9199,7 +9199,7 @@
         <v>61</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -9455,7 +9455,7 @@
         <v>350</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
     </row>
     <row r="130" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10103,7 +10103,7 @@
         <v>510</v>
       </c>
       <c r="B210" s="3" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="211" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -10127,7 +10127,7 @@
         <v>516</v>
       </c>
       <c r="B213" s="3" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
     </row>
     <row r="214" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10183,7 +10183,7 @@
         <v>266</v>
       </c>
       <c r="B220" s="3" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="221" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -10487,7 +10487,7 @@
         <v>132</v>
       </c>
       <c r="B258" s="3" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="259" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10719,7 +10719,7 @@
         <v>146</v>
       </c>
       <c r="B287" s="3" t="s">
-        <v>910</v>
+        <v>1165</v>
       </c>
     </row>
     <row r="288" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10727,7 +10727,7 @@
         <v>147</v>
       </c>
       <c r="B288" s="3" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
     </row>
     <row r="289" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10735,7 +10735,7 @@
         <v>148</v>
       </c>
       <c r="B289" s="3" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
     </row>
     <row r="290" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10743,7 +10743,7 @@
         <v>149</v>
       </c>
       <c r="B290" s="3" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
     </row>
     <row r="291" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10751,7 +10751,7 @@
         <v>605</v>
       </c>
       <c r="B291" s="3" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
     </row>
     <row r="292" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10759,7 +10759,7 @@
         <v>604</v>
       </c>
       <c r="B292" s="3" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
     </row>
     <row r="293" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10767,7 +10767,7 @@
         <v>606</v>
       </c>
       <c r="B293" s="3" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="294" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10775,7 +10775,7 @@
         <v>150</v>
       </c>
       <c r="B294" s="3" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
     </row>
     <row r="295" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10783,7 +10783,7 @@
         <v>607</v>
       </c>
       <c r="B295" s="3" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
     </row>
     <row r="296" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -10791,7 +10791,7 @@
         <v>151</v>
       </c>
       <c r="B296" s="3" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
     </row>
     <row r="297" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10799,7 +10799,7 @@
         <v>243</v>
       </c>
       <c r="B297" s="3" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
     </row>
     <row r="298" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10807,7 +10807,7 @@
         <v>244</v>
       </c>
       <c r="B298" s="3" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
     </row>
     <row r="299" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10815,7 +10815,7 @@
         <v>245</v>
       </c>
       <c r="B299" s="3" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
     </row>
     <row r="300" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10823,7 +10823,7 @@
         <v>152</v>
       </c>
       <c r="B300" s="3" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
     </row>
     <row r="301" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10831,7 +10831,7 @@
         <v>153</v>
       </c>
       <c r="B301" s="3" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
     </row>
     <row r="302" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10839,7 +10839,7 @@
         <v>154</v>
       </c>
       <c r="B302" s="3" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
     </row>
     <row r="303" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -10847,7 +10847,7 @@
         <v>155</v>
       </c>
       <c r="B303" s="3" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
     </row>
     <row r="304" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10855,7 +10855,7 @@
         <v>156</v>
       </c>
       <c r="B304" s="3" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
     </row>
     <row r="305" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10871,7 +10871,7 @@
         <v>246</v>
       </c>
       <c r="B306" s="3" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
     </row>
     <row r="307" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10879,7 +10879,7 @@
         <v>247</v>
       </c>
       <c r="B307" s="3" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
     </row>
     <row r="308" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10887,7 +10887,7 @@
         <v>248</v>
       </c>
       <c r="B308" s="3" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
     </row>
     <row r="309" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10903,7 +10903,7 @@
         <v>159</v>
       </c>
       <c r="B310" s="3" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
     </row>
     <row r="311" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10911,7 +10911,7 @@
         <v>160</v>
       </c>
       <c r="B311" s="3" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
     </row>
     <row r="312" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -10919,7 +10919,7 @@
         <v>161</v>
       </c>
       <c r="B312" s="3" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
     </row>
     <row r="313" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -10927,7 +10927,7 @@
         <v>162</v>
       </c>
       <c r="B313" s="3" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
     </row>
     <row r="314" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -10935,7 +10935,7 @@
         <v>599</v>
       </c>
       <c r="B314" s="3" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
     </row>
     <row r="315" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10943,7 +10943,7 @@
         <v>600</v>
       </c>
       <c r="B315" s="3" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
     </row>
     <row r="316" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10951,7 +10951,7 @@
         <v>601</v>
       </c>
       <c r="B316" s="3" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
     </row>
     <row r="317" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10959,7 +10959,7 @@
         <v>163</v>
       </c>
       <c r="B317" s="3" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
     </row>
     <row r="318" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10967,7 +10967,7 @@
         <v>164</v>
       </c>
       <c r="B318" s="3" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
     </row>
     <row r="319" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10975,7 +10975,7 @@
         <v>175</v>
       </c>
       <c r="B319" s="3" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
     </row>
     <row r="320" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -10983,7 +10983,7 @@
         <v>176</v>
       </c>
       <c r="B320" s="3" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
     </row>
     <row r="321" spans="1:2" ht="390" x14ac:dyDescent="0.25">
@@ -10991,7 +10991,7 @@
         <v>177</v>
       </c>
       <c r="B321" s="3" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
     </row>
     <row r="322" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -11007,7 +11007,7 @@
         <v>414</v>
       </c>
       <c r="B323" s="3" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
     </row>
     <row r="324" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11015,7 +11015,7 @@
         <v>415</v>
       </c>
       <c r="B324" s="3" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
     </row>
     <row r="325" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -11023,7 +11023,7 @@
         <v>416</v>
       </c>
       <c r="B325" s="3" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
     </row>
     <row r="326" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -11031,7 +11031,7 @@
         <v>417</v>
       </c>
       <c r="B326" s="3" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
     </row>
     <row r="327" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11039,7 +11039,7 @@
         <v>418</v>
       </c>
       <c r="B327" s="3" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
     </row>
     <row r="328" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11047,7 +11047,7 @@
         <v>613</v>
       </c>
       <c r="B328" s="3" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
     </row>
     <row r="329" spans="1:2" ht="390" x14ac:dyDescent="0.25">
@@ -11055,7 +11055,7 @@
         <v>178</v>
       </c>
       <c r="B329" s="3" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
     </row>
     <row r="330" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -11071,7 +11071,7 @@
         <v>426</v>
       </c>
       <c r="B331" s="3" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
     </row>
     <row r="332" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11079,7 +11079,7 @@
         <v>427</v>
       </c>
       <c r="B332" s="3" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
     </row>
     <row r="333" spans="1:2" ht="315" x14ac:dyDescent="0.25">
@@ -11087,7 +11087,7 @@
         <v>179</v>
       </c>
       <c r="B333" s="3" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
     </row>
     <row r="334" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -11095,7 +11095,7 @@
         <v>249</v>
       </c>
       <c r="B334" s="3" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
     </row>
     <row r="335" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -11103,7 +11103,7 @@
         <v>250</v>
       </c>
       <c r="B335" s="3" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
     </row>
     <row r="336" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -11111,7 +11111,7 @@
         <v>251</v>
       </c>
       <c r="B336" s="3" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
     </row>
     <row r="337" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11119,7 +11119,7 @@
         <v>252</v>
       </c>
       <c r="B337" s="3" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
     </row>
     <row r="338" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -11127,7 +11127,7 @@
         <v>253</v>
       </c>
       <c r="B338" s="3" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
     </row>
     <row r="339" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -11135,7 +11135,7 @@
         <v>545</v>
       </c>
       <c r="B339" s="3" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
     </row>
     <row r="340" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -11143,7 +11143,7 @@
         <v>546</v>
       </c>
       <c r="B340" s="3" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
     </row>
     <row r="341" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11151,7 +11151,7 @@
         <v>180</v>
       </c>
       <c r="B341" s="3" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="342" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11159,7 +11159,7 @@
         <v>181</v>
       </c>
       <c r="B342" s="3" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
     </row>
     <row r="343" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11167,7 +11167,7 @@
         <v>386</v>
       </c>
       <c r="B343" s="3" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
     </row>
     <row r="344" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -11183,7 +11183,7 @@
         <v>622</v>
       </c>
       <c r="B345" s="3" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
     </row>
     <row r="346" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11191,7 +11191,7 @@
         <v>183</v>
       </c>
       <c r="B346" s="3" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
     </row>
     <row r="347" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -11199,7 +11199,7 @@
         <v>184</v>
       </c>
       <c r="B347" s="3" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
     </row>
     <row r="348" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -11215,7 +11215,7 @@
         <v>185</v>
       </c>
       <c r="B349" s="3" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
     </row>
     <row r="350" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -11223,7 +11223,7 @@
         <v>186</v>
       </c>
       <c r="B350" s="3" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
     </row>
     <row r="351" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -11231,7 +11231,7 @@
         <v>187</v>
       </c>
       <c r="B351" s="3" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
     </row>
     <row r="352" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11247,7 +11247,7 @@
         <v>188</v>
       </c>
       <c r="B353" s="3" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
     </row>
     <row r="354" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -11255,7 +11255,7 @@
         <v>189</v>
       </c>
       <c r="B354" s="3" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
     </row>
     <row r="355" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -11263,7 +11263,7 @@
         <v>383</v>
       </c>
       <c r="B355" s="3" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
     </row>
     <row r="356" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -11271,7 +11271,7 @@
         <v>384</v>
       </c>
       <c r="B356" s="3" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
     </row>
     <row r="357" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -11279,7 +11279,7 @@
         <v>190</v>
       </c>
       <c r="B357" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="358" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -11287,7 +11287,7 @@
         <v>191</v>
       </c>
       <c r="B358" s="3" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
     </row>
     <row r="359" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -11295,7 +11295,7 @@
         <v>192</v>
       </c>
       <c r="B359" s="3" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
     </row>
     <row r="360" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -11303,7 +11303,7 @@
         <v>465</v>
       </c>
       <c r="B360" s="3" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
     </row>
     <row r="361" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -11311,7 +11311,7 @@
         <v>193</v>
       </c>
       <c r="B361" s="3" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
     </row>
     <row r="362" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -11327,7 +11327,7 @@
         <v>333</v>
       </c>
       <c r="B363" s="3" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="364" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -11335,7 +11335,7 @@
         <v>624</v>
       </c>
       <c r="B364" s="3" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
     </row>
     <row r="365" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -11343,7 +11343,7 @@
         <v>625</v>
       </c>
       <c r="B365" s="3" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="366" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11351,7 +11351,7 @@
         <v>627</v>
       </c>
       <c r="B366" s="3" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
     </row>
     <row r="367" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11359,7 +11359,7 @@
         <v>628</v>
       </c>
       <c r="B367" s="3" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
     </row>
     <row r="368" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11367,7 +11367,7 @@
         <v>629</v>
       </c>
       <c r="B368" s="3" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
     </row>
     <row r="369" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11375,7 +11375,7 @@
         <v>630</v>
       </c>
       <c r="B369" s="3" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
     </row>
     <row r="370" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11383,7 +11383,7 @@
         <v>631</v>
       </c>
       <c r="B370" s="3" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
     </row>
     <row r="371" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11391,7 +11391,7 @@
         <v>632</v>
       </c>
       <c r="B371" s="3" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
     </row>
     <row r="372" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -11399,7 +11399,7 @@
         <v>194</v>
       </c>
       <c r="B372" s="3" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
     </row>
     <row r="373" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -11407,7 +11407,7 @@
         <v>195</v>
       </c>
       <c r="B373" s="3" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
     </row>
     <row r="374" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -11415,7 +11415,7 @@
         <v>620</v>
       </c>
       <c r="B374" s="3" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
     </row>
     <row r="375" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -11423,7 +11423,7 @@
         <v>196</v>
       </c>
       <c r="B375" s="3" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
     </row>
     <row r="376" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -11431,7 +11431,7 @@
         <v>328</v>
       </c>
       <c r="B376" s="3" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="377" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -11439,7 +11439,7 @@
         <v>197</v>
       </c>
       <c r="B377" s="3" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
     </row>
     <row r="378" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11447,7 +11447,7 @@
         <v>487</v>
       </c>
       <c r="B378" s="3" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
     </row>
     <row r="379" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11455,7 +11455,7 @@
         <v>198</v>
       </c>
       <c r="B379" s="3" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
     </row>
     <row r="380" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11463,7 +11463,7 @@
         <v>199</v>
       </c>
       <c r="B380" s="3" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
     </row>
     <row r="381" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -11471,7 +11471,7 @@
         <v>200</v>
       </c>
       <c r="B381" s="3" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
     </row>
     <row r="382" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11479,7 +11479,7 @@
         <v>201</v>
       </c>
       <c r="B382" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="383" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11487,7 +11487,7 @@
         <v>202</v>
       </c>
       <c r="B383" s="3" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
     </row>
     <row r="384" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -11495,7 +11495,7 @@
         <v>203</v>
       </c>
       <c r="B384" s="3" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
     </row>
     <row r="385" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -11543,7 +11543,7 @@
         <v>204</v>
       </c>
       <c r="B390" s="3" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
     </row>
     <row r="391" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11551,7 +11551,7 @@
         <v>459</v>
       </c>
       <c r="B391" s="3" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="392" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11559,7 +11559,7 @@
         <v>460</v>
       </c>
       <c r="B392" s="3" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="393" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11567,7 +11567,7 @@
         <v>461</v>
       </c>
       <c r="B393" s="3" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="394" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11575,7 +11575,7 @@
         <v>462</v>
       </c>
       <c r="B394" s="3" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="395" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11583,7 +11583,7 @@
         <v>463</v>
       </c>
       <c r="B395" s="3" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="396" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11591,7 +11591,7 @@
         <v>464</v>
       </c>
       <c r="B396" s="3" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="397" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -11599,7 +11599,7 @@
         <v>205</v>
       </c>
       <c r="B397" s="3" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="398" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -11671,7 +11671,7 @@
         <v>207</v>
       </c>
       <c r="B406" s="3" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="407" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -11679,7 +11679,7 @@
         <v>208</v>
       </c>
       <c r="B407" s="3" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="408" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -11687,7 +11687,7 @@
         <v>209</v>
       </c>
       <c r="B408" s="3" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="409" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11695,7 +11695,7 @@
         <v>476</v>
       </c>
       <c r="B409" s="3" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="410" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11703,7 +11703,7 @@
         <v>477</v>
       </c>
       <c r="B410" s="3" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="411" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11711,7 +11711,7 @@
         <v>478</v>
       </c>
       <c r="B411" s="3" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="412" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -11719,7 +11719,7 @@
         <v>479</v>
       </c>
       <c r="B412" s="3" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="413" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -11727,7 +11727,7 @@
         <v>480</v>
       </c>
       <c r="B413" s="4" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="414" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -11735,7 +11735,7 @@
         <v>481</v>
       </c>
       <c r="B414" s="3" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="415" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -11743,7 +11743,7 @@
         <v>621</v>
       </c>
       <c r="B415" s="3" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="416" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -11751,7 +11751,7 @@
         <v>210</v>
       </c>
       <c r="B416" s="3" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="417" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11759,7 +11759,7 @@
         <v>469</v>
       </c>
       <c r="B417" s="3" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="418" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11767,7 +11767,7 @@
         <v>470</v>
       </c>
       <c r="B418" s="3" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="419" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11775,7 +11775,7 @@
         <v>471</v>
       </c>
       <c r="B419" s="3" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="420" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11783,7 +11783,7 @@
         <v>472</v>
       </c>
       <c r="B420" s="3" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="421" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11791,7 +11791,7 @@
         <v>473</v>
       </c>
       <c r="B421" s="3" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="422" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11799,7 +11799,7 @@
         <v>474</v>
       </c>
       <c r="B422" s="3" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="423" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11807,7 +11807,7 @@
         <v>475</v>
       </c>
       <c r="B423" s="3" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="424" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11815,7 +11815,7 @@
         <v>619</v>
       </c>
       <c r="B424" s="3" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="425" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -11823,7 +11823,7 @@
         <v>211</v>
       </c>
       <c r="B425" s="3" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="426" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11831,7 +11831,7 @@
         <v>212</v>
       </c>
       <c r="B426" s="3" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="427" spans="1:2" ht="300" x14ac:dyDescent="0.25">
@@ -11839,7 +11839,7 @@
         <v>419</v>
       </c>
       <c r="B427" s="3" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="428" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11847,7 +11847,7 @@
         <v>420</v>
       </c>
       <c r="B428" s="3" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="429" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -11855,7 +11855,7 @@
         <v>421</v>
       </c>
       <c r="B429" s="3" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="430" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11863,7 +11863,7 @@
         <v>422</v>
       </c>
       <c r="B430" s="3" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="431" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -11871,7 +11871,7 @@
         <v>213</v>
       </c>
       <c r="B431" s="3" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="432" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -11879,7 +11879,7 @@
         <v>214</v>
       </c>
       <c r="B432" s="3" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="433" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -11887,7 +11887,7 @@
         <v>215</v>
       </c>
       <c r="B433" s="3" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="434" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11895,7 +11895,7 @@
         <v>216</v>
       </c>
       <c r="B434" s="3" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="435" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11903,7 +11903,7 @@
         <v>217</v>
       </c>
       <c r="B435" s="3" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="436" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11911,7 +11911,7 @@
         <v>218</v>
       </c>
       <c r="B436" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="437" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11919,7 +11919,7 @@
         <v>219</v>
       </c>
       <c r="B437" s="3" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="438" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11927,7 +11927,7 @@
         <v>220</v>
       </c>
       <c r="B438" s="3" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="439" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11935,7 +11935,7 @@
         <v>221</v>
       </c>
       <c r="B439" s="3" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="440" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11943,7 +11943,7 @@
         <v>222</v>
       </c>
       <c r="B440" s="3" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="441" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11951,7 +11951,7 @@
         <v>223</v>
       </c>
       <c r="B441" s="3" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="442" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -11959,7 +11959,7 @@
         <v>224</v>
       </c>
       <c r="B442" s="3" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="443" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -11967,7 +11967,7 @@
         <v>329</v>
       </c>
       <c r="B443" s="3" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="444" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11975,7 +11975,7 @@
         <v>385</v>
       </c>
       <c r="B444" s="3" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="445" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11983,7 +11983,7 @@
         <v>225</v>
       </c>
       <c r="B445" s="3" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="446" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -11991,7 +11991,7 @@
         <v>226</v>
       </c>
       <c r="B446" s="3" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="447" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -11999,7 +11999,7 @@
         <v>227</v>
       </c>
       <c r="B447" s="3" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="448" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -12007,7 +12007,7 @@
         <v>228</v>
       </c>
       <c r="B448" s="3" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="449" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -12015,7 +12015,7 @@
         <v>618</v>
       </c>
       <c r="B449" s="3" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="450" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12023,7 +12023,7 @@
         <v>229</v>
       </c>
       <c r="B450" s="3" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="451" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -12031,7 +12031,7 @@
         <v>230</v>
       </c>
       <c r="B451" s="3" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="452" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -12039,7 +12039,7 @@
         <v>231</v>
       </c>
       <c r="B452" s="3" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="453" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12047,7 +12047,7 @@
         <v>257</v>
       </c>
       <c r="B453" s="3" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="454" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -12055,7 +12055,7 @@
         <v>379</v>
       </c>
       <c r="B454" s="3" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="455" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12063,7 +12063,7 @@
         <v>380</v>
       </c>
       <c r="B455" s="3" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="456" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12071,7 +12071,7 @@
         <v>444</v>
       </c>
       <c r="B456" s="3" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="457" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12087,15 +12087,15 @@
         <v>531</v>
       </c>
       <c r="B458" s="3" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="459" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A459" s="2" t="s">
+        <v>1161</v>
+      </c>
+      <c r="B459" s="3" t="s">
         <v>1162</v>
-      </c>
-      <c r="B459" s="3" t="s">
-        <v>1163</v>
       </c>
     </row>
     <row r="460" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -12135,7 +12135,7 @@
         <v>602</v>
       </c>
       <c r="B464" s="3" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="465" spans="1:2" ht="255" x14ac:dyDescent="0.25">
@@ -12143,7 +12143,7 @@
         <v>322</v>
       </c>
       <c r="B465" s="3" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="466" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12151,7 +12151,7 @@
         <v>395</v>
       </c>
       <c r="B466" s="3" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="467" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -12159,7 +12159,7 @@
         <v>394</v>
       </c>
       <c r="B467" s="3" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="468" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12167,7 +12167,7 @@
         <v>396</v>
       </c>
       <c r="B468" s="3" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="469" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12175,7 +12175,7 @@
         <v>397</v>
       </c>
       <c r="B469" s="3" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="470" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12183,7 +12183,7 @@
         <v>398</v>
       </c>
       <c r="B470" s="3" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="471" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12191,7 +12191,7 @@
         <v>399</v>
       </c>
       <c r="B471" s="3" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="472" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12199,7 +12199,7 @@
         <v>400</v>
       </c>
       <c r="B472" s="3" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="473" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12207,7 +12207,7 @@
         <v>431</v>
       </c>
       <c r="B473" s="3" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="474" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -12215,7 +12215,7 @@
         <v>432</v>
       </c>
       <c r="B474" s="3" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="475" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -12223,7 +12223,7 @@
         <v>433</v>
       </c>
       <c r="B475" s="3" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="476" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12231,7 +12231,7 @@
         <v>434</v>
       </c>
       <c r="B476" s="3" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="477" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12239,7 +12239,7 @@
         <v>435</v>
       </c>
       <c r="B477" s="3" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="478" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12247,7 +12247,7 @@
         <v>436</v>
       </c>
       <c r="B478" s="3" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="479" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -12255,7 +12255,7 @@
         <v>437</v>
       </c>
       <c r="B479" s="3" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="480" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12263,7 +12263,7 @@
         <v>438</v>
       </c>
       <c r="B480" s="3" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="481" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12271,7 +12271,7 @@
         <v>439</v>
       </c>
       <c r="B481" s="3" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="482" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -12279,7 +12279,7 @@
         <v>440</v>
       </c>
       <c r="B482" s="3" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="483" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12287,7 +12287,7 @@
         <v>441</v>
       </c>
       <c r="B483" s="3" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="484" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -12295,7 +12295,7 @@
         <v>442</v>
       </c>
       <c r="B484" s="3" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="485" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -12303,7 +12303,7 @@
         <v>443</v>
       </c>
       <c r="B485" s="3" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="486" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -12311,7 +12311,7 @@
         <v>458</v>
       </c>
       <c r="B486" s="3" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="487" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -12319,7 +12319,7 @@
         <v>466</v>
       </c>
       <c r="B487" s="3" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="488" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -12327,7 +12327,7 @@
         <v>467</v>
       </c>
       <c r="B488" s="3" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="489" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -12335,7 +12335,7 @@
         <v>468</v>
       </c>
       <c r="B489" s="3" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="490" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -12343,7 +12343,7 @@
         <v>552</v>
       </c>
       <c r="B490" s="3" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="491" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -12351,7 +12351,7 @@
         <v>633</v>
       </c>
       <c r="B491" s="3" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="492" spans="1:2" ht="255" x14ac:dyDescent="0.25">
@@ -12359,7 +12359,7 @@
         <v>488</v>
       </c>
       <c r="B492" s="1" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="493" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12367,7 +12367,7 @@
         <v>489</v>
       </c>
       <c r="B493" s="1" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="494" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12375,7 +12375,7 @@
         <v>490</v>
       </c>
       <c r="B494" s="1" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="495" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12383,7 +12383,7 @@
         <v>491</v>
       </c>
       <c r="B495" s="1" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="496" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12391,7 +12391,7 @@
         <v>492</v>
       </c>
       <c r="B496" s="1" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="497" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12399,7 +12399,7 @@
         <v>493</v>
       </c>
       <c r="B497" s="1" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="498" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12407,7 +12407,7 @@
         <v>494</v>
       </c>
       <c r="B498" s="1" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="499" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12415,7 +12415,7 @@
         <v>495</v>
       </c>
       <c r="B499" s="1" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="500" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12423,7 +12423,7 @@
         <v>496</v>
       </c>
       <c r="B500" s="1" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="501" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -12431,7 +12431,7 @@
         <v>497</v>
       </c>
       <c r="B501" s="1" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="502" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12439,7 +12439,7 @@
         <v>498</v>
       </c>
       <c r="B502" s="1" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="503" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12447,7 +12447,7 @@
         <v>499</v>
       </c>
       <c r="B503" s="1" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="504" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -12455,7 +12455,7 @@
         <v>500</v>
       </c>
       <c r="B504" s="1" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="505" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12463,7 +12463,7 @@
         <v>501</v>
       </c>
       <c r="B505" s="1" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="506" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12471,7 +12471,7 @@
         <v>502</v>
       </c>
       <c r="B506" s="1" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="507" spans="1:2" ht="255" x14ac:dyDescent="0.25">
@@ -12479,7 +12479,7 @@
         <v>597</v>
       </c>
       <c r="B507" s="1" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="508" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12487,7 +12487,7 @@
         <v>598</v>
       </c>
       <c r="B508" s="1" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="509" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12495,7 +12495,7 @@
         <v>503</v>
       </c>
       <c r="B509" s="1" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="510" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12503,7 +12503,7 @@
         <v>515</v>
       </c>
       <c r="B510" s="3" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="511" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -12511,7 +12511,7 @@
         <v>423</v>
       </c>
       <c r="B511" s="3" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="512" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12535,7 +12535,7 @@
         <v>267</v>
       </c>
       <c r="B514" s="1" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="515" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12543,7 +12543,7 @@
         <v>268</v>
       </c>
       <c r="B515" s="1" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="516" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12551,7 +12551,7 @@
         <v>269</v>
       </c>
       <c r="B516" s="1" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="517" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12559,7 +12559,7 @@
         <v>270</v>
       </c>
       <c r="B517" s="1" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="518" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12567,7 +12567,7 @@
         <v>271</v>
       </c>
       <c r="B518" s="1" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="519" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12575,7 +12575,7 @@
         <v>272</v>
       </c>
       <c r="B519" s="1" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="520" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12583,7 +12583,7 @@
         <v>273</v>
       </c>
       <c r="B520" s="1" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="521" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12591,7 +12591,7 @@
         <v>274</v>
       </c>
       <c r="B521" s="1" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="522" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12599,7 +12599,7 @@
         <v>275</v>
       </c>
       <c r="B522" s="1" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="523" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12607,7 +12607,7 @@
         <v>276</v>
       </c>
       <c r="B523" s="1" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="524" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12615,7 +12615,7 @@
         <v>277</v>
       </c>
       <c r="B524" s="1" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="525" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12695,7 +12695,7 @@
         <v>280</v>
       </c>
       <c r="B534" s="1" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="535" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12703,7 +12703,7 @@
         <v>281</v>
       </c>
       <c r="B535" s="1" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="536" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12719,7 +12719,7 @@
         <v>283</v>
       </c>
       <c r="B537" s="1" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="538" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12727,7 +12727,7 @@
         <v>284</v>
       </c>
       <c r="B538" s="1" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="539" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12735,7 +12735,7 @@
         <v>285</v>
       </c>
       <c r="B539" s="1" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="540" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12743,7 +12743,7 @@
         <v>286</v>
       </c>
       <c r="B540" s="1" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="541" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12791,7 +12791,7 @@
         <v>292</v>
       </c>
       <c r="B546" s="1" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="547" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12799,7 +12799,7 @@
         <v>293</v>
       </c>
       <c r="B547" s="1" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="548" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12807,7 +12807,7 @@
         <v>294</v>
       </c>
       <c r="B548" s="1" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="549" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12815,7 +12815,7 @@
         <v>295</v>
       </c>
       <c r="B549" s="1" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="550" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -12823,7 +12823,7 @@
         <v>296</v>
       </c>
       <c r="B550" s="1" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="551" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12831,7 +12831,7 @@
         <v>297</v>
       </c>
       <c r="B551" s="1" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="552" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -12839,7 +12839,7 @@
         <v>353</v>
       </c>
       <c r="B552" s="1" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="553" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12847,7 +12847,7 @@
         <v>365</v>
       </c>
       <c r="B553" s="3" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="554" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12855,7 +12855,7 @@
         <v>366</v>
       </c>
       <c r="B554" s="1" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="555" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12863,7 +12863,7 @@
         <v>298</v>
       </c>
       <c r="B555" s="1" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="556" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -12871,7 +12871,7 @@
         <v>364</v>
       </c>
       <c r="B556" s="1" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="557" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12879,7 +12879,7 @@
         <v>299</v>
       </c>
       <c r="B557" s="1" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="558" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -12887,7 +12887,7 @@
         <v>354</v>
       </c>
       <c r="B558" s="1" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
     </row>
     <row r="559" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -12903,7 +12903,7 @@
         <v>300</v>
       </c>
       <c r="B560" s="1" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
     </row>
     <row r="561" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12911,7 +12911,7 @@
         <v>301</v>
       </c>
       <c r="B561" s="1" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="562" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12919,7 +12919,7 @@
         <v>302</v>
       </c>
       <c r="B562" s="1" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="563" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12927,7 +12927,7 @@
         <v>303</v>
       </c>
       <c r="B563" s="1" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="564" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -12935,7 +12935,7 @@
         <v>363</v>
       </c>
       <c r="B564" s="1" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="565" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12943,7 +12943,7 @@
         <v>304</v>
       </c>
       <c r="B565" s="1" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="566" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12951,7 +12951,7 @@
         <v>361</v>
       </c>
       <c r="B566" s="1" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="567" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -12967,7 +12967,7 @@
         <v>517</v>
       </c>
       <c r="B568" s="1" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="569" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12975,7 +12975,7 @@
         <v>305</v>
       </c>
       <c r="B569" s="1" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="570" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12983,7 +12983,7 @@
         <v>358</v>
       </c>
       <c r="B570" s="1" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="571" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12991,7 +12991,7 @@
         <v>359</v>
       </c>
       <c r="B571" s="1" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="572" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -13007,7 +13007,7 @@
         <v>518</v>
       </c>
       <c r="B573" s="1" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="574" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -13015,7 +13015,7 @@
         <v>306</v>
       </c>
       <c r="B574" s="1" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="575" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -13023,7 +13023,7 @@
         <v>352</v>
       </c>
       <c r="B575" s="1" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="576" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -13031,7 +13031,7 @@
         <v>355</v>
       </c>
       <c r="B576" s="3" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="577" spans="1:2" ht="405" x14ac:dyDescent="0.25">
@@ -13039,7 +13039,7 @@
         <v>307</v>
       </c>
       <c r="B577" s="1" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="578" spans="1:2" ht="375" x14ac:dyDescent="0.25">
@@ -13047,7 +13047,7 @@
         <v>311</v>
       </c>
       <c r="B578" s="1" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="579" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -13071,7 +13071,7 @@
         <v>349</v>
       </c>
       <c r="B581" s="3" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="582" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -13079,7 +13079,7 @@
         <v>519</v>
       </c>
       <c r="B582" s="3" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="583" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -13087,7 +13087,7 @@
         <v>326</v>
       </c>
       <c r="B583" s="3" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add new option for easy route.  Change easy monster to only degrade combat by 2
</commit_message>
<xml_diff>
--- a/Documentation/Events.xlsx
+++ b/Documentation/Events.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\happysulla\BarbarianPrince\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstewa01\Documents\Visual Studio 2022\Projects\BarbarianPrince\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4400EF6A-9D95-4150-BF11-AEEAA5F61C21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9F54493C-0147-4F21-AB8D-5B8F8466B4E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="-25320" yWindow="15" windowWidth="25440" windowHeight="15390" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" r:id="rId1"/>
@@ -4321,17 +4321,6 @@
                                              &lt;InlineUIContainer&gt;&lt;Image Source='../bin/Images/Orc.gif'  Height='250' Width='170'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e055a Following Orcs&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;You are following goblins
- &lt;InlineUIContainer&gt;&lt;Button Content='r219' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
- Roll a die and if the result equals or is less than your wit and wiles, the band does not discover you. If it exceeds, they discover you and your party gets the first strike in combat
- &lt;InlineUIContainer&gt;&lt;Button Content='r220' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
- If they do not discover you, see
- &lt;InlineUIContainer&gt;&lt;Button Content='e055b' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
- where they lead you.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt; Roll one die:  &lt;InlineUIContainer&gt;&lt;Image Source='../bin/Images/dieRoll.gif' Name='DieRoll' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;e055b Following Orcs Undiscovered&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;You are following orcs and not discovered
  &lt;InlineUIContainer&gt;&lt;Button Content='r219' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
@@ -8028,6 +8017,17 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;The falcon can only act as a guide. It has no combat skill or endurance value. Any wound will kill it. Click image to continue if not feeding.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
                                         &lt;InlineUIContainer&gt;&lt;Image Name='FalconNoFeed' Source='../bin/Images/Falcon.gif' Height='188' Width='250'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e055a Following Orcs&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;You are following orcs
+ &lt;InlineUIContainer&gt;&lt;Button Content='r219' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
+ Roll a die and if the result equals or is less than your wit and wiles, the band does not discover you. If it exceeds, they discover you and your party gets the first strike in combat
+ &lt;InlineUIContainer&gt;&lt;Button Content='r220' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
+ If they do not discover you, see
+ &lt;InlineUIContainer&gt;&lt;Button Content='e055b' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+ where they lead you.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt; Roll one die:  &lt;InlineUIContainer&gt;&lt;Image Source='../bin/Images/dieRoll.gif' Name='DieRoll' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
 </sst>
 </file>
@@ -8416,8 +8416,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B583"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A285" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B287" sqref="B287"/>
+    <sheetView tabSelected="1" topLeftCell="B157" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B154" sqref="B154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9199,7 +9199,7 @@
         <v>61</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -9455,7 +9455,7 @@
         <v>350</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="130" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -9791,7 +9791,7 @@
         <v>542</v>
       </c>
       <c r="B171" s="3" t="s">
-        <v>806</v>
+        <v>1165</v>
       </c>
     </row>
     <row r="172" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -9799,7 +9799,7 @@
         <v>543</v>
       </c>
       <c r="B172" s="3" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
     </row>
     <row r="173" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -9807,7 +9807,7 @@
         <v>91</v>
       </c>
       <c r="B173" s="3" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
     </row>
     <row r="174" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -9815,7 +9815,7 @@
         <v>382</v>
       </c>
       <c r="B174" s="3" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
     </row>
     <row r="175" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -9823,7 +9823,7 @@
         <v>92</v>
       </c>
       <c r="B175" s="3" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
     </row>
     <row r="176" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -9831,7 +9831,7 @@
         <v>93</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
     </row>
     <row r="177" spans="1:2" ht="270" x14ac:dyDescent="0.25">
@@ -9855,7 +9855,7 @@
         <v>96</v>
       </c>
       <c r="B179" s="3" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
     </row>
     <row r="180" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -9863,7 +9863,7 @@
         <v>547</v>
       </c>
       <c r="B180" s="3" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
     </row>
     <row r="181" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -9871,7 +9871,7 @@
         <v>548</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
     </row>
     <row r="182" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -9879,7 +9879,7 @@
         <v>549</v>
       </c>
       <c r="B182" s="3" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
     </row>
     <row r="183" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -9887,7 +9887,7 @@
         <v>550</v>
       </c>
       <c r="B183" s="3" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
     </row>
     <row r="184" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -9895,7 +9895,7 @@
         <v>556</v>
       </c>
       <c r="B184" s="3" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
     </row>
     <row r="185" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -9911,7 +9911,7 @@
         <v>97</v>
       </c>
       <c r="B186" s="3" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
     </row>
     <row r="187" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -9919,7 +9919,7 @@
         <v>98</v>
       </c>
       <c r="B187" s="3" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="188" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -9927,7 +9927,7 @@
         <v>99</v>
       </c>
       <c r="B188" s="3" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
     </row>
     <row r="189" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -9935,7 +9935,7 @@
         <v>101</v>
       </c>
       <c r="B189" s="3" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
     </row>
     <row r="190" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -9943,7 +9943,7 @@
         <v>100</v>
       </c>
       <c r="B190" s="3" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
     </row>
     <row r="191" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -9951,7 +9951,7 @@
         <v>102</v>
       </c>
       <c r="B191" s="3" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
     </row>
     <row r="192" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -9959,7 +9959,7 @@
         <v>103</v>
       </c>
       <c r="B192" s="3" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
     </row>
     <row r="193" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -9967,7 +9967,7 @@
         <v>104</v>
       </c>
       <c r="B193" s="3" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
     </row>
     <row r="194" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -9975,7 +9975,7 @@
         <v>105</v>
       </c>
       <c r="B194" s="3" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
     </row>
     <row r="195" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -9983,7 +9983,7 @@
         <v>504</v>
       </c>
       <c r="B195" s="3" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
     </row>
     <row r="196" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -9991,7 +9991,7 @@
         <v>505</v>
       </c>
       <c r="B196" s="3" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
     <row r="197" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -9999,7 +9999,7 @@
         <v>106</v>
       </c>
       <c r="B197" s="3" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
     </row>
     <row r="198" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10007,7 +10007,7 @@
         <v>107</v>
       </c>
       <c r="B198" s="3" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
     </row>
     <row r="199" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -10015,7 +10015,7 @@
         <v>165</v>
       </c>
       <c r="B199" s="3" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
     </row>
     <row r="200" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -10023,7 +10023,7 @@
         <v>544</v>
       </c>
       <c r="B200" s="3" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
     </row>
     <row r="201" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -10031,7 +10031,7 @@
         <v>108</v>
       </c>
       <c r="B201" s="3" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
     </row>
     <row r="202" spans="1:2" ht="285" x14ac:dyDescent="0.25">
@@ -10039,7 +10039,7 @@
         <v>109</v>
       </c>
       <c r="B202" s="3" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
     </row>
     <row r="203" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -10047,7 +10047,7 @@
         <v>110</v>
       </c>
       <c r="B203" s="3" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
     <row r="204" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -10055,7 +10055,7 @@
         <v>166</v>
       </c>
       <c r="B204" s="3" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="205" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -10063,7 +10063,7 @@
         <v>167</v>
       </c>
       <c r="B205" s="3" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
     <row r="206" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -10071,7 +10071,7 @@
         <v>168</v>
       </c>
       <c r="B206" s="3" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
     </row>
     <row r="207" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -10079,7 +10079,7 @@
         <v>562</v>
       </c>
       <c r="B207" s="3" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
     </row>
     <row r="208" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10095,7 +10095,7 @@
         <v>111</v>
       </c>
       <c r="B209" s="3" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
     </row>
     <row r="210" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10103,7 +10103,7 @@
         <v>510</v>
       </c>
       <c r="B210" s="3" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
     </row>
     <row r="211" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -10111,7 +10111,7 @@
         <v>511</v>
       </c>
       <c r="B211" s="3" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
     </row>
     <row r="212" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -10127,7 +10127,7 @@
         <v>516</v>
       </c>
       <c r="B213" s="3" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
     </row>
     <row r="214" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10135,7 +10135,7 @@
         <v>112</v>
       </c>
       <c r="B214" s="3" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
     </row>
     <row r="215" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10143,7 +10143,7 @@
         <v>169</v>
       </c>
       <c r="B215" s="3" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
     </row>
     <row r="216" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10151,7 +10151,7 @@
         <v>170</v>
       </c>
       <c r="B216" s="3" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
     </row>
     <row r="217" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10159,7 +10159,7 @@
         <v>171</v>
       </c>
       <c r="B217" s="3" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="218" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -10167,7 +10167,7 @@
         <v>113</v>
       </c>
       <c r="B218" s="3" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
     </row>
     <row r="219" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -10175,7 +10175,7 @@
         <v>114</v>
       </c>
       <c r="B219" s="3" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="220" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10183,7 +10183,7 @@
         <v>266</v>
       </c>
       <c r="B220" s="3" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="221" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -10191,7 +10191,7 @@
         <v>570</v>
       </c>
       <c r="B221" s="3" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
     </row>
     <row r="222" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10199,7 +10199,7 @@
         <v>115</v>
       </c>
       <c r="B222" s="3" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="223" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10207,7 +10207,7 @@
         <v>522</v>
       </c>
       <c r="B223" s="3" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="224" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -10215,7 +10215,7 @@
         <v>116</v>
       </c>
       <c r="B224" s="3" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
     </row>
     <row r="225" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10223,7 +10223,7 @@
         <v>520</v>
       </c>
       <c r="B225" s="3" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
     </row>
     <row r="226" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10231,7 +10231,7 @@
         <v>117</v>
       </c>
       <c r="B226" s="4" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
     </row>
     <row r="227" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10239,7 +10239,7 @@
         <v>523</v>
       </c>
       <c r="B227" s="4" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
     </row>
     <row r="228" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10247,7 +10247,7 @@
         <v>524</v>
       </c>
       <c r="B228" s="4" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
     </row>
     <row r="229" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10255,7 +10255,7 @@
         <v>525</v>
       </c>
       <c r="B229" s="4" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
     </row>
     <row r="230" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10263,7 +10263,7 @@
         <v>118</v>
       </c>
       <c r="B230" s="3" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
     </row>
     <row r="231" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -10271,7 +10271,7 @@
         <v>573</v>
       </c>
       <c r="B231" s="3" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
     </row>
     <row r="232" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10279,7 +10279,7 @@
         <v>574</v>
       </c>
       <c r="B232" s="3" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
     </row>
     <row r="233" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10287,7 +10287,7 @@
         <v>119</v>
       </c>
       <c r="B233" s="3" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
     </row>
     <row r="234" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10295,7 +10295,7 @@
         <v>566</v>
       </c>
       <c r="B234" s="3" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
     </row>
     <row r="235" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10303,7 +10303,7 @@
         <v>565</v>
       </c>
       <c r="B235" s="3" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
     </row>
     <row r="236" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10311,7 +10311,7 @@
         <v>120</v>
       </c>
       <c r="B236" s="3" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
     </row>
     <row r="237" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -10319,7 +10319,7 @@
         <v>172</v>
       </c>
       <c r="B237" s="3" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
     </row>
     <row r="238" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10327,7 +10327,7 @@
         <v>173</v>
       </c>
       <c r="B238" s="3" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="239" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10335,7 +10335,7 @@
         <v>174</v>
       </c>
       <c r="B239" s="3" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
     </row>
     <row r="240" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -10343,7 +10343,7 @@
         <v>121</v>
       </c>
       <c r="B240" s="3" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
     </row>
     <row r="241" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10351,7 +10351,7 @@
         <v>122</v>
       </c>
       <c r="B241" s="3" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
     </row>
     <row r="242" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10359,7 +10359,7 @@
         <v>521</v>
       </c>
       <c r="B242" s="3" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
     </row>
     <row r="243" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -10367,7 +10367,7 @@
         <v>123</v>
       </c>
       <c r="B243" s="3" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
     </row>
     <row r="244" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10375,7 +10375,7 @@
         <v>571</v>
       </c>
       <c r="B244" s="3" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
     </row>
     <row r="245" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10383,7 +10383,7 @@
         <v>572</v>
       </c>
       <c r="B245" s="3" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
     </row>
     <row r="246" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10391,7 +10391,7 @@
         <v>124</v>
       </c>
       <c r="B246" s="3" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
     </row>
     <row r="247" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10399,7 +10399,7 @@
         <v>617</v>
       </c>
       <c r="B247" s="3" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
     </row>
     <row r="248" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10407,7 +10407,7 @@
         <v>125</v>
       </c>
       <c r="B248" s="3" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
     </row>
     <row r="249" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -10415,7 +10415,7 @@
         <v>589</v>
       </c>
       <c r="B249" s="3" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
     </row>
     <row r="250" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10423,7 +10423,7 @@
         <v>126</v>
       </c>
       <c r="B250" s="3" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
     </row>
     <row r="251" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -10431,7 +10431,7 @@
         <v>127</v>
       </c>
       <c r="B251" s="3" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
     </row>
     <row r="252" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10439,7 +10439,7 @@
         <v>128</v>
       </c>
       <c r="B252" s="3" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
     </row>
     <row r="253" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -10447,7 +10447,7 @@
         <v>129</v>
       </c>
       <c r="B253" s="3" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
     </row>
     <row r="254" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10455,7 +10455,7 @@
         <v>130</v>
       </c>
       <c r="B254" s="3" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
     </row>
     <row r="255" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -10463,7 +10463,7 @@
         <v>131</v>
       </c>
       <c r="B255" s="3" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
     </row>
     <row r="256" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -10471,7 +10471,7 @@
         <v>576</v>
       </c>
       <c r="B256" s="3" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
     </row>
     <row r="257" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10479,7 +10479,7 @@
         <v>577</v>
       </c>
       <c r="B257" s="3" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
     </row>
     <row r="258" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -10487,7 +10487,7 @@
         <v>132</v>
       </c>
       <c r="B258" s="3" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
     </row>
     <row r="259" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10495,7 +10495,7 @@
         <v>133</v>
       </c>
       <c r="B259" s="3" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
     </row>
     <row r="260" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10503,7 +10503,7 @@
         <v>575</v>
       </c>
       <c r="B260" s="3" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
     </row>
     <row r="261" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -10511,7 +10511,7 @@
         <v>134</v>
       </c>
       <c r="B261" s="3" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="262" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10519,7 +10519,7 @@
         <v>590</v>
       </c>
       <c r="B262" s="3" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="263" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10527,7 +10527,7 @@
         <v>591</v>
       </c>
       <c r="B263" s="3" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
     </row>
     <row r="264" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -10535,7 +10535,7 @@
         <v>135</v>
       </c>
       <c r="B264" s="3" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="265" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -10543,7 +10543,7 @@
         <v>592</v>
       </c>
       <c r="B265" s="3" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
     </row>
     <row r="266" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10551,7 +10551,7 @@
         <v>136</v>
       </c>
       <c r="B266" s="3" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
     </row>
     <row r="267" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -10559,7 +10559,7 @@
         <v>137</v>
       </c>
       <c r="B267" s="3" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
     </row>
     <row r="268" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10567,7 +10567,7 @@
         <v>232</v>
       </c>
       <c r="B268" s="3" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
     </row>
     <row r="269" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10575,7 +10575,7 @@
         <v>233</v>
       </c>
       <c r="B269" s="3" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
     </row>
     <row r="270" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -10591,7 +10591,7 @@
         <v>234</v>
       </c>
       <c r="B271" s="3" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
     </row>
     <row r="272" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10599,7 +10599,7 @@
         <v>235</v>
       </c>
       <c r="B272" s="3" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
     </row>
     <row r="273" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -10615,7 +10615,7 @@
         <v>239</v>
       </c>
       <c r="B274" s="3" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
     </row>
     <row r="275" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10623,7 +10623,7 @@
         <v>240</v>
       </c>
       <c r="B275" s="3" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
     </row>
     <row r="276" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10631,7 +10631,7 @@
         <v>241</v>
       </c>
       <c r="B276" s="3" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="277" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10647,7 +10647,7 @@
         <v>236</v>
       </c>
       <c r="B278" s="3" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
     </row>
     <row r="279" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10655,7 +10655,7 @@
         <v>237</v>
       </c>
       <c r="B279" s="3" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
     </row>
     <row r="280" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10663,7 +10663,7 @@
         <v>238</v>
       </c>
       <c r="B280" s="3" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
     </row>
     <row r="281" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10671,7 +10671,7 @@
         <v>141</v>
       </c>
       <c r="B281" s="3" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
     </row>
     <row r="282" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10679,7 +10679,7 @@
         <v>142</v>
       </c>
       <c r="B282" s="3" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
     </row>
     <row r="283" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10687,7 +10687,7 @@
         <v>143</v>
       </c>
       <c r="B283" s="3" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="284" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -10695,7 +10695,7 @@
         <v>144</v>
       </c>
       <c r="B284" s="3" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="285" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10703,7 +10703,7 @@
         <v>242</v>
       </c>
       <c r="B285" s="3" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
     </row>
     <row r="286" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10711,7 +10711,7 @@
         <v>145</v>
       </c>
       <c r="B286" s="3" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
     </row>
     <row r="287" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10719,7 +10719,7 @@
         <v>146</v>
       </c>
       <c r="B287" s="3" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="288" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10727,7 +10727,7 @@
         <v>147</v>
       </c>
       <c r="B288" s="3" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
     </row>
     <row r="289" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10735,7 +10735,7 @@
         <v>148</v>
       </c>
       <c r="B289" s="3" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
     </row>
     <row r="290" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10743,7 +10743,7 @@
         <v>149</v>
       </c>
       <c r="B290" s="3" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
     </row>
     <row r="291" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10751,7 +10751,7 @@
         <v>605</v>
       </c>
       <c r="B291" s="3" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
     </row>
     <row r="292" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10759,7 +10759,7 @@
         <v>604</v>
       </c>
       <c r="B292" s="3" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
     </row>
     <row r="293" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10767,7 +10767,7 @@
         <v>606</v>
       </c>
       <c r="B293" s="3" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
     </row>
     <row r="294" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10775,7 +10775,7 @@
         <v>150</v>
       </c>
       <c r="B294" s="3" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="295" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10783,7 +10783,7 @@
         <v>607</v>
       </c>
       <c r="B295" s="3" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
     </row>
     <row r="296" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -10791,7 +10791,7 @@
         <v>151</v>
       </c>
       <c r="B296" s="3" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
     </row>
     <row r="297" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10799,7 +10799,7 @@
         <v>243</v>
       </c>
       <c r="B297" s="3" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
     </row>
     <row r="298" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10807,7 +10807,7 @@
         <v>244</v>
       </c>
       <c r="B298" s="3" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
     </row>
     <row r="299" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10815,7 +10815,7 @@
         <v>245</v>
       </c>
       <c r="B299" s="3" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
     </row>
     <row r="300" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10823,7 +10823,7 @@
         <v>152</v>
       </c>
       <c r="B300" s="3" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
     </row>
     <row r="301" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10831,7 +10831,7 @@
         <v>153</v>
       </c>
       <c r="B301" s="3" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
     </row>
     <row r="302" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10839,7 +10839,7 @@
         <v>154</v>
       </c>
       <c r="B302" s="3" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
     </row>
     <row r="303" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -10847,7 +10847,7 @@
         <v>155</v>
       </c>
       <c r="B303" s="3" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
     </row>
     <row r="304" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10855,7 +10855,7 @@
         <v>156</v>
       </c>
       <c r="B304" s="3" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
     </row>
     <row r="305" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10871,7 +10871,7 @@
         <v>246</v>
       </c>
       <c r="B306" s="3" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
     </row>
     <row r="307" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10879,7 +10879,7 @@
         <v>247</v>
       </c>
       <c r="B307" s="3" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
     </row>
     <row r="308" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10887,7 +10887,7 @@
         <v>248</v>
       </c>
       <c r="B308" s="3" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
     </row>
     <row r="309" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10903,7 +10903,7 @@
         <v>159</v>
       </c>
       <c r="B310" s="3" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
     </row>
     <row r="311" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10911,7 +10911,7 @@
         <v>160</v>
       </c>
       <c r="B311" s="3" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
     </row>
     <row r="312" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -10919,7 +10919,7 @@
         <v>161</v>
       </c>
       <c r="B312" s="3" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
     </row>
     <row r="313" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -10927,7 +10927,7 @@
         <v>162</v>
       </c>
       <c r="B313" s="3" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
     </row>
     <row r="314" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -10935,7 +10935,7 @@
         <v>599</v>
       </c>
       <c r="B314" s="3" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
     </row>
     <row r="315" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10943,7 +10943,7 @@
         <v>600</v>
       </c>
       <c r="B315" s="3" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
     </row>
     <row r="316" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10951,7 +10951,7 @@
         <v>601</v>
       </c>
       <c r="B316" s="3" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
     </row>
     <row r="317" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10959,7 +10959,7 @@
         <v>163</v>
       </c>
       <c r="B317" s="3" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
     </row>
     <row r="318" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10967,7 +10967,7 @@
         <v>164</v>
       </c>
       <c r="B318" s="3" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
     </row>
     <row r="319" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10975,7 +10975,7 @@
         <v>175</v>
       </c>
       <c r="B319" s="3" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
     </row>
     <row r="320" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -10983,7 +10983,7 @@
         <v>176</v>
       </c>
       <c r="B320" s="3" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
     </row>
     <row r="321" spans="1:2" ht="390" x14ac:dyDescent="0.25">
@@ -10991,7 +10991,7 @@
         <v>177</v>
       </c>
       <c r="B321" s="3" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
     </row>
     <row r="322" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -11007,7 +11007,7 @@
         <v>414</v>
       </c>
       <c r="B323" s="3" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
     </row>
     <row r="324" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11015,7 +11015,7 @@
         <v>415</v>
       </c>
       <c r="B324" s="3" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
     </row>
     <row r="325" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -11023,7 +11023,7 @@
         <v>416</v>
       </c>
       <c r="B325" s="3" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
     </row>
     <row r="326" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -11031,7 +11031,7 @@
         <v>417</v>
       </c>
       <c r="B326" s="3" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
     </row>
     <row r="327" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11039,7 +11039,7 @@
         <v>418</v>
       </c>
       <c r="B327" s="3" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
     </row>
     <row r="328" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11047,7 +11047,7 @@
         <v>613</v>
       </c>
       <c r="B328" s="3" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
     </row>
     <row r="329" spans="1:2" ht="390" x14ac:dyDescent="0.25">
@@ -11055,7 +11055,7 @@
         <v>178</v>
       </c>
       <c r="B329" s="3" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
     </row>
     <row r="330" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -11071,7 +11071,7 @@
         <v>426</v>
       </c>
       <c r="B331" s="3" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
     </row>
     <row r="332" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11079,7 +11079,7 @@
         <v>427</v>
       </c>
       <c r="B332" s="3" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
     </row>
     <row r="333" spans="1:2" ht="315" x14ac:dyDescent="0.25">
@@ -11087,7 +11087,7 @@
         <v>179</v>
       </c>
       <c r="B333" s="3" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
     </row>
     <row r="334" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -11095,7 +11095,7 @@
         <v>249</v>
       </c>
       <c r="B334" s="3" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
     </row>
     <row r="335" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -11103,7 +11103,7 @@
         <v>250</v>
       </c>
       <c r="B335" s="3" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
     </row>
     <row r="336" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -11111,7 +11111,7 @@
         <v>251</v>
       </c>
       <c r="B336" s="3" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
     </row>
     <row r="337" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11119,7 +11119,7 @@
         <v>252</v>
       </c>
       <c r="B337" s="3" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
     </row>
     <row r="338" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -11127,7 +11127,7 @@
         <v>253</v>
       </c>
       <c r="B338" s="3" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
     </row>
     <row r="339" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -11135,7 +11135,7 @@
         <v>545</v>
       </c>
       <c r="B339" s="3" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
     </row>
     <row r="340" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -11143,7 +11143,7 @@
         <v>546</v>
       </c>
       <c r="B340" s="3" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
     </row>
     <row r="341" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11151,7 +11151,7 @@
         <v>180</v>
       </c>
       <c r="B341" s="3" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
     </row>
     <row r="342" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11159,7 +11159,7 @@
         <v>181</v>
       </c>
       <c r="B342" s="3" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="343" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11167,7 +11167,7 @@
         <v>386</v>
       </c>
       <c r="B343" s="3" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
     </row>
     <row r="344" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -11183,7 +11183,7 @@
         <v>622</v>
       </c>
       <c r="B345" s="3" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
     </row>
     <row r="346" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11191,7 +11191,7 @@
         <v>183</v>
       </c>
       <c r="B346" s="3" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
     </row>
     <row r="347" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -11199,7 +11199,7 @@
         <v>184</v>
       </c>
       <c r="B347" s="3" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
     </row>
     <row r="348" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -11215,7 +11215,7 @@
         <v>185</v>
       </c>
       <c r="B349" s="3" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
     </row>
     <row r="350" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -11223,7 +11223,7 @@
         <v>186</v>
       </c>
       <c r="B350" s="3" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
     </row>
     <row r="351" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -11231,7 +11231,7 @@
         <v>187</v>
       </c>
       <c r="B351" s="3" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
     </row>
     <row r="352" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11247,7 +11247,7 @@
         <v>188</v>
       </c>
       <c r="B353" s="3" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
     </row>
     <row r="354" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -11255,7 +11255,7 @@
         <v>189</v>
       </c>
       <c r="B354" s="3" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
     </row>
     <row r="355" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -11263,7 +11263,7 @@
         <v>383</v>
       </c>
       <c r="B355" s="3" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
     </row>
     <row r="356" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -11271,7 +11271,7 @@
         <v>384</v>
       </c>
       <c r="B356" s="3" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
     </row>
     <row r="357" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -11279,7 +11279,7 @@
         <v>190</v>
       </c>
       <c r="B357" s="3" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
     </row>
     <row r="358" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -11287,7 +11287,7 @@
         <v>191</v>
       </c>
       <c r="B358" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="359" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -11295,7 +11295,7 @@
         <v>192</v>
       </c>
       <c r="B359" s="3" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
     </row>
     <row r="360" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -11303,7 +11303,7 @@
         <v>465</v>
       </c>
       <c r="B360" s="3" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
     </row>
     <row r="361" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -11311,7 +11311,7 @@
         <v>193</v>
       </c>
       <c r="B361" s="3" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
     </row>
     <row r="362" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -11327,7 +11327,7 @@
         <v>333</v>
   